<commit_message>
Customer and Sales class creaton.
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0194EA04-08D5-1A48-BDE6-F2E41BBAEE96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96DA2A9-DB86-E14C-9C91-0EBA98B0B5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="1000" windowWidth="27640" windowHeight="16160" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
+    <workbookView xWindow="300" yWindow="1000" windowWidth="27640" windowHeight="16160" activeTab="1" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="SPEC - 1.1" sheetId="1" r:id="rId1"/>
+    <sheet name="SPEC - 1.2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="100">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -1611,12 +1612,551 @@
         new file:   js/index.js</t>
     </r>
   </si>
+  <si>
+    <t>GIT BRANCH - init</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create the git branch </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>init</t>
+    </r>
+  </si>
+  <si>
+    <t>git branch init</t>
+  </si>
+  <si>
+    <t>git checkout init</t>
+  </si>
+  <si>
+    <t>Switched to branch 'init'</t>
+  </si>
+  <si>
+    <t>touch js/customer.js</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/customer.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> file</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ls js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> will display </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>customer.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> file</t>
+    </r>
+  </si>
+  <si>
+    <t>/* * The Customer class.
+ *  @author   Sanket Rajgarhia
+ *  @date 30/03/2022 (dd/mm/yyyy)
+ *  @version 1.0
+ * */
+class Customer {
+   /* *Constructor
+    * @param    {String} customerName    Name of the customer
+    * @param    {String} phoneNumber    10 Digit Phone Number of the customer
+    * @param    {String} address        150 characters address
+    * */
+    constructor(customerName, phoneNumber, address) {
+        this._customerName = customerName;
+        this._phoneNumber = phoneNumber;
+        this._address = address;
+    }
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Switch to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">init </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>branch.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>git branch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> displays the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>init</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> branch.</t>
+    </r>
+  </si>
+  <si>
+    <t>touch js/sales.js</t>
+  </si>
+  <si>
+    <r>
+      <t>Create the j</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>s/sales.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> file</t>
+    </r>
+  </si>
+  <si>
+    <t>ls js will display sales.js file</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add the getter and setter methods for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Customer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> class</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">    /* Get the customer name
+     * @return {String} Customer name
+     */
+    get customerName() {
+        return this._customerName;
+    }
+    /* Set the customer name
+     * @param   {String} customerName  Name of the customer
+     */
+    set customerName(customerName) {
+        this._customerName = customerName;
+    }
+    /* Get the customer phone number
+     * @return  {String} Customer phone number
+     */
+    get phoneNumber() {
+        return this._phoneNumber;
+    }
+    /* Set the phone number
+     * @param   {String} phoneNumber    10 Digit Phone Number of the customer
+     */
+    set phoneNumber(phoneNumber) {
+        this._phoneNumber = phoneNumber;
+    }
+    /* Get the customer address
+     * @return  {String} Customer address
+     */
+    get address() {
+        return this._address;
+    }
+    /* Set the address
+     * @param   {String} address   150 characters address
+     */
+    set address(address) {
+        this._address = address;
+    }</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Added the getter and setter methods for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Customer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> class</t>
+    </r>
+  </si>
+  <si>
+    <t>Customer and Sales Object Creation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Customer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> class as per specification.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Customer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> class has been created.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Sales</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> class as per specification.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Sales</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> class has been created.</t>
+    </r>
+  </si>
+  <si>
+    <t>/* * The Sales class.
+ *  @author   Sanket Rajgarhia
+ *  @date 30/03/2022 (dd/mm/yyyy)
+ *  @version 1.0
+ * */
+class Sales {
+    /* *Constructor
+     * @param    {String} salesPersonId     ID of the sales person
+     * @param    {String} salesPersonName   Name of the sales person
+     * @param    {String} salesLocation     150 characters sales location/address
+     * */
+    constructor(salesPersonId, salesPersonName, salesLocation) {
+        this._salesPersonId = salesPersonId;
+        this._salesPersonName = salesPersonName;
+        this._salesLocation = salesLocation;
+    }
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    /* Get the ID of the sales person
+     * @return  {String}    ID of the sales person
+     */
+    get salesPersonId() {
+        return this._salesPersonId;
+    }
+    /* Set the ID of the sales person
+     * @param  {String} salesPersonId   ID of the sales person
+     */
+    set salesPersonId(salesPersonId) {
+        this._salesPersonId = salesPersonId;
+    }
+    /* Get the name of the sales person
+     * @return  {String}    Name of the sales person
+     */
+    get salesPersonName() {
+        return this._salesPersonName;
+    }
+    /* Set the name of the sales person
+     * @param    {String} salesPersonName   Name of the sales person
+     */
+    set salesPersonName(salesPersonName) {
+        this.salesPersonName = salesPersonName;
+    }
+    /* Get the location of the sale
+     * @return  {String}    150 characters sales location/address
+     */
+    get salesLocation() {
+        return this._salesLocation;
+    }
+    /* Set the location of the sale
+     * @param    {String} salesLocation     150 characters sales location/address
+     */
+    set salesLocation(salesLocation) {
+        this._salesLocation = salesLocation;
+    }</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add the getter and setter methods for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Sales</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> class</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Added the getter and setter methods for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Sales</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> class</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>git status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - would display the following files.                                                                                                                                                                                                   new file:   js/customer.js
+new file:   js/sales.js                                                                                                          modified:   docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx</t>
+    </r>
+  </si>
+  <si>
+    <t>git commit -m "Customer and Sales class creaton."</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">On branch </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>init</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> nothing to commit, working tree clean</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1684,8 +2224,34 @@
       <name val="Century Gothic"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFC000"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFC000"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1716,8 +2282,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1740,12 +2312,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1801,6 +2399,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2120,7 +2745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5478EA92-7E5A-F546-AF17-9135CC9AA7B9}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -2410,4 +3035,215 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB926B8F-5A7D-9B4E-BEE4-06FF437DD437}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="65.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="22"/>
+    </row>
+    <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+    </row>
+    <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="356" x14ac:dyDescent="0.2">
+      <c r="A12" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="24"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="24"/>
+    </row>
+    <row r="15" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="404" x14ac:dyDescent="0.2">
+      <c r="A16" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="24"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="24"/>
+    </row>
+    <row r="19" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A19" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="9">
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:C14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Door Enumeration (EN) and Door class creaton.
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E96DA2A9-DB86-E14C-9C91-0EBA98B0B5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA851E79-2EB4-BC4D-8ADF-6C6E74EBC8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="1000" windowWidth="27640" windowHeight="16160" activeTab="1" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
+    <workbookView xWindow="300" yWindow="1000" windowWidth="27640" windowHeight="16160" activeTab="2" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="SPEC - 1.1" sheetId="1" r:id="rId1"/>
     <sheet name="SPEC - 1.2" sheetId="2" r:id="rId2"/>
+    <sheet name="SPEC - 1.3" sheetId="4" r:id="rId3"/>
+    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId4"/>
+    <sheet name="PLAYGROUND" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="299">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -1899,9 +1902,6 @@
     </r>
   </si>
   <si>
-    <t>Customer and Sales Object Creation</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Create the </t>
     </r>
@@ -2151,12 +2151,1327 @@
       <t xml:space="preserve"> nothing to commit, working tree clean</t>
     </r>
   </si>
+  <si>
+    <t>Customer and Sales Class Creation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create the folder </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/door</t>
+    </r>
+  </si>
+  <si>
+    <t>mkdir -p js/door</t>
+  </si>
+  <si>
+    <r>
+      <t>ls js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> will display the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">door </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>directory</t>
+    </r>
+  </si>
+  <si>
+    <t>touch js/door/door.js</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/door/door.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> file</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ls js/door</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> will display </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>door.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> file</t>
+    </r>
+  </si>
+  <si>
+    <t>New DDL purchase Checklist</t>
+  </si>
+  <si>
+    <t>Version 1</t>
+  </si>
+  <si>
+    <t>Online Survey:</t>
+  </si>
+  <si>
+    <t>"Door InstaCheck"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Input fields / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=mandatory</t>
+    </r>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>Thai</t>
+  </si>
+  <si>
+    <t>Field Type</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Survey information</t>
+  </si>
+  <si>
+    <t>ข้อมูลสำหรับติดต่อ</t>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Customer Name:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ชื่อลูกค้า:</t>
+    </r>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>50 characters</t>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Customer Mobile Phone:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>เบอร์มือถือลูกค้า:</t>
+    </r>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>10 digits</t>
+  </si>
+  <si>
+    <t>Customer Address:</t>
+  </si>
+  <si>
+    <t>ที่อยู่ลูกค้า:</t>
+  </si>
+  <si>
+    <t>150 characters</t>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Sales Person Name/ID:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ชื่อ/รหัสพนักงานขาย:</t>
+    </r>
+  </si>
+  <si>
+    <t>Sale location:</t>
+  </si>
+  <si>
+    <t>ชื่อห้างร้าน, สาขา:</t>
+  </si>
+  <si>
+    <t>Model Selection</t>
+  </si>
+  <si>
+    <t>รุ่นของล็อคตามลักษณะการเปิดประตู</t>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Select Door Type:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>กรุณาเลือกวิธีการเปิดประตู:</t>
+    </r>
+  </si>
+  <si>
+    <t>Drop Down</t>
+  </si>
+  <si>
+    <t>A: Swing Door</t>
+  </si>
+  <si>
+    <t>ก. บานเปิดสวิง</t>
+  </si>
+  <si>
+    <t>B: Sliding Door</t>
+  </si>
+  <si>
+    <t>ข. บานเลื่อน</t>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Select  Model:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>กรุณาเลือกรุ่นล็อค:</t>
+    </r>
+  </si>
+  <si>
+    <t>LockName</t>
+  </si>
+  <si>
+    <t>List depends on selection A or B</t>
+  </si>
+  <si>
+    <t>"LockName"</t>
+  </si>
+  <si>
+    <t>"ชื่อรุ่น"</t>
+  </si>
+  <si>
+    <t>Door information</t>
+  </si>
+  <si>
+    <t>ข้อมูลเกี่ยวกับประตู</t>
+  </si>
+  <si>
+    <t>The door is:</t>
+  </si>
+  <si>
+    <t>การติดตั้งมือจับ/ล็อคที่ประตู:</t>
+  </si>
+  <si>
+    <t>A or B</t>
+  </si>
+  <si>
+    <t>A: Existing</t>
+  </si>
+  <si>
+    <t>ก. มีการติดตั้งมือจับหรือล็อคไว้แล้ว</t>
+  </si>
+  <si>
+    <t>B: New</t>
+  </si>
+  <si>
+    <t>ข. ประตูใหม่/ไม่เคยติดมือจับหรือล็อคใดๆ</t>
+  </si>
+  <si>
+    <t>Location:</t>
+  </si>
+  <si>
+    <t>สถานที่ติดตั้งประตู:</t>
+  </si>
+  <si>
+    <t>Checkbox</t>
+  </si>
+  <si>
+    <t>A or B-C</t>
+  </si>
+  <si>
+    <t>IF C is selected: Show Message 1</t>
+  </si>
+  <si>
+    <t>A: Indoor</t>
+  </si>
+  <si>
+    <t>ก. ภายในร่ม ห่างจากแดดและฝน</t>
+  </si>
+  <si>
+    <t>B: Outdoor; protected from water + strong sunlight</t>
+  </si>
+  <si>
+    <t>ข. ภายนอก; มีหลังคาป้องกันน้ำและแดดจัด</t>
+  </si>
+  <si>
+    <t>C: Outdoor; exposed to water + strong sunlight</t>
+  </si>
+  <si>
+    <t>ค. ภายนอก; โดนน้ำและแดดจัดโดยตรง</t>
+  </si>
+  <si>
+    <t>Material of Door:</t>
+  </si>
+  <si>
+    <t>วัสดุของประตู:</t>
+  </si>
+  <si>
+    <t>A or B-E</t>
+  </si>
+  <si>
+    <t>IF B, E, F or G is selected: Show Message 1</t>
+  </si>
+  <si>
+    <t>A: Wood</t>
+  </si>
+  <si>
+    <t>ก. ไม้</t>
+  </si>
+  <si>
+    <t>B: Glass</t>
+  </si>
+  <si>
+    <t>ข. กระจกเปลือย</t>
+  </si>
+  <si>
+    <t>C: Steel</t>
+  </si>
+  <si>
+    <t>ค. เหล็ก</t>
+  </si>
+  <si>
+    <t>D: Aluminium</t>
+  </si>
+  <si>
+    <t>ง. อะลูมิเนียม</t>
+  </si>
+  <si>
+    <t>E: PVC</t>
+  </si>
+  <si>
+    <t>จ. พลาสติก PVC</t>
+  </si>
+  <si>
+    <t>F: UPVC</t>
+  </si>
+  <si>
+    <t>ฉ. UPVC</t>
+  </si>
+  <si>
+    <t>G: WPC</t>
+  </si>
+  <si>
+    <t>ช. WPC</t>
+  </si>
+  <si>
+    <t>Thickness of Door</t>
+  </si>
+  <si>
+    <t>ความหนาประตู</t>
+  </si>
+  <si>
+    <t>IF B is selected: Show Message 2</t>
+  </si>
+  <si>
+    <t>The selected lock supports:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ล็อคที่เลือกสามารถใช้กับประตูที่มีความหนาตั้งแต่: </t>
+  </si>
+  <si>
+    <t>"display input from locklist"</t>
+  </si>
+  <si>
+    <t>"display input from locklis"</t>
+  </si>
+  <si>
+    <t>A: Confirm</t>
+  </si>
+  <si>
+    <t>ก. ยืนยันความหนาบานตรงกับที่กำหนดไว้</t>
+  </si>
+  <si>
+    <t>B: Decline</t>
+  </si>
+  <si>
+    <t>ข. ความหนาบานไม่ตรงกับที่กำหนดไว้</t>
+  </si>
+  <si>
+    <t>Door Leaf Details</t>
+  </si>
+  <si>
+    <t>รายละเอียดบานประตู</t>
+  </si>
+  <si>
+    <t>Type of leaf</t>
+  </si>
+  <si>
+    <t>ประเภทของบานประตู</t>
+  </si>
+  <si>
+    <t>A: Door leaf with Mullion</t>
+  </si>
+  <si>
+    <t>ก. ประตูมีลูกฟัก</t>
+  </si>
+  <si>
+    <t>"pic1" + "Pic2"</t>
+  </si>
+  <si>
+    <t>pics</t>
+  </si>
+  <si>
+    <t>B: Door leaf with Frame</t>
+  </si>
+  <si>
+    <t>ข. ประตูมีกรอบ/บานกระจก</t>
+  </si>
+  <si>
+    <t>"pic2" + "Pic3"</t>
+  </si>
+  <si>
+    <t>X = Not less than 130mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">กรอบบานต้องมีระยะติดตั้งไม่น้อยกว่า 130มม. </t>
+  </si>
+  <si>
+    <t>Door Frame Details</t>
+  </si>
+  <si>
+    <t>รายละเอียดวงกบ</t>
+  </si>
+  <si>
+    <t>Door Jamb</t>
+  </si>
+  <si>
+    <t>วงกบประตู</t>
+  </si>
+  <si>
+    <t>IF LockName = PP8100 + C is selected: Show Message 3</t>
+  </si>
+  <si>
+    <t>A: Flush Door</t>
+  </si>
+  <si>
+    <t>ก. วงกบแบบเรียบ</t>
+  </si>
+  <si>
+    <t>"Pic4"</t>
+  </si>
+  <si>
+    <t>B: Rebated Door</t>
+  </si>
+  <si>
+    <t>ข. วงกบแบบมีซับวงกบ</t>
+  </si>
+  <si>
+    <t>"Pic5"</t>
+  </si>
+  <si>
+    <t>C: Double Leaf Door</t>
+  </si>
+  <si>
+    <t>ค. ประตูบานคู่</t>
+  </si>
+  <si>
+    <t>"Pic6"</t>
+  </si>
+  <si>
+    <t>Caution:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Installer may need to cut or engrave where to install the striking plate at the door jam, in order to make the door lock working properly. </t>
+  </si>
+  <si>
+    <t>ข้อควรระวัง:</t>
+  </si>
+  <si>
+    <t>ช่างอาจมีการตัดหรือเซาะวงกบในตำแหน่งที่จะทำการติดตั้งตัวรับลิ้นล็อค เพื่อให้การทำงาน/การล็อคของอุปกรณ์ทำงานได้อย่างเหมาะสม และมีประสิทธิภาพ</t>
+  </si>
+  <si>
+    <t>Existing Door Retrofit</t>
+  </si>
+  <si>
+    <t>ประตูที่มีการติดตั้งมือจับหรือล็อคไว้แล้ว</t>
+  </si>
+  <si>
+    <t>Only Show IF 3.1 = Existing</t>
+  </si>
+  <si>
+    <t>Existing Door</t>
+  </si>
+  <si>
+    <t>A: Door with Lever Handle Set</t>
+  </si>
+  <si>
+    <t>ก. ประตูติดตั้งมือจับไว้แล้ว</t>
+  </si>
+  <si>
+    <t>"Pic7"</t>
+  </si>
+  <si>
+    <t>B: Door with Knob Lock Set</t>
+  </si>
+  <si>
+    <t>ข.ประตูติดตั้งลูกบิดทั่วไป</t>
+  </si>
+  <si>
+    <t>"Pic8"</t>
+  </si>
+  <si>
+    <t>C: Door with Grip Handle</t>
+  </si>
+  <si>
+    <t>ค.ประตูที่ติดตั้งมือจับ Grip handle</t>
+  </si>
+  <si>
+    <t>"Pic9"</t>
+  </si>
+  <si>
+    <t>Installer may need to fill old holes or previous drillings with silicon or wood filler.</t>
+  </si>
+  <si>
+    <t>สำหรับการติดตั้งแทนมือจับเดิมที่มีอยู่ก่อนแล้ว ช่างอาจมีการเก็บรูเจาะเดิมด้วยซิลิโคนหรือวัสดุที่ใช้อุดอื่นๆ</t>
+  </si>
+  <si>
+    <t>Sliding Door Details</t>
+  </si>
+  <si>
+    <t>ข้อมูลสำหรับล็อคประตูบานเลื่อน</t>
+  </si>
+  <si>
+    <t>Door Leaf</t>
+  </si>
+  <si>
+    <t>ประเภทบานประตู</t>
+  </si>
+  <si>
+    <t>A: Plain Leaf</t>
+  </si>
+  <si>
+    <t>ก. บานเต็ม หรือบานทึบ</t>
+  </si>
+  <si>
+    <t>"Pic10"</t>
+  </si>
+  <si>
+    <t>B: Wooden Leaf</t>
+  </si>
+  <si>
+    <t>ข. บานกระจกมีกรอบไม้</t>
+  </si>
+  <si>
+    <t>"Pic11"</t>
+  </si>
+  <si>
+    <t>X = Not less than 50mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">กรอบบานต้องมีระยะติดตั้งไม่น้อยกว่า 50มม. </t>
+  </si>
+  <si>
+    <t>C: Aluminium/Steel Leaf</t>
+  </si>
+  <si>
+    <t>ค. บานอะลูมิเนียม/บานเหล็ก</t>
+  </si>
+  <si>
+    <t>"Pic12"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step </t>
+  </si>
+  <si>
+    <t>Additional Details</t>
+  </si>
+  <si>
+    <t>ข้อมูลเพิ่มเติม</t>
+  </si>
+  <si>
+    <t>"Text Field"</t>
+  </si>
+  <si>
+    <t>250 characters</t>
+  </si>
+  <si>
+    <t>Confirmation</t>
+  </si>
+  <si>
+    <t>ขั้นตอนยืนยัน</t>
+  </si>
+  <si>
+    <t>Option</t>
+  </si>
+  <si>
+    <t>ตัวเลือก</t>
+  </si>
+  <si>
+    <t>Send Summary by Email:</t>
+  </si>
+  <si>
+    <t>ส่งข้อมูลที่กรอกยังอีเมลล์:</t>
+  </si>
+  <si>
+    <t>Email: "address1, address2, etc…"</t>
+  </si>
+  <si>
+    <t>อีเมล์: "address1, address2, etc…"</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Check Valid</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>ยืนยันข้อมูล</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>IF submit is clicked: Show Message 4</t>
+  </si>
+  <si>
+    <t>mkdir -p lib/lang/en/enum/door</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create the folder </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lib/lang/en/enum/door</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>HAFELE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> directory</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ls lib/lang/en/enum </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">will display the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">door </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>directory</t>
+    </r>
+  </si>
+  <si>
+    <t>touch lib/lang/en/enum/door/door-enum.js</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Createthe file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lib/lang/en/enum/door/door-enum.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ls lib/lang/en/enum/door </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">will display the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>door-enum.js</t>
+    </r>
+  </si>
+  <si>
+    <t>30-50mm</t>
+  </si>
+  <si>
+    <t>32-50mm</t>
+  </si>
+  <si>
+    <t>35-50mm</t>
+  </si>
+  <si>
+    <t>35-90mm</t>
+  </si>
+  <si>
+    <t>35-60mm</t>
+  </si>
+  <si>
+    <t>Door CLASS CREATION AND CREATION OF ASSOCIATED ENUMERATIONS (EN)</t>
+  </si>
+  <si>
+    <t>use strict';
+/* * The Door Enumeration Values (EN).
+ *  @author   Sanket Rajgarhia
+ *  @date 31/03/2022 (dd/mm/yyyy)
+ *  @version 1.0
+ *  @language: en
+ * */
+/*****************************************************************************/
+/* DOOR ENUMERATION (EN)                                                     */
+/*****************************************************************************/
+/* Door Material specification */
+const DOOR_MATERIAL = {
+    WOOD: "WOOD",
+    GLASS: "GLASS",
+    STEEL: "STEEL",
+    ALUMINIUM: "ALUMINIUM",
+    PVC: "PVC",
+    UPVC: "UPVC",
+    WPC: "WPC"
+};
+/* Door Condition Specification */
+const DOOR_CONDITION = {
+    INSTALLED: "EXISTING",
+    NEW: "NEW"
+}
+/* Door Installation Location */
+const DOOR_INSTALLATION_LOCATION = {
+    INDOOR: "INDOOR",
+    OUTDOOR_PROTECTED: "OUTDOOR PROTECTED (FROM WATER AND STRONG SUNLIGHT)",
+    OUTDOOR_EXPOSED: "OUTDOOR EXPOSED (TO WATER AND SUNLIGHT)"
+}
+/* Thickness of the door */
+const DOOR_THICKNESS_IN_MM = {
+    MM_30_TO_50: "30-50 MM",
+    MM_32_TO_50: "32-50 MM",
+    MM_35_TO_50: "35-50 MM",
+    MM_35_TO_60: "35-60 MM",
+    MM_35_TO_90: "35-90 MM"
+}
+/*****************************************************************************/
+/* FREEZE - TO EMULATE ENUMERATION                                           */
+/*****************************************************************************/
+// Prevent addition of properties to the json Object
+Object.freeze(DOOR_MATERIAL);
+Object.freeze(DOOR_CONDITION);
+Object.freeze(DOOR_INSTALLATION_LOCATION);
+Object.freeze(DOOR_THICKNESS_IN_MM);
+/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Declare the enumerated values for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>DOOR_MATERIAL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>DOOR_CONDITION</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>DOOR_INSTALLATION_LOCATION</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">DOOR_THICKNESS. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Language - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Declared the enumerated values for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>DOOR_MATERIAL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>DOOR_CONDITION</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>DOOR_INSTALLATION_LOCATION</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">DOOR_THICKNESS. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Language - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>en</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Door</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> class as per specification.</t>
+    </r>
+  </si>
+  <si>
+    <t>use strict';
+/* * The generic Door class.
+ *  @author Sanket Rajgarhia
+ *  @date   30/03/2022 (dd/mm/yyyy)
+ *  @version 1.0
+ * */
+/*****************************************************************************/
+/* DOOR CLASS IMPLEMENTATION                                                 */
+/*****************************************************************************/
+class Door {
+    /* *Constructor
+     * @param    {DOOR_MATERIAL} material                           Material of the door
+     * @param    {DOOR_CONDITION} condition                         Existing/New door
+     * @param    {DOOR_INSTALLATION_LOCATION} installationLocation  Door Installation location
+     * @param    {DOOR_THICKNESS} thickness                         Thickness of the door
+     * */
+    constructor(material, condition, installationLocation) {
+        this._material = material;
+        this._condition = condition;
+        this._installationLocation = installationLocation;
+        this._thickness = thickness;
+    }
+    /* Get the material of the door
+     * @return {DOOR_MATERIAL}  Material of the door
+     */
+    get material() {
+        return this._material;
+    }
+    /* Set the material of the door
+     * @param    {DOOR_MATERIAL} material   Material of the door
+     */
+    set material(material) {
+        this._material = material;
+    }
+    /* Get the condition of the door
+     * @return {DOOR_CONDITION}     Existing/New door
+     */
+    get condition() {
+        return this._condition;
+    }
+    /* Set the condition of the door
+     * @param    {DOOR_CONDITION} condition     Existing/New door
+     */
+    set condition(condition) {
+        this._condition = condition;
+    }
+    /* Get the installation location of the door
+     * @return {DOOR_INSTALLATION_LOCATION}     Door Installation location
+     */
+    get installationLocation() {
+        return this._installationLocation;
+    }
+    /* Set the installation location of the door
+     * @param    {DOOR_INSTALLATION_LOCATION}   Door Installation location
+     */
+    set installationLocation(installationLocation) {
+        this._installationLocation = installationLocation;
+    }
+    /* Get the thickness of the door
+     * @return {DOOR_THICKNESS}     Thickness of the door
+     */
+    get thickness() {
+        return this._thickness;
+    }
+    /* Set the thickness of the door
+     * @param    {DOOR_THICKNESS} thickness     Thickness of the door
+     */
+    set thickness(thickness) {
+        this._thickness = thickness;
+    }
+}
+/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Created the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Door</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> class as per specification.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>git status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - would display the following files.                                                                                                                                                                                                                                  new file:   .vscode/settings.json
+        modified:   docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+        new file:   js/door/door.js
+        new file:   lib/lang/en/enum/door/door-enum.js</t>
+    </r>
+  </si>
+  <si>
+    <t>git commit -m "Door Enumeration (EN) and Door class creaton."</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2250,8 +3565,67 @@
       <name val="Century Gothic"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF4472C4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2288,8 +3662,50 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF2CC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE2EFDA"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -2338,12 +3754,82 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2395,28 +3881,62 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2428,6 +3948,37 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2758,18 +4309,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -3002,7 +4553,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="238" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" ht="255" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
         <v>66</v>
       </c>
@@ -3041,7 +4592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB926B8F-5A7D-9B4E-BEE4-06FF437DD437}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -3054,18 +4605,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -3106,9 +4657,9 @@
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="22"/>
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="20"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
@@ -3116,11 +4667,11 @@
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
+      <c r="A9" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -3145,31 +4696,31 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="356" x14ac:dyDescent="0.2">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="B12" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="25" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="13" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="51" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="24"/>
+      <c r="A14" s="52"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="52"/>
     </row>
     <row r="15" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
@@ -3183,33 +4734,33 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="404" x14ac:dyDescent="0.2">
-      <c r="A16" s="25" t="s">
+      <c r="A16" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B16" s="26" t="s">
+    </row>
+    <row r="17" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="53" t="s">
         <v>93</v>
       </c>
-      <c r="C16" s="25" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="23" t="s">
+      <c r="C17" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="B17" s="27" t="s">
-        <v>94</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="18" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="24"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="24"/>
-    </row>
-    <row r="19" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A18" s="52"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="52"/>
+    </row>
+    <row r="19" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>66</v>
       </c>
@@ -3217,7 +4768,7 @@
         <v>65</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -3225,10 +4776,10 @@
         <v>67</v>
       </c>
       <c r="B20" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" s="18" t="s">
         <v>98</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -3246,4 +4797,1932 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFF4F95A-9EF6-1A4F-9376-E584C178A6F0}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="55" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="51" t="s">
+        <v>292</v>
+      </c>
+      <c r="B6" s="56" t="s">
+        <v>291</v>
+      </c>
+      <c r="C6" s="51" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="59"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="59"/>
+    </row>
+    <row r="8" spans="1:3" s="13" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="52"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="52"/>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="60" t="s">
+        <v>294</v>
+      </c>
+      <c r="B11" s="56" t="s">
+        <v>295</v>
+      </c>
+      <c r="C11" s="60" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="61"/>
+      <c r="B12" s="57"/>
+      <c r="C12" s="61"/>
+    </row>
+    <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="62"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="62"/>
+    </row>
+    <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="8">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C6:C8"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:C13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE113606-3FFA-8545-9BE3-5643B52A7CE9}">
+  <dimension ref="A1:H116"/>
+  <sheetViews>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="24"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="66" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="66"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="27"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27" t="s">
+        <v>111</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>115</v>
+      </c>
+      <c r="H8" s="27"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="28">
+        <v>1</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="24"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="24"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="24"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="D11" s="46" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="G11" s="44"/>
+      <c r="H11" s="24"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="24"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" s="40" t="s">
+        <v>125</v>
+      </c>
+      <c r="F12" s="40" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" s="44"/>
+      <c r="H12" s="24"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="24"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="47" t="s">
+        <v>127</v>
+      </c>
+      <c r="D13" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="E13" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="G13" s="44"/>
+      <c r="H13" s="24"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="24"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="D14" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>121</v>
+      </c>
+      <c r="F14" s="40" t="s">
+        <v>122</v>
+      </c>
+      <c r="G14" s="44"/>
+      <c r="H14" s="24"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="47" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" s="47" t="s">
+        <v>133</v>
+      </c>
+      <c r="E15" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="F15" s="47" t="s">
+        <v>129</v>
+      </c>
+      <c r="G15" s="44"/>
+      <c r="H15" s="24"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="24"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" s="28">
+        <v>2</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="24"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="24"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="24"/>
+      <c r="B19" s="24">
+        <v>2.1</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>137</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="F19" s="24"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="24"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="24"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="24"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="24"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="24"/>
+      <c r="B23" s="24">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="D23" s="30" t="s">
+        <v>144</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>145</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>146</v>
+      </c>
+      <c r="H23" s="24"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="24"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="24"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="24"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" s="28">
+        <v>3</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>150</v>
+      </c>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="24"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="24"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="24"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="24"/>
+      <c r="B28" s="24">
+        <v>3.1</v>
+      </c>
+      <c r="C28" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="D28" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="E28" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="F28" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="G28" s="44"/>
+      <c r="H28" s="24"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="24"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="40" t="s">
+        <v>154</v>
+      </c>
+      <c r="D29" s="40" t="s">
+        <v>155</v>
+      </c>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="24"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="24"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="40" t="s">
+        <v>156</v>
+      </c>
+      <c r="D30" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="E30" s="40"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="24"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="24"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="24"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="24"/>
+      <c r="B32" s="24">
+        <v>3.2</v>
+      </c>
+      <c r="C32" s="43" t="s">
+        <v>158</v>
+      </c>
+      <c r="D32" s="40" t="s">
+        <v>159</v>
+      </c>
+      <c r="E32" s="40" t="s">
+        <v>160</v>
+      </c>
+      <c r="F32" s="40" t="s">
+        <v>161</v>
+      </c>
+      <c r="G32" s="44" t="s">
+        <v>162</v>
+      </c>
+      <c r="H32" s="24"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="24"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="40" t="s">
+        <v>163</v>
+      </c>
+      <c r="D33" s="40" t="s">
+        <v>164</v>
+      </c>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="44"/>
+      <c r="H33" s="24"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="24"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="40" t="s">
+        <v>165</v>
+      </c>
+      <c r="D34" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="24"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="24"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="40" t="s">
+        <v>167</v>
+      </c>
+      <c r="D35" s="40" t="s">
+        <v>168</v>
+      </c>
+      <c r="E35" s="40"/>
+      <c r="F35" s="40"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="24"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="24"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="24"/>
+      <c r="E36" s="24"/>
+      <c r="F36" s="24"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="24"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="24"/>
+      <c r="B37" s="24">
+        <v>3.3</v>
+      </c>
+      <c r="C37" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="D37" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="E37" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="F37" s="40" t="s">
+        <v>171</v>
+      </c>
+      <c r="G37" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="H37" s="24"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="24"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="40" t="s">
+        <v>173</v>
+      </c>
+      <c r="D38" s="40" t="s">
+        <v>174</v>
+      </c>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="24"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="24"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="40" t="s">
+        <v>175</v>
+      </c>
+      <c r="D39" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="E39" s="40"/>
+      <c r="F39" s="40"/>
+      <c r="G39" s="44"/>
+      <c r="H39" s="24"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="24"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="40" t="s">
+        <v>177</v>
+      </c>
+      <c r="D40" s="40" t="s">
+        <v>178</v>
+      </c>
+      <c r="E40" s="40"/>
+      <c r="F40" s="40"/>
+      <c r="G40" s="44"/>
+      <c r="H40" s="24"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="24"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="40" t="s">
+        <v>179</v>
+      </c>
+      <c r="D41" s="40" t="s">
+        <v>180</v>
+      </c>
+      <c r="E41" s="40"/>
+      <c r="F41" s="40"/>
+      <c r="G41" s="44"/>
+      <c r="H41" s="24"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="24"/>
+      <c r="B42" s="24"/>
+      <c r="C42" s="40" t="s">
+        <v>181</v>
+      </c>
+      <c r="D42" s="40" t="s">
+        <v>182</v>
+      </c>
+      <c r="E42" s="40"/>
+      <c r="F42" s="40"/>
+      <c r="G42" s="44"/>
+      <c r="H42" s="24"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="24"/>
+      <c r="B43" s="24"/>
+      <c r="C43" s="40" t="s">
+        <v>183</v>
+      </c>
+      <c r="D43" s="40" t="s">
+        <v>184</v>
+      </c>
+      <c r="E43" s="40"/>
+      <c r="F43" s="40"/>
+      <c r="G43" s="44"/>
+      <c r="H43" s="24"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="24"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="D44" s="40" t="s">
+        <v>186</v>
+      </c>
+      <c r="E44" s="40"/>
+      <c r="F44" s="40"/>
+      <c r="G44" s="44"/>
+      <c r="H44" s="24"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="24"/>
+      <c r="B45" s="24"/>
+      <c r="C45" s="24"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="24"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="24"/>
+      <c r="B46" s="24">
+        <v>3.4</v>
+      </c>
+      <c r="C46" s="38" t="s">
+        <v>187</v>
+      </c>
+      <c r="D46" s="37" t="s">
+        <v>188</v>
+      </c>
+      <c r="E46" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="F46" s="37" t="s">
+        <v>153</v>
+      </c>
+      <c r="G46" s="39" t="s">
+        <v>189</v>
+      </c>
+      <c r="H46" s="24"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="24"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="D47" s="37" t="s">
+        <v>191</v>
+      </c>
+      <c r="E47" s="37"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="39"/>
+      <c r="H47" s="24"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="24"/>
+      <c r="B48" s="24"/>
+      <c r="C48" s="48" t="s">
+        <v>192</v>
+      </c>
+      <c r="D48" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="E48" s="37"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="39"/>
+      <c r="H48" s="24"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="24"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="37" t="s">
+        <v>194</v>
+      </c>
+      <c r="D49" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="E49" s="37"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="39"/>
+      <c r="H49" s="24"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="24"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="D50" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="E50" s="37"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="39"/>
+      <c r="H50" s="24"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="24"/>
+      <c r="B51" s="24"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
+      <c r="F51" s="24"/>
+      <c r="G51" s="26"/>
+      <c r="H51" s="24"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="24" t="s">
+        <v>116</v>
+      </c>
+      <c r="B52" s="28">
+        <v>4</v>
+      </c>
+      <c r="C52" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="D52" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="E52" s="24"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="26"/>
+      <c r="H52" s="24"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="24"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="24"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="24"/>
+      <c r="B54" s="24">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C54" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="D54" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="E54" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="F54" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="G54" s="26"/>
+      <c r="H54" s="24"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="24"/>
+      <c r="B55" s="24"/>
+      <c r="C55" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="D55" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="E55" s="24"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="26"/>
+      <c r="H55" s="24"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="24"/>
+      <c r="B56" s="24"/>
+      <c r="C56" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="D56" s="24"/>
+      <c r="E56" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="F56" s="24"/>
+      <c r="G56" s="26"/>
+      <c r="H56" s="24"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="24"/>
+      <c r="B57" s="24"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="24"/>
+      <c r="E57" s="24"/>
+      <c r="F57" s="24"/>
+      <c r="G57" s="26"/>
+      <c r="H57" s="24"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="24"/>
+      <c r="B58" s="24"/>
+      <c r="C58" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="D58" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="E58" s="24"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="24"/>
+      <c r="H58" s="24"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="24"/>
+      <c r="B59" s="24"/>
+      <c r="C59" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="D59" s="24"/>
+      <c r="E59" s="24" t="s">
+        <v>205</v>
+      </c>
+      <c r="F59" s="24"/>
+      <c r="G59" s="26"/>
+      <c r="H59" s="24"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="24"/>
+      <c r="B60" s="24"/>
+      <c r="C60" s="24"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="24"/>
+      <c r="F60" s="24"/>
+      <c r="G60" s="26"/>
+      <c r="H60" s="24"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="24"/>
+      <c r="B61" s="24"/>
+      <c r="C61" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="D61" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="E61" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="F61" s="24"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="24"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="24"/>
+      <c r="B62" s="24"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="24"/>
+      <c r="E62" s="24"/>
+      <c r="F62" s="24"/>
+      <c r="G62" s="26"/>
+      <c r="H62" s="24"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B63" s="28">
+        <v>5</v>
+      </c>
+      <c r="C63" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="D63" s="24" t="s">
+        <v>212</v>
+      </c>
+      <c r="E63" s="24"/>
+      <c r="F63" s="24"/>
+      <c r="G63" s="26"/>
+      <c r="H63" s="24"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="24"/>
+      <c r="B64" s="24"/>
+      <c r="C64" s="24"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="24"/>
+      <c r="F64" s="24"/>
+      <c r="G64" s="26"/>
+      <c r="H64" s="24"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="24"/>
+      <c r="B65" s="24">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C65" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="D65" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="E65" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="F65" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="G65" s="26" t="s">
+        <v>215</v>
+      </c>
+      <c r="H65" s="24"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="24"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="D66" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="E66" s="24"/>
+      <c r="F66" s="24"/>
+      <c r="G66" s="26"/>
+      <c r="H66" s="24"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="24"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="D67" s="24"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="26"/>
+      <c r="H67" s="24"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="24"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="24"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="24"/>
+      <c r="F68" s="24"/>
+      <c r="G68" s="26"/>
+      <c r="H68" s="24"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="24"/>
+      <c r="B69" s="24"/>
+      <c r="C69" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="D69" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="E69" s="24"/>
+      <c r="F69" s="24"/>
+      <c r="G69" s="26"/>
+      <c r="H69" s="24"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="24"/>
+      <c r="B70" s="24"/>
+      <c r="C70" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="D70" s="24"/>
+      <c r="E70" s="24"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="26"/>
+      <c r="H70" s="24"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="24"/>
+      <c r="B71" s="24"/>
+      <c r="C71" s="24"/>
+      <c r="D71" s="24"/>
+      <c r="E71" s="24"/>
+      <c r="F71" s="24"/>
+      <c r="G71" s="24"/>
+      <c r="H71" s="24"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="24"/>
+      <c r="B72" s="24"/>
+      <c r="C72" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="D72" s="24" t="s">
+        <v>223</v>
+      </c>
+      <c r="E72" s="24"/>
+      <c r="F72" s="24"/>
+      <c r="G72" s="26"/>
+      <c r="H72" s="24"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="24"/>
+      <c r="B73" s="24"/>
+      <c r="C73" s="24" t="s">
+        <v>224</v>
+      </c>
+      <c r="D73" s="24"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="24"/>
+      <c r="G73" s="26"/>
+      <c r="H73" s="24"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="63"/>
+      <c r="B74" s="67"/>
+      <c r="C74" s="33" t="s">
+        <v>225</v>
+      </c>
+      <c r="D74" s="33" t="s">
+        <v>227</v>
+      </c>
+      <c r="E74" s="68"/>
+      <c r="F74" s="63"/>
+      <c r="G74" s="65"/>
+      <c r="H74" s="63"/>
+    </row>
+    <row r="75" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+      <c r="A75" s="63"/>
+      <c r="B75" s="67"/>
+      <c r="C75" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="D75" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="E75" s="68"/>
+      <c r="F75" s="63"/>
+      <c r="G75" s="65"/>
+      <c r="H75" s="63"/>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="24"/>
+      <c r="B76" s="24"/>
+      <c r="C76" s="35"/>
+      <c r="D76" s="24"/>
+      <c r="E76" s="24"/>
+      <c r="F76" s="24"/>
+      <c r="G76" s="26"/>
+      <c r="H76" s="24"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B77" s="28">
+        <v>6</v>
+      </c>
+      <c r="C77" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="D77" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="E77" s="24"/>
+      <c r="F77" s="24"/>
+      <c r="G77" s="26" t="s">
+        <v>231</v>
+      </c>
+      <c r="H77" s="24"/>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="24"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="24"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="24"/>
+      <c r="G78" s="26"/>
+      <c r="H78" s="24"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="24"/>
+      <c r="B79" s="24">
+        <v>6.1</v>
+      </c>
+      <c r="C79" s="32" t="s">
+        <v>232</v>
+      </c>
+      <c r="D79" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="E79" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="F79" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="G79" s="26" t="s">
+        <v>162</v>
+      </c>
+      <c r="H79" s="24"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="24"/>
+      <c r="B80" s="24"/>
+      <c r="C80" s="24" t="s">
+        <v>233</v>
+      </c>
+      <c r="D80" s="24" t="s">
+        <v>234</v>
+      </c>
+      <c r="E80" s="24"/>
+      <c r="F80" s="24"/>
+      <c r="G80" s="26"/>
+      <c r="H80" s="24"/>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="24"/>
+      <c r="B81" s="24"/>
+      <c r="C81" s="31" t="s">
+        <v>235</v>
+      </c>
+      <c r="D81" s="24"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="26"/>
+      <c r="H81" s="24"/>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="24"/>
+      <c r="B82" s="24"/>
+      <c r="C82" s="24"/>
+      <c r="D82" s="24"/>
+      <c r="E82" s="24"/>
+      <c r="F82" s="24"/>
+      <c r="G82" s="24"/>
+      <c r="H82" s="24"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="24"/>
+      <c r="B83" s="24"/>
+      <c r="C83" s="24" t="s">
+        <v>236</v>
+      </c>
+      <c r="D83" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="E83" s="24"/>
+      <c r="F83" s="24"/>
+      <c r="G83" s="24"/>
+      <c r="H83" s="24"/>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="24"/>
+      <c r="B84" s="24"/>
+      <c r="C84" s="31" t="s">
+        <v>238</v>
+      </c>
+      <c r="D84" s="24"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="24"/>
+      <c r="G84" s="24"/>
+      <c r="H84" s="24"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="24"/>
+      <c r="B85" s="24"/>
+      <c r="C85" s="24"/>
+      <c r="D85" s="24"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="24"/>
+      <c r="G85" s="24"/>
+      <c r="H85" s="24"/>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="24"/>
+      <c r="B86" s="24"/>
+      <c r="C86" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="D86" s="24" t="s">
+        <v>240</v>
+      </c>
+      <c r="E86" s="24"/>
+      <c r="F86" s="24"/>
+      <c r="G86" s="24"/>
+      <c r="H86" s="24"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="24"/>
+      <c r="B87" s="24"/>
+      <c r="C87" s="31" t="s">
+        <v>241</v>
+      </c>
+      <c r="D87" s="24"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="24"/>
+      <c r="H87" s="24"/>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="24"/>
+      <c r="B88" s="24"/>
+      <c r="C88" s="24"/>
+      <c r="D88" s="24"/>
+      <c r="E88" s="24"/>
+      <c r="F88" s="24"/>
+      <c r="G88" s="24"/>
+      <c r="H88" s="24"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="63"/>
+      <c r="B89" s="63"/>
+      <c r="C89" s="36" t="s">
+        <v>225</v>
+      </c>
+      <c r="D89" s="36" t="s">
+        <v>227</v>
+      </c>
+      <c r="E89" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="F89" s="64"/>
+      <c r="G89" s="65"/>
+      <c r="H89" s="63"/>
+    </row>
+    <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A90" s="63"/>
+      <c r="B90" s="63"/>
+      <c r="C90" s="36" t="s">
+        <v>242</v>
+      </c>
+      <c r="D90" s="36" t="s">
+        <v>243</v>
+      </c>
+      <c r="E90" s="64"/>
+      <c r="F90" s="64"/>
+      <c r="G90" s="65"/>
+      <c r="H90" s="63"/>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="24"/>
+      <c r="B91" s="24"/>
+      <c r="C91" s="24"/>
+      <c r="D91" s="24"/>
+      <c r="E91" s="24"/>
+      <c r="F91" s="24"/>
+      <c r="G91" s="24"/>
+      <c r="H91" s="24"/>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B92" s="28">
+        <v>8</v>
+      </c>
+      <c r="C92" s="28" t="s">
+        <v>244</v>
+      </c>
+      <c r="D92" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="E92" s="24"/>
+      <c r="F92" s="24"/>
+      <c r="G92" s="24"/>
+      <c r="H92" s="24"/>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="24"/>
+      <c r="B93" s="24"/>
+      <c r="C93" s="24"/>
+      <c r="D93" s="24"/>
+      <c r="E93" s="24"/>
+      <c r="F93" s="24"/>
+      <c r="G93" s="24"/>
+      <c r="H93" s="24"/>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="24"/>
+      <c r="B94" s="24">
+        <v>8.1</v>
+      </c>
+      <c r="C94" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="D94" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="E94" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="F94" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="G94" s="24"/>
+      <c r="H94" s="24"/>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="24"/>
+      <c r="B95" s="24"/>
+      <c r="C95" s="24" t="s">
+        <v>248</v>
+      </c>
+      <c r="D95" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="E95" s="24"/>
+      <c r="F95" s="24"/>
+      <c r="G95" s="24"/>
+      <c r="H95" s="24"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="24"/>
+      <c r="B96" s="24"/>
+      <c r="C96" s="31" t="s">
+        <v>250</v>
+      </c>
+      <c r="D96" s="24"/>
+      <c r="E96" s="24"/>
+      <c r="F96" s="24"/>
+      <c r="G96" s="24"/>
+      <c r="H96" s="24"/>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="24"/>
+      <c r="B97" s="24"/>
+      <c r="C97" s="24"/>
+      <c r="D97" s="24"/>
+      <c r="E97" s="24"/>
+      <c r="F97" s="24"/>
+      <c r="G97" s="24"/>
+      <c r="H97" s="24"/>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="24"/>
+      <c r="B98" s="24"/>
+      <c r="C98" s="24" t="s">
+        <v>251</v>
+      </c>
+      <c r="D98" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="E98" s="24"/>
+      <c r="F98" s="24"/>
+      <c r="G98" s="24"/>
+      <c r="H98" s="24"/>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="24"/>
+      <c r="B99" s="24"/>
+      <c r="C99" s="31" t="s">
+        <v>253</v>
+      </c>
+      <c r="D99" s="24"/>
+      <c r="E99" s="24"/>
+      <c r="F99" s="24"/>
+      <c r="G99" s="24"/>
+      <c r="H99" s="24"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="24"/>
+      <c r="B100" s="24"/>
+      <c r="C100" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="D100" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="E100" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="F100" s="24"/>
+      <c r="G100" s="24"/>
+      <c r="H100" s="24"/>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="24"/>
+      <c r="B101" s="24"/>
+      <c r="C101" s="24"/>
+      <c r="D101" s="24"/>
+      <c r="E101" s="24"/>
+      <c r="F101" s="24"/>
+      <c r="G101" s="24"/>
+      <c r="H101" s="24"/>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="24"/>
+      <c r="B102" s="24"/>
+      <c r="C102" s="24" t="s">
+        <v>256</v>
+      </c>
+      <c r="D102" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="E102" s="24"/>
+      <c r="F102" s="24"/>
+      <c r="G102" s="24"/>
+      <c r="H102" s="24"/>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="24"/>
+      <c r="B103" s="24"/>
+      <c r="C103" s="31" t="s">
+        <v>258</v>
+      </c>
+      <c r="D103" s="24"/>
+      <c r="E103" s="24"/>
+      <c r="F103" s="24"/>
+      <c r="G103" s="24"/>
+      <c r="H103" s="24"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="24" t="s">
+        <v>259</v>
+      </c>
+      <c r="B104" s="24"/>
+      <c r="C104" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="D104" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="E104" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="F104" s="24"/>
+      <c r="G104" s="24"/>
+      <c r="H104" s="24"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="24"/>
+      <c r="B105" s="24"/>
+      <c r="C105" s="24"/>
+      <c r="D105" s="24"/>
+      <c r="E105" s="24"/>
+      <c r="F105" s="24"/>
+      <c r="G105" s="24"/>
+      <c r="H105" s="24"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="28" t="s">
+        <v>260</v>
+      </c>
+      <c r="B106" s="28">
+        <v>9</v>
+      </c>
+      <c r="C106" s="28" t="s">
+        <v>261</v>
+      </c>
+      <c r="D106" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="E106" s="24"/>
+      <c r="F106" s="24"/>
+      <c r="G106" s="24"/>
+      <c r="H106" s="24"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" s="24"/>
+      <c r="B107" s="24">
+        <v>9.1</v>
+      </c>
+      <c r="C107" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="D107" s="24"/>
+      <c r="E107" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="F107" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="G107" s="24"/>
+      <c r="H107" s="24"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" s="24"/>
+      <c r="B108" s="24"/>
+      <c r="C108" s="24"/>
+      <c r="D108" s="24"/>
+      <c r="E108" s="24"/>
+      <c r="F108" s="24"/>
+      <c r="G108" s="24"/>
+      <c r="H108" s="24"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" s="24"/>
+      <c r="B109" s="24"/>
+      <c r="C109" s="24"/>
+      <c r="D109" s="24"/>
+      <c r="E109" s="24"/>
+      <c r="F109" s="24"/>
+      <c r="G109" s="24"/>
+      <c r="H109" s="24"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="B110" s="28">
+        <v>10</v>
+      </c>
+      <c r="C110" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="D110" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="E110" s="24"/>
+      <c r="F110" s="24"/>
+      <c r="G110" s="24"/>
+      <c r="H110" s="24"/>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" s="24"/>
+      <c r="B111" s="24">
+        <v>10.1</v>
+      </c>
+      <c r="C111" s="32" t="s">
+        <v>267</v>
+      </c>
+      <c r="D111" s="24" t="s">
+        <v>268</v>
+      </c>
+      <c r="E111" s="24"/>
+      <c r="F111" s="24"/>
+      <c r="G111" s="24"/>
+      <c r="H111" s="24"/>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" s="24"/>
+      <c r="B112" s="24"/>
+      <c r="C112" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="D112" s="24" t="s">
+        <v>270</v>
+      </c>
+      <c r="E112" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="F112" s="24"/>
+      <c r="G112" s="24"/>
+      <c r="H112" s="24"/>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A113" s="24"/>
+      <c r="B113" s="24"/>
+      <c r="C113" s="24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D113" s="24" t="s">
+        <v>272</v>
+      </c>
+      <c r="E113" s="24" t="s">
+        <v>273</v>
+      </c>
+      <c r="F113" s="24" t="s">
+        <v>274</v>
+      </c>
+      <c r="G113" s="24"/>
+      <c r="H113" s="24"/>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A114" s="24"/>
+      <c r="B114" s="24"/>
+      <c r="C114" s="24"/>
+      <c r="D114" s="24"/>
+      <c r="E114" s="24"/>
+      <c r="F114" s="24"/>
+      <c r="G114" s="24"/>
+      <c r="H114" s="24"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A115" s="24"/>
+      <c r="B115" s="24">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="C115" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="D115" s="24" t="s">
+        <v>276</v>
+      </c>
+      <c r="E115" s="24" t="s">
+        <v>277</v>
+      </c>
+      <c r="F115" s="24"/>
+      <c r="G115" s="24" t="s">
+        <v>278</v>
+      </c>
+      <c r="H115" s="24"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A116" s="24"/>
+      <c r="B116" s="24"/>
+      <c r="C116" s="24"/>
+      <c r="D116" s="24"/>
+      <c r="E116" s="24"/>
+      <c r="F116" s="24"/>
+      <c r="G116" s="24"/>
+      <c r="H116" s="24"/>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="H74:H75"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="E89:E90"/>
+    <mergeCell ref="F89:F90"/>
+    <mergeCell ref="G89:G90"/>
+    <mergeCell ref="H89:H90"/>
+    <mergeCell ref="G74:G75"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="37" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="37" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="37" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="37" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="40" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="41" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="41" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="41" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="41" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="41" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="41" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="41" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="42" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="42" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="42" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="24" t="s">
+        <v>288</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A16">
+    <sortCondition ref="A1:A16"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactored Customer and Sales class - use strict directive and sectional comments introduced.
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA851E79-2EB4-BC4D-8ADF-6C6E74EBC8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C200126C-AD13-AB41-981F-F4FD9ED18CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="1000" windowWidth="27640" windowHeight="16160" activeTab="2" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
+    <workbookView xWindow="300" yWindow="1000" windowWidth="27640" windowHeight="16160" activeTab="3" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="SPEC - 1.1" sheetId="1" r:id="rId1"/>
     <sheet name="SPEC - 1.2" sheetId="2" r:id="rId2"/>
     <sheet name="SPEC - 1.3" sheetId="4" r:id="rId3"/>
-    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId4"/>
-    <sheet name="PLAYGROUND" sheetId="6" r:id="rId5"/>
+    <sheet name="SPEC - 1.4" sheetId="7" r:id="rId4"/>
+    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId5"/>
+    <sheet name="PLAYGROUND" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="308">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -3466,12 +3467,477 @@
   <si>
     <t>git commit -m "Door Enumeration (EN) and Door class creaton."</t>
   </si>
+  <si>
+    <t>REFACTOR THE Customer CLASS AND Sales CLASS</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>'use strict';</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> directive to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Customer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> class. Additionally add the sectional comments.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Added the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>'use strict';</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> directive to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Customer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> class. Additionally added the sectional comments.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>'use strict';</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> directive to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Sales</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> class. Additionally add the sectional comments.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">use strict';
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">/* * The Sales class.
+ *  @author Sanket Rajgarhia
+ *  @date   30/03/2022 (dd/mm/yyyy)
+ *  @version 1.0
+ * */
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+/*****************************************************************************/
+/* SALES CLASS IMPLEMENTATION                                                */
+/*****************************************************************************/
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+class Sales {
+    /* *Constructor
+     * @param    {String} salesPersonId     ID of the sales person
+     * @param    {String} salesPersonName   Name of the sales person
+     * @param    {String} salesLocation     150 characters sales location/address
+     * */
+    constructor(salesPersonId, salesPersonName, salesLocation) {
+        this._salesPersonId = salesPersonId;
+        this._salesPersonName = salesPersonName;
+        this._salesLocation = salesLocation;
+    }
+    /* Get the ID of the sales person
+     * @return  {String}    ID of the sales person
+     */
+    get salesPersonId() {
+        return this._salesPersonId;
+    }
+    /* Set the ID of the sales person
+     * @param  {String} salesPersonId   ID of the sales person
+     */
+    set salesPersonId(salesPersonId) {
+        this._salesPersonId = salesPersonId;
+    }
+    /* Get the name of the sales person
+     * @return  {String}    Name of the sales person
+     */
+    get salesPersonName() {
+        return this._salesPersonName;
+    }
+    /* Set the name of the sales person
+     * @param    {String} salesPersonName   Name of the sales person
+     */
+    set salesPersonName(salesPersonName) {
+        this.salesPersonName = salesPersonName;
+    }
+    /* Get the location of the sale
+     * @return  {String}    150 characters sales location/address
+     */
+    get salesLocation() {
+        return this._salesLocation;
+    }
+    /* Set the location of the sale
+     * @param    {String} salesLocation     150 characters sales location/address
+     */
+    set salesLocation(salesLocation) {
+        this._salesLocation = salesLocation;
+    }
+}
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Added the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>'use strict';</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> directive to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Sales</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> class. Additionally added the sectional comments.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>use strict';</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">/* * The Customer class.
+ *  @author Sanket Rajgarhia
+ *  @date   30/03/2022 (dd/mm/yyyy)
+ *  @version 1.0
+ * */
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">/*****************************************************************************/
+/* CUSTOMER CLASS IMPLEMENTATION                                             */
+/*****************************************************************************/
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">class Customer {
+    /* *Constructor
+     * @param    {String} customerName    Name of the customer
+     * @param    {String} phoneNumber    10 Digit Phone Number of the customer
+     * @param    {String} address        150 characters address
+     * */
+    constructor(customerName, phoneNumber, address) {
+        this._customerName = customerName;
+        this._phoneNumber = phoneNumber;
+        this._address = address;
+    }
+    /* Get the customer name
+     * @return {String} Customer name
+     */
+    get customerName() {
+        return this._customerName;
+    }
+    /* Set the customer name
+     * @param   {String} customerName  Name of the customer
+     */
+    set customerName(customerName) {
+        this._customerName = customerName;
+    }
+    /* Get the customer phone number
+     * @return  {String} Customer phone number
+     */
+    get phoneNumber() {
+        return this._phoneNumber;
+    }
+    /* Set the phone number
+     * @param   {String} phoneNumber    10 Digit Phone Number of the customer
+     */
+    set phoneNumber(phoneNumber) {
+        this._phoneNumber = phoneNumber;
+    }
+    /* Get the customer address
+     * @return  {String} Customer address
+     */
+    get address() {
+        return this._address;
+    }
+    /* Set the address
+     * @param   {String} address   150 characters address
+     */
+    set address(address) {
+        this._address = address;
+    }
+}
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>git status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - would display the following files.                                                                                                                                                                                                                                          modified:   docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+        modified:   js/customer.js
+        modified:   js/sales.js</t>
+    </r>
+  </si>
+  <si>
+    <t>git commit -m "Refactored Customer and Sales class - use strict directive and sectional comments introduced."</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3623,6 +4089,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF002060"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="14">
@@ -3829,7 +4307,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3890,9 +4368,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3927,6 +4402,21 @@
     <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3939,25 +4429,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3969,6 +4456,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -3979,6 +4484,9 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4309,18 +4817,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -4337,7 +4845,7 @@
       <c r="A4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="48" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -4348,7 +4856,7 @@
       <c r="A5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="48" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -4359,7 +4867,7 @@
       <c r="A6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="48" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -4370,7 +4878,7 @@
       <c r="A7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="48" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="5" t="s">
@@ -4381,7 +4889,7 @@
       <c r="A8" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="48" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -4392,7 +4900,7 @@
       <c r="A9" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="49" t="s">
         <v>48</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -4403,7 +4911,7 @@
       <c r="A10" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="49" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -4414,7 +4922,7 @@
       <c r="A11" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="49" t="s">
         <v>54</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -4425,7 +4933,7 @@
       <c r="A12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="49" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -4436,7 +4944,7 @@
       <c r="A13" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="49" t="s">
         <v>58</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -4447,7 +4955,7 @@
       <c r="A14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="49" t="s">
         <v>14</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -4458,7 +4966,7 @@
       <c r="A15" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="49" t="s">
         <v>61</v>
       </c>
       <c r="C15" s="15" t="s">
@@ -4469,7 +4977,7 @@
       <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="49" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="10" t="s">
@@ -4480,7 +4988,7 @@
       <c r="A17" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="49" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="10" t="s">
@@ -4535,7 +5043,7 @@
       <c r="A22" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="50" t="s">
         <v>46</v>
       </c>
       <c r="C22" s="12" t="s">
@@ -4546,7 +5054,7 @@
       <c r="A23" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="51" t="s">
         <v>52</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -4605,18 +5113,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -4633,7 +5141,7 @@
       <c r="A4" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="48" t="s">
         <v>73</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -4644,7 +5152,7 @@
       <c r="A5" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="48" t="s">
         <v>74</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -4667,11 +5175,11 @@
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="55" t="s">
+      <c r="A9" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="55"/>
-      <c r="C9" s="55"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="59"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -4688,18 +5196,18 @@
       <c r="A11" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="48" t="s">
         <v>76</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="356" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="293" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="52" t="s">
         <v>79</v>
       </c>
       <c r="C12" s="21" t="s">
@@ -4707,37 +5215,37 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="51" t="s">
+      <c r="A13" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="53" t="s">
+      <c r="B13" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="55" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="52"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="52"/>
+      <c r="A14" s="56"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="56"/>
     </row>
     <row r="15" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="49" t="s">
         <v>82</v>
       </c>
       <c r="C15" s="15" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="404" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="306" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="52" t="s">
         <v>92</v>
       </c>
       <c r="C16" s="21" t="s">
@@ -4745,20 +5253,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="55" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="53" t="s">
+      <c r="B17" s="57" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="55" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="52"/>
-      <c r="B18" s="54"/>
-      <c r="C18" s="52"/>
+      <c r="A18" s="56"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="56"/>
     </row>
     <row r="19" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -4803,6 +5311,171 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFF4F95A-9EF6-1A4F-9376-E584C178A6F0}">
   <dimension ref="A1:C15"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="59" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>279</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>282</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="55" t="s">
+        <v>292</v>
+      </c>
+      <c r="B6" s="60" t="s">
+        <v>291</v>
+      </c>
+      <c r="C6" s="55" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="66"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="66"/>
+    </row>
+    <row r="8" spans="1:3" s="13" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="56"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="56"/>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="63" t="s">
+        <v>294</v>
+      </c>
+      <c r="B11" s="60" t="s">
+        <v>295</v>
+      </c>
+      <c r="C11" s="63" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="64"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="64"/>
+    </row>
+    <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="65"/>
+      <c r="B13" s="62"/>
+      <c r="C13" s="65"/>
+    </row>
+    <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="8">
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="C6:C8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5ECDD1-7F28-8F45-BB61-7AD00F9ECBDC}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
@@ -4816,18 +5489,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="55" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
+      <c r="A2" s="59" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -4840,131 +5513,87 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>283</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="51" t="s">
-        <v>292</v>
-      </c>
-      <c r="B6" s="56" t="s">
-        <v>291</v>
-      </c>
-      <c r="C6" s="51" t="s">
-        <v>293</v>
-      </c>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="67" t="s">
+        <v>300</v>
+      </c>
+      <c r="B4" s="71" t="s">
+        <v>305</v>
+      </c>
+      <c r="C4" s="67" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="67"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="67"/>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="67"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="67"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="59"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="59"/>
-    </row>
-    <row r="8" spans="1:3" s="13" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="52"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="52"/>
-    </row>
-    <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="60" t="s">
-        <v>294</v>
-      </c>
-      <c r="B11" s="56" t="s">
-        <v>295</v>
-      </c>
-      <c r="C11" s="60" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="61"/>
-      <c r="B12" s="57"/>
-      <c r="C12" s="61"/>
-    </row>
-    <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="62"/>
-      <c r="B13" s="58"/>
-      <c r="C13" s="62"/>
-    </row>
-    <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
+      <c r="A7" s="55" t="s">
+        <v>302</v>
+      </c>
+      <c r="B7" s="68" t="s">
+        <v>303</v>
+      </c>
+      <c r="C7" s="55" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="66"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="66"/>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" ht="228" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="56"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="56"/>
+    </row>
+    <row r="10" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A10" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B10" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
+      <c r="C10" s="17" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="18" t="s">
-        <v>298</v>
-      </c>
-      <c r="C15" s="18" t="s">
+      <c r="B11" s="78" t="s">
+        <v>307</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>98</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="8">
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="C7:C9"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A4:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE113606-3FFA-8545-9BE3-5643B52A7CE9}">
   <dimension ref="A1:H116"/>
   <sheetViews>
@@ -4984,1630 +5613,1630 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="75" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="24"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27" t="s">
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="H8" s="27"/>
+      <c r="H8" s="26"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="B9" s="28">
+      <c r="B9" s="27">
         <v>1</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="24"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="24"/>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="24"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="23"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="45" t="s">
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="D11" s="46" t="s">
+      <c r="D11" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="G11" s="44"/>
-      <c r="H11" s="24"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="23"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
-      <c r="B12" s="24"/>
-      <c r="C12" s="45" t="s">
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="E12" s="40" t="s">
+      <c r="E12" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="G12" s="44"/>
-      <c r="H12" s="24"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="23"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="24"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="47" t="s">
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="D13" s="47" t="s">
+      <c r="D13" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="E13" s="47" t="s">
+      <c r="E13" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="F13" s="47" t="s">
+      <c r="F13" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="G13" s="44"/>
-      <c r="H13" s="24"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="23"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="24"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="45" t="s">
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="D14" s="46" t="s">
+      <c r="D14" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="F14" s="40" t="s">
+      <c r="F14" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="G14" s="44"/>
-      <c r="H14" s="24"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="23"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="47" t="s">
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="D15" s="47" t="s">
+      <c r="D15" s="46" t="s">
         <v>133</v>
       </c>
-      <c r="E15" s="47" t="s">
+      <c r="E15" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="F15" s="47" t="s">
+      <c r="F15" s="46" t="s">
         <v>129</v>
       </c>
-      <c r="G15" s="44"/>
-      <c r="H15" s="24"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="23"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="24"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="23"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="B17" s="28">
+      <c r="B17" s="27">
         <v>2</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="D17" s="23" t="s">
         <v>135</v>
       </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="24"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="23"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="24"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="24"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="23"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24">
+      <c r="A19" s="23"/>
+      <c r="B19" s="23">
         <v>2.1</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="F19" s="24"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="24"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="23"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="24"/>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24" t="s">
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="D20" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="24"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="23"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="24"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="24" t="s">
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="D21" s="24" t="s">
+      <c r="D21" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="24"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="23"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="24"/>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="24"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="23"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="24"/>
-      <c r="B23" s="24">
+      <c r="A23" s="23"/>
+      <c r="B23" s="23">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="29" t="s">
         <v>144</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="23" t="s">
         <v>138</v>
       </c>
-      <c r="F23" s="24" t="s">
+      <c r="F23" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="G23" s="26" t="s">
+      <c r="G23" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="H23" s="24"/>
+      <c r="H23" s="23"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="24"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="31" t="s">
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="30" t="s">
         <v>147</v>
       </c>
-      <c r="D24" s="24" t="s">
+      <c r="D24" s="23" t="s">
         <v>148</v>
       </c>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="24"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="23"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="24"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="24"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="23"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="28" t="s">
+      <c r="A26" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="B26" s="28">
+      <c r="B26" s="27">
         <v>3</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="D26" s="24" t="s">
+      <c r="D26" s="23" t="s">
         <v>150</v>
       </c>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="24"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="25"/>
+      <c r="H26" s="23"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="24"/>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="24"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="23"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="24"/>
-      <c r="B28" s="24">
+      <c r="A28" s="23"/>
+      <c r="B28" s="23">
         <v>3.1</v>
       </c>
-      <c r="C28" s="43" t="s">
+      <c r="C28" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="D28" s="40" t="s">
+      <c r="D28" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="E28" s="40" t="s">
+      <c r="E28" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="F28" s="40" t="s">
+      <c r="F28" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="G28" s="44"/>
-      <c r="H28" s="24"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="23"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="24"/>
-      <c r="B29" s="24"/>
-      <c r="C29" s="40" t="s">
+      <c r="A29" s="23"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="D29" s="40" t="s">
+      <c r="D29" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="24"/>
+      <c r="E29" s="39"/>
+      <c r="F29" s="39"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="23"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="24"/>
-      <c r="B30" s="24"/>
-      <c r="C30" s="40" t="s">
+      <c r="A30" s="23"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="D30" s="40" t="s">
+      <c r="D30" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="E30" s="40"/>
-      <c r="F30" s="40"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="24"/>
+      <c r="E30" s="39"/>
+      <c r="F30" s="39"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="23"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="24"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="24"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="25"/>
+      <c r="H31" s="23"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="24"/>
-      <c r="B32" s="24">
+      <c r="A32" s="23"/>
+      <c r="B32" s="23">
         <v>3.2</v>
       </c>
-      <c r="C32" s="43" t="s">
+      <c r="C32" s="42" t="s">
         <v>158</v>
       </c>
-      <c r="D32" s="40" t="s">
+      <c r="D32" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="E32" s="40" t="s">
+      <c r="E32" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="F32" s="40" t="s">
+      <c r="F32" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="G32" s="44" t="s">
+      <c r="G32" s="43" t="s">
         <v>162</v>
       </c>
-      <c r="H32" s="24"/>
+      <c r="H32" s="23"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="24"/>
-      <c r="B33" s="24"/>
-      <c r="C33" s="40" t="s">
+      <c r="A33" s="23"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="D33" s="40" t="s">
+      <c r="D33" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="44"/>
-      <c r="H33" s="24"/>
+      <c r="E33" s="39"/>
+      <c r="F33" s="39"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="23"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="24"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="40" t="s">
+      <c r="A34" s="23"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="D34" s="40" t="s">
+      <c r="D34" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="44"/>
-      <c r="H34" s="24"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="43"/>
+      <c r="H34" s="23"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="24"/>
-      <c r="B35" s="24"/>
-      <c r="C35" s="40" t="s">
+      <c r="A35" s="23"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="D35" s="40" t="s">
+      <c r="D35" s="39" t="s">
         <v>168</v>
       </c>
-      <c r="E35" s="40"/>
-      <c r="F35" s="40"/>
-      <c r="G35" s="44"/>
-      <c r="H35" s="24"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="23"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="24"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="24"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="26"/>
-      <c r="H36" s="24"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="23"/>
+      <c r="E36" s="23"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="25"/>
+      <c r="H36" s="23"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="24"/>
-      <c r="B37" s="24">
+      <c r="A37" s="23"/>
+      <c r="B37" s="23">
         <v>3.3</v>
       </c>
-      <c r="C37" s="43" t="s">
+      <c r="C37" s="42" t="s">
         <v>169</v>
       </c>
-      <c r="D37" s="40" t="s">
+      <c r="D37" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="E37" s="40" t="s">
+      <c r="E37" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="F37" s="40" t="s">
+      <c r="F37" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="G37" s="44" t="s">
+      <c r="G37" s="43" t="s">
         <v>172</v>
       </c>
-      <c r="H37" s="24"/>
+      <c r="H37" s="23"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="24"/>
-      <c r="B38" s="24"/>
-      <c r="C38" s="40" t="s">
+      <c r="A38" s="23"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="D38" s="40" t="s">
+      <c r="D38" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="E38" s="40"/>
-      <c r="F38" s="40"/>
-      <c r="G38" s="44"/>
-      <c r="H38" s="24"/>
+      <c r="E38" s="39"/>
+      <c r="F38" s="39"/>
+      <c r="G38" s="43"/>
+      <c r="H38" s="23"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="24"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="40" t="s">
+      <c r="A39" s="23"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="D39" s="40" t="s">
+      <c r="D39" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="E39" s="40"/>
-      <c r="F39" s="40"/>
-      <c r="G39" s="44"/>
-      <c r="H39" s="24"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="23"/>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="24"/>
-      <c r="B40" s="24"/>
-      <c r="C40" s="40" t="s">
+      <c r="A40" s="23"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="D40" s="40" t="s">
+      <c r="D40" s="39" t="s">
         <v>178</v>
       </c>
-      <c r="E40" s="40"/>
-      <c r="F40" s="40"/>
-      <c r="G40" s="44"/>
-      <c r="H40" s="24"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="23"/>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="24"/>
-      <c r="B41" s="24"/>
-      <c r="C41" s="40" t="s">
+      <c r="A41" s="23"/>
+      <c r="B41" s="23"/>
+      <c r="C41" s="39" t="s">
         <v>179</v>
       </c>
-      <c r="D41" s="40" t="s">
+      <c r="D41" s="39" t="s">
         <v>180</v>
       </c>
-      <c r="E41" s="40"/>
-      <c r="F41" s="40"/>
-      <c r="G41" s="44"/>
-      <c r="H41" s="24"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="23"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="24"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="40" t="s">
+      <c r="A42" s="23"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="D42" s="40" t="s">
+      <c r="D42" s="39" t="s">
         <v>182</v>
       </c>
-      <c r="E42" s="40"/>
-      <c r="F42" s="40"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="24"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="23"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="24"/>
-      <c r="B43" s="24"/>
-      <c r="C43" s="40" t="s">
+      <c r="A43" s="23"/>
+      <c r="B43" s="23"/>
+      <c r="C43" s="39" t="s">
         <v>183</v>
       </c>
-      <c r="D43" s="40" t="s">
+      <c r="D43" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="E43" s="40"/>
-      <c r="F43" s="40"/>
-      <c r="G43" s="44"/>
-      <c r="H43" s="24"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="23"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="24"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="40" t="s">
+      <c r="A44" s="23"/>
+      <c r="B44" s="23"/>
+      <c r="C44" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="D44" s="40" t="s">
+      <c r="D44" s="39" t="s">
         <v>186</v>
       </c>
-      <c r="E44" s="40"/>
-      <c r="F44" s="40"/>
-      <c r="G44" s="44"/>
-      <c r="H44" s="24"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="23"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="24"/>
-      <c r="B45" s="24"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="26"/>
-      <c r="H45" s="24"/>
+      <c r="A45" s="23"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="23"/>
+      <c r="F45" s="23"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="23"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="24"/>
-      <c r="B46" s="24">
+      <c r="A46" s="23"/>
+      <c r="B46" s="23">
         <v>3.4</v>
       </c>
-      <c r="C46" s="38" t="s">
+      <c r="C46" s="37" t="s">
         <v>187</v>
       </c>
-      <c r="D46" s="37" t="s">
+      <c r="D46" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="E46" s="37" t="s">
+      <c r="E46" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="F46" s="37" t="s">
+      <c r="F46" s="36" t="s">
         <v>153</v>
       </c>
-      <c r="G46" s="39" t="s">
+      <c r="G46" s="38" t="s">
         <v>189</v>
       </c>
-      <c r="H46" s="24"/>
+      <c r="H46" s="23"/>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="24"/>
-      <c r="B47" s="24"/>
-      <c r="C47" s="37" t="s">
+      <c r="A47" s="23"/>
+      <c r="B47" s="23"/>
+      <c r="C47" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="D47" s="37" t="s">
+      <c r="D47" s="36" t="s">
         <v>191</v>
       </c>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="39"/>
-      <c r="H47" s="24"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="38"/>
+      <c r="H47" s="23"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="24"/>
-      <c r="B48" s="24"/>
-      <c r="C48" s="48" t="s">
+      <c r="A48" s="23"/>
+      <c r="B48" s="23"/>
+      <c r="C48" s="47" t="s">
         <v>192</v>
       </c>
-      <c r="D48" s="37" t="s">
+      <c r="D48" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="E48" s="37"/>
-      <c r="F48" s="37"/>
-      <c r="G48" s="39"/>
-      <c r="H48" s="24"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="38"/>
+      <c r="H48" s="23"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="24"/>
-      <c r="B49" s="24"/>
-      <c r="C49" s="37" t="s">
+      <c r="A49" s="23"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="D49" s="37" t="s">
+      <c r="D49" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="E49" s="37"/>
-      <c r="F49" s="37"/>
-      <c r="G49" s="39"/>
-      <c r="H49" s="24"/>
+      <c r="E49" s="36"/>
+      <c r="F49" s="36"/>
+      <c r="G49" s="38"/>
+      <c r="H49" s="23"/>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="24"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="37" t="s">
+      <c r="A50" s="23"/>
+      <c r="B50" s="23"/>
+      <c r="C50" s="36" t="s">
         <v>196</v>
       </c>
-      <c r="D50" s="37" t="s">
+      <c r="D50" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="39"/>
-      <c r="H50" s="24"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="36"/>
+      <c r="G50" s="38"/>
+      <c r="H50" s="23"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="24"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="26"/>
-      <c r="H51" s="24"/>
+      <c r="A51" s="23"/>
+      <c r="B51" s="23"/>
+      <c r="C51" s="23"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="23"/>
+      <c r="F51" s="23"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="23"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="24" t="s">
+      <c r="A52" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="B52" s="28">
+      <c r="B52" s="27">
         <v>4</v>
       </c>
-      <c r="C52" s="28" t="s">
+      <c r="C52" s="27" t="s">
         <v>198</v>
       </c>
-      <c r="D52" s="24" t="s">
+      <c r="D52" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="26"/>
-      <c r="H52" s="24"/>
+      <c r="E52" s="23"/>
+      <c r="F52" s="23"/>
+      <c r="G52" s="25"/>
+      <c r="H52" s="23"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="24"/>
-      <c r="B53" s="28"/>
-      <c r="C53" s="28"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
-      <c r="F53" s="24"/>
-      <c r="G53" s="26"/>
-      <c r="H53" s="24"/>
+      <c r="A53" s="23"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="23"/>
+      <c r="E53" s="23"/>
+      <c r="F53" s="23"/>
+      <c r="G53" s="25"/>
+      <c r="H53" s="23"/>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="24"/>
-      <c r="B54" s="24">
+      <c r="A54" s="23"/>
+      <c r="B54" s="23">
         <v>4.0999999999999996</v>
       </c>
-      <c r="C54" s="32" t="s">
+      <c r="C54" s="31" t="s">
         <v>200</v>
       </c>
-      <c r="D54" s="24" t="s">
+      <c r="D54" s="23" t="s">
         <v>201</v>
       </c>
-      <c r="E54" s="24" t="s">
+      <c r="E54" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="F54" s="24" t="s">
+      <c r="F54" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="G54" s="26"/>
-      <c r="H54" s="24"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="23"/>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="24"/>
-      <c r="B55" s="24"/>
-      <c r="C55" s="24" t="s">
+      <c r="A55" s="23"/>
+      <c r="B55" s="23"/>
+      <c r="C55" s="23" t="s">
         <v>202</v>
       </c>
-      <c r="D55" s="24" t="s">
+      <c r="D55" s="23" t="s">
         <v>203</v>
       </c>
-      <c r="E55" s="24"/>
-      <c r="F55" s="24"/>
-      <c r="G55" s="26"/>
-      <c r="H55" s="24"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="23"/>
+      <c r="G55" s="25"/>
+      <c r="H55" s="23"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="24"/>
-      <c r="B56" s="24"/>
-      <c r="C56" s="24" t="s">
+      <c r="A56" s="23"/>
+      <c r="B56" s="23"/>
+      <c r="C56" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="D56" s="24"/>
-      <c r="E56" s="24" t="s">
+      <c r="D56" s="23"/>
+      <c r="E56" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="F56" s="24"/>
-      <c r="G56" s="26"/>
-      <c r="H56" s="24"/>
+      <c r="F56" s="23"/>
+      <c r="G56" s="25"/>
+      <c r="H56" s="23"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="24"/>
-      <c r="B57" s="24"/>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
-      <c r="E57" s="24"/>
-      <c r="F57" s="24"/>
-      <c r="G57" s="26"/>
-      <c r="H57" s="24"/>
+      <c r="A57" s="23"/>
+      <c r="B57" s="23"/>
+      <c r="C57" s="23"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="23"/>
+      <c r="G57" s="25"/>
+      <c r="H57" s="23"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="24"/>
-      <c r="B58" s="24"/>
-      <c r="C58" s="24" t="s">
+      <c r="A58" s="23"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="23" t="s">
         <v>206</v>
       </c>
-      <c r="D58" s="24" t="s">
+      <c r="D58" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="E58" s="24"/>
-      <c r="F58" s="24"/>
-      <c r="G58" s="24"/>
-      <c r="H58" s="24"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="23"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="24"/>
-      <c r="B59" s="24"/>
-      <c r="C59" s="24" t="s">
+      <c r="A59" s="23"/>
+      <c r="B59" s="23"/>
+      <c r="C59" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="D59" s="24"/>
-      <c r="E59" s="24" t="s">
+      <c r="D59" s="23"/>
+      <c r="E59" s="23" t="s">
         <v>205</v>
       </c>
-      <c r="F59" s="24"/>
-      <c r="G59" s="26"/>
-      <c r="H59" s="24"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="25"/>
+      <c r="H59" s="23"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="24"/>
-      <c r="B60" s="24"/>
-      <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24"/>
-      <c r="G60" s="26"/>
-      <c r="H60" s="24"/>
+      <c r="A60" s="23"/>
+      <c r="B60" s="23"/>
+      <c r="C60" s="23"/>
+      <c r="D60" s="23"/>
+      <c r="E60" s="23"/>
+      <c r="F60" s="23"/>
+      <c r="G60" s="25"/>
+      <c r="H60" s="23"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="24"/>
-      <c r="B61" s="24"/>
-      <c r="C61" s="24" t="s">
+      <c r="A61" s="23"/>
+      <c r="B61" s="23"/>
+      <c r="C61" s="23" t="s">
         <v>209</v>
       </c>
-      <c r="D61" s="24" t="s">
+      <c r="D61" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="E61" s="24" t="s">
+      <c r="E61" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="F61" s="24"/>
-      <c r="G61" s="26"/>
-      <c r="H61" s="24"/>
+      <c r="F61" s="23"/>
+      <c r="G61" s="25"/>
+      <c r="H61" s="23"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="24"/>
-      <c r="B62" s="24"/>
-      <c r="C62" s="24"/>
-      <c r="D62" s="24"/>
-      <c r="E62" s="24"/>
-      <c r="F62" s="24"/>
-      <c r="G62" s="26"/>
-      <c r="H62" s="24"/>
+      <c r="A62" s="23"/>
+      <c r="B62" s="23"/>
+      <c r="C62" s="23"/>
+      <c r="D62" s="23"/>
+      <c r="E62" s="23"/>
+      <c r="F62" s="23"/>
+      <c r="G62" s="25"/>
+      <c r="H62" s="23"/>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="28" t="s">
+      <c r="A63" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="B63" s="28">
+      <c r="B63" s="27">
         <v>5</v>
       </c>
-      <c r="C63" s="28" t="s">
+      <c r="C63" s="27" t="s">
         <v>211</v>
       </c>
-      <c r="D63" s="24" t="s">
+      <c r="D63" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="E63" s="24"/>
-      <c r="F63" s="24"/>
-      <c r="G63" s="26"/>
-      <c r="H63" s="24"/>
+      <c r="E63" s="23"/>
+      <c r="F63" s="23"/>
+      <c r="G63" s="25"/>
+      <c r="H63" s="23"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="24"/>
-      <c r="B64" s="24"/>
-      <c r="C64" s="24"/>
-      <c r="D64" s="24"/>
-      <c r="E64" s="24"/>
-      <c r="F64" s="24"/>
-      <c r="G64" s="26"/>
-      <c r="H64" s="24"/>
+      <c r="A64" s="23"/>
+      <c r="B64" s="23"/>
+      <c r="C64" s="23"/>
+      <c r="D64" s="23"/>
+      <c r="E64" s="23"/>
+      <c r="F64" s="23"/>
+      <c r="G64" s="25"/>
+      <c r="H64" s="23"/>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" s="24"/>
-      <c r="B65" s="24">
+      <c r="A65" s="23"/>
+      <c r="B65" s="23">
         <v>5.0999999999999996</v>
       </c>
-      <c r="C65" s="32" t="s">
+      <c r="C65" s="31" t="s">
         <v>213</v>
       </c>
-      <c r="D65" s="24" t="s">
+      <c r="D65" s="23" t="s">
         <v>214</v>
       </c>
-      <c r="E65" s="24" t="s">
+      <c r="E65" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="F65" s="24" t="s">
+      <c r="F65" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="G65" s="26" t="s">
+      <c r="G65" s="25" t="s">
         <v>215</v>
       </c>
-      <c r="H65" s="24"/>
+      <c r="H65" s="23"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" s="24"/>
-      <c r="B66" s="24"/>
-      <c r="C66" s="24" t="s">
+      <c r="A66" s="23"/>
+      <c r="B66" s="23"/>
+      <c r="C66" s="23" t="s">
         <v>216</v>
       </c>
-      <c r="D66" s="24" t="s">
+      <c r="D66" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="E66" s="24"/>
-      <c r="F66" s="24"/>
-      <c r="G66" s="26"/>
-      <c r="H66" s="24"/>
+      <c r="E66" s="23"/>
+      <c r="F66" s="23"/>
+      <c r="G66" s="25"/>
+      <c r="H66" s="23"/>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="24"/>
-      <c r="B67" s="24"/>
-      <c r="C67" s="24" t="s">
+      <c r="A67" s="23"/>
+      <c r="B67" s="23"/>
+      <c r="C67" s="23" t="s">
         <v>218</v>
       </c>
-      <c r="D67" s="24"/>
-      <c r="E67" s="24"/>
-      <c r="F67" s="24"/>
-      <c r="G67" s="26"/>
-      <c r="H67" s="24"/>
+      <c r="D67" s="23"/>
+      <c r="E67" s="23"/>
+      <c r="F67" s="23"/>
+      <c r="G67" s="25"/>
+      <c r="H67" s="23"/>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" s="24"/>
-      <c r="B68" s="24"/>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
-      <c r="E68" s="24"/>
-      <c r="F68" s="24"/>
-      <c r="G68" s="26"/>
-      <c r="H68" s="24"/>
+      <c r="A68" s="23"/>
+      <c r="B68" s="23"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="23"/>
+      <c r="F68" s="23"/>
+      <c r="G68" s="25"/>
+      <c r="H68" s="23"/>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" s="24"/>
-      <c r="B69" s="24"/>
-      <c r="C69" s="24" t="s">
+      <c r="A69" s="23"/>
+      <c r="B69" s="23"/>
+      <c r="C69" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="D69" s="24" t="s">
+      <c r="D69" s="23" t="s">
         <v>220</v>
       </c>
-      <c r="E69" s="24"/>
-      <c r="F69" s="24"/>
-      <c r="G69" s="26"/>
-      <c r="H69" s="24"/>
+      <c r="E69" s="23"/>
+      <c r="F69" s="23"/>
+      <c r="G69" s="25"/>
+      <c r="H69" s="23"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A70" s="24"/>
-      <c r="B70" s="24"/>
-      <c r="C70" s="24" t="s">
+      <c r="A70" s="23"/>
+      <c r="B70" s="23"/>
+      <c r="C70" s="23" t="s">
         <v>221</v>
       </c>
-      <c r="D70" s="24"/>
-      <c r="E70" s="24"/>
-      <c r="F70" s="24"/>
-      <c r="G70" s="26"/>
-      <c r="H70" s="24"/>
+      <c r="D70" s="23"/>
+      <c r="E70" s="23"/>
+      <c r="F70" s="23"/>
+      <c r="G70" s="25"/>
+      <c r="H70" s="23"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="24"/>
-      <c r="B71" s="24"/>
-      <c r="C71" s="24"/>
-      <c r="D71" s="24"/>
-      <c r="E71" s="24"/>
-      <c r="F71" s="24"/>
-      <c r="G71" s="24"/>
-      <c r="H71" s="24"/>
+      <c r="A71" s="23"/>
+      <c r="B71" s="23"/>
+      <c r="C71" s="23"/>
+      <c r="D71" s="23"/>
+      <c r="E71" s="23"/>
+      <c r="F71" s="23"/>
+      <c r="G71" s="23"/>
+      <c r="H71" s="23"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="24"/>
-      <c r="B72" s="24"/>
-      <c r="C72" s="24" t="s">
+      <c r="A72" s="23"/>
+      <c r="B72" s="23"/>
+      <c r="C72" s="23" t="s">
         <v>222</v>
       </c>
-      <c r="D72" s="24" t="s">
+      <c r="D72" s="23" t="s">
         <v>223</v>
       </c>
-      <c r="E72" s="24"/>
-      <c r="F72" s="24"/>
-      <c r="G72" s="26"/>
-      <c r="H72" s="24"/>
+      <c r="E72" s="23"/>
+      <c r="F72" s="23"/>
+      <c r="G72" s="25"/>
+      <c r="H72" s="23"/>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" s="24"/>
-      <c r="B73" s="24"/>
-      <c r="C73" s="24" t="s">
+      <c r="A73" s="23"/>
+      <c r="B73" s="23"/>
+      <c r="C73" s="23" t="s">
         <v>224</v>
       </c>
-      <c r="D73" s="24"/>
-      <c r="E73" s="24"/>
-      <c r="F73" s="24"/>
-      <c r="G73" s="26"/>
-      <c r="H73" s="24"/>
+      <c r="D73" s="23"/>
+      <c r="E73" s="23"/>
+      <c r="F73" s="23"/>
+      <c r="G73" s="25"/>
+      <c r="H73" s="23"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="63"/>
-      <c r="B74" s="67"/>
-      <c r="C74" s="33" t="s">
+      <c r="A74" s="72"/>
+      <c r="B74" s="76"/>
+      <c r="C74" s="32" t="s">
         <v>225</v>
       </c>
-      <c r="D74" s="33" t="s">
+      <c r="D74" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="E74" s="68"/>
-      <c r="F74" s="63"/>
-      <c r="G74" s="65"/>
-      <c r="H74" s="63"/>
+      <c r="E74" s="77"/>
+      <c r="F74" s="72"/>
+      <c r="G74" s="74"/>
+      <c r="H74" s="72"/>
     </row>
     <row r="75" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A75" s="63"/>
-      <c r="B75" s="67"/>
-      <c r="C75" s="34" t="s">
+      <c r="A75" s="72"/>
+      <c r="B75" s="76"/>
+      <c r="C75" s="33" t="s">
         <v>226</v>
       </c>
-      <c r="D75" s="34" t="s">
+      <c r="D75" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="E75" s="68"/>
-      <c r="F75" s="63"/>
-      <c r="G75" s="65"/>
-      <c r="H75" s="63"/>
+      <c r="E75" s="77"/>
+      <c r="F75" s="72"/>
+      <c r="G75" s="74"/>
+      <c r="H75" s="72"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="24"/>
-      <c r="B76" s="24"/>
-      <c r="C76" s="35"/>
-      <c r="D76" s="24"/>
-      <c r="E76" s="24"/>
-      <c r="F76" s="24"/>
-      <c r="G76" s="26"/>
-      <c r="H76" s="24"/>
+      <c r="A76" s="23"/>
+      <c r="B76" s="23"/>
+      <c r="C76" s="34"/>
+      <c r="D76" s="23"/>
+      <c r="E76" s="23"/>
+      <c r="F76" s="23"/>
+      <c r="G76" s="25"/>
+      <c r="H76" s="23"/>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" s="28" t="s">
+      <c r="A77" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="B77" s="28">
+      <c r="B77" s="27">
         <v>6</v>
       </c>
-      <c r="C77" s="28" t="s">
+      <c r="C77" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="D77" s="24" t="s">
+      <c r="D77" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="E77" s="24"/>
-      <c r="F77" s="24"/>
-      <c r="G77" s="26" t="s">
+      <c r="E77" s="23"/>
+      <c r="F77" s="23"/>
+      <c r="G77" s="25" t="s">
         <v>231</v>
       </c>
-      <c r="H77" s="24"/>
+      <c r="H77" s="23"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" s="24"/>
-      <c r="B78" s="24"/>
-      <c r="C78" s="24"/>
-      <c r="D78" s="24"/>
-      <c r="E78" s="24"/>
-      <c r="F78" s="24"/>
-      <c r="G78" s="26"/>
-      <c r="H78" s="24"/>
+      <c r="A78" s="23"/>
+      <c r="B78" s="23"/>
+      <c r="C78" s="23"/>
+      <c r="D78" s="23"/>
+      <c r="E78" s="23"/>
+      <c r="F78" s="23"/>
+      <c r="G78" s="25"/>
+      <c r="H78" s="23"/>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" s="24"/>
-      <c r="B79" s="24">
+      <c r="A79" s="23"/>
+      <c r="B79" s="23">
         <v>6.1</v>
       </c>
-      <c r="C79" s="32" t="s">
+      <c r="C79" s="31" t="s">
         <v>232</v>
       </c>
-      <c r="D79" s="24" t="s">
+      <c r="D79" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="E79" s="24" t="s">
+      <c r="E79" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="F79" s="24" t="s">
+      <c r="F79" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="G79" s="26" t="s">
+      <c r="G79" s="25" t="s">
         <v>162</v>
       </c>
-      <c r="H79" s="24"/>
+      <c r="H79" s="23"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="24"/>
-      <c r="B80" s="24"/>
-      <c r="C80" s="24" t="s">
+      <c r="A80" s="23"/>
+      <c r="B80" s="23"/>
+      <c r="C80" s="23" t="s">
         <v>233</v>
       </c>
-      <c r="D80" s="24" t="s">
+      <c r="D80" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="E80" s="24"/>
-      <c r="F80" s="24"/>
-      <c r="G80" s="26"/>
-      <c r="H80" s="24"/>
+      <c r="E80" s="23"/>
+      <c r="F80" s="23"/>
+      <c r="G80" s="25"/>
+      <c r="H80" s="23"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="24"/>
-      <c r="B81" s="24"/>
-      <c r="C81" s="31" t="s">
+      <c r="A81" s="23"/>
+      <c r="B81" s="23"/>
+      <c r="C81" s="30" t="s">
         <v>235</v>
       </c>
-      <c r="D81" s="24"/>
-      <c r="E81" s="24"/>
-      <c r="F81" s="24"/>
-      <c r="G81" s="26"/>
-      <c r="H81" s="24"/>
+      <c r="D81" s="23"/>
+      <c r="E81" s="23"/>
+      <c r="F81" s="23"/>
+      <c r="G81" s="25"/>
+      <c r="H81" s="23"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="24"/>
-      <c r="B82" s="24"/>
-      <c r="C82" s="24"/>
-      <c r="D82" s="24"/>
-      <c r="E82" s="24"/>
-      <c r="F82" s="24"/>
-      <c r="G82" s="24"/>
-      <c r="H82" s="24"/>
+      <c r="A82" s="23"/>
+      <c r="B82" s="23"/>
+      <c r="C82" s="23"/>
+      <c r="D82" s="23"/>
+      <c r="E82" s="23"/>
+      <c r="F82" s="23"/>
+      <c r="G82" s="23"/>
+      <c r="H82" s="23"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="24"/>
-      <c r="B83" s="24"/>
-      <c r="C83" s="24" t="s">
+      <c r="A83" s="23"/>
+      <c r="B83" s="23"/>
+      <c r="C83" s="23" t="s">
         <v>236</v>
       </c>
-      <c r="D83" s="24" t="s">
+      <c r="D83" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="E83" s="24"/>
-      <c r="F83" s="24"/>
-      <c r="G83" s="24"/>
-      <c r="H83" s="24"/>
+      <c r="E83" s="23"/>
+      <c r="F83" s="23"/>
+      <c r="G83" s="23"/>
+      <c r="H83" s="23"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="24"/>
-      <c r="B84" s="24"/>
-      <c r="C84" s="31" t="s">
+      <c r="A84" s="23"/>
+      <c r="B84" s="23"/>
+      <c r="C84" s="30" t="s">
         <v>238</v>
       </c>
-      <c r="D84" s="24"/>
-      <c r="E84" s="24"/>
-      <c r="F84" s="24"/>
-      <c r="G84" s="24"/>
-      <c r="H84" s="24"/>
+      <c r="D84" s="23"/>
+      <c r="E84" s="23"/>
+      <c r="F84" s="23"/>
+      <c r="G84" s="23"/>
+      <c r="H84" s="23"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="24"/>
-      <c r="B85" s="24"/>
-      <c r="C85" s="24"/>
-      <c r="D85" s="24"/>
-      <c r="E85" s="24"/>
-      <c r="F85" s="24"/>
-      <c r="G85" s="24"/>
-      <c r="H85" s="24"/>
+      <c r="A85" s="23"/>
+      <c r="B85" s="23"/>
+      <c r="C85" s="23"/>
+      <c r="D85" s="23"/>
+      <c r="E85" s="23"/>
+      <c r="F85" s="23"/>
+      <c r="G85" s="23"/>
+      <c r="H85" s="23"/>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="24"/>
-      <c r="B86" s="24"/>
-      <c r="C86" s="24" t="s">
+      <c r="A86" s="23"/>
+      <c r="B86" s="23"/>
+      <c r="C86" s="23" t="s">
         <v>239</v>
       </c>
-      <c r="D86" s="24" t="s">
+      <c r="D86" s="23" t="s">
         <v>240</v>
       </c>
-      <c r="E86" s="24"/>
-      <c r="F86" s="24"/>
-      <c r="G86" s="24"/>
-      <c r="H86" s="24"/>
+      <c r="E86" s="23"/>
+      <c r="F86" s="23"/>
+      <c r="G86" s="23"/>
+      <c r="H86" s="23"/>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="24"/>
-      <c r="B87" s="24"/>
-      <c r="C87" s="31" t="s">
+      <c r="A87" s="23"/>
+      <c r="B87" s="23"/>
+      <c r="C87" s="30" t="s">
         <v>241</v>
       </c>
-      <c r="D87" s="24"/>
-      <c r="E87" s="24"/>
-      <c r="F87" s="24"/>
-      <c r="G87" s="24"/>
-      <c r="H87" s="24"/>
+      <c r="D87" s="23"/>
+      <c r="E87" s="23"/>
+      <c r="F87" s="23"/>
+      <c r="G87" s="23"/>
+      <c r="H87" s="23"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="24"/>
-      <c r="B88" s="24"/>
-      <c r="C88" s="24"/>
-      <c r="D88" s="24"/>
-      <c r="E88" s="24"/>
-      <c r="F88" s="24"/>
-      <c r="G88" s="24"/>
-      <c r="H88" s="24"/>
+      <c r="A88" s="23"/>
+      <c r="B88" s="23"/>
+      <c r="C88" s="23"/>
+      <c r="D88" s="23"/>
+      <c r="E88" s="23"/>
+      <c r="F88" s="23"/>
+      <c r="G88" s="23"/>
+      <c r="H88" s="23"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="63"/>
-      <c r="B89" s="63"/>
-      <c r="C89" s="36" t="s">
+      <c r="A89" s="72"/>
+      <c r="B89" s="72"/>
+      <c r="C89" s="35" t="s">
         <v>225</v>
       </c>
-      <c r="D89" s="36" t="s">
+      <c r="D89" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="E89" s="64" t="s">
+      <c r="E89" s="73" t="s">
         <v>121</v>
       </c>
-      <c r="F89" s="64"/>
-      <c r="G89" s="65"/>
-      <c r="H89" s="63"/>
+      <c r="F89" s="73"/>
+      <c r="G89" s="74"/>
+      <c r="H89" s="72"/>
     </row>
     <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A90" s="63"/>
-      <c r="B90" s="63"/>
-      <c r="C90" s="36" t="s">
+      <c r="A90" s="72"/>
+      <c r="B90" s="72"/>
+      <c r="C90" s="35" t="s">
         <v>242</v>
       </c>
-      <c r="D90" s="36" t="s">
+      <c r="D90" s="35" t="s">
         <v>243</v>
       </c>
-      <c r="E90" s="64"/>
-      <c r="F90" s="64"/>
-      <c r="G90" s="65"/>
-      <c r="H90" s="63"/>
+      <c r="E90" s="73"/>
+      <c r="F90" s="73"/>
+      <c r="G90" s="74"/>
+      <c r="H90" s="72"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" s="24"/>
-      <c r="B91" s="24"/>
-      <c r="C91" s="24"/>
-      <c r="D91" s="24"/>
-      <c r="E91" s="24"/>
-      <c r="F91" s="24"/>
-      <c r="G91" s="24"/>
-      <c r="H91" s="24"/>
+      <c r="A91" s="23"/>
+      <c r="B91" s="23"/>
+      <c r="C91" s="23"/>
+      <c r="D91" s="23"/>
+      <c r="E91" s="23"/>
+      <c r="F91" s="23"/>
+      <c r="G91" s="23"/>
+      <c r="H91" s="23"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A92" s="28" t="s">
+      <c r="A92" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="B92" s="28">
+      <c r="B92" s="27">
         <v>8</v>
       </c>
-      <c r="C92" s="28" t="s">
+      <c r="C92" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="D92" s="24" t="s">
+      <c r="D92" s="23" t="s">
         <v>245</v>
       </c>
-      <c r="E92" s="24"/>
-      <c r="F92" s="24"/>
-      <c r="G92" s="24"/>
-      <c r="H92" s="24"/>
+      <c r="E92" s="23"/>
+      <c r="F92" s="23"/>
+      <c r="G92" s="23"/>
+      <c r="H92" s="23"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="24"/>
-      <c r="B93" s="24"/>
-      <c r="C93" s="24"/>
-      <c r="D93" s="24"/>
-      <c r="E93" s="24"/>
-      <c r="F93" s="24"/>
-      <c r="G93" s="24"/>
-      <c r="H93" s="24"/>
+      <c r="A93" s="23"/>
+      <c r="B93" s="23"/>
+      <c r="C93" s="23"/>
+      <c r="D93" s="23"/>
+      <c r="E93" s="23"/>
+      <c r="F93" s="23"/>
+      <c r="G93" s="23"/>
+      <c r="H93" s="23"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="24"/>
-      <c r="B94" s="24">
+      <c r="A94" s="23"/>
+      <c r="B94" s="23">
         <v>8.1</v>
       </c>
-      <c r="C94" s="32" t="s">
+      <c r="C94" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="D94" s="24" t="s">
+      <c r="D94" s="23" t="s">
         <v>247</v>
       </c>
-      <c r="E94" s="24" t="s">
+      <c r="E94" s="23" t="s">
         <v>160</v>
       </c>
-      <c r="F94" s="24" t="s">
+      <c r="F94" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="G94" s="24"/>
-      <c r="H94" s="24"/>
+      <c r="G94" s="23"/>
+      <c r="H94" s="23"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="24"/>
-      <c r="B95" s="24"/>
-      <c r="C95" s="24" t="s">
+      <c r="A95" s="23"/>
+      <c r="B95" s="23"/>
+      <c r="C95" s="23" t="s">
         <v>248</v>
       </c>
-      <c r="D95" s="24" t="s">
+      <c r="D95" s="23" t="s">
         <v>249</v>
       </c>
-      <c r="E95" s="24"/>
-      <c r="F95" s="24"/>
-      <c r="G95" s="24"/>
-      <c r="H95" s="24"/>
+      <c r="E95" s="23"/>
+      <c r="F95" s="23"/>
+      <c r="G95" s="23"/>
+      <c r="H95" s="23"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="24"/>
-      <c r="B96" s="24"/>
-      <c r="C96" s="31" t="s">
+      <c r="A96" s="23"/>
+      <c r="B96" s="23"/>
+      <c r="C96" s="30" t="s">
         <v>250</v>
       </c>
-      <c r="D96" s="24"/>
-      <c r="E96" s="24"/>
-      <c r="F96" s="24"/>
-      <c r="G96" s="24"/>
-      <c r="H96" s="24"/>
+      <c r="D96" s="23"/>
+      <c r="E96" s="23"/>
+      <c r="F96" s="23"/>
+      <c r="G96" s="23"/>
+      <c r="H96" s="23"/>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A97" s="24"/>
-      <c r="B97" s="24"/>
-      <c r="C97" s="24"/>
-      <c r="D97" s="24"/>
-      <c r="E97" s="24"/>
-      <c r="F97" s="24"/>
-      <c r="G97" s="24"/>
-      <c r="H97" s="24"/>
+      <c r="A97" s="23"/>
+      <c r="B97" s="23"/>
+      <c r="C97" s="23"/>
+      <c r="D97" s="23"/>
+      <c r="E97" s="23"/>
+      <c r="F97" s="23"/>
+      <c r="G97" s="23"/>
+      <c r="H97" s="23"/>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="24"/>
-      <c r="B98" s="24"/>
-      <c r="C98" s="24" t="s">
+      <c r="A98" s="23"/>
+      <c r="B98" s="23"/>
+      <c r="C98" s="23" t="s">
         <v>251</v>
       </c>
-      <c r="D98" s="24" t="s">
+      <c r="D98" s="23" t="s">
         <v>252</v>
       </c>
-      <c r="E98" s="24"/>
-      <c r="F98" s="24"/>
-      <c r="G98" s="24"/>
-      <c r="H98" s="24"/>
+      <c r="E98" s="23"/>
+      <c r="F98" s="23"/>
+      <c r="G98" s="23"/>
+      <c r="H98" s="23"/>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="24"/>
-      <c r="B99" s="24"/>
-      <c r="C99" s="31" t="s">
+      <c r="A99" s="23"/>
+      <c r="B99" s="23"/>
+      <c r="C99" s="30" t="s">
         <v>253</v>
       </c>
-      <c r="D99" s="24"/>
-      <c r="E99" s="24"/>
-      <c r="F99" s="24"/>
-      <c r="G99" s="24"/>
-      <c r="H99" s="24"/>
+      <c r="D99" s="23"/>
+      <c r="E99" s="23"/>
+      <c r="F99" s="23"/>
+      <c r="G99" s="23"/>
+      <c r="H99" s="23"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" s="24"/>
-      <c r="B100" s="24"/>
-      <c r="C100" s="24" t="s">
+      <c r="A100" s="23"/>
+      <c r="B100" s="23"/>
+      <c r="C100" s="23" t="s">
         <v>254</v>
       </c>
-      <c r="D100" s="24" t="s">
+      <c r="D100" s="23" t="s">
         <v>255</v>
       </c>
-      <c r="E100" s="24" t="s">
+      <c r="E100" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="F100" s="24"/>
-      <c r="G100" s="24"/>
-      <c r="H100" s="24"/>
+      <c r="F100" s="23"/>
+      <c r="G100" s="23"/>
+      <c r="H100" s="23"/>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A101" s="24"/>
-      <c r="B101" s="24"/>
-      <c r="C101" s="24"/>
-      <c r="D101" s="24"/>
-      <c r="E101" s="24"/>
-      <c r="F101" s="24"/>
-      <c r="G101" s="24"/>
-      <c r="H101" s="24"/>
+      <c r="A101" s="23"/>
+      <c r="B101" s="23"/>
+      <c r="C101" s="23"/>
+      <c r="D101" s="23"/>
+      <c r="E101" s="23"/>
+      <c r="F101" s="23"/>
+      <c r="G101" s="23"/>
+      <c r="H101" s="23"/>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="24"/>
-      <c r="B102" s="24"/>
-      <c r="C102" s="24" t="s">
+      <c r="A102" s="23"/>
+      <c r="B102" s="23"/>
+      <c r="C102" s="23" t="s">
         <v>256</v>
       </c>
-      <c r="D102" s="24" t="s">
+      <c r="D102" s="23" t="s">
         <v>257</v>
       </c>
-      <c r="E102" s="24"/>
-      <c r="F102" s="24"/>
-      <c r="G102" s="24"/>
-      <c r="H102" s="24"/>
+      <c r="E102" s="23"/>
+      <c r="F102" s="23"/>
+      <c r="G102" s="23"/>
+      <c r="H102" s="23"/>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" s="24"/>
-      <c r="B103" s="24"/>
-      <c r="C103" s="31" t="s">
+      <c r="A103" s="23"/>
+      <c r="B103" s="23"/>
+      <c r="C103" s="30" t="s">
         <v>258</v>
       </c>
-      <c r="D103" s="24"/>
-      <c r="E103" s="24"/>
-      <c r="F103" s="24"/>
-      <c r="G103" s="24"/>
-      <c r="H103" s="24"/>
+      <c r="D103" s="23"/>
+      <c r="E103" s="23"/>
+      <c r="F103" s="23"/>
+      <c r="G103" s="23"/>
+      <c r="H103" s="23"/>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" s="24" t="s">
+      <c r="A104" s="23" t="s">
         <v>259</v>
       </c>
-      <c r="B104" s="24"/>
-      <c r="C104" s="24" t="s">
+      <c r="B104" s="23"/>
+      <c r="C104" s="23" t="s">
         <v>254</v>
       </c>
-      <c r="D104" s="24" t="s">
+      <c r="D104" s="23" t="s">
         <v>255</v>
       </c>
-      <c r="E104" s="24" t="s">
+      <c r="E104" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="F104" s="24"/>
-      <c r="G104" s="24"/>
-      <c r="H104" s="24"/>
+      <c r="F104" s="23"/>
+      <c r="G104" s="23"/>
+      <c r="H104" s="23"/>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A105" s="24"/>
-      <c r="B105" s="24"/>
-      <c r="C105" s="24"/>
-      <c r="D105" s="24"/>
-      <c r="E105" s="24"/>
-      <c r="F105" s="24"/>
-      <c r="G105" s="24"/>
-      <c r="H105" s="24"/>
+      <c r="A105" s="23"/>
+      <c r="B105" s="23"/>
+      <c r="C105" s="23"/>
+      <c r="D105" s="23"/>
+      <c r="E105" s="23"/>
+      <c r="F105" s="23"/>
+      <c r="G105" s="23"/>
+      <c r="H105" s="23"/>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="28" t="s">
+      <c r="A106" s="27" t="s">
         <v>260</v>
       </c>
-      <c r="B106" s="28">
+      <c r="B106" s="27">
         <v>9</v>
       </c>
-      <c r="C106" s="28" t="s">
+      <c r="C106" s="27" t="s">
         <v>261</v>
       </c>
-      <c r="D106" s="24" t="s">
+      <c r="D106" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="E106" s="24"/>
-      <c r="F106" s="24"/>
-      <c r="G106" s="24"/>
-      <c r="H106" s="24"/>
+      <c r="E106" s="23"/>
+      <c r="F106" s="23"/>
+      <c r="G106" s="23"/>
+      <c r="H106" s="23"/>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="24"/>
-      <c r="B107" s="24">
+      <c r="A107" s="23"/>
+      <c r="B107" s="23">
         <v>9.1</v>
       </c>
-      <c r="C107" s="32" t="s">
+      <c r="C107" s="31" t="s">
         <v>263</v>
       </c>
-      <c r="D107" s="24"/>
-      <c r="E107" s="24" t="s">
+      <c r="D107" s="23"/>
+      <c r="E107" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="F107" s="24" t="s">
+      <c r="F107" s="23" t="s">
         <v>264</v>
       </c>
-      <c r="G107" s="24"/>
-      <c r="H107" s="24"/>
+      <c r="G107" s="23"/>
+      <c r="H107" s="23"/>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" s="24"/>
-      <c r="B108" s="24"/>
-      <c r="C108" s="24"/>
-      <c r="D108" s="24"/>
-      <c r="E108" s="24"/>
-      <c r="F108" s="24"/>
-      <c r="G108" s="24"/>
-      <c r="H108" s="24"/>
+      <c r="A108" s="23"/>
+      <c r="B108" s="23"/>
+      <c r="C108" s="23"/>
+      <c r="D108" s="23"/>
+      <c r="E108" s="23"/>
+      <c r="F108" s="23"/>
+      <c r="G108" s="23"/>
+      <c r="H108" s="23"/>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="24"/>
-      <c r="B109" s="24"/>
-      <c r="C109" s="24"/>
-      <c r="D109" s="24"/>
-      <c r="E109" s="24"/>
-      <c r="F109" s="24"/>
-      <c r="G109" s="24"/>
-      <c r="H109" s="24"/>
+      <c r="A109" s="23"/>
+      <c r="B109" s="23"/>
+      <c r="C109" s="23"/>
+      <c r="D109" s="23"/>
+      <c r="E109" s="23"/>
+      <c r="F109" s="23"/>
+      <c r="G109" s="23"/>
+      <c r="H109" s="23"/>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A110" s="28" t="s">
+      <c r="A110" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="B110" s="28">
+      <c r="B110" s="27">
         <v>10</v>
       </c>
-      <c r="C110" s="28" t="s">
+      <c r="C110" s="27" t="s">
         <v>265</v>
       </c>
-      <c r="D110" s="24" t="s">
+      <c r="D110" s="23" t="s">
         <v>266</v>
       </c>
-      <c r="E110" s="24"/>
-      <c r="F110" s="24"/>
-      <c r="G110" s="24"/>
-      <c r="H110" s="24"/>
+      <c r="E110" s="23"/>
+      <c r="F110" s="23"/>
+      <c r="G110" s="23"/>
+      <c r="H110" s="23"/>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A111" s="24"/>
-      <c r="B111" s="24">
+      <c r="A111" s="23"/>
+      <c r="B111" s="23">
         <v>10.1</v>
       </c>
-      <c r="C111" s="32" t="s">
+      <c r="C111" s="31" t="s">
         <v>267</v>
       </c>
-      <c r="D111" s="24" t="s">
+      <c r="D111" s="23" t="s">
         <v>268</v>
       </c>
-      <c r="E111" s="24"/>
-      <c r="F111" s="24"/>
-      <c r="G111" s="24"/>
-      <c r="H111" s="24"/>
+      <c r="E111" s="23"/>
+      <c r="F111" s="23"/>
+      <c r="G111" s="23"/>
+      <c r="H111" s="23"/>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A112" s="24"/>
-      <c r="B112" s="24"/>
-      <c r="C112" s="24" t="s">
+      <c r="A112" s="23"/>
+      <c r="B112" s="23"/>
+      <c r="C112" s="23" t="s">
         <v>269</v>
       </c>
-      <c r="D112" s="24" t="s">
+      <c r="D112" s="23" t="s">
         <v>270</v>
       </c>
-      <c r="E112" s="24" t="s">
+      <c r="E112" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="F112" s="24"/>
-      <c r="G112" s="24"/>
-      <c r="H112" s="24"/>
+      <c r="F112" s="23"/>
+      <c r="G112" s="23"/>
+      <c r="H112" s="23"/>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A113" s="24"/>
-      <c r="B113" s="24"/>
-      <c r="C113" s="24" t="s">
+      <c r="A113" s="23"/>
+      <c r="B113" s="23"/>
+      <c r="C113" s="23" t="s">
         <v>271</v>
       </c>
-      <c r="D113" s="24" t="s">
+      <c r="D113" s="23" t="s">
         <v>272</v>
       </c>
-      <c r="E113" s="24" t="s">
+      <c r="E113" s="23" t="s">
         <v>273</v>
       </c>
-      <c r="F113" s="24" t="s">
+      <c r="F113" s="23" t="s">
         <v>274</v>
       </c>
-      <c r="G113" s="24"/>
-      <c r="H113" s="24"/>
+      <c r="G113" s="23"/>
+      <c r="H113" s="23"/>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A114" s="24"/>
-      <c r="B114" s="24"/>
-      <c r="C114" s="24"/>
-      <c r="D114" s="24"/>
-      <c r="E114" s="24"/>
-      <c r="F114" s="24"/>
-      <c r="G114" s="24"/>
-      <c r="H114" s="24"/>
+      <c r="A114" s="23"/>
+      <c r="B114" s="23"/>
+      <c r="C114" s="23"/>
+      <c r="D114" s="23"/>
+      <c r="E114" s="23"/>
+      <c r="F114" s="23"/>
+      <c r="G114" s="23"/>
+      <c r="H114" s="23"/>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A115" s="24"/>
-      <c r="B115" s="24">
+      <c r="A115" s="23"/>
+      <c r="B115" s="23">
         <v>10.199999999999999</v>
       </c>
-      <c r="C115" s="32" t="s">
+      <c r="C115" s="31" t="s">
         <v>275</v>
       </c>
-      <c r="D115" s="24" t="s">
+      <c r="D115" s="23" t="s">
         <v>276</v>
       </c>
-      <c r="E115" s="24" t="s">
+      <c r="E115" s="23" t="s">
         <v>277</v>
       </c>
-      <c r="F115" s="24"/>
-      <c r="G115" s="24" t="s">
+      <c r="F115" s="23"/>
+      <c r="G115" s="23" t="s">
         <v>278</v>
       </c>
-      <c r="H115" s="24"/>
+      <c r="H115" s="23"/>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A116" s="24"/>
-      <c r="B116" s="24"/>
-      <c r="C116" s="24"/>
-      <c r="D116" s="24"/>
-      <c r="E116" s="24"/>
-      <c r="F116" s="24"/>
-      <c r="G116" s="24"/>
-      <c r="H116" s="24"/>
+      <c r="A116" s="23"/>
+      <c r="B116" s="23"/>
+      <c r="C116" s="23"/>
+      <c r="D116" s="23"/>
+      <c r="E116" s="23"/>
+      <c r="F116" s="23"/>
+      <c r="G116" s="23"/>
+      <c r="H116" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -6629,7 +7258,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -6640,82 +7269,82 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="36" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="36" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="36" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="39" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="40" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="40" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="40" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="40" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="40" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="40" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="40" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="42" t="s">
+      <c r="A13" s="41" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="41" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="41" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="23" t="s">
         <v>288</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Creation of html/lock-selection-survey.html and implementation of related js and css for customer information capture.
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C200126C-AD13-AB41-981F-F4FD9ED18CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26FA078-FE3C-044C-A79B-C24631BEC6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="1000" windowWidth="27640" windowHeight="16160" activeTab="3" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
+    <workbookView xWindow="300" yWindow="1000" windowWidth="27640" windowHeight="16160" activeTab="4" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="SPEC - 1.1" sheetId="1" r:id="rId1"/>
     <sheet name="SPEC - 1.2" sheetId="2" r:id="rId2"/>
     <sheet name="SPEC - 1.3" sheetId="4" r:id="rId3"/>
     <sheet name="SPEC - 1.4" sheetId="7" r:id="rId4"/>
-    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId5"/>
-    <sheet name="PLAYGROUND" sheetId="6" r:id="rId6"/>
+    <sheet name="SPEC - 1.5" sheetId="9" r:id="rId5"/>
+    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId6"/>
+    <sheet name="PLAYGROUND" sheetId="6" r:id="rId7"/>
+    <sheet name="TEMPLATE" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="332">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -3931,6 +3933,1277 @@
   </si>
   <si>
     <t>git commit -m "Refactored Customer and Sales class - use strict directive and sectional comments introduced."</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html/lock-selection-survey.html</t>
+    </r>
+  </si>
+  <si>
+    <t>touch html/lock-selection-survey.html</t>
+  </si>
+  <si>
+    <t>touch css/lock-selection-survey.css</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/lock-selection-survey.css</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>ls</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">html </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">displays the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lock-selection-survey.html</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ls css </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>displays the file</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> lock-selection-survey.css</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Initialize the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">html/lock-selection-survey.html </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>and create the customer card</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Initialized the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">html/lock-selection-survey.html </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>and created the customer card</t>
+    </r>
+  </si>
+  <si>
+    <t>/* The callback function fired on 'get focus' - for customer 
+ * mobile input control.
+ * @param    
+ * @return   
+ * */
+const resetCustomerMobileInputOnGetFocus = () =&gt; {
+    // Preserve the original placeholder text - the first time the control
+    // gets focus.
+    // The customerMobileInputPlaceholder variable will be empty 
+    // the first time control gets focus
+    if (customerMobileInputPlaceholder.length === 0) {
+        customerMobileInputPlaceholder = customerMobileInput.placeholder;
+    }
+    // If the customer mobile input control has the class SWAP_VALUE 
+    // attached - it means that an incorrect value was entered in the field
+    // the last time the control had focus.
+    if (customerMobileInput.classList.contains(SWAP_VALUE) === true) {
+        // Remove the class SWAP_VALUE - as the user is preparing to re-enter
+        // a valid value
+        customerMobileInput.classList.remove(SWAP_VALUE);
+        // Set the value of the input control to the placeholder value.
+        // The erroneous/invalid value was preserved in the placeholder 
+        // value - the last time input control lost focus.
+        customerMobileInput.value = customerMobileInput.placeholder;
+        // Set the placeholder value of the input control to the original
+        // placeholder value of the field.
+        customerMobileInput.placeholder = customerMobileInputPlaceholder;
+        // Select the value set in the input field
+        customerMobileInput.select();
+    }
+    // Reset all validation related classes
+    resetValidation(customerMobilePrependDiv, customerMobileInputGroupTextDiv);
+    // Refresh to original state of the container div
+    customerMobileDiv.classList.remove("was-validated");
+}
+/* The callback function fired on 'blur' - for customer mobile input control. 
+ * @param    
+ * @return   
+ * */
+const validateCustomerMobileInputOnBlur = () =&gt; {
+    // Check for white spaces
+    if (customerMobileInput.value.trim().length === 0) {
+        // White spaces are present - reset the value to be empty
+        customerMobileInput.value = "";
+        // Update the invalid feedback message
+        customerMobileInvalidFeedback.innerHTML = "Mobile number cannot " +
+            "be blank.";
+        invalidateInputControl(customerMobilePrependDiv,
+            customerMobileInputGroupTextDiv);
+    } // Check for the length of the mobile no. to be exactly 10 characters
+    // and contains only numeric digits starting with a 0
+    else if (customerMobileInput.value.trim().length &lt; 10 ||
+        customerMobileInput.value.trim().length &gt; 10 ||
+        isNaN(parseInt(customerMobileInput.value.trim())) === true ||
+        String("0" + parseInt(customerMobileInput.value.trim())) !==
+        customerMobileInput.value.trim()) {
+        // Update the placeholder to display the erroneous/invalid 
+        // entered value and reset the input value to blank to invalidate the 
+        // input control
+        customerMobileInput.placeholder = customerMobileInput.value;
+        customerMobileInput.value = "";
+        // Update the invalid feedback message
+        customerMobileInvalidFeedback.innerHTML = "Mobile No. must contain " +
+            "10 digits, starting with a 0."
+        // Add the SWAP_VALUE class to the customer mobile input control
+        customerMobileInput.classList.add(SWAP_VALUE);
+        invalidateInputControl(customerMobilePrependDiv,
+            customerMobileInputGroupTextDiv);
+    } else // Passed all validation checks
+    {
+        validateInputControl(customerMobilePrependDiv,
+            customerMobileInputGroupTextDiv);
+    }
+    customerMobileDiv.classList.add("was-validated");
+    // Enable/Disable the navigation button(s)
+    if (allInputsAreValidated() === true) {
+        customerCardNextButton.disabled = false;
+    } else {
+        customerCardNextButton.disabled = true;
+    }
+}
+/* The callback function fired on 'get focus' - for customer 
+ * Address1 input control.
+ * @param    
+ * @return   
+ * */
+const resetCustomerAddress1InputOnGetFocus = () =&gt; {
+    // Preserve the original placeholder text - the first time the control 
+    // gets focus.
+    // The customerAddress1InputPlaceholder variable will be empty 
+    // the first time
+    // control gets focus
+    if (customerAddress1InputPlaceholder.length === 0) {
+        customerAddress1InputPlaceholder = customerAddress1Input.placeholder;
+    }
+    // If the customer Address1 input control has the class SWAP_VALUE 
+    // attached - it means that an incorrect value was entered in the field
+    // the last time the control had focus.
+    if (customerAddress1Input.classList.contains(SWAP_VALUE) === true) {
+        // Remove the class SWAP_VALUE - as the user is preparing to re-enter
+        // a valid value
+        customerAddress1Input.classList.remove(SWAP_VALUE);
+        // Set the value of the input control to the placeholder value.
+        // The erroneous/invalid value was preserved in the placeholder 
+        // value - the last time input control lost focus.
+        customerAddress1Input.value = customerAddress1Input.placeholder;
+        // Set the placeholder value of the input control to the original
+        // placeholder value of the field.
+        customerAddress1Input.placeholder = customerAddress1InputPlaceholder;
+        // Select the value set in the input field
+        customerAddress1Input.select();
+    }
+    // Reset all validation related classes
+    resetValidation(customerAddress1PrependDiv,
+        customerAddress1InputGroupTextDiv);
+    // Refresh to original state of the container div
+    customerAddress1Div.classList.remove("was-validated");
+}
+/* The callback function fired on 'blur' - for customer Address1 input control.
+ * @param    
+ * @return   
+ * */
+const validateCustomerAddress1InputOnBlur = () =&gt; {
+    // Check for white spaces
+    if (customerAddress1Input.value.trim().length === 0) {
+        // White spaces are present - reset the value to be empty
+        customerAddress1Input.value = "";
+        // Update the invalid feedback message
+        customerAddress1InvalidFeedback.innerHTML = "Address cannot be blank.";
+        invalidateInputControl(customerAddress1PrependDiv,
+            customerAddress1InputGroupTextDiv);
+    } // Check for the length of the Address1 to be not more than 50 characters
+    else if (customerAddress1Input.value.trim().length &gt; 50) {
+        // Update the placeholder to display the erroneous/invalid
+        // entered value and reset the input value to blank to invalidate the
+        // input control
+        customerAddress1Input.placeholder = customerAddress1Input.value;
+        customerAddress1Input.value = "";
+        // Update the invalid feedback message
+        customerAddress1InvalidFeedback.innerHTML = "Address Line 1 cannot " +
+            "contain more than 50 characters.";
+        // Add the SWAP_VALUE class to the customer Address1 input control
+        customerAddress1Input.classList.add(SWAP_VALUE);
+        invalidateInputControl(customerAddress1PrependDiv,
+            customerAddress1InputGroupTextDiv);
+    } else // Passed all validation checks
+    {
+        validateInputControl(customerAddress1PrependDiv,
+            customerAddress1InputGroupTextDiv);
+    }
+    customerAddress1Div.classList.add("was-validated");
+    // Enable/Disable the navigation button(s)
+    if (allInputsAreValidated() === true) {
+        customerCardNextButton.disabled = false;
+    } else {
+        customerCardNextButton.disabled = true;
+    }
+}</t>
+  </si>
+  <si>
+    <t>/* The callback function fired on 'get focus' - for customer 
+ * Address2 input control.
+ * @param    
+ * @return   
+ * */
+const resetCustomerAddress2InputOnGetFocus = () =&gt; {
+    // Remove the required attribute - if present
+    customerAddress2Input.removeAttribute("required", "");
+    // Preserve the original placeholder text - the first time the control 
+    // gets focus.
+    // The customerAddress2InputPlaceholder variable will be empty 
+    // the first time
+    // control gets focus
+    if (customerAddress2InputPlaceholder.length === 0) {
+        customerAddress2InputPlaceholder = customerAddress2Input.placeholder;
+    }
+    // If the customer Address2 input control has the class SWAP_VALUE 
+    // attached - it means that an incorrect value was entered in the field
+    // the last time the control had focus.
+    if (customerAddress2Input.classList.contains(SWAP_VALUE) === true) {
+        // Remove the class SWAP_VALUE - as the user is preparing to re-enter
+        // a valid value
+        customerAddress2Input.classList.remove(SWAP_VALUE);
+        // Set the value of the input control to the placeholder value.
+        // The erroneous/invalid value was preserved in the placeholder 
+        // value - the last time input control lost focus.
+        customerAddress2Input.value = customerAddress2Input.placeholder;
+        // Set the placeholder value of the input control to the original
+        // placeholder value of the field.
+        customerAddress2Input.placeholder = customerAddress2InputPlaceholder;
+        // Select the value set in the input field
+        customerAddress2Input.select();
+    }
+    // Reset all validation related classes
+    resetValidation(customerAddress2PrependDiv,
+        customerAddress2InputGroupTextDiv);
+    // Refresh to original state of the container div
+    customerAddress2Div.classList.remove("was-validated");
+}
+/* The callback function fired on 'blur' - for customer Address2 input control.
+ * @param    
+ * @return   
+ * */
+const validateCustomerAddress2InputOnBlur = () =&gt; {
+    // Check for white spaces
+    if (customerAddress2Input.value.trim().length === 0) {
+        // White spaces are present - reset the value to be empty
+        customerAddress2Input.value = "";
+        // Update the invalid feedback message
+        customerAddress2InvalidFeedback.innerHTML = "";
+        validateInputControl(customerAddress2PrependDiv,
+            customerAddress2InputGroupTextDiv);
+    } // Check for the length of the Address2 to be not more than 50 characters
+    else if (customerAddress2Input.value.trim().length &gt; 50) {
+        // Set the required attribute
+        customerAddress2Input.setAttribute("required", "");
+        // Update the placeholder to display the erroneous/invalid
+        // entered value and reset the input value to blank to invalidate the
+        // input control
+        customerAddress2Input.placeholder = customerAddress2Input.value;
+        customerAddress2Input.value = "";
+        // Update the invalid feedback message
+        customerAddress2InvalidFeedback.innerHTML = "Address Line 2 cannot " +
+            "contain more than 50 characters.";
+        // Add the SWAP_VALUE class to the customer Address2 input control
+        customerAddress2Input.classList.add(SWAP_VALUE);
+        invalidateInputControl(customerAddress2PrependDiv,
+            customerAddress2InputGroupTextDiv);
+    } else // Passed all validation checks
+    {
+        validateInputControl(customerAddress2PrependDiv,
+            customerAddress2InputGroupTextDiv);
+    }
+    customerAddress2Div.classList.add("was-validated");
+    // Enable/Disable the navigation button(s)
+    if (allInputsAreValidated() === true) {
+        customerCardNextButton.disabled = false;
+    } else {
+        customerCardNextButton.disabled = true;
+    }
+}
+/* The callback function fired on 'get focus' - for customer 
+ * Address3 input control.
+ * @param    
+ * @return   
+ * */
+const resetCustomerAddress3InputOnGetFocus = () =&gt; {
+    // Remove the required attribute - if present
+    customerAddress3Input.removeAttribute("required", "");
+    // Preserve the original placeholder text - the first time the control 
+    // gets focus.
+    // The customerAddress3InputPlaceholder variable will be empty 
+    // the first time
+    // control gets focus
+    if (customerAddress3InputPlaceholder.length === 0) {
+        customerAddress3InputPlaceholder = customerAddress3Input.placeholder;
+    }
+    // If the customer Address3 input control has the class SWAP_VALUE 
+    // attached - it means that an incorrect value was entered in the field
+    // the last time the control had focus.
+    if (customerAddress3Input.classList.contains(SWAP_VALUE) === true) {
+        // Remove the class SWAP_VALUE - as the user is preparing to re-enter
+        // a valid value
+        customerAddress3Input.classList.remove(SWAP_VALUE);
+        // Set the value of the input control to the placeholder value.
+        // The erroneous/invalid value was preserved in the placeholder 
+        // value - the last time input control lost focus.
+        customerAddress3Input.value = customerAddress3Input.placeholder;
+        // Set the placeholder value of the input control to the original
+        // placeholder value of the field.
+        customerAddress3Input.placeholder = customerAddress3InputPlaceholder;
+        // Select the value set in the input field
+        customerAddress3Input.select();
+    }
+    // Reset all validation related classes
+    resetValidation(customerAddress3PrependDiv,
+        customerAddress3InputGroupTextDiv);
+    // Refresh to original state of the container div
+    customerAddress3Div.classList.remove("was-validated");
+}
+/* The callback function fired on 'blur' - for customer Address3 input control.
+ * @param    
+ * @return   
+ * */
+const validateCustomerAddress3InputOnBlur = () =&gt; {
+    // Check for white spaces
+    if (customerAddress3Input.value.trim().length === 0) {
+        // White spaces are present - reset the value to be empty
+        customerAddress3Input.value = "";
+        // Update the invalid feedback message
+        customerAddress3InvalidFeedback.innerHTML = "";
+        validateInputControl(customerAddress3PrependDiv,
+            customerAddress3InputGroupTextDiv);
+    } // Check for the length of the Address3 to be not more than 50 characters
+    else if (customerAddress3Input.value.trim().length &gt; 50) {
+        // Set the required attribute
+        customerAddress3Input.setAttribute("required", "");
+        // Update the placeholder to display the erroneous/invalid
+        // entered value and reset the input value to blank to invalidate the
+        // input control
+        customerAddress3Input.placeholder = customerAddress3Input.value;
+        customerAddress3Input.value = "";
+        // Update the invalid feedback message
+        customerAddress3InvalidFeedback.innerHTML = "Address Line 3 cannot " +
+            "contain more than 50 characters.";
+        // Add the SWAP_VALUE class to the customer Address3 input control
+        customerAddress3Input.classList.add(SWAP_VALUE);
+        invalidateInputControl(customerAddress3PrependDiv,
+            customerAddress3InputGroupTextDiv);
+    } else // Passed all validation checks
+    {
+        validateInputControl(customerAddress3PrependDiv,
+            customerAddress3InputGroupTextDiv);
+    }
+    customerAddress3Div.classList.add("was-validated");
+    // Enable/Disable the navigation button(s)
+    if (allInputsAreValidated() === true) {
+        customerCardNextButton.disabled = false;
+    } else {
+        customerCardNextButton.disabled = true;
+    }
+}</t>
+  </si>
+  <si>
+    <t>/*****************************************************************************/
+/* HELPER FUNCTIONS                                                          */
+/*****************************************************************************/
+/* Helper function to provide the invalidate style for the input control. 
+ * @param   {HTMLElement}   prependDiv   &lt;div class="input-group-prepend"&gt;
+ * @param   {HTMLElement}   inputGroupTextDiv  &lt;span class="input-group-text"&gt;
+ * @return   
+ * */
+const invalidateInputControl = (prependDiv, inputGroupTextDiv) =&gt; {
+    // Add the class - prepend-invalid to the customer name prepend div
+    prependDiv.classList.remove("prepend-valid");
+    prependDiv.classList.add("prepend-invalid");
+    // Make the input-group-text &lt;div&gt; transparent
+    inputGroupTextDiv.classList.remove("input-group-text-opaque");
+    inputGroupTextDiv.classList.add("input-group-text-transparent");
+}
+/* Helper function to provide the validate style for input the control. 
+ * @param   {HTMLElement}   prependDiv   &lt;div class="input-group-prepend"&gt;
+ * @param   {HTMLElement}   inputGroupTextDiv  &lt;span class="input-group-text"&gt;
+ * @return   
+ * */
+const validateInputControl = (prependDiv, inputGroupTextDiv) =&gt; {
+    // Add the class - prepend-valid to the customer name prepend div
+    prependDiv.classList.remove("prepend-invalid");
+    prependDiv.classList.add("prepend-valid");
+    // Make the input-group-text &lt;div&gt; transparent
+    inputGroupTextDiv.classList.remove("input-group-text-opaque");
+    inputGroupTextDiv.classList.add("input-group-text-transparent");
+}
+/* Helper function to remove the validate and invalidate style for 
+ * the input control.
+ * @param   {HTMLElement}   prependDiv   &lt;div class="input-group-prepend"&gt;
+ * @param   {HTMLElement}   inputGroupTextDiv  &lt;span class="input-group-text"&gt;
+ * @return   
+ * */
+const resetValidation = (prependDiv, inputGroupTextDiv) =&gt; {
+    // Remove the class - prepend-invalid to the customer name prepend div
+    // if present
+    prependDiv.classList.remove("prepend-invalid");
+    // Remove the class - prepend-invalid to the customer name prepend div 
+    // if present 
+    prependDiv.classList.remove("prepend-valid");
+    // Make the input-group-text &lt;div&gt; opaque
+    inputGroupTextDiv.classList.remove("input-group-text-transparent");
+    inputGroupTextDiv.classList.add("input-group-text-opaque");
+}
+/* Helper function to check if all input fields are validated.
+ * @param  
+ * @return {boolean}    true if all fields are validated - false otherwise  
+ * */
+const allInputsAreValidated = () =&gt; {
+    // Flag to check if all input fields were validated
+    let allFieldsAreValidated = false;
+    // Get all the div elements which have the class "input-group"
+    let allInputContainerDivElements = document
+        .getElementsByClassName("input-group");
+    // Iterate over all the div elements 
+    for (let containerDiv of allInputContainerDivElements) {
+        // Get the div element with the class "input-group-prepend"
+        // inside the container div
+        let prependDiv = containerDiv
+            .getElementsByClassName("input-group-prepend")[0];
+        // If the container div contains the class "optional"
+        // check if the input box has any value - if it does not have any
+        // value - consider it to be validated
+        if (containerDiv.classList.contains("optional") === true) {
+            if (containerDiv.getElementsByTagName("input")[0].value.length === 0) {
+                allFieldsAreValidated = true;
+                continue;
+            }
+        }
+        if (prependDiv.classList.contains("prepend-valid")) {
+            allFieldsAreValidated = true;
+        } else {
+            allFieldsAreValidated = false;
+            break;
+        }
+    }
+    return allFieldsAreValidated;
+}
+/*****************************************************************************/
+/* REGISTER EVENT LISTENERS                                                  */
+/*****************************************************************************/
+// Event listeners registered for the Customer Name input control
+customerNameInput.addEventListener("blur", validateCustomerNameInputOnBlur);
+customerNameInput.addEventListener("focus", resetCustomerNameInputOnGetFocus);
+// Event listeners registered for the Customer Mobile input control
+customerMobileInput.addEventListener("blur",
+    validateCustomerMobileInputOnBlur);
+customerMobileInput.addEventListener("focus",
+    resetCustomerMobileInputOnGetFocus);
+// Event listeners registered for the Customer Address1 input control
+customerAddress1Input.addEventListener("blur",
+    validateCustomerAddress1InputOnBlur);
+customerAddress1Input.addEventListener("focus",
+    resetCustomerAddress1InputOnGetFocus);
+// Event listeners registered for the Customer Address2 input control
+customerAddress2Input.addEventListener("blur",
+    validateCustomerAddress2InputOnBlur);
+customerAddress2Input.addEventListener("focus",
+    resetCustomerAddress2InputOnGetFocus);
+// Event listeners registered for the Customer Address3 input control
+customerAddress3Input.addEventListener("blur",
+    validateCustomerAddress3InputOnBlur);
+customerAddress3Input.addEventListener("focus",
+    resetCustomerAddress3InputOnGetFocus);
+/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/lock-selection-survey-customer-card.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>ls js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> displays the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/lock-selection-survey-customer-card.js</t>
+    </r>
+  </si>
+  <si>
+    <t>touch js/lock-selection-survey-customer-card.js</t>
+  </si>
+  <si>
+    <t>&lt;!DOCTYPE html&gt;
+&lt;html lang="en"&gt;
+  &lt;head&gt;
+    &lt;!-- Required meta tags --&gt;
+    &lt;meta charset="UTF-8"&gt;
+    &lt;meta http-equiv="X-UA-Compatible" content="IE=edge"&gt;
+    &lt;meta name="viewport"
+      content="width=device-width, initial-scale=1.0, shrink-to-fit=no"&gt;
+    &lt;!-- Bootstrap v 4.6.0 Style Sheet --&gt;
+    &lt;link rel="stylesheet"
+      href="https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/css/bootstrap.min.css"
+      integrity="sha384-B0vP5xmATw1+K9KRQjQERJvTumQW0nPEzvF6L/Z6nronJ3oUOFUFpCjEUQouq2+l"
+      crossorigin="anonymous"&gt;
+    &lt;!-- Custom Styles CSS --&gt;
+    &lt;link rel="stylesheet" type="text/css"
+      href="./../css/lock-selection-survey.css"&gt;
+    &lt;!-- Font Awesome Kit --&gt;
+    &lt;script src="https://kit.fontawesome.com/94f1334f9a.js"
+      crossorigin="anonymous"&gt;&lt;/script&gt;
+    &lt;!-- Google Fonts --&gt;
+    &lt;link rel="preconnect" href="https://fonts.googleapis.com"&gt;
+    &lt;link rel="preconnect" href="https://fonts.gstatic.com" crossorigin&gt;
+    &lt;link
+      href="https://fonts.googleapis.com/css2?family=Noto+Sans+JP&amp;display=swap"
+      rel="stylesheet"&gt;
+      &lt;!-- Favicon --&gt;
+    &lt;link rel="shortcut icon" type="image/ico"
+      href="./../favicon/favicon.ico" /&gt;
+      &lt;!-- Page Title --&gt;
+    &lt;title&gt;Lock Selection Survey&lt;/title&gt;
+  &lt;/head&gt;
+  &lt;body&gt;
+    &lt;!-- Main container --&gt;
+    &lt;div class="container"&gt;
+      &lt;!-- Page Heading --&gt;
+      &lt;div id="survey-heading"&gt;
+        &lt;h1&gt;Lock Selection Survey&lt;/h1&gt;
+        &lt;h2&gt;Lorem Ipsum&lt;/h2&gt;
+        &lt;!-- Start Status Message --&gt;
+        &lt;div id="status" class="status-hidden"&gt;
+          &lt;p class="normal-severity status-message"&gt;Placeholder text&lt;/p&gt;
+        &lt;/div&gt;
+        &lt;!-- End Status Message --&gt;
+      &lt;/div&gt;
+      &lt;!-- End Page Heading --&gt;
+      &lt;!-- Page Body --&gt;
+      &lt;div id="survey-body"&gt;
+        &lt;!-- Capture Customer Details --&gt;
+        &lt;div id="customer-information-capture" class="flex-component"&gt;
+          &lt;!-- Card 1 --&gt;
+          &lt;div id="card-1" class="bg-white rounded-lg shadow"&gt;
+            &lt;!-- Card Heading --&gt;
+            &lt;div class="card-heading"&gt;
+              &lt;h3&gt;Customer Information&lt;/h3&gt;
+            &lt;/div&gt;
+            &lt;!-- End Card Heading --&gt;
+            &lt;!-- Card Body --&gt;
+            &lt;div class="card-body"&gt;
+              &lt;!-- Customer Name Field --&gt;
+              &lt;div id="customer-name-div" class="input-group form-group"&gt;
+                &lt;div class="input-group-prepend"&gt;
+                  &lt;span class="input-group-text"&gt;&lt;i
+                      class="fas fa-user"&gt;&lt;/i&gt;&lt;/span&gt;
+                &lt;/div&gt;
+                &lt;input id="input-customer-name" type="text" class="form-control"
+                  placeholder="Customer name" required&gt;
+                &lt;div class="invalid-feedback"&gt;Customer name cannot be blank.
+                &lt;/div&gt;
+              &lt;/div&gt;
+              &lt;!-- End Customer Name Field --&gt;
+              &lt;!-- Customer Mobile No. --&gt;
+              &lt;div id="customer-mobile-div" class="input-group form-group"&gt;
+                &lt;div class="input-group-prepend"&gt;
+                  &lt;span class="input-group-text"&gt;&lt;i
+                      class="fas fa-mobile"&gt;&lt;/i&gt;&lt;/span&gt;
+                &lt;/div&gt;
+                &lt;input id="input-customer-mobile" type="text"
+                  class="form-control" placeholder="Mobile No. (10 digit)"
+                  required&gt;
+                &lt;div class="invalid-feedback"&gt;Mobile number cannot be blank.
+                &lt;/div&gt;
+              &lt;/div&gt;
+              &lt;!-- End Customer Mobile No. --&gt;
+              &lt;!-- Customer Address - Line 1 --&gt;
+              &lt;div id="customer-address1-div" class="input-group form-group"&gt;
+                &lt;div class="input-group-prepend"&gt;
+                  &lt;span class="input-group-text"&gt;&lt;i
+                      class="fas fa-building"&gt;&lt;/i&gt;&lt;/span&gt;
+                &lt;/div&gt;
+                &lt;input id="input-customer-address1" type="text"
+                  class="form-control" placeholder="Customer Address - Line 1"
+                  required&gt;
+                &lt;div class="invalid-feedback"&gt;Address cannot be blank.&lt;/div&gt;
+              &lt;/div&gt;
+              &lt;!-- End Customer Address - Line 1 --&gt;
+              &lt;!-- Customer Address - Line 2 --&gt;
+              &lt;div id="customer-address2-div"
+                class="input-group form-group optional"&gt;
+                &lt;div class="input-group-prepend"&gt;
+                  &lt;span class="input-group-text"&gt;&lt;i
+                      class="fas fa-building"&gt;&lt;/i&gt;&lt;/span&gt;
+                &lt;/div&gt;
+                &lt;input id="input-customer-address2" type="text"
+                  class="form-control" placeholder="Customer Address - Line 2"&gt;
+                &lt;div class="invalid-feedback"&gt;Address Line 2 cannot contain more
+                  than 50 characters.&lt;/div&gt;
+              &lt;/div&gt;
+              &lt;!-- End Customer Address - Line 2 --&gt;
+              &lt;!-- Customer Address - Line 3 --&gt;
+              &lt;div id="customer-address3-div"
+                class="input-group form-group optional"&gt;
+                &lt;div class="input-group-prepend"&gt;
+                  &lt;span class="input-group-text"&gt;&lt;i
+                      class="fas fa-building"&gt;&lt;/i&gt;&lt;/span&gt;
+                &lt;/div&gt;
+                &lt;input id="input-customer-address3" type="text"
+                  class="form-control" placeholder="Customer Address - Line 3"&gt;
+                &lt;div class="invalid-feedback"&gt;Address Line 3 cannot contain more
+                  than 50 characters.&lt;/div&gt;
+              &lt;/div&gt;
+              &lt;!-- End Customer Address - Line 3 --&gt;
+            &lt;/div&gt;
+            &lt;!-- Card Body --&gt;
+            &lt;!-- Card Footer --&gt;
+            &lt;div class="card-footer text-center"&gt;
+              &lt;input id="customer-previous" class="btn btn-primary"
+                type="button" value="Previous"&gt;
+              &lt;input id="customer-next" class="btn btn-success" type="button"
+                value="   Next   "&gt;
+            &lt;/div&gt;
+            &lt;!-- Card Footer --&gt;
+          &lt;/div&gt;
+          &lt;!-- End Card 1 --&gt;
+        &lt;/div&gt;
+        &lt;!-- End Capture Customer Details --&gt;
+      &lt;/div&gt;
+      &lt;!-- End Page Body --&gt;
+    &lt;/div&gt;
+    &lt;!-- End Main container --&gt;
+    &lt;!-- Bootstrap v 4.6.0 javascript --&gt;
+    &lt;script src="https://code.jquery.com/jquery-3.5.1.slim.min.js"
+      integrity="sha384-DfXdz2htPH0lsSSs5nCTpuj/zy4C+OGpamoFVy38MVBnE+IbbVYUew+OrCXaRkfj"
+      crossorigin="anonymous"&gt;
+    &lt;/script&gt;
+    &lt;script
+      src="https://cdn.jsdelivr.net/npm/popper.js@1.16.1/dist/umd/popper.min.js"
+      integrity="sha384-9/reFTGAW83EW2RDu2S0VKaIzap3H66lZH81PoYlFhbGU+6BZp6G7niu735Sk7lN"
+      crossorigin="anonymous"&gt;
+    &lt;/script&gt;
+    &lt;script
+      src="https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/js/bootstrap.min.js"
+      integrity="sha384-+YQ4JLhjyBLPDQt//I+STsc9iw4uQqACwlvpslubQzn4u2UU2UFM80nGisd026JF"
+      crossorigin="anonymous"&gt;
+    &lt;/script&gt;
+    &lt;!-- Information Capture Javascript --&gt;
+    &lt;script src="https://apis.google.com/js/api.js"&gt;&lt;/script&gt;
+    &lt;script src="./../js/lock-selection-survey-customer-card.js" type="text/javascript"&gt;
+    &lt;/script&gt;
+  &lt;/body&gt;
+&lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>"use strict";
+/* * JavaScript for the file lock-selection-survey.html - customer card
+ *  section.
+ *  @author Sanket Rajgarhia
+ *  @date   31/03/2022 (dd/mm/yyyy)
+ *  @version 1.0
+ * */
+/*****************************************************************************/
+/* GLOBAL CONSTANTS                                                          */
+/*****************************************************************************/
+// A constant value to be used as a css class name for determining if an input 
+// control received an invalid input which it is holding in its placeholder 
+// property
+const SWAP_VALUE = "swapValue";
+/*****************************************************************************/
+/* GLOBAL VARIABLES                                                          */
+/*****************************************************************************/
+// Global variables - associated with the - Customer Name input control
+let customerNameInputPlaceholder = "";
+let customerNameDiv = document.getElementById("customer-name-div");
+let customerNameInput = document.getElementById("input-customer-name");
+let customerNameInvalidFeedback = customerNameDiv
+    .getElementsByClassName("invalid-feedback")[0];
+let customerNamePrependDiv = customerNameDiv
+    .getElementsByClassName("input-group-prepend")[0];
+let customerNameInputGroupTextDiv = customerNameDiv
+    .getElementsByClassName("input-group-text")[0];
+// Global variables - associated with the - Customer Mobile input control
+let customerMobileInputPlaceholder = "";
+let customerMobileDiv = document.getElementById("customer-mobile-div");
+let customerMobileInput = document.getElementById("input-customer-mobile");
+let customerMobileInvalidFeedback = customerMobileDiv
+    .getElementsByClassName("invalid-feedback")[0];
+let customerMobilePrependDiv = customerMobileDiv
+    .getElementsByClassName("input-group-prepend")[0];
+let customerMobileInputGroupTextDiv = customerMobileDiv
+    .getElementsByClassName("input-group-text")[0];
+// Global variables - associated with the - Customer Address1 input control
+let customerAddress1InputPlaceholder = "";
+let customerAddress1Div = document.getElementById("customer-address1-div");
+let customerAddress1Input = document.getElementById("input-customer-address1");
+let customerAddress1InvalidFeedback = customerAddress1Div
+    .getElementsByClassName("invalid-feedback")[0];
+let customerAddress1PrependDiv = customerAddress1Div
+    .getElementsByClassName("input-group-prepend")[0];
+let customerAddress1InputGroupTextDiv = customerAddress1Div
+    .getElementsByClassName("input-group-text")[0];
+// Global variables - associated with the - Customer Address2 input control
+let customerAddress2InputPlaceholder = "";
+let customerAddress2Div = document.getElementById("customer-address2-div");
+let customerAddress2Input = document.getElementById("input-customer-address2");
+let customerAddress2InvalidFeedback = customerAddress2Div
+    .getElementsByClassName("invalid-feedback")[0];
+let customerAddress2PrependDiv = customerAddress2Div
+    .getElementsByClassName("input-group-prepend")[0];
+let customerAddress2InputGroupTextDiv = customerAddress2Div
+    .getElementsByClassName("input-group-text")[0];
+// Global variables - associated with the - Customer Address3 input control
+let customerAddress3InputPlaceholder = "";
+let customerAddress3Div = document.getElementById("customer-address3-div");
+let customerAddress3Input = document.getElementById("input-customer-address3");
+let customerAddress3InvalidFeedback = customerAddress3Div
+    .getElementsByClassName("invalid-feedback")[0];
+let customerAddress3PrependDiv = customerAddress3Div
+    .getElementsByClassName("input-group-prepend")[0];
+let customerAddress3InputGroupTextDiv = customerAddress3Div
+    .getElementsByClassName("input-group-text")[0];
+// Global variables - associated with the - Next button control
+let customerCardNextButton = document.getElementById("customer-next");
+/*****************************************************************************/
+/* WINDOWS ONLOAD                                                            */
+/*****************************************************************************/
+/* Anonymous function fired on window load. 
+ * @param    
+ * @return   
+ * */
+window.onload = function() {
+    // Disable the Next button in Customer Card
+    customerCardNextButton.disabled = true;
+};
+/*****************************************************************************/
+/* EVENT LISTENER - CALLBACKS                                                */
+/*****************************************************************************/
+/* The callback function fired on 'get focus' - for customer 
+ * name input control. 
+ * @param    
+ * @return   
+ * */
+const resetCustomerNameInputOnGetFocus = () =&gt; {
+    // Preserve the original placeholder text - the first time the control 
+    // gets focus.
+    // The customerNameInputPlaceholder variable will be empty - the first time
+    // control gets focus
+    if (customerNameInputPlaceholder.length === 0) {
+        customerNameInputPlaceholder = customerNameInput.placeholder;
+    }
+    // If the customer name input control has the class SWAP_VALUE 
+    // attached - it means that an incorrect value was entered in the field
+    // the last time the control had focus.
+    if (customerNameInput.classList.contains(SWAP_VALUE) === true) {
+        // Remove the class SWAP_VALUE - as the user is preparing to re-enter
+        // a valid value
+        customerNameInput.classList.remove(SWAP_VALUE);
+        // Set the value of the input control to the placeholder value.
+        // The erroneous/invalid value was preserved in the placeholder 
+        // value - the last time input control lost focus.
+        customerNameInput.value = customerNameInput.placeholder;
+        // Set the placeholder value of the input control to the original
+        // placeholder value of the field.
+        customerNameInput.placeholder = customerNameInputPlaceholder;
+        // Select the value set in the input field
+        customerNameInput.select();
+    }
+    // Reset all validation related classes
+    resetValidation(customerNamePrependDiv, customerNameInputGroupTextDiv);
+    // Refresh to original state of the container div
+    customerNameDiv.classList.remove("was-validated");
+}
+/* The callback function fired on 'blur' - for customer name input control.
+ * @param    
+ * @return   
+ * */
+const validateCustomerNameInputOnBlur = () =&gt; {
+    // Check for white spaces
+    if (customerNameInput.value.trim().length === 0) {
+        // White spaces are present - reset the value to be empty
+        customerNameInput.value = "";
+        // Update the invalid feedback message
+        customerNameInvalidFeedback.innerHTML = "Customer name cannot " +
+            "be blank.";
+        invalidateInputControl(customerNamePrependDiv,
+            customerNameInputGroupTextDiv);
+    } // Check for the length of the name to be not more than 50 characters
+    else if (customerNameInput.value.trim().length &gt; 50) {
+        // Update the placeholder to display the erroneous/invalid 
+        // entered value and reset the input value to blank to invalidate the 
+        // input control
+        customerNameInput.placeholder = customerNameInput.value;
+        customerNameInput.value = "";
+        // Update the invalid feedback message
+        customerNameInvalidFeedback.innerHTML = "Name cannot contain more " +
+            "than 50 characters.";
+        // Add the SWAP_VALUE class to the customer name input control
+        customerNameInput.classList.add(SWAP_VALUE);
+        invalidateInputControl(customerNamePrependDiv,
+            customerNameInputGroupTextDiv);
+    } else // Passed all validation checks
+    {
+        validateInputControl(customerNamePrependDiv,
+            customerNameInputGroupTextDiv);
+    }
+    customerNameDiv.classList.add("was-validated");
+    // Enable/Disable the navigation button(s)
+    if (allInputsAreValidated() === true) {
+        customerCardNextButton.disabled = false;
+    } else {
+        customerCardNextButton.disabled = true;
+    }
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implemented the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">js/lock-selection-survey-customer-card.js </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">to validate and style the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">customer card </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html section.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implement the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">js/lock-selection-survey-customer-card.js </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">to validate and style the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>customer card</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> html section.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implement the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/css/lock-selection-survey.css</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to style the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html/lock-selection-survey.html</t>
+    </r>
+  </si>
+  <si>
+    <t>/* * CSS for the file lock-selection-survey.html
+ *  @author Sanket Rajgarhia
+ *  @date   31/03/2022 (dd/mm/yyyy)
+ *  @version 1.0
+ * */
+/*****************************************************************************/
+/* TOP LEVEL TAGS - &lt;html&gt; &lt;header&gt; and &lt;body&gt;                               */
+/*****************************************************************************/
+/* html, header and body tags */
+html,
+header,
+body {
+    background-color: white;
+    font-size: 1rem;
+    font-weight: 400;
+    margin: 30px;
+    min-height: 100vh;
+    padding: 0;
+}
+/*****************************************************************************/
+/* HEADER TAGS - &lt;h1&gt; &lt;h2&gt; and &lt;H3&gt;                                          */
+/*****************************************************************************/
+h1 {
+    background-color: #F1F1F1;
+    font-family: 'Noto Sans JP', sans-serif;
+    font-size: 20px;
+    padding: 15px;
+    text-align: center;
+}
+h2 {
+    color: #080E64;
+    font-family: 'Noto Sans JP', sans-serif;
+    font-size: 18px;
+    padding-bottom: 20px;
+    padding-top: 20px;
+    text-align: center;
+}
+h3 {
+    color:rgb(182, 21, 21);
+    font-family: 'Noto Sans JP', sans-serif;
+    font-size: 16px;
+    font-weight: 900;
+    padding-bottom: 20px;
+    padding-top: 20px;
+    text-align: center;
+}
+/*****************************************************************************/
+/* INPUT TAGS - &lt;input&gt;                                                      */
+/*****************************************************************************/
+input {
+    font-size: calc(10px + (14 - 10) * ((100vw - 500px) / (1200 - 300))) !important;
+}
+/*****************************************************************************/
+/* STATUS MESSAGE (ERROR) DISPLAY &lt;div&gt; AND ASSOCIATED CLASSES               */
+/*****************************************************************************/
+/* Status div */
+#status {
+    position: relative;
+}
+.status-message {
+    text-align: center;
+}
+/* Severity of status (error) message */
+.high-severity {
+    color: rgb(182, 21, 21);
+}
+.normal-severity {
+    color: black;
+}
+.low-severity {
+    color: grey;
+}
+/* Hide and Display the status (error) message display &lt;div&gt; */
+.status-hidden {
+    max-height: 0;
+    opacity: 0;
+    transition: opacity 3000ms, max-height 4000ms ease-out;
+}
+.status-displayed {
+    max-height: 1000px;
+    opacity: 1;
+    transition: max-height 3000ms ease-in, opacity 4000ms;
+}
+/*****************************************************************************/
+/* SURVEY BODY &lt;div&gt; AND ASSOCIATED CLASSES                                  */
+/*****************************************************************************/
+/* survey-body page body &lt;div&gt; */
+#survey-body {
+    display: flex;
+    justify-content: center;
+    flex-grow: 1;
+}
+/* Flex component to layout the cards inside the survey-body &lt;div&gt; */
+.flex-component {
+    flex-basis: 50%;
+    flex-grow: 0;
+    flex-shrink: 0;
+    margin: 25px;
+}
+/*****************************************************************************/
+/* INPUT VALIDATION - AND ASSOCIATED CLASSES                                 */
+/*****************************************************************************/
+.prepend-invalid{
+    background-color: red;
+}
+.prepend-valid{
+    background-color: green;
+}
+/*****************************************************************************/
+/* INPUT PREPEND GROUP TRANSPARENCY CONTROL - AND ASSOCIATED CLASSES         */
+/*****************************************************************************/
+.input-group-text-transparent{
+    opacity: 0.5;
+}
+.input-group-text-opaque{
+    opacity: 1;
+}
+/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implemented the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/css/lock-selection-survey.css</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to style the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html/lock-selection-survey.html</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>git status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - would display the following files.                                                                                                                                                                                                                                          new file:   css/lock-selection-survey.css
+        modified:   docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+        new file:   html/lock-selection-survey.html
+        new file:   js/lock-selection-survey-customer-card.js</t>
+    </r>
+  </si>
+  <si>
+    <t>git commit -m "Creation of html/lock-selection-survey.html and implementation of related js and css for customer information capture."</t>
+  </si>
+  <si>
+    <t>CREATE AND IMPLEMENT THE html/lock-selection-survey.html HTML FILE - CUSTOMER INFORMATION CAPTURE SECTION</t>
   </si>
 </sst>
 </file>
@@ -4307,7 +5580,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4417,6 +5690,18 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4474,19 +5759,16 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4805,7 +6087,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4817,18 +6099,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -5100,8 +6382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB926B8F-5A7D-9B4E-BEE4-06FF437DD437}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5113,18 +6395,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -5175,11 +6457,11 @@
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="63" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="59"/>
-      <c r="C9" s="59"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -5215,20 +6497,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="59" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="61" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="55" t="s">
+      <c r="C13" s="59" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="56"/>
-      <c r="B14" s="58"/>
-      <c r="C14" s="56"/>
+      <c r="A14" s="60"/>
+      <c r="B14" s="62"/>
+      <c r="C14" s="60"/>
     </row>
     <row r="15" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
@@ -5253,20 +6535,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="55" t="s">
+      <c r="A17" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="61" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="55" t="s">
+      <c r="C17" s="59" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="56"/>
-      <c r="B18" s="58"/>
-      <c r="C18" s="56"/>
+      <c r="A18" s="60"/>
+      <c r="B18" s="62"/>
+      <c r="C18" s="60"/>
     </row>
     <row r="19" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -5312,7 +6594,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5324,18 +6606,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="63" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -5371,25 +6653,25 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="59" t="s">
         <v>292</v>
       </c>
-      <c r="B6" s="60" t="s">
+      <c r="B6" s="64" t="s">
         <v>291</v>
       </c>
-      <c r="C6" s="55" t="s">
+      <c r="C6" s="59" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="66"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="66"/>
+      <c r="A7" s="70"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="70"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="56"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="56"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="60"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -5414,25 +6696,25 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="63" t="s">
+      <c r="A11" s="67" t="s">
         <v>294</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="64" t="s">
         <v>295</v>
       </c>
-      <c r="C11" s="63" t="s">
+      <c r="C11" s="67" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="64"/>
-      <c r="B12" s="61"/>
-      <c r="C12" s="64"/>
+      <c r="A12" s="68"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="68"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="65"/>
-      <c r="B13" s="62"/>
-      <c r="C13" s="65"/>
+      <c r="A13" s="69"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="69"/>
     </row>
     <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
@@ -5476,7 +6758,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5ECDD1-7F28-8F45-BB61-7AD00F9ECBDC}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -5489,18 +6771,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="63" t="s">
         <v>299</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -5514,46 +6796,46 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="71" t="s">
         <v>300</v>
       </c>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="75" t="s">
         <v>305</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="71" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="67"/>
-      <c r="B5" s="71"/>
-      <c r="C5" s="67"/>
+      <c r="A5" s="71"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="71"/>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="67"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="67"/>
+      <c r="A6" s="71"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="71"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="59" t="s">
         <v>302</v>
       </c>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="72" t="s">
         <v>303</v>
       </c>
-      <c r="C7" s="55" t="s">
+      <c r="C7" s="59" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="66"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="66"/>
+      <c r="A8" s="70"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="70"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="228" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="56"/>
-      <c r="B9" s="70"/>
-      <c r="C9" s="56"/>
+      <c r="A9" s="60"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="60"/>
     </row>
     <row r="10" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
@@ -5570,7 +6852,7 @@
       <c r="A11" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="53" t="s">
         <v>307</v>
       </c>
       <c r="C11" s="16" t="s">
@@ -5594,6 +6876,353 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D78F71-19B8-4A40-929A-3EEAE507D273}">
+  <dimension ref="A1:C49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="63" t="s">
+        <v>331</v>
+      </c>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>309</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>310</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>321</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="59" t="s">
+        <v>314</v>
+      </c>
+      <c r="B7" s="64" t="s">
+        <v>322</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="70"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="70"/>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="70"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="70"/>
+    </row>
+    <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="70"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="70"/>
+    </row>
+    <row r="11" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="70"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="70"/>
+    </row>
+    <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="70"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="70"/>
+    </row>
+    <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="60"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="60"/>
+    </row>
+    <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="59" t="s">
+        <v>325</v>
+      </c>
+      <c r="B14" s="64" t="s">
+        <v>323</v>
+      </c>
+      <c r="C14" s="59" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="70"/>
+      <c r="B15" s="65"/>
+      <c r="C15" s="70"/>
+    </row>
+    <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="70"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="70"/>
+    </row>
+    <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="70"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="70"/>
+    </row>
+    <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="70"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="70"/>
+    </row>
+    <row r="19" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="70"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="70"/>
+    </row>
+    <row r="20" spans="1:3" ht="155" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="70"/>
+      <c r="B20" s="66"/>
+      <c r="C20" s="70"/>
+    </row>
+    <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="70"/>
+      <c r="B21" s="64" t="s">
+        <v>316</v>
+      </c>
+      <c r="C21" s="70"/>
+    </row>
+    <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="70"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="70"/>
+    </row>
+    <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="70"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="70"/>
+    </row>
+    <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="70"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="70"/>
+    </row>
+    <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="70"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="70"/>
+    </row>
+    <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="70"/>
+      <c r="B26" s="65"/>
+      <c r="C26" s="70"/>
+    </row>
+    <row r="27" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="70"/>
+      <c r="B27" s="66"/>
+      <c r="C27" s="70"/>
+    </row>
+    <row r="28" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="70"/>
+      <c r="B28" s="64" t="s">
+        <v>317</v>
+      </c>
+      <c r="C28" s="70"/>
+    </row>
+    <row r="29" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="70"/>
+      <c r="B29" s="65"/>
+      <c r="C29" s="70"/>
+    </row>
+    <row r="30" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="70"/>
+      <c r="B30" s="65"/>
+      <c r="C30" s="70"/>
+    </row>
+    <row r="31" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="70"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="70"/>
+    </row>
+    <row r="32" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="70"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="70"/>
+    </row>
+    <row r="33" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="70"/>
+      <c r="B33" s="65"/>
+      <c r="C33" s="70"/>
+    </row>
+    <row r="34" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="70"/>
+      <c r="B34" s="65"/>
+      <c r="C34" s="70"/>
+    </row>
+    <row r="35" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="70"/>
+      <c r="B35" s="65"/>
+      <c r="C35" s="70"/>
+    </row>
+    <row r="36" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="70"/>
+      <c r="B36" s="65"/>
+      <c r="C36" s="70"/>
+    </row>
+    <row r="37" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="70"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="70"/>
+    </row>
+    <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="70"/>
+      <c r="B38" s="64" t="s">
+        <v>318</v>
+      </c>
+      <c r="C38" s="70"/>
+    </row>
+    <row r="39" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="70"/>
+      <c r="B39" s="65"/>
+      <c r="C39" s="70"/>
+    </row>
+    <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="70"/>
+      <c r="B40" s="65"/>
+      <c r="C40" s="70"/>
+    </row>
+    <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="70"/>
+      <c r="B41" s="65"/>
+      <c r="C41" s="70"/>
+    </row>
+    <row r="42" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="60"/>
+      <c r="B42" s="66"/>
+      <c r="C42" s="60"/>
+    </row>
+    <row r="43" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="59" t="s">
+        <v>326</v>
+      </c>
+      <c r="B43" s="64" t="s">
+        <v>327</v>
+      </c>
+      <c r="C43" s="59" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="70"/>
+      <c r="B44" s="65"/>
+      <c r="C44" s="70"/>
+    </row>
+    <row r="45" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="70"/>
+      <c r="B45" s="65"/>
+      <c r="C45" s="70"/>
+    </row>
+    <row r="46" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="70"/>
+      <c r="B46" s="65"/>
+      <c r="C46" s="70"/>
+    </row>
+    <row r="47" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="60"/>
+      <c r="B47" s="66"/>
+      <c r="C47" s="60"/>
+    </row>
+    <row r="48" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A48" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A49" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B49" s="53" t="s">
+        <v>330</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="14">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B7:B13"/>
+    <mergeCell ref="A7:A13"/>
+    <mergeCell ref="C7:C13"/>
+    <mergeCell ref="B38:B42"/>
+    <mergeCell ref="A14:A42"/>
+    <mergeCell ref="C14:C42"/>
+    <mergeCell ref="B43:B47"/>
+    <mergeCell ref="A43:A47"/>
+    <mergeCell ref="C43:C47"/>
+    <mergeCell ref="B28:B37"/>
+    <mergeCell ref="B14:B20"/>
+    <mergeCell ref="B21:B27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE113606-3FFA-8545-9BE3-5643B52A7CE9}">
   <dimension ref="A1:H116"/>
   <sheetViews>
@@ -5671,10 +7300,10 @@
       <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="76" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="75"/>
+      <c r="B6" s="76"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -6647,32 +8276,32 @@
       <c r="H73" s="23"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="72"/>
-      <c r="B74" s="76"/>
+      <c r="A74" s="77"/>
+      <c r="B74" s="78"/>
       <c r="C74" s="32" t="s">
         <v>225</v>
       </c>
       <c r="D74" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="E74" s="77"/>
-      <c r="F74" s="72"/>
-      <c r="G74" s="74"/>
-      <c r="H74" s="72"/>
+      <c r="E74" s="79"/>
+      <c r="F74" s="77"/>
+      <c r="G74" s="81"/>
+      <c r="H74" s="77"/>
     </row>
     <row r="75" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A75" s="72"/>
-      <c r="B75" s="76"/>
+      <c r="A75" s="77"/>
+      <c r="B75" s="78"/>
       <c r="C75" s="33" t="s">
         <v>226</v>
       </c>
       <c r="D75" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="E75" s="77"/>
-      <c r="F75" s="72"/>
-      <c r="G75" s="74"/>
-      <c r="H75" s="72"/>
+      <c r="E75" s="79"/>
+      <c r="F75" s="77"/>
+      <c r="G75" s="81"/>
+      <c r="H75" s="77"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="23"/>
@@ -6845,34 +8474,34 @@
       <c r="H88" s="23"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="72"/>
-      <c r="B89" s="72"/>
+      <c r="A89" s="77"/>
+      <c r="B89" s="77"/>
       <c r="C89" s="35" t="s">
         <v>225</v>
       </c>
       <c r="D89" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="E89" s="73" t="s">
+      <c r="E89" s="80" t="s">
         <v>121</v>
       </c>
-      <c r="F89" s="73"/>
-      <c r="G89" s="74"/>
-      <c r="H89" s="72"/>
+      <c r="F89" s="80"/>
+      <c r="G89" s="81"/>
+      <c r="H89" s="77"/>
     </row>
     <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A90" s="72"/>
-      <c r="B90" s="72"/>
+      <c r="A90" s="77"/>
+      <c r="B90" s="77"/>
       <c r="C90" s="35" t="s">
         <v>242</v>
       </c>
       <c r="D90" s="35" t="s">
         <v>243</v>
       </c>
-      <c r="E90" s="73"/>
-      <c r="F90" s="73"/>
-      <c r="G90" s="74"/>
-      <c r="H90" s="72"/>
+      <c r="E90" s="80"/>
+      <c r="F90" s="80"/>
+      <c r="G90" s="81"/>
+      <c r="H90" s="77"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="23"/>
@@ -7240,11 +8869,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F74:F75"/>
     <mergeCell ref="H74:H75"/>
     <mergeCell ref="A89:A90"/>
     <mergeCell ref="B89:B90"/>
@@ -7253,17 +8877,22 @@
     <mergeCell ref="G89:G90"/>
     <mergeCell ref="H89:H90"/>
     <mergeCell ref="G74:G75"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F74:F75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:A15"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7354,4 +8983,132 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0BB7-C151-C94B-945C-E2CA92034B13}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="63" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>279</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="54"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="54"/>
+    </row>
+    <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="54"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="54"/>
+    </row>
+    <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="54"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="54"/>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="56"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="56"/>
+    </row>
+    <row r="12" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="56"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="56"/>
+    </row>
+    <row r="13" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="56"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="56"/>
+    </row>
+    <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
REFACTORED: Project js folder to contain model and controller folders
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26FA078-FE3C-044C-A79B-C24631BEC6E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB78C98E-B80E-3741-8BCC-7EF2837F14BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="1000" windowWidth="27640" windowHeight="16160" activeTab="4" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
+    <workbookView xWindow="300" yWindow="1000" windowWidth="27640" windowHeight="16160" activeTab="5" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="SPEC - 1.1" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="SPEC - 1.3" sheetId="4" r:id="rId3"/>
     <sheet name="SPEC - 1.4" sheetId="7" r:id="rId4"/>
     <sheet name="SPEC - 1.5" sheetId="9" r:id="rId5"/>
-    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId6"/>
-    <sheet name="PLAYGROUND" sheetId="6" r:id="rId7"/>
-    <sheet name="TEMPLATE" sheetId="8" r:id="rId8"/>
+    <sheet name="SPEC - 1.6" sheetId="10" r:id="rId6"/>
+    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId7"/>
+    <sheet name="PLAYGROUND" sheetId="6" r:id="rId8"/>
+    <sheet name="TEMPLATE" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="356">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -5204,6 +5205,535 @@
   </si>
   <si>
     <t>CREATE AND IMPLEMENT THE html/lock-selection-survey.html HTML FILE - CUSTOMER INFORMATION CAPTURE SECTION</t>
+  </si>
+  <si>
+    <t>REFACTOR PROJECT FORDER - ORGANIZE JS SCRIPTS (MODEL AND CONTROLLER)</t>
+  </si>
+  <si>
+    <t>mkdir js/model</t>
+  </si>
+  <si>
+    <t>mv js/door js/model/door</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create the folder </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/model</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ls js </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">will display the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">model </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>directory</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Move the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/door</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> folder into the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> folder</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ls js/model/door/ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">will display the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>door.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> file</t>
+    </r>
+  </si>
+  <si>
+    <t>mv js/customer.js js/model/customer.js</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>ls js/model/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> will display the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">customer.js </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>file</t>
+    </r>
+  </si>
+  <si>
+    <t>mv js/sales.js js/model/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Move file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/customer.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> into the folder </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/model</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Move the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/sales.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> into the folder </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/model</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>ls js/model/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> will display the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">sales.js </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>file</t>
+    </r>
+  </si>
+  <si>
+    <t>mkdir js/controller</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create the folder </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">ls js </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">will display the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>controller</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> directory</t>
+    </r>
+  </si>
+  <si>
+    <t>mv js/lock-selection-survey-customer-card.js js/controller/</t>
+  </si>
+  <si>
+    <r>
+      <t>Move the file</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> js/lock-selection-survey-customer-card.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> into the folder </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller</t>
+    </r>
+  </si>
+  <si>
+    <t>mv js/index.js js/controller/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Move the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>index.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> into the folder </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">ls js/controller/ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">will display the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>index.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> file</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">ls js/controller/ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">will display the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lock-selection-survey-customer-card.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> file</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>git status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - would display the following files.                                                                                                                                                                                                                                   modified:   docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+        modified:   html/lock-selection-survey.html
+        renamed:    js/index.js -&gt; js/controller/index.js
+        renamed:    js/lock-selection-survey-customer-card.js -&gt; js/controller/lock-selection-survey-customer-card.js
+        renamed:    js/customer.js -&gt; js/model/customer.js
+        renamed:    js/door/door.js -&gt; js/model/door/door.js
+        renamed:    js/sales.js -&gt; js/model/sales.js</t>
+    </r>
+  </si>
+  <si>
+    <t>git commit -m "REFACTORED: Project js folder to contain model and controller folders"</t>
   </si>
 </sst>
 </file>
@@ -6879,7 +7409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52D78F71-19B8-4A40-929A-3EEAE507D273}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -7223,6 +7753,156 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC086211-4490-5344-9303-AF96F282E8C7}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="53.5" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="57" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="63" t="s">
+        <v>332</v>
+      </c>
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>333</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>334</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="54" t="s">
+        <v>342</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>339</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="54" t="s">
+        <v>343</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>341</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="54" t="s">
+        <v>346</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>345</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="54" t="s">
+        <v>351</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>350</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>348</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="170" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>355</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE113606-3FFA-8545-9BE3-5643B52A7CE9}">
   <dimension ref="A1:H116"/>
   <sheetViews>
@@ -8887,7 +9567,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -8985,7 +9665,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0BB7-C151-C94B-945C-E2CA92034B13}">
   <dimension ref="A1:C15"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated the Customer class to have the additionalInformation field.
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB78C98E-B80E-3741-8BCC-7EF2837F14BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B2FF8C-641E-9349-98EE-24A815F41878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="1000" windowWidth="27640" windowHeight="16160" activeTab="5" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
+    <workbookView xWindow="300" yWindow="1000" windowWidth="27640" windowHeight="16160" activeTab="6" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="SPEC - 1.1" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,10 @@
     <sheet name="SPEC - 1.4" sheetId="7" r:id="rId4"/>
     <sheet name="SPEC - 1.5" sheetId="9" r:id="rId5"/>
     <sheet name="SPEC - 1.6" sheetId="10" r:id="rId6"/>
-    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId7"/>
-    <sheet name="PLAYGROUND" sheetId="6" r:id="rId8"/>
-    <sheet name="TEMPLATE" sheetId="8" r:id="rId9"/>
+    <sheet name="SPEC - 1.7" sheetId="11" r:id="rId7"/>
+    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId8"/>
+    <sheet name="PLAYGROUND" sheetId="6" r:id="rId9"/>
+    <sheet name="TEMPLATE" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="365">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -5734,6 +5735,196 @@
   </si>
   <si>
     <t>git commit -m "REFACTORED: Project js folder to contain model and controller folders"</t>
+  </si>
+  <si>
+    <t>UPDATE THE CUSTOMER CLASS TO HAVE A FIELD - ADDITIONAL INFORMATION</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    /* *Constructor
+     * @param    {String} customerName          Name of the customer
+     * @param    {String} phoneNumber           10 Digit Phone Number of the customer
+     * @param    {String} address               150 characters address
+     * @param    {String} additionalInformation 250 characters additional information
+     * */
+    constructor(customerName, phoneNumber, address, additionalInformation) {
+        this._customerName = customerName;
+        this._phoneNumber = phoneNumber;
+        this._address = address;
+        this._additionalInformation = additionalInformation;
+    }</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>constructo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">r of the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Custome</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>r class to have the additional information field.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>constructo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">r of the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Custome</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>r class to have the additional information field.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">    /* Get the additional information
+     * @return  {String} Additional information
+     */
+    get additionalInformation() {
+        return this._additionalInformation;
+    }
+    /* Set the additional information
+     * @param   {String} additionalInformation  250 characters additional information
+     */
+    set additionalInformation(additionalInformation) {
+        this._additionalInformation = additionalInformation;
+    }</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implement the getter and setter methods for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>additionalInformation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> field</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implemented the getter and setter methods for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>additionalInformation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> field</t>
+    </r>
+  </si>
+  <si>
+    <t>git commit -m "Updated the Customer class to have the additionalInformation field."</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>git status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - would display the following files.                                                                                                                                                                                                                                          modified:   docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+        modified:   js/model/customer.js</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -6110,7 +6301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6231,6 +6422,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -6629,18 +6826,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -6904,6 +7101,134 @@
   <hyperlinks>
     <hyperlink ref="B19" r:id="rId1" xr:uid="{82A47956-2C1F-B942-93C6-EE56AEAFA3A5}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0BB7-C151-C94B-945C-E2CA92034B13}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="65" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>279</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="54"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="54"/>
+    </row>
+    <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="54"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="54"/>
+    </row>
+    <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="54"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="54"/>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="56"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="56"/>
+    </row>
+    <row r="12" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="56"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="56"/>
+    </row>
+    <row r="13" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="56"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="56"/>
+    </row>
+    <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6925,18 +7250,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -6987,11 +7312,11 @@
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="65" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="63"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="65"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -7027,20 +7352,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="59" t="s">
+      <c r="A13" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="61" t="s">
+      <c r="B13" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="59" t="s">
+      <c r="C13" s="61" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="60"/>
-      <c r="B14" s="62"/>
-      <c r="C14" s="60"/>
+      <c r="A14" s="62"/>
+      <c r="B14" s="64"/>
+      <c r="C14" s="62"/>
     </row>
     <row r="15" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
@@ -7065,20 +7390,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="61" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="61" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="60"/>
-      <c r="B18" s="62"/>
-      <c r="C18" s="60"/>
+      <c r="A18" s="62"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="62"/>
     </row>
     <row r="19" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -7136,18 +7461,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="65" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -7183,25 +7508,25 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="61" t="s">
         <v>292</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="66" t="s">
         <v>291</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="61" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="70"/>
-      <c r="B7" s="65"/>
-      <c r="C7" s="70"/>
+      <c r="A7" s="72"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="72"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="60"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="60"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="62"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -7226,25 +7551,25 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="67" t="s">
+      <c r="A11" s="69" t="s">
         <v>294</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="66" t="s">
         <v>295</v>
       </c>
-      <c r="C11" s="67" t="s">
+      <c r="C11" s="69" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="68"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="68"/>
+      <c r="A12" s="70"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="70"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="69"/>
-      <c r="B13" s="66"/>
-      <c r="C13" s="69"/>
+      <c r="A13" s="71"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="71"/>
     </row>
     <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
@@ -7301,18 +7626,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="65" t="s">
         <v>299</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -7326,46 +7651,46 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="71" t="s">
+      <c r="A4" s="73" t="s">
         <v>300</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="77" t="s">
         <v>305</v>
       </c>
-      <c r="C4" s="71" t="s">
+      <c r="C4" s="73" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="71"/>
-      <c r="B5" s="75"/>
-      <c r="C5" s="71"/>
+      <c r="A5" s="73"/>
+      <c r="B5" s="77"/>
+      <c r="C5" s="73"/>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="71"/>
-      <c r="B6" s="75"/>
-      <c r="C6" s="71"/>
+      <c r="A6" s="73"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="73"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="61" t="s">
         <v>302</v>
       </c>
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="74" t="s">
         <v>303</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="61" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="70"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="70"/>
+      <c r="A8" s="72"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="72"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="228" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="60"/>
-      <c r="B9" s="74"/>
-      <c r="C9" s="60"/>
+      <c r="A9" s="62"/>
+      <c r="B9" s="76"/>
+      <c r="C9" s="62"/>
     </row>
     <row r="10" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
@@ -7422,18 +7747,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="65" t="s">
         <v>331</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -7480,233 +7805,233 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="61" t="s">
         <v>314</v>
       </c>
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="66" t="s">
         <v>322</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="61" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="70"/>
-      <c r="B8" s="65"/>
-      <c r="C8" s="70"/>
+      <c r="A8" s="72"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="72"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="70"/>
-      <c r="B9" s="65"/>
-      <c r="C9" s="70"/>
+      <c r="A9" s="72"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="72"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="70"/>
-      <c r="B10" s="65"/>
-      <c r="C10" s="70"/>
+      <c r="A10" s="72"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="72"/>
     </row>
     <row r="11" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="70"/>
-      <c r="B11" s="65"/>
-      <c r="C11" s="70"/>
+      <c r="A11" s="72"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="72"/>
     </row>
     <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="70"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="70"/>
+      <c r="A12" s="72"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="72"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="60"/>
-      <c r="B13" s="66"/>
-      <c r="C13" s="60"/>
+      <c r="A13" s="62"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="62"/>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="59" t="s">
+      <c r="A14" s="61" t="s">
         <v>325</v>
       </c>
-      <c r="B14" s="64" t="s">
+      <c r="B14" s="66" t="s">
         <v>323</v>
       </c>
-      <c r="C14" s="59" t="s">
+      <c r="C14" s="61" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="70"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="70"/>
+      <c r="A15" s="72"/>
+      <c r="B15" s="67"/>
+      <c r="C15" s="72"/>
     </row>
     <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="70"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="70"/>
+      <c r="A16" s="72"/>
+      <c r="B16" s="67"/>
+      <c r="C16" s="72"/>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="70"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="70"/>
+      <c r="A17" s="72"/>
+      <c r="B17" s="67"/>
+      <c r="C17" s="72"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="70"/>
-      <c r="B18" s="65"/>
-      <c r="C18" s="70"/>
+      <c r="A18" s="72"/>
+      <c r="B18" s="67"/>
+      <c r="C18" s="72"/>
     </row>
     <row r="19" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="70"/>
-      <c r="B19" s="65"/>
-      <c r="C19" s="70"/>
+      <c r="A19" s="72"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="72"/>
     </row>
     <row r="20" spans="1:3" ht="155" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="70"/>
-      <c r="B20" s="66"/>
-      <c r="C20" s="70"/>
+      <c r="A20" s="72"/>
+      <c r="B20" s="68"/>
+      <c r="C20" s="72"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="70"/>
-      <c r="B21" s="64" t="s">
+      <c r="A21" s="72"/>
+      <c r="B21" s="66" t="s">
         <v>316</v>
       </c>
-      <c r="C21" s="70"/>
+      <c r="C21" s="72"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="70"/>
-      <c r="B22" s="65"/>
-      <c r="C22" s="70"/>
+      <c r="A22" s="72"/>
+      <c r="B22" s="67"/>
+      <c r="C22" s="72"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="70"/>
-      <c r="B23" s="65"/>
-      <c r="C23" s="70"/>
+      <c r="A23" s="72"/>
+      <c r="B23" s="67"/>
+      <c r="C23" s="72"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="70"/>
-      <c r="B24" s="65"/>
-      <c r="C24" s="70"/>
+      <c r="A24" s="72"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="72"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="70"/>
-      <c r="B25" s="65"/>
-      <c r="C25" s="70"/>
+      <c r="A25" s="72"/>
+      <c r="B25" s="67"/>
+      <c r="C25" s="72"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="70"/>
-      <c r="B26" s="65"/>
-      <c r="C26" s="70"/>
+      <c r="A26" s="72"/>
+      <c r="B26" s="67"/>
+      <c r="C26" s="72"/>
     </row>
     <row r="27" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="70"/>
-      <c r="B27" s="66"/>
-      <c r="C27" s="70"/>
+      <c r="A27" s="72"/>
+      <c r="B27" s="68"/>
+      <c r="C27" s="72"/>
     </row>
     <row r="28" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="70"/>
-      <c r="B28" s="64" t="s">
+      <c r="A28" s="72"/>
+      <c r="B28" s="66" t="s">
         <v>317</v>
       </c>
-      <c r="C28" s="70"/>
+      <c r="C28" s="72"/>
     </row>
     <row r="29" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="70"/>
-      <c r="B29" s="65"/>
-      <c r="C29" s="70"/>
+      <c r="A29" s="72"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="72"/>
     </row>
     <row r="30" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="70"/>
-      <c r="B30" s="65"/>
-      <c r="C30" s="70"/>
+      <c r="A30" s="72"/>
+      <c r="B30" s="67"/>
+      <c r="C30" s="72"/>
     </row>
     <row r="31" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="70"/>
-      <c r="B31" s="65"/>
-      <c r="C31" s="70"/>
+      <c r="A31" s="72"/>
+      <c r="B31" s="67"/>
+      <c r="C31" s="72"/>
     </row>
     <row r="32" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="70"/>
-      <c r="B32" s="65"/>
-      <c r="C32" s="70"/>
+      <c r="A32" s="72"/>
+      <c r="B32" s="67"/>
+      <c r="C32" s="72"/>
     </row>
     <row r="33" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="70"/>
-      <c r="B33" s="65"/>
-      <c r="C33" s="70"/>
+      <c r="A33" s="72"/>
+      <c r="B33" s="67"/>
+      <c r="C33" s="72"/>
     </row>
     <row r="34" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="70"/>
-      <c r="B34" s="65"/>
-      <c r="C34" s="70"/>
+      <c r="A34" s="72"/>
+      <c r="B34" s="67"/>
+      <c r="C34" s="72"/>
     </row>
     <row r="35" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="70"/>
-      <c r="B35" s="65"/>
-      <c r="C35" s="70"/>
+      <c r="A35" s="72"/>
+      <c r="B35" s="67"/>
+      <c r="C35" s="72"/>
     </row>
     <row r="36" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="70"/>
-      <c r="B36" s="65"/>
-      <c r="C36" s="70"/>
+      <c r="A36" s="72"/>
+      <c r="B36" s="67"/>
+      <c r="C36" s="72"/>
     </row>
     <row r="37" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="70"/>
-      <c r="B37" s="66"/>
-      <c r="C37" s="70"/>
+      <c r="A37" s="72"/>
+      <c r="B37" s="68"/>
+      <c r="C37" s="72"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="70"/>
-      <c r="B38" s="64" t="s">
+      <c r="A38" s="72"/>
+      <c r="B38" s="66" t="s">
         <v>318</v>
       </c>
-      <c r="C38" s="70"/>
+      <c r="C38" s="72"/>
     </row>
     <row r="39" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="70"/>
-      <c r="B39" s="65"/>
-      <c r="C39" s="70"/>
+      <c r="A39" s="72"/>
+      <c r="B39" s="67"/>
+      <c r="C39" s="72"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="70"/>
-      <c r="B40" s="65"/>
-      <c r="C40" s="70"/>
+      <c r="A40" s="72"/>
+      <c r="B40" s="67"/>
+      <c r="C40" s="72"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="70"/>
-      <c r="B41" s="65"/>
-      <c r="C41" s="70"/>
+      <c r="A41" s="72"/>
+      <c r="B41" s="67"/>
+      <c r="C41" s="72"/>
     </row>
     <row r="42" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="60"/>
-      <c r="B42" s="66"/>
-      <c r="C42" s="60"/>
+      <c r="A42" s="62"/>
+      <c r="B42" s="68"/>
+      <c r="C42" s="62"/>
     </row>
     <row r="43" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="59" t="s">
+      <c r="A43" s="61" t="s">
         <v>326</v>
       </c>
-      <c r="B43" s="64" t="s">
+      <c r="B43" s="66" t="s">
         <v>327</v>
       </c>
-      <c r="C43" s="59" t="s">
+      <c r="C43" s="61" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="70"/>
-      <c r="B44" s="65"/>
-      <c r="C44" s="70"/>
+      <c r="A44" s="72"/>
+      <c r="B44" s="67"/>
+      <c r="C44" s="72"/>
     </row>
     <row r="45" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="70"/>
-      <c r="B45" s="65"/>
-      <c r="C45" s="70"/>
+      <c r="A45" s="72"/>
+      <c r="B45" s="67"/>
+      <c r="C45" s="72"/>
     </row>
     <row r="46" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="70"/>
-      <c r="B46" s="65"/>
-      <c r="C46" s="70"/>
+      <c r="A46" s="72"/>
+      <c r="B46" s="67"/>
+      <c r="C46" s="72"/>
     </row>
     <row r="47" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="60"/>
-      <c r="B47" s="66"/>
-      <c r="C47" s="60"/>
+      <c r="A47" s="62"/>
+      <c r="B47" s="68"/>
+      <c r="C47" s="62"/>
     </row>
     <row r="48" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
@@ -7756,7 +8081,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC086211-4490-5344-9303-AF96F282E8C7}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -7769,18 +8094,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="65" t="s">
         <v>332</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -7903,6 +8228,101 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4431450A-9C71-854E-855D-098E661E41E5}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="59" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="65" t="s">
+        <v>356</v>
+      </c>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="238" x14ac:dyDescent="0.2">
+      <c r="A4" s="57" t="s">
+        <v>358</v>
+      </c>
+      <c r="B4" s="58" t="s">
+        <v>357</v>
+      </c>
+      <c r="C4" s="57" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="221" x14ac:dyDescent="0.2">
+      <c r="A5" s="57" t="s">
+        <v>361</v>
+      </c>
+      <c r="B5" s="58" t="s">
+        <v>360</v>
+      </c>
+      <c r="C5" s="57" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE113606-3FFA-8545-9BE3-5643B52A7CE9}">
   <dimension ref="A1:H116"/>
   <sheetViews>
@@ -7980,10 +8400,10 @@
       <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="76" t="s">
+      <c r="A6" s="78" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="76"/>
+      <c r="B6" s="78"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -8956,32 +9376,32 @@
       <c r="H73" s="23"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="77"/>
-      <c r="B74" s="78"/>
+      <c r="A74" s="79"/>
+      <c r="B74" s="80"/>
       <c r="C74" s="32" t="s">
         <v>225</v>
       </c>
       <c r="D74" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="E74" s="79"/>
-      <c r="F74" s="77"/>
-      <c r="G74" s="81"/>
-      <c r="H74" s="77"/>
+      <c r="E74" s="81"/>
+      <c r="F74" s="79"/>
+      <c r="G74" s="83"/>
+      <c r="H74" s="79"/>
     </row>
     <row r="75" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A75" s="77"/>
-      <c r="B75" s="78"/>
+      <c r="A75" s="79"/>
+      <c r="B75" s="80"/>
       <c r="C75" s="33" t="s">
         <v>226</v>
       </c>
       <c r="D75" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="E75" s="79"/>
-      <c r="F75" s="77"/>
-      <c r="G75" s="81"/>
-      <c r="H75" s="77"/>
+      <c r="E75" s="81"/>
+      <c r="F75" s="79"/>
+      <c r="G75" s="83"/>
+      <c r="H75" s="79"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="23"/>
@@ -9154,34 +9574,34 @@
       <c r="H88" s="23"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="77"/>
-      <c r="B89" s="77"/>
+      <c r="A89" s="79"/>
+      <c r="B89" s="79"/>
       <c r="C89" s="35" t="s">
         <v>225</v>
       </c>
       <c r="D89" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="E89" s="80" t="s">
+      <c r="E89" s="82" t="s">
         <v>121</v>
       </c>
-      <c r="F89" s="80"/>
-      <c r="G89" s="81"/>
-      <c r="H89" s="77"/>
+      <c r="F89" s="82"/>
+      <c r="G89" s="83"/>
+      <c r="H89" s="79"/>
     </row>
     <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A90" s="77"/>
-      <c r="B90" s="77"/>
+      <c r="A90" s="79"/>
+      <c r="B90" s="79"/>
       <c r="C90" s="35" t="s">
         <v>242</v>
       </c>
       <c r="D90" s="35" t="s">
         <v>243</v>
       </c>
-      <c r="E90" s="80"/>
-      <c r="F90" s="80"/>
-      <c r="G90" s="81"/>
-      <c r="H90" s="77"/>
+      <c r="E90" s="82"/>
+      <c r="F90" s="82"/>
+      <c r="G90" s="83"/>
+      <c r="H90" s="79"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="23"/>
@@ -9567,7 +9987,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -9663,132 +10083,4 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0BB7-C151-C94B-945C-E2CA92034B13}">
-  <dimension ref="A1:C15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="57" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-    </row>
-    <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="63" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-    </row>
-    <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="B4" s="48" t="s">
-        <v>279</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
-      <c r="C6" s="54"/>
-    </row>
-    <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="54"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="54"/>
-    </row>
-    <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="54"/>
-      <c r="B8" s="55"/>
-      <c r="C8" s="54"/>
-    </row>
-    <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="56"/>
-      <c r="B11" s="55"/>
-      <c r="C11" s="56"/>
-    </row>
-    <row r="12" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="56"/>
-      <c r="B12" s="55"/>
-      <c r="C12" s="56"/>
-    </row>
-    <row r="13" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="56"/>
-      <c r="B13" s="55"/>
-      <c r="C13" s="56"/>
-    </row>
-    <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>298</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the  html/lock-selection-survey.html file and associated js file to accomodate the Additional Information field.
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B2FF8C-641E-9349-98EE-24A815F41878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D3EC0F-590E-B04A-85C1-BCBD6DD0F136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="1000" windowWidth="27640" windowHeight="16160" activeTab="6" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
+    <workbookView xWindow="300" yWindow="1000" windowWidth="27640" windowHeight="16160" activeTab="7" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="SPEC - 1.1" sheetId="1" r:id="rId1"/>
@@ -20,9 +20,10 @@
     <sheet name="SPEC - 1.5" sheetId="9" r:id="rId5"/>
     <sheet name="SPEC - 1.6" sheetId="10" r:id="rId6"/>
     <sheet name="SPEC - 1.7" sheetId="11" r:id="rId7"/>
-    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId8"/>
-    <sheet name="PLAYGROUND" sheetId="6" r:id="rId9"/>
-    <sheet name="TEMPLATE" sheetId="8" r:id="rId10"/>
+    <sheet name="SPEC - 1.8" sheetId="12" r:id="rId8"/>
+    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId9"/>
+    <sheet name="PLAYGROUND" sheetId="6" r:id="rId10"/>
+    <sheet name="TEMPLATE" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="386">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -5926,12 +5927,824 @@
         modified:   js/model/customer.js</t>
     </r>
   </si>
+  <si>
+    <t>UPDATE THE lock-selection-survey.html AND ASSOCIATED FILES TO ACCOMMODATE THE Additional Information FIELD</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">lock-selection-survey.html </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>to</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>accommodate the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Additional Information </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>field</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">              &lt;!-- Customer Additional Information --&gt;
+              &lt;div id="customer-info-div"
+                class="input-group form-group optional"&gt;
+                &lt;div class="input-group-prepend"&gt;
+                  &lt;span class="input-group-text"&gt;&lt;i
+                      class="fa fa-info"&gt;&lt;/i&gt;&lt;/span&gt;
+                &lt;/div&gt;
+                &lt;textarea id="input-customer-info" class="form-control"
+                  placeholder="Additional Information" rows="5" cols="50"
+                  maxlength="250"&gt;&lt;/textarea&gt;
+                &lt;div class="invalid-feedback"&gt;Additional Information cannot
+                  contain more
+                  than 250 characters.&lt;/div&gt;
+              &lt;/div&gt;
+              &lt;!-- End Customer Additional Information --&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">lock-selection-survey.html </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>to</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>accommodate the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Additional Information </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>field</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">js/controller/lock-selection-survey-customer-card.js </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - add the required global variables</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">js/controller/lock-selection-survey-customer-card.js </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - added the required global variables</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">js/controller/lock-selection-survey-customer-card.js </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - add the required event listeners</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">// Global variables - associated with the - Customer Address3 input control
+let customerAddress3InputPlaceholder = "";
+let customerAddress3Div = document.getElementById("customer-address3-div");
+let customerAddress3Input = document.getElementById("input-customer-address3");
+let customerAddress3InvalidFeedback = customerAddress3Div
+    .getElementsByClassName("invalid-feedback")[0];
+let customerAddress3PrependDiv = customerAddress3Div
+    .getElementsByClassName("input-group-prepend")[0];
+let customerAddress3InputGroupTextDiv = customerAddress3Div
+    .getElementsByClassName("input-group-text")[0];
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+// Global variables - associated with the - Customer Information input control
+let customerInformationTextAreaPlaceholder = "";
+let customerInformationDiv = document.getElementById("customer-info-div");
+let customerInformationTextArea = document.getElementById("input-customer-info");
+let customerInformationInvalidFeedback = customerInformationDiv
+    .getElementsByClassName("invalid-feedback")[0];
+let customerInformationPrependDiv = customerInformationDiv
+    .getElementsByClassName("input-group-prepend")[0];
+let customerInformationTextAreaGroupTextDiv = customerInformationDiv
+    .getElementsByClassName("input-group-text")[0];
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+// Global variables - associated with the - Next button control
+let customerCardNextButton = document.getElementById("customer-next");
+/*****************************************************************************/
+/* WINDOWS ONLOAD                                                            */
+/*****************************************************************************/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">// Event listeners registered for the Customer Information text area control
+customerInformationTextArea.addEventListener("blur",
+    validateCustomerInformationTextAreaOnBlur);
+customerInformationTextArea.addEventListener("focus",
+    resetCustomerInformationTextAreaOnGetFocus);
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">js/controller/lock-selection-survey-customer-card.js </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - add the required event listeners</t>
+    </r>
+  </si>
+  <si>
+    <t>/* The callback function fired on 'get focus' - for customer 
+ * Information textarea control.
+ * @param    
+ * @return   
+ * */
+const resetCustomerInformationTextAreaOnGetFocus = () =&gt; {
+    // Remove the required attribute - if present
+    customerInformationTextArea.removeAttribute("required", "");
+    // Preserve the original placeholder text - the first time the control 
+    // gets focus.
+    // The customerInformationTextAreaPlaceholder variable will be empty 
+    // the first time control gets focus
+    if (customerInformationTextAreaPlaceholder.length === 0) {
+        customerInformationTextAreaPlaceholder = customerInformationTextArea
+            .placeholder;
+    }
+    // If the customer Information TextArea control has the class SWAP_VALUE 
+    // attached - it means that an incorrect value was entered in the field
+    // the last time the control had focus.
+    if (customerInformationTextArea.classList.contains(SWAP_VALUE) === true) {
+        // Remove the class SWAP_VALUE - as the user is preparing to re-enter
+        // a valid value
+        customerInformationTextArea.classList.remove(SWAP_VALUE);
+        // Set the value of the textarea control to the placeholder value.
+        // The erroneous/invalid value was preserved in the placeholder 
+        // value - the last time textarea control lost focus.
+        customerInformationTextArea.value = customerInformationTextArea
+            .placeholder;
+        // Set the placeholder value of the textarea control to the original
+        // placeholder value of the field.
+        customerInformationTextArea.placeholder =
+            customerInformationTextAreaPlaceholder;
+        // Select the value set in the textarea field
+        customerInformationTextArea.select();
+    }
+    // Reset all validation related classes
+    resetValidation(customerInformationPrependDiv,
+        customerInformationTextAreaGroupTextDiv);
+    // Refresh to original state of the container div
+    customerInformationDiv.classList.remove("was-validated");
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implement the callback function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>resetCustomerInformationTextAreaOnGetFocus()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller/lock-selection-survey-customer-card.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implemented the callback function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>resetCustomerInformationTextAreaOnGetFocus()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller/lock-selection-survey-customer-card.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implement the callback function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>validateCustomerInformationTextAreaOnBlur()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller/lock-selection-survey-customer-card.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implemented the callback function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>validateCustomerInformationTextAreaOnBlur()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller/lock-selection-survey-customer-card.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the validation function - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>allInputsAreValidated()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller/lock-selection-survey-customer-card.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to incorporate conditions for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>textarea</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> control</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the validation function - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>allInputsAreValidated()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller/lock-selection-survey-customer-card.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to incorporate conditions for the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>textarea</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> control</t>
+    </r>
+  </si>
+  <si>
+    <t>git commit -m "Updated the  html/lock-selection-survey.html file and associated js file to accomodate the Additional Information field."</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">/* Helper function to check if all input fields are validated.
+ * @param  
+ * @return {boolean}    true if all fields are validated - false otherwise  
+ * */
+const allInputsAreValidated = () =&gt; {
+    // Flag to check if all input fields were validated
+    let allFieldsAreValidated = false;
+    // Get all the div elements which have the class "input-group"
+    let allInputContainerDivElements = document
+        .getElementsByClassName("input-group");
+    // Iterate over all the div elements 
+    for (let containerDiv of allInputContainerDivElements) {
+        // Get the div element with the class "input-group-prepend"
+        // inside the container div
+        let prependDiv = containerDiv
+            .getElementsByClassName("input-group-prepend")[0];
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">        // If the container div contains the class "optional"
+        // check if the input box has any value - if it does not have any
+        // value - consider it to be validated
+        if (containerDiv.classList.contains("optional") === true) {
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+            // Check if the container div has an input control
+            if (containerDiv.getElementsByTagName("input").length &gt; 0) {
+                // If the length of the input value in the input control is 0
+                if (containerDiv.getElementsByTagName("input")[0]
+                    .value.length === 0) {
+                    allFieldsAreValidated = true;
+                }
+            } else {
+                // If the length of the textarea value in the textarea control is 0
+                if (containerDiv.getElementsByTagName("textarea")[0]
+                    .value.length === 0) {
+                    allFieldsAreValidated = true;
+                }
+            }
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+        }
+        if (prependDiv.classList.contains("prepend-valid")) {
+            allFieldsAreValidated = true;
+        } else {
+            allFieldsAreValidated = false;
+            break;
+        }
+    }
+    return allFieldsAreValidated;
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">/* Helper function to check if all input fields are validated.
+ * @param  
+ * @return {boolean}    true if all fields are validated - false otherwise  
+ * */
+const allInputsAreValidated = () =&gt; {
+    // Flag to check if all input fields were validated
+    let allFieldsAreValidated = false;
+    // Get all the div elements which have the class "input-group"
+    let allInputContainerDivElements = document
+        .getElementsByClassName("input-group");
+    // Iterate over all the div elements 
+    for (let containerDiv of allInputContainerDivElements) {
+        // Get the div element with the class "input-group-prepend"
+        // inside the container div
+        let prependDiv = containerDiv
+            .getElementsByClassName("input-group-prepend")[0];
+        // If the container div contains the class "optional"
+        // check if the input box has any value - if it does not have any
+        // value - consider it to be validated
+        if (containerDiv.classList.contains("optional") === true) {
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+            // Check if the container div has an input control
+            if (containerDiv.getElementsByTagName("input").length &gt; 0) {
+                // If the length of the input value in the input control is 0
+                if (containerDiv.getElementsByTagName("input")[0]
+                    .value.length === 0) {
+                    allFieldsAreValidated = true;
+                }
+            }  // The container div has a textarea control
+            else {
+                // If the length of the textarea value in the textarea control is 0
+                if (containerDiv.getElementsByTagName("textarea")[0]
+                    .value.length === 0) {
+                    allFieldsAreValidated = true;
+                }
+            }
+        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>}
+        if (prependDiv.classList.contains("prepend-valid")) {
+            allFieldsAreValidated = true;
+        } else {
+            allFieldsAreValidated = false;
+            break;
+        }
+    }
+    return allFieldsAreValidated;
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>git status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - would display the following files.                                                                                                                                                                                                                                                  modified:   docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+        modified:   html/lock-selection-survey.html
+        modified:   js/controller/lock-selection-survey-customer-card.js</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -6093,6 +6906,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF002060"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="2" tint="-9.9978637043366805E-2"/>
       <name val="Century Gothic"/>
       <family val="1"/>
     </font>
@@ -6301,7 +7120,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -6429,6 +7248,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6486,16 +7308,25 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6826,18 +7657,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -7106,6 +7937,104 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="36" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="36" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="36" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="36" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="39" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="40" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="40" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="40" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="40" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="40" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="40" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="40" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="41" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="41" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="41" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
+        <v>288</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A16">
+    <sortCondition ref="A1:A16"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0BB7-C151-C94B-945C-E2CA92034B13}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -7122,18 +8051,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="66" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -7250,18 +8179,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -7312,11 +8241,11 @@
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="66" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="65"/>
-      <c r="C9" s="65"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="66"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -7352,20 +8281,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="63" t="s">
+      <c r="B13" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="61" t="s">
+      <c r="C13" s="62" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="62"/>
-      <c r="B14" s="64"/>
-      <c r="C14" s="62"/>
+      <c r="A14" s="63"/>
+      <c r="B14" s="65"/>
+      <c r="C14" s="63"/>
     </row>
     <row r="15" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
@@ -7390,20 +8319,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="61" t="s">
+      <c r="A17" s="62" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="61" t="s">
+      <c r="C17" s="62" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="62"/>
-      <c r="B18" s="64"/>
-      <c r="C18" s="62"/>
+      <c r="A18" s="63"/>
+      <c r="B18" s="65"/>
+      <c r="C18" s="63"/>
     </row>
     <row r="19" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -7461,18 +8390,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="66" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -7508,25 +8437,25 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="61" t="s">
+      <c r="A6" s="62" t="s">
         <v>292</v>
       </c>
-      <c r="B6" s="66" t="s">
+      <c r="B6" s="67" t="s">
         <v>291</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="62" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="72"/>
-      <c r="B7" s="67"/>
-      <c r="C7" s="72"/>
+      <c r="A7" s="73"/>
+      <c r="B7" s="68"/>
+      <c r="C7" s="73"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="62"/>
-      <c r="B8" s="68"/>
-      <c r="C8" s="62"/>
+      <c r="A8" s="63"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="63"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -7551,25 +8480,25 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="69" t="s">
+      <c r="A11" s="70" t="s">
         <v>294</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="67" t="s">
         <v>295</v>
       </c>
-      <c r="C11" s="69" t="s">
+      <c r="C11" s="70" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="70"/>
-      <c r="B12" s="67"/>
-      <c r="C12" s="70"/>
+      <c r="A12" s="71"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="71"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="71"/>
-      <c r="B13" s="68"/>
-      <c r="C13" s="71"/>
+      <c r="A13" s="72"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="72"/>
     </row>
     <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
@@ -7626,18 +8555,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="66" t="s">
         <v>299</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -7651,46 +8580,46 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="73" t="s">
+      <c r="A4" s="74" t="s">
         <v>300</v>
       </c>
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="78" t="s">
         <v>305</v>
       </c>
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="74" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="73"/>
-      <c r="B5" s="77"/>
-      <c r="C5" s="73"/>
+      <c r="A5" s="74"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="74"/>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="73"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="73"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="74"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="62" t="s">
         <v>302</v>
       </c>
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="75" t="s">
         <v>303</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="62" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="72"/>
-      <c r="B8" s="75"/>
-      <c r="C8" s="72"/>
+      <c r="A8" s="73"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="73"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="228" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="62"/>
-      <c r="B9" s="76"/>
-      <c r="C9" s="62"/>
+      <c r="A9" s="63"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="63"/>
     </row>
     <row r="10" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
@@ -7747,18 +8676,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="66" t="s">
         <v>331</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -7805,233 +8734,233 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="61" t="s">
+      <c r="A7" s="62" t="s">
         <v>314</v>
       </c>
-      <c r="B7" s="66" t="s">
+      <c r="B7" s="67" t="s">
         <v>322</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="62" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="72"/>
-      <c r="B8" s="67"/>
-      <c r="C8" s="72"/>
+      <c r="A8" s="73"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="73"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="72"/>
-      <c r="B9" s="67"/>
-      <c r="C9" s="72"/>
+      <c r="A9" s="73"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="73"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="72"/>
-      <c r="B10" s="67"/>
-      <c r="C10" s="72"/>
+      <c r="A10" s="73"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="73"/>
     </row>
     <row r="11" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="72"/>
-      <c r="B11" s="67"/>
-      <c r="C11" s="72"/>
+      <c r="A11" s="73"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="73"/>
     </row>
     <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="72"/>
-      <c r="B12" s="67"/>
-      <c r="C12" s="72"/>
+      <c r="A12" s="73"/>
+      <c r="B12" s="68"/>
+      <c r="C12" s="73"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="62"/>
-      <c r="B13" s="68"/>
-      <c r="C13" s="62"/>
+      <c r="A13" s="63"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="63"/>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="61" t="s">
+      <c r="A14" s="62" t="s">
         <v>325</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="67" t="s">
         <v>323</v>
       </c>
-      <c r="C14" s="61" t="s">
+      <c r="C14" s="62" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="72"/>
-      <c r="B15" s="67"/>
-      <c r="C15" s="72"/>
+      <c r="A15" s="73"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="73"/>
     </row>
     <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="72"/>
-      <c r="B16" s="67"/>
-      <c r="C16" s="72"/>
+      <c r="A16" s="73"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="73"/>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="72"/>
-      <c r="B17" s="67"/>
-      <c r="C17" s="72"/>
+      <c r="A17" s="73"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="73"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="72"/>
-      <c r="B18" s="67"/>
-      <c r="C18" s="72"/>
+      <c r="A18" s="73"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="73"/>
     </row>
     <row r="19" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="72"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="72"/>
+      <c r="A19" s="73"/>
+      <c r="B19" s="68"/>
+      <c r="C19" s="73"/>
     </row>
     <row r="20" spans="1:3" ht="155" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="72"/>
-      <c r="B20" s="68"/>
-      <c r="C20" s="72"/>
+      <c r="A20" s="73"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="73"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="72"/>
-      <c r="B21" s="66" t="s">
+      <c r="A21" s="73"/>
+      <c r="B21" s="67" t="s">
         <v>316</v>
       </c>
-      <c r="C21" s="72"/>
+      <c r="C21" s="73"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="72"/>
-      <c r="B22" s="67"/>
-      <c r="C22" s="72"/>
+      <c r="A22" s="73"/>
+      <c r="B22" s="68"/>
+      <c r="C22" s="73"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="72"/>
-      <c r="B23" s="67"/>
-      <c r="C23" s="72"/>
+      <c r="A23" s="73"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="73"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="72"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="72"/>
+      <c r="A24" s="73"/>
+      <c r="B24" s="68"/>
+      <c r="C24" s="73"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="72"/>
-      <c r="B25" s="67"/>
-      <c r="C25" s="72"/>
+      <c r="A25" s="73"/>
+      <c r="B25" s="68"/>
+      <c r="C25" s="73"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="72"/>
-      <c r="B26" s="67"/>
-      <c r="C26" s="72"/>
+      <c r="A26" s="73"/>
+      <c r="B26" s="68"/>
+      <c r="C26" s="73"/>
     </row>
     <row r="27" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="72"/>
-      <c r="B27" s="68"/>
-      <c r="C27" s="72"/>
+      <c r="A27" s="73"/>
+      <c r="B27" s="69"/>
+      <c r="C27" s="73"/>
     </row>
     <row r="28" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="72"/>
-      <c r="B28" s="66" t="s">
+      <c r="A28" s="73"/>
+      <c r="B28" s="67" t="s">
         <v>317</v>
       </c>
-      <c r="C28" s="72"/>
+      <c r="C28" s="73"/>
     </row>
     <row r="29" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="72"/>
-      <c r="B29" s="67"/>
-      <c r="C29" s="72"/>
+      <c r="A29" s="73"/>
+      <c r="B29" s="68"/>
+      <c r="C29" s="73"/>
     </row>
     <row r="30" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="72"/>
-      <c r="B30" s="67"/>
-      <c r="C30" s="72"/>
+      <c r="A30" s="73"/>
+      <c r="B30" s="68"/>
+      <c r="C30" s="73"/>
     </row>
     <row r="31" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="72"/>
-      <c r="B31" s="67"/>
-      <c r="C31" s="72"/>
+      <c r="A31" s="73"/>
+      <c r="B31" s="68"/>
+      <c r="C31" s="73"/>
     </row>
     <row r="32" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="72"/>
-      <c r="B32" s="67"/>
-      <c r="C32" s="72"/>
+      <c r="A32" s="73"/>
+      <c r="B32" s="68"/>
+      <c r="C32" s="73"/>
     </row>
     <row r="33" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="72"/>
-      <c r="B33" s="67"/>
-      <c r="C33" s="72"/>
+      <c r="A33" s="73"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="73"/>
     </row>
     <row r="34" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="72"/>
-      <c r="B34" s="67"/>
-      <c r="C34" s="72"/>
+      <c r="A34" s="73"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="73"/>
     </row>
     <row r="35" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="72"/>
-      <c r="B35" s="67"/>
-      <c r="C35" s="72"/>
+      <c r="A35" s="73"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="73"/>
     </row>
     <row r="36" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="72"/>
-      <c r="B36" s="67"/>
-      <c r="C36" s="72"/>
+      <c r="A36" s="73"/>
+      <c r="B36" s="68"/>
+      <c r="C36" s="73"/>
     </row>
     <row r="37" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="72"/>
-      <c r="B37" s="68"/>
-      <c r="C37" s="72"/>
+      <c r="A37" s="73"/>
+      <c r="B37" s="69"/>
+      <c r="C37" s="73"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="72"/>
-      <c r="B38" s="66" t="s">
+      <c r="A38" s="73"/>
+      <c r="B38" s="67" t="s">
         <v>318</v>
       </c>
-      <c r="C38" s="72"/>
+      <c r="C38" s="73"/>
     </row>
     <row r="39" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="72"/>
-      <c r="B39" s="67"/>
-      <c r="C39" s="72"/>
+      <c r="A39" s="73"/>
+      <c r="B39" s="68"/>
+      <c r="C39" s="73"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="72"/>
-      <c r="B40" s="67"/>
-      <c r="C40" s="72"/>
+      <c r="A40" s="73"/>
+      <c r="B40" s="68"/>
+      <c r="C40" s="73"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="72"/>
-      <c r="B41" s="67"/>
-      <c r="C41" s="72"/>
+      <c r="A41" s="73"/>
+      <c r="B41" s="68"/>
+      <c r="C41" s="73"/>
     </row>
     <row r="42" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="62"/>
-      <c r="B42" s="68"/>
-      <c r="C42" s="62"/>
+      <c r="A42" s="63"/>
+      <c r="B42" s="69"/>
+      <c r="C42" s="63"/>
     </row>
     <row r="43" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="61" t="s">
+      <c r="A43" s="62" t="s">
         <v>326</v>
       </c>
-      <c r="B43" s="66" t="s">
+      <c r="B43" s="67" t="s">
         <v>327</v>
       </c>
-      <c r="C43" s="61" t="s">
+      <c r="C43" s="62" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="72"/>
-      <c r="B44" s="67"/>
-      <c r="C44" s="72"/>
+      <c r="A44" s="73"/>
+      <c r="B44" s="68"/>
+      <c r="C44" s="73"/>
     </row>
     <row r="45" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="72"/>
-      <c r="B45" s="67"/>
-      <c r="C45" s="72"/>
+      <c r="A45" s="73"/>
+      <c r="B45" s="68"/>
+      <c r="C45" s="73"/>
     </row>
     <row r="46" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="72"/>
-      <c r="B46" s="67"/>
-      <c r="C46" s="72"/>
+      <c r="A46" s="73"/>
+      <c r="B46" s="68"/>
+      <c r="C46" s="73"/>
     </row>
     <row r="47" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="62"/>
-      <c r="B47" s="68"/>
-      <c r="C47" s="62"/>
+      <c r="A47" s="63"/>
+      <c r="B47" s="69"/>
+      <c r="C47" s="63"/>
     </row>
     <row r="48" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
@@ -8058,11 +8987,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B7:B13"/>
-    <mergeCell ref="A7:A13"/>
-    <mergeCell ref="C7:C13"/>
     <mergeCell ref="B38:B42"/>
     <mergeCell ref="A14:A42"/>
     <mergeCell ref="C14:C42"/>
@@ -8072,6 +8996,11 @@
     <mergeCell ref="B28:B37"/>
     <mergeCell ref="B14:B20"/>
     <mergeCell ref="B21:B27"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B7:B13"/>
+    <mergeCell ref="A7:A13"/>
+    <mergeCell ref="C7:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8094,18 +9023,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="66" t="s">
         <v>332</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -8231,6 +9160,101 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4431450A-9C71-854E-855D-098E661E41E5}">
   <dimension ref="A1:C7"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="66" t="s">
+        <v>356</v>
+      </c>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="238" x14ac:dyDescent="0.2">
+      <c r="A4" s="57" t="s">
+        <v>358</v>
+      </c>
+      <c r="B4" s="58" t="s">
+        <v>357</v>
+      </c>
+      <c r="C4" s="57" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="221" x14ac:dyDescent="0.2">
+      <c r="A5" s="57" t="s">
+        <v>361</v>
+      </c>
+      <c r="B5" s="58" t="s">
+        <v>360</v>
+      </c>
+      <c r="C5" s="57" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA2D3523-DE23-E44E-AB5A-E85653D30CCE}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
@@ -8244,18 +9268,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="65" t="s">
-        <v>356</v>
-      </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
+      <c r="A2" s="66" t="s">
+        <v>365</v>
+      </c>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -8268,61 +9292,152 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="13" customFormat="1" ht="238" x14ac:dyDescent="0.2">
-      <c r="A4" s="57" t="s">
-        <v>358</v>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="289" x14ac:dyDescent="0.2">
+      <c r="A4" s="59" t="s">
+        <v>366</v>
       </c>
       <c r="B4" s="58" t="s">
-        <v>357</v>
-      </c>
-      <c r="C4" s="57" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="13" customFormat="1" ht="221" x14ac:dyDescent="0.2">
-      <c r="A5" s="57" t="s">
-        <v>361</v>
-      </c>
-      <c r="B5" s="58" t="s">
-        <v>360</v>
-      </c>
-      <c r="C5" s="57" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
+        <v>367</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="62" t="s">
+        <v>369</v>
+      </c>
+      <c r="B5" s="79" t="s">
+        <v>372</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="63"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="63"/>
+    </row>
+    <row r="7" spans="1:3" s="13" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+      <c r="A7" s="59" t="s">
+        <v>371</v>
+      </c>
+      <c r="B7" s="58" t="s">
+        <v>373</v>
+      </c>
+      <c r="C7" s="59" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="62" t="s">
+        <v>376</v>
+      </c>
+      <c r="B8" s="79" t="s">
+        <v>375</v>
+      </c>
+      <c r="C8" s="62" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="73"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="73"/>
+    </row>
+    <row r="10" spans="1:3" s="13" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="63"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="63"/>
+    </row>
+    <row r="11" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="62" t="s">
+        <v>378</v>
+      </c>
+      <c r="B11" s="79" t="s">
+        <v>384</v>
+      </c>
+      <c r="C11" s="62" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="73"/>
+      <c r="B12" s="80"/>
+      <c r="C12" s="73"/>
+    </row>
+    <row r="13" spans="1:3" s="13" customFormat="1" ht="187" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="63"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="63"/>
+    </row>
+    <row r="14" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="62" t="s">
+        <v>380</v>
+      </c>
+      <c r="B14" s="79" t="s">
+        <v>383</v>
+      </c>
+      <c r="C14" s="62" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="73"/>
+      <c r="B15" s="80"/>
+      <c r="C15" s="73"/>
+    </row>
+    <row r="16" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="63"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="63"/>
+    </row>
+    <row r="17" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B17" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
+      <c r="C17" s="17" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="C7" s="18" t="s">
+      <c r="B18" s="53" t="s">
+        <v>382</v>
+      </c>
+      <c r="C18" s="18" t="s">
         <v>98</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="2">
+  <mergeCells count="14">
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:C10"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="C5:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE113606-3FFA-8545-9BE3-5643B52A7CE9}">
   <dimension ref="A1:H116"/>
   <sheetViews>
@@ -8400,10 +9515,10 @@
       <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="85" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="78"/>
+      <c r="B6" s="85"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -9376,32 +10491,32 @@
       <c r="H73" s="23"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="79"/>
-      <c r="B74" s="80"/>
+      <c r="A74" s="82"/>
+      <c r="B74" s="86"/>
       <c r="C74" s="32" t="s">
         <v>225</v>
       </c>
       <c r="D74" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="E74" s="81"/>
-      <c r="F74" s="79"/>
-      <c r="G74" s="83"/>
-      <c r="H74" s="79"/>
+      <c r="E74" s="87"/>
+      <c r="F74" s="82"/>
+      <c r="G74" s="84"/>
+      <c r="H74" s="82"/>
     </row>
     <row r="75" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A75" s="79"/>
-      <c r="B75" s="80"/>
+      <c r="A75" s="82"/>
+      <c r="B75" s="86"/>
       <c r="C75" s="33" t="s">
         <v>226</v>
       </c>
       <c r="D75" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="E75" s="81"/>
-      <c r="F75" s="79"/>
-      <c r="G75" s="83"/>
-      <c r="H75" s="79"/>
+      <c r="E75" s="87"/>
+      <c r="F75" s="82"/>
+      <c r="G75" s="84"/>
+      <c r="H75" s="82"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="23"/>
@@ -9574,34 +10689,34 @@
       <c r="H88" s="23"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="79"/>
-      <c r="B89" s="79"/>
+      <c r="A89" s="82"/>
+      <c r="B89" s="82"/>
       <c r="C89" s="35" t="s">
         <v>225</v>
       </c>
       <c r="D89" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="E89" s="82" t="s">
+      <c r="E89" s="83" t="s">
         <v>121</v>
       </c>
-      <c r="F89" s="82"/>
-      <c r="G89" s="83"/>
-      <c r="H89" s="79"/>
+      <c r="F89" s="83"/>
+      <c r="G89" s="84"/>
+      <c r="H89" s="82"/>
     </row>
     <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A90" s="79"/>
-      <c r="B90" s="79"/>
+      <c r="A90" s="82"/>
+      <c r="B90" s="82"/>
       <c r="C90" s="35" t="s">
         <v>242</v>
       </c>
       <c r="D90" s="35" t="s">
         <v>243</v>
       </c>
-      <c r="E90" s="82"/>
-      <c r="F90" s="82"/>
-      <c r="G90" s="83"/>
-      <c r="H90" s="79"/>
+      <c r="E90" s="83"/>
+      <c r="F90" s="83"/>
+      <c r="G90" s="84"/>
+      <c r="H90" s="82"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="23"/>
@@ -9969,6 +11084,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F74:F75"/>
     <mergeCell ref="H74:H75"/>
     <mergeCell ref="A89:A90"/>
     <mergeCell ref="B89:B90"/>
@@ -9977,110 +11097,7 @@
     <mergeCell ref="G89:G90"/>
     <mergeCell ref="H89:H90"/>
     <mergeCell ref="G74:G75"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F74:F75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
-  <dimension ref="A1:A16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="40" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="40" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="40" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="40" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="40" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="41" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="41" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="41" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
-        <v>288</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A16">
-    <sortCondition ref="A1:A16"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Implementation of the Lock class and associated enumerations.
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A305EE-3894-C84F-8E34-7CE747E40E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A71396-0F63-CB43-84AE-26B0AFDDC1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="1000" windowWidth="27640" windowHeight="16160" firstSheet="2" activeTab="10" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
+    <workbookView xWindow="300" yWindow="1000" windowWidth="27640" windowHeight="16160" firstSheet="3" activeTab="11" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="SPEC - 1.1" sheetId="1" r:id="rId1"/>
@@ -24,9 +24,10 @@
     <sheet name="SPEC - 1.9" sheetId="13" r:id="rId9"/>
     <sheet name="SPEC - 1.10" sheetId="14" r:id="rId10"/>
     <sheet name="SPEC - 1.11" sheetId="15" r:id="rId11"/>
-    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId12"/>
-    <sheet name="PLAYGROUND" sheetId="6" r:id="rId13"/>
-    <sheet name="TEMPLATE" sheetId="8" r:id="rId14"/>
+    <sheet name="SPEC - 2.0" sheetId="16" r:id="rId12"/>
+    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId13"/>
+    <sheet name="PLAYGROUND" sheetId="6" r:id="rId14"/>
+    <sheet name="TEMPLATE" sheetId="8" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="504">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -9762,6 +9763,512 @@
   </si>
   <si>
     <t>git commit -m "Merged the init branch to the master branch."</t>
+  </si>
+  <si>
+    <t>CREATE A NEW GIT BRANCH - workflow</t>
+  </si>
+  <si>
+    <t>git branch workflow</t>
+  </si>
+  <si>
+    <r>
+      <t>git branch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> displays the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">workflow </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>branch</t>
+    </r>
+  </si>
+  <si>
+    <t>Create a new git branch - workflow</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Switch to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>workflow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> branch</t>
+    </r>
+  </si>
+  <si>
+    <t>git checkout workflow</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">git branch </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>displays the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> workflow </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">branch with a prefixed </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to indicate that it is the currently selected branch</t>
+    </r>
+  </si>
+  <si>
+    <t>CREATE A NEW LOCK CLASS AND ASSOCIATED ENUMERATION</t>
+  </si>
+  <si>
+    <t>touch js/model/lock.js</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create a new file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/model/lock.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>ls js/model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> displays the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lock.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> file</t>
+    </r>
+  </si>
+  <si>
+    <t>use strict';
+/* * The Lock class.
+ *  @author Sanket Rajgarhia
+ *  @date   03/04/2022 (dd/mm/yyyy)
+ *  @version 1.0
+ * */
+/*****************************************************************************/
+/* LOCK CLASS IMPLEMENTATION                                                */
+/*****************************************************************************/
+class Lock {
+    /* *Constructor
+     * @param    {String} model     Model of the lock
+     * */
+    constructor(model) {
+        this._model = model;
+    }
+    /* Get the lock model
+     * @return  {String}    Model of the lock
+     */
+    get model() {
+        return this._model;
+    }
+    /* Set the lock model
+     * @param    {String} model     Model of the lock
+     */
+    set model(model) {
+        this._model = model;
+    }
+}
+/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implement the class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Lock</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/model/lock.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implemented the class </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Lock</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/model/lock.js</t>
+    </r>
+  </si>
+  <si>
+    <t>mkdir -p lib/lang/en/enum/lock</t>
+  </si>
+  <si>
+    <t>touch lib/lang/en/enum/lock/lock-enum.js</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create the directory </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lib/lang/en/enum/lock</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lib/lang/en/enum/lock/lock-enum.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>ls lib/lang/en/enum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> displays the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">lock </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>directory</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>ls lib/lang/en/enum/lock</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> displays the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lock-enum.js</t>
+    </r>
+  </si>
+  <si>
+    <t>use strict';
+/* * The Lock Enumeration Values (EN).
+ *  @author   Sanket Rajgarhia
+ *  @date 03/04/2022 (dd/mm/yyyy)
+ *  @version 1.0
+ *  @language: en
+ * */
+/*****************************************************************************/
+/* LOCK ENUMERATION (EN)                                                     */
+/*****************************************************************************/
+/* Lock model names */
+const LOCK_MODEL = {
+    DC1000: "DC1000",
+    DH2000: "DH2000",
+    ER4900: "ER4900",
+    ER5100: "ER5100",
+    ER5200: "ER5200",
+    EL6000: "EL6000",
+    EL7200: "EL7200",
+    EL7500: "EL7500",
+    DL6500: "DL6500",
+    DL6600: "DL6600",
+    DL7000: "DL7000",
+    DL7100: "DL7100",
+    DL7600: "DL7600",
+    DL7900: "DL7900",
+    PP8100: "PP8100",
+    PP9000: "PP9000"
+};
+/*****************************************************************************/
+/* FREEZE - TO EMULATE ENUMERATION                                           */
+/*****************************************************************************/
+// Prevent addition of properties to the json Object
+Object.freeze(LOCK_MODEL);
+/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implement the Lock model enumerations in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>ib/lang/en/enum/lock/lock-enum.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implemented the Lock model enumerations in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>ib/lang/en/enum/lock/lock-enum.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>git status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - would display the following files.                                                                                                                                                                                                                                  On branch workflow
+Changes to be committed:
+  (use "git restore --staged &lt;file&gt;..." to unstage)
+        modified:   docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+        new file:   js/model/lock.js
+        new file:   lib/lang/en/enum/lock/lock-enum.js</t>
+    </r>
+  </si>
+  <si>
+    <t>git commit -m "Implementation of the Lock class and associated enumerations."</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">On branch </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>workflow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> nothing to commit, working tree clean</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -10181,7 +10688,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -10350,6 +10857,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -10790,18 +11309,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -11086,18 +11605,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="83" t="s">
         <v>426</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -11111,7 +11630,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="104" t="s">
         <v>438</v>
       </c>
       <c r="B4" s="48" t="s">
@@ -11122,7 +11641,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="101"/>
+      <c r="A5" s="105"/>
       <c r="B5" s="48" t="s">
         <v>441</v>
       </c>
@@ -11131,51 +11650,51 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="101"/>
+      <c r="A6" s="105"/>
       <c r="B6" s="48" t="s">
         <v>434</v>
       </c>
-      <c r="C6" s="103" t="s">
+      <c r="C6" s="107" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="101"/>
+      <c r="A7" s="105"/>
       <c r="B7" s="48" t="s">
         <v>435</v>
       </c>
-      <c r="C7" s="104"/>
+      <c r="C7" s="108"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="101"/>
+      <c r="A8" s="105"/>
       <c r="B8" s="48" t="s">
         <v>427</v>
       </c>
-      <c r="C8" s="104"/>
+      <c r="C8" s="108"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="101"/>
+      <c r="A9" s="105"/>
       <c r="B9" s="48" t="s">
         <v>428</v>
       </c>
-      <c r="C9" s="104"/>
+      <c r="C9" s="108"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="101"/>
+      <c r="A10" s="105"/>
       <c r="B10" s="48" t="s">
         <v>436</v>
       </c>
-      <c r="C10" s="104"/>
+      <c r="C10" s="108"/>
     </row>
     <row r="11" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="101"/>
+      <c r="A11" s="105"/>
       <c r="B11" s="48" t="s">
         <v>443</v>
       </c>
-      <c r="C11" s="105"/>
+      <c r="C11" s="109"/>
     </row>
     <row r="12" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="102"/>
+      <c r="A12" s="106"/>
       <c r="B12" s="48" t="s">
         <v>445</v>
       </c>
@@ -11301,6 +11820,123 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E9535A-D76D-CC41-8B17-54B2B9EC8C5F}">
   <dimension ref="A1:C9"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="83" t="s">
+        <v>464</v>
+      </c>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="B4" s="51" t="s">
+        <v>448</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>471</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>470</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
+        <v>473</v>
+      </c>
+      <c r="B6" s="51" t="s">
+        <v>474</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>469</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>475</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="372" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>477</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4437CF02-82B5-C74B-B6B5-F1F00EF2719A}">
+  <dimension ref="A1:C20"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
@@ -11314,18 +11950,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
-        <v>464</v>
-      </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
+      <c r="A2" s="83" t="s">
+        <v>478</v>
+      </c>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -11339,82 +11975,176 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>447</v>
-      </c>
-      <c r="B4" s="51" t="s">
-        <v>448</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>467</v>
+      <c r="A4" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>479</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>471</v>
-      </c>
-      <c r="B5" s="51" t="s">
-        <v>470</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>472</v>
+      <c r="A5" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>483</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>473</v>
-      </c>
-      <c r="B6" s="51" t="s">
-        <v>474</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>468</v>
-      </c>
+      <c r="A6" s="54"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="54"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="12" t="s">
-        <v>469</v>
-      </c>
-      <c r="B7" s="51" t="s">
-        <v>475</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="372" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
+      <c r="A7" s="74"/>
+      <c r="B7" s="75"/>
+      <c r="C7" s="74"/>
+    </row>
+    <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="54"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="54"/>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="83" t="s">
+        <v>485</v>
+      </c>
+      <c r="B9" s="83"/>
+      <c r="C9" s="83"/>
+    </row>
+    <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>487</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>486</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="B12" s="48" t="s">
+        <v>483</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="79" t="s">
+        <v>490</v>
+      </c>
+      <c r="B13" s="84" t="s">
+        <v>489</v>
+      </c>
+      <c r="C13" s="79" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="80"/>
+      <c r="B14" s="86"/>
+      <c r="C14" s="80"/>
+    </row>
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="73" t="s">
+        <v>494</v>
+      </c>
+      <c r="B15" s="76" t="s">
+        <v>492</v>
+      </c>
+      <c r="C15" s="73" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="73" t="s">
+        <v>495</v>
+      </c>
+      <c r="B16" s="76" t="s">
+        <v>493</v>
+      </c>
+      <c r="C16" s="73" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="79" t="s">
+        <v>499</v>
+      </c>
+      <c r="B17" s="84" t="s">
+        <v>498</v>
+      </c>
+      <c r="C17" s="79" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="222" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="80"/>
+      <c r="B18" s="86"/>
+      <c r="C18" s="80"/>
+    </row>
+    <row r="19" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A19" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B19" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C8" s="17" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
+      <c r="C19" s="17" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="18" t="s">
-        <v>477</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>98</v>
+      <c r="B20" s="18" t="s">
+        <v>502</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>503</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="2">
+  <mergeCells count="9">
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="C17:C18"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE113606-3FFA-8545-9BE3-5643B52A7CE9}">
   <dimension ref="A1:H116"/>
   <sheetViews>
@@ -11492,10 +12222,10 @@
       <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="109" t="s">
+      <c r="A6" s="113" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="109"/>
+      <c r="B6" s="113"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -12468,32 +13198,32 @@
       <c r="H73" s="23"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="106"/>
-      <c r="B74" s="110"/>
+      <c r="A74" s="110"/>
+      <c r="B74" s="114"/>
       <c r="C74" s="32" t="s">
         <v>225</v>
       </c>
       <c r="D74" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="E74" s="111"/>
-      <c r="F74" s="106"/>
-      <c r="G74" s="108"/>
-      <c r="H74" s="106"/>
+      <c r="E74" s="115"/>
+      <c r="F74" s="110"/>
+      <c r="G74" s="112"/>
+      <c r="H74" s="110"/>
     </row>
     <row r="75" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A75" s="106"/>
-      <c r="B75" s="110"/>
+      <c r="A75" s="110"/>
+      <c r="B75" s="114"/>
       <c r="C75" s="33" t="s">
         <v>226</v>
       </c>
       <c r="D75" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="E75" s="111"/>
-      <c r="F75" s="106"/>
-      <c r="G75" s="108"/>
-      <c r="H75" s="106"/>
+      <c r="E75" s="115"/>
+      <c r="F75" s="110"/>
+      <c r="G75" s="112"/>
+      <c r="H75" s="110"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="23"/>
@@ -12666,34 +13396,34 @@
       <c r="H88" s="23"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="106"/>
-      <c r="B89" s="106"/>
+      <c r="A89" s="110"/>
+      <c r="B89" s="110"/>
       <c r="C89" s="35" t="s">
         <v>225</v>
       </c>
       <c r="D89" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="E89" s="107" t="s">
+      <c r="E89" s="111" t="s">
         <v>121</v>
       </c>
-      <c r="F89" s="107"/>
-      <c r="G89" s="108"/>
-      <c r="H89" s="106"/>
+      <c r="F89" s="111"/>
+      <c r="G89" s="112"/>
+      <c r="H89" s="110"/>
     </row>
     <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A90" s="106"/>
-      <c r="B90" s="106"/>
+      <c r="A90" s="110"/>
+      <c r="B90" s="110"/>
       <c r="C90" s="35" t="s">
         <v>242</v>
       </c>
       <c r="D90" s="35" t="s">
         <v>243</v>
       </c>
-      <c r="E90" s="107"/>
-      <c r="F90" s="107"/>
-      <c r="G90" s="108"/>
-      <c r="H90" s="106"/>
+      <c r="E90" s="111"/>
+      <c r="F90" s="111"/>
+      <c r="G90" s="112"/>
+      <c r="H90" s="110"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="23"/>
@@ -13079,7 +13809,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -13177,7 +13907,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0BB7-C151-C94B-945C-E2CA92034B13}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -13194,18 +13924,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="83" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -13322,18 +14052,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="83" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -13384,11 +14114,11 @@
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="79" t="s">
+      <c r="A9" s="83" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="83"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -13424,20 +14154,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="75" t="s">
+      <c r="A13" s="79" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="77" t="s">
+      <c r="B13" s="81" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="75" t="s">
+      <c r="C13" s="79" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="76"/>
-      <c r="B14" s="78"/>
-      <c r="C14" s="76"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="82"/>
+      <c r="C14" s="80"/>
     </row>
     <row r="15" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
@@ -13462,20 +14192,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="75" t="s">
+      <c r="A17" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="77" t="s">
+      <c r="B17" s="81" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="75" t="s">
+      <c r="C17" s="79" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="76"/>
-      <c r="B18" s="78"/>
-      <c r="C18" s="76"/>
+      <c r="A18" s="80"/>
+      <c r="B18" s="82"/>
+      <c r="C18" s="80"/>
     </row>
     <row r="19" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -13533,18 +14263,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="83" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -13580,25 +14310,25 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="79" t="s">
         <v>292</v>
       </c>
-      <c r="B6" s="80" t="s">
+      <c r="B6" s="84" t="s">
         <v>291</v>
       </c>
-      <c r="C6" s="75" t="s">
+      <c r="C6" s="79" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="86"/>
-      <c r="B7" s="81"/>
-      <c r="C7" s="86"/>
+      <c r="A7" s="90"/>
+      <c r="B7" s="85"/>
+      <c r="C7" s="90"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="76"/>
-      <c r="B8" s="82"/>
-      <c r="C8" s="76"/>
+      <c r="A8" s="80"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="80"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -13623,25 +14353,25 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="83" t="s">
+      <c r="A11" s="87" t="s">
         <v>294</v>
       </c>
-      <c r="B11" s="80" t="s">
+      <c r="B11" s="84" t="s">
         <v>295</v>
       </c>
-      <c r="C11" s="83" t="s">
+      <c r="C11" s="87" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="84"/>
-      <c r="B12" s="81"/>
-      <c r="C12" s="84"/>
+      <c r="A12" s="88"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="88"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="85"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="85"/>
+      <c r="A13" s="89"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="89"/>
     </row>
     <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
@@ -13698,18 +14428,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="83" t="s">
         <v>299</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -13723,46 +14453,46 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="91" t="s">
         <v>300</v>
       </c>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="95" t="s">
         <v>305</v>
       </c>
-      <c r="C4" s="87" t="s">
+      <c r="C4" s="91" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="87"/>
-      <c r="B5" s="91"/>
-      <c r="C5" s="87"/>
+      <c r="A5" s="91"/>
+      <c r="B5" s="95"/>
+      <c r="C5" s="91"/>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="87"/>
-      <c r="B6" s="91"/>
-      <c r="C6" s="87"/>
+      <c r="A6" s="91"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="91"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="79" t="s">
         <v>302</v>
       </c>
-      <c r="B7" s="88" t="s">
+      <c r="B7" s="92" t="s">
         <v>303</v>
       </c>
-      <c r="C7" s="75" t="s">
+      <c r="C7" s="79" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="86"/>
-      <c r="B8" s="89"/>
-      <c r="C8" s="86"/>
+      <c r="A8" s="90"/>
+      <c r="B8" s="93"/>
+      <c r="C8" s="90"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="228" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="76"/>
-      <c r="B9" s="90"/>
-      <c r="C9" s="76"/>
+      <c r="A9" s="80"/>
+      <c r="B9" s="94"/>
+      <c r="C9" s="80"/>
     </row>
     <row r="10" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
@@ -13819,18 +14549,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="83" t="s">
         <v>331</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -13877,233 +14607,233 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="79" t="s">
         <v>314</v>
       </c>
-      <c r="B7" s="80" t="s">
+      <c r="B7" s="84" t="s">
         <v>322</v>
       </c>
-      <c r="C7" s="75" t="s">
+      <c r="C7" s="79" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="86"/>
-      <c r="B8" s="81"/>
-      <c r="C8" s="86"/>
+      <c r="A8" s="90"/>
+      <c r="B8" s="85"/>
+      <c r="C8" s="90"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="86"/>
-      <c r="B9" s="81"/>
-      <c r="C9" s="86"/>
+      <c r="A9" s="90"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="90"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="86"/>
-      <c r="B10" s="81"/>
-      <c r="C10" s="86"/>
+      <c r="A10" s="90"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="90"/>
     </row>
     <row r="11" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="86"/>
-      <c r="B11" s="81"/>
-      <c r="C11" s="86"/>
+      <c r="A11" s="90"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="90"/>
     </row>
     <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="86"/>
-      <c r="B12" s="81"/>
-      <c r="C12" s="86"/>
+      <c r="A12" s="90"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="90"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="76"/>
-      <c r="B13" s="82"/>
-      <c r="C13" s="76"/>
+      <c r="A13" s="80"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="80"/>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="75" t="s">
+      <c r="A14" s="79" t="s">
         <v>325</v>
       </c>
-      <c r="B14" s="80" t="s">
+      <c r="B14" s="84" t="s">
         <v>323</v>
       </c>
-      <c r="C14" s="75" t="s">
+      <c r="C14" s="79" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="86"/>
-      <c r="B15" s="81"/>
-      <c r="C15" s="86"/>
+      <c r="A15" s="90"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="90"/>
     </row>
     <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="86"/>
-      <c r="B16" s="81"/>
-      <c r="C16" s="86"/>
+      <c r="A16" s="90"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="90"/>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="86"/>
-      <c r="B17" s="81"/>
-      <c r="C17" s="86"/>
+      <c r="A17" s="90"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="90"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="86"/>
-      <c r="B18" s="81"/>
-      <c r="C18" s="86"/>
+      <c r="A18" s="90"/>
+      <c r="B18" s="85"/>
+      <c r="C18" s="90"/>
     </row>
     <row r="19" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="86"/>
-      <c r="B19" s="81"/>
-      <c r="C19" s="86"/>
+      <c r="A19" s="90"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="90"/>
     </row>
     <row r="20" spans="1:3" ht="155" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="86"/>
-      <c r="B20" s="82"/>
-      <c r="C20" s="86"/>
+      <c r="A20" s="90"/>
+      <c r="B20" s="86"/>
+      <c r="C20" s="90"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="86"/>
-      <c r="B21" s="80" t="s">
+      <c r="A21" s="90"/>
+      <c r="B21" s="84" t="s">
         <v>316</v>
       </c>
-      <c r="C21" s="86"/>
+      <c r="C21" s="90"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="86"/>
-      <c r="B22" s="81"/>
-      <c r="C22" s="86"/>
+      <c r="A22" s="90"/>
+      <c r="B22" s="85"/>
+      <c r="C22" s="90"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="86"/>
-      <c r="B23" s="81"/>
-      <c r="C23" s="86"/>
+      <c r="A23" s="90"/>
+      <c r="B23" s="85"/>
+      <c r="C23" s="90"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="86"/>
-      <c r="B24" s="81"/>
-      <c r="C24" s="86"/>
+      <c r="A24" s="90"/>
+      <c r="B24" s="85"/>
+      <c r="C24" s="90"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="86"/>
-      <c r="B25" s="81"/>
-      <c r="C25" s="86"/>
+      <c r="A25" s="90"/>
+      <c r="B25" s="85"/>
+      <c r="C25" s="90"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="86"/>
-      <c r="B26" s="81"/>
-      <c r="C26" s="86"/>
+      <c r="A26" s="90"/>
+      <c r="B26" s="85"/>
+      <c r="C26" s="90"/>
     </row>
     <row r="27" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="86"/>
-      <c r="B27" s="82"/>
-      <c r="C27" s="86"/>
+      <c r="A27" s="90"/>
+      <c r="B27" s="86"/>
+      <c r="C27" s="90"/>
     </row>
     <row r="28" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="86"/>
-      <c r="B28" s="80" t="s">
+      <c r="A28" s="90"/>
+      <c r="B28" s="84" t="s">
         <v>317</v>
       </c>
-      <c r="C28" s="86"/>
+      <c r="C28" s="90"/>
     </row>
     <row r="29" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="86"/>
-      <c r="B29" s="81"/>
-      <c r="C29" s="86"/>
+      <c r="A29" s="90"/>
+      <c r="B29" s="85"/>
+      <c r="C29" s="90"/>
     </row>
     <row r="30" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="86"/>
-      <c r="B30" s="81"/>
-      <c r="C30" s="86"/>
+      <c r="A30" s="90"/>
+      <c r="B30" s="85"/>
+      <c r="C30" s="90"/>
     </row>
     <row r="31" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="86"/>
-      <c r="B31" s="81"/>
-      <c r="C31" s="86"/>
+      <c r="A31" s="90"/>
+      <c r="B31" s="85"/>
+      <c r="C31" s="90"/>
     </row>
     <row r="32" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="86"/>
-      <c r="B32" s="81"/>
-      <c r="C32" s="86"/>
+      <c r="A32" s="90"/>
+      <c r="B32" s="85"/>
+      <c r="C32" s="90"/>
     </row>
     <row r="33" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="86"/>
-      <c r="B33" s="81"/>
-      <c r="C33" s="86"/>
+      <c r="A33" s="90"/>
+      <c r="B33" s="85"/>
+      <c r="C33" s="90"/>
     </row>
     <row r="34" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="86"/>
-      <c r="B34" s="81"/>
-      <c r="C34" s="86"/>
+      <c r="A34" s="90"/>
+      <c r="B34" s="85"/>
+      <c r="C34" s="90"/>
     </row>
     <row r="35" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="86"/>
-      <c r="B35" s="81"/>
-      <c r="C35" s="86"/>
+      <c r="A35" s="90"/>
+      <c r="B35" s="85"/>
+      <c r="C35" s="90"/>
     </row>
     <row r="36" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="86"/>
-      <c r="B36" s="81"/>
-      <c r="C36" s="86"/>
+      <c r="A36" s="90"/>
+      <c r="B36" s="85"/>
+      <c r="C36" s="90"/>
     </row>
     <row r="37" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="86"/>
-      <c r="B37" s="82"/>
-      <c r="C37" s="86"/>
+      <c r="A37" s="90"/>
+      <c r="B37" s="86"/>
+      <c r="C37" s="90"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="86"/>
-      <c r="B38" s="80" t="s">
+      <c r="A38" s="90"/>
+      <c r="B38" s="84" t="s">
         <v>318</v>
       </c>
-      <c r="C38" s="86"/>
+      <c r="C38" s="90"/>
     </row>
     <row r="39" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="86"/>
-      <c r="B39" s="81"/>
-      <c r="C39" s="86"/>
+      <c r="A39" s="90"/>
+      <c r="B39" s="85"/>
+      <c r="C39" s="90"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="86"/>
-      <c r="B40" s="81"/>
-      <c r="C40" s="86"/>
+      <c r="A40" s="90"/>
+      <c r="B40" s="85"/>
+      <c r="C40" s="90"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="86"/>
-      <c r="B41" s="81"/>
-      <c r="C41" s="86"/>
+      <c r="A41" s="90"/>
+      <c r="B41" s="85"/>
+      <c r="C41" s="90"/>
     </row>
     <row r="42" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="76"/>
-      <c r="B42" s="82"/>
-      <c r="C42" s="76"/>
+      <c r="A42" s="80"/>
+      <c r="B42" s="86"/>
+      <c r="C42" s="80"/>
     </row>
     <row r="43" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="75" t="s">
+      <c r="A43" s="79" t="s">
         <v>326</v>
       </c>
-      <c r="B43" s="80" t="s">
+      <c r="B43" s="84" t="s">
         <v>327</v>
       </c>
-      <c r="C43" s="75" t="s">
+      <c r="C43" s="79" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="86"/>
-      <c r="B44" s="81"/>
-      <c r="C44" s="86"/>
+      <c r="A44" s="90"/>
+      <c r="B44" s="85"/>
+      <c r="C44" s="90"/>
     </row>
     <row r="45" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="86"/>
-      <c r="B45" s="81"/>
-      <c r="C45" s="86"/>
+      <c r="A45" s="90"/>
+      <c r="B45" s="85"/>
+      <c r="C45" s="90"/>
     </row>
     <row r="46" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="86"/>
-      <c r="B46" s="81"/>
-      <c r="C46" s="86"/>
+      <c r="A46" s="90"/>
+      <c r="B46" s="85"/>
+      <c r="C46" s="90"/>
     </row>
     <row r="47" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="76"/>
-      <c r="B47" s="82"/>
-      <c r="C47" s="76"/>
+      <c r="A47" s="80"/>
+      <c r="B47" s="86"/>
+      <c r="C47" s="80"/>
     </row>
     <row r="48" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
@@ -14166,18 +14896,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="83" t="s">
         <v>332</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -14316,18 +15046,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="83" t="s">
         <v>356</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -14411,18 +15141,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="83" t="s">
         <v>365</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -14447,20 +15177,20 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="79" t="s">
         <v>369</v>
       </c>
-      <c r="B5" s="92" t="s">
+      <c r="B5" s="96" t="s">
         <v>372</v>
       </c>
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="79" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="76"/>
-      <c r="B6" s="94"/>
-      <c r="C6" s="76"/>
+      <c r="A6" s="80"/>
+      <c r="B6" s="98"/>
+      <c r="C6" s="80"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A7" s="59" t="s">
@@ -14474,67 +15204,67 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="79" t="s">
         <v>376</v>
       </c>
-      <c r="B8" s="92" t="s">
+      <c r="B8" s="96" t="s">
         <v>375</v>
       </c>
-      <c r="C8" s="75" t="s">
+      <c r="C8" s="79" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="86"/>
-      <c r="B9" s="93"/>
-      <c r="C9" s="86"/>
+      <c r="A9" s="90"/>
+      <c r="B9" s="97"/>
+      <c r="C9" s="90"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="76"/>
-      <c r="B10" s="94"/>
-      <c r="C10" s="76"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="98"/>
+      <c r="C10" s="80"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="75" t="s">
+      <c r="A11" s="79" t="s">
         <v>378</v>
       </c>
-      <c r="B11" s="92" t="s">
+      <c r="B11" s="96" t="s">
         <v>384</v>
       </c>
-      <c r="C11" s="75" t="s">
+      <c r="C11" s="79" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="86"/>
-      <c r="B12" s="93"/>
-      <c r="C12" s="86"/>
+      <c r="A12" s="90"/>
+      <c r="B12" s="97"/>
+      <c r="C12" s="90"/>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="187" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="76"/>
-      <c r="B13" s="94"/>
-      <c r="C13" s="76"/>
+      <c r="A13" s="80"/>
+      <c r="B13" s="98"/>
+      <c r="C13" s="80"/>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="75" t="s">
+      <c r="A14" s="79" t="s">
         <v>380</v>
       </c>
-      <c r="B14" s="92" t="s">
+      <c r="B14" s="96" t="s">
         <v>383</v>
       </c>
-      <c r="C14" s="75" t="s">
+      <c r="C14" s="79" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="86"/>
-      <c r="B15" s="93"/>
-      <c r="C15" s="86"/>
+      <c r="A15" s="90"/>
+      <c r="B15" s="97"/>
+      <c r="C15" s="90"/>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="76"/>
-      <c r="B16" s="94"/>
-      <c r="C16" s="76"/>
+      <c r="A16" s="80"/>
+      <c r="B16" s="98"/>
+      <c r="C16" s="80"/>
     </row>
     <row r="17" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
@@ -14597,18 +15327,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="83" t="s">
         <v>395</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -14631,217 +15361,217 @@
       <c r="C4" s="60"/>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="79" t="s">
         <v>397</v>
       </c>
-      <c r="B5" s="97" t="s">
+      <c r="B5" s="101" t="s">
         <v>396</v>
       </c>
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="79" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="283" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="86"/>
-      <c r="B6" s="98"/>
-      <c r="C6" s="86"/>
+      <c r="A6" s="90"/>
+      <c r="B6" s="102"/>
+      <c r="C6" s="90"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="86"/>
-      <c r="B7" s="98"/>
-      <c r="C7" s="86"/>
+      <c r="A7" s="90"/>
+      <c r="B7" s="102"/>
+      <c r="C7" s="90"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="86"/>
-      <c r="B8" s="98"/>
-      <c r="C8" s="86"/>
+      <c r="A8" s="90"/>
+      <c r="B8" s="102"/>
+      <c r="C8" s="90"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="86"/>
-      <c r="B9" s="98"/>
-      <c r="C9" s="86"/>
+      <c r="A9" s="90"/>
+      <c r="B9" s="102"/>
+      <c r="C9" s="90"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="86"/>
-      <c r="B10" s="98"/>
-      <c r="C10" s="86"/>
+      <c r="A10" s="90"/>
+      <c r="B10" s="102"/>
+      <c r="C10" s="90"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="86"/>
-      <c r="B11" s="98"/>
-      <c r="C11" s="86"/>
+      <c r="A11" s="90"/>
+      <c r="B11" s="102"/>
+      <c r="C11" s="90"/>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="76"/>
-      <c r="B12" s="99"/>
-      <c r="C12" s="76"/>
+      <c r="A12" s="80"/>
+      <c r="B12" s="103"/>
+      <c r="C12" s="80"/>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="75" t="s">
+      <c r="A13" s="79" t="s">
         <v>399</v>
       </c>
-      <c r="B13" s="80" t="s">
+      <c r="B13" s="84" t="s">
         <v>400</v>
       </c>
-      <c r="C13" s="75" t="s">
+      <c r="C13" s="79" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="86"/>
-      <c r="B14" s="81"/>
-      <c r="C14" s="86"/>
+      <c r="A14" s="90"/>
+      <c r="B14" s="85"/>
+      <c r="C14" s="90"/>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="86"/>
-      <c r="B15" s="81"/>
-      <c r="C15" s="86"/>
+      <c r="A15" s="90"/>
+      <c r="B15" s="85"/>
+      <c r="C15" s="90"/>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="86"/>
-      <c r="B16" s="80" t="s">
+      <c r="A16" s="90"/>
+      <c r="B16" s="84" t="s">
         <v>401</v>
       </c>
-      <c r="C16" s="86"/>
+      <c r="C16" s="90"/>
     </row>
     <row r="17" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="86"/>
-      <c r="B17" s="81"/>
-      <c r="C17" s="86"/>
+      <c r="A17" s="90"/>
+      <c r="B17" s="85"/>
+      <c r="C17" s="90"/>
     </row>
     <row r="18" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="86"/>
-      <c r="B18" s="81"/>
-      <c r="C18" s="86"/>
+      <c r="A18" s="90"/>
+      <c r="B18" s="85"/>
+      <c r="C18" s="90"/>
     </row>
     <row r="19" spans="1:3" s="13" customFormat="1" ht="159" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="86"/>
-      <c r="B19" s="81"/>
-      <c r="C19" s="86"/>
+      <c r="A19" s="90"/>
+      <c r="B19" s="85"/>
+      <c r="C19" s="90"/>
     </row>
     <row r="20" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="86"/>
-      <c r="B20" s="81" t="s">
+      <c r="A20" s="90"/>
+      <c r="B20" s="85" t="s">
         <v>402</v>
       </c>
-      <c r="C20" s="86"/>
+      <c r="C20" s="90"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="86"/>
-      <c r="B21" s="81"/>
-      <c r="C21" s="86"/>
+      <c r="A21" s="90"/>
+      <c r="B21" s="85"/>
+      <c r="C21" s="90"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="86"/>
-      <c r="B22" s="81"/>
-      <c r="C22" s="86"/>
+      <c r="A22" s="90"/>
+      <c r="B22" s="85"/>
+      <c r="C22" s="90"/>
     </row>
     <row r="23" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="86"/>
-      <c r="B23" s="81"/>
-      <c r="C23" s="86"/>
+      <c r="A23" s="90"/>
+      <c r="B23" s="85"/>
+      <c r="C23" s="90"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="86"/>
-      <c r="B24" s="81" t="s">
+      <c r="A24" s="90"/>
+      <c r="B24" s="85" t="s">
         <v>403</v>
       </c>
-      <c r="C24" s="86"/>
+      <c r="C24" s="90"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="86"/>
-      <c r="B25" s="81"/>
-      <c r="C25" s="86"/>
+      <c r="A25" s="90"/>
+      <c r="B25" s="85"/>
+      <c r="C25" s="90"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="86"/>
-      <c r="B26" s="81" t="s">
+      <c r="A26" s="90"/>
+      <c r="B26" s="85" t="s">
         <v>317</v>
       </c>
-      <c r="C26" s="86"/>
+      <c r="C26" s="90"/>
     </row>
     <row r="27" spans="1:3" ht="144" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="86"/>
-      <c r="B27" s="81"/>
-      <c r="C27" s="86"/>
+      <c r="A27" s="90"/>
+      <c r="B27" s="85"/>
+      <c r="C27" s="90"/>
     </row>
     <row r="28" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="86"/>
-      <c r="B28" s="81" t="s">
+      <c r="A28" s="90"/>
+      <c r="B28" s="85" t="s">
         <v>404</v>
       </c>
-      <c r="C28" s="86"/>
+      <c r="C28" s="90"/>
     </row>
     <row r="29" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="86"/>
-      <c r="B29" s="81"/>
-      <c r="C29" s="86"/>
+      <c r="A29" s="90"/>
+      <c r="B29" s="85"/>
+      <c r="C29" s="90"/>
     </row>
     <row r="30" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="86"/>
-      <c r="B30" s="81"/>
-      <c r="C30" s="86"/>
+      <c r="A30" s="90"/>
+      <c r="B30" s="85"/>
+      <c r="C30" s="90"/>
     </row>
     <row r="31" spans="1:3" ht="196" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="86"/>
-      <c r="B31" s="81"/>
-      <c r="C31" s="86"/>
+      <c r="A31" s="90"/>
+      <c r="B31" s="85"/>
+      <c r="C31" s="90"/>
     </row>
     <row r="32" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="86"/>
-      <c r="B32" s="81" t="s">
+      <c r="A32" s="90"/>
+      <c r="B32" s="85" t="s">
         <v>405</v>
       </c>
-      <c r="C32" s="86"/>
+      <c r="C32" s="90"/>
     </row>
     <row r="33" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="86"/>
-      <c r="B33" s="81"/>
-      <c r="C33" s="86"/>
+      <c r="A33" s="90"/>
+      <c r="B33" s="85"/>
+      <c r="C33" s="90"/>
     </row>
     <row r="34" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="86"/>
-      <c r="B34" s="81"/>
-      <c r="C34" s="86"/>
+      <c r="A34" s="90"/>
+      <c r="B34" s="85"/>
+      <c r="C34" s="90"/>
     </row>
     <row r="35" spans="1:3" ht="201" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="86"/>
-      <c r="B35" s="81"/>
-      <c r="C35" s="86"/>
+      <c r="A35" s="90"/>
+      <c r="B35" s="85"/>
+      <c r="C35" s="90"/>
     </row>
     <row r="36" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="86"/>
-      <c r="B36" s="81" t="s">
+      <c r="A36" s="90"/>
+      <c r="B36" s="85" t="s">
         <v>406</v>
       </c>
-      <c r="C36" s="86"/>
+      <c r="C36" s="90"/>
     </row>
     <row r="37" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="86"/>
-      <c r="B37" s="81"/>
-      <c r="C37" s="86"/>
+      <c r="A37" s="90"/>
+      <c r="B37" s="85"/>
+      <c r="C37" s="90"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="86"/>
-      <c r="B38" s="81"/>
-      <c r="C38" s="86"/>
+      <c r="A38" s="90"/>
+      <c r="B38" s="85"/>
+      <c r="C38" s="90"/>
     </row>
     <row r="39" spans="1:3" ht="239" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="86"/>
-      <c r="B39" s="81"/>
-      <c r="C39" s="86"/>
+      <c r="A39" s="90"/>
+      <c r="B39" s="85"/>
+      <c r="C39" s="90"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="86"/>
-      <c r="B40" s="81" t="s">
+      <c r="A40" s="90"/>
+      <c r="B40" s="85" t="s">
         <v>407</v>
       </c>
-      <c r="C40" s="86"/>
+      <c r="C40" s="90"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="76"/>
-      <c r="B41" s="82"/>
-      <c r="C41" s="76"/>
+      <c r="A41" s="80"/>
+      <c r="B41" s="86"/>
+      <c r="C41" s="80"/>
     </row>
     <row r="42" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A42" s="60" t="s">
@@ -14881,11 +15611,11 @@
       <c r="C46" s="60"/>
     </row>
     <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A47" s="79" t="s">
+      <c r="A47" s="83" t="s">
         <v>386</v>
       </c>
-      <c r="B47" s="79"/>
-      <c r="C47" s="79"/>
+      <c r="B47" s="83"/>
+      <c r="C47" s="83"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
@@ -14899,25 +15629,25 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="75" t="s">
+      <c r="A49" s="79" t="s">
         <v>388</v>
       </c>
-      <c r="B49" s="77" t="s">
+      <c r="B49" s="81" t="s">
         <v>413</v>
       </c>
-      <c r="C49" s="75" t="s">
+      <c r="C49" s="79" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="86"/>
-      <c r="B50" s="96"/>
-      <c r="C50" s="86"/>
+      <c r="A50" s="90"/>
+      <c r="B50" s="100"/>
+      <c r="C50" s="90"/>
     </row>
     <row r="51" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="76"/>
-      <c r="B51" s="78"/>
-      <c r="C51" s="76"/>
+      <c r="A51" s="80"/>
+      <c r="B51" s="82"/>
+      <c r="C51" s="80"/>
     </row>
     <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="54" t="s">
@@ -14931,91 +15661,91 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="75" t="s">
+      <c r="A53" s="79" t="s">
         <v>415</v>
       </c>
-      <c r="B53" s="95" t="s">
+      <c r="B53" s="99" t="s">
         <v>416</v>
       </c>
-      <c r="C53" s="75" t="s">
+      <c r="C53" s="79" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="238" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="86"/>
-      <c r="B54" s="95"/>
-      <c r="C54" s="86"/>
+      <c r="A54" s="90"/>
+      <c r="B54" s="99"/>
+      <c r="C54" s="90"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="86"/>
-      <c r="B55" s="77" t="s">
+      <c r="A55" s="90"/>
+      <c r="B55" s="81" t="s">
         <v>417</v>
       </c>
-      <c r="C55" s="86"/>
+      <c r="C55" s="90"/>
     </row>
     <row r="56" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="86"/>
-      <c r="B56" s="96"/>
-      <c r="C56" s="86"/>
+      <c r="A56" s="90"/>
+      <c r="B56" s="100"/>
+      <c r="C56" s="90"/>
     </row>
     <row r="57" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="86"/>
-      <c r="B57" s="96"/>
-      <c r="C57" s="86"/>
+      <c r="A57" s="90"/>
+      <c r="B57" s="100"/>
+      <c r="C57" s="90"/>
     </row>
     <row r="58" spans="1:3" ht="172" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="86"/>
-      <c r="B58" s="78"/>
-      <c r="C58" s="86"/>
+      <c r="A58" s="90"/>
+      <c r="B58" s="82"/>
+      <c r="C58" s="90"/>
     </row>
     <row r="59" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="86"/>
-      <c r="B59" s="77" t="s">
+      <c r="A59" s="90"/>
+      <c r="B59" s="81" t="s">
         <v>418</v>
       </c>
-      <c r="C59" s="86"/>
+      <c r="C59" s="90"/>
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="86"/>
-      <c r="B60" s="96"/>
-      <c r="C60" s="86"/>
+      <c r="A60" s="90"/>
+      <c r="B60" s="100"/>
+      <c r="C60" s="90"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="86"/>
-      <c r="B61" s="96"/>
-      <c r="C61" s="86"/>
+      <c r="A61" s="90"/>
+      <c r="B61" s="100"/>
+      <c r="C61" s="90"/>
     </row>
     <row r="62" spans="1:3" ht="125" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="86"/>
-      <c r="B62" s="78"/>
-      <c r="C62" s="86"/>
+      <c r="A62" s="90"/>
+      <c r="B62" s="82"/>
+      <c r="C62" s="90"/>
     </row>
     <row r="63" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="86"/>
-      <c r="B63" s="77" t="s">
+      <c r="A63" s="90"/>
+      <c r="B63" s="81" t="s">
         <v>419</v>
       </c>
-      <c r="C63" s="86"/>
+      <c r="C63" s="90"/>
     </row>
     <row r="64" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="86"/>
-      <c r="B64" s="96"/>
-      <c r="C64" s="86"/>
+      <c r="A64" s="90"/>
+      <c r="B64" s="100"/>
+      <c r="C64" s="90"/>
     </row>
     <row r="65" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="86"/>
-      <c r="B65" s="96"/>
-      <c r="C65" s="86"/>
+      <c r="A65" s="90"/>
+      <c r="B65" s="100"/>
+      <c r="C65" s="90"/>
     </row>
     <row r="66" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="86"/>
-      <c r="B66" s="96"/>
-      <c r="C66" s="86"/>
+      <c r="A66" s="90"/>
+      <c r="B66" s="100"/>
+      <c r="C66" s="90"/>
     </row>
     <row r="67" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="76"/>
-      <c r="B67" s="78"/>
-      <c r="C67" s="76"/>
+      <c r="A67" s="80"/>
+      <c r="B67" s="82"/>
+      <c r="C67" s="80"/>
     </row>
     <row r="68" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A68" s="60" t="s">

</xml_diff>

<commit_message>
Implementation of index.html landing page and associated js and css files.
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A71396-0F63-CB43-84AE-26B0AFDDC1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1772F940-AF06-E541-8E7B-13AFE897B2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="1000" windowWidth="27640" windowHeight="16160" firstSheet="3" activeTab="11" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27640" windowHeight="16160" firstSheet="4" activeTab="12" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="SPEC - 1.1" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,10 @@
     <sheet name="SPEC - 1.10" sheetId="14" r:id="rId10"/>
     <sheet name="SPEC - 1.11" sheetId="15" r:id="rId11"/>
     <sheet name="SPEC - 2.0" sheetId="16" r:id="rId12"/>
-    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId13"/>
-    <sheet name="PLAYGROUND" sheetId="6" r:id="rId14"/>
-    <sheet name="TEMPLATE" sheetId="8" r:id="rId15"/>
+    <sheet name="SPEC - 2.1" sheetId="17" r:id="rId13"/>
+    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId14"/>
+    <sheet name="PLAYGROUND" sheetId="6" r:id="rId15"/>
+    <sheet name="TEMPLATE" sheetId="8" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="540">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -10268,6 +10269,1272 @@
         <family val="1"/>
       </rPr>
       <t xml:space="preserve"> nothing to commit, working tree clean</t>
+    </r>
+  </si>
+  <si>
+    <t>touch css/global.css</t>
+  </si>
+  <si>
+    <t>LANDING PAGE - index.html AND ASSOCIATED js AND css</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create thecss file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/global.css</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ls css </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">displays the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>global.css</t>
+    </r>
+  </si>
+  <si>
+    <t>/* Door Type */
+const DOOR_TYPE = {
+    SLIDING_DOOR: "Sliding door",
+    SWING_DOOR: "Swing door"
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Created the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>DOOR_TYPE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> enumerated value for sliding and swing door in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lib/lang/en/enum/door/door-enum.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>DOOR_TYPE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> enumerated value for sliding and swing door in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lib/lang/en/enum/door/door-enum.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Freeze the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>DOOR_TYPE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> object in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lib/lang/en/enum/door/door-enum.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Froze the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>DOOR_TYPE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> object in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lib/lang/en/enum/door/door-enum.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller/lock-compatibility.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">ls js/controller </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> displays the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lock-compatibility.js</t>
+    </r>
+  </si>
+  <si>
+    <t>touch js/controller/lock-compatibility.js</t>
+  </si>
+  <si>
+    <t>use strict';
+/* * The Lock compatibility with specific door types of specified range
+ *  of thickness.
+ *  @author   Sanket Rajgarhia
+ *  @date 03/04/2022 (dd/mm/yyyy)
+ *  @version 1.0
+ * */
+/*****************************************************************************/
+/* FUNCTIONS                                                                 */
+/*****************************************************************************/
+/* The function forms an object containing  the door type and door thickness 
+ * range - determined by the lock model value.
+ * name input control. 
+ * @param    {LOCK_MODEL} lockModel The model of the lock
+ * @return   {Object}   An Object containing doorType and doorThickness
+ * */
+const lockCompatibility = (lockModel) =&gt; {
+    switch (lockModel) {
+        case LOCK_MODEL.DC1000:
+            return {
+                doorType: DOOR_TYPE.SWING_DOOR,
+                    doorThickness: DOOR_THICKNESS_IN_MM.MM_30_TO_50
+            };
+        case LOCK_MODEL.DH2000:
+            return {
+                doorType: DOOR_TYPE.SWING_DOOR,
+                    doorThickness: DOOR_THICKNESS_IN_MM.MM_32_TO_50
+            };
+        case LOCK_MODEL.DL6500:
+        case LOCK_MODEL.DL7000:
+        case LOCK_MODEL.DL7100:
+        case LOCK_MODEL.DL7900:
+        case LOCK_MODEL.EL6000:
+        case LOCK_MODEL.EL7200:
+        case LOCK_MODEL.EL7500:
+        case LOCK_MODEL.ER4900:
+        case LOCK_MODEL.ER5100:
+            return {
+                doorType: DOOR_TYPE.SWING_DOOR,
+                    doorThickness: DOOR_THICKNESS_IN_MM.MM_35_TO_50
+            };
+        case LOCK_MODEL.ER5200:
+            return {
+                doorType: DOOR_TYPE.SLIDING_DOOR,
+                    doorThickness: DOOR_THICKNESS_IN_MM.MM_35_TO_50
+            };
+        case LOCK_MODEL.DL7600:
+        case LOCK_MODEL.PP8100:
+        case LOCK_MODEL.PP9000:
+            return {
+                doorType: DOOR_TYPE.SWING_DOOR,
+                    doorThickness: DOOR_THICKNESS_IN_MM.MM_35_TO_60
+            };
+        case LOCK_MODEL.DL6600:
+            return {
+                doorType: DOOR_TYPE.SWING_DOOR + "/" + DOOR_TYPE.SLIDING_DOOR,
+                    doorThickness: DOOR_THICKNESS_IN_MM.MM_35_TO_90
+            };
+        default:
+            return {
+                doorType: "",
+                    doorThickness: ""
+            }
+    }
+}
+/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implement the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">lockCompatibility() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">function to return an object with the door type and door thickness range supported for the specified lock model - in the  file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>ls/controller/lock-compatibilty.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implemented the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">lockCompatibility() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">function to return an object with the door type and door thickness range supported for the specified lock model - in the  file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>ls/controller/lock-compatibilty.js</t>
+    </r>
+  </si>
+  <si>
+    <t>/* Thickness of the door */
+const DOOR_THICKNESS_IN_MM = {
+    MM_30_TO_50: "30-50 mm",
+    MM_32_TO_50: "32-50 mm",
+    MM_35_TO_50: "35-50 mm",
+    MM_35_TO_60: "35-60 mm",
+    MM_35_TO_90: "35-90 mm"
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>DOOR_THICKNESS_IN_MM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> object in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lib/lang/en/enum/door/door-enum.js. MM to mm.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>DOOR_THICKNESS_IN_MM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> object in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lib/lang/en/enum/door/door-enum.js. MM to mm.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Object.freeze(DOOR_THICKNESS_IN_MM);</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+Object.freeze(DOOR_TYPE);
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> assets/images/HAFELE-LOGO.jpg
+ assets/images/HAFELE-LOGO.psd</t>
+  </si>
+  <si>
+    <t>Search for the suitable hafele logo on the internet and download it</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Download the HAFELE logo jpg file to the folder </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>asstes/images</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Impement the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html/index.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> web page. The landing page has the option to select a lock and start the flow or alternatively proceed to lock selection.</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;!DOCTYPE html&gt;
+&lt;html lang="en"&gt;
+  &lt;head&gt;
+    &lt;!-- Required meta tags --&gt;
+    &lt;meta charset="UTF-8"&gt;
+    &lt;meta http-equiv="X-UA-Compatible" content="IE=edge"&gt;
+    &lt;meta name="viewport"
+      content="width=device-width, initial-scale=1.0, shrink-to-fit=no"&gt;
+    &lt;!-- Bootstrap v 4.6.0 Style Sheet --&gt;
+    &lt;link rel="stylesheet"
+      href="https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/css/bootstrap.min.css"
+      integrity="sha384-B0vP5xmATw1+K9KRQjQERJvTumQW0nPEzvF6L/Z6nronJ3oUOFUFpCjEUQouq2+l"
+      crossorigin="anonymous"&gt;
+    &lt;!-- Custom Styles CSS --&gt;
+    &lt;link rel="stylesheet" type="text/css" href="./../css/global.css"&gt;
+    &lt;link rel="stylesheet" type="text/css" href="./../css/index.css"&gt;
+    &lt;!-- Font Awesome Kit --&gt;
+    &lt;script src="https://kit.fontawesome.com/94f1334f9a.js"
+      crossorigin="anonymous"&gt;&lt;/script&gt;
+    &lt;!-- Google Fonts --&gt;
+    &lt;link rel="preconnect" href="https://fonts.googleapis.com"&gt;
+    &lt;link rel="preconnect" href="https://fonts.gstatic.com" crossorigin&gt;
+    &lt;link
+      href="https://fonts.googleapis.com/css2?family=Noto+Sans+JP&amp;display=swap"
+      rel="stylesheet"&gt;
+    &lt;!-- Favicon --&gt;
+    &lt;link rel="shortcut icon" type="image/ico"
+      href="./../favicon/favicon.ico" /&gt;
+    &lt;!-- Page Title --&gt;
+    &lt;title&gt;Lock Selection Survey&lt;/title&gt;
+  &lt;/head&gt;
+  &lt;body&gt;
+    &lt;!-- Page Header --&gt;
+    &lt;div id="page-header" class="container-fluid"&gt;
+    &lt;/div&gt;
+    &lt;!-- End Page Header --&gt;
+    &lt;!-- Hafele Logo --&gt;
+    &lt;div id="hafele-logo"&gt;
+      &lt;img id="hafele-logo-img" src="./../assets/images/HAFELE-LOGO.jpg"
+        alt="Hafele"&gt;
+    &lt;/div&gt;
+    &lt;!-- End Hafele Logo --&gt;
+    &lt;!-- Main container --&gt;
+    &lt;div id="page-body" class="container"&gt;
+      &lt;!-- Row 1  --&gt;
+      &lt;div class="row"&gt;
+        &lt;!-- Row 1 Column 1 --&gt;
+        &lt;div class="col-lg-6 col-md-6 col-margin"&gt;
+          &lt;!-- Lock Selection Card --&gt;
+          &lt;div class="card h-100"&gt;
+            &lt;!-- Lock Selection Card Header --&gt;
+            &lt;div class="card-header card-header-extended"&gt;
+              &lt;h5&gt;Lock Model Lookup&lt;/h5&gt;
+            &lt;/div&gt;
+            &lt;!-- End Lock Selection Card Header --&gt;
+            &lt;!-- Lock Selection Card Body --&gt;
+            &lt;div class="card-body"&gt;
+              &lt;!-- Lock Model Selection Field --&gt;
+              &lt;div id="lock-model-selection-div" class="input-group form-group"&gt;
+                &lt;div class="input-group-prepend"&gt;
+                  &lt;span class="input-group-text"&gt;&lt;i
+                      class="fa-solid fa-lock"&gt;&lt;/i&gt;&lt;/span&gt;
+                &lt;/div&gt;
+                &lt;select id="lockModelGroup"
+                  class="custom-select custom-select-extended"&gt;
+                  &lt;option value="" selected&gt;Select a lock model&lt;/option&gt;
+                &lt;/select&gt;
+              &lt;/div&gt;
+              &lt;!-- End Lock Model Selection Field --&gt;
+              &lt;div id="suggestion" class="hide-suggestion"&gt;
+                &lt;p id="suitability-message"&gt;This lock is suitable for the
+                  following door type&lt;/p&gt;
+                &lt;p id="door-type"&gt;&lt;span class="field-name"&gt;Door Type :
+                  &lt;/span&gt;&lt;span id="type-value"&gt;&lt;/span&gt;&lt;/p&gt;
+                &lt;p id="door-thickness"&gt;&lt;span class="field-name"&gt;Door Thickness
+                    Range : &lt;/span&gt;&lt;span id="thickness-value"&gt;&lt;/span&gt;&lt;/p&gt;
+              &lt;/div&gt;
+            &lt;/div&gt;
+            &lt;!-- End Lock Selection Card Body --&gt;
+            &lt;!-- Lock Selection Card Footer --&gt;
+            &lt;div class="card-footer text-center card-footer-extended"&gt;
+              &lt;form action="./lock-selection-survey.html"&gt;
+                &lt;input id="lock-selection-next" class="btn btn-success"
+                  type="submit" value="     Select     "&gt;
+              &lt;/form&gt;
+            &lt;/div&gt;
+            &lt;!-- End Lock Selection Card Footer --&gt;
+          &lt;/div&gt;
+          &lt;!-- End Lock Selection Card --&gt;
+        &lt;/div&gt;
+        &lt;!-- End Row 1 Column 1 --&gt;
+        &lt;!-- Row 1 Column 2 --&gt;
+        &lt;div class="col-lg-6 col-md-6 col-margin"&gt;
+          &lt;!-- Door Specification Card --&gt;
+          &lt;div class="card h-100"&gt;
+            &lt;!-- Door Specification Card Header --&gt;
+            &lt;div class="card-header card-header-extended"&gt;
+              &lt;h5&gt;Door Specification&lt;/h5&gt;
+            &lt;/div&gt;
+            &lt;!-- End Door Specification Card Header --&gt;
+            &lt;!-- Door Specification Card Body --&gt;
+            &lt;div class="card-body"&gt;
+              &lt;div id="message"&gt;
+                &lt;p&gt;Click on the &lt;span class="highlight-text"&gt;Next&lt;/span&gt; button
+                  and provide the door specification to determine the
+                  suitability of a lock model.&lt;/p&gt;
+              &lt;/div&gt;
+            &lt;/div&gt;
+            &lt;!-- End Door Specification Card Body --&gt;
+            &lt;!-- Door Specification Card Footer --&gt;
+            &lt;div class="card-footer text-center card-footer-extended"&gt;
+              &lt;form action="./lock-selection-survey.html"&gt;
+                &lt;input id="door-specification-next" class="btn btn-primary"
+                  type="submit" value="      Next      "&gt;
+              &lt;/form&gt;
+            &lt;/div&gt;
+            &lt;!-- End Door Specification Card Footer --&gt;
+          &lt;/div&gt;
+          &lt;!-- End Door Specification Card --&gt;
+        &lt;/div&gt;
+        &lt;!-- End Row 1 Column 2 --&gt;
+      &lt;/div&gt;
+      &lt;!-- End Row 1  --&gt;
+    &lt;/div&gt;
+    &lt;!-- End Main container --&gt;
+    &lt;!-- Spacer div --&gt;
+    &lt;div id="spacer"&gt;
+      &lt;!-- A &lt;div&gt; having the same heigh as the &lt;footer&gt; tag to prevent contents of &lt;body&gt;
+        from going under the absolutely positioned &lt;footer&gt; tag when screen resizes. --&gt;
+    &lt;/div&gt;
+    &lt;!-- End div --&gt;
+    &lt;!-- Page Footer --&gt;
+    &lt;footer id="page-footer" class="container-fluid" text-center&gt;
+      &lt;p class="copyright"&gt;Copyright © Hafele 2022&lt;/p&gt;
+    &lt;/footer&gt;
+    &lt;!-- End Page Footer --&gt;
+    &lt;!-- Bootstrap v 4.6.0 javascript --&gt;
+    &lt;script src="https://code.jquery.com/jquery-3.5.1.slim.min.js"
+      integrity="sha384-DfXdz2htPH0lsSSs5nCTpuj/zy4C+OGpamoFVy38MVBnE+IbbVYUew+OrCXaRkfj"
+      crossorigin="anonymous"&gt;
+    &lt;/script&gt;
+    &lt;script
+      src="https://cdn.jsdelivr.net/npm/popper.js@1.16.1/dist/umd/popper.min.js"
+      integrity="sha384-9/reFTGAW83EW2RDu2S0VKaIzap3H66lZH81PoYlFhbGU+6BZp6G7niu735Sk7lN"
+      crossorigin="anonymous"&gt;
+    &lt;/script&gt;
+    &lt;script
+      src="https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/js/bootstrap.min.js"
+      integrity="sha384-+YQ4JLhjyBLPDQt//I+STsc9iw4uQqACwlvpslubQzn4u2UU2UFM80nGisd026JF"
+      crossorigin="anonymous"&gt;
+    &lt;/script&gt;
+    &lt;!-- Information Capture Javascript --&gt;
+    &lt;script src="https://apis.google.com/js/api.js"&gt;&lt;/script&gt;
+    &lt;script src="./../lib/lang/en/enum/door/door-enum.js"
+      type="text/javascript"&gt;&lt;/script&gt;
+    &lt;script src="./../lib/lang/en/enum/lock/lock-enum.js"
+      type="text/javascript"&gt;&lt;/script&gt;
+    &lt;script src="./../js/controller/lock-compatibility.js"
+      type="text/javascript"&gt;&lt;/script&gt;
+    &lt;script src="./../js/controller/index.js" type="text/javascript"&gt;&lt;/script&gt;
+  &lt;/body&gt;
+&lt;/html&gt;</t>
+  </si>
+  <si>
+    <t>"use strict";
+/* * JavaScript for the file index.html
+ *  @author Sanket Rajgarhia
+ *  @date   03/04/2022 (dd/mm/yyyy)
+ *  @version 1.0
+ * */
+/*****************************************************************************/
+/* GLOBAL VARIABLES                                                        */
+/*****************************************************************************/
+// Global variable - associated with the - lock model select control
+let lockModelSelectionGroup = document.getElementById("lockModelGroup");
+// Global variable - associated with the - lock model selection next button
+let lockSelectionNextButton = document.getElementById("lock-selection-next");
+// Global variable - associated with the - door specification next button
+let doorSpecificationNextButton = document.getElementById(
+    "door-specification-next");
+/*****************************************************************************/
+/* WINDOWS ONLOAD                                                            */
+/*****************************************************************************/
+/* Anonymous function fired on window load. 
+ * @param    
+ * @return   
+ * */
+window.onload = function() {
+    // Add all the lock model names to the lock model group selection combo box
+    Object.keys(LOCK_MODEL).forEach(key =&gt; {
+        let optionTag = document.createElement("option");
+        optionTag.setAttribute("value", LOCK_MODEL[key])
+        let lockTextNode = document.createTextNode(LOCK_MODEL[key]);
+        optionTag.appendChild(lockTextNode);
+        lockModelSelectionGroup.appendChild(optionTag);
+    });
+    //If storage data is found -  set the lock model select control to have
+    // the value of the selected lock and display the door type and door
+    // thickness suggestions.
+    // Delete the session storage items and enable the selection button.
+    // This scenario check if the user has pressed the back button of the
+    // browser to reach this page.
+    if (sessionStorage.getItem('lockModelSelected') !== null) {
+        // Set the lock model select control to have the value of the
+        // previously selected lock
+        lockModelSelectionGroup.value = sessionStorage.getItem(
+            'lockModelSelected');
+        // Fetch the object specifying the door type and door thickness range
+        let lock = lockCompatibility(
+            lockModelSelectionGroup.value.toUpperCase());
+        // Display the door type and door thickness suggestion &lt;div&gt;
+        let suggestionDiv = document.getElementById("suggestion");
+        let doorTypeValueElement = document.getElementById("type-value");
+        let doorThicknessValueElement = document.getElementById("thickness-value");
+        suggestionDiv.classList.remove("hide-suggestion");
+        let text = document.createTextNode(lock.doorType);
+        doorTypeValueElement.appendChild(text);
+        text = document.createTextNode(lock.doorThickness);
+        doorThicknessValueElement.appendChild(text);
+        // Delete the session storage items
+        sessionStorage.removeItem('lockModelSelected');
+        sessionStorage.removeItem('compatibleDoor');
+        // Enable the lock model selection next button
+        lockSelectionNextButton.disabled = false;
+    } else {
+        // Ensure that no lock models are selected by default
+        lockModelSelectionGroup.options[0].selected = true
+        // Ensure that the lock model selection next button is disabled by default
+        lockSelectionNextButton.disabled = true;
+    }
+};
+/*****************************************************************************/
+/* EVENT LISTENER - CALLBACKS                                                */
+/*****************************************************************************/
+/* The callback function fired on 'change' - for lock model select control. 
+ * @param    
+ * @return   
+ * */
+const lockSelectionOnChange = (event) =&gt; {
+    // The suggestion &lt;div&gt; element
+    let suggestionDiv = document.getElementById("suggestion");
+    // The &lt;span&gt; elements withing the suggestion &lt;div&gt; to display value for 
+    // the door type and door thickness range
+    let doorTypeValueElement = document.getElementById("type-value");
+    let doorThicknessValueElement = document.getElementById("thickness-value");
+    // Reset the door type and door thickness values
+    doorTypeValueElement.innerHTML = "";
+    doorThicknessValueElement.innerHTML = "";
+    // If a valid door model has been selected
+    if (lockModelSelectionGroup.selectedIndex &gt; 0) {
+        // Enable the lock model selection next button
+        lockSelectionNextButton.disabled = false;
+        // Display the door type and door thickness suggestion &lt;div&gt;
+        suggestionDiv.classList.remove("hide-suggestion");
+        // Fetch the object specifying the door type and door thickness range
+        let lock = lockCompatibility(
+            lockModelSelectionGroup.value.toUpperCase());
+        // Display the suggestion
+        let text = document.createTextNode(lock.doorType);
+        doorTypeValueElement.appendChild(text);
+        text = document.createTextNode(lock.doorThickness);
+        doorThicknessValueElement.appendChild(text);
+    } // No valid door model is selected
+    else {
+        // Enable the lock model selection next button
+        lockSelectionNextButton.disabled = true;
+        // Hide the door type and door thickness suggestion &lt;div&gt;
+        suggestionDiv.classList.add("hide-suggestion");
+    }
+}
+/* The callback function fired on 'click' - for lock model next button control.
+ * @param    
+ * @return   
+ * */
+const loadSurveyPageOnClick = () =&gt; {
+    // Save the selected lock and associated door type and door thickness
+    // range object to the session storage
+    sessionStorage.setItem('lockModelSelected', lockModelSelectionGroup.value);
+    sessionStorage.setItem('compatibleDoor',
+        JSON.stringify(lockCompatibility(
+            lockModelSelectionGroup.value.toUpperCase())));
+}
+/* The callback function fired on 'click' - for door specification 
+ * next button control.
+ * @param    
+ * @return   
+ * */
+const loadSurveyPageOnSpecificationClick = () =&gt; {
+    // Ensure that no lock models are selected by default
+    lockModelSelectionGroup.options[0].selected = true
+    // Remove all data from session store
+    sessionStorage.removeItem('lockModelSelected');
+    sessionStorage.removeItem('compatibleDoor');
+}
+/*****************************************************************************/
+/* REGISTER EVENT LISTENERS                                                  */
+/*****************************************************************************/
+// Event listeners registered for the lock model select control
+lockModelSelectionGroup.addEventListener("change", lockSelectionOnChange);
+// Event listeners registered for the lock model selection next button
+lockSelectionNextButton.addEventListener("click", loadSurveyPageOnClick);
+// Event listeners registered for the door specification next button
+doorSpecificationNextButton.addEventListener("click",
+    loadSurveyPageOnSpecificationClick);
+/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implement the javascript for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">html/index.html </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller/index.html</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Impemented the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html/index.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> web page. The landing page has the option to select a lock and start the flow or alternatively proceed to lock selection.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implemented the javascript for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">html/index.html </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller/index.html</t>
+    </r>
+  </si>
+  <si>
+    <t>/* * CSS for all web pages.
+ *  @author Sanket Rajgarhia
+ *  @date   03/04/2022 (dd/mm/yyyy)
+ *  @version 1.0
+ * */
+/*****************************************************************************/
+/* TOP LEVEL TAGS - &lt;html&gt; &lt;header&gt; and &lt;body&gt;                               */
+/*****************************************************************************/
+/* &lt;html&gt;, &lt;header&gt; and &lt;body&gt; tags */
+html,
+header,
+body {
+    background-color: #F9F9F9;
+    font-size: 1rem;
+    font-weight: 400;
+    min-height: 100vh;
+    min-width: 100vw;
+    padding: 0;
+}
+/* &lt;body&gt; needs to be relatively positioned to accommodate the absolutely
+positioned footer tag */
+body {
+    position: relative;
+}
+/*****************************************************************************/
+/* HEADER AND FOOTER SECTION                                                 */
+/*****************************************************************************/
+/* The page header */
+#page-header {
+    background-color: black;
+    min-height: 10vh;
+}
+/* The spacer div has the same minimum height as that of the absolutely
+positioned page footer to prevent contents of the body div from going
+under the absolutely positioned footer div - when screen resizes */
+#spacer {
+    min-height: 5vh;
+}
+/* The page footer */
+#page-footer {
+    background-color: black;
+    color: white;
+    text-align: center;
+    vertical-align: middle;
+    line-height: 40px;
+    position: absolute;
+    bottom: 0;
+    max-height: 5vh;
+}
+/* Copy right information in the footer */
+.copyright {
+    font-size: 0.7rem;
+}
+/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implement the styles to be used globally by all the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> files in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/global.css</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implemented the styles to be used globally by all the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> files in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/global.css</t>
+    </r>
+  </si>
+  <si>
+    <t>/* * CSS for the file index.html
+ *  @author Sanket Rajgarhia
+ *  @date   03/04/2022 (dd/mm/yyyy)
+ *  @version 1.0
+ * */
+/*****************************************************************************/
+/* HTML TAGS                                                                 */
+/*****************************************************************************/
+h5 {
+    font-size: 1rem;
+}
+/*****************************************************************************/
+/* HAFELE LOGO - &lt;div&gt; and containing &lt;img&gt; tag                              */
+/*****************************************************************************/
+/* Ensure that the &lt;div&gt; stretches across the full width of the screen */
+#hafele-logo {
+    background-color: white;
+    text-align: center;
+    width: 100vw;
+}
+/* Ensure that the Hafele logo image fills the container &lt;div&gt; */
+#hafele-logo-img {
+    border: 1px solid white;
+    width: 60vw;
+    object-fit: fill;
+}
+/*****************************************************************************/
+/* page-body - CONTAINER DIV                                                 */
+/*****************************************************************************/
+/* Provide spacing to the body from the Hafele Logo section */
+#page-body {
+    font-family: 'Noto Sans JP', sans-serif;
+    font-size: calc(10px + (14 - 10) * ((100vw - 500px) / (1200 - 300))) !important;
+    padding-top: 5%;
+}
+/*****************************************************************************/
+/* GENERAL CARDS STYLING                                                     */
+/*****************************************************************************/
+/* Provides the top and bottom margin for all columns (cards) being laid out in
+the layout grid. This is important when the cards collapse for smaller screens and
+stack vertically. */
+.col-margin {
+    margin-top: 0.8%;
+    margin-bottom: 0.8%;
+}
+/* Styling the card header */
+.card-header-extended {
+    background-color: rgb(41, 39, 39);
+    color: white;
+}
+/* Styling the card footer */
+.card-footer-extended {
+    border-top: 0px;
+}
+.custom-select-extended {
+    font-size: calc(10px + (14 - 10) * ((100vw - 500px) / (1200 - 300))) !important;
+}
+/*****************************************************************************/
+/* LOCK SELECTION STYLING                                                    */
+/*****************************************************************************/
+/* Hide the suggestion message - but ensure that it occupies space on the 
+page */
+.hide-suggestion {
+    visibility: hidden;
+}
+#suitability-message {
+    color: #343131b8;
+}
+p&gt;.field-name {
+    color: red;
+}
+/*****************************************************************************/
+/* DOOR SPECIFICATION STYLING                                                */
+/*****************************************************************************/
+.highlight-text {
+    color: red;
+}
+/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implement the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/index.css</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to style </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html/index.html</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implemented the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/index.css</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to style </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html/index.html</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>git commit -m "Implementation of index.html</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>landing page and associated js and css files."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>git status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - would display the following files.                                                                                                                                                                                                                                          On branch workflow
+Changes to be committed:
+  (use "git restore --staged &lt;file&gt;..." to unstage)
+        modified:   .vscode/settings.json
+        new file:   assets/images/HAFELE-LOGO.jpg
+        new file:   assets/images/HAFELE-LOGO.psd
+        new file:   css/global.css
+        modified:   css/index.css
+        modified:   docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+        modified:   html/index.html
+        modified:   js/controller/index.js
+        new file:   js/controller/lock-compatibility.js
+        modified:   lib/lang/en/enum/door/door-enum.js</t>
     </r>
   </si>
 </sst>
@@ -10688,7 +11955,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="116">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -10869,6 +12136,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -11309,18 +12582,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -11605,18 +12878,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="85" t="s">
         <v>426</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -11630,7 +12903,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="104" t="s">
+      <c r="A4" s="106" t="s">
         <v>438</v>
       </c>
       <c r="B4" s="48" t="s">
@@ -11641,7 +12914,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="105"/>
+      <c r="A5" s="107"/>
       <c r="B5" s="48" t="s">
         <v>441</v>
       </c>
@@ -11650,51 +12923,51 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="105"/>
+      <c r="A6" s="107"/>
       <c r="B6" s="48" t="s">
         <v>434</v>
       </c>
-      <c r="C6" s="107" t="s">
+      <c r="C6" s="109" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="105"/>
+      <c r="A7" s="107"/>
       <c r="B7" s="48" t="s">
         <v>435</v>
       </c>
-      <c r="C7" s="108"/>
+      <c r="C7" s="110"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="105"/>
+      <c r="A8" s="107"/>
       <c r="B8" s="48" t="s">
         <v>427</v>
       </c>
-      <c r="C8" s="108"/>
+      <c r="C8" s="110"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="105"/>
+      <c r="A9" s="107"/>
       <c r="B9" s="48" t="s">
         <v>428</v>
       </c>
-      <c r="C9" s="108"/>
+      <c r="C9" s="110"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="105"/>
+      <c r="A10" s="107"/>
       <c r="B10" s="48" t="s">
         <v>436</v>
       </c>
-      <c r="C10" s="108"/>
+      <c r="C10" s="110"/>
     </row>
     <row r="11" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="105"/>
+      <c r="A11" s="107"/>
       <c r="B11" s="48" t="s">
         <v>443</v>
       </c>
-      <c r="C11" s="109"/>
+      <c r="C11" s="111"/>
     </row>
     <row r="12" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="106"/>
+      <c r="A12" s="108"/>
       <c r="B12" s="48" t="s">
         <v>445</v>
       </c>
@@ -11833,18 +13106,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="85" t="s">
         <v>464</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -11937,7 +13210,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4437CF02-82B5-C74B-B6B5-F1F00EF2719A}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -11950,18 +13223,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="85" t="s">
         <v>478</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -12012,11 +13285,11 @@
       <c r="C8" s="54"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="83" t="s">
+      <c r="A9" s="85" t="s">
         <v>485</v>
       </c>
-      <c r="B9" s="83"/>
-      <c r="C9" s="83"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -12052,20 +13325,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="79" t="s">
+      <c r="A13" s="81" t="s">
         <v>490</v>
       </c>
-      <c r="B13" s="84" t="s">
+      <c r="B13" s="86" t="s">
         <v>489</v>
       </c>
-      <c r="C13" s="79" t="s">
+      <c r="C13" s="81" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="80"/>
-      <c r="B14" s="86"/>
-      <c r="C14" s="80"/>
+      <c r="A14" s="82"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="82"/>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="73" t="s">
@@ -12090,20 +13363,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="79" t="s">
+      <c r="A17" s="81" t="s">
         <v>499</v>
       </c>
-      <c r="B17" s="84" t="s">
+      <c r="B17" s="86" t="s">
         <v>498</v>
       </c>
-      <c r="C17" s="79" t="s">
+      <c r="C17" s="81" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="222" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="80"/>
-      <c r="B18" s="86"/>
-      <c r="C18" s="80"/>
+      <c r="A18" s="82"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="82"/>
     </row>
     <row r="19" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -12145,6 +13418,310 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1132A7EE-237B-8045-8FB6-82D91553ABA4}">
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="79" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="85" t="s">
+        <v>505</v>
+      </c>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" s="77" t="s">
+        <v>510</v>
+      </c>
+      <c r="B4" s="58" t="s">
+        <v>508</v>
+      </c>
+      <c r="C4" s="77" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A5" s="54" t="s">
+        <v>511</v>
+      </c>
+      <c r="B5" s="78" t="s">
+        <v>522</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="140" x14ac:dyDescent="0.2">
+      <c r="A6" s="54" t="s">
+        <v>520</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>519</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="54" t="s">
+        <v>513</v>
+      </c>
+      <c r="B7" s="78" t="s">
+        <v>515</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="81" t="s">
+        <v>517</v>
+      </c>
+      <c r="B8" s="86" t="s">
+        <v>516</v>
+      </c>
+      <c r="C8" s="81" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="92"/>
+      <c r="B9" s="87"/>
+      <c r="C9" s="92"/>
+    </row>
+    <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="82"/>
+      <c r="B10" s="88"/>
+      <c r="C10" s="82"/>
+    </row>
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="54" t="s">
+        <v>525</v>
+      </c>
+      <c r="B11" s="55" t="s">
+        <v>524</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="81" t="s">
+        <v>526</v>
+      </c>
+      <c r="B12" s="86" t="s">
+        <v>527</v>
+      </c>
+      <c r="C12" s="81" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="92"/>
+      <c r="B13" s="87"/>
+      <c r="C13" s="92"/>
+    </row>
+    <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="92"/>
+      <c r="B14" s="87"/>
+      <c r="C14" s="92"/>
+    </row>
+    <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="92"/>
+      <c r="B15" s="87"/>
+      <c r="C15" s="92"/>
+    </row>
+    <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="92"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="92"/>
+    </row>
+    <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="92"/>
+      <c r="B17" s="87"/>
+      <c r="C17" s="92"/>
+    </row>
+    <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="82"/>
+      <c r="B18" s="87"/>
+      <c r="C18" s="82"/>
+    </row>
+    <row r="19" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="81" t="s">
+        <v>529</v>
+      </c>
+      <c r="B19" s="86" t="s">
+        <v>528</v>
+      </c>
+      <c r="C19" s="81" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="92"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="92"/>
+    </row>
+    <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="92"/>
+      <c r="B21" s="87"/>
+      <c r="C21" s="92"/>
+    </row>
+    <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="92"/>
+      <c r="B22" s="87"/>
+      <c r="C22" s="92"/>
+    </row>
+    <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="92"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="92"/>
+    </row>
+    <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="92"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="92"/>
+    </row>
+    <row r="25" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="82"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="82"/>
+    </row>
+    <row r="26" spans="1:3" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="B26" s="48" t="s">
+        <v>504</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="81" t="s">
+        <v>533</v>
+      </c>
+      <c r="B27" s="86" t="s">
+        <v>532</v>
+      </c>
+      <c r="C27" s="81" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="92"/>
+      <c r="B28" s="87"/>
+      <c r="C28" s="92"/>
+    </row>
+    <row r="29" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="82"/>
+      <c r="B29" s="88"/>
+      <c r="C29" s="82"/>
+    </row>
+    <row r="30" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="81" t="s">
+        <v>536</v>
+      </c>
+      <c r="B30" s="86" t="s">
+        <v>535</v>
+      </c>
+      <c r="C30" s="81" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="92"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="92"/>
+    </row>
+    <row r="32" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="92"/>
+      <c r="B32" s="87"/>
+      <c r="C32" s="92"/>
+    </row>
+    <row r="33" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="82"/>
+      <c r="B33" s="88"/>
+      <c r="C33" s="82"/>
+    </row>
+    <row r="34" spans="1:3" ht="255" x14ac:dyDescent="0.2">
+      <c r="A34" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="53" t="s">
+        <v>538</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>503</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="17">
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="A12:A18"/>
+    <mergeCell ref="C12:C18"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="B19:B25"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="C19:C25"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="C27:C29"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE113606-3FFA-8545-9BE3-5643B52A7CE9}">
   <dimension ref="A1:H116"/>
   <sheetViews>
@@ -12222,10 +13799,10 @@
       <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="113" t="s">
+      <c r="A6" s="115" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="113"/>
+      <c r="B6" s="115"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -13198,32 +14775,32 @@
       <c r="H73" s="23"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="110"/>
-      <c r="B74" s="114"/>
+      <c r="A74" s="112"/>
+      <c r="B74" s="116"/>
       <c r="C74" s="32" t="s">
         <v>225</v>
       </c>
       <c r="D74" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="E74" s="115"/>
-      <c r="F74" s="110"/>
-      <c r="G74" s="112"/>
-      <c r="H74" s="110"/>
+      <c r="E74" s="117"/>
+      <c r="F74" s="112"/>
+      <c r="G74" s="114"/>
+      <c r="H74" s="112"/>
     </row>
     <row r="75" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A75" s="110"/>
-      <c r="B75" s="114"/>
+      <c r="A75" s="112"/>
+      <c r="B75" s="116"/>
       <c r="C75" s="33" t="s">
         <v>226</v>
       </c>
       <c r="D75" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="E75" s="115"/>
-      <c r="F75" s="110"/>
-      <c r="G75" s="112"/>
-      <c r="H75" s="110"/>
+      <c r="E75" s="117"/>
+      <c r="F75" s="112"/>
+      <c r="G75" s="114"/>
+      <c r="H75" s="112"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="23"/>
@@ -13396,34 +14973,34 @@
       <c r="H88" s="23"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="110"/>
-      <c r="B89" s="110"/>
+      <c r="A89" s="112"/>
+      <c r="B89" s="112"/>
       <c r="C89" s="35" t="s">
         <v>225</v>
       </c>
       <c r="D89" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="E89" s="111" t="s">
+      <c r="E89" s="113" t="s">
         <v>121</v>
       </c>
-      <c r="F89" s="111"/>
-      <c r="G89" s="112"/>
-      <c r="H89" s="110"/>
+      <c r="F89" s="113"/>
+      <c r="G89" s="114"/>
+      <c r="H89" s="112"/>
     </row>
     <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A90" s="110"/>
-      <c r="B90" s="110"/>
+      <c r="A90" s="112"/>
+      <c r="B90" s="112"/>
       <c r="C90" s="35" t="s">
         <v>242</v>
       </c>
       <c r="D90" s="35" t="s">
         <v>243</v>
       </c>
-      <c r="E90" s="111"/>
-      <c r="F90" s="111"/>
-      <c r="G90" s="112"/>
-      <c r="H90" s="110"/>
+      <c r="E90" s="113"/>
+      <c r="F90" s="113"/>
+      <c r="G90" s="114"/>
+      <c r="H90" s="112"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="23"/>
@@ -13809,7 +15386,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -13907,7 +15484,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0BB7-C151-C94B-945C-E2CA92034B13}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -13924,18 +15501,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="85" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -14052,18 +15629,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -14114,11 +15691,11 @@
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="83" t="s">
+      <c r="A9" s="85" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="83"/>
-      <c r="C9" s="83"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="85"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -14154,20 +15731,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="79" t="s">
+      <c r="A13" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="83" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="79" t="s">
+      <c r="C13" s="81" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="80"/>
-      <c r="B14" s="82"/>
-      <c r="C14" s="80"/>
+      <c r="A14" s="82"/>
+      <c r="B14" s="84"/>
+      <c r="C14" s="82"/>
     </row>
     <row r="15" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
@@ -14192,20 +15769,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="79" t="s">
+      <c r="A17" s="81" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="81" t="s">
+      <c r="B17" s="83" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="79" t="s">
+      <c r="C17" s="81" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="80"/>
-      <c r="B18" s="82"/>
-      <c r="C18" s="80"/>
+      <c r="A18" s="82"/>
+      <c r="B18" s="84"/>
+      <c r="C18" s="82"/>
     </row>
     <row r="19" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -14263,18 +15840,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="85" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -14310,25 +15887,25 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="79" t="s">
+      <c r="A6" s="81" t="s">
         <v>292</v>
       </c>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="86" t="s">
         <v>291</v>
       </c>
-      <c r="C6" s="79" t="s">
+      <c r="C6" s="81" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="90"/>
-      <c r="B7" s="85"/>
-      <c r="C7" s="90"/>
+      <c r="A7" s="92"/>
+      <c r="B7" s="87"/>
+      <c r="C7" s="92"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="80"/>
-      <c r="B8" s="86"/>
-      <c r="C8" s="80"/>
+      <c r="A8" s="82"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="82"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -14353,25 +15930,25 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="87" t="s">
+      <c r="A11" s="89" t="s">
         <v>294</v>
       </c>
-      <c r="B11" s="84" t="s">
+      <c r="B11" s="86" t="s">
         <v>295</v>
       </c>
-      <c r="C11" s="87" t="s">
+      <c r="C11" s="89" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="88"/>
-      <c r="B12" s="85"/>
-      <c r="C12" s="88"/>
+      <c r="A12" s="90"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="90"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="89"/>
-      <c r="B13" s="86"/>
-      <c r="C13" s="89"/>
+      <c r="A13" s="91"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="91"/>
     </row>
     <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
@@ -14428,18 +16005,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="85" t="s">
         <v>299</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -14453,46 +16030,46 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="93" t="s">
         <v>300</v>
       </c>
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="97" t="s">
         <v>305</v>
       </c>
-      <c r="C4" s="91" t="s">
+      <c r="C4" s="93" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="91"/>
-      <c r="B5" s="95"/>
-      <c r="C5" s="91"/>
+      <c r="A5" s="93"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="93"/>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="91"/>
-      <c r="B6" s="95"/>
-      <c r="C6" s="91"/>
+      <c r="A6" s="93"/>
+      <c r="B6" s="97"/>
+      <c r="C6" s="93"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="79" t="s">
+      <c r="A7" s="81" t="s">
         <v>302</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="94" t="s">
         <v>303</v>
       </c>
-      <c r="C7" s="79" t="s">
+      <c r="C7" s="81" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="90"/>
-      <c r="B8" s="93"/>
-      <c r="C8" s="90"/>
+      <c r="A8" s="92"/>
+      <c r="B8" s="95"/>
+      <c r="C8" s="92"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="228" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="80"/>
-      <c r="B9" s="94"/>
-      <c r="C9" s="80"/>
+      <c r="A9" s="82"/>
+      <c r="B9" s="96"/>
+      <c r="C9" s="82"/>
     </row>
     <row r="10" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
@@ -14549,18 +16126,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="85" t="s">
         <v>331</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -14607,233 +16184,233 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="79" t="s">
+      <c r="A7" s="81" t="s">
         <v>314</v>
       </c>
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="86" t="s">
         <v>322</v>
       </c>
-      <c r="C7" s="79" t="s">
+      <c r="C7" s="81" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="90"/>
-      <c r="B8" s="85"/>
-      <c r="C8" s="90"/>
+      <c r="A8" s="92"/>
+      <c r="B8" s="87"/>
+      <c r="C8" s="92"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="90"/>
-      <c r="B9" s="85"/>
-      <c r="C9" s="90"/>
+      <c r="A9" s="92"/>
+      <c r="B9" s="87"/>
+      <c r="C9" s="92"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="90"/>
-      <c r="B10" s="85"/>
-      <c r="C10" s="90"/>
+      <c r="A10" s="92"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="92"/>
     </row>
     <row r="11" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="90"/>
-      <c r="B11" s="85"/>
-      <c r="C11" s="90"/>
+      <c r="A11" s="92"/>
+      <c r="B11" s="87"/>
+      <c r="C11" s="92"/>
     </row>
     <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="90"/>
-      <c r="B12" s="85"/>
-      <c r="C12" s="90"/>
+      <c r="A12" s="92"/>
+      <c r="B12" s="87"/>
+      <c r="C12" s="92"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="80"/>
-      <c r="B13" s="86"/>
-      <c r="C13" s="80"/>
+      <c r="A13" s="82"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="82"/>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="81" t="s">
         <v>325</v>
       </c>
-      <c r="B14" s="84" t="s">
+      <c r="B14" s="86" t="s">
         <v>323</v>
       </c>
-      <c r="C14" s="79" t="s">
+      <c r="C14" s="81" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="90"/>
-      <c r="B15" s="85"/>
-      <c r="C15" s="90"/>
+      <c r="A15" s="92"/>
+      <c r="B15" s="87"/>
+      <c r="C15" s="92"/>
     </row>
     <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="90"/>
-      <c r="B16" s="85"/>
-      <c r="C16" s="90"/>
+      <c r="A16" s="92"/>
+      <c r="B16" s="87"/>
+      <c r="C16" s="92"/>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="90"/>
-      <c r="B17" s="85"/>
-      <c r="C17" s="90"/>
+      <c r="A17" s="92"/>
+      <c r="B17" s="87"/>
+      <c r="C17" s="92"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="90"/>
-      <c r="B18" s="85"/>
-      <c r="C18" s="90"/>
+      <c r="A18" s="92"/>
+      <c r="B18" s="87"/>
+      <c r="C18" s="92"/>
     </row>
     <row r="19" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="90"/>
-      <c r="B19" s="85"/>
-      <c r="C19" s="90"/>
+      <c r="A19" s="92"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="92"/>
     </row>
     <row r="20" spans="1:3" ht="155" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="90"/>
-      <c r="B20" s="86"/>
-      <c r="C20" s="90"/>
+      <c r="A20" s="92"/>
+      <c r="B20" s="88"/>
+      <c r="C20" s="92"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="90"/>
-      <c r="B21" s="84" t="s">
+      <c r="A21" s="92"/>
+      <c r="B21" s="86" t="s">
         <v>316</v>
       </c>
-      <c r="C21" s="90"/>
+      <c r="C21" s="92"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="90"/>
-      <c r="B22" s="85"/>
-      <c r="C22" s="90"/>
+      <c r="A22" s="92"/>
+      <c r="B22" s="87"/>
+      <c r="C22" s="92"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="90"/>
-      <c r="B23" s="85"/>
-      <c r="C23" s="90"/>
+      <c r="A23" s="92"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="92"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="90"/>
-      <c r="B24" s="85"/>
-      <c r="C24" s="90"/>
+      <c r="A24" s="92"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="92"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="90"/>
-      <c r="B25" s="85"/>
-      <c r="C25" s="90"/>
+      <c r="A25" s="92"/>
+      <c r="B25" s="87"/>
+      <c r="C25" s="92"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="90"/>
-      <c r="B26" s="85"/>
-      <c r="C26" s="90"/>
+      <c r="A26" s="92"/>
+      <c r="B26" s="87"/>
+      <c r="C26" s="92"/>
     </row>
     <row r="27" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="90"/>
-      <c r="B27" s="86"/>
-      <c r="C27" s="90"/>
+      <c r="A27" s="92"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="92"/>
     </row>
     <row r="28" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="90"/>
-      <c r="B28" s="84" t="s">
+      <c r="A28" s="92"/>
+      <c r="B28" s="86" t="s">
         <v>317</v>
       </c>
-      <c r="C28" s="90"/>
+      <c r="C28" s="92"/>
     </row>
     <row r="29" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="90"/>
-      <c r="B29" s="85"/>
-      <c r="C29" s="90"/>
+      <c r="A29" s="92"/>
+      <c r="B29" s="87"/>
+      <c r="C29" s="92"/>
     </row>
     <row r="30" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="90"/>
-      <c r="B30" s="85"/>
-      <c r="C30" s="90"/>
+      <c r="A30" s="92"/>
+      <c r="B30" s="87"/>
+      <c r="C30" s="92"/>
     </row>
     <row r="31" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="90"/>
-      <c r="B31" s="85"/>
-      <c r="C31" s="90"/>
+      <c r="A31" s="92"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="92"/>
     </row>
     <row r="32" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="90"/>
-      <c r="B32" s="85"/>
-      <c r="C32" s="90"/>
+      <c r="A32" s="92"/>
+      <c r="B32" s="87"/>
+      <c r="C32" s="92"/>
     </row>
     <row r="33" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="90"/>
-      <c r="B33" s="85"/>
-      <c r="C33" s="90"/>
+      <c r="A33" s="92"/>
+      <c r="B33" s="87"/>
+      <c r="C33" s="92"/>
     </row>
     <row r="34" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="90"/>
-      <c r="B34" s="85"/>
-      <c r="C34" s="90"/>
+      <c r="A34" s="92"/>
+      <c r="B34" s="87"/>
+      <c r="C34" s="92"/>
     </row>
     <row r="35" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="90"/>
-      <c r="B35" s="85"/>
-      <c r="C35" s="90"/>
+      <c r="A35" s="92"/>
+      <c r="B35" s="87"/>
+      <c r="C35" s="92"/>
     </row>
     <row r="36" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="90"/>
-      <c r="B36" s="85"/>
-      <c r="C36" s="90"/>
+      <c r="A36" s="92"/>
+      <c r="B36" s="87"/>
+      <c r="C36" s="92"/>
     </row>
     <row r="37" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="90"/>
-      <c r="B37" s="86"/>
-      <c r="C37" s="90"/>
+      <c r="A37" s="92"/>
+      <c r="B37" s="88"/>
+      <c r="C37" s="92"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="90"/>
-      <c r="B38" s="84" t="s">
+      <c r="A38" s="92"/>
+      <c r="B38" s="86" t="s">
         <v>318</v>
       </c>
-      <c r="C38" s="90"/>
+      <c r="C38" s="92"/>
     </row>
     <row r="39" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="90"/>
-      <c r="B39" s="85"/>
-      <c r="C39" s="90"/>
+      <c r="A39" s="92"/>
+      <c r="B39" s="87"/>
+      <c r="C39" s="92"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="90"/>
-      <c r="B40" s="85"/>
-      <c r="C40" s="90"/>
+      <c r="A40" s="92"/>
+      <c r="B40" s="87"/>
+      <c r="C40" s="92"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="90"/>
-      <c r="B41" s="85"/>
-      <c r="C41" s="90"/>
+      <c r="A41" s="92"/>
+      <c r="B41" s="87"/>
+      <c r="C41" s="92"/>
     </row>
     <row r="42" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="80"/>
-      <c r="B42" s="86"/>
-      <c r="C42" s="80"/>
+      <c r="A42" s="82"/>
+      <c r="B42" s="88"/>
+      <c r="C42" s="82"/>
     </row>
     <row r="43" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="79" t="s">
+      <c r="A43" s="81" t="s">
         <v>326</v>
       </c>
-      <c r="B43" s="84" t="s">
+      <c r="B43" s="86" t="s">
         <v>327</v>
       </c>
-      <c r="C43" s="79" t="s">
+      <c r="C43" s="81" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="90"/>
-      <c r="B44" s="85"/>
-      <c r="C44" s="90"/>
+      <c r="A44" s="92"/>
+      <c r="B44" s="87"/>
+      <c r="C44" s="92"/>
     </row>
     <row r="45" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="90"/>
-      <c r="B45" s="85"/>
-      <c r="C45" s="90"/>
+      <c r="A45" s="92"/>
+      <c r="B45" s="87"/>
+      <c r="C45" s="92"/>
     </row>
     <row r="46" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="90"/>
-      <c r="B46" s="85"/>
-      <c r="C46" s="90"/>
+      <c r="A46" s="92"/>
+      <c r="B46" s="87"/>
+      <c r="C46" s="92"/>
     </row>
     <row r="47" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="80"/>
-      <c r="B47" s="86"/>
-      <c r="C47" s="80"/>
+      <c r="A47" s="82"/>
+      <c r="B47" s="88"/>
+      <c r="C47" s="82"/>
     </row>
     <row r="48" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
@@ -14896,18 +16473,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="85" t="s">
         <v>332</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -15046,18 +16623,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="85" t="s">
         <v>356</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -15141,18 +16718,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="85" t="s">
         <v>365</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -15177,20 +16754,20 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="79" t="s">
+      <c r="A5" s="81" t="s">
         <v>369</v>
       </c>
-      <c r="B5" s="96" t="s">
+      <c r="B5" s="98" t="s">
         <v>372</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="81" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="80"/>
-      <c r="B6" s="98"/>
-      <c r="C6" s="80"/>
+      <c r="A6" s="82"/>
+      <c r="B6" s="100"/>
+      <c r="C6" s="82"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A7" s="59" t="s">
@@ -15204,67 +16781,67 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="79" t="s">
+      <c r="A8" s="81" t="s">
         <v>376</v>
       </c>
-      <c r="B8" s="96" t="s">
+      <c r="B8" s="98" t="s">
         <v>375</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="81" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="90"/>
-      <c r="B9" s="97"/>
-      <c r="C9" s="90"/>
+      <c r="A9" s="92"/>
+      <c r="B9" s="99"/>
+      <c r="C9" s="92"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="80"/>
-      <c r="B10" s="98"/>
-      <c r="C10" s="80"/>
+      <c r="A10" s="82"/>
+      <c r="B10" s="100"/>
+      <c r="C10" s="82"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="79" t="s">
+      <c r="A11" s="81" t="s">
         <v>378</v>
       </c>
-      <c r="B11" s="96" t="s">
+      <c r="B11" s="98" t="s">
         <v>384</v>
       </c>
-      <c r="C11" s="79" t="s">
+      <c r="C11" s="81" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="90"/>
-      <c r="B12" s="97"/>
-      <c r="C12" s="90"/>
+      <c r="A12" s="92"/>
+      <c r="B12" s="99"/>
+      <c r="C12" s="92"/>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="187" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="80"/>
-      <c r="B13" s="98"/>
-      <c r="C13" s="80"/>
+      <c r="A13" s="82"/>
+      <c r="B13" s="100"/>
+      <c r="C13" s="82"/>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="79" t="s">
+      <c r="A14" s="81" t="s">
         <v>380</v>
       </c>
-      <c r="B14" s="96" t="s">
+      <c r="B14" s="98" t="s">
         <v>383</v>
       </c>
-      <c r="C14" s="79" t="s">
+      <c r="C14" s="81" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="90"/>
-      <c r="B15" s="97"/>
-      <c r="C15" s="90"/>
+      <c r="A15" s="92"/>
+      <c r="B15" s="99"/>
+      <c r="C15" s="92"/>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="80"/>
-      <c r="B16" s="98"/>
-      <c r="C16" s="80"/>
+      <c r="A16" s="82"/>
+      <c r="B16" s="100"/>
+      <c r="C16" s="82"/>
     </row>
     <row r="17" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
@@ -15327,18 +16904,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="85" t="s">
         <v>395</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -15361,217 +16938,217 @@
       <c r="C4" s="60"/>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="79" t="s">
+      <c r="A5" s="81" t="s">
         <v>397</v>
       </c>
-      <c r="B5" s="101" t="s">
+      <c r="B5" s="103" t="s">
         <v>396</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="81" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="283" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="90"/>
-      <c r="B6" s="102"/>
-      <c r="C6" s="90"/>
+      <c r="A6" s="92"/>
+      <c r="B6" s="104"/>
+      <c r="C6" s="92"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="90"/>
-      <c r="B7" s="102"/>
-      <c r="C7" s="90"/>
+      <c r="A7" s="92"/>
+      <c r="B7" s="104"/>
+      <c r="C7" s="92"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="90"/>
-      <c r="B8" s="102"/>
-      <c r="C8" s="90"/>
+      <c r="A8" s="92"/>
+      <c r="B8" s="104"/>
+      <c r="C8" s="92"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="90"/>
-      <c r="B9" s="102"/>
-      <c r="C9" s="90"/>
+      <c r="A9" s="92"/>
+      <c r="B9" s="104"/>
+      <c r="C9" s="92"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="90"/>
-      <c r="B10" s="102"/>
-      <c r="C10" s="90"/>
+      <c r="A10" s="92"/>
+      <c r="B10" s="104"/>
+      <c r="C10" s="92"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="90"/>
-      <c r="B11" s="102"/>
-      <c r="C11" s="90"/>
+      <c r="A11" s="92"/>
+      <c r="B11" s="104"/>
+      <c r="C11" s="92"/>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="80"/>
-      <c r="B12" s="103"/>
-      <c r="C12" s="80"/>
+      <c r="A12" s="82"/>
+      <c r="B12" s="105"/>
+      <c r="C12" s="82"/>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="79" t="s">
+      <c r="A13" s="81" t="s">
         <v>399</v>
       </c>
-      <c r="B13" s="84" t="s">
+      <c r="B13" s="86" t="s">
         <v>400</v>
       </c>
-      <c r="C13" s="79" t="s">
+      <c r="C13" s="81" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="90"/>
-      <c r="B14" s="85"/>
-      <c r="C14" s="90"/>
+      <c r="A14" s="92"/>
+      <c r="B14" s="87"/>
+      <c r="C14" s="92"/>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="90"/>
-      <c r="B15" s="85"/>
-      <c r="C15" s="90"/>
+      <c r="A15" s="92"/>
+      <c r="B15" s="87"/>
+      <c r="C15" s="92"/>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="90"/>
-      <c r="B16" s="84" t="s">
+      <c r="A16" s="92"/>
+      <c r="B16" s="86" t="s">
         <v>401</v>
       </c>
-      <c r="C16" s="90"/>
+      <c r="C16" s="92"/>
     </row>
     <row r="17" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="90"/>
-      <c r="B17" s="85"/>
-      <c r="C17" s="90"/>
+      <c r="A17" s="92"/>
+      <c r="B17" s="87"/>
+      <c r="C17" s="92"/>
     </row>
     <row r="18" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="90"/>
-      <c r="B18" s="85"/>
-      <c r="C18" s="90"/>
+      <c r="A18" s="92"/>
+      <c r="B18" s="87"/>
+      <c r="C18" s="92"/>
     </row>
     <row r="19" spans="1:3" s="13" customFormat="1" ht="159" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="90"/>
-      <c r="B19" s="85"/>
-      <c r="C19" s="90"/>
+      <c r="A19" s="92"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="92"/>
     </row>
     <row r="20" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="90"/>
-      <c r="B20" s="85" t="s">
+      <c r="A20" s="92"/>
+      <c r="B20" s="87" t="s">
         <v>402</v>
       </c>
-      <c r="C20" s="90"/>
+      <c r="C20" s="92"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="90"/>
-      <c r="B21" s="85"/>
-      <c r="C21" s="90"/>
+      <c r="A21" s="92"/>
+      <c r="B21" s="87"/>
+      <c r="C21" s="92"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="90"/>
-      <c r="B22" s="85"/>
-      <c r="C22" s="90"/>
+      <c r="A22" s="92"/>
+      <c r="B22" s="87"/>
+      <c r="C22" s="92"/>
     </row>
     <row r="23" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="90"/>
-      <c r="B23" s="85"/>
-      <c r="C23" s="90"/>
+      <c r="A23" s="92"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="92"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="90"/>
-      <c r="B24" s="85" t="s">
+      <c r="A24" s="92"/>
+      <c r="B24" s="87" t="s">
         <v>403</v>
       </c>
-      <c r="C24" s="90"/>
+      <c r="C24" s="92"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="90"/>
-      <c r="B25" s="85"/>
-      <c r="C25" s="90"/>
+      <c r="A25" s="92"/>
+      <c r="B25" s="87"/>
+      <c r="C25" s="92"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="90"/>
-      <c r="B26" s="85" t="s">
+      <c r="A26" s="92"/>
+      <c r="B26" s="87" t="s">
         <v>317</v>
       </c>
-      <c r="C26" s="90"/>
+      <c r="C26" s="92"/>
     </row>
     <row r="27" spans="1:3" ht="144" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="90"/>
-      <c r="B27" s="85"/>
-      <c r="C27" s="90"/>
+      <c r="A27" s="92"/>
+      <c r="B27" s="87"/>
+      <c r="C27" s="92"/>
     </row>
     <row r="28" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="90"/>
-      <c r="B28" s="85" t="s">
+      <c r="A28" s="92"/>
+      <c r="B28" s="87" t="s">
         <v>404</v>
       </c>
-      <c r="C28" s="90"/>
+      <c r="C28" s="92"/>
     </row>
     <row r="29" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="90"/>
-      <c r="B29" s="85"/>
-      <c r="C29" s="90"/>
+      <c r="A29" s="92"/>
+      <c r="B29" s="87"/>
+      <c r="C29" s="92"/>
     </row>
     <row r="30" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="90"/>
-      <c r="B30" s="85"/>
-      <c r="C30" s="90"/>
+      <c r="A30" s="92"/>
+      <c r="B30" s="87"/>
+      <c r="C30" s="92"/>
     </row>
     <row r="31" spans="1:3" ht="196" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="90"/>
-      <c r="B31" s="85"/>
-      <c r="C31" s="90"/>
+      <c r="A31" s="92"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="92"/>
     </row>
     <row r="32" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="90"/>
-      <c r="B32" s="85" t="s">
+      <c r="A32" s="92"/>
+      <c r="B32" s="87" t="s">
         <v>405</v>
       </c>
-      <c r="C32" s="90"/>
+      <c r="C32" s="92"/>
     </row>
     <row r="33" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="90"/>
-      <c r="B33" s="85"/>
-      <c r="C33" s="90"/>
+      <c r="A33" s="92"/>
+      <c r="B33" s="87"/>
+      <c r="C33" s="92"/>
     </row>
     <row r="34" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="90"/>
-      <c r="B34" s="85"/>
-      <c r="C34" s="90"/>
+      <c r="A34" s="92"/>
+      <c r="B34" s="87"/>
+      <c r="C34" s="92"/>
     </row>
     <row r="35" spans="1:3" ht="201" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="90"/>
-      <c r="B35" s="85"/>
-      <c r="C35" s="90"/>
+      <c r="A35" s="92"/>
+      <c r="B35" s="87"/>
+      <c r="C35" s="92"/>
     </row>
     <row r="36" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="90"/>
-      <c r="B36" s="85" t="s">
+      <c r="A36" s="92"/>
+      <c r="B36" s="87" t="s">
         <v>406</v>
       </c>
-      <c r="C36" s="90"/>
+      <c r="C36" s="92"/>
     </row>
     <row r="37" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="90"/>
-      <c r="B37" s="85"/>
-      <c r="C37" s="90"/>
+      <c r="A37" s="92"/>
+      <c r="B37" s="87"/>
+      <c r="C37" s="92"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="90"/>
-      <c r="B38" s="85"/>
-      <c r="C38" s="90"/>
+      <c r="A38" s="92"/>
+      <c r="B38" s="87"/>
+      <c r="C38" s="92"/>
     </row>
     <row r="39" spans="1:3" ht="239" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="90"/>
-      <c r="B39" s="85"/>
-      <c r="C39" s="90"/>
+      <c r="A39" s="92"/>
+      <c r="B39" s="87"/>
+      <c r="C39" s="92"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="90"/>
-      <c r="B40" s="85" t="s">
+      <c r="A40" s="92"/>
+      <c r="B40" s="87" t="s">
         <v>407</v>
       </c>
-      <c r="C40" s="90"/>
+      <c r="C40" s="92"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="80"/>
-      <c r="B41" s="86"/>
-      <c r="C41" s="80"/>
+      <c r="A41" s="82"/>
+      <c r="B41" s="88"/>
+      <c r="C41" s="82"/>
     </row>
     <row r="42" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A42" s="60" t="s">
@@ -15611,11 +17188,11 @@
       <c r="C46" s="60"/>
     </row>
     <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A47" s="83" t="s">
+      <c r="A47" s="85" t="s">
         <v>386</v>
       </c>
-      <c r="B47" s="83"/>
-      <c r="C47" s="83"/>
+      <c r="B47" s="85"/>
+      <c r="C47" s="85"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
@@ -15629,25 +17206,25 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="79" t="s">
+      <c r="A49" s="81" t="s">
         <v>388</v>
       </c>
-      <c r="B49" s="81" t="s">
+      <c r="B49" s="83" t="s">
         <v>413</v>
       </c>
-      <c r="C49" s="79" t="s">
+      <c r="C49" s="81" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="90"/>
-      <c r="B50" s="100"/>
-      <c r="C50" s="90"/>
+      <c r="A50" s="92"/>
+      <c r="B50" s="102"/>
+      <c r="C50" s="92"/>
     </row>
     <row r="51" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="80"/>
-      <c r="B51" s="82"/>
-      <c r="C51" s="80"/>
+      <c r="A51" s="82"/>
+      <c r="B51" s="84"/>
+      <c r="C51" s="82"/>
     </row>
     <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="54" t="s">
@@ -15661,91 +17238,91 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="79" t="s">
+      <c r="A53" s="81" t="s">
         <v>415</v>
       </c>
-      <c r="B53" s="99" t="s">
+      <c r="B53" s="101" t="s">
         <v>416</v>
       </c>
-      <c r="C53" s="79" t="s">
+      <c r="C53" s="81" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="238" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="90"/>
-      <c r="B54" s="99"/>
-      <c r="C54" s="90"/>
+      <c r="A54" s="92"/>
+      <c r="B54" s="101"/>
+      <c r="C54" s="92"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="90"/>
-      <c r="B55" s="81" t="s">
+      <c r="A55" s="92"/>
+      <c r="B55" s="83" t="s">
         <v>417</v>
       </c>
-      <c r="C55" s="90"/>
+      <c r="C55" s="92"/>
     </row>
     <row r="56" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="90"/>
-      <c r="B56" s="100"/>
-      <c r="C56" s="90"/>
+      <c r="A56" s="92"/>
+      <c r="B56" s="102"/>
+      <c r="C56" s="92"/>
     </row>
     <row r="57" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="90"/>
-      <c r="B57" s="100"/>
-      <c r="C57" s="90"/>
+      <c r="A57" s="92"/>
+      <c r="B57" s="102"/>
+      <c r="C57" s="92"/>
     </row>
     <row r="58" spans="1:3" ht="172" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="90"/>
-      <c r="B58" s="82"/>
-      <c r="C58" s="90"/>
+      <c r="A58" s="92"/>
+      <c r="B58" s="84"/>
+      <c r="C58" s="92"/>
     </row>
     <row r="59" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="90"/>
-      <c r="B59" s="81" t="s">
+      <c r="A59" s="92"/>
+      <c r="B59" s="83" t="s">
         <v>418</v>
       </c>
-      <c r="C59" s="90"/>
+      <c r="C59" s="92"/>
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="90"/>
-      <c r="B60" s="100"/>
-      <c r="C60" s="90"/>
+      <c r="A60" s="92"/>
+      <c r="B60" s="102"/>
+      <c r="C60" s="92"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="90"/>
-      <c r="B61" s="100"/>
-      <c r="C61" s="90"/>
+      <c r="A61" s="92"/>
+      <c r="B61" s="102"/>
+      <c r="C61" s="92"/>
     </row>
     <row r="62" spans="1:3" ht="125" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="90"/>
-      <c r="B62" s="82"/>
-      <c r="C62" s="90"/>
+      <c r="A62" s="92"/>
+      <c r="B62" s="84"/>
+      <c r="C62" s="92"/>
     </row>
     <row r="63" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="90"/>
-      <c r="B63" s="81" t="s">
+      <c r="A63" s="92"/>
+      <c r="B63" s="83" t="s">
         <v>419</v>
       </c>
-      <c r="C63" s="90"/>
+      <c r="C63" s="92"/>
     </row>
     <row r="64" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="90"/>
-      <c r="B64" s="100"/>
-      <c r="C64" s="90"/>
+      <c r="A64" s="92"/>
+      <c r="B64" s="102"/>
+      <c r="C64" s="92"/>
     </row>
     <row r="65" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="90"/>
-      <c r="B65" s="100"/>
-      <c r="C65" s="90"/>
+      <c r="A65" s="92"/>
+      <c r="B65" s="102"/>
+      <c r="C65" s="92"/>
     </row>
     <row r="66" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="90"/>
-      <c r="B66" s="100"/>
-      <c r="C66" s="90"/>
+      <c r="A66" s="92"/>
+      <c r="B66" s="102"/>
+      <c r="C66" s="92"/>
     </row>
     <row r="67" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="80"/>
-      <c r="B67" s="82"/>
-      <c r="C67" s="80"/>
+      <c r="A67" s="82"/>
+      <c r="B67" s="84"/>
+      <c r="C67" s="82"/>
     </row>
     <row r="68" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A68" s="60" t="s">

</xml_diff>

<commit_message>
Updated the documentation for repo push after merge with workflow branch.
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1772F940-AF06-E541-8E7B-13AFE897B2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{854D32FF-DC63-F443-8A9B-5FDC484168C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27640" windowHeight="16160" firstSheet="4" activeTab="12" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
+    <workbookView xWindow="640" yWindow="500" windowWidth="27640" windowHeight="16160" firstSheet="3" activeTab="13" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="SPEC - 1.1" sheetId="1" r:id="rId1"/>
@@ -26,9 +26,10 @@
     <sheet name="SPEC - 1.11" sheetId="15" r:id="rId11"/>
     <sheet name="SPEC - 2.0" sheetId="16" r:id="rId12"/>
     <sheet name="SPEC - 2.1" sheetId="17" r:id="rId13"/>
-    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId14"/>
-    <sheet name="PLAYGROUND" sheetId="6" r:id="rId15"/>
-    <sheet name="TEMPLATE" sheetId="8" r:id="rId16"/>
+    <sheet name="SPEC - 2.2" sheetId="18" r:id="rId14"/>
+    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId15"/>
+    <sheet name="PLAYGROUND" sheetId="6" r:id="rId16"/>
+    <sheet name="TEMPLATE" sheetId="8" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="552">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -11535,6 +11536,205 @@
         modified:   js/controller/index.js
         new file:   js/controller/lock-compatibility.js
         modified:   lib/lang/en/enum/door/door-enum.js</t>
+    </r>
+  </si>
+  <si>
+    <t>git commit -m "Updated the documentation for repo push after merge with workflow branch."</t>
+  </si>
+  <si>
+    <t>GitHub repor is updated.</t>
+  </si>
+  <si>
+    <t>git push master</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Push the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>master</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> repor to github</t>
+    </r>
+  </si>
+  <si>
+    <t>Updating e20f4f0..35c429b
+Fast-forward
+ .vscode/settings.json                              |   1 +
+ assets/images/HAFELE-LOGO.jpg                      | Bin 0 -&gt; 35850 bytes
+ assets/images/HAFELE-LOGO.psd                      | Bin 0 -&gt; 287088 bytes
+ css/global.css                                     |  67 +++++++++++++++++++++++++++
+ css/index.css                                      |  99 ++++++++++++++++++++++++++++++++++++++++
+ docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx | Bin 63450 -&gt; 74656 bytes
+ html/index.html                                    | 211 +++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++
+ js/controller/index.js                             | 189 ++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++++
+ js/controller/lock-compatibility.js                |  78 ++++++++++++++++++++++++++++++++
+ js/model/lock.js                                   |  42 +++++++++++++++++
+ lib/lang/en/enum/door/door-enum.js                 |  17 +++++--
+ lib/lang/en/enum/lock/lock-enum.js                 |  45 ++++++++++++++++++
+ 12 files changed, 744 insertions(+), 5 deletions(-)
+ create mode 100644 assets/images/HAFELE-LOGO.jpg
+ create mode 100644 assets/images/HAFELE-LOGO.psd
+ create mode 100644 css/global.css
+ create mode 100644 js/controller/lock-compatibility.js
+ create mode 100644 js/model/lock.js
+ create mode 100644 lib/lang/en/enum/lock/lock-enum.js</t>
+  </si>
+  <si>
+    <t>git merge workflow</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Merge the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>workflow</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> branch into </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>master branch</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>git branch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> shows the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> master</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> branch with an </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> indicating that it is selected</t>
+    </r>
+  </si>
+  <si>
+    <t>git switch master</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Select the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">master </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>branch</t>
+    </r>
+  </si>
+  <si>
+    <t>MERGE workflow BRANCH INTO master</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>git status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - would display the following files.                                                                                                                                                                                                                                  On branch master
+Changes to be committed:
+  (use "git restore --staged &lt;file&gt;..." to unstage)
+        modified:   docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx</t>
     </r>
   </si>
 </sst>
@@ -11955,7 +12155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -12143,6 +12343,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -12209,12 +12412,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -12222,6 +12419,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -12242,16 +12445,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -12582,18 +12785,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -12878,18 +13081,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="86" t="s">
         <v>426</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -12903,7 +13106,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="106" t="s">
+      <c r="A4" s="107" t="s">
         <v>438</v>
       </c>
       <c r="B4" s="48" t="s">
@@ -12914,7 +13117,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="107"/>
+      <c r="A5" s="108"/>
       <c r="B5" s="48" t="s">
         <v>441</v>
       </c>
@@ -12923,51 +13126,51 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="107"/>
+      <c r="A6" s="108"/>
       <c r="B6" s="48" t="s">
         <v>434</v>
       </c>
-      <c r="C6" s="109" t="s">
+      <c r="C6" s="110" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="107"/>
+      <c r="A7" s="108"/>
       <c r="B7" s="48" t="s">
         <v>435</v>
       </c>
-      <c r="C7" s="110"/>
+      <c r="C7" s="111"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="107"/>
+      <c r="A8" s="108"/>
       <c r="B8" s="48" t="s">
         <v>427</v>
       </c>
-      <c r="C8" s="110"/>
+      <c r="C8" s="111"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="107"/>
+      <c r="A9" s="108"/>
       <c r="B9" s="48" t="s">
         <v>428</v>
       </c>
-      <c r="C9" s="110"/>
+      <c r="C9" s="111"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="107"/>
+      <c r="A10" s="108"/>
       <c r="B10" s="48" t="s">
         <v>436</v>
       </c>
-      <c r="C10" s="110"/>
+      <c r="C10" s="111"/>
     </row>
     <row r="11" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="107"/>
+      <c r="A11" s="108"/>
       <c r="B11" s="48" t="s">
         <v>443</v>
       </c>
-      <c r="C11" s="111"/>
+      <c r="C11" s="112"/>
     </row>
     <row r="12" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="108"/>
+      <c r="A12" s="109"/>
       <c r="B12" s="48" t="s">
         <v>445</v>
       </c>
@@ -13106,18 +13309,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="86" t="s">
         <v>464</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -13223,18 +13426,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="86" t="s">
         <v>478</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -13285,11 +13488,11 @@
       <c r="C8" s="54"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="85" t="s">
+      <c r="A9" s="86" t="s">
         <v>485</v>
       </c>
-      <c r="B9" s="85"/>
-      <c r="C9" s="85"/>
+      <c r="B9" s="86"/>
+      <c r="C9" s="86"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -13325,20 +13528,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="82" t="s">
         <v>490</v>
       </c>
-      <c r="B13" s="86" t="s">
+      <c r="B13" s="87" t="s">
         <v>489</v>
       </c>
-      <c r="C13" s="81" t="s">
+      <c r="C13" s="82" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="82"/>
-      <c r="B14" s="88"/>
-      <c r="C14" s="82"/>
+      <c r="A14" s="83"/>
+      <c r="B14" s="89"/>
+      <c r="C14" s="83"/>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="73" t="s">
@@ -13363,20 +13566,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="81" t="s">
+      <c r="A17" s="82" t="s">
         <v>499</v>
       </c>
-      <c r="B17" s="86" t="s">
+      <c r="B17" s="87" t="s">
         <v>498</v>
       </c>
-      <c r="C17" s="81" t="s">
+      <c r="C17" s="82" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="222" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="82"/>
-      <c r="B18" s="88"/>
-      <c r="C18" s="82"/>
+      <c r="A18" s="83"/>
+      <c r="B18" s="89"/>
+      <c r="C18" s="83"/>
     </row>
     <row r="19" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -13421,6 +13624,310 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1132A7EE-237B-8045-8FB6-82D91553ABA4}">
   <dimension ref="A1:C35"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="80" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="86" t="s">
+        <v>505</v>
+      </c>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A4" s="77" t="s">
+        <v>510</v>
+      </c>
+      <c r="B4" s="58" t="s">
+        <v>508</v>
+      </c>
+      <c r="C4" s="77" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A5" s="54" t="s">
+        <v>511</v>
+      </c>
+      <c r="B5" s="78" t="s">
+        <v>522</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="140" x14ac:dyDescent="0.2">
+      <c r="A6" s="54" t="s">
+        <v>520</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>519</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="54" t="s">
+        <v>513</v>
+      </c>
+      <c r="B7" s="78" t="s">
+        <v>515</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="82" t="s">
+        <v>517</v>
+      </c>
+      <c r="B8" s="87" t="s">
+        <v>516</v>
+      </c>
+      <c r="C8" s="82" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="93"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="93"/>
+    </row>
+    <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="83"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="83"/>
+    </row>
+    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="54" t="s">
+        <v>525</v>
+      </c>
+      <c r="B11" s="55" t="s">
+        <v>524</v>
+      </c>
+      <c r="C11" s="54" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="82" t="s">
+        <v>526</v>
+      </c>
+      <c r="B12" s="87" t="s">
+        <v>527</v>
+      </c>
+      <c r="C12" s="82" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="93"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="93"/>
+    </row>
+    <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="93"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="93"/>
+    </row>
+    <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="93"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="93"/>
+    </row>
+    <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="93"/>
+      <c r="B16" s="88"/>
+      <c r="C16" s="93"/>
+    </row>
+    <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="93"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="93"/>
+    </row>
+    <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="83"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="83"/>
+    </row>
+    <row r="19" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="82" t="s">
+        <v>529</v>
+      </c>
+      <c r="B19" s="87" t="s">
+        <v>528</v>
+      </c>
+      <c r="C19" s="82" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="93"/>
+      <c r="B20" s="88"/>
+      <c r="C20" s="93"/>
+    </row>
+    <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="93"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="93"/>
+    </row>
+    <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="93"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="93"/>
+    </row>
+    <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="93"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="93"/>
+    </row>
+    <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="93"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="93"/>
+    </row>
+    <row r="25" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="83"/>
+      <c r="B25" s="89"/>
+      <c r="C25" s="83"/>
+    </row>
+    <row r="26" spans="1:3" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="B26" s="48" t="s">
+        <v>504</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="82" t="s">
+        <v>533</v>
+      </c>
+      <c r="B27" s="87" t="s">
+        <v>532</v>
+      </c>
+      <c r="C27" s="82" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="93"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="93"/>
+    </row>
+    <row r="29" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="83"/>
+      <c r="B29" s="89"/>
+      <c r="C29" s="83"/>
+    </row>
+    <row r="30" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="82" t="s">
+        <v>536</v>
+      </c>
+      <c r="B30" s="87" t="s">
+        <v>535</v>
+      </c>
+      <c r="C30" s="82" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="93"/>
+      <c r="B31" s="88"/>
+      <c r="C31" s="93"/>
+    </row>
+    <row r="32" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="93"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="93"/>
+    </row>
+    <row r="33" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="83"/>
+      <c r="B33" s="89"/>
+      <c r="C33" s="83"/>
+    </row>
+    <row r="34" spans="1:3" ht="255" x14ac:dyDescent="0.2">
+      <c r="A34" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A35" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="53" t="s">
+        <v>538</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>503</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="17">
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="A30:A33"/>
+    <mergeCell ref="C30:C33"/>
+    <mergeCell ref="B19:B25"/>
+    <mergeCell ref="A19:A25"/>
+    <mergeCell ref="C19:C25"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="A12:A18"/>
+    <mergeCell ref="C12:C18"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:C10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49DEF94E-1D4D-C245-B403-44CD44B7811F}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
@@ -13434,18 +13941,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="85" t="s">
-        <v>505</v>
-      </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
+      <c r="A2" s="86" t="s">
+        <v>550</v>
+      </c>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -13458,270 +13965,72 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="13" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A4" s="77" t="s">
-        <v>510</v>
-      </c>
-      <c r="B4" s="58" t="s">
-        <v>508</v>
-      </c>
-      <c r="C4" s="77" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="13" customFormat="1" ht="102" x14ac:dyDescent="0.2">
-      <c r="A5" s="54" t="s">
-        <v>511</v>
-      </c>
-      <c r="B5" s="78" t="s">
-        <v>522</v>
-      </c>
-      <c r="C5" s="54" t="s">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="13" customFormat="1" ht="140" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>548</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="358" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>545</v>
+      </c>
+      <c r="C5" s="79" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="54" t="s">
-        <v>520</v>
-      </c>
-      <c r="B6" s="55" t="s">
-        <v>519</v>
+        <v>543</v>
+      </c>
+      <c r="B6" s="78" t="s">
+        <v>542</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="54" t="s">
-        <v>513</v>
-      </c>
-      <c r="B7" s="78" t="s">
-        <v>515</v>
-      </c>
-      <c r="C7" s="54" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="81" t="s">
-        <v>517</v>
-      </c>
-      <c r="B8" s="86" t="s">
-        <v>516</v>
-      </c>
-      <c r="C8" s="81" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="92"/>
-      <c r="B9" s="87"/>
-      <c r="C9" s="92"/>
-    </row>
-    <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="82"/>
-      <c r="B10" s="88"/>
-      <c r="C10" s="82"/>
-    </row>
-    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="54" t="s">
-        <v>525</v>
-      </c>
-      <c r="B11" s="55" t="s">
-        <v>524</v>
-      </c>
-      <c r="C11" s="54" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="81" t="s">
-        <v>526</v>
-      </c>
-      <c r="B12" s="86" t="s">
-        <v>527</v>
-      </c>
-      <c r="C12" s="81" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="92"/>
-      <c r="B13" s="87"/>
-      <c r="C13" s="92"/>
-    </row>
-    <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="92"/>
-      <c r="B14" s="87"/>
-      <c r="C14" s="92"/>
-    </row>
-    <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="92"/>
-      <c r="B15" s="87"/>
-      <c r="C15" s="92"/>
-    </row>
-    <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="92"/>
-      <c r="B16" s="87"/>
-      <c r="C16" s="92"/>
-    </row>
-    <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="92"/>
-      <c r="B17" s="87"/>
-      <c r="C17" s="92"/>
-    </row>
-    <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="82"/>
-      <c r="B18" s="87"/>
-      <c r="C18" s="82"/>
-    </row>
-    <row r="19" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="81" t="s">
-        <v>529</v>
-      </c>
-      <c r="B19" s="86" t="s">
-        <v>528</v>
-      </c>
-      <c r="C19" s="81" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="92"/>
-      <c r="B20" s="87"/>
-      <c r="C20" s="92"/>
-    </row>
-    <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="92"/>
-      <c r="B21" s="87"/>
-      <c r="C21" s="92"/>
-    </row>
-    <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="92"/>
-      <c r="B22" s="87"/>
-      <c r="C22" s="92"/>
-    </row>
-    <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="92"/>
-      <c r="B23" s="87"/>
-      <c r="C23" s="92"/>
-    </row>
-    <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="92"/>
-      <c r="B24" s="87"/>
-      <c r="C24" s="92"/>
-    </row>
-    <row r="25" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="82"/>
-      <c r="B25" s="88"/>
-      <c r="C25" s="82"/>
-    </row>
-    <row r="26" spans="1:3" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>506</v>
-      </c>
-      <c r="B26" s="48" t="s">
-        <v>504</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="81" t="s">
-        <v>533</v>
-      </c>
-      <c r="B27" s="86" t="s">
-        <v>532</v>
-      </c>
-      <c r="C27" s="81" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="92"/>
-      <c r="B28" s="87"/>
-      <c r="C28" s="92"/>
-    </row>
-    <row r="29" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="82"/>
-      <c r="B29" s="88"/>
-      <c r="C29" s="82"/>
-    </row>
-    <row r="30" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="81" t="s">
-        <v>536</v>
-      </c>
-      <c r="B30" s="86" t="s">
-        <v>535</v>
-      </c>
-      <c r="C30" s="81" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="92"/>
-      <c r="B31" s="87"/>
-      <c r="C31" s="92"/>
-    </row>
-    <row r="32" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="92"/>
-      <c r="B32" s="87"/>
-      <c r="C32" s="92"/>
-    </row>
-    <row r="33" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="82"/>
-      <c r="B33" s="88"/>
-      <c r="C33" s="82"/>
-    </row>
-    <row r="34" spans="1:3" ht="255" x14ac:dyDescent="0.2">
-      <c r="A34" s="16" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B7" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="17" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A35" s="16" t="s">
+      <c r="C7" s="17" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="53" t="s">
-        <v>538</v>
-      </c>
-      <c r="C35" s="16" t="s">
-        <v>503</v>
+      <c r="B8" s="53" t="s">
+        <v>540</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>463</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="17">
-    <mergeCell ref="B12:B18"/>
-    <mergeCell ref="A12:A18"/>
-    <mergeCell ref="C12:C18"/>
+  <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="B19:B25"/>
-    <mergeCell ref="A19:A25"/>
-    <mergeCell ref="C19:C25"/>
-    <mergeCell ref="B27:B29"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="C27:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE113606-3FFA-8545-9BE3-5643B52A7CE9}">
   <dimension ref="A1:H116"/>
   <sheetViews>
@@ -13799,10 +14108,10 @@
       <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="115" t="s">
+      <c r="A6" s="113" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="115"/>
+      <c r="B6" s="113"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -14775,32 +15084,32 @@
       <c r="H73" s="23"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="112"/>
-      <c r="B74" s="116"/>
+      <c r="A74" s="114"/>
+      <c r="B74" s="115"/>
       <c r="C74" s="32" t="s">
         <v>225</v>
       </c>
       <c r="D74" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="E74" s="117"/>
-      <c r="F74" s="112"/>
-      <c r="G74" s="114"/>
-      <c r="H74" s="112"/>
+      <c r="E74" s="116"/>
+      <c r="F74" s="114"/>
+      <c r="G74" s="118"/>
+      <c r="H74" s="114"/>
     </row>
     <row r="75" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A75" s="112"/>
-      <c r="B75" s="116"/>
+      <c r="A75" s="114"/>
+      <c r="B75" s="115"/>
       <c r="C75" s="33" t="s">
         <v>226</v>
       </c>
       <c r="D75" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="E75" s="117"/>
-      <c r="F75" s="112"/>
-      <c r="G75" s="114"/>
-      <c r="H75" s="112"/>
+      <c r="E75" s="116"/>
+      <c r="F75" s="114"/>
+      <c r="G75" s="118"/>
+      <c r="H75" s="114"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="23"/>
@@ -14973,34 +15282,34 @@
       <c r="H88" s="23"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="112"/>
-      <c r="B89" s="112"/>
+      <c r="A89" s="114"/>
+      <c r="B89" s="114"/>
       <c r="C89" s="35" t="s">
         <v>225</v>
       </c>
       <c r="D89" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="E89" s="113" t="s">
+      <c r="E89" s="117" t="s">
         <v>121</v>
       </c>
-      <c r="F89" s="113"/>
-      <c r="G89" s="114"/>
-      <c r="H89" s="112"/>
+      <c r="F89" s="117"/>
+      <c r="G89" s="118"/>
+      <c r="H89" s="114"/>
     </row>
     <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A90" s="112"/>
-      <c r="B90" s="112"/>
+      <c r="A90" s="114"/>
+      <c r="B90" s="114"/>
       <c r="C90" s="35" t="s">
         <v>242</v>
       </c>
       <c r="D90" s="35" t="s">
         <v>243</v>
       </c>
-      <c r="E90" s="113"/>
-      <c r="F90" s="113"/>
-      <c r="G90" s="114"/>
-      <c r="H90" s="112"/>
+      <c r="E90" s="117"/>
+      <c r="F90" s="117"/>
+      <c r="G90" s="118"/>
+      <c r="H90" s="114"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="23"/>
@@ -15368,11 +15677,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F74:F75"/>
     <mergeCell ref="H74:H75"/>
     <mergeCell ref="A89:A90"/>
     <mergeCell ref="B89:B90"/>
@@ -15381,12 +15685,17 @@
     <mergeCell ref="G89:G90"/>
     <mergeCell ref="H89:H90"/>
     <mergeCell ref="G74:G75"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F74:F75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -15484,7 +15793,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0BB7-C151-C94B-945C-E2CA92034B13}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -15501,18 +15810,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="86" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -15629,18 +15938,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="86" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -15691,11 +16000,11 @@
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="85" t="s">
+      <c r="A9" s="86" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="85"/>
-      <c r="C9" s="85"/>
+      <c r="B9" s="86"/>
+      <c r="C9" s="86"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -15731,20 +16040,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="83" t="s">
+      <c r="B13" s="84" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="81" t="s">
+      <c r="C13" s="82" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="82"/>
-      <c r="B14" s="84"/>
-      <c r="C14" s="82"/>
+      <c r="A14" s="83"/>
+      <c r="B14" s="85"/>
+      <c r="C14" s="83"/>
     </row>
     <row r="15" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
@@ -15769,20 +16078,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="81" t="s">
+      <c r="A17" s="82" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="83" t="s">
+      <c r="B17" s="84" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="81" t="s">
+      <c r="C17" s="82" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="82"/>
-      <c r="B18" s="84"/>
-      <c r="C18" s="82"/>
+      <c r="A18" s="83"/>
+      <c r="B18" s="85"/>
+      <c r="C18" s="83"/>
     </row>
     <row r="19" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -15840,18 +16149,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="86" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -15887,25 +16196,25 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="81" t="s">
+      <c r="A6" s="82" t="s">
         <v>292</v>
       </c>
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="87" t="s">
         <v>291</v>
       </c>
-      <c r="C6" s="81" t="s">
+      <c r="C6" s="82" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="92"/>
-      <c r="B7" s="87"/>
-      <c r="C7" s="92"/>
+      <c r="A7" s="93"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="93"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="82"/>
-      <c r="B8" s="88"/>
-      <c r="C8" s="82"/>
+      <c r="A8" s="83"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="83"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -15930,25 +16239,25 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="89" t="s">
+      <c r="A11" s="90" t="s">
         <v>294</v>
       </c>
-      <c r="B11" s="86" t="s">
+      <c r="B11" s="87" t="s">
         <v>295</v>
       </c>
-      <c r="C11" s="89" t="s">
+      <c r="C11" s="90" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="90"/>
-      <c r="B12" s="87"/>
-      <c r="C12" s="90"/>
+      <c r="A12" s="91"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="91"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="91"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="91"/>
+      <c r="A13" s="92"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="92"/>
     </row>
     <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
@@ -16005,18 +16314,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="86" t="s">
         <v>299</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -16030,46 +16339,46 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="94" t="s">
         <v>300</v>
       </c>
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="98" t="s">
         <v>305</v>
       </c>
-      <c r="C4" s="93" t="s">
+      <c r="C4" s="94" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="93"/>
-      <c r="B5" s="97"/>
-      <c r="C5" s="93"/>
+      <c r="A5" s="94"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="94"/>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="93"/>
-      <c r="B6" s="97"/>
-      <c r="C6" s="93"/>
+      <c r="A6" s="94"/>
+      <c r="B6" s="98"/>
+      <c r="C6" s="94"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="82" t="s">
         <v>302</v>
       </c>
-      <c r="B7" s="94" t="s">
+      <c r="B7" s="95" t="s">
         <v>303</v>
       </c>
-      <c r="C7" s="81" t="s">
+      <c r="C7" s="82" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="92"/>
-      <c r="B8" s="95"/>
-      <c r="C8" s="92"/>
+      <c r="A8" s="93"/>
+      <c r="B8" s="96"/>
+      <c r="C8" s="93"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="228" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="82"/>
-      <c r="B9" s="96"/>
-      <c r="C9" s="82"/>
+      <c r="A9" s="83"/>
+      <c r="B9" s="97"/>
+      <c r="C9" s="83"/>
     </row>
     <row r="10" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
@@ -16126,18 +16435,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="86" t="s">
         <v>331</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -16184,233 +16493,233 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="82" t="s">
         <v>314</v>
       </c>
-      <c r="B7" s="86" t="s">
+      <c r="B7" s="87" t="s">
         <v>322</v>
       </c>
-      <c r="C7" s="81" t="s">
+      <c r="C7" s="82" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="92"/>
-      <c r="B8" s="87"/>
-      <c r="C8" s="92"/>
+      <c r="A8" s="93"/>
+      <c r="B8" s="88"/>
+      <c r="C8" s="93"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="92"/>
-      <c r="B9" s="87"/>
-      <c r="C9" s="92"/>
+      <c r="A9" s="93"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="93"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="92"/>
-      <c r="B10" s="87"/>
-      <c r="C10" s="92"/>
+      <c r="A10" s="93"/>
+      <c r="B10" s="88"/>
+      <c r="C10" s="93"/>
     </row>
     <row r="11" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="92"/>
-      <c r="B11" s="87"/>
-      <c r="C11" s="92"/>
+      <c r="A11" s="93"/>
+      <c r="B11" s="88"/>
+      <c r="C11" s="93"/>
     </row>
     <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="92"/>
-      <c r="B12" s="87"/>
-      <c r="C12" s="92"/>
+      <c r="A12" s="93"/>
+      <c r="B12" s="88"/>
+      <c r="C12" s="93"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="82"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="82"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="89"/>
+      <c r="C13" s="83"/>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="82" t="s">
         <v>325</v>
       </c>
-      <c r="B14" s="86" t="s">
+      <c r="B14" s="87" t="s">
         <v>323</v>
       </c>
-      <c r="C14" s="81" t="s">
+      <c r="C14" s="82" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="92"/>
-      <c r="B15" s="87"/>
-      <c r="C15" s="92"/>
+      <c r="A15" s="93"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="93"/>
     </row>
     <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="92"/>
-      <c r="B16" s="87"/>
-      <c r="C16" s="92"/>
+      <c r="A16" s="93"/>
+      <c r="B16" s="88"/>
+      <c r="C16" s="93"/>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="92"/>
-      <c r="B17" s="87"/>
-      <c r="C17" s="92"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="93"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="92"/>
-      <c r="B18" s="87"/>
-      <c r="C18" s="92"/>
+      <c r="A18" s="93"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="93"/>
     </row>
     <row r="19" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="92"/>
-      <c r="B19" s="87"/>
-      <c r="C19" s="92"/>
+      <c r="A19" s="93"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="93"/>
     </row>
     <row r="20" spans="1:3" ht="155" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="92"/>
-      <c r="B20" s="88"/>
-      <c r="C20" s="92"/>
+      <c r="A20" s="93"/>
+      <c r="B20" s="89"/>
+      <c r="C20" s="93"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="92"/>
-      <c r="B21" s="86" t="s">
+      <c r="A21" s="93"/>
+      <c r="B21" s="87" t="s">
         <v>316</v>
       </c>
-      <c r="C21" s="92"/>
+      <c r="C21" s="93"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="92"/>
-      <c r="B22" s="87"/>
-      <c r="C22" s="92"/>
+      <c r="A22" s="93"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="93"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="92"/>
-      <c r="B23" s="87"/>
-      <c r="C23" s="92"/>
+      <c r="A23" s="93"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="93"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="92"/>
-      <c r="B24" s="87"/>
-      <c r="C24" s="92"/>
+      <c r="A24" s="93"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="93"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="92"/>
-      <c r="B25" s="87"/>
-      <c r="C25" s="92"/>
+      <c r="A25" s="93"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="93"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="92"/>
-      <c r="B26" s="87"/>
-      <c r="C26" s="92"/>
+      <c r="A26" s="93"/>
+      <c r="B26" s="88"/>
+      <c r="C26" s="93"/>
     </row>
     <row r="27" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="92"/>
-      <c r="B27" s="88"/>
-      <c r="C27" s="92"/>
+      <c r="A27" s="93"/>
+      <c r="B27" s="89"/>
+      <c r="C27" s="93"/>
     </row>
     <row r="28" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="92"/>
-      <c r="B28" s="86" t="s">
+      <c r="A28" s="93"/>
+      <c r="B28" s="87" t="s">
         <v>317</v>
       </c>
-      <c r="C28" s="92"/>
+      <c r="C28" s="93"/>
     </row>
     <row r="29" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="92"/>
-      <c r="B29" s="87"/>
-      <c r="C29" s="92"/>
+      <c r="A29" s="93"/>
+      <c r="B29" s="88"/>
+      <c r="C29" s="93"/>
     </row>
     <row r="30" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="92"/>
-      <c r="B30" s="87"/>
-      <c r="C30" s="92"/>
+      <c r="A30" s="93"/>
+      <c r="B30" s="88"/>
+      <c r="C30" s="93"/>
     </row>
     <row r="31" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="92"/>
-      <c r="B31" s="87"/>
-      <c r="C31" s="92"/>
+      <c r="A31" s="93"/>
+      <c r="B31" s="88"/>
+      <c r="C31" s="93"/>
     </row>
     <row r="32" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="92"/>
-      <c r="B32" s="87"/>
-      <c r="C32" s="92"/>
+      <c r="A32" s="93"/>
+      <c r="B32" s="88"/>
+      <c r="C32" s="93"/>
     </row>
     <row r="33" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="92"/>
-      <c r="B33" s="87"/>
-      <c r="C33" s="92"/>
+      <c r="A33" s="93"/>
+      <c r="B33" s="88"/>
+      <c r="C33" s="93"/>
     </row>
     <row r="34" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="92"/>
-      <c r="B34" s="87"/>
-      <c r="C34" s="92"/>
+      <c r="A34" s="93"/>
+      <c r="B34" s="88"/>
+      <c r="C34" s="93"/>
     </row>
     <row r="35" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="92"/>
-      <c r="B35" s="87"/>
-      <c r="C35" s="92"/>
+      <c r="A35" s="93"/>
+      <c r="B35" s="88"/>
+      <c r="C35" s="93"/>
     </row>
     <row r="36" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="92"/>
-      <c r="B36" s="87"/>
-      <c r="C36" s="92"/>
+      <c r="A36" s="93"/>
+      <c r="B36" s="88"/>
+      <c r="C36" s="93"/>
     </row>
     <row r="37" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="92"/>
-      <c r="B37" s="88"/>
-      <c r="C37" s="92"/>
+      <c r="A37" s="93"/>
+      <c r="B37" s="89"/>
+      <c r="C37" s="93"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="92"/>
-      <c r="B38" s="86" t="s">
+      <c r="A38" s="93"/>
+      <c r="B38" s="87" t="s">
         <v>318</v>
       </c>
-      <c r="C38" s="92"/>
+      <c r="C38" s="93"/>
     </row>
     <row r="39" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="92"/>
-      <c r="B39" s="87"/>
-      <c r="C39" s="92"/>
+      <c r="A39" s="93"/>
+      <c r="B39" s="88"/>
+      <c r="C39" s="93"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="92"/>
-      <c r="B40" s="87"/>
-      <c r="C40" s="92"/>
+      <c r="A40" s="93"/>
+      <c r="B40" s="88"/>
+      <c r="C40" s="93"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="92"/>
-      <c r="B41" s="87"/>
-      <c r="C41" s="92"/>
+      <c r="A41" s="93"/>
+      <c r="B41" s="88"/>
+      <c r="C41" s="93"/>
     </row>
     <row r="42" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="82"/>
-      <c r="B42" s="88"/>
-      <c r="C42" s="82"/>
+      <c r="A42" s="83"/>
+      <c r="B42" s="89"/>
+      <c r="C42" s="83"/>
     </row>
     <row r="43" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="81" t="s">
+      <c r="A43" s="82" t="s">
         <v>326</v>
       </c>
-      <c r="B43" s="86" t="s">
+      <c r="B43" s="87" t="s">
         <v>327</v>
       </c>
-      <c r="C43" s="81" t="s">
+      <c r="C43" s="82" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="92"/>
-      <c r="B44" s="87"/>
-      <c r="C44" s="92"/>
+      <c r="A44" s="93"/>
+      <c r="B44" s="88"/>
+      <c r="C44" s="93"/>
     </row>
     <row r="45" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="92"/>
-      <c r="B45" s="87"/>
-      <c r="C45" s="92"/>
+      <c r="A45" s="93"/>
+      <c r="B45" s="88"/>
+      <c r="C45" s="93"/>
     </row>
     <row r="46" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="92"/>
-      <c r="B46" s="87"/>
-      <c r="C46" s="92"/>
+      <c r="A46" s="93"/>
+      <c r="B46" s="88"/>
+      <c r="C46" s="93"/>
     </row>
     <row r="47" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="82"/>
-      <c r="B47" s="88"/>
-      <c r="C47" s="82"/>
+      <c r="A47" s="83"/>
+      <c r="B47" s="89"/>
+      <c r="C47" s="83"/>
     </row>
     <row r="48" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
@@ -16437,6 +16746,11 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B7:B13"/>
+    <mergeCell ref="A7:A13"/>
+    <mergeCell ref="C7:C13"/>
     <mergeCell ref="B38:B42"/>
     <mergeCell ref="A14:A42"/>
     <mergeCell ref="C14:C42"/>
@@ -16446,11 +16760,6 @@
     <mergeCell ref="B28:B37"/>
     <mergeCell ref="B14:B20"/>
     <mergeCell ref="B21:B27"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B7:B13"/>
-    <mergeCell ref="A7:A13"/>
-    <mergeCell ref="C7:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16473,18 +16782,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="86" t="s">
         <v>332</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -16623,18 +16932,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="86" t="s">
         <v>356</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -16718,18 +17027,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="86" t="s">
         <v>365</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -16754,20 +17063,20 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="82" t="s">
         <v>369</v>
       </c>
-      <c r="B5" s="98" t="s">
+      <c r="B5" s="99" t="s">
         <v>372</v>
       </c>
-      <c r="C5" s="81" t="s">
+      <c r="C5" s="82" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="82"/>
-      <c r="B6" s="100"/>
-      <c r="C6" s="82"/>
+      <c r="A6" s="83"/>
+      <c r="B6" s="101"/>
+      <c r="C6" s="83"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A7" s="59" t="s">
@@ -16781,67 +17090,67 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="82" t="s">
         <v>376</v>
       </c>
-      <c r="B8" s="98" t="s">
+      <c r="B8" s="99" t="s">
         <v>375</v>
       </c>
-      <c r="C8" s="81" t="s">
+      <c r="C8" s="82" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="92"/>
-      <c r="B9" s="99"/>
-      <c r="C9" s="92"/>
+      <c r="A9" s="93"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="93"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="82"/>
-      <c r="B10" s="100"/>
-      <c r="C10" s="82"/>
+      <c r="A10" s="83"/>
+      <c r="B10" s="101"/>
+      <c r="C10" s="83"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="81" t="s">
+      <c r="A11" s="82" t="s">
         <v>378</v>
       </c>
-      <c r="B11" s="98" t="s">
+      <c r="B11" s="99" t="s">
         <v>384</v>
       </c>
-      <c r="C11" s="81" t="s">
+      <c r="C11" s="82" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="92"/>
-      <c r="B12" s="99"/>
-      <c r="C12" s="92"/>
+      <c r="A12" s="93"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="93"/>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="187" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="82"/>
-      <c r="B13" s="100"/>
-      <c r="C13" s="82"/>
+      <c r="A13" s="83"/>
+      <c r="B13" s="101"/>
+      <c r="C13" s="83"/>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="81" t="s">
+      <c r="A14" s="82" t="s">
         <v>380</v>
       </c>
-      <c r="B14" s="98" t="s">
+      <c r="B14" s="99" t="s">
         <v>383</v>
       </c>
-      <c r="C14" s="81" t="s">
+      <c r="C14" s="82" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="92"/>
-      <c r="B15" s="99"/>
-      <c r="C15" s="92"/>
+      <c r="A15" s="93"/>
+      <c r="B15" s="100"/>
+      <c r="C15" s="93"/>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="82"/>
-      <c r="B16" s="100"/>
-      <c r="C16" s="82"/>
+      <c r="A16" s="83"/>
+      <c r="B16" s="101"/>
+      <c r="C16" s="83"/>
     </row>
     <row r="17" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
@@ -16868,12 +17177,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="C14:C16"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="C8:C10"/>
@@ -16882,6 +17185,12 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C14:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16904,18 +17213,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="79"/>
-      <c r="C1" s="79"/>
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="86" t="s">
         <v>395</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -16938,217 +17247,217 @@
       <c r="C4" s="60"/>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="81" t="s">
+      <c r="A5" s="82" t="s">
         <v>397</v>
       </c>
-      <c r="B5" s="103" t="s">
+      <c r="B5" s="102" t="s">
         <v>396</v>
       </c>
-      <c r="C5" s="81" t="s">
+      <c r="C5" s="82" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="283" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="92"/>
-      <c r="B6" s="104"/>
-      <c r="C6" s="92"/>
+      <c r="A6" s="93"/>
+      <c r="B6" s="103"/>
+      <c r="C6" s="93"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="92"/>
-      <c r="B7" s="104"/>
-      <c r="C7" s="92"/>
+      <c r="A7" s="93"/>
+      <c r="B7" s="103"/>
+      <c r="C7" s="93"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="92"/>
-      <c r="B8" s="104"/>
-      <c r="C8" s="92"/>
+      <c r="A8" s="93"/>
+      <c r="B8" s="103"/>
+      <c r="C8" s="93"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="92"/>
-      <c r="B9" s="104"/>
-      <c r="C9" s="92"/>
+      <c r="A9" s="93"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="93"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="92"/>
-      <c r="B10" s="104"/>
-      <c r="C10" s="92"/>
+      <c r="A10" s="93"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="93"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="92"/>
-      <c r="B11" s="104"/>
-      <c r="C11" s="92"/>
+      <c r="A11" s="93"/>
+      <c r="B11" s="103"/>
+      <c r="C11" s="93"/>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="82"/>
-      <c r="B12" s="105"/>
-      <c r="C12" s="82"/>
+      <c r="A12" s="83"/>
+      <c r="B12" s="104"/>
+      <c r="C12" s="83"/>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="82" t="s">
         <v>399</v>
       </c>
-      <c r="B13" s="86" t="s">
+      <c r="B13" s="87" t="s">
         <v>400</v>
       </c>
-      <c r="C13" s="81" t="s">
+      <c r="C13" s="82" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="92"/>
-      <c r="B14" s="87"/>
-      <c r="C14" s="92"/>
+      <c r="A14" s="93"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="93"/>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="92"/>
-      <c r="B15" s="87"/>
-      <c r="C15" s="92"/>
+      <c r="A15" s="93"/>
+      <c r="B15" s="88"/>
+      <c r="C15" s="93"/>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="92"/>
-      <c r="B16" s="86" t="s">
+      <c r="A16" s="93"/>
+      <c r="B16" s="87" t="s">
         <v>401</v>
       </c>
-      <c r="C16" s="92"/>
+      <c r="C16" s="93"/>
     </row>
     <row r="17" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="92"/>
-      <c r="B17" s="87"/>
-      <c r="C17" s="92"/>
+      <c r="A17" s="93"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="93"/>
     </row>
     <row r="18" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="92"/>
-      <c r="B18" s="87"/>
-      <c r="C18" s="92"/>
+      <c r="A18" s="93"/>
+      <c r="B18" s="88"/>
+      <c r="C18" s="93"/>
     </row>
     <row r="19" spans="1:3" s="13" customFormat="1" ht="159" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="92"/>
-      <c r="B19" s="87"/>
-      <c r="C19" s="92"/>
+      <c r="A19" s="93"/>
+      <c r="B19" s="88"/>
+      <c r="C19" s="93"/>
     </row>
     <row r="20" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="92"/>
-      <c r="B20" s="87" t="s">
+      <c r="A20" s="93"/>
+      <c r="B20" s="88" t="s">
         <v>402</v>
       </c>
-      <c r="C20" s="92"/>
+      <c r="C20" s="93"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="92"/>
-      <c r="B21" s="87"/>
-      <c r="C21" s="92"/>
+      <c r="A21" s="93"/>
+      <c r="B21" s="88"/>
+      <c r="C21" s="93"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="92"/>
-      <c r="B22" s="87"/>
-      <c r="C22" s="92"/>
+      <c r="A22" s="93"/>
+      <c r="B22" s="88"/>
+      <c r="C22" s="93"/>
     </row>
     <row r="23" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="92"/>
-      <c r="B23" s="87"/>
-      <c r="C23" s="92"/>
+      <c r="A23" s="93"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="93"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="92"/>
-      <c r="B24" s="87" t="s">
+      <c r="A24" s="93"/>
+      <c r="B24" s="88" t="s">
         <v>403</v>
       </c>
-      <c r="C24" s="92"/>
+      <c r="C24" s="93"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="92"/>
-      <c r="B25" s="87"/>
-      <c r="C25" s="92"/>
+      <c r="A25" s="93"/>
+      <c r="B25" s="88"/>
+      <c r="C25" s="93"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="92"/>
-      <c r="B26" s="87" t="s">
+      <c r="A26" s="93"/>
+      <c r="B26" s="88" t="s">
         <v>317</v>
       </c>
-      <c r="C26" s="92"/>
+      <c r="C26" s="93"/>
     </row>
     <row r="27" spans="1:3" ht="144" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="92"/>
-      <c r="B27" s="87"/>
-      <c r="C27" s="92"/>
+      <c r="A27" s="93"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="93"/>
     </row>
     <row r="28" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="92"/>
-      <c r="B28" s="87" t="s">
+      <c r="A28" s="93"/>
+      <c r="B28" s="88" t="s">
         <v>404</v>
       </c>
-      <c r="C28" s="92"/>
+      <c r="C28" s="93"/>
     </row>
     <row r="29" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="92"/>
-      <c r="B29" s="87"/>
-      <c r="C29" s="92"/>
+      <c r="A29" s="93"/>
+      <c r="B29" s="88"/>
+      <c r="C29" s="93"/>
     </row>
     <row r="30" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="92"/>
-      <c r="B30" s="87"/>
-      <c r="C30" s="92"/>
+      <c r="A30" s="93"/>
+      <c r="B30" s="88"/>
+      <c r="C30" s="93"/>
     </row>
     <row r="31" spans="1:3" ht="196" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="92"/>
-      <c r="B31" s="87"/>
-      <c r="C31" s="92"/>
+      <c r="A31" s="93"/>
+      <c r="B31" s="88"/>
+      <c r="C31" s="93"/>
     </row>
     <row r="32" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="92"/>
-      <c r="B32" s="87" t="s">
+      <c r="A32" s="93"/>
+      <c r="B32" s="88" t="s">
         <v>405</v>
       </c>
-      <c r="C32" s="92"/>
+      <c r="C32" s="93"/>
     </row>
     <row r="33" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="92"/>
-      <c r="B33" s="87"/>
-      <c r="C33" s="92"/>
+      <c r="A33" s="93"/>
+      <c r="B33" s="88"/>
+      <c r="C33" s="93"/>
     </row>
     <row r="34" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="92"/>
-      <c r="B34" s="87"/>
-      <c r="C34" s="92"/>
+      <c r="A34" s="93"/>
+      <c r="B34" s="88"/>
+      <c r="C34" s="93"/>
     </row>
     <row r="35" spans="1:3" ht="201" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="92"/>
-      <c r="B35" s="87"/>
-      <c r="C35" s="92"/>
+      <c r="A35" s="93"/>
+      <c r="B35" s="88"/>
+      <c r="C35" s="93"/>
     </row>
     <row r="36" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="92"/>
-      <c r="B36" s="87" t="s">
+      <c r="A36" s="93"/>
+      <c r="B36" s="88" t="s">
         <v>406</v>
       </c>
-      <c r="C36" s="92"/>
+      <c r="C36" s="93"/>
     </row>
     <row r="37" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="92"/>
-      <c r="B37" s="87"/>
-      <c r="C37" s="92"/>
+      <c r="A37" s="93"/>
+      <c r="B37" s="88"/>
+      <c r="C37" s="93"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="92"/>
-      <c r="B38" s="87"/>
-      <c r="C38" s="92"/>
+      <c r="A38" s="93"/>
+      <c r="B38" s="88"/>
+      <c r="C38" s="93"/>
     </row>
     <row r="39" spans="1:3" ht="239" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="92"/>
-      <c r="B39" s="87"/>
-      <c r="C39" s="92"/>
+      <c r="A39" s="93"/>
+      <c r="B39" s="88"/>
+      <c r="C39" s="93"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="92"/>
-      <c r="B40" s="87" t="s">
+      <c r="A40" s="93"/>
+      <c r="B40" s="88" t="s">
         <v>407</v>
       </c>
-      <c r="C40" s="92"/>
+      <c r="C40" s="93"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="82"/>
-      <c r="B41" s="88"/>
-      <c r="C41" s="82"/>
+      <c r="A41" s="83"/>
+      <c r="B41" s="89"/>
+      <c r="C41" s="83"/>
     </row>
     <row r="42" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A42" s="60" t="s">
@@ -17188,11 +17497,11 @@
       <c r="C46" s="60"/>
     </row>
     <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A47" s="85" t="s">
+      <c r="A47" s="86" t="s">
         <v>386</v>
       </c>
-      <c r="B47" s="85"/>
-      <c r="C47" s="85"/>
+      <c r="B47" s="86"/>
+      <c r="C47" s="86"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
@@ -17206,25 +17515,25 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="81" t="s">
+      <c r="A49" s="82" t="s">
         <v>388</v>
       </c>
-      <c r="B49" s="83" t="s">
+      <c r="B49" s="84" t="s">
         <v>413</v>
       </c>
-      <c r="C49" s="81" t="s">
+      <c r="C49" s="82" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="92"/>
-      <c r="B50" s="102"/>
-      <c r="C50" s="92"/>
+      <c r="A50" s="93"/>
+      <c r="B50" s="105"/>
+      <c r="C50" s="93"/>
     </row>
     <row r="51" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="82"/>
-      <c r="B51" s="84"/>
-      <c r="C51" s="82"/>
+      <c r="A51" s="83"/>
+      <c r="B51" s="85"/>
+      <c r="C51" s="83"/>
     </row>
     <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="54" t="s">
@@ -17238,91 +17547,91 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="81" t="s">
+      <c r="A53" s="82" t="s">
         <v>415</v>
       </c>
-      <c r="B53" s="101" t="s">
+      <c r="B53" s="106" t="s">
         <v>416</v>
       </c>
-      <c r="C53" s="81" t="s">
+      <c r="C53" s="82" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="238" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="92"/>
-      <c r="B54" s="101"/>
-      <c r="C54" s="92"/>
+      <c r="A54" s="93"/>
+      <c r="B54" s="106"/>
+      <c r="C54" s="93"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="92"/>
-      <c r="B55" s="83" t="s">
+      <c r="A55" s="93"/>
+      <c r="B55" s="84" t="s">
         <v>417</v>
       </c>
-      <c r="C55" s="92"/>
+      <c r="C55" s="93"/>
     </row>
     <row r="56" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="92"/>
-      <c r="B56" s="102"/>
-      <c r="C56" s="92"/>
+      <c r="A56" s="93"/>
+      <c r="B56" s="105"/>
+      <c r="C56" s="93"/>
     </row>
     <row r="57" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="92"/>
-      <c r="B57" s="102"/>
-      <c r="C57" s="92"/>
+      <c r="A57" s="93"/>
+      <c r="B57" s="105"/>
+      <c r="C57" s="93"/>
     </row>
     <row r="58" spans="1:3" ht="172" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="92"/>
-      <c r="B58" s="84"/>
-      <c r="C58" s="92"/>
+      <c r="A58" s="93"/>
+      <c r="B58" s="85"/>
+      <c r="C58" s="93"/>
     </row>
     <row r="59" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="92"/>
-      <c r="B59" s="83" t="s">
+      <c r="A59" s="93"/>
+      <c r="B59" s="84" t="s">
         <v>418</v>
       </c>
-      <c r="C59" s="92"/>
+      <c r="C59" s="93"/>
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="92"/>
-      <c r="B60" s="102"/>
-      <c r="C60" s="92"/>
+      <c r="A60" s="93"/>
+      <c r="B60" s="105"/>
+      <c r="C60" s="93"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="92"/>
-      <c r="B61" s="102"/>
-      <c r="C61" s="92"/>
+      <c r="A61" s="93"/>
+      <c r="B61" s="105"/>
+      <c r="C61" s="93"/>
     </row>
     <row r="62" spans="1:3" ht="125" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="92"/>
-      <c r="B62" s="84"/>
-      <c r="C62" s="92"/>
+      <c r="A62" s="93"/>
+      <c r="B62" s="85"/>
+      <c r="C62" s="93"/>
     </row>
     <row r="63" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="92"/>
-      <c r="B63" s="83" t="s">
+      <c r="A63" s="93"/>
+      <c r="B63" s="84" t="s">
         <v>419</v>
       </c>
-      <c r="C63" s="92"/>
+      <c r="C63" s="93"/>
     </row>
     <row r="64" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="92"/>
-      <c r="B64" s="102"/>
-      <c r="C64" s="92"/>
+      <c r="A64" s="93"/>
+      <c r="B64" s="105"/>
+      <c r="C64" s="93"/>
     </row>
     <row r="65" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="92"/>
-      <c r="B65" s="102"/>
-      <c r="C65" s="92"/>
+      <c r="A65" s="93"/>
+      <c r="B65" s="105"/>
+      <c r="C65" s="93"/>
     </row>
     <row r="66" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="92"/>
-      <c r="B66" s="102"/>
-      <c r="C66" s="92"/>
+      <c r="A66" s="93"/>
+      <c r="B66" s="105"/>
+      <c r="C66" s="93"/>
     </row>
     <row r="67" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="82"/>
-      <c r="B67" s="84"/>
-      <c r="C67" s="82"/>
+      <c r="A67" s="83"/>
+      <c r="B67" s="85"/>
+      <c r="C67" s="83"/>
     </row>
     <row r="68" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A68" s="60" t="s">
@@ -17360,18 +17669,11 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="25">
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B5:B12"/>
-    <mergeCell ref="A5:A12"/>
-    <mergeCell ref="C5:C12"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="C13:C41"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C53:C67"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="B63:B67"/>
     <mergeCell ref="A53:A67"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="B32:B35"/>
@@ -17380,11 +17682,18 @@
     <mergeCell ref="A13:A41"/>
     <mergeCell ref="B49:B51"/>
     <mergeCell ref="A49:A51"/>
-    <mergeCell ref="C53:C67"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="B63:B67"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="C13:C41"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B5:B12"/>
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="C5:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated errata in documentation: git push hefele master.
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{854D32FF-DC63-F443-8A9B-5FDC484168C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C1B4EF-4C6E-AD45-ADB2-B04C8B5744BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="640" yWindow="500" windowWidth="27640" windowHeight="16160" firstSheet="3" activeTab="13" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="551">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -11543,9 +11543,6 @@
   </si>
   <si>
     <t>GitHub repor is updated.</t>
-  </si>
-  <si>
-    <t>git push master</t>
   </si>
   <si>
     <r>
@@ -12412,6 +12409,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -12419,12 +12422,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -12445,16 +12442,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -13902,6 +13899,14 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="17">
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="A12:A18"/>
+    <mergeCell ref="C12:C18"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:C10"/>
     <mergeCell ref="B30:B33"/>
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="C30:C33"/>
@@ -13911,14 +13916,6 @@
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="C27:C29"/>
-    <mergeCell ref="B12:B18"/>
-    <mergeCell ref="A12:A18"/>
-    <mergeCell ref="C12:C18"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="C8:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13949,7 +13946,7 @@
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="86" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="B2" s="86"/>
       <c r="C2" s="86"/>
@@ -13967,32 +13964,32 @@
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="358" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C5" s="79" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="54" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B6" s="78" t="s">
-        <v>542</v>
+        <v>475</v>
       </c>
       <c r="C6" s="54" t="s">
         <v>541</v>
@@ -14006,7 +14003,7 @@
         <v>65</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -14108,10 +14105,10 @@
       <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="113" t="s">
+      <c r="A6" s="116" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="113"/>
+      <c r="B6" s="116"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -15084,32 +15081,32 @@
       <c r="H73" s="23"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="114"/>
-      <c r="B74" s="115"/>
+      <c r="A74" s="113"/>
+      <c r="B74" s="117"/>
       <c r="C74" s="32" t="s">
         <v>225</v>
       </c>
       <c r="D74" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="E74" s="116"/>
-      <c r="F74" s="114"/>
-      <c r="G74" s="118"/>
-      <c r="H74" s="114"/>
+      <c r="E74" s="118"/>
+      <c r="F74" s="113"/>
+      <c r="G74" s="115"/>
+      <c r="H74" s="113"/>
     </row>
     <row r="75" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A75" s="114"/>
-      <c r="B75" s="115"/>
+      <c r="A75" s="113"/>
+      <c r="B75" s="117"/>
       <c r="C75" s="33" t="s">
         <v>226</v>
       </c>
       <c r="D75" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="E75" s="116"/>
-      <c r="F75" s="114"/>
-      <c r="G75" s="118"/>
-      <c r="H75" s="114"/>
+      <c r="E75" s="118"/>
+      <c r="F75" s="113"/>
+      <c r="G75" s="115"/>
+      <c r="H75" s="113"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="23"/>
@@ -15282,34 +15279,34 @@
       <c r="H88" s="23"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="114"/>
-      <c r="B89" s="114"/>
+      <c r="A89" s="113"/>
+      <c r="B89" s="113"/>
       <c r="C89" s="35" t="s">
         <v>225</v>
       </c>
       <c r="D89" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="E89" s="117" t="s">
+      <c r="E89" s="114" t="s">
         <v>121</v>
       </c>
-      <c r="F89" s="117"/>
-      <c r="G89" s="118"/>
-      <c r="H89" s="114"/>
+      <c r="F89" s="114"/>
+      <c r="G89" s="115"/>
+      <c r="H89" s="113"/>
     </row>
     <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A90" s="114"/>
-      <c r="B90" s="114"/>
+      <c r="A90" s="113"/>
+      <c r="B90" s="113"/>
       <c r="C90" s="35" t="s">
         <v>242</v>
       </c>
       <c r="D90" s="35" t="s">
         <v>243</v>
       </c>
-      <c r="E90" s="117"/>
-      <c r="F90" s="117"/>
-      <c r="G90" s="118"/>
-      <c r="H90" s="114"/>
+      <c r="E90" s="114"/>
+      <c r="F90" s="114"/>
+      <c r="G90" s="115"/>
+      <c r="H90" s="113"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="23"/>
@@ -15677,6 +15674,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F74:F75"/>
     <mergeCell ref="H74:H75"/>
     <mergeCell ref="A89:A90"/>
     <mergeCell ref="B89:B90"/>
@@ -15685,11 +15687,6 @@
     <mergeCell ref="G89:G90"/>
     <mergeCell ref="H89:H90"/>
     <mergeCell ref="G74:G75"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F74:F75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -16746,11 +16743,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B7:B13"/>
-    <mergeCell ref="A7:A13"/>
-    <mergeCell ref="C7:C13"/>
     <mergeCell ref="B38:B42"/>
     <mergeCell ref="A14:A42"/>
     <mergeCell ref="C14:C42"/>
@@ -16760,6 +16752,11 @@
     <mergeCell ref="B28:B37"/>
     <mergeCell ref="B14:B20"/>
     <mergeCell ref="B21:B27"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B7:B13"/>
+    <mergeCell ref="A7:A13"/>
+    <mergeCell ref="C7:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17177,6 +17174,12 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C14:C16"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="C8:C10"/>
@@ -17185,12 +17188,6 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="C14:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17250,7 +17247,7 @@
       <c r="A5" s="82" t="s">
         <v>397</v>
       </c>
-      <c r="B5" s="102" t="s">
+      <c r="B5" s="104" t="s">
         <v>396</v>
       </c>
       <c r="C5" s="82" t="s">
@@ -17259,37 +17256,37 @@
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="283" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="93"/>
-      <c r="B6" s="103"/>
+      <c r="B6" s="105"/>
       <c r="C6" s="93"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="93"/>
-      <c r="B7" s="103"/>
+      <c r="B7" s="105"/>
       <c r="C7" s="93"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="93"/>
-      <c r="B8" s="103"/>
+      <c r="B8" s="105"/>
       <c r="C8" s="93"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="93"/>
-      <c r="B9" s="103"/>
+      <c r="B9" s="105"/>
       <c r="C9" s="93"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="93"/>
-      <c r="B10" s="103"/>
+      <c r="B10" s="105"/>
       <c r="C10" s="93"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="93"/>
-      <c r="B11" s="103"/>
+      <c r="B11" s="105"/>
       <c r="C11" s="93"/>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="83"/>
-      <c r="B12" s="104"/>
+      <c r="B12" s="106"/>
       <c r="C12" s="83"/>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -17527,7 +17524,7 @@
     </row>
     <row r="50" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="93"/>
-      <c r="B50" s="105"/>
+      <c r="B50" s="103"/>
       <c r="C50" s="93"/>
     </row>
     <row r="51" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -17550,7 +17547,7 @@
       <c r="A53" s="82" t="s">
         <v>415</v>
       </c>
-      <c r="B53" s="106" t="s">
+      <c r="B53" s="102" t="s">
         <v>416</v>
       </c>
       <c r="C53" s="82" t="s">
@@ -17559,7 +17556,7 @@
     </row>
     <row r="54" spans="1:3" ht="238" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="93"/>
-      <c r="B54" s="106"/>
+      <c r="B54" s="102"/>
       <c r="C54" s="93"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -17571,12 +17568,12 @@
     </row>
     <row r="56" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="93"/>
-      <c r="B56" s="105"/>
+      <c r="B56" s="103"/>
       <c r="C56" s="93"/>
     </row>
     <row r="57" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="93"/>
-      <c r="B57" s="105"/>
+      <c r="B57" s="103"/>
       <c r="C57" s="93"/>
     </row>
     <row r="58" spans="1:3" ht="172" customHeight="1" x14ac:dyDescent="0.2">
@@ -17593,12 +17590,12 @@
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="93"/>
-      <c r="B60" s="105"/>
+      <c r="B60" s="103"/>
       <c r="C60" s="93"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="93"/>
-      <c r="B61" s="105"/>
+      <c r="B61" s="103"/>
       <c r="C61" s="93"/>
     </row>
     <row r="62" spans="1:3" ht="125" customHeight="1" x14ac:dyDescent="0.2">
@@ -17615,17 +17612,17 @@
     </row>
     <row r="64" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="93"/>
-      <c r="B64" s="105"/>
+      <c r="B64" s="103"/>
       <c r="C64" s="93"/>
     </row>
     <row r="65" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="93"/>
-      <c r="B65" s="105"/>
+      <c r="B65" s="103"/>
       <c r="C65" s="93"/>
     </row>
     <row r="66" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="93"/>
-      <c r="B66" s="105"/>
+      <c r="B66" s="103"/>
       <c r="C66" s="93"/>
     </row>
     <row r="67" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -17669,11 +17666,18 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="25">
-    <mergeCell ref="C53:C67"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="B63:B67"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B5:B12"/>
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="C5:C12"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="C13:C41"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B24:B27"/>
     <mergeCell ref="A53:A67"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="B32:B35"/>
@@ -17682,18 +17686,11 @@
     <mergeCell ref="A13:A41"/>
     <mergeCell ref="B49:B51"/>
     <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="C13:C41"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B5:B12"/>
-    <mergeCell ref="A5:A12"/>
-    <mergeCell ref="C5:C12"/>
+    <mergeCell ref="C53:C67"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="B63:B67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adjused the html/lock-selection-survey.html file and assicated css file to use global styling.
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C1B4EF-4C6E-AD45-ADB2-B04C8B5744BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3177FCE5-3122-A549-8F5C-9E3BD5972419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="500" windowWidth="27640" windowHeight="16160" firstSheet="3" activeTab="13" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
+    <workbookView xWindow="640" yWindow="500" windowWidth="27640" windowHeight="16160" firstSheet="4" activeTab="14" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="SPEC - 1.1" sheetId="1" r:id="rId1"/>
@@ -27,9 +27,10 @@
     <sheet name="SPEC - 2.0" sheetId="16" r:id="rId12"/>
     <sheet name="SPEC - 2.1" sheetId="17" r:id="rId13"/>
     <sheet name="SPEC - 2.2" sheetId="18" r:id="rId14"/>
-    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId15"/>
-    <sheet name="PLAYGROUND" sheetId="6" r:id="rId16"/>
-    <sheet name="TEMPLATE" sheetId="8" r:id="rId17"/>
+    <sheet name="SPEC - 3.0" sheetId="19" r:id="rId15"/>
+    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId16"/>
+    <sheet name="PLAYGROUND" sheetId="6" r:id="rId17"/>
+    <sheet name="TEMPLATE" sheetId="8" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="578">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -11732,6 +11733,788 @@
 Changes to be committed:
   (use "git restore --staged &lt;file&gt;..." to unstage)
         modified:   docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ensure that you are on the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">master </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>branch of git</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">git branch </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>displays the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> master </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">branch with a prefixed </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to indicate that it is the currently selected branch</t>
+    </r>
+  </si>
+  <si>
+    <t>Create a new git branch - lock</t>
+  </si>
+  <si>
+    <t>git branch lock</t>
+  </si>
+  <si>
+    <r>
+      <t>git branch</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> displays the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">lock </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>branch</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Switch to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lock</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> branch</t>
+    </r>
+  </si>
+  <si>
+    <t>git checkout lock</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">git branch </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>displays the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> lock </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">branch with a prefixed </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to indicate that it is the currently selected branch</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">On branch </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lock</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> nothing to commit, working tree clean</t>
+    </r>
+  </si>
+  <si>
+    <t>CREATE A NEW GIT BRANCH - lock</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Refactor the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/lock-selection-survey.css</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  - remove all styling for &lt;html&gt; &lt;header&gt; and &lt;body&gt; tag from the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">css/lock-selection-survey.css </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">(as the ones in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/global.css</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>) will be used instead</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Refactored the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/lock-selection-survey.css</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  - removed all styling for &lt;html&gt; &lt;header&gt; and &lt;body&gt; tag from the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">css/lock-selection-survey.css </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">(as the ones in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/global.css</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>) will be used instead</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Insert the link to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>global</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> css file at the first css link in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html/lock-selection-survey.html</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">    &lt;!-- Custom Styles CSS --&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+    &lt;link rel="stylesheet" type="text/css" href="./../css/global.css"&gt;
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;link rel="stylesheet" type="text/css"
+      href="./../css/lock-selection-survey.css"&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Inserted the link to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>global</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> css file at the first css link in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html/lock-selection-survey.html</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;body&gt;
+    &lt;!-- Page Header --&gt;
+    &lt;div id="page-header" class="container-fluid"&gt;
+    &lt;/div&gt;
+    &lt;!-- End Page Header --&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add the page header &lt;div&gt; in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html/lock-selection-survey.html</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Added the page header &lt;div&gt; in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html/lock-selection-survey.html</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">    &lt;!-- Spacer div --&gt;
+    &lt;div id="spacer"&gt;
+      &lt;!-- A &lt;div&gt; having the same heigh as the &lt;footer&gt; tag to prevent contents of &lt;body&gt;
+        from going under the absolutely positioned &lt;footer&gt; tag when screen resizes. --&gt;
+    &lt;/div&gt;
+    &lt;!-- End div --&gt;
+    &lt;!-- Page Footer --&gt;
+    &lt;footer id="page-footer" class="container-fluid" text-center&gt;
+      &lt;p class="copyright"&gt;Copyright © Hafele 2022&lt;/p&gt;
+    &lt;/footer&gt;
+    &lt;!-- End Page Footer --&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add the spacer &lt;div&gt; and &lt;footer&gt; tag in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">html/lock-selection-survey.html just above the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>&lt;/body&gt; closing tag</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Added the spacer &lt;div&gt; and &lt;footer&gt; tag in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">html/lock-selection-survey.html just above the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>&lt;/body&gt; closing tag</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">    &lt;!-- Page Header --&gt;
+    &lt;div id="page-header" class="container-fluid"&gt;
+    &lt;/div&gt;
+    &lt;!-- End Page Header --&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+    &lt;!-- Page Heading --&gt;
+    &lt;div id="survey-heading" class="container-fluid"&gt;
+      &lt;h1&gt;Lock Selection Survey&lt;/h1&gt;
+      &lt;!-- Start Status Message --&gt;
+      &lt;div id="status" class="status-hidden"&gt;
+        &lt;p class="normal-severity status-message"&gt;Placeholder text&lt;/p&gt;
+      &lt;/div&gt;
+      &lt;!-- End Status Message --&gt;
+    &lt;/div&gt;
+    &lt;!-- End Page Heading --&gt;
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">   &lt;!-- Main container --&gt;
+    &lt;div class="container"&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Reposition the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">survey-heading </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;div&gt; outside the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Main container</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;div&gt; and refactor it to have a class - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>container-fluid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">. Also remove the unwanted </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;h2&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>tag.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Repositioned the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">survey-heading </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;div&gt; outside the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Main container</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;div&gt; and refactored it to have a class - </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>container-fluid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">. Also removed the unwanted </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;h2&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>tag.</t>
+    </r>
+  </si>
+  <si>
+    <t>PREPARE THE html/lock-selection-survey.html FOR INTEGRATION AND ADJUST THE CSS FILE</t>
+  </si>
+  <si>
+    <t>git commit -m "Adjused the html/lock-selection-survey.html file and assicated css file to use global styling."</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>git status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - would display the following files.                                                                                                                                                                                                                                  On branch lock
+Changes to be committed:
+  (use "git restore --staged &lt;file&gt;..." to unstage)
+        modified:   css/lock-selection-survey.css
+        modified:   docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+        modified:   html/lock-selection-survey.html</t>
     </r>
   </si>
 </sst>
@@ -12152,7 +12935,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="119">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -12342,6 +13125,12 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -12782,18 +13571,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -13078,18 +13867,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="88" t="s">
         <v>426</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -13103,7 +13892,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="107" t="s">
+      <c r="A4" s="109" t="s">
         <v>438</v>
       </c>
       <c r="B4" s="48" t="s">
@@ -13114,7 +13903,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="108"/>
+      <c r="A5" s="110"/>
       <c r="B5" s="48" t="s">
         <v>441</v>
       </c>
@@ -13123,51 +13912,51 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="108"/>
+      <c r="A6" s="110"/>
       <c r="B6" s="48" t="s">
         <v>434</v>
       </c>
-      <c r="C6" s="110" t="s">
+      <c r="C6" s="112" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="108"/>
+      <c r="A7" s="110"/>
       <c r="B7" s="48" t="s">
         <v>435</v>
       </c>
-      <c r="C7" s="111"/>
+      <c r="C7" s="113"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="108"/>
+      <c r="A8" s="110"/>
       <c r="B8" s="48" t="s">
         <v>427</v>
       </c>
-      <c r="C8" s="111"/>
+      <c r="C8" s="113"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="108"/>
+      <c r="A9" s="110"/>
       <c r="B9" s="48" t="s">
         <v>428</v>
       </c>
-      <c r="C9" s="111"/>
+      <c r="C9" s="113"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="108"/>
+      <c r="A10" s="110"/>
       <c r="B10" s="48" t="s">
         <v>436</v>
       </c>
-      <c r="C10" s="111"/>
+      <c r="C10" s="113"/>
     </row>
     <row r="11" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="108"/>
+      <c r="A11" s="110"/>
       <c r="B11" s="48" t="s">
         <v>443</v>
       </c>
-      <c r="C11" s="112"/>
+      <c r="C11" s="114"/>
     </row>
     <row r="12" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="109"/>
+      <c r="A12" s="111"/>
       <c r="B12" s="48" t="s">
         <v>445</v>
       </c>
@@ -13306,18 +14095,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="88" t="s">
         <v>464</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -13411,7 +14200,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="C7" sqref="A2:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13423,18 +14212,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="88" t="s">
         <v>478</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -13485,11 +14274,11 @@
       <c r="C8" s="54"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="86" t="s">
+      <c r="A9" s="88" t="s">
         <v>485</v>
       </c>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -13525,20 +14314,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="82" t="s">
+      <c r="A13" s="84" t="s">
         <v>490</v>
       </c>
-      <c r="B13" s="87" t="s">
+      <c r="B13" s="89" t="s">
         <v>489</v>
       </c>
-      <c r="C13" s="82" t="s">
+      <c r="C13" s="84" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="83"/>
-      <c r="B14" s="89"/>
-      <c r="C14" s="83"/>
+      <c r="A14" s="85"/>
+      <c r="B14" s="91"/>
+      <c r="C14" s="85"/>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="73" t="s">
@@ -13563,20 +14352,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="82" t="s">
+      <c r="A17" s="84" t="s">
         <v>499</v>
       </c>
-      <c r="B17" s="87" t="s">
+      <c r="B17" s="89" t="s">
         <v>498</v>
       </c>
-      <c r="C17" s="82" t="s">
+      <c r="C17" s="84" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="222" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="83"/>
-      <c r="B18" s="89"/>
-      <c r="C18" s="83"/>
+      <c r="A18" s="85"/>
+      <c r="B18" s="91"/>
+      <c r="C18" s="85"/>
     </row>
     <row r="19" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -13634,18 +14423,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="88" t="s">
         <v>505</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -13703,25 +14492,25 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="82" t="s">
+      <c r="A8" s="84" t="s">
         <v>517</v>
       </c>
-      <c r="B8" s="87" t="s">
+      <c r="B8" s="89" t="s">
         <v>516</v>
       </c>
-      <c r="C8" s="82" t="s">
+      <c r="C8" s="84" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="93"/>
-      <c r="B9" s="88"/>
-      <c r="C9" s="93"/>
+      <c r="A9" s="95"/>
+      <c r="B9" s="90"/>
+      <c r="C9" s="95"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="83"/>
-      <c r="B10" s="89"/>
-      <c r="C10" s="83"/>
+      <c r="A10" s="85"/>
+      <c r="B10" s="91"/>
+      <c r="C10" s="85"/>
     </row>
     <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="54" t="s">
@@ -13735,86 +14524,86 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="82" t="s">
+      <c r="A12" s="84" t="s">
         <v>526</v>
       </c>
-      <c r="B12" s="87" t="s">
+      <c r="B12" s="89" t="s">
         <v>527</v>
       </c>
-      <c r="C12" s="82" t="s">
+      <c r="C12" s="84" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="93"/>
-      <c r="B13" s="88"/>
-      <c r="C13" s="93"/>
+      <c r="A13" s="95"/>
+      <c r="B13" s="90"/>
+      <c r="C13" s="95"/>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="93"/>
-      <c r="B14" s="88"/>
-      <c r="C14" s="93"/>
+      <c r="A14" s="95"/>
+      <c r="B14" s="90"/>
+      <c r="C14" s="95"/>
     </row>
     <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="93"/>
-      <c r="B15" s="88"/>
-      <c r="C15" s="93"/>
+      <c r="A15" s="95"/>
+      <c r="B15" s="90"/>
+      <c r="C15" s="95"/>
     </row>
     <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="93"/>
-      <c r="B16" s="88"/>
-      <c r="C16" s="93"/>
+      <c r="A16" s="95"/>
+      <c r="B16" s="90"/>
+      <c r="C16" s="95"/>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="93"/>
-      <c r="B17" s="88"/>
-      <c r="C17" s="93"/>
+      <c r="A17" s="95"/>
+      <c r="B17" s="90"/>
+      <c r="C17" s="95"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="83"/>
-      <c r="B18" s="88"/>
-      <c r="C18" s="83"/>
+      <c r="A18" s="85"/>
+      <c r="B18" s="90"/>
+      <c r="C18" s="85"/>
     </row>
     <row r="19" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="82" t="s">
+      <c r="A19" s="84" t="s">
         <v>529</v>
       </c>
-      <c r="B19" s="87" t="s">
+      <c r="B19" s="89" t="s">
         <v>528</v>
       </c>
-      <c r="C19" s="82" t="s">
+      <c r="C19" s="84" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="93"/>
-      <c r="B20" s="88"/>
-      <c r="C20" s="93"/>
+      <c r="A20" s="95"/>
+      <c r="B20" s="90"/>
+      <c r="C20" s="95"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="93"/>
-      <c r="B21" s="88"/>
-      <c r="C21" s="93"/>
+      <c r="A21" s="95"/>
+      <c r="B21" s="90"/>
+      <c r="C21" s="95"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="93"/>
-      <c r="B22" s="88"/>
-      <c r="C22" s="93"/>
+      <c r="A22" s="95"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="95"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="93"/>
-      <c r="B23" s="88"/>
-      <c r="C23" s="93"/>
+      <c r="A23" s="95"/>
+      <c r="B23" s="90"/>
+      <c r="C23" s="95"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="93"/>
-      <c r="B24" s="88"/>
-      <c r="C24" s="93"/>
+      <c r="A24" s="95"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="95"/>
     </row>
     <row r="25" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="83"/>
-      <c r="B25" s="89"/>
-      <c r="C25" s="83"/>
+      <c r="A25" s="85"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="85"/>
     </row>
     <row r="26" spans="1:3" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
@@ -13828,51 +14617,51 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="82" t="s">
+      <c r="A27" s="84" t="s">
         <v>533</v>
       </c>
-      <c r="B27" s="87" t="s">
+      <c r="B27" s="89" t="s">
         <v>532</v>
       </c>
-      <c r="C27" s="82" t="s">
+      <c r="C27" s="84" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="93"/>
-      <c r="B28" s="88"/>
-      <c r="C28" s="93"/>
+      <c r="A28" s="95"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="95"/>
     </row>
     <row r="29" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="83"/>
-      <c r="B29" s="89"/>
-      <c r="C29" s="83"/>
+      <c r="A29" s="85"/>
+      <c r="B29" s="91"/>
+      <c r="C29" s="85"/>
     </row>
     <row r="30" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="82" t="s">
+      <c r="A30" s="84" t="s">
         <v>536</v>
       </c>
-      <c r="B30" s="87" t="s">
+      <c r="B30" s="89" t="s">
         <v>535</v>
       </c>
-      <c r="C30" s="82" t="s">
+      <c r="C30" s="84" t="s">
         <v>537</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="93"/>
-      <c r="B31" s="88"/>
-      <c r="C31" s="93"/>
+      <c r="A31" s="95"/>
+      <c r="B31" s="90"/>
+      <c r="C31" s="95"/>
     </row>
     <row r="32" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="93"/>
-      <c r="B32" s="88"/>
-      <c r="C32" s="93"/>
+      <c r="A32" s="95"/>
+      <c r="B32" s="90"/>
+      <c r="C32" s="95"/>
     </row>
     <row r="33" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="83"/>
-      <c r="B33" s="89"/>
-      <c r="C33" s="83"/>
+      <c r="A33" s="85"/>
+      <c r="B33" s="91"/>
+      <c r="C33" s="85"/>
     </row>
     <row r="34" spans="1:3" ht="255" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
@@ -13925,6 +14714,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49DEF94E-1D4D-C245-B403-44CD44B7811F}">
   <dimension ref="A1:C8"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="82" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="88" t="s">
+        <v>549</v>
+      </c>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>547</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="358" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>544</v>
+      </c>
+      <c r="C5" s="79" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="54" t="s">
+        <v>542</v>
+      </c>
+      <c r="B6" s="78" t="s">
+        <v>475</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="53" t="s">
+        <v>540</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>463</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF81AA88-FEED-494A-BECA-2979613FBD88}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
@@ -13938,18 +14833,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
-        <v>549</v>
-      </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
+      <c r="A2" s="88" t="s">
+        <v>560</v>
+      </c>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -13962,72 +14857,159 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="B4" s="48" t="s">
-        <v>547</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="13" customFormat="1" ht="358" x14ac:dyDescent="0.2">
+        <v>448</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>545</v>
+        <v>553</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>544</v>
-      </c>
-      <c r="C5" s="79" t="s">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="54" t="s">
-        <v>542</v>
-      </c>
-      <c r="B6" s="78" t="s">
-        <v>475</v>
-      </c>
-      <c r="C6" s="54" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="119" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
+        <v>554</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>557</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="54"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="54"/>
+    </row>
+    <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="74"/>
+      <c r="B8" s="75"/>
+      <c r="C8" s="74"/>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="54"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="54"/>
+    </row>
+    <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="88" t="s">
+        <v>575</v>
+      </c>
+      <c r="B10" s="88"/>
+      <c r="C10" s="88"/>
+    </row>
+    <row r="11" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="B12" s="48"/>
+      <c r="C12" s="4" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="B13" s="58" t="s">
+        <v>564</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="129" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="54" t="s">
+        <v>567</v>
+      </c>
+      <c r="B14" s="55" t="s">
+        <v>566</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="54" t="s">
+        <v>570</v>
+      </c>
+      <c r="B15" s="81" t="s">
+        <v>569</v>
+      </c>
+      <c r="C15" s="54" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="372" x14ac:dyDescent="0.2">
+      <c r="A16" s="80" t="s">
+        <v>573</v>
+      </c>
+      <c r="B16" s="76" t="s">
+        <v>572</v>
+      </c>
+      <c r="C16" s="80" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B17" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="17" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
+      <c r="C17" s="17" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="B8" s="53" t="s">
-        <v>540</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>463</v>
+      <c r="B18" s="53" t="s">
+        <v>576</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>559</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE113606-3FFA-8545-9BE3-5643B52A7CE9}">
   <dimension ref="A1:H116"/>
   <sheetViews>
@@ -14105,10 +15087,10 @@
       <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="118" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="116"/>
+      <c r="B6" s="118"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -15081,32 +16063,32 @@
       <c r="H73" s="23"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="113"/>
-      <c r="B74" s="117"/>
+      <c r="A74" s="115"/>
+      <c r="B74" s="119"/>
       <c r="C74" s="32" t="s">
         <v>225</v>
       </c>
       <c r="D74" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="E74" s="118"/>
-      <c r="F74" s="113"/>
-      <c r="G74" s="115"/>
-      <c r="H74" s="113"/>
+      <c r="E74" s="120"/>
+      <c r="F74" s="115"/>
+      <c r="G74" s="117"/>
+      <c r="H74" s="115"/>
     </row>
     <row r="75" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A75" s="113"/>
-      <c r="B75" s="117"/>
+      <c r="A75" s="115"/>
+      <c r="B75" s="119"/>
       <c r="C75" s="33" t="s">
         <v>226</v>
       </c>
       <c r="D75" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="E75" s="118"/>
-      <c r="F75" s="113"/>
-      <c r="G75" s="115"/>
-      <c r="H75" s="113"/>
+      <c r="E75" s="120"/>
+      <c r="F75" s="115"/>
+      <c r="G75" s="117"/>
+      <c r="H75" s="115"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="23"/>
@@ -15279,34 +16261,34 @@
       <c r="H88" s="23"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="113"/>
-      <c r="B89" s="113"/>
+      <c r="A89" s="115"/>
+      <c r="B89" s="115"/>
       <c r="C89" s="35" t="s">
         <v>225</v>
       </c>
       <c r="D89" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="E89" s="114" t="s">
+      <c r="E89" s="116" t="s">
         <v>121</v>
       </c>
-      <c r="F89" s="114"/>
-      <c r="G89" s="115"/>
-      <c r="H89" s="113"/>
+      <c r="F89" s="116"/>
+      <c r="G89" s="117"/>
+      <c r="H89" s="115"/>
     </row>
     <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A90" s="113"/>
-      <c r="B90" s="113"/>
+      <c r="A90" s="115"/>
+      <c r="B90" s="115"/>
       <c r="C90" s="35" t="s">
         <v>242</v>
       </c>
       <c r="D90" s="35" t="s">
         <v>243</v>
       </c>
-      <c r="E90" s="114"/>
-      <c r="F90" s="114"/>
-      <c r="G90" s="115"/>
-      <c r="H90" s="113"/>
+      <c r="E90" s="116"/>
+      <c r="F90" s="116"/>
+      <c r="G90" s="117"/>
+      <c r="H90" s="115"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="23"/>
@@ -15692,7 +16674,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -15790,7 +16772,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0BB7-C151-C94B-945C-E2CA92034B13}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -15807,18 +16789,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="88" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -15935,18 +16917,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="88" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -15997,11 +16979,11 @@
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="86" t="s">
+      <c r="A9" s="88" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -16037,20 +17019,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="82" t="s">
+      <c r="A13" s="84" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="84" t="s">
+      <c r="B13" s="86" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="82" t="s">
+      <c r="C13" s="84" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="83"/>
-      <c r="B14" s="85"/>
-      <c r="C14" s="83"/>
+      <c r="A14" s="85"/>
+      <c r="B14" s="87"/>
+      <c r="C14" s="85"/>
     </row>
     <row r="15" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
@@ -16075,20 +17057,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="82" t="s">
+      <c r="A17" s="84" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="84" t="s">
+      <c r="B17" s="86" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="82" t="s">
+      <c r="C17" s="84" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="83"/>
-      <c r="B18" s="85"/>
-      <c r="C18" s="83"/>
+      <c r="A18" s="85"/>
+      <c r="B18" s="87"/>
+      <c r="C18" s="85"/>
     </row>
     <row r="19" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -16146,18 +17128,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="88" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -16193,25 +17175,25 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="84" t="s">
         <v>292</v>
       </c>
-      <c r="B6" s="87" t="s">
+      <c r="B6" s="89" t="s">
         <v>291</v>
       </c>
-      <c r="C6" s="82" t="s">
+      <c r="C6" s="84" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="93"/>
-      <c r="B7" s="88"/>
-      <c r="C7" s="93"/>
+      <c r="A7" s="95"/>
+      <c r="B7" s="90"/>
+      <c r="C7" s="95"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="83"/>
-      <c r="B8" s="89"/>
-      <c r="C8" s="83"/>
+      <c r="A8" s="85"/>
+      <c r="B8" s="91"/>
+      <c r="C8" s="85"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -16236,25 +17218,25 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="90" t="s">
+      <c r="A11" s="92" t="s">
         <v>294</v>
       </c>
-      <c r="B11" s="87" t="s">
+      <c r="B11" s="89" t="s">
         <v>295</v>
       </c>
-      <c r="C11" s="90" t="s">
+      <c r="C11" s="92" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="91"/>
-      <c r="B12" s="88"/>
-      <c r="C12" s="91"/>
+      <c r="A12" s="93"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="93"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="92"/>
-      <c r="B13" s="89"/>
-      <c r="C13" s="92"/>
+      <c r="A13" s="94"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="94"/>
     </row>
     <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
@@ -16311,18 +17293,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="88" t="s">
         <v>299</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -16336,46 +17318,46 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="96" t="s">
         <v>300</v>
       </c>
-      <c r="B4" s="98" t="s">
+      <c r="B4" s="100" t="s">
         <v>305</v>
       </c>
-      <c r="C4" s="94" t="s">
+      <c r="C4" s="96" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="94"/>
-      <c r="B5" s="98"/>
-      <c r="C5" s="94"/>
+      <c r="A5" s="96"/>
+      <c r="B5" s="100"/>
+      <c r="C5" s="96"/>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="94"/>
-      <c r="B6" s="98"/>
-      <c r="C6" s="94"/>
+      <c r="A6" s="96"/>
+      <c r="B6" s="100"/>
+      <c r="C6" s="96"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="84" t="s">
         <v>302</v>
       </c>
-      <c r="B7" s="95" t="s">
+      <c r="B7" s="97" t="s">
         <v>303</v>
       </c>
-      <c r="C7" s="82" t="s">
+      <c r="C7" s="84" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="93"/>
-      <c r="B8" s="96"/>
-      <c r="C8" s="93"/>
+      <c r="A8" s="95"/>
+      <c r="B8" s="98"/>
+      <c r="C8" s="95"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="228" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="83"/>
-      <c r="B9" s="97"/>
-      <c r="C9" s="83"/>
+      <c r="A9" s="85"/>
+      <c r="B9" s="99"/>
+      <c r="C9" s="85"/>
     </row>
     <row r="10" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
@@ -16432,18 +17414,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="88" t="s">
         <v>331</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -16490,233 +17472,233 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="82" t="s">
+      <c r="A7" s="84" t="s">
         <v>314</v>
       </c>
-      <c r="B7" s="87" t="s">
+      <c r="B7" s="89" t="s">
         <v>322</v>
       </c>
-      <c r="C7" s="82" t="s">
+      <c r="C7" s="84" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="93"/>
-      <c r="B8" s="88"/>
-      <c r="C8" s="93"/>
+      <c r="A8" s="95"/>
+      <c r="B8" s="90"/>
+      <c r="C8" s="95"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="93"/>
-      <c r="B9" s="88"/>
-      <c r="C9" s="93"/>
+      <c r="A9" s="95"/>
+      <c r="B9" s="90"/>
+      <c r="C9" s="95"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="93"/>
-      <c r="B10" s="88"/>
-      <c r="C10" s="93"/>
+      <c r="A10" s="95"/>
+      <c r="B10" s="90"/>
+      <c r="C10" s="95"/>
     </row>
     <row r="11" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="93"/>
-      <c r="B11" s="88"/>
-      <c r="C11" s="93"/>
+      <c r="A11" s="95"/>
+      <c r="B11" s="90"/>
+      <c r="C11" s="95"/>
     </row>
     <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="93"/>
-      <c r="B12" s="88"/>
-      <c r="C12" s="93"/>
+      <c r="A12" s="95"/>
+      <c r="B12" s="90"/>
+      <c r="C12" s="95"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="83"/>
-      <c r="B13" s="89"/>
-      <c r="C13" s="83"/>
+      <c r="A13" s="85"/>
+      <c r="B13" s="91"/>
+      <c r="C13" s="85"/>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="82" t="s">
+      <c r="A14" s="84" t="s">
         <v>325</v>
       </c>
-      <c r="B14" s="87" t="s">
+      <c r="B14" s="89" t="s">
         <v>323</v>
       </c>
-      <c r="C14" s="82" t="s">
+      <c r="C14" s="84" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="93"/>
-      <c r="B15" s="88"/>
-      <c r="C15" s="93"/>
+      <c r="A15" s="95"/>
+      <c r="B15" s="90"/>
+      <c r="C15" s="95"/>
     </row>
     <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="93"/>
-      <c r="B16" s="88"/>
-      <c r="C16" s="93"/>
+      <c r="A16" s="95"/>
+      <c r="B16" s="90"/>
+      <c r="C16" s="95"/>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="93"/>
-      <c r="B17" s="88"/>
-      <c r="C17" s="93"/>
+      <c r="A17" s="95"/>
+      <c r="B17" s="90"/>
+      <c r="C17" s="95"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="93"/>
-      <c r="B18" s="88"/>
-      <c r="C18" s="93"/>
+      <c r="A18" s="95"/>
+      <c r="B18" s="90"/>
+      <c r="C18" s="95"/>
     </row>
     <row r="19" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="93"/>
-      <c r="B19" s="88"/>
-      <c r="C19" s="93"/>
+      <c r="A19" s="95"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="95"/>
     </row>
     <row r="20" spans="1:3" ht="155" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="93"/>
-      <c r="B20" s="89"/>
-      <c r="C20" s="93"/>
+      <c r="A20" s="95"/>
+      <c r="B20" s="91"/>
+      <c r="C20" s="95"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="93"/>
-      <c r="B21" s="87" t="s">
+      <c r="A21" s="95"/>
+      <c r="B21" s="89" t="s">
         <v>316</v>
       </c>
-      <c r="C21" s="93"/>
+      <c r="C21" s="95"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="93"/>
-      <c r="B22" s="88"/>
-      <c r="C22" s="93"/>
+      <c r="A22" s="95"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="95"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="93"/>
-      <c r="B23" s="88"/>
-      <c r="C23" s="93"/>
+      <c r="A23" s="95"/>
+      <c r="B23" s="90"/>
+      <c r="C23" s="95"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="93"/>
-      <c r="B24" s="88"/>
-      <c r="C24" s="93"/>
+      <c r="A24" s="95"/>
+      <c r="B24" s="90"/>
+      <c r="C24" s="95"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="93"/>
-      <c r="B25" s="88"/>
-      <c r="C25" s="93"/>
+      <c r="A25" s="95"/>
+      <c r="B25" s="90"/>
+      <c r="C25" s="95"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="93"/>
-      <c r="B26" s="88"/>
-      <c r="C26" s="93"/>
+      <c r="A26" s="95"/>
+      <c r="B26" s="90"/>
+      <c r="C26" s="95"/>
     </row>
     <row r="27" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="93"/>
-      <c r="B27" s="89"/>
-      <c r="C27" s="93"/>
+      <c r="A27" s="95"/>
+      <c r="B27" s="91"/>
+      <c r="C27" s="95"/>
     </row>
     <row r="28" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="93"/>
-      <c r="B28" s="87" t="s">
+      <c r="A28" s="95"/>
+      <c r="B28" s="89" t="s">
         <v>317</v>
       </c>
-      <c r="C28" s="93"/>
+      <c r="C28" s="95"/>
     </row>
     <row r="29" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="93"/>
-      <c r="B29" s="88"/>
-      <c r="C29" s="93"/>
+      <c r="A29" s="95"/>
+      <c r="B29" s="90"/>
+      <c r="C29" s="95"/>
     </row>
     <row r="30" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="93"/>
-      <c r="B30" s="88"/>
-      <c r="C30" s="93"/>
+      <c r="A30" s="95"/>
+      <c r="B30" s="90"/>
+      <c r="C30" s="95"/>
     </row>
     <row r="31" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="93"/>
-      <c r="B31" s="88"/>
-      <c r="C31" s="93"/>
+      <c r="A31" s="95"/>
+      <c r="B31" s="90"/>
+      <c r="C31" s="95"/>
     </row>
     <row r="32" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="93"/>
-      <c r="B32" s="88"/>
-      <c r="C32" s="93"/>
+      <c r="A32" s="95"/>
+      <c r="B32" s="90"/>
+      <c r="C32" s="95"/>
     </row>
     <row r="33" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="93"/>
-      <c r="B33" s="88"/>
-      <c r="C33" s="93"/>
+      <c r="A33" s="95"/>
+      <c r="B33" s="90"/>
+      <c r="C33" s="95"/>
     </row>
     <row r="34" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="93"/>
-      <c r="B34" s="88"/>
-      <c r="C34" s="93"/>
+      <c r="A34" s="95"/>
+      <c r="B34" s="90"/>
+      <c r="C34" s="95"/>
     </row>
     <row r="35" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="93"/>
-      <c r="B35" s="88"/>
-      <c r="C35" s="93"/>
+      <c r="A35" s="95"/>
+      <c r="B35" s="90"/>
+      <c r="C35" s="95"/>
     </row>
     <row r="36" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="93"/>
-      <c r="B36" s="88"/>
-      <c r="C36" s="93"/>
+      <c r="A36" s="95"/>
+      <c r="B36" s="90"/>
+      <c r="C36" s="95"/>
     </row>
     <row r="37" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="93"/>
-      <c r="B37" s="89"/>
-      <c r="C37" s="93"/>
+      <c r="A37" s="95"/>
+      <c r="B37" s="91"/>
+      <c r="C37" s="95"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="93"/>
-      <c r="B38" s="87" t="s">
+      <c r="A38" s="95"/>
+      <c r="B38" s="89" t="s">
         <v>318</v>
       </c>
-      <c r="C38" s="93"/>
+      <c r="C38" s="95"/>
     </row>
     <row r="39" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="93"/>
-      <c r="B39" s="88"/>
-      <c r="C39" s="93"/>
+      <c r="A39" s="95"/>
+      <c r="B39" s="90"/>
+      <c r="C39" s="95"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="93"/>
-      <c r="B40" s="88"/>
-      <c r="C40" s="93"/>
+      <c r="A40" s="95"/>
+      <c r="B40" s="90"/>
+      <c r="C40" s="95"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="93"/>
-      <c r="B41" s="88"/>
-      <c r="C41" s="93"/>
+      <c r="A41" s="95"/>
+      <c r="B41" s="90"/>
+      <c r="C41" s="95"/>
     </row>
     <row r="42" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="83"/>
-      <c r="B42" s="89"/>
-      <c r="C42" s="83"/>
+      <c r="A42" s="85"/>
+      <c r="B42" s="91"/>
+      <c r="C42" s="85"/>
     </row>
     <row r="43" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="82" t="s">
+      <c r="A43" s="84" t="s">
         <v>326</v>
       </c>
-      <c r="B43" s="87" t="s">
+      <c r="B43" s="89" t="s">
         <v>327</v>
       </c>
-      <c r="C43" s="82" t="s">
+      <c r="C43" s="84" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="93"/>
-      <c r="B44" s="88"/>
-      <c r="C44" s="93"/>
+      <c r="A44" s="95"/>
+      <c r="B44" s="90"/>
+      <c r="C44" s="95"/>
     </row>
     <row r="45" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="93"/>
-      <c r="B45" s="88"/>
-      <c r="C45" s="93"/>
+      <c r="A45" s="95"/>
+      <c r="B45" s="90"/>
+      <c r="C45" s="95"/>
     </row>
     <row r="46" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="93"/>
-      <c r="B46" s="88"/>
-      <c r="C46" s="93"/>
+      <c r="A46" s="95"/>
+      <c r="B46" s="90"/>
+      <c r="C46" s="95"/>
     </row>
     <row r="47" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="83"/>
-      <c r="B47" s="89"/>
-      <c r="C47" s="83"/>
+      <c r="A47" s="85"/>
+      <c r="B47" s="91"/>
+      <c r="C47" s="85"/>
     </row>
     <row r="48" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
@@ -16779,18 +17761,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="88" t="s">
         <v>332</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -16929,18 +17911,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="88" t="s">
         <v>356</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -17024,18 +18006,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="88" t="s">
         <v>365</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -17060,20 +18042,20 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="84" t="s">
         <v>369</v>
       </c>
-      <c r="B5" s="99" t="s">
+      <c r="B5" s="101" t="s">
         <v>372</v>
       </c>
-      <c r="C5" s="82" t="s">
+      <c r="C5" s="84" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="83"/>
-      <c r="B6" s="101"/>
-      <c r="C6" s="83"/>
+      <c r="A6" s="85"/>
+      <c r="B6" s="103"/>
+      <c r="C6" s="85"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A7" s="59" t="s">
@@ -17087,67 +18069,67 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="82" t="s">
+      <c r="A8" s="84" t="s">
         <v>376</v>
       </c>
-      <c r="B8" s="99" t="s">
+      <c r="B8" s="101" t="s">
         <v>375</v>
       </c>
-      <c r="C8" s="82" t="s">
+      <c r="C8" s="84" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="93"/>
-      <c r="B9" s="100"/>
-      <c r="C9" s="93"/>
+      <c r="A9" s="95"/>
+      <c r="B9" s="102"/>
+      <c r="C9" s="95"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="83"/>
-      <c r="B10" s="101"/>
-      <c r="C10" s="83"/>
+      <c r="A10" s="85"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="85"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="82" t="s">
+      <c r="A11" s="84" t="s">
         <v>378</v>
       </c>
-      <c r="B11" s="99" t="s">
+      <c r="B11" s="101" t="s">
         <v>384</v>
       </c>
-      <c r="C11" s="82" t="s">
+      <c r="C11" s="84" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="93"/>
-      <c r="B12" s="100"/>
-      <c r="C12" s="93"/>
+      <c r="A12" s="95"/>
+      <c r="B12" s="102"/>
+      <c r="C12" s="95"/>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="187" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="83"/>
-      <c r="B13" s="101"/>
-      <c r="C13" s="83"/>
+      <c r="A13" s="85"/>
+      <c r="B13" s="103"/>
+      <c r="C13" s="85"/>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="82" t="s">
+      <c r="A14" s="84" t="s">
         <v>380</v>
       </c>
-      <c r="B14" s="99" t="s">
+      <c r="B14" s="101" t="s">
         <v>383</v>
       </c>
-      <c r="C14" s="82" t="s">
+      <c r="C14" s="84" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="93"/>
-      <c r="B15" s="100"/>
-      <c r="C15" s="93"/>
+      <c r="A15" s="95"/>
+      <c r="B15" s="102"/>
+      <c r="C15" s="95"/>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="83"/>
-      <c r="B16" s="101"/>
-      <c r="C16" s="83"/>
+      <c r="A16" s="85"/>
+      <c r="B16" s="103"/>
+      <c r="C16" s="85"/>
     </row>
     <row r="17" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
@@ -17210,18 +18192,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="80" t="s">
+      <c r="A1" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="86" t="s">
+      <c r="A2" s="88" t="s">
         <v>395</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -17244,217 +18226,217 @@
       <c r="C4" s="60"/>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="84" t="s">
         <v>397</v>
       </c>
-      <c r="B5" s="104" t="s">
+      <c r="B5" s="106" t="s">
         <v>396</v>
       </c>
-      <c r="C5" s="82" t="s">
+      <c r="C5" s="84" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="283" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="93"/>
-      <c r="B6" s="105"/>
-      <c r="C6" s="93"/>
+      <c r="A6" s="95"/>
+      <c r="B6" s="107"/>
+      <c r="C6" s="95"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="93"/>
-      <c r="B7" s="105"/>
-      <c r="C7" s="93"/>
+      <c r="A7" s="95"/>
+      <c r="B7" s="107"/>
+      <c r="C7" s="95"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="93"/>
-      <c r="B8" s="105"/>
-      <c r="C8" s="93"/>
+      <c r="A8" s="95"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="95"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="93"/>
-      <c r="B9" s="105"/>
-      <c r="C9" s="93"/>
+      <c r="A9" s="95"/>
+      <c r="B9" s="107"/>
+      <c r="C9" s="95"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="93"/>
-      <c r="B10" s="105"/>
-      <c r="C10" s="93"/>
+      <c r="A10" s="95"/>
+      <c r="B10" s="107"/>
+      <c r="C10" s="95"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="93"/>
-      <c r="B11" s="105"/>
-      <c r="C11" s="93"/>
+      <c r="A11" s="95"/>
+      <c r="B11" s="107"/>
+      <c r="C11" s="95"/>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="83"/>
-      <c r="B12" s="106"/>
-      <c r="C12" s="83"/>
+      <c r="A12" s="85"/>
+      <c r="B12" s="108"/>
+      <c r="C12" s="85"/>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="82" t="s">
+      <c r="A13" s="84" t="s">
         <v>399</v>
       </c>
-      <c r="B13" s="87" t="s">
+      <c r="B13" s="89" t="s">
         <v>400</v>
       </c>
-      <c r="C13" s="82" t="s">
+      <c r="C13" s="84" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="93"/>
-      <c r="B14" s="88"/>
-      <c r="C14" s="93"/>
+      <c r="A14" s="95"/>
+      <c r="B14" s="90"/>
+      <c r="C14" s="95"/>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="93"/>
-      <c r="B15" s="88"/>
-      <c r="C15" s="93"/>
+      <c r="A15" s="95"/>
+      <c r="B15" s="90"/>
+      <c r="C15" s="95"/>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="93"/>
-      <c r="B16" s="87" t="s">
+      <c r="A16" s="95"/>
+      <c r="B16" s="89" t="s">
         <v>401</v>
       </c>
-      <c r="C16" s="93"/>
+      <c r="C16" s="95"/>
     </row>
     <row r="17" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="93"/>
-      <c r="B17" s="88"/>
-      <c r="C17" s="93"/>
+      <c r="A17" s="95"/>
+      <c r="B17" s="90"/>
+      <c r="C17" s="95"/>
     </row>
     <row r="18" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="93"/>
-      <c r="B18" s="88"/>
-      <c r="C18" s="93"/>
+      <c r="A18" s="95"/>
+      <c r="B18" s="90"/>
+      <c r="C18" s="95"/>
     </row>
     <row r="19" spans="1:3" s="13" customFormat="1" ht="159" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="93"/>
-      <c r="B19" s="88"/>
-      <c r="C19" s="93"/>
+      <c r="A19" s="95"/>
+      <c r="B19" s="90"/>
+      <c r="C19" s="95"/>
     </row>
     <row r="20" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="93"/>
-      <c r="B20" s="88" t="s">
+      <c r="A20" s="95"/>
+      <c r="B20" s="90" t="s">
         <v>402</v>
       </c>
-      <c r="C20" s="93"/>
+      <c r="C20" s="95"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="93"/>
-      <c r="B21" s="88"/>
-      <c r="C21" s="93"/>
+      <c r="A21" s="95"/>
+      <c r="B21" s="90"/>
+      <c r="C21" s="95"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="93"/>
-      <c r="B22" s="88"/>
-      <c r="C22" s="93"/>
+      <c r="A22" s="95"/>
+      <c r="B22" s="90"/>
+      <c r="C22" s="95"/>
     </row>
     <row r="23" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="93"/>
-      <c r="B23" s="88"/>
-      <c r="C23" s="93"/>
+      <c r="A23" s="95"/>
+      <c r="B23" s="90"/>
+      <c r="C23" s="95"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="93"/>
-      <c r="B24" s="88" t="s">
+      <c r="A24" s="95"/>
+      <c r="B24" s="90" t="s">
         <v>403</v>
       </c>
-      <c r="C24" s="93"/>
+      <c r="C24" s="95"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="93"/>
-      <c r="B25" s="88"/>
-      <c r="C25" s="93"/>
+      <c r="A25" s="95"/>
+      <c r="B25" s="90"/>
+      <c r="C25" s="95"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="93"/>
-      <c r="B26" s="88" t="s">
+      <c r="A26" s="95"/>
+      <c r="B26" s="90" t="s">
         <v>317</v>
       </c>
-      <c r="C26" s="93"/>
+      <c r="C26" s="95"/>
     </row>
     <row r="27" spans="1:3" ht="144" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="93"/>
-      <c r="B27" s="88"/>
-      <c r="C27" s="93"/>
+      <c r="A27" s="95"/>
+      <c r="B27" s="90"/>
+      <c r="C27" s="95"/>
     </row>
     <row r="28" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="93"/>
-      <c r="B28" s="88" t="s">
+      <c r="A28" s="95"/>
+      <c r="B28" s="90" t="s">
         <v>404</v>
       </c>
-      <c r="C28" s="93"/>
+      <c r="C28" s="95"/>
     </row>
     <row r="29" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="93"/>
-      <c r="B29" s="88"/>
-      <c r="C29" s="93"/>
+      <c r="A29" s="95"/>
+      <c r="B29" s="90"/>
+      <c r="C29" s="95"/>
     </row>
     <row r="30" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="93"/>
-      <c r="B30" s="88"/>
-      <c r="C30" s="93"/>
+      <c r="A30" s="95"/>
+      <c r="B30" s="90"/>
+      <c r="C30" s="95"/>
     </row>
     <row r="31" spans="1:3" ht="196" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="93"/>
-      <c r="B31" s="88"/>
-      <c r="C31" s="93"/>
+      <c r="A31" s="95"/>
+      <c r="B31" s="90"/>
+      <c r="C31" s="95"/>
     </row>
     <row r="32" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="93"/>
-      <c r="B32" s="88" t="s">
+      <c r="A32" s="95"/>
+      <c r="B32" s="90" t="s">
         <v>405</v>
       </c>
-      <c r="C32" s="93"/>
+      <c r="C32" s="95"/>
     </row>
     <row r="33" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="93"/>
-      <c r="B33" s="88"/>
-      <c r="C33" s="93"/>
+      <c r="A33" s="95"/>
+      <c r="B33" s="90"/>
+      <c r="C33" s="95"/>
     </row>
     <row r="34" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="93"/>
-      <c r="B34" s="88"/>
-      <c r="C34" s="93"/>
+      <c r="A34" s="95"/>
+      <c r="B34" s="90"/>
+      <c r="C34" s="95"/>
     </row>
     <row r="35" spans="1:3" ht="201" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="93"/>
-      <c r="B35" s="88"/>
-      <c r="C35" s="93"/>
+      <c r="A35" s="95"/>
+      <c r="B35" s="90"/>
+      <c r="C35" s="95"/>
     </row>
     <row r="36" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="93"/>
-      <c r="B36" s="88" t="s">
+      <c r="A36" s="95"/>
+      <c r="B36" s="90" t="s">
         <v>406</v>
       </c>
-      <c r="C36" s="93"/>
+      <c r="C36" s="95"/>
     </row>
     <row r="37" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="93"/>
-      <c r="B37" s="88"/>
-      <c r="C37" s="93"/>
+      <c r="A37" s="95"/>
+      <c r="B37" s="90"/>
+      <c r="C37" s="95"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="93"/>
-      <c r="B38" s="88"/>
-      <c r="C38" s="93"/>
+      <c r="A38" s="95"/>
+      <c r="B38" s="90"/>
+      <c r="C38" s="95"/>
     </row>
     <row r="39" spans="1:3" ht="239" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="93"/>
-      <c r="B39" s="88"/>
-      <c r="C39" s="93"/>
+      <c r="A39" s="95"/>
+      <c r="B39" s="90"/>
+      <c r="C39" s="95"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="93"/>
-      <c r="B40" s="88" t="s">
+      <c r="A40" s="95"/>
+      <c r="B40" s="90" t="s">
         <v>407</v>
       </c>
-      <c r="C40" s="93"/>
+      <c r="C40" s="95"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="83"/>
-      <c r="B41" s="89"/>
-      <c r="C41" s="83"/>
+      <c r="A41" s="85"/>
+      <c r="B41" s="91"/>
+      <c r="C41" s="85"/>
     </row>
     <row r="42" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A42" s="60" t="s">
@@ -17494,11 +18476,11 @@
       <c r="C46" s="60"/>
     </row>
     <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A47" s="86" t="s">
+      <c r="A47" s="88" t="s">
         <v>386</v>
       </c>
-      <c r="B47" s="86"/>
-      <c r="C47" s="86"/>
+      <c r="B47" s="88"/>
+      <c r="C47" s="88"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
@@ -17512,25 +18494,25 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="82" t="s">
+      <c r="A49" s="84" t="s">
         <v>388</v>
       </c>
-      <c r="B49" s="84" t="s">
+      <c r="B49" s="86" t="s">
         <v>413</v>
       </c>
-      <c r="C49" s="82" t="s">
+      <c r="C49" s="84" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="93"/>
-      <c r="B50" s="103"/>
-      <c r="C50" s="93"/>
+      <c r="A50" s="95"/>
+      <c r="B50" s="105"/>
+      <c r="C50" s="95"/>
     </row>
     <row r="51" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="83"/>
-      <c r="B51" s="85"/>
-      <c r="C51" s="83"/>
+      <c r="A51" s="85"/>
+      <c r="B51" s="87"/>
+      <c r="C51" s="85"/>
     </row>
     <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="54" t="s">
@@ -17544,91 +18526,91 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="82" t="s">
+      <c r="A53" s="84" t="s">
         <v>415</v>
       </c>
-      <c r="B53" s="102" t="s">
+      <c r="B53" s="104" t="s">
         <v>416</v>
       </c>
-      <c r="C53" s="82" t="s">
+      <c r="C53" s="84" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="238" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="93"/>
-      <c r="B54" s="102"/>
-      <c r="C54" s="93"/>
+      <c r="A54" s="95"/>
+      <c r="B54" s="104"/>
+      <c r="C54" s="95"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="93"/>
-      <c r="B55" s="84" t="s">
+      <c r="A55" s="95"/>
+      <c r="B55" s="86" t="s">
         <v>417</v>
       </c>
-      <c r="C55" s="93"/>
+      <c r="C55" s="95"/>
     </row>
     <row r="56" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="93"/>
-      <c r="B56" s="103"/>
-      <c r="C56" s="93"/>
+      <c r="A56" s="95"/>
+      <c r="B56" s="105"/>
+      <c r="C56" s="95"/>
     </row>
     <row r="57" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="93"/>
-      <c r="B57" s="103"/>
-      <c r="C57" s="93"/>
+      <c r="A57" s="95"/>
+      <c r="B57" s="105"/>
+      <c r="C57" s="95"/>
     </row>
     <row r="58" spans="1:3" ht="172" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="93"/>
-      <c r="B58" s="85"/>
-      <c r="C58" s="93"/>
+      <c r="A58" s="95"/>
+      <c r="B58" s="87"/>
+      <c r="C58" s="95"/>
     </row>
     <row r="59" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="93"/>
-      <c r="B59" s="84" t="s">
+      <c r="A59" s="95"/>
+      <c r="B59" s="86" t="s">
         <v>418</v>
       </c>
-      <c r="C59" s="93"/>
+      <c r="C59" s="95"/>
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="93"/>
-      <c r="B60" s="103"/>
-      <c r="C60" s="93"/>
+      <c r="A60" s="95"/>
+      <c r="B60" s="105"/>
+      <c r="C60" s="95"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="93"/>
-      <c r="B61" s="103"/>
-      <c r="C61" s="93"/>
+      <c r="A61" s="95"/>
+      <c r="B61" s="105"/>
+      <c r="C61" s="95"/>
     </row>
     <row r="62" spans="1:3" ht="125" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="93"/>
-      <c r="B62" s="85"/>
-      <c r="C62" s="93"/>
+      <c r="A62" s="95"/>
+      <c r="B62" s="87"/>
+      <c r="C62" s="95"/>
     </row>
     <row r="63" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="93"/>
-      <c r="B63" s="84" t="s">
+      <c r="A63" s="95"/>
+      <c r="B63" s="86" t="s">
         <v>419</v>
       </c>
-      <c r="C63" s="93"/>
+      <c r="C63" s="95"/>
     </row>
     <row r="64" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="93"/>
-      <c r="B64" s="103"/>
-      <c r="C64" s="93"/>
+      <c r="A64" s="95"/>
+      <c r="B64" s="105"/>
+      <c r="C64" s="95"/>
     </row>
     <row r="65" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="93"/>
-      <c r="B65" s="103"/>
-      <c r="C65" s="93"/>
+      <c r="A65" s="95"/>
+      <c r="B65" s="105"/>
+      <c r="C65" s="95"/>
     </row>
     <row r="66" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="93"/>
-      <c r="B66" s="103"/>
-      <c r="C66" s="93"/>
+      <c r="A66" s="95"/>
+      <c r="B66" s="105"/>
+      <c r="C66" s="95"/>
     </row>
     <row r="67" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="83"/>
-      <c r="B67" s="85"/>
-      <c r="C67" s="83"/>
+      <c r="A67" s="85"/>
+      <c r="B67" s="87"/>
+      <c r="C67" s="85"/>
     </row>
     <row r="68" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A68" s="60" t="s">

</xml_diff>

<commit_message>
Updated the html/index.html to display locks by door type and changed the session data storage and removal.
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DAA5C1-6352-DA4E-90DA-986D1C3695F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CD71D2-D9F6-5244-ADDC-D9890C3D05CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16160" firstSheet="5" activeTab="15" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16160" firstSheet="8" activeTab="16" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="SPEC - 1.1" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,10 @@
     <sheet name="SPEC - 2.2" sheetId="18" r:id="rId14"/>
     <sheet name="SPEC - 3.0" sheetId="19" r:id="rId15"/>
     <sheet name="SPEC - 3.1" sheetId="20" r:id="rId16"/>
-    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId17"/>
-    <sheet name="PLAYGROUND" sheetId="6" r:id="rId18"/>
-    <sheet name="TEMPLATE" sheetId="8" r:id="rId19"/>
+    <sheet name="SPEC - 3.2" sheetId="21" r:id="rId17"/>
+    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId18"/>
+    <sheet name="PLAYGROUND" sheetId="6" r:id="rId19"/>
+    <sheet name="TEMPLATE" sheetId="8" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="679">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -17418,6 +17419,752 @@
         new file:   js/controller/lock-selection-survey-lock-card.js
         modified:   lib/lang/en/enum/door/door-enum.js
         new file:   lib/lang/en/enum/message/message-enum.js</t>
+    </r>
+  </si>
+  <si>
+    <t>IMPLEMENT THE LOCK AND DOOR INFORMATION CAPTURE CARD IN html/lock-selection-survey.html WITH ASSOCIATED JS AND CSS FILES</t>
+  </si>
+  <si>
+    <t>UPDATE THE html/index.html FILE AND ASSOCIATED JS TO INCORPORATE PAGES NO. FOR TRAVERSAL AND DATA MANAGEMENT</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>&lt;body&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> tag in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">html/index.html </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">fileto have the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>page-fade-in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> class</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>&lt;body&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> tag in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">html/index.html </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">fileto have the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>page-fade-in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> class</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">            &lt;!-- Lock Model Selection Field --&gt;
+              &lt;div id="lock-model-selection-div" class="form-group"&gt;
+                &lt;div class="input-group"&gt;
+                  &lt;div class="input-group-prepend"&gt;
+                    &lt;span class="input-group-text"&gt;&lt;i
+                        class="fa-solid fa-lock"&gt;&lt;/i&gt;&lt;/span&gt;
+                  &lt;/div&gt;
+                  &lt;select id="lock-model-group"
+                    class="custom-select custom-select-extended"&gt;
+                    &lt;optgroup&gt;
+                      &lt;option value="" selected&gt;Lock Model&lt;/option&gt;
+                    &lt;/optgroup&gt;
+                  &lt;/select&gt;
+                &lt;/div&gt;
+              &lt;/div&gt;
+              &lt;!-- End Lock Model Selection Field --&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Lock Model Selection Field </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;div&gt; structure in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">html/index.html </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">to support </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>optgroup</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Lock Model Selection Field </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;div&gt; structure in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">html/index.html </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">to support </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>optgroup</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>/*****************************************************************************/
+/* GLOBAL VARIABLES                                                        */
+/*****************************************************************************/
+// Global variable - associated with the - lock model select control
+let lockModelSelectionGroup = document.getElementById("lock-model-group");</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the global variable </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">lockModelSelectionGroup </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">to point to the updated Lock Model Selection Field &lt;div&gt; id </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lock-model-selection-div</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the global variable </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">lockModelSelectionGroup </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">to point to the updated Lock Model Selection Field &lt;div&gt; id </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lock-model-selection-div</t>
+    </r>
+  </si>
+  <si>
+    <t>/*****************************************************************************/
+/* WINDOWS ONLOAD                                                            */
+/*****************************************************************************/
+/* Anonymous function fired on window load. 
+ * @param    
+ * @return   
+ * */
+window.onload = function() {
+    // Add all the swing door - lock model name options to the lock model
+    // group selection combo box
+    let optionGroup = document.createElement("optgroup");
+    optionGroup.setAttribute("label", DOOR_TYPE.SWING_DOOR);
+    let optionGroupAdded = false;
+    Object.keys(LOCK_MODEL).forEach(key =&gt; {
+        let lockModelSelectionGroup = document.getElementById("lock-model-group");
+        // The lock and door type compatibility object
+        let compatibleDoor = lockCompatibility(
+            key.toUpperCase());
+        // Add only if the lock is meant for swing doors
+        if (compatibleDoor.doorType.toUpperCase() ===
+            DOOR_TYPE.SWING_DOOR.toUpperCase()) {
+            if (optionGroupAdded === false) {
+                lockModelSelectionGroup.appendChild(optionGroup);
+                optionGroupAdded = true;
+            }
+            let optionTag = document.createElement("option");
+            optionTag.setAttribute("value", LOCK_MODEL[key]);
+            optionTag.setAttribute("data-door-type", DOOR_TYPE.SWING_DOOR);
+            let textNode = document.createTextNode(LOCK_MODEL[key]);
+            optionTag.appendChild(textNode);
+            optionGroup.appendChild(optionTag);
+        }
+    });
+    // Add all the sliding door - lock model name options to the lock model
+    // group selection combo box
+    optionGroup = document.createElement("optgroup");
+    optionGroup.setAttribute("label", DOOR_TYPE.SLIDING_DOOR);
+    optionGroupAdded = false;
+    Object.keys(LOCK_MODEL).forEach(key =&gt; {
+        let lockModelSelectionGroup = document.getElementById("lock-model-group");
+        // The lock and door type compatibility object
+        let compatibleDoor = lockCompatibility(
+            key.toUpperCase());
+        // Add only if the lock is meant for swing doors
+        if (compatibleDoor.doorType.toUpperCase() ===
+            DOOR_TYPE.SLIDING_DOOR.toUpperCase()) {
+            if (optionGroupAdded === false) {
+                lockModelSelectionGroup.appendChild(optionGroup);
+                optionGroupAdded = true;
+            }
+            let optionTag = document.createElement("option");
+            optionTag.setAttribute("value", LOCK_MODEL[key]);
+            optionTag.setAttribute("data-door-type", DOOR_TYPE.SLIDING_DOOR);
+            let textNode = document.createTextNode(LOCK_MODEL[key]);
+            optionTag.appendChild(textNode);
+            optionGroup.appendChild(optionTag);
+        }
+    });
+    // Add all the swing and sliding door - lock model name options to the
+    // lock model group selection combo box
+    optionGroup = document.createElement("optgroup");
+    optionGroup.setAttribute("label", DOOR_TYPE.SWING_DOOR + " AND " +
+        DOOR_TYPE.SLIDING_DOOR);
+    optionGroupAdded = false;
+    Object.keys(LOCK_MODEL).forEach(key =&gt; {
+        let lockModelSelectionGroup = document.getElementById("lock-model-group");
+        // The lock and door type compatibility object
+        let compatibleDoor = lockCompatibility(
+            key.toUpperCase());
+        // Add only if the lock is meant for swing doors
+        if (compatibleDoor.doorType.indexOf("/") &gt; -1) {
+            if (optionGroupAdded === false) {
+                lockModelSelectionGroup.appendChild(optionGroup);
+                optionGroupAdded = true;
+            }
+            let optionTag = document.createElement("option");
+            optionTag.setAttribute("value", LOCK_MODEL[key]);
+            optionTag.setAttribute("data-door-type", compatibleDoor.doorType);
+            let textNode = document.createTextNode(LOCK_MODEL[key]);
+            optionTag.appendChild(textNode);
+            optionGroup.appendChild(optionTag);
+        }
+    });
+    //If storage data is found -  set the lock model select control to have
+    // the value of the selected lock and display the door type and door
+    // thickness suggestions.
+    // Delete the session storage items and enable the selection button.
+    // This scenario check if the user has pressed the back button of the
+    // browser to reach this page.
+    if (sessionStorage.getItem('lockModelSelected') !== null) {
+        // Set the lock model select control to have the value of the
+        // previously selected lock
+        lockModelSelectionGroup.value = sessionStorage.getItem(
+            'lockModelSelected');
+        // Fetch the object specifying the door type and door thickness range
+        let lock = lockCompatibility(
+            lockModelSelectionGroup.value.toUpperCase());
+        // Display the door type and door thickness suggestion &lt;div&gt;
+        let suggestionDiv = document.getElementById("suggestion");
+        let doorTypeValueElement = document.getElementById("type-value");
+        let doorThicknessValueElement = document.getElementById("thickness-value");
+        suggestionDiv.classList.remove("hide-suggestion");
+        let text = document.createTextNode(lock.doorType);
+        doorTypeValueElement.appendChild(text);
+        text = document.createTextNode(lock.doorThickness);
+        doorThicknessValueElement.appendChild(text);
+        // Enable the lock model selection next button
+        lockSelectionNextButton.disabled = false;
+    } else {
+        // Ensure that no lock models are selected by default
+        lockModelSelectionGroup.options[0].selected = true
+        // Ensure that the lock model selection next button is disabled by default
+        lockSelectionNextButton.disabled = true;
+    }
+    // Delete the session storage items - at start of flow
+    sessionStorage.removeItem('page');
+    sessionStorage.removeItem('lockModelSelected');
+    sessionStorage.removeItem('compatibleDoor');
+    sessionStorage.removeItem('lockAndDoorData');
+    sessionStorage.removeItem('customerData');
+    sessionStorage.removeItem('salesPersonData');
+};</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Re-implement the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">window.onload </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">function in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">html/index.html </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>to - structure the Lock Model selection combo box to accommodate segregation of locks by door type and also reset all data added to session storage</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Re-implemented the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">window.onload </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">function in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">html/index.html </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>to - structure the Lock Model selection combo box to accommodate segregation of locks by door type and also reset all data added to session storage</t>
+    </r>
+  </si>
+  <si>
+    <t>/* The callback function fired on 'click' - for lock model next button control.
+ * @param    
+ * @return   
+ * */
+const loadSurveyPageOnClick = () =&gt; {
+    // Save the page data, selected lock and associated door type and
+    // door thickness range object to the session storage
+    sessionStorage.setItem('page', "1");
+    sessionStorage.setItem('lockModelSelected', lockModelSelectionGroup.value);
+    sessionStorage.setItem('compatibleDoor',
+        JSON.stringify(lockCompatibility(
+            lockModelSelectionGroup.value.toUpperCase())));
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>loadSurveyPageOnClick()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">html/index.html </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">to add the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">page </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">data to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>session store</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>loadSurveyPageOnClick()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">html/index.html </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">to add the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">page </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">data to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>session store</t>
+    </r>
+  </si>
+  <si>
+    <t>git commit -m "Updated the html/index.html to display locks by door type and changed the session data storage and removal."</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>git status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - would display the following files.                                                                                                                                                                                                                                  On branch lock
+Changes not staged for commit:
+  (use "git add &lt;file&gt;..." to update what will be committed)
+  (use "git restore &lt;file&gt;..." to discard changes in working directory)
+        modified:   docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+        modified:   html/index.html
+        modified:   js/controller/index.js</t>
     </r>
   </si>
 </sst>
@@ -17844,7 +18591,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -18056,6 +18803,18 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -18171,6 +18930,12 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -18501,18 +19266,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -18797,18 +19562,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="97" t="s">
         <v>426</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -18822,7 +19587,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="114" t="s">
+      <c r="A4" s="118" t="s">
         <v>438</v>
       </c>
       <c r="B4" s="48" t="s">
@@ -18833,7 +19598,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="115"/>
+      <c r="A5" s="119"/>
       <c r="B5" s="48" t="s">
         <v>441</v>
       </c>
@@ -18842,51 +19607,51 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="115"/>
+      <c r="A6" s="119"/>
       <c r="B6" s="48" t="s">
         <v>434</v>
       </c>
-      <c r="C6" s="117" t="s">
+      <c r="C6" s="121" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="115"/>
+      <c r="A7" s="119"/>
       <c r="B7" s="48" t="s">
         <v>435</v>
       </c>
-      <c r="C7" s="118"/>
+      <c r="C7" s="122"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="115"/>
+      <c r="A8" s="119"/>
       <c r="B8" s="48" t="s">
         <v>427</v>
       </c>
-      <c r="C8" s="118"/>
+      <c r="C8" s="122"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="115"/>
+      <c r="A9" s="119"/>
       <c r="B9" s="48" t="s">
         <v>428</v>
       </c>
-      <c r="C9" s="118"/>
+      <c r="C9" s="122"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="115"/>
+      <c r="A10" s="119"/>
       <c r="B10" s="48" t="s">
         <v>436</v>
       </c>
-      <c r="C10" s="118"/>
+      <c r="C10" s="122"/>
     </row>
     <row r="11" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="115"/>
+      <c r="A11" s="119"/>
       <c r="B11" s="48" t="s">
         <v>443</v>
       </c>
-      <c r="C11" s="119"/>
+      <c r="C11" s="123"/>
     </row>
     <row r="12" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="116"/>
+      <c r="A12" s="120"/>
       <c r="B12" s="48" t="s">
         <v>445</v>
       </c>
@@ -19025,18 +19790,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="97" t="s">
         <v>464</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -19142,18 +19907,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="97" t="s">
         <v>478</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -19204,11 +19969,11 @@
       <c r="C8" s="54"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="97" t="s">
         <v>485</v>
       </c>
-      <c r="B9" s="93"/>
-      <c r="C9" s="93"/>
+      <c r="B9" s="97"/>
+      <c r="C9" s="97"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -19244,20 +20009,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="89" t="s">
+      <c r="A13" s="93" t="s">
         <v>490</v>
       </c>
-      <c r="B13" s="94" t="s">
+      <c r="B13" s="98" t="s">
         <v>489</v>
       </c>
-      <c r="C13" s="89" t="s">
+      <c r="C13" s="93" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="90"/>
-      <c r="B14" s="96"/>
-      <c r="C14" s="90"/>
+      <c r="A14" s="94"/>
+      <c r="B14" s="100"/>
+      <c r="C14" s="94"/>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="73" t="s">
@@ -19282,20 +20047,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="89" t="s">
+      <c r="A17" s="93" t="s">
         <v>499</v>
       </c>
-      <c r="B17" s="94" t="s">
+      <c r="B17" s="98" t="s">
         <v>498</v>
       </c>
-      <c r="C17" s="89" t="s">
+      <c r="C17" s="93" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="222" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="90"/>
-      <c r="B18" s="96"/>
-      <c r="C18" s="90"/>
+      <c r="A18" s="94"/>
+      <c r="B18" s="100"/>
+      <c r="C18" s="94"/>
     </row>
     <row r="19" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -19353,18 +20118,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="97" t="s">
         <v>505</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -19422,25 +20187,25 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="89" t="s">
+      <c r="A8" s="93" t="s">
         <v>517</v>
       </c>
-      <c r="B8" s="94" t="s">
+      <c r="B8" s="98" t="s">
         <v>516</v>
       </c>
-      <c r="C8" s="89" t="s">
+      <c r="C8" s="93" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="100"/>
-      <c r="B9" s="95"/>
-      <c r="C9" s="100"/>
+      <c r="A9" s="104"/>
+      <c r="B9" s="99"/>
+      <c r="C9" s="104"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="90"/>
-      <c r="B10" s="96"/>
-      <c r="C10" s="90"/>
+      <c r="A10" s="94"/>
+      <c r="B10" s="100"/>
+      <c r="C10" s="94"/>
     </row>
     <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="54" t="s">
@@ -19454,86 +20219,86 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="89" t="s">
+      <c r="A12" s="93" t="s">
         <v>526</v>
       </c>
-      <c r="B12" s="94" t="s">
+      <c r="B12" s="98" t="s">
         <v>527</v>
       </c>
-      <c r="C12" s="89" t="s">
+      <c r="C12" s="93" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="100"/>
-      <c r="B13" s="95"/>
-      <c r="C13" s="100"/>
+      <c r="A13" s="104"/>
+      <c r="B13" s="99"/>
+      <c r="C13" s="104"/>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="100"/>
-      <c r="B14" s="95"/>
-      <c r="C14" s="100"/>
+      <c r="A14" s="104"/>
+      <c r="B14" s="99"/>
+      <c r="C14" s="104"/>
     </row>
     <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="100"/>
-      <c r="B15" s="95"/>
-      <c r="C15" s="100"/>
+      <c r="A15" s="104"/>
+      <c r="B15" s="99"/>
+      <c r="C15" s="104"/>
     </row>
     <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="100"/>
-      <c r="B16" s="95"/>
-      <c r="C16" s="100"/>
+      <c r="A16" s="104"/>
+      <c r="B16" s="99"/>
+      <c r="C16" s="104"/>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="100"/>
-      <c r="B17" s="95"/>
-      <c r="C17" s="100"/>
+      <c r="A17" s="104"/>
+      <c r="B17" s="99"/>
+      <c r="C17" s="104"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="90"/>
-      <c r="B18" s="95"/>
-      <c r="C18" s="90"/>
+      <c r="A18" s="94"/>
+      <c r="B18" s="99"/>
+      <c r="C18" s="94"/>
     </row>
     <row r="19" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="89" t="s">
+      <c r="A19" s="93" t="s">
         <v>529</v>
       </c>
-      <c r="B19" s="94" t="s">
+      <c r="B19" s="98" t="s">
         <v>528</v>
       </c>
-      <c r="C19" s="89" t="s">
+      <c r="C19" s="93" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="100"/>
-      <c r="B20" s="95"/>
-      <c r="C20" s="100"/>
+      <c r="A20" s="104"/>
+      <c r="B20" s="99"/>
+      <c r="C20" s="104"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="100"/>
-      <c r="B21" s="95"/>
-      <c r="C21" s="100"/>
+      <c r="A21" s="104"/>
+      <c r="B21" s="99"/>
+      <c r="C21" s="104"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="100"/>
-      <c r="B22" s="95"/>
-      <c r="C22" s="100"/>
+      <c r="A22" s="104"/>
+      <c r="B22" s="99"/>
+      <c r="C22" s="104"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="100"/>
-      <c r="B23" s="95"/>
-      <c r="C23" s="100"/>
+      <c r="A23" s="104"/>
+      <c r="B23" s="99"/>
+      <c r="C23" s="104"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="100"/>
-      <c r="B24" s="95"/>
-      <c r="C24" s="100"/>
+      <c r="A24" s="104"/>
+      <c r="B24" s="99"/>
+      <c r="C24" s="104"/>
     </row>
     <row r="25" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="90"/>
-      <c r="B25" s="96"/>
-      <c r="C25" s="90"/>
+      <c r="A25" s="94"/>
+      <c r="B25" s="100"/>
+      <c r="C25" s="94"/>
     </row>
     <row r="26" spans="1:3" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
@@ -19547,51 +20312,51 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="89" t="s">
+      <c r="A27" s="93" t="s">
         <v>533</v>
       </c>
-      <c r="B27" s="94" t="s">
+      <c r="B27" s="98" t="s">
         <v>532</v>
       </c>
-      <c r="C27" s="89" t="s">
+      <c r="C27" s="93" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="100"/>
-      <c r="B28" s="95"/>
-      <c r="C28" s="100"/>
+      <c r="A28" s="104"/>
+      <c r="B28" s="99"/>
+      <c r="C28" s="104"/>
     </row>
     <row r="29" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="90"/>
-      <c r="B29" s="96"/>
-      <c r="C29" s="90"/>
+      <c r="A29" s="94"/>
+      <c r="B29" s="100"/>
+      <c r="C29" s="94"/>
     </row>
     <row r="30" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="89" t="s">
+      <c r="A30" s="93" t="s">
         <v>536</v>
       </c>
-      <c r="B30" s="94" t="s">
+      <c r="B30" s="98" t="s">
         <v>535</v>
       </c>
-      <c r="C30" s="89" t="s">
+      <c r="C30" s="93" t="s">
         <v>537</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="100"/>
-      <c r="B31" s="95"/>
-      <c r="C31" s="100"/>
+      <c r="A31" s="104"/>
+      <c r="B31" s="99"/>
+      <c r="C31" s="104"/>
     </row>
     <row r="32" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="100"/>
-      <c r="B32" s="95"/>
-      <c r="C32" s="100"/>
+      <c r="A32" s="104"/>
+      <c r="B32" s="99"/>
+      <c r="C32" s="104"/>
     </row>
     <row r="33" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="90"/>
-      <c r="B33" s="96"/>
-      <c r="C33" s="90"/>
+      <c r="A33" s="94"/>
+      <c r="B33" s="100"/>
+      <c r="C33" s="94"/>
     </row>
     <row r="34" spans="1:3" ht="255" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
@@ -19657,18 +20422,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="97" t="s">
         <v>549</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -19763,18 +20528,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="97" t="s">
         <v>560</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -19836,11 +20601,11 @@
       <c r="C9" s="54"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="93" t="s">
+      <c r="A10" s="97" t="s">
         <v>575</v>
       </c>
-      <c r="B10" s="93"/>
-      <c r="C10" s="93"/>
+      <c r="B10" s="97"/>
+      <c r="C10" s="97"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
@@ -19943,8 +20708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28F7059E-AEF4-8341-85CB-91D20F555A19}">
   <dimension ref="A1:C93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19956,18 +20721,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="s">
-        <v>575</v>
-      </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
+      <c r="A2" s="97" t="s">
+        <v>661</v>
+      </c>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -20025,20 +20790,20 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="89" t="s">
+      <c r="A8" s="93" t="s">
         <v>587</v>
       </c>
-      <c r="B8" s="94" t="s">
+      <c r="B8" s="98" t="s">
         <v>590</v>
       </c>
-      <c r="C8" s="89" t="s">
+      <c r="C8" s="93" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="109" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="90"/>
-      <c r="B9" s="96"/>
-      <c r="C9" s="90"/>
+      <c r="A9" s="94"/>
+      <c r="B9" s="100"/>
+      <c r="C9" s="94"/>
     </row>
     <row r="10" spans="1:3" ht="109" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="82" t="s">
@@ -20074,20 +20839,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="89" t="s">
+      <c r="A13" s="93" t="s">
         <v>603</v>
       </c>
-      <c r="B13" s="94" t="s">
+      <c r="B13" s="98" t="s">
         <v>602</v>
       </c>
-      <c r="C13" s="89" t="s">
+      <c r="C13" s="93" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="90"/>
-      <c r="B14" s="96"/>
-      <c r="C14" s="90"/>
+      <c r="A14" s="94"/>
+      <c r="B14" s="100"/>
+      <c r="C14" s="94"/>
     </row>
     <row r="15" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="82" t="s">
@@ -20101,67 +20866,67 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="121" t="s">
+      <c r="A16" s="125" t="s">
         <v>609</v>
       </c>
-      <c r="B16" s="120" t="s">
+      <c r="B16" s="124" t="s">
         <v>608</v>
       </c>
-      <c r="C16" s="121" t="s">
+      <c r="C16" s="125" t="s">
         <v>610</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="121"/>
-      <c r="B17" s="120"/>
-      <c r="C17" s="121"/>
+      <c r="A17" s="125"/>
+      <c r="B17" s="124"/>
+      <c r="C17" s="125"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="121"/>
-      <c r="B18" s="120"/>
-      <c r="C18" s="121"/>
+      <c r="A18" s="125"/>
+      <c r="B18" s="124"/>
+      <c r="C18" s="125"/>
     </row>
     <row r="19" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="121"/>
-      <c r="B19" s="120"/>
-      <c r="C19" s="121"/>
+      <c r="A19" s="125"/>
+      <c r="B19" s="124"/>
+      <c r="C19" s="125"/>
     </row>
     <row r="20" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="121"/>
-      <c r="B20" s="120"/>
-      <c r="C20" s="121"/>
+      <c r="A20" s="125"/>
+      <c r="B20" s="124"/>
+      <c r="C20" s="125"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="121"/>
-      <c r="B21" s="120"/>
-      <c r="C21" s="121"/>
+      <c r="A21" s="125"/>
+      <c r="B21" s="124"/>
+      <c r="C21" s="125"/>
     </row>
     <row r="22" spans="1:3" ht="139" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="121"/>
-      <c r="B22" s="120"/>
-      <c r="C22" s="121"/>
+      <c r="A22" s="125"/>
+      <c r="B22" s="124"/>
+      <c r="C22" s="125"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="121"/>
-      <c r="B23" s="120" t="s">
+      <c r="A23" s="125"/>
+      <c r="B23" s="124" t="s">
         <v>611</v>
       </c>
-      <c r="C23" s="121"/>
+      <c r="C23" s="125"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="121"/>
-      <c r="B24" s="120"/>
-      <c r="C24" s="121"/>
+      <c r="A24" s="125"/>
+      <c r="B24" s="124"/>
+      <c r="C24" s="125"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="121"/>
-      <c r="B25" s="120"/>
-      <c r="C25" s="121"/>
+      <c r="A25" s="125"/>
+      <c r="B25" s="124"/>
+      <c r="C25" s="125"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="121"/>
-      <c r="B26" s="120"/>
-      <c r="C26" s="121"/>
+      <c r="A26" s="125"/>
+      <c r="B26" s="124"/>
+      <c r="C26" s="125"/>
     </row>
     <row r="27" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="85" t="s">
@@ -20230,185 +20995,185 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="89" t="s">
+      <c r="A33" s="93" t="s">
         <v>633</v>
       </c>
-      <c r="B33" s="91" t="s">
+      <c r="B33" s="95" t="s">
         <v>627</v>
       </c>
-      <c r="C33" s="89" t="s">
+      <c r="C33" s="93" t="s">
         <v>633</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="100"/>
-      <c r="B34" s="110"/>
-      <c r="C34" s="100"/>
+      <c r="A34" s="104"/>
+      <c r="B34" s="114"/>
+      <c r="C34" s="104"/>
     </row>
     <row r="35" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="100"/>
-      <c r="B35" s="110"/>
-      <c r="C35" s="100"/>
+      <c r="A35" s="104"/>
+      <c r="B35" s="114"/>
+      <c r="C35" s="104"/>
     </row>
     <row r="36" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="100"/>
-      <c r="B36" s="92"/>
-      <c r="C36" s="100"/>
+      <c r="A36" s="104"/>
+      <c r="B36" s="96"/>
+      <c r="C36" s="104"/>
     </row>
     <row r="37" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="100"/>
-      <c r="B37" s="91" t="s">
+      <c r="A37" s="104"/>
+      <c r="B37" s="95" t="s">
         <v>628</v>
       </c>
-      <c r="C37" s="100"/>
+      <c r="C37" s="104"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="100"/>
-      <c r="B38" s="110"/>
-      <c r="C38" s="100"/>
+      <c r="A38" s="104"/>
+      <c r="B38" s="114"/>
+      <c r="C38" s="104"/>
     </row>
     <row r="39" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="100"/>
-      <c r="B39" s="110"/>
-      <c r="C39" s="100"/>
+      <c r="A39" s="104"/>
+      <c r="B39" s="114"/>
+      <c r="C39" s="104"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="100"/>
-      <c r="B40" s="110"/>
-      <c r="C40" s="100"/>
+      <c r="A40" s="104"/>
+      <c r="B40" s="114"/>
+      <c r="C40" s="104"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="100"/>
-      <c r="B41" s="110"/>
-      <c r="C41" s="100"/>
+      <c r="A41" s="104"/>
+      <c r="B41" s="114"/>
+      <c r="C41" s="104"/>
     </row>
     <row r="42" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="100"/>
-      <c r="B42" s="110"/>
-      <c r="C42" s="100"/>
+      <c r="A42" s="104"/>
+      <c r="B42" s="114"/>
+      <c r="C42" s="104"/>
     </row>
     <row r="43" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="100"/>
-      <c r="B43" s="91" t="s">
+      <c r="A43" s="104"/>
+      <c r="B43" s="95" t="s">
         <v>629</v>
       </c>
-      <c r="C43" s="100"/>
+      <c r="C43" s="104"/>
     </row>
     <row r="44" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="100"/>
-      <c r="B44" s="110"/>
-      <c r="C44" s="100"/>
+      <c r="A44" s="104"/>
+      <c r="B44" s="114"/>
+      <c r="C44" s="104"/>
     </row>
     <row r="45" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="100"/>
-      <c r="B45" s="110"/>
-      <c r="C45" s="100"/>
+      <c r="A45" s="104"/>
+      <c r="B45" s="114"/>
+      <c r="C45" s="104"/>
     </row>
     <row r="46" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="100"/>
-      <c r="B46" s="110"/>
-      <c r="C46" s="100"/>
+      <c r="A46" s="104"/>
+      <c r="B46" s="114"/>
+      <c r="C46" s="104"/>
     </row>
     <row r="47" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="100"/>
-      <c r="B47" s="110"/>
-      <c r="C47" s="100"/>
+      <c r="A47" s="104"/>
+      <c r="B47" s="114"/>
+      <c r="C47" s="104"/>
     </row>
     <row r="48" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="100"/>
-      <c r="B48" s="110"/>
-      <c r="C48" s="100"/>
+      <c r="A48" s="104"/>
+      <c r="B48" s="114"/>
+      <c r="C48" s="104"/>
     </row>
     <row r="49" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="100"/>
-      <c r="B49" s="110"/>
-      <c r="C49" s="100"/>
+      <c r="A49" s="104"/>
+      <c r="B49" s="114"/>
+      <c r="C49" s="104"/>
     </row>
     <row r="50" spans="1:3" ht="320" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="100"/>
-      <c r="B50" s="92"/>
-      <c r="C50" s="100"/>
+      <c r="A50" s="104"/>
+      <c r="B50" s="96"/>
+      <c r="C50" s="104"/>
     </row>
     <row r="51" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="100"/>
-      <c r="B51" s="91" t="s">
+      <c r="A51" s="104"/>
+      <c r="B51" s="95" t="s">
         <v>630</v>
       </c>
-      <c r="C51" s="100"/>
+      <c r="C51" s="104"/>
     </row>
     <row r="52" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="100"/>
-      <c r="B52" s="110"/>
-      <c r="C52" s="100"/>
+      <c r="A52" s="104"/>
+      <c r="B52" s="114"/>
+      <c r="C52" s="104"/>
     </row>
     <row r="53" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="100"/>
-      <c r="B53" s="110"/>
-      <c r="C53" s="100"/>
+      <c r="A53" s="104"/>
+      <c r="B53" s="114"/>
+      <c r="C53" s="104"/>
     </row>
     <row r="54" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="100"/>
-      <c r="B54" s="110"/>
-      <c r="C54" s="100"/>
+      <c r="A54" s="104"/>
+      <c r="B54" s="114"/>
+      <c r="C54" s="104"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="100"/>
-      <c r="B55" s="110"/>
-      <c r="C55" s="100"/>
+      <c r="A55" s="104"/>
+      <c r="B55" s="114"/>
+      <c r="C55" s="104"/>
     </row>
     <row r="56" spans="1:3" ht="97" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="100"/>
-      <c r="B56" s="92"/>
-      <c r="C56" s="100"/>
+      <c r="A56" s="104"/>
+      <c r="B56" s="96"/>
+      <c r="C56" s="104"/>
     </row>
     <row r="57" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="100"/>
-      <c r="B57" s="91" t="s">
+      <c r="A57" s="104"/>
+      <c r="B57" s="95" t="s">
         <v>631</v>
       </c>
-      <c r="C57" s="100"/>
+      <c r="C57" s="104"/>
     </row>
     <row r="58" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="100"/>
-      <c r="B58" s="110"/>
-      <c r="C58" s="100"/>
+      <c r="A58" s="104"/>
+      <c r="B58" s="114"/>
+      <c r="C58" s="104"/>
     </row>
     <row r="59" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="100"/>
-      <c r="B59" s="110"/>
-      <c r="C59" s="100"/>
+      <c r="A59" s="104"/>
+      <c r="B59" s="114"/>
+      <c r="C59" s="104"/>
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="100"/>
-      <c r="B60" s="110"/>
-      <c r="C60" s="100"/>
+      <c r="A60" s="104"/>
+      <c r="B60" s="114"/>
+      <c r="C60" s="104"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="100"/>
-      <c r="B61" s="110"/>
-      <c r="C61" s="100"/>
+      <c r="A61" s="104"/>
+      <c r="B61" s="114"/>
+      <c r="C61" s="104"/>
     </row>
     <row r="62" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="100"/>
-      <c r="B62" s="110"/>
-      <c r="C62" s="100"/>
+      <c r="A62" s="104"/>
+      <c r="B62" s="114"/>
+      <c r="C62" s="104"/>
     </row>
     <row r="63" spans="1:3" ht="146" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="100"/>
-      <c r="B63" s="92"/>
-      <c r="C63" s="100"/>
+      <c r="A63" s="104"/>
+      <c r="B63" s="96"/>
+      <c r="C63" s="104"/>
     </row>
     <row r="64" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="100"/>
-      <c r="B64" s="91" t="s">
+      <c r="A64" s="104"/>
+      <c r="B64" s="95" t="s">
         <v>632</v>
       </c>
-      <c r="C64" s="100"/>
+      <c r="C64" s="104"/>
     </row>
     <row r="65" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="90"/>
-      <c r="B65" s="92"/>
-      <c r="C65" s="90"/>
+      <c r="A65" s="94"/>
+      <c r="B65" s="96"/>
+      <c r="C65" s="94"/>
     </row>
     <row r="66" spans="1:3" ht="397" x14ac:dyDescent="0.2">
       <c r="A66" s="85" t="s">
@@ -20422,93 +21187,93 @@
       </c>
     </row>
     <row r="67" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="101" t="s">
+      <c r="A67" s="105" t="s">
         <v>638</v>
       </c>
-      <c r="B67" s="109" t="s">
+      <c r="B67" s="113" t="s">
         <v>637</v>
       </c>
-      <c r="C67" s="101" t="s">
+      <c r="C67" s="105" t="s">
         <v>639</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="101"/>
-      <c r="B68" s="109"/>
-      <c r="C68" s="101"/>
+      <c r="A68" s="105"/>
+      <c r="B68" s="113"/>
+      <c r="C68" s="105"/>
     </row>
     <row r="69" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="101"/>
-      <c r="B69" s="109"/>
-      <c r="C69" s="101"/>
+      <c r="A69" s="105"/>
+      <c r="B69" s="113"/>
+      <c r="C69" s="105"/>
     </row>
     <row r="70" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="101" t="s">
+      <c r="A70" s="105" t="s">
         <v>643</v>
       </c>
-      <c r="B70" s="109" t="s">
+      <c r="B70" s="113" t="s">
         <v>640</v>
       </c>
-      <c r="C70" s="101" t="s">
+      <c r="C70" s="105" t="s">
         <v>642</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="101"/>
-      <c r="B71" s="109"/>
-      <c r="C71" s="101"/>
+      <c r="A71" s="105"/>
+      <c r="B71" s="113"/>
+      <c r="C71" s="105"/>
     </row>
     <row r="72" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="101"/>
-      <c r="B72" s="109"/>
-      <c r="C72" s="101"/>
+      <c r="A72" s="105"/>
+      <c r="B72" s="113"/>
+      <c r="C72" s="105"/>
     </row>
     <row r="73" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="101"/>
-      <c r="B73" s="109"/>
-      <c r="C73" s="101"/>
+      <c r="A73" s="105"/>
+      <c r="B73" s="113"/>
+      <c r="C73" s="105"/>
     </row>
     <row r="74" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="101"/>
-      <c r="B74" s="109"/>
-      <c r="C74" s="101"/>
+      <c r="A74" s="105"/>
+      <c r="B74" s="113"/>
+      <c r="C74" s="105"/>
     </row>
     <row r="75" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="101"/>
-      <c r="B75" s="109"/>
-      <c r="C75" s="101"/>
+      <c r="A75" s="105"/>
+      <c r="B75" s="113"/>
+      <c r="C75" s="105"/>
     </row>
     <row r="76" spans="1:3" ht="214" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="101"/>
-      <c r="B76" s="109"/>
-      <c r="C76" s="101"/>
+      <c r="A76" s="105"/>
+      <c r="B76" s="113"/>
+      <c r="C76" s="105"/>
     </row>
     <row r="77" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="101"/>
-      <c r="B77" s="109" t="s">
+      <c r="A77" s="105"/>
+      <c r="B77" s="113" t="s">
         <v>641</v>
       </c>
-      <c r="C77" s="101"/>
+      <c r="C77" s="105"/>
     </row>
     <row r="78" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="101"/>
-      <c r="B78" s="109"/>
-      <c r="C78" s="101"/>
+      <c r="A78" s="105"/>
+      <c r="B78" s="113"/>
+      <c r="C78" s="105"/>
     </row>
     <row r="79" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="101"/>
-      <c r="B79" s="109"/>
-      <c r="C79" s="101"/>
+      <c r="A79" s="105"/>
+      <c r="B79" s="113"/>
+      <c r="C79" s="105"/>
     </row>
     <row r="80" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="101"/>
-      <c r="B80" s="109"/>
-      <c r="C80" s="101"/>
+      <c r="A80" s="105"/>
+      <c r="B80" s="113"/>
+      <c r="C80" s="105"/>
     </row>
     <row r="81" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="101"/>
-      <c r="B81" s="109"/>
-      <c r="C81" s="101"/>
+      <c r="A81" s="105"/>
+      <c r="B81" s="113"/>
+      <c r="C81" s="105"/>
     </row>
     <row r="82" spans="1:3" ht="56" x14ac:dyDescent="0.2">
       <c r="A82" s="82" t="s">
@@ -20555,40 +21320,40 @@
       </c>
     </row>
     <row r="86" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="89" t="s">
+      <c r="A86" s="93" t="s">
         <v>657</v>
       </c>
-      <c r="B86" s="94" t="s">
+      <c r="B86" s="98" t="s">
         <v>656</v>
       </c>
-      <c r="C86" s="89" t="s">
+      <c r="C86" s="93" t="s">
         <v>658</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="100"/>
-      <c r="B87" s="95"/>
-      <c r="C87" s="100"/>
+      <c r="A87" s="104"/>
+      <c r="B87" s="99"/>
+      <c r="C87" s="104"/>
     </row>
     <row r="88" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="100"/>
-      <c r="B88" s="95"/>
-      <c r="C88" s="100"/>
+      <c r="A88" s="104"/>
+      <c r="B88" s="99"/>
+      <c r="C88" s="104"/>
     </row>
     <row r="89" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="100"/>
-      <c r="B89" s="95"/>
-      <c r="C89" s="100"/>
+      <c r="A89" s="104"/>
+      <c r="B89" s="99"/>
+      <c r="C89" s="104"/>
     </row>
     <row r="90" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="100"/>
-      <c r="B90" s="95"/>
-      <c r="C90" s="100"/>
+      <c r="A90" s="104"/>
+      <c r="B90" s="99"/>
+      <c r="C90" s="104"/>
     </row>
     <row r="91" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="90"/>
-      <c r="B91" s="96"/>
-      <c r="C91" s="90"/>
+      <c r="A91" s="94"/>
+      <c r="B91" s="100"/>
+      <c r="C91" s="94"/>
     </row>
     <row r="92" spans="1:3" ht="221" x14ac:dyDescent="0.2">
       <c r="A92" s="16" t="s">
@@ -20651,6 +21416,162 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C21A766-C376-EB46-A7F6-E0E4ECA4E1CD}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="91" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="97" t="s">
+        <v>662</v>
+      </c>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="89" t="s">
+        <v>663</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>605</v>
+      </c>
+      <c r="C4" s="89" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="323" x14ac:dyDescent="0.2">
+      <c r="A5" s="89" t="s">
+        <v>666</v>
+      </c>
+      <c r="B5" s="58" t="s">
+        <v>665</v>
+      </c>
+      <c r="C5" s="89" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="84" x14ac:dyDescent="0.2">
+      <c r="A6" s="90" t="s">
+        <v>669</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>668</v>
+      </c>
+      <c r="C6" s="90" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="93" t="s">
+        <v>672</v>
+      </c>
+      <c r="B7" s="98" t="s">
+        <v>671</v>
+      </c>
+      <c r="C7" s="93" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="104"/>
+      <c r="B8" s="99"/>
+      <c r="C8" s="104"/>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="104"/>
+      <c r="B9" s="99"/>
+      <c r="C9" s="104"/>
+    </row>
+    <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="104"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="104"/>
+    </row>
+    <row r="11" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="104"/>
+      <c r="B11" s="99"/>
+      <c r="C11" s="104"/>
+    </row>
+    <row r="12" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="94"/>
+      <c r="B12" s="100"/>
+      <c r="C12" s="94"/>
+    </row>
+    <row r="13" spans="1:3" ht="210" x14ac:dyDescent="0.2">
+      <c r="A13" s="87" t="s">
+        <v>675</v>
+      </c>
+      <c r="B13" s="88" t="s">
+        <v>674</v>
+      </c>
+      <c r="C13" s="87" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="132" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="133" t="s">
+        <v>677</v>
+      </c>
+      <c r="C15" s="132" t="s">
+        <v>559</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="5">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="C7:C12"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE113606-3FFA-8545-9BE3-5643B52A7CE9}">
   <dimension ref="A1:H116"/>
   <sheetViews>
@@ -20728,10 +21649,10 @@
       <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="125" t="s">
+      <c r="A6" s="129" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="125"/>
+      <c r="B6" s="129"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -21704,32 +22625,32 @@
       <c r="H73" s="23"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="122"/>
-      <c r="B74" s="126"/>
+      <c r="A74" s="126"/>
+      <c r="B74" s="130"/>
       <c r="C74" s="32" t="s">
         <v>225</v>
       </c>
       <c r="D74" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="E74" s="127"/>
-      <c r="F74" s="122"/>
-      <c r="G74" s="124"/>
-      <c r="H74" s="122"/>
+      <c r="E74" s="131"/>
+      <c r="F74" s="126"/>
+      <c r="G74" s="128"/>
+      <c r="H74" s="126"/>
     </row>
     <row r="75" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A75" s="122"/>
-      <c r="B75" s="126"/>
+      <c r="A75" s="126"/>
+      <c r="B75" s="130"/>
       <c r="C75" s="33" t="s">
         <v>226</v>
       </c>
       <c r="D75" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="E75" s="127"/>
-      <c r="F75" s="122"/>
-      <c r="G75" s="124"/>
-      <c r="H75" s="122"/>
+      <c r="E75" s="131"/>
+      <c r="F75" s="126"/>
+      <c r="G75" s="128"/>
+      <c r="H75" s="126"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="23"/>
@@ -21902,34 +22823,34 @@
       <c r="H88" s="23"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="122"/>
-      <c r="B89" s="122"/>
+      <c r="A89" s="126"/>
+      <c r="B89" s="126"/>
       <c r="C89" s="35" t="s">
         <v>225</v>
       </c>
       <c r="D89" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="E89" s="123" t="s">
+      <c r="E89" s="127" t="s">
         <v>121</v>
       </c>
-      <c r="F89" s="123"/>
-      <c r="G89" s="124"/>
-      <c r="H89" s="122"/>
+      <c r="F89" s="127"/>
+      <c r="G89" s="128"/>
+      <c r="H89" s="126"/>
     </row>
     <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A90" s="122"/>
-      <c r="B90" s="122"/>
+      <c r="A90" s="126"/>
+      <c r="B90" s="126"/>
       <c r="C90" s="35" t="s">
         <v>242</v>
       </c>
       <c r="D90" s="35" t="s">
         <v>243</v>
       </c>
-      <c r="E90" s="123"/>
-      <c r="F90" s="123"/>
-      <c r="G90" s="124"/>
-      <c r="H90" s="122"/>
+      <c r="E90" s="127"/>
+      <c r="F90" s="127"/>
+      <c r="G90" s="128"/>
+      <c r="H90" s="126"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="23"/>
@@ -22315,7 +23236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -22409,134 +23330,6 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A16">
     <sortCondition ref="A1:A16"/>
   </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0BB7-C151-C94B-945C-E2CA92034B13}">
-  <dimension ref="A1:C15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-    </row>
-    <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-    </row>
-    <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="B4" s="48" t="s">
-        <v>279</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="54"/>
-      <c r="B6" s="55"/>
-      <c r="C6" s="54"/>
-    </row>
-    <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="54"/>
-      <c r="B7" s="55"/>
-      <c r="C7" s="54"/>
-    </row>
-    <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="54"/>
-      <c r="B8" s="55"/>
-      <c r="C8" s="54"/>
-    </row>
-    <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="56"/>
-      <c r="B11" s="55"/>
-      <c r="C11" s="56"/>
-    </row>
-    <row r="12" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="56"/>
-      <c r="B12" s="55"/>
-      <c r="C12" s="56"/>
-    </row>
-    <row r="13" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="56"/>
-      <c r="B13" s="55"/>
-      <c r="C13" s="56"/>
-    </row>
-    <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A14" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>298</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>98</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -22558,18 +23351,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="97" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -22620,11 +23413,11 @@
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="93" t="s">
+      <c r="A9" s="97" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="93"/>
-      <c r="C9" s="93"/>
+      <c r="B9" s="97"/>
+      <c r="C9" s="97"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -22660,20 +23453,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="89" t="s">
+      <c r="A13" s="93" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="91" t="s">
+      <c r="B13" s="95" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="89" t="s">
+      <c r="C13" s="93" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="90"/>
-      <c r="B14" s="92"/>
-      <c r="C14" s="90"/>
+      <c r="A14" s="94"/>
+      <c r="B14" s="96"/>
+      <c r="C14" s="94"/>
     </row>
     <row r="15" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
@@ -22698,20 +23491,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="89" t="s">
+      <c r="A17" s="93" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="91" t="s">
+      <c r="B17" s="95" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="89" t="s">
+      <c r="C17" s="93" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="90"/>
-      <c r="B18" s="92"/>
-      <c r="C18" s="90"/>
+      <c r="A18" s="94"/>
+      <c r="B18" s="96"/>
+      <c r="C18" s="94"/>
     </row>
     <row r="19" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -22747,6 +23540,134 @@
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="C13:C14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0BB7-C151-C94B-945C-E2CA92034B13}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="91" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="97" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>279</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="48"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="54"/>
+      <c r="B6" s="55"/>
+      <c r="C6" s="54"/>
+    </row>
+    <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="54"/>
+      <c r="B7" s="55"/>
+      <c r="C7" s="54"/>
+    </row>
+    <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="54"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="54"/>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="56"/>
+      <c r="B11" s="55"/>
+      <c r="C11" s="56"/>
+    </row>
+    <row r="12" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="56"/>
+      <c r="B12" s="55"/>
+      <c r="C12" s="56"/>
+    </row>
+    <row r="13" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="56"/>
+      <c r="B13" s="55"/>
+      <c r="C13" s="56"/>
+    </row>
+    <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A14" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="18" t="s">
+        <v>298</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22769,18 +23690,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="97" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -22816,25 +23737,25 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="89" t="s">
+      <c r="A6" s="93" t="s">
         <v>292</v>
       </c>
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="98" t="s">
         <v>291</v>
       </c>
-      <c r="C6" s="89" t="s">
+      <c r="C6" s="93" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="100"/>
-      <c r="B7" s="95"/>
-      <c r="C7" s="100"/>
+      <c r="A7" s="104"/>
+      <c r="B7" s="99"/>
+      <c r="C7" s="104"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="90"/>
-      <c r="B8" s="96"/>
-      <c r="C8" s="90"/>
+      <c r="A8" s="94"/>
+      <c r="B8" s="100"/>
+      <c r="C8" s="94"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -22859,25 +23780,25 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="97" t="s">
+      <c r="A11" s="101" t="s">
         <v>294</v>
       </c>
-      <c r="B11" s="94" t="s">
+      <c r="B11" s="98" t="s">
         <v>295</v>
       </c>
-      <c r="C11" s="97" t="s">
+      <c r="C11" s="101" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="98"/>
-      <c r="B12" s="95"/>
-      <c r="C12" s="98"/>
+      <c r="A12" s="102"/>
+      <c r="B12" s="99"/>
+      <c r="C12" s="102"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="99"/>
-      <c r="B13" s="96"/>
-      <c r="C13" s="99"/>
+      <c r="A13" s="103"/>
+      <c r="B13" s="100"/>
+      <c r="C13" s="103"/>
     </row>
     <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
@@ -22934,18 +23855,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="97" t="s">
         <v>299</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -22959,46 +23880,46 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="101" t="s">
+      <c r="A4" s="105" t="s">
         <v>300</v>
       </c>
-      <c r="B4" s="105" t="s">
+      <c r="B4" s="109" t="s">
         <v>305</v>
       </c>
-      <c r="C4" s="101" t="s">
+      <c r="C4" s="105" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="101"/>
-      <c r="B5" s="105"/>
-      <c r="C5" s="101"/>
+      <c r="A5" s="105"/>
+      <c r="B5" s="109"/>
+      <c r="C5" s="105"/>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="101"/>
-      <c r="B6" s="105"/>
-      <c r="C6" s="101"/>
+      <c r="A6" s="105"/>
+      <c r="B6" s="109"/>
+      <c r="C6" s="105"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="93" t="s">
         <v>302</v>
       </c>
-      <c r="B7" s="102" t="s">
+      <c r="B7" s="106" t="s">
         <v>303</v>
       </c>
-      <c r="C7" s="89" t="s">
+      <c r="C7" s="93" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="100"/>
-      <c r="B8" s="103"/>
-      <c r="C8" s="100"/>
+      <c r="A8" s="104"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="104"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="228" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="90"/>
-      <c r="B9" s="104"/>
-      <c r="C9" s="90"/>
+      <c r="A9" s="94"/>
+      <c r="B9" s="108"/>
+      <c r="C9" s="94"/>
     </row>
     <row r="10" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
@@ -23055,18 +23976,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="97" t="s">
         <v>331</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -23113,233 +24034,233 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="89" t="s">
+      <c r="A7" s="93" t="s">
         <v>314</v>
       </c>
-      <c r="B7" s="94" t="s">
+      <c r="B7" s="98" t="s">
         <v>322</v>
       </c>
-      <c r="C7" s="89" t="s">
+      <c r="C7" s="93" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="100"/>
-      <c r="B8" s="95"/>
-      <c r="C8" s="100"/>
+      <c r="A8" s="104"/>
+      <c r="B8" s="99"/>
+      <c r="C8" s="104"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="100"/>
-      <c r="B9" s="95"/>
-      <c r="C9" s="100"/>
+      <c r="A9" s="104"/>
+      <c r="B9" s="99"/>
+      <c r="C9" s="104"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="100"/>
-      <c r="B10" s="95"/>
-      <c r="C10" s="100"/>
+      <c r="A10" s="104"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="104"/>
     </row>
     <row r="11" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="100"/>
-      <c r="B11" s="95"/>
-      <c r="C11" s="100"/>
+      <c r="A11" s="104"/>
+      <c r="B11" s="99"/>
+      <c r="C11" s="104"/>
     </row>
     <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="100"/>
-      <c r="B12" s="95"/>
-      <c r="C12" s="100"/>
+      <c r="A12" s="104"/>
+      <c r="B12" s="99"/>
+      <c r="C12" s="104"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="90"/>
-      <c r="B13" s="96"/>
-      <c r="C13" s="90"/>
+      <c r="A13" s="94"/>
+      <c r="B13" s="100"/>
+      <c r="C13" s="94"/>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="89" t="s">
+      <c r="A14" s="93" t="s">
         <v>325</v>
       </c>
-      <c r="B14" s="94" t="s">
+      <c r="B14" s="98" t="s">
         <v>323</v>
       </c>
-      <c r="C14" s="89" t="s">
+      <c r="C14" s="93" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="100"/>
-      <c r="B15" s="95"/>
-      <c r="C15" s="100"/>
+      <c r="A15" s="104"/>
+      <c r="B15" s="99"/>
+      <c r="C15" s="104"/>
     </row>
     <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="100"/>
-      <c r="B16" s="95"/>
-      <c r="C16" s="100"/>
+      <c r="A16" s="104"/>
+      <c r="B16" s="99"/>
+      <c r="C16" s="104"/>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="100"/>
-      <c r="B17" s="95"/>
-      <c r="C17" s="100"/>
+      <c r="A17" s="104"/>
+      <c r="B17" s="99"/>
+      <c r="C17" s="104"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="100"/>
-      <c r="B18" s="95"/>
-      <c r="C18" s="100"/>
+      <c r="A18" s="104"/>
+      <c r="B18" s="99"/>
+      <c r="C18" s="104"/>
     </row>
     <row r="19" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="100"/>
-      <c r="B19" s="95"/>
-      <c r="C19" s="100"/>
+      <c r="A19" s="104"/>
+      <c r="B19" s="99"/>
+      <c r="C19" s="104"/>
     </row>
     <row r="20" spans="1:3" ht="155" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="100"/>
-      <c r="B20" s="96"/>
-      <c r="C20" s="100"/>
+      <c r="A20" s="104"/>
+      <c r="B20" s="100"/>
+      <c r="C20" s="104"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="100"/>
-      <c r="B21" s="94" t="s">
+      <c r="A21" s="104"/>
+      <c r="B21" s="98" t="s">
         <v>316</v>
       </c>
-      <c r="C21" s="100"/>
+      <c r="C21" s="104"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="100"/>
-      <c r="B22" s="95"/>
-      <c r="C22" s="100"/>
+      <c r="A22" s="104"/>
+      <c r="B22" s="99"/>
+      <c r="C22" s="104"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="100"/>
-      <c r="B23" s="95"/>
-      <c r="C23" s="100"/>
+      <c r="A23" s="104"/>
+      <c r="B23" s="99"/>
+      <c r="C23" s="104"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="100"/>
-      <c r="B24" s="95"/>
-      <c r="C24" s="100"/>
+      <c r="A24" s="104"/>
+      <c r="B24" s="99"/>
+      <c r="C24" s="104"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="100"/>
-      <c r="B25" s="95"/>
-      <c r="C25" s="100"/>
+      <c r="A25" s="104"/>
+      <c r="B25" s="99"/>
+      <c r="C25" s="104"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="100"/>
-      <c r="B26" s="95"/>
-      <c r="C26" s="100"/>
+      <c r="A26" s="104"/>
+      <c r="B26" s="99"/>
+      <c r="C26" s="104"/>
     </row>
     <row r="27" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="100"/>
-      <c r="B27" s="96"/>
-      <c r="C27" s="100"/>
+      <c r="A27" s="104"/>
+      <c r="B27" s="100"/>
+      <c r="C27" s="104"/>
     </row>
     <row r="28" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="100"/>
-      <c r="B28" s="94" t="s">
+      <c r="A28" s="104"/>
+      <c r="B28" s="98" t="s">
         <v>317</v>
       </c>
-      <c r="C28" s="100"/>
+      <c r="C28" s="104"/>
     </row>
     <row r="29" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="100"/>
-      <c r="B29" s="95"/>
-      <c r="C29" s="100"/>
+      <c r="A29" s="104"/>
+      <c r="B29" s="99"/>
+      <c r="C29" s="104"/>
     </row>
     <row r="30" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="100"/>
-      <c r="B30" s="95"/>
-      <c r="C30" s="100"/>
+      <c r="A30" s="104"/>
+      <c r="B30" s="99"/>
+      <c r="C30" s="104"/>
     </row>
     <row r="31" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="100"/>
-      <c r="B31" s="95"/>
-      <c r="C31" s="100"/>
+      <c r="A31" s="104"/>
+      <c r="B31" s="99"/>
+      <c r="C31" s="104"/>
     </row>
     <row r="32" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="100"/>
-      <c r="B32" s="95"/>
-      <c r="C32" s="100"/>
+      <c r="A32" s="104"/>
+      <c r="B32" s="99"/>
+      <c r="C32" s="104"/>
     </row>
     <row r="33" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="100"/>
-      <c r="B33" s="95"/>
-      <c r="C33" s="100"/>
+      <c r="A33" s="104"/>
+      <c r="B33" s="99"/>
+      <c r="C33" s="104"/>
     </row>
     <row r="34" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="100"/>
-      <c r="B34" s="95"/>
-      <c r="C34" s="100"/>
+      <c r="A34" s="104"/>
+      <c r="B34" s="99"/>
+      <c r="C34" s="104"/>
     </row>
     <row r="35" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="100"/>
-      <c r="B35" s="95"/>
-      <c r="C35" s="100"/>
+      <c r="A35" s="104"/>
+      <c r="B35" s="99"/>
+      <c r="C35" s="104"/>
     </row>
     <row r="36" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="100"/>
-      <c r="B36" s="95"/>
-      <c r="C36" s="100"/>
+      <c r="A36" s="104"/>
+      <c r="B36" s="99"/>
+      <c r="C36" s="104"/>
     </row>
     <row r="37" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="100"/>
-      <c r="B37" s="96"/>
-      <c r="C37" s="100"/>
+      <c r="A37" s="104"/>
+      <c r="B37" s="100"/>
+      <c r="C37" s="104"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="100"/>
-      <c r="B38" s="94" t="s">
+      <c r="A38" s="104"/>
+      <c r="B38" s="98" t="s">
         <v>318</v>
       </c>
-      <c r="C38" s="100"/>
+      <c r="C38" s="104"/>
     </row>
     <row r="39" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="100"/>
-      <c r="B39" s="95"/>
-      <c r="C39" s="100"/>
+      <c r="A39" s="104"/>
+      <c r="B39" s="99"/>
+      <c r="C39" s="104"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="100"/>
-      <c r="B40" s="95"/>
-      <c r="C40" s="100"/>
+      <c r="A40" s="104"/>
+      <c r="B40" s="99"/>
+      <c r="C40" s="104"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="100"/>
-      <c r="B41" s="95"/>
-      <c r="C41" s="100"/>
+      <c r="A41" s="104"/>
+      <c r="B41" s="99"/>
+      <c r="C41" s="104"/>
     </row>
     <row r="42" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="90"/>
-      <c r="B42" s="96"/>
-      <c r="C42" s="90"/>
+      <c r="A42" s="94"/>
+      <c r="B42" s="100"/>
+      <c r="C42" s="94"/>
     </row>
     <row r="43" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="89" t="s">
+      <c r="A43" s="93" t="s">
         <v>326</v>
       </c>
-      <c r="B43" s="94" t="s">
+      <c r="B43" s="98" t="s">
         <v>327</v>
       </c>
-      <c r="C43" s="89" t="s">
+      <c r="C43" s="93" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="100"/>
-      <c r="B44" s="95"/>
-      <c r="C44" s="100"/>
+      <c r="A44" s="104"/>
+      <c r="B44" s="99"/>
+      <c r="C44" s="104"/>
     </row>
     <row r="45" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="100"/>
-      <c r="B45" s="95"/>
-      <c r="C45" s="100"/>
+      <c r="A45" s="104"/>
+      <c r="B45" s="99"/>
+      <c r="C45" s="104"/>
     </row>
     <row r="46" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="100"/>
-      <c r="B46" s="95"/>
-      <c r="C46" s="100"/>
+      <c r="A46" s="104"/>
+      <c r="B46" s="99"/>
+      <c r="C46" s="104"/>
     </row>
     <row r="47" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="90"/>
-      <c r="B47" s="96"/>
-      <c r="C47" s="90"/>
+      <c r="A47" s="94"/>
+      <c r="B47" s="100"/>
+      <c r="C47" s="94"/>
     </row>
     <row r="48" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
@@ -23402,18 +24323,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="97" t="s">
         <v>332</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -23552,18 +24473,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="97" t="s">
         <v>356</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -23647,18 +24568,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="97" t="s">
         <v>365</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -23683,20 +24604,20 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="89" t="s">
+      <c r="A5" s="93" t="s">
         <v>369</v>
       </c>
-      <c r="B5" s="106" t="s">
+      <c r="B5" s="110" t="s">
         <v>372</v>
       </c>
-      <c r="C5" s="89" t="s">
+      <c r="C5" s="93" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="90"/>
-      <c r="B6" s="108"/>
-      <c r="C6" s="90"/>
+      <c r="A6" s="94"/>
+      <c r="B6" s="112"/>
+      <c r="C6" s="94"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A7" s="59" t="s">
@@ -23710,67 +24631,67 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="89" t="s">
+      <c r="A8" s="93" t="s">
         <v>376</v>
       </c>
-      <c r="B8" s="106" t="s">
+      <c r="B8" s="110" t="s">
         <v>375</v>
       </c>
-      <c r="C8" s="89" t="s">
+      <c r="C8" s="93" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="100"/>
-      <c r="B9" s="107"/>
-      <c r="C9" s="100"/>
+      <c r="A9" s="104"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="104"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="90"/>
-      <c r="B10" s="108"/>
-      <c r="C10" s="90"/>
+      <c r="A10" s="94"/>
+      <c r="B10" s="112"/>
+      <c r="C10" s="94"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="89" t="s">
+      <c r="A11" s="93" t="s">
         <v>378</v>
       </c>
-      <c r="B11" s="106" t="s">
+      <c r="B11" s="110" t="s">
         <v>384</v>
       </c>
-      <c r="C11" s="89" t="s">
+      <c r="C11" s="93" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="100"/>
-      <c r="B12" s="107"/>
-      <c r="C12" s="100"/>
+      <c r="A12" s="104"/>
+      <c r="B12" s="111"/>
+      <c r="C12" s="104"/>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="187" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="90"/>
-      <c r="B13" s="108"/>
-      <c r="C13" s="90"/>
+      <c r="A13" s="94"/>
+      <c r="B13" s="112"/>
+      <c r="C13" s="94"/>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="89" t="s">
+      <c r="A14" s="93" t="s">
         <v>380</v>
       </c>
-      <c r="B14" s="106" t="s">
+      <c r="B14" s="110" t="s">
         <v>383</v>
       </c>
-      <c r="C14" s="89" t="s">
+      <c r="C14" s="93" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="100"/>
-      <c r="B15" s="107"/>
-      <c r="C15" s="100"/>
+      <c r="A15" s="104"/>
+      <c r="B15" s="111"/>
+      <c r="C15" s="104"/>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="90"/>
-      <c r="B16" s="108"/>
-      <c r="C16" s="90"/>
+      <c r="A16" s="94"/>
+      <c r="B16" s="112"/>
+      <c r="C16" s="94"/>
     </row>
     <row r="17" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
@@ -23833,18 +24754,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="91" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="93" t="s">
+      <c r="A2" s="97" t="s">
         <v>395</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
+      <c r="B2" s="97"/>
+      <c r="C2" s="97"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -23867,217 +24788,217 @@
       <c r="C4" s="60"/>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="89" t="s">
+      <c r="A5" s="93" t="s">
         <v>397</v>
       </c>
-      <c r="B5" s="111" t="s">
+      <c r="B5" s="115" t="s">
         <v>396</v>
       </c>
-      <c r="C5" s="89" t="s">
+      <c r="C5" s="93" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="283" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="100"/>
-      <c r="B6" s="112"/>
-      <c r="C6" s="100"/>
+      <c r="A6" s="104"/>
+      <c r="B6" s="116"/>
+      <c r="C6" s="104"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="100"/>
-      <c r="B7" s="112"/>
-      <c r="C7" s="100"/>
+      <c r="A7" s="104"/>
+      <c r="B7" s="116"/>
+      <c r="C7" s="104"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="100"/>
-      <c r="B8" s="112"/>
-      <c r="C8" s="100"/>
+      <c r="A8" s="104"/>
+      <c r="B8" s="116"/>
+      <c r="C8" s="104"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="100"/>
-      <c r="B9" s="112"/>
-      <c r="C9" s="100"/>
+      <c r="A9" s="104"/>
+      <c r="B9" s="116"/>
+      <c r="C9" s="104"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="100"/>
-      <c r="B10" s="112"/>
-      <c r="C10" s="100"/>
+      <c r="A10" s="104"/>
+      <c r="B10" s="116"/>
+      <c r="C10" s="104"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="100"/>
-      <c r="B11" s="112"/>
-      <c r="C11" s="100"/>
+      <c r="A11" s="104"/>
+      <c r="B11" s="116"/>
+      <c r="C11" s="104"/>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="90"/>
-      <c r="B12" s="113"/>
-      <c r="C12" s="90"/>
+      <c r="A12" s="94"/>
+      <c r="B12" s="117"/>
+      <c r="C12" s="94"/>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="89" t="s">
+      <c r="A13" s="93" t="s">
         <v>399</v>
       </c>
-      <c r="B13" s="94" t="s">
+      <c r="B13" s="98" t="s">
         <v>400</v>
       </c>
-      <c r="C13" s="89" t="s">
+      <c r="C13" s="93" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="100"/>
-      <c r="B14" s="95"/>
-      <c r="C14" s="100"/>
+      <c r="A14" s="104"/>
+      <c r="B14" s="99"/>
+      <c r="C14" s="104"/>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="100"/>
-      <c r="B15" s="95"/>
-      <c r="C15" s="100"/>
+      <c r="A15" s="104"/>
+      <c r="B15" s="99"/>
+      <c r="C15" s="104"/>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="100"/>
-      <c r="B16" s="94" t="s">
+      <c r="A16" s="104"/>
+      <c r="B16" s="98" t="s">
         <v>401</v>
       </c>
-      <c r="C16" s="100"/>
+      <c r="C16" s="104"/>
     </row>
     <row r="17" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="100"/>
-      <c r="B17" s="95"/>
-      <c r="C17" s="100"/>
+      <c r="A17" s="104"/>
+      <c r="B17" s="99"/>
+      <c r="C17" s="104"/>
     </row>
     <row r="18" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="100"/>
-      <c r="B18" s="95"/>
-      <c r="C18" s="100"/>
+      <c r="A18" s="104"/>
+      <c r="B18" s="99"/>
+      <c r="C18" s="104"/>
     </row>
     <row r="19" spans="1:3" s="13" customFormat="1" ht="159" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="100"/>
-      <c r="B19" s="95"/>
-      <c r="C19" s="100"/>
+      <c r="A19" s="104"/>
+      <c r="B19" s="99"/>
+      <c r="C19" s="104"/>
     </row>
     <row r="20" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="100"/>
-      <c r="B20" s="95" t="s">
+      <c r="A20" s="104"/>
+      <c r="B20" s="99" t="s">
         <v>402</v>
       </c>
-      <c r="C20" s="100"/>
+      <c r="C20" s="104"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="100"/>
-      <c r="B21" s="95"/>
-      <c r="C21" s="100"/>
+      <c r="A21" s="104"/>
+      <c r="B21" s="99"/>
+      <c r="C21" s="104"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="100"/>
-      <c r="B22" s="95"/>
-      <c r="C22" s="100"/>
+      <c r="A22" s="104"/>
+      <c r="B22" s="99"/>
+      <c r="C22" s="104"/>
     </row>
     <row r="23" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="100"/>
-      <c r="B23" s="95"/>
-      <c r="C23" s="100"/>
+      <c r="A23" s="104"/>
+      <c r="B23" s="99"/>
+      <c r="C23" s="104"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="100"/>
-      <c r="B24" s="95" t="s">
+      <c r="A24" s="104"/>
+      <c r="B24" s="99" t="s">
         <v>403</v>
       </c>
-      <c r="C24" s="100"/>
+      <c r="C24" s="104"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="100"/>
-      <c r="B25" s="95"/>
-      <c r="C25" s="100"/>
+      <c r="A25" s="104"/>
+      <c r="B25" s="99"/>
+      <c r="C25" s="104"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="100"/>
-      <c r="B26" s="95" t="s">
+      <c r="A26" s="104"/>
+      <c r="B26" s="99" t="s">
         <v>317</v>
       </c>
-      <c r="C26" s="100"/>
+      <c r="C26" s="104"/>
     </row>
     <row r="27" spans="1:3" ht="144" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="100"/>
-      <c r="B27" s="95"/>
-      <c r="C27" s="100"/>
+      <c r="A27" s="104"/>
+      <c r="B27" s="99"/>
+      <c r="C27" s="104"/>
     </row>
     <row r="28" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="100"/>
-      <c r="B28" s="95" t="s">
+      <c r="A28" s="104"/>
+      <c r="B28" s="99" t="s">
         <v>404</v>
       </c>
-      <c r="C28" s="100"/>
+      <c r="C28" s="104"/>
     </row>
     <row r="29" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="100"/>
-      <c r="B29" s="95"/>
-      <c r="C29" s="100"/>
+      <c r="A29" s="104"/>
+      <c r="B29" s="99"/>
+      <c r="C29" s="104"/>
     </row>
     <row r="30" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="100"/>
-      <c r="B30" s="95"/>
-      <c r="C30" s="100"/>
+      <c r="A30" s="104"/>
+      <c r="B30" s="99"/>
+      <c r="C30" s="104"/>
     </row>
     <row r="31" spans="1:3" ht="196" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="100"/>
-      <c r="B31" s="95"/>
-      <c r="C31" s="100"/>
+      <c r="A31" s="104"/>
+      <c r="B31" s="99"/>
+      <c r="C31" s="104"/>
     </row>
     <row r="32" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="100"/>
-      <c r="B32" s="95" t="s">
+      <c r="A32" s="104"/>
+      <c r="B32" s="99" t="s">
         <v>405</v>
       </c>
-      <c r="C32" s="100"/>
+      <c r="C32" s="104"/>
     </row>
     <row r="33" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="100"/>
-      <c r="B33" s="95"/>
-      <c r="C33" s="100"/>
+      <c r="A33" s="104"/>
+      <c r="B33" s="99"/>
+      <c r="C33" s="104"/>
     </row>
     <row r="34" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="100"/>
-      <c r="B34" s="95"/>
-      <c r="C34" s="100"/>
+      <c r="A34" s="104"/>
+      <c r="B34" s="99"/>
+      <c r="C34" s="104"/>
     </row>
     <row r="35" spans="1:3" ht="201" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="100"/>
-      <c r="B35" s="95"/>
-      <c r="C35" s="100"/>
+      <c r="A35" s="104"/>
+      <c r="B35" s="99"/>
+      <c r="C35" s="104"/>
     </row>
     <row r="36" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="100"/>
-      <c r="B36" s="95" t="s">
+      <c r="A36" s="104"/>
+      <c r="B36" s="99" t="s">
         <v>406</v>
       </c>
-      <c r="C36" s="100"/>
+      <c r="C36" s="104"/>
     </row>
     <row r="37" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="100"/>
-      <c r="B37" s="95"/>
-      <c r="C37" s="100"/>
+      <c r="A37" s="104"/>
+      <c r="B37" s="99"/>
+      <c r="C37" s="104"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="100"/>
-      <c r="B38" s="95"/>
-      <c r="C38" s="100"/>
+      <c r="A38" s="104"/>
+      <c r="B38" s="99"/>
+      <c r="C38" s="104"/>
     </row>
     <row r="39" spans="1:3" ht="239" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="100"/>
-      <c r="B39" s="95"/>
-      <c r="C39" s="100"/>
+      <c r="A39" s="104"/>
+      <c r="B39" s="99"/>
+      <c r="C39" s="104"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="100"/>
-      <c r="B40" s="95" t="s">
+      <c r="A40" s="104"/>
+      <c r="B40" s="99" t="s">
         <v>407</v>
       </c>
-      <c r="C40" s="100"/>
+      <c r="C40" s="104"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="90"/>
-      <c r="B41" s="96"/>
-      <c r="C41" s="90"/>
+      <c r="A41" s="94"/>
+      <c r="B41" s="100"/>
+      <c r="C41" s="94"/>
     </row>
     <row r="42" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A42" s="60" t="s">
@@ -24117,11 +25038,11 @@
       <c r="C46" s="60"/>
     </row>
     <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A47" s="93" t="s">
+      <c r="A47" s="97" t="s">
         <v>386</v>
       </c>
-      <c r="B47" s="93"/>
-      <c r="C47" s="93"/>
+      <c r="B47" s="97"/>
+      <c r="C47" s="97"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
@@ -24135,25 +25056,25 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="89" t="s">
+      <c r="A49" s="93" t="s">
         <v>388</v>
       </c>
-      <c r="B49" s="91" t="s">
+      <c r="B49" s="95" t="s">
         <v>413</v>
       </c>
-      <c r="C49" s="89" t="s">
+      <c r="C49" s="93" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="100"/>
-      <c r="B50" s="110"/>
-      <c r="C50" s="100"/>
+      <c r="A50" s="104"/>
+      <c r="B50" s="114"/>
+      <c r="C50" s="104"/>
     </row>
     <row r="51" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="90"/>
-      <c r="B51" s="92"/>
-      <c r="C51" s="90"/>
+      <c r="A51" s="94"/>
+      <c r="B51" s="96"/>
+      <c r="C51" s="94"/>
     </row>
     <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="54" t="s">
@@ -24167,91 +25088,91 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="89" t="s">
+      <c r="A53" s="93" t="s">
         <v>415</v>
       </c>
-      <c r="B53" s="109" t="s">
+      <c r="B53" s="113" t="s">
         <v>416</v>
       </c>
-      <c r="C53" s="89" t="s">
+      <c r="C53" s="93" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="238" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="100"/>
-      <c r="B54" s="109"/>
-      <c r="C54" s="100"/>
+      <c r="A54" s="104"/>
+      <c r="B54" s="113"/>
+      <c r="C54" s="104"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="100"/>
-      <c r="B55" s="91" t="s">
+      <c r="A55" s="104"/>
+      <c r="B55" s="95" t="s">
         <v>417</v>
       </c>
-      <c r="C55" s="100"/>
+      <c r="C55" s="104"/>
     </row>
     <row r="56" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="100"/>
-      <c r="B56" s="110"/>
-      <c r="C56" s="100"/>
+      <c r="A56" s="104"/>
+      <c r="B56" s="114"/>
+      <c r="C56" s="104"/>
     </row>
     <row r="57" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="100"/>
-      <c r="B57" s="110"/>
-      <c r="C57" s="100"/>
+      <c r="A57" s="104"/>
+      <c r="B57" s="114"/>
+      <c r="C57" s="104"/>
     </row>
     <row r="58" spans="1:3" ht="172" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="100"/>
-      <c r="B58" s="92"/>
-      <c r="C58" s="100"/>
+      <c r="A58" s="104"/>
+      <c r="B58" s="96"/>
+      <c r="C58" s="104"/>
     </row>
     <row r="59" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="100"/>
-      <c r="B59" s="91" t="s">
+      <c r="A59" s="104"/>
+      <c r="B59" s="95" t="s">
         <v>418</v>
       </c>
-      <c r="C59" s="100"/>
+      <c r="C59" s="104"/>
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="100"/>
-      <c r="B60" s="110"/>
-      <c r="C60" s="100"/>
+      <c r="A60" s="104"/>
+      <c r="B60" s="114"/>
+      <c r="C60" s="104"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="100"/>
-      <c r="B61" s="110"/>
-      <c r="C61" s="100"/>
+      <c r="A61" s="104"/>
+      <c r="B61" s="114"/>
+      <c r="C61" s="104"/>
     </row>
     <row r="62" spans="1:3" ht="125" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="100"/>
-      <c r="B62" s="92"/>
-      <c r="C62" s="100"/>
+      <c r="A62" s="104"/>
+      <c r="B62" s="96"/>
+      <c r="C62" s="104"/>
     </row>
     <row r="63" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="100"/>
-      <c r="B63" s="91" t="s">
+      <c r="A63" s="104"/>
+      <c r="B63" s="95" t="s">
         <v>419</v>
       </c>
-      <c r="C63" s="100"/>
+      <c r="C63" s="104"/>
     </row>
     <row r="64" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="100"/>
-      <c r="B64" s="110"/>
-      <c r="C64" s="100"/>
+      <c r="A64" s="104"/>
+      <c r="B64" s="114"/>
+      <c r="C64" s="104"/>
     </row>
     <row r="65" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="100"/>
-      <c r="B65" s="110"/>
-      <c r="C65" s="100"/>
+      <c r="A65" s="104"/>
+      <c r="B65" s="114"/>
+      <c r="C65" s="104"/>
     </row>
     <row r="66" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="100"/>
-      <c r="B66" s="110"/>
-      <c r="C66" s="100"/>
+      <c r="A66" s="104"/>
+      <c r="B66" s="114"/>
+      <c r="C66" s="104"/>
     </row>
     <row r="67" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="90"/>
-      <c r="B67" s="92"/>
-      <c r="C67" s="90"/>
+      <c r="A67" s="94"/>
+      <c r="B67" s="96"/>
+      <c r="C67" s="94"/>
     </row>
     <row r="68" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A68" s="60" t="s">

</xml_diff>

<commit_message>
Prevent lock-selection-survey from direct load and wired the Previous button on the lock card.
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9CD71D2-D9F6-5244-ADDC-D9890C3D05CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F48BCBC-D0F6-DB48-B058-4878A567A3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16160" firstSheet="8" activeTab="16" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16160" firstSheet="8" activeTab="17" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="SPEC - 1.1" sheetId="1" r:id="rId1"/>
@@ -30,9 +30,10 @@
     <sheet name="SPEC - 3.0" sheetId="19" r:id="rId15"/>
     <sheet name="SPEC - 3.1" sheetId="20" r:id="rId16"/>
     <sheet name="SPEC - 3.2" sheetId="21" r:id="rId17"/>
-    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId18"/>
-    <sheet name="PLAYGROUND" sheetId="6" r:id="rId19"/>
-    <sheet name="TEMPLATE" sheetId="8" r:id="rId20"/>
+    <sheet name="SPEC - 3.3" sheetId="22" r:id="rId18"/>
+    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId19"/>
+    <sheet name="PLAYGROUND" sheetId="6" r:id="rId20"/>
+    <sheet name="TEMPLATE" sheetId="8" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="917" uniqueCount="696">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -18166,6 +18167,502 @@
         modified:   html/index.html
         modified:   js/controller/index.js</t>
     </r>
+  </si>
+  <si>
+    <t>/*****************************************************************************/
+/* WINDOWS ONLOAD                                                            */
+/*****************************************************************************/
+/* Anonymous function fired on window load. 
+ * @param    
+ * @return   
+ * */
+window.onload = function(event) {
+    let page = sessionStorage.getItem("page");
+    if (page !== null) {
+        // Coming from home page
+        if (page === "1") {
+            // Initialize the lock selection card controls
+            initializeLockCardControls();
+        }
+        // Scroll to the top
+        window.scrollTo(0, 0);
+    } else {
+        // Redirect to the index page
+        window.location.replace("./../html/index.html");
+    }
+};</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>window.onload()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">js/controller/global.js </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>to prevent survey page from being loaded without going through the index page.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>window.onload()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">js/controller/global.js </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>to prevent survey page from being loaded without going through the index page.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the Lock and Door Details Footer card to have a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Previous </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">button in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html/lock-selection-survey.html</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the Lock and Door Details Footer card to have a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">Previous </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">button in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html/lock-selection-survey.html</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;!-- Card Footer --&gt;
+            &lt;div class="card-footer text-center"&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">              &lt;input id="lock-selection-previous" class="btn btn-primary"
+                type="submit" value="    Previous    "&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">              &lt;input id="lock-selection-next" class="btn btn-success"
+                type="submit" value="      Next      "&gt;
+            &lt;/div&gt;
+            &lt;!-- End Card Footer --&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">// Reference to the Previous and Next button
+let lockCardPreviousButton = document.getElementById("lock-selection-previous");
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>let lockCardNextButton = document.getElementById("lock-selection-next");</t>
+    </r>
+  </si>
+  <si>
+    <t>/* The callback function fired on 'click' - for lock card previous button
+ * control. 
+ * @param    
+ * @return   
+ * */
+const lockCardPreviousButtonClick = (event) =&gt; {
+    // Redirect to the index page
+    window.location.replace("../html/index.html");
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add a reference to the previous button in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Lock and Door Details - Footer card</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> js/controller/lock-selection-survey-lock-card.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Added a reference to the previous button in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Lock and Door Details - Footer card</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> js/controller/lock-selection-survey-lock-card.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implement the callback function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lockCardPreviousButtonClick()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> js/controller/lock-selection-survey-lock-card.js</t>
+    </r>
+  </si>
+  <si>
+    <t>lockCardPreviousButton.addEventListener("click", lockCardPreviousButtonClick);
+lockCardNextButton.addEventListener("click", lockCardNextButtonClick);
+/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Register the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lockCardPreviousButtonClick()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> callback function to be called when the lock card </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Previous</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> button is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>clicked</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Registered the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lockCardPreviousButtonClick()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> callback function to be called when the lock card </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>Previous</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> button is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>clicked</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implemented the callback function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lockCardPreviousButtonClick()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> js/controller/lock-selection-survey-lock-card.js</t>
+    </r>
+  </si>
+  <si>
+    <t>PREVENT LOCK AND DOOR HTML FROM LOADING DIRECTLY WITHOUT ACCESSING THE index.html PAGE AND PROGRAM THE PREVIOUS BUTTON FOR THE LOCK CARD</t>
+  </si>
+  <si>
+    <t>git commit -m "Prevent lock-selection-survey from direct load and wired the Previous button on the lock card."</t>
   </si>
 </sst>
 </file>
@@ -18591,7 +19088,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -18815,6 +19312,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -18881,12 +19396,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -18894,6 +19403,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -18920,22 +19435,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -19266,18 +19775,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -19562,18 +20071,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="103" t="s">
         <v>426</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -19587,7 +20096,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="118" t="s">
+      <c r="A4" s="124" t="s">
         <v>438</v>
       </c>
       <c r="B4" s="48" t="s">
@@ -19598,7 +20107,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="119"/>
+      <c r="A5" s="125"/>
       <c r="B5" s="48" t="s">
         <v>441</v>
       </c>
@@ -19607,51 +20116,51 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="119"/>
+      <c r="A6" s="125"/>
       <c r="B6" s="48" t="s">
         <v>434</v>
       </c>
-      <c r="C6" s="121" t="s">
+      <c r="C6" s="127" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="119"/>
+      <c r="A7" s="125"/>
       <c r="B7" s="48" t="s">
         <v>435</v>
       </c>
-      <c r="C7" s="122"/>
+      <c r="C7" s="128"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="119"/>
+      <c r="A8" s="125"/>
       <c r="B8" s="48" t="s">
         <v>427</v>
       </c>
-      <c r="C8" s="122"/>
+      <c r="C8" s="128"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="119"/>
+      <c r="A9" s="125"/>
       <c r="B9" s="48" t="s">
         <v>428</v>
       </c>
-      <c r="C9" s="122"/>
+      <c r="C9" s="128"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="119"/>
+      <c r="A10" s="125"/>
       <c r="B10" s="48" t="s">
         <v>436</v>
       </c>
-      <c r="C10" s="122"/>
+      <c r="C10" s="128"/>
     </row>
     <row r="11" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="119"/>
+      <c r="A11" s="125"/>
       <c r="B11" s="48" t="s">
         <v>443</v>
       </c>
-      <c r="C11" s="123"/>
+      <c r="C11" s="129"/>
     </row>
     <row r="12" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="120"/>
+      <c r="A12" s="126"/>
       <c r="B12" s="48" t="s">
         <v>445</v>
       </c>
@@ -19790,18 +20299,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="103" t="s">
         <v>464</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -19907,18 +20416,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="103" t="s">
         <v>478</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -19969,11 +20478,11 @@
       <c r="C8" s="54"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="97" t="s">
+      <c r="A9" s="103" t="s">
         <v>485</v>
       </c>
-      <c r="B9" s="97"/>
-      <c r="C9" s="97"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="103"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -20009,20 +20518,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="99" t="s">
         <v>490</v>
       </c>
-      <c r="B13" s="98" t="s">
+      <c r="B13" s="104" t="s">
         <v>489</v>
       </c>
-      <c r="C13" s="93" t="s">
+      <c r="C13" s="99" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="94"/>
-      <c r="B14" s="100"/>
-      <c r="C14" s="94"/>
+      <c r="A14" s="100"/>
+      <c r="B14" s="106"/>
+      <c r="C14" s="100"/>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="73" t="s">
@@ -20047,20 +20556,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="93" t="s">
+      <c r="A17" s="99" t="s">
         <v>499</v>
       </c>
-      <c r="B17" s="98" t="s">
+      <c r="B17" s="104" t="s">
         <v>498</v>
       </c>
-      <c r="C17" s="93" t="s">
+      <c r="C17" s="99" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="222" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="94"/>
-      <c r="B18" s="100"/>
-      <c r="C18" s="94"/>
+      <c r="A18" s="100"/>
+      <c r="B18" s="106"/>
+      <c r="C18" s="100"/>
     </row>
     <row r="19" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -20118,18 +20627,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="103" t="s">
         <v>505</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -20187,25 +20696,25 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="99" t="s">
         <v>517</v>
       </c>
-      <c r="B8" s="98" t="s">
+      <c r="B8" s="104" t="s">
         <v>516</v>
       </c>
-      <c r="C8" s="93" t="s">
+      <c r="C8" s="99" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="104"/>
-      <c r="B9" s="99"/>
-      <c r="C9" s="104"/>
+      <c r="A9" s="110"/>
+      <c r="B9" s="105"/>
+      <c r="C9" s="110"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="94"/>
-      <c r="B10" s="100"/>
-      <c r="C10" s="94"/>
+      <c r="A10" s="100"/>
+      <c r="B10" s="106"/>
+      <c r="C10" s="100"/>
     </row>
     <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="54" t="s">
@@ -20219,86 +20728,86 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="93" t="s">
+      <c r="A12" s="99" t="s">
         <v>526</v>
       </c>
-      <c r="B12" s="98" t="s">
+      <c r="B12" s="104" t="s">
         <v>527</v>
       </c>
-      <c r="C12" s="93" t="s">
+      <c r="C12" s="99" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="104"/>
-      <c r="B13" s="99"/>
-      <c r="C13" s="104"/>
+      <c r="A13" s="110"/>
+      <c r="B13" s="105"/>
+      <c r="C13" s="110"/>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="104"/>
-      <c r="B14" s="99"/>
-      <c r="C14" s="104"/>
+      <c r="A14" s="110"/>
+      <c r="B14" s="105"/>
+      <c r="C14" s="110"/>
     </row>
     <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="104"/>
-      <c r="B15" s="99"/>
-      <c r="C15" s="104"/>
+      <c r="A15" s="110"/>
+      <c r="B15" s="105"/>
+      <c r="C15" s="110"/>
     </row>
     <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="104"/>
-      <c r="B16" s="99"/>
-      <c r="C16" s="104"/>
+      <c r="A16" s="110"/>
+      <c r="B16" s="105"/>
+      <c r="C16" s="110"/>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="104"/>
-      <c r="B17" s="99"/>
-      <c r="C17" s="104"/>
+      <c r="A17" s="110"/>
+      <c r="B17" s="105"/>
+      <c r="C17" s="110"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="94"/>
-      <c r="B18" s="99"/>
-      <c r="C18" s="94"/>
+      <c r="A18" s="100"/>
+      <c r="B18" s="105"/>
+      <c r="C18" s="100"/>
     </row>
     <row r="19" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="93" t="s">
+      <c r="A19" s="99" t="s">
         <v>529</v>
       </c>
-      <c r="B19" s="98" t="s">
+      <c r="B19" s="104" t="s">
         <v>528</v>
       </c>
-      <c r="C19" s="93" t="s">
+      <c r="C19" s="99" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="104"/>
-      <c r="B20" s="99"/>
-      <c r="C20" s="104"/>
+      <c r="A20" s="110"/>
+      <c r="B20" s="105"/>
+      <c r="C20" s="110"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="104"/>
-      <c r="B21" s="99"/>
-      <c r="C21" s="104"/>
+      <c r="A21" s="110"/>
+      <c r="B21" s="105"/>
+      <c r="C21" s="110"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="104"/>
-      <c r="B22" s="99"/>
-      <c r="C22" s="104"/>
+      <c r="A22" s="110"/>
+      <c r="B22" s="105"/>
+      <c r="C22" s="110"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="104"/>
-      <c r="B23" s="99"/>
-      <c r="C23" s="104"/>
+      <c r="A23" s="110"/>
+      <c r="B23" s="105"/>
+      <c r="C23" s="110"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="104"/>
-      <c r="B24" s="99"/>
-      <c r="C24" s="104"/>
+      <c r="A24" s="110"/>
+      <c r="B24" s="105"/>
+      <c r="C24" s="110"/>
     </row>
     <row r="25" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="94"/>
-      <c r="B25" s="100"/>
-      <c r="C25" s="94"/>
+      <c r="A25" s="100"/>
+      <c r="B25" s="106"/>
+      <c r="C25" s="100"/>
     </row>
     <row r="26" spans="1:3" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
@@ -20312,51 +20821,51 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="93" t="s">
+      <c r="A27" s="99" t="s">
         <v>533</v>
       </c>
-      <c r="B27" s="98" t="s">
+      <c r="B27" s="104" t="s">
         <v>532</v>
       </c>
-      <c r="C27" s="93" t="s">
+      <c r="C27" s="99" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="104"/>
-      <c r="B28" s="99"/>
-      <c r="C28" s="104"/>
+      <c r="A28" s="110"/>
+      <c r="B28" s="105"/>
+      <c r="C28" s="110"/>
     </row>
     <row r="29" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="94"/>
-      <c r="B29" s="100"/>
-      <c r="C29" s="94"/>
+      <c r="A29" s="100"/>
+      <c r="B29" s="106"/>
+      <c r="C29" s="100"/>
     </row>
     <row r="30" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="93" t="s">
+      <c r="A30" s="99" t="s">
         <v>536</v>
       </c>
-      <c r="B30" s="98" t="s">
+      <c r="B30" s="104" t="s">
         <v>535</v>
       </c>
-      <c r="C30" s="93" t="s">
+      <c r="C30" s="99" t="s">
         <v>537</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="104"/>
-      <c r="B31" s="99"/>
-      <c r="C31" s="104"/>
+      <c r="A31" s="110"/>
+      <c r="B31" s="105"/>
+      <c r="C31" s="110"/>
     </row>
     <row r="32" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="104"/>
-      <c r="B32" s="99"/>
-      <c r="C32" s="104"/>
+      <c r="A32" s="110"/>
+      <c r="B32" s="105"/>
+      <c r="C32" s="110"/>
     </row>
     <row r="33" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="94"/>
-      <c r="B33" s="100"/>
-      <c r="C33" s="94"/>
+      <c r="A33" s="100"/>
+      <c r="B33" s="106"/>
+      <c r="C33" s="100"/>
     </row>
     <row r="34" spans="1:3" ht="255" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
@@ -20383,14 +20892,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="17">
-    <mergeCell ref="B12:B18"/>
-    <mergeCell ref="A12:A18"/>
-    <mergeCell ref="C12:C18"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="C8:C10"/>
     <mergeCell ref="B30:B33"/>
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="C30:C33"/>
@@ -20400,6 +20901,14 @@
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="C27:C29"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="A12:A18"/>
+    <mergeCell ref="C12:C18"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -20422,18 +20931,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="103" t="s">
         <v>549</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -20528,18 +21037,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="103" t="s">
         <v>560</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -20601,11 +21110,11 @@
       <c r="C9" s="54"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="97" t="s">
+      <c r="A10" s="103" t="s">
         <v>575</v>
       </c>
-      <c r="B10" s="97"/>
-      <c r="C10" s="97"/>
+      <c r="B10" s="103"/>
+      <c r="C10" s="103"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
@@ -20721,18 +21230,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="103" t="s">
         <v>661</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -20790,20 +21299,20 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="99" t="s">
         <v>587</v>
       </c>
-      <c r="B8" s="98" t="s">
+      <c r="B8" s="104" t="s">
         <v>590</v>
       </c>
-      <c r="C8" s="93" t="s">
+      <c r="C8" s="99" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="109" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="94"/>
-      <c r="B9" s="100"/>
-      <c r="C9" s="94"/>
+      <c r="A9" s="100"/>
+      <c r="B9" s="106"/>
+      <c r="C9" s="100"/>
     </row>
     <row r="10" spans="1:3" ht="109" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="82" t="s">
@@ -20839,20 +21348,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="99" t="s">
         <v>603</v>
       </c>
-      <c r="B13" s="98" t="s">
+      <c r="B13" s="104" t="s">
         <v>602</v>
       </c>
-      <c r="C13" s="93" t="s">
+      <c r="C13" s="99" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="94"/>
-      <c r="B14" s="100"/>
-      <c r="C14" s="94"/>
+      <c r="A14" s="100"/>
+      <c r="B14" s="106"/>
+      <c r="C14" s="100"/>
     </row>
     <row r="15" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="82" t="s">
@@ -20866,67 +21375,67 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="125" t="s">
+      <c r="A16" s="131" t="s">
         <v>609</v>
       </c>
-      <c r="B16" s="124" t="s">
+      <c r="B16" s="130" t="s">
         <v>608</v>
       </c>
-      <c r="C16" s="125" t="s">
+      <c r="C16" s="131" t="s">
         <v>610</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="125"/>
-      <c r="B17" s="124"/>
-      <c r="C17" s="125"/>
+      <c r="A17" s="131"/>
+      <c r="B17" s="130"/>
+      <c r="C17" s="131"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="125"/>
-      <c r="B18" s="124"/>
-      <c r="C18" s="125"/>
+      <c r="A18" s="131"/>
+      <c r="B18" s="130"/>
+      <c r="C18" s="131"/>
     </row>
     <row r="19" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="125"/>
-      <c r="B19" s="124"/>
-      <c r="C19" s="125"/>
+      <c r="A19" s="131"/>
+      <c r="B19" s="130"/>
+      <c r="C19" s="131"/>
     </row>
     <row r="20" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="125"/>
-      <c r="B20" s="124"/>
-      <c r="C20" s="125"/>
+      <c r="A20" s="131"/>
+      <c r="B20" s="130"/>
+      <c r="C20" s="131"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="125"/>
-      <c r="B21" s="124"/>
-      <c r="C21" s="125"/>
+      <c r="A21" s="131"/>
+      <c r="B21" s="130"/>
+      <c r="C21" s="131"/>
     </row>
     <row r="22" spans="1:3" ht="139" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="125"/>
-      <c r="B22" s="124"/>
-      <c r="C22" s="125"/>
+      <c r="A22" s="131"/>
+      <c r="B22" s="130"/>
+      <c r="C22" s="131"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="125"/>
-      <c r="B23" s="124" t="s">
+      <c r="A23" s="131"/>
+      <c r="B23" s="130" t="s">
         <v>611</v>
       </c>
-      <c r="C23" s="125"/>
+      <c r="C23" s="131"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="125"/>
-      <c r="B24" s="124"/>
-      <c r="C24" s="125"/>
+      <c r="A24" s="131"/>
+      <c r="B24" s="130"/>
+      <c r="C24" s="131"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="125"/>
-      <c r="B25" s="124"/>
-      <c r="C25" s="125"/>
+      <c r="A25" s="131"/>
+      <c r="B25" s="130"/>
+      <c r="C25" s="131"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="125"/>
-      <c r="B26" s="124"/>
-      <c r="C26" s="125"/>
+      <c r="A26" s="131"/>
+      <c r="B26" s="130"/>
+      <c r="C26" s="131"/>
     </row>
     <row r="27" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="85" t="s">
@@ -20995,185 +21504,185 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="93" t="s">
+      <c r="A33" s="99" t="s">
         <v>633</v>
       </c>
-      <c r="B33" s="95" t="s">
+      <c r="B33" s="101" t="s">
         <v>627</v>
       </c>
-      <c r="C33" s="93" t="s">
+      <c r="C33" s="99" t="s">
         <v>633</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="104"/>
-      <c r="B34" s="114"/>
-      <c r="C34" s="104"/>
+      <c r="A34" s="110"/>
+      <c r="B34" s="122"/>
+      <c r="C34" s="110"/>
     </row>
     <row r="35" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="104"/>
-      <c r="B35" s="114"/>
-      <c r="C35" s="104"/>
+      <c r="A35" s="110"/>
+      <c r="B35" s="122"/>
+      <c r="C35" s="110"/>
     </row>
     <row r="36" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="104"/>
-      <c r="B36" s="96"/>
-      <c r="C36" s="104"/>
+      <c r="A36" s="110"/>
+      <c r="B36" s="102"/>
+      <c r="C36" s="110"/>
     </row>
     <row r="37" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="104"/>
-      <c r="B37" s="95" t="s">
+      <c r="A37" s="110"/>
+      <c r="B37" s="101" t="s">
         <v>628</v>
       </c>
-      <c r="C37" s="104"/>
+      <c r="C37" s="110"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="104"/>
-      <c r="B38" s="114"/>
-      <c r="C38" s="104"/>
+      <c r="A38" s="110"/>
+      <c r="B38" s="122"/>
+      <c r="C38" s="110"/>
     </row>
     <row r="39" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="104"/>
-      <c r="B39" s="114"/>
-      <c r="C39" s="104"/>
+      <c r="A39" s="110"/>
+      <c r="B39" s="122"/>
+      <c r="C39" s="110"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="104"/>
-      <c r="B40" s="114"/>
-      <c r="C40" s="104"/>
+      <c r="A40" s="110"/>
+      <c r="B40" s="122"/>
+      <c r="C40" s="110"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="104"/>
-      <c r="B41" s="114"/>
-      <c r="C41" s="104"/>
+      <c r="A41" s="110"/>
+      <c r="B41" s="122"/>
+      <c r="C41" s="110"/>
     </row>
     <row r="42" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="104"/>
-      <c r="B42" s="114"/>
-      <c r="C42" s="104"/>
+      <c r="A42" s="110"/>
+      <c r="B42" s="122"/>
+      <c r="C42" s="110"/>
     </row>
     <row r="43" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="104"/>
-      <c r="B43" s="95" t="s">
+      <c r="A43" s="110"/>
+      <c r="B43" s="101" t="s">
         <v>629</v>
       </c>
-      <c r="C43" s="104"/>
+      <c r="C43" s="110"/>
     </row>
     <row r="44" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="104"/>
-      <c r="B44" s="114"/>
-      <c r="C44" s="104"/>
+      <c r="A44" s="110"/>
+      <c r="B44" s="122"/>
+      <c r="C44" s="110"/>
     </row>
     <row r="45" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="104"/>
-      <c r="B45" s="114"/>
-      <c r="C45" s="104"/>
+      <c r="A45" s="110"/>
+      <c r="B45" s="122"/>
+      <c r="C45" s="110"/>
     </row>
     <row r="46" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="104"/>
-      <c r="B46" s="114"/>
-      <c r="C46" s="104"/>
+      <c r="A46" s="110"/>
+      <c r="B46" s="122"/>
+      <c r="C46" s="110"/>
     </row>
     <row r="47" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="104"/>
-      <c r="B47" s="114"/>
-      <c r="C47" s="104"/>
+      <c r="A47" s="110"/>
+      <c r="B47" s="122"/>
+      <c r="C47" s="110"/>
     </row>
     <row r="48" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="104"/>
-      <c r="B48" s="114"/>
-      <c r="C48" s="104"/>
+      <c r="A48" s="110"/>
+      <c r="B48" s="122"/>
+      <c r="C48" s="110"/>
     </row>
     <row r="49" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="104"/>
-      <c r="B49" s="114"/>
-      <c r="C49" s="104"/>
+      <c r="A49" s="110"/>
+      <c r="B49" s="122"/>
+      <c r="C49" s="110"/>
     </row>
     <row r="50" spans="1:3" ht="320" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="104"/>
-      <c r="B50" s="96"/>
-      <c r="C50" s="104"/>
+      <c r="A50" s="110"/>
+      <c r="B50" s="102"/>
+      <c r="C50" s="110"/>
     </row>
     <row r="51" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="104"/>
-      <c r="B51" s="95" t="s">
+      <c r="A51" s="110"/>
+      <c r="B51" s="101" t="s">
         <v>630</v>
       </c>
-      <c r="C51" s="104"/>
+      <c r="C51" s="110"/>
     </row>
     <row r="52" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="104"/>
-      <c r="B52" s="114"/>
-      <c r="C52" s="104"/>
+      <c r="A52" s="110"/>
+      <c r="B52" s="122"/>
+      <c r="C52" s="110"/>
     </row>
     <row r="53" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="104"/>
-      <c r="B53" s="114"/>
-      <c r="C53" s="104"/>
+      <c r="A53" s="110"/>
+      <c r="B53" s="122"/>
+      <c r="C53" s="110"/>
     </row>
     <row r="54" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="104"/>
-      <c r="B54" s="114"/>
-      <c r="C54" s="104"/>
+      <c r="A54" s="110"/>
+      <c r="B54" s="122"/>
+      <c r="C54" s="110"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="104"/>
-      <c r="B55" s="114"/>
-      <c r="C55" s="104"/>
+      <c r="A55" s="110"/>
+      <c r="B55" s="122"/>
+      <c r="C55" s="110"/>
     </row>
     <row r="56" spans="1:3" ht="97" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="104"/>
-      <c r="B56" s="96"/>
-      <c r="C56" s="104"/>
+      <c r="A56" s="110"/>
+      <c r="B56" s="102"/>
+      <c r="C56" s="110"/>
     </row>
     <row r="57" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="104"/>
-      <c r="B57" s="95" t="s">
+      <c r="A57" s="110"/>
+      <c r="B57" s="101" t="s">
         <v>631</v>
       </c>
-      <c r="C57" s="104"/>
+      <c r="C57" s="110"/>
     </row>
     <row r="58" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="104"/>
-      <c r="B58" s="114"/>
-      <c r="C58" s="104"/>
+      <c r="A58" s="110"/>
+      <c r="B58" s="122"/>
+      <c r="C58" s="110"/>
     </row>
     <row r="59" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="104"/>
-      <c r="B59" s="114"/>
-      <c r="C59" s="104"/>
+      <c r="A59" s="110"/>
+      <c r="B59" s="122"/>
+      <c r="C59" s="110"/>
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="104"/>
-      <c r="B60" s="114"/>
-      <c r="C60" s="104"/>
+      <c r="A60" s="110"/>
+      <c r="B60" s="122"/>
+      <c r="C60" s="110"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="104"/>
-      <c r="B61" s="114"/>
-      <c r="C61" s="104"/>
+      <c r="A61" s="110"/>
+      <c r="B61" s="122"/>
+      <c r="C61" s="110"/>
     </row>
     <row r="62" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="104"/>
-      <c r="B62" s="114"/>
-      <c r="C62" s="104"/>
+      <c r="A62" s="110"/>
+      <c r="B62" s="122"/>
+      <c r="C62" s="110"/>
     </row>
     <row r="63" spans="1:3" ht="146" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="104"/>
-      <c r="B63" s="96"/>
-      <c r="C63" s="104"/>
+      <c r="A63" s="110"/>
+      <c r="B63" s="102"/>
+      <c r="C63" s="110"/>
     </row>
     <row r="64" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="104"/>
-      <c r="B64" s="95" t="s">
+      <c r="A64" s="110"/>
+      <c r="B64" s="101" t="s">
         <v>632</v>
       </c>
-      <c r="C64" s="104"/>
+      <c r="C64" s="110"/>
     </row>
     <row r="65" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="94"/>
-      <c r="B65" s="96"/>
-      <c r="C65" s="94"/>
+      <c r="A65" s="100"/>
+      <c r="B65" s="102"/>
+      <c r="C65" s="100"/>
     </row>
     <row r="66" spans="1:3" ht="397" x14ac:dyDescent="0.2">
       <c r="A66" s="85" t="s">
@@ -21187,93 +21696,93 @@
       </c>
     </row>
     <row r="67" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="105" t="s">
+      <c r="A67" s="111" t="s">
         <v>638</v>
       </c>
-      <c r="B67" s="113" t="s">
+      <c r="B67" s="123" t="s">
         <v>637</v>
       </c>
-      <c r="C67" s="105" t="s">
+      <c r="C67" s="111" t="s">
         <v>639</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="105"/>
-      <c r="B68" s="113"/>
-      <c r="C68" s="105"/>
+      <c r="A68" s="111"/>
+      <c r="B68" s="123"/>
+      <c r="C68" s="111"/>
     </row>
     <row r="69" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="105"/>
-      <c r="B69" s="113"/>
-      <c r="C69" s="105"/>
+      <c r="A69" s="111"/>
+      <c r="B69" s="123"/>
+      <c r="C69" s="111"/>
     </row>
     <row r="70" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="105" t="s">
+      <c r="A70" s="111" t="s">
         <v>643</v>
       </c>
-      <c r="B70" s="113" t="s">
+      <c r="B70" s="123" t="s">
         <v>640</v>
       </c>
-      <c r="C70" s="105" t="s">
+      <c r="C70" s="111" t="s">
         <v>642</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="105"/>
-      <c r="B71" s="113"/>
-      <c r="C71" s="105"/>
+      <c r="A71" s="111"/>
+      <c r="B71" s="123"/>
+      <c r="C71" s="111"/>
     </row>
     <row r="72" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="105"/>
-      <c r="B72" s="113"/>
-      <c r="C72" s="105"/>
+      <c r="A72" s="111"/>
+      <c r="B72" s="123"/>
+      <c r="C72" s="111"/>
     </row>
     <row r="73" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="105"/>
-      <c r="B73" s="113"/>
-      <c r="C73" s="105"/>
+      <c r="A73" s="111"/>
+      <c r="B73" s="123"/>
+      <c r="C73" s="111"/>
     </row>
     <row r="74" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="105"/>
-      <c r="B74" s="113"/>
-      <c r="C74" s="105"/>
+      <c r="A74" s="111"/>
+      <c r="B74" s="123"/>
+      <c r="C74" s="111"/>
     </row>
     <row r="75" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="105"/>
-      <c r="B75" s="113"/>
-      <c r="C75" s="105"/>
+      <c r="A75" s="111"/>
+      <c r="B75" s="123"/>
+      <c r="C75" s="111"/>
     </row>
     <row r="76" spans="1:3" ht="214" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="105"/>
-      <c r="B76" s="113"/>
-      <c r="C76" s="105"/>
+      <c r="A76" s="111"/>
+      <c r="B76" s="123"/>
+      <c r="C76" s="111"/>
     </row>
     <row r="77" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="105"/>
-      <c r="B77" s="113" t="s">
+      <c r="A77" s="111"/>
+      <c r="B77" s="123" t="s">
         <v>641</v>
       </c>
-      <c r="C77" s="105"/>
+      <c r="C77" s="111"/>
     </row>
     <row r="78" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="105"/>
-      <c r="B78" s="113"/>
-      <c r="C78" s="105"/>
+      <c r="A78" s="111"/>
+      <c r="B78" s="123"/>
+      <c r="C78" s="111"/>
     </row>
     <row r="79" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="105"/>
-      <c r="B79" s="113"/>
-      <c r="C79" s="105"/>
+      <c r="A79" s="111"/>
+      <c r="B79" s="123"/>
+      <c r="C79" s="111"/>
     </row>
     <row r="80" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="105"/>
-      <c r="B80" s="113"/>
-      <c r="C80" s="105"/>
+      <c r="A80" s="111"/>
+      <c r="B80" s="123"/>
+      <c r="C80" s="111"/>
     </row>
     <row r="81" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="105"/>
-      <c r="B81" s="113"/>
-      <c r="C81" s="105"/>
+      <c r="A81" s="111"/>
+      <c r="B81" s="123"/>
+      <c r="C81" s="111"/>
     </row>
     <row r="82" spans="1:3" ht="56" x14ac:dyDescent="0.2">
       <c r="A82" s="82" t="s">
@@ -21320,40 +21829,40 @@
       </c>
     </row>
     <row r="86" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="93" t="s">
+      <c r="A86" s="99" t="s">
         <v>657</v>
       </c>
-      <c r="B86" s="98" t="s">
+      <c r="B86" s="104" t="s">
         <v>656</v>
       </c>
-      <c r="C86" s="93" t="s">
+      <c r="C86" s="99" t="s">
         <v>658</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="104"/>
-      <c r="B87" s="99"/>
-      <c r="C87" s="104"/>
+      <c r="A87" s="110"/>
+      <c r="B87" s="105"/>
+      <c r="C87" s="110"/>
     </row>
     <row r="88" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="104"/>
-      <c r="B88" s="99"/>
-      <c r="C88" s="104"/>
+      <c r="A88" s="110"/>
+      <c r="B88" s="105"/>
+      <c r="C88" s="110"/>
     </row>
     <row r="89" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="104"/>
-      <c r="B89" s="99"/>
-      <c r="C89" s="104"/>
+      <c r="A89" s="110"/>
+      <c r="B89" s="105"/>
+      <c r="C89" s="110"/>
     </row>
     <row r="90" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="104"/>
-      <c r="B90" s="99"/>
-      <c r="C90" s="104"/>
+      <c r="A90" s="110"/>
+      <c r="B90" s="105"/>
+      <c r="C90" s="110"/>
     </row>
     <row r="91" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="94"/>
-      <c r="B91" s="100"/>
-      <c r="C91" s="94"/>
+      <c r="A91" s="100"/>
+      <c r="B91" s="106"/>
+      <c r="C91" s="100"/>
     </row>
     <row r="92" spans="1:3" ht="221" x14ac:dyDescent="0.2">
       <c r="A92" s="16" t="s">
@@ -21380,18 +21889,12 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="30">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="A16:A26"/>
-    <mergeCell ref="C16:C26"/>
+    <mergeCell ref="B77:B81"/>
+    <mergeCell ref="A70:A81"/>
+    <mergeCell ref="C70:C81"/>
+    <mergeCell ref="B86:B91"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="C86:C91"/>
     <mergeCell ref="B67:B69"/>
     <mergeCell ref="A67:A69"/>
     <mergeCell ref="C67:C69"/>
@@ -21404,12 +21907,18 @@
     <mergeCell ref="B33:B36"/>
     <mergeCell ref="B37:B42"/>
     <mergeCell ref="B43:B50"/>
-    <mergeCell ref="B77:B81"/>
-    <mergeCell ref="A70:A81"/>
-    <mergeCell ref="C70:C81"/>
-    <mergeCell ref="B86:B91"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="C86:C91"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="A16:A26"/>
+    <mergeCell ref="C16:C26"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="C8:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -21419,7 +21928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C21A766-C376-EB46-A7F6-E0E4ECA4E1CD}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -21432,18 +21941,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="103" t="s">
         <v>662</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -21490,40 +21999,40 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="93" t="s">
+      <c r="A7" s="99" t="s">
         <v>672</v>
       </c>
-      <c r="B7" s="98" t="s">
+      <c r="B7" s="104" t="s">
         <v>671</v>
       </c>
-      <c r="C7" s="93" t="s">
+      <c r="C7" s="99" t="s">
         <v>673</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="104"/>
-      <c r="B8" s="99"/>
-      <c r="C8" s="104"/>
+      <c r="A8" s="110"/>
+      <c r="B8" s="105"/>
+      <c r="C8" s="110"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="104"/>
-      <c r="B9" s="99"/>
-      <c r="C9" s="104"/>
+      <c r="A9" s="110"/>
+      <c r="B9" s="105"/>
+      <c r="C9" s="110"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="104"/>
-      <c r="B10" s="99"/>
-      <c r="C10" s="104"/>
+      <c r="A10" s="110"/>
+      <c r="B10" s="105"/>
+      <c r="C10" s="110"/>
     </row>
     <row r="11" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="104"/>
-      <c r="B11" s="99"/>
-      <c r="C11" s="104"/>
+      <c r="A11" s="110"/>
+      <c r="B11" s="105"/>
+      <c r="C11" s="110"/>
     </row>
     <row r="12" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="94"/>
-      <c r="B12" s="100"/>
-      <c r="C12" s="94"/>
+      <c r="A12" s="100"/>
+      <c r="B12" s="106"/>
+      <c r="C12" s="100"/>
     </row>
     <row r="13" spans="1:3" ht="210" x14ac:dyDescent="0.2">
       <c r="A13" s="87" t="s">
@@ -21548,13 +22057,13 @@
       </c>
     </row>
     <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="132" t="s">
+      <c r="A15" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="133" t="s">
+      <c r="B15" s="96" t="s">
         <v>677</v>
       </c>
-      <c r="C15" s="132" t="s">
+      <c r="C15" s="95" t="s">
         <v>559</v>
       </c>
     </row>
@@ -21572,6 +22081,133 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A22312-5578-CF4C-8666-672A40E7C4BD}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="97" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="103" t="s">
+        <v>694</v>
+      </c>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="397" x14ac:dyDescent="0.2">
+      <c r="A4" s="93" t="s">
+        <v>680</v>
+      </c>
+      <c r="B4" s="86" t="s">
+        <v>679</v>
+      </c>
+      <c r="C4" s="93" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="136" x14ac:dyDescent="0.2">
+      <c r="A5" s="93" t="s">
+        <v>682</v>
+      </c>
+      <c r="B5" s="58" t="s">
+        <v>684</v>
+      </c>
+      <c r="C5" s="93" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A6" s="94" t="s">
+        <v>687</v>
+      </c>
+      <c r="B6" s="55" t="s">
+        <v>685</v>
+      </c>
+      <c r="C6" s="94" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="154" x14ac:dyDescent="0.2">
+      <c r="A7" s="91" t="s">
+        <v>689</v>
+      </c>
+      <c r="B7" s="92" t="s">
+        <v>686</v>
+      </c>
+      <c r="C7" s="91" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="84" x14ac:dyDescent="0.2">
+      <c r="A8" s="91" t="s">
+        <v>691</v>
+      </c>
+      <c r="B8" s="92" t="s">
+        <v>690</v>
+      </c>
+      <c r="C8" s="91" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="95" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="96" t="s">
+        <v>695</v>
+      </c>
+      <c r="C10" s="95" t="s">
+        <v>559</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE113606-3FFA-8545-9BE3-5643B52A7CE9}">
   <dimension ref="A1:H116"/>
   <sheetViews>
@@ -21649,10 +22285,10 @@
       <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="129" t="s">
+      <c r="A6" s="132" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="129"/>
+      <c r="B6" s="132"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -22625,32 +23261,32 @@
       <c r="H73" s="23"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="126"/>
-      <c r="B74" s="130"/>
+      <c r="A74" s="133"/>
+      <c r="B74" s="134"/>
       <c r="C74" s="32" t="s">
         <v>225</v>
       </c>
       <c r="D74" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="E74" s="131"/>
-      <c r="F74" s="126"/>
-      <c r="G74" s="128"/>
-      <c r="H74" s="126"/>
+      <c r="E74" s="135"/>
+      <c r="F74" s="133"/>
+      <c r="G74" s="137"/>
+      <c r="H74" s="133"/>
     </row>
     <row r="75" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A75" s="126"/>
-      <c r="B75" s="130"/>
+      <c r="A75" s="133"/>
+      <c r="B75" s="134"/>
       <c r="C75" s="33" t="s">
         <v>226</v>
       </c>
       <c r="D75" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="E75" s="131"/>
-      <c r="F75" s="126"/>
-      <c r="G75" s="128"/>
-      <c r="H75" s="126"/>
+      <c r="E75" s="135"/>
+      <c r="F75" s="133"/>
+      <c r="G75" s="137"/>
+      <c r="H75" s="133"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="23"/>
@@ -22823,34 +23459,34 @@
       <c r="H88" s="23"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="126"/>
-      <c r="B89" s="126"/>
+      <c r="A89" s="133"/>
+      <c r="B89" s="133"/>
       <c r="C89" s="35" t="s">
         <v>225</v>
       </c>
       <c r="D89" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="E89" s="127" t="s">
+      <c r="E89" s="136" t="s">
         <v>121</v>
       </c>
-      <c r="F89" s="127"/>
-      <c r="G89" s="128"/>
-      <c r="H89" s="126"/>
+      <c r="F89" s="136"/>
+      <c r="G89" s="137"/>
+      <c r="H89" s="133"/>
     </row>
     <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A90" s="126"/>
-      <c r="B90" s="126"/>
+      <c r="A90" s="133"/>
+      <c r="B90" s="133"/>
       <c r="C90" s="35" t="s">
         <v>242</v>
       </c>
       <c r="D90" s="35" t="s">
         <v>243</v>
       </c>
-      <c r="E90" s="127"/>
-      <c r="F90" s="127"/>
-      <c r="G90" s="128"/>
-      <c r="H90" s="126"/>
+      <c r="E90" s="136"/>
+      <c r="F90" s="136"/>
+      <c r="G90" s="137"/>
+      <c r="H90" s="133"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="23"/>
@@ -23218,11 +23854,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F74:F75"/>
     <mergeCell ref="H74:H75"/>
     <mergeCell ref="A89:A90"/>
     <mergeCell ref="B89:B90"/>
@@ -23231,105 +23862,12 @@
     <mergeCell ref="G89:G90"/>
     <mergeCell ref="H89:H90"/>
     <mergeCell ref="G74:G75"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F74:F75"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
-  <dimension ref="A1:A16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="36" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="36" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="39" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="40" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="40" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="40" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="40" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="40" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="40" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="40" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="41" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="41" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="41" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
-        <v>288</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A16">
-    <sortCondition ref="A1:A16"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -23351,18 +23889,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="103" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -23413,11 +23951,11 @@
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="97" t="s">
+      <c r="A9" s="103" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="97"/>
-      <c r="C9" s="97"/>
+      <c r="B9" s="103"/>
+      <c r="C9" s="103"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -23453,20 +23991,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="99" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="95" t="s">
+      <c r="B13" s="101" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="93" t="s">
+      <c r="C13" s="99" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="94"/>
-      <c r="B14" s="96"/>
-      <c r="C14" s="94"/>
+      <c r="A14" s="100"/>
+      <c r="B14" s="102"/>
+      <c r="C14" s="100"/>
     </row>
     <row r="15" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
@@ -23491,20 +24029,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="93" t="s">
+      <c r="A17" s="99" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="95" t="s">
+      <c r="B17" s="101" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="93" t="s">
+      <c r="C17" s="99" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="94"/>
-      <c r="B18" s="96"/>
-      <c r="C18" s="94"/>
+      <c r="A18" s="100"/>
+      <c r="B18" s="102"/>
+      <c r="C18" s="100"/>
     </row>
     <row r="19" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -23546,6 +24084,104 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
+  <dimension ref="A1:A16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="36" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="36" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="36" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="36" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="39" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="40" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="40" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="40" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="40" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="40" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="40" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="40" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="41" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="41" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="41" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="23" t="s">
+        <v>288</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A16">
+    <sortCondition ref="A1:A16"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0BB7-C151-C94B-945C-E2CA92034B13}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -23562,18 +24198,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="103" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -23690,18 +24326,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="103" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -23737,25 +24373,25 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="93" t="s">
+      <c r="A6" s="99" t="s">
         <v>292</v>
       </c>
-      <c r="B6" s="98" t="s">
+      <c r="B6" s="104" t="s">
         <v>291</v>
       </c>
-      <c r="C6" s="93" t="s">
+      <c r="C6" s="99" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="104"/>
-      <c r="B7" s="99"/>
-      <c r="C7" s="104"/>
+      <c r="A7" s="110"/>
+      <c r="B7" s="105"/>
+      <c r="C7" s="110"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="94"/>
-      <c r="B8" s="100"/>
-      <c r="C8" s="94"/>
+      <c r="A8" s="100"/>
+      <c r="B8" s="106"/>
+      <c r="C8" s="100"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -23780,25 +24416,25 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="101" t="s">
+      <c r="A11" s="107" t="s">
         <v>294</v>
       </c>
-      <c r="B11" s="98" t="s">
+      <c r="B11" s="104" t="s">
         <v>295</v>
       </c>
-      <c r="C11" s="101" t="s">
+      <c r="C11" s="107" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="102"/>
-      <c r="B12" s="99"/>
-      <c r="C12" s="102"/>
+      <c r="A12" s="108"/>
+      <c r="B12" s="105"/>
+      <c r="C12" s="108"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="103"/>
-      <c r="B13" s="100"/>
-      <c r="C13" s="103"/>
+      <c r="A13" s="109"/>
+      <c r="B13" s="106"/>
+      <c r="C13" s="109"/>
     </row>
     <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
@@ -23855,18 +24491,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="103" t="s">
         <v>299</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -23880,46 +24516,46 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="105" t="s">
+      <c r="A4" s="111" t="s">
         <v>300</v>
       </c>
-      <c r="B4" s="109" t="s">
+      <c r="B4" s="115" t="s">
         <v>305</v>
       </c>
-      <c r="C4" s="105" t="s">
+      <c r="C4" s="111" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="105"/>
-      <c r="B5" s="109"/>
-      <c r="C5" s="105"/>
+      <c r="A5" s="111"/>
+      <c r="B5" s="115"/>
+      <c r="C5" s="111"/>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="105"/>
-      <c r="B6" s="109"/>
-      <c r="C6" s="105"/>
+      <c r="A6" s="111"/>
+      <c r="B6" s="115"/>
+      <c r="C6" s="111"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="93" t="s">
+      <c r="A7" s="99" t="s">
         <v>302</v>
       </c>
-      <c r="B7" s="106" t="s">
+      <c r="B7" s="112" t="s">
         <v>303</v>
       </c>
-      <c r="C7" s="93" t="s">
+      <c r="C7" s="99" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="104"/>
-      <c r="B8" s="107"/>
-      <c r="C8" s="104"/>
+      <c r="A8" s="110"/>
+      <c r="B8" s="113"/>
+      <c r="C8" s="110"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="228" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="94"/>
-      <c r="B9" s="108"/>
-      <c r="C9" s="94"/>
+      <c r="A9" s="100"/>
+      <c r="B9" s="114"/>
+      <c r="C9" s="100"/>
     </row>
     <row r="10" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
@@ -23976,18 +24612,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="103" t="s">
         <v>331</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -24034,233 +24670,233 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="93" t="s">
+      <c r="A7" s="99" t="s">
         <v>314</v>
       </c>
-      <c r="B7" s="98" t="s">
+      <c r="B7" s="104" t="s">
         <v>322</v>
       </c>
-      <c r="C7" s="93" t="s">
+      <c r="C7" s="99" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="104"/>
-      <c r="B8" s="99"/>
-      <c r="C8" s="104"/>
+      <c r="A8" s="110"/>
+      <c r="B8" s="105"/>
+      <c r="C8" s="110"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="104"/>
-      <c r="B9" s="99"/>
-      <c r="C9" s="104"/>
+      <c r="A9" s="110"/>
+      <c r="B9" s="105"/>
+      <c r="C9" s="110"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="104"/>
-      <c r="B10" s="99"/>
-      <c r="C10" s="104"/>
+      <c r="A10" s="110"/>
+      <c r="B10" s="105"/>
+      <c r="C10" s="110"/>
     </row>
     <row r="11" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="104"/>
-      <c r="B11" s="99"/>
-      <c r="C11" s="104"/>
+      <c r="A11" s="110"/>
+      <c r="B11" s="105"/>
+      <c r="C11" s="110"/>
     </row>
     <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="104"/>
-      <c r="B12" s="99"/>
-      <c r="C12" s="104"/>
+      <c r="A12" s="110"/>
+      <c r="B12" s="105"/>
+      <c r="C12" s="110"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="94"/>
-      <c r="B13" s="100"/>
-      <c r="C13" s="94"/>
+      <c r="A13" s="100"/>
+      <c r="B13" s="106"/>
+      <c r="C13" s="100"/>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="99" t="s">
         <v>325</v>
       </c>
-      <c r="B14" s="98" t="s">
+      <c r="B14" s="104" t="s">
         <v>323</v>
       </c>
-      <c r="C14" s="93" t="s">
+      <c r="C14" s="99" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="104"/>
-      <c r="B15" s="99"/>
-      <c r="C15" s="104"/>
+      <c r="A15" s="110"/>
+      <c r="B15" s="105"/>
+      <c r="C15" s="110"/>
     </row>
     <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="104"/>
-      <c r="B16" s="99"/>
-      <c r="C16" s="104"/>
+      <c r="A16" s="110"/>
+      <c r="B16" s="105"/>
+      <c r="C16" s="110"/>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="104"/>
-      <c r="B17" s="99"/>
-      <c r="C17" s="104"/>
+      <c r="A17" s="110"/>
+      <c r="B17" s="105"/>
+      <c r="C17" s="110"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="104"/>
-      <c r="B18" s="99"/>
-      <c r="C18" s="104"/>
+      <c r="A18" s="110"/>
+      <c r="B18" s="105"/>
+      <c r="C18" s="110"/>
     </row>
     <row r="19" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="104"/>
-      <c r="B19" s="99"/>
-      <c r="C19" s="104"/>
+      <c r="A19" s="110"/>
+      <c r="B19" s="105"/>
+      <c r="C19" s="110"/>
     </row>
     <row r="20" spans="1:3" ht="155" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="104"/>
-      <c r="B20" s="100"/>
-      <c r="C20" s="104"/>
+      <c r="A20" s="110"/>
+      <c r="B20" s="106"/>
+      <c r="C20" s="110"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="104"/>
-      <c r="B21" s="98" t="s">
+      <c r="A21" s="110"/>
+      <c r="B21" s="104" t="s">
         <v>316</v>
       </c>
-      <c r="C21" s="104"/>
+      <c r="C21" s="110"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="104"/>
-      <c r="B22" s="99"/>
-      <c r="C22" s="104"/>
+      <c r="A22" s="110"/>
+      <c r="B22" s="105"/>
+      <c r="C22" s="110"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="104"/>
-      <c r="B23" s="99"/>
-      <c r="C23" s="104"/>
+      <c r="A23" s="110"/>
+      <c r="B23" s="105"/>
+      <c r="C23" s="110"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="104"/>
-      <c r="B24" s="99"/>
-      <c r="C24" s="104"/>
+      <c r="A24" s="110"/>
+      <c r="B24" s="105"/>
+      <c r="C24" s="110"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="104"/>
-      <c r="B25" s="99"/>
-      <c r="C25" s="104"/>
+      <c r="A25" s="110"/>
+      <c r="B25" s="105"/>
+      <c r="C25" s="110"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="104"/>
-      <c r="B26" s="99"/>
-      <c r="C26" s="104"/>
+      <c r="A26" s="110"/>
+      <c r="B26" s="105"/>
+      <c r="C26" s="110"/>
     </row>
     <row r="27" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="104"/>
-      <c r="B27" s="100"/>
-      <c r="C27" s="104"/>
+      <c r="A27" s="110"/>
+      <c r="B27" s="106"/>
+      <c r="C27" s="110"/>
     </row>
     <row r="28" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="104"/>
-      <c r="B28" s="98" t="s">
+      <c r="A28" s="110"/>
+      <c r="B28" s="104" t="s">
         <v>317</v>
       </c>
-      <c r="C28" s="104"/>
+      <c r="C28" s="110"/>
     </row>
     <row r="29" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="104"/>
-      <c r="B29" s="99"/>
-      <c r="C29" s="104"/>
+      <c r="A29" s="110"/>
+      <c r="B29" s="105"/>
+      <c r="C29" s="110"/>
     </row>
     <row r="30" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="104"/>
-      <c r="B30" s="99"/>
-      <c r="C30" s="104"/>
+      <c r="A30" s="110"/>
+      <c r="B30" s="105"/>
+      <c r="C30" s="110"/>
     </row>
     <row r="31" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="104"/>
-      <c r="B31" s="99"/>
-      <c r="C31" s="104"/>
+      <c r="A31" s="110"/>
+      <c r="B31" s="105"/>
+      <c r="C31" s="110"/>
     </row>
     <row r="32" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="104"/>
-      <c r="B32" s="99"/>
-      <c r="C32" s="104"/>
+      <c r="A32" s="110"/>
+      <c r="B32" s="105"/>
+      <c r="C32" s="110"/>
     </row>
     <row r="33" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="104"/>
-      <c r="B33" s="99"/>
-      <c r="C33" s="104"/>
+      <c r="A33" s="110"/>
+      <c r="B33" s="105"/>
+      <c r="C33" s="110"/>
     </row>
     <row r="34" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="104"/>
-      <c r="B34" s="99"/>
-      <c r="C34" s="104"/>
+      <c r="A34" s="110"/>
+      <c r="B34" s="105"/>
+      <c r="C34" s="110"/>
     </row>
     <row r="35" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="104"/>
-      <c r="B35" s="99"/>
-      <c r="C35" s="104"/>
+      <c r="A35" s="110"/>
+      <c r="B35" s="105"/>
+      <c r="C35" s="110"/>
     </row>
     <row r="36" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="104"/>
-      <c r="B36" s="99"/>
-      <c r="C36" s="104"/>
+      <c r="A36" s="110"/>
+      <c r="B36" s="105"/>
+      <c r="C36" s="110"/>
     </row>
     <row r="37" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="104"/>
-      <c r="B37" s="100"/>
-      <c r="C37" s="104"/>
+      <c r="A37" s="110"/>
+      <c r="B37" s="106"/>
+      <c r="C37" s="110"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="104"/>
-      <c r="B38" s="98" t="s">
+      <c r="A38" s="110"/>
+      <c r="B38" s="104" t="s">
         <v>318</v>
       </c>
-      <c r="C38" s="104"/>
+      <c r="C38" s="110"/>
     </row>
     <row r="39" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="104"/>
-      <c r="B39" s="99"/>
-      <c r="C39" s="104"/>
+      <c r="A39" s="110"/>
+      <c r="B39" s="105"/>
+      <c r="C39" s="110"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="104"/>
-      <c r="B40" s="99"/>
-      <c r="C40" s="104"/>
+      <c r="A40" s="110"/>
+      <c r="B40" s="105"/>
+      <c r="C40" s="110"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="104"/>
-      <c r="B41" s="99"/>
-      <c r="C41" s="104"/>
+      <c r="A41" s="110"/>
+      <c r="B41" s="105"/>
+      <c r="C41" s="110"/>
     </row>
     <row r="42" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="94"/>
-      <c r="B42" s="100"/>
-      <c r="C42" s="94"/>
+      <c r="A42" s="100"/>
+      <c r="B42" s="106"/>
+      <c r="C42" s="100"/>
     </row>
     <row r="43" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="93" t="s">
+      <c r="A43" s="99" t="s">
         <v>326</v>
       </c>
-      <c r="B43" s="98" t="s">
+      <c r="B43" s="104" t="s">
         <v>327</v>
       </c>
-      <c r="C43" s="93" t="s">
+      <c r="C43" s="99" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="104"/>
-      <c r="B44" s="99"/>
-      <c r="C44" s="104"/>
+      <c r="A44" s="110"/>
+      <c r="B44" s="105"/>
+      <c r="C44" s="110"/>
     </row>
     <row r="45" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="104"/>
-      <c r="B45" s="99"/>
-      <c r="C45" s="104"/>
+      <c r="A45" s="110"/>
+      <c r="B45" s="105"/>
+      <c r="C45" s="110"/>
     </row>
     <row r="46" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="104"/>
-      <c r="B46" s="99"/>
-      <c r="C46" s="104"/>
+      <c r="A46" s="110"/>
+      <c r="B46" s="105"/>
+      <c r="C46" s="110"/>
     </row>
     <row r="47" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="94"/>
-      <c r="B47" s="100"/>
-      <c r="C47" s="94"/>
+      <c r="A47" s="100"/>
+      <c r="B47" s="106"/>
+      <c r="C47" s="100"/>
     </row>
     <row r="48" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
@@ -24287,6 +24923,11 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B7:B13"/>
+    <mergeCell ref="A7:A13"/>
+    <mergeCell ref="C7:C13"/>
     <mergeCell ref="B38:B42"/>
     <mergeCell ref="A14:A42"/>
     <mergeCell ref="C14:C42"/>
@@ -24296,11 +24937,6 @@
     <mergeCell ref="B28:B37"/>
     <mergeCell ref="B14:B20"/>
     <mergeCell ref="B21:B27"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B7:B13"/>
-    <mergeCell ref="A7:A13"/>
-    <mergeCell ref="C7:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24323,18 +24959,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="103" t="s">
         <v>332</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -24473,18 +25109,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="103" t="s">
         <v>356</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -24568,18 +25204,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="103" t="s">
         <v>365</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -24604,20 +25240,20 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="93" t="s">
+      <c r="A5" s="99" t="s">
         <v>369</v>
       </c>
-      <c r="B5" s="110" t="s">
+      <c r="B5" s="116" t="s">
         <v>372</v>
       </c>
-      <c r="C5" s="93" t="s">
+      <c r="C5" s="99" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="94"/>
-      <c r="B6" s="112"/>
-      <c r="C6" s="94"/>
+      <c r="A6" s="100"/>
+      <c r="B6" s="118"/>
+      <c r="C6" s="100"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A7" s="59" t="s">
@@ -24631,67 +25267,67 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="93" t="s">
+      <c r="A8" s="99" t="s">
         <v>376</v>
       </c>
-      <c r="B8" s="110" t="s">
+      <c r="B8" s="116" t="s">
         <v>375</v>
       </c>
-      <c r="C8" s="93" t="s">
+      <c r="C8" s="99" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="104"/>
-      <c r="B9" s="111"/>
-      <c r="C9" s="104"/>
+      <c r="A9" s="110"/>
+      <c r="B9" s="117"/>
+      <c r="C9" s="110"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="94"/>
-      <c r="B10" s="112"/>
-      <c r="C10" s="94"/>
+      <c r="A10" s="100"/>
+      <c r="B10" s="118"/>
+      <c r="C10" s="100"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="93" t="s">
+      <c r="A11" s="99" t="s">
         <v>378</v>
       </c>
-      <c r="B11" s="110" t="s">
+      <c r="B11" s="116" t="s">
         <v>384</v>
       </c>
-      <c r="C11" s="93" t="s">
+      <c r="C11" s="99" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="104"/>
-      <c r="B12" s="111"/>
-      <c r="C12" s="104"/>
+      <c r="A12" s="110"/>
+      <c r="B12" s="117"/>
+      <c r="C12" s="110"/>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="187" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="94"/>
-      <c r="B13" s="112"/>
-      <c r="C13" s="94"/>
+      <c r="A13" s="100"/>
+      <c r="B13" s="118"/>
+      <c r="C13" s="100"/>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="99" t="s">
         <v>380</v>
       </c>
-      <c r="B14" s="110" t="s">
+      <c r="B14" s="116" t="s">
         <v>383</v>
       </c>
-      <c r="C14" s="93" t="s">
+      <c r="C14" s="99" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="104"/>
-      <c r="B15" s="111"/>
-      <c r="C15" s="104"/>
+      <c r="A15" s="110"/>
+      <c r="B15" s="117"/>
+      <c r="C15" s="110"/>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="94"/>
-      <c r="B16" s="112"/>
-      <c r="C16" s="94"/>
+      <c r="A16" s="100"/>
+      <c r="B16" s="118"/>
+      <c r="C16" s="100"/>
     </row>
     <row r="17" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
@@ -24718,12 +25354,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="C14:C16"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="C8:C10"/>
@@ -24732,6 +25362,12 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C14:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -24754,18 +25390,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="97" t="s">
+      <c r="A2" s="103" t="s">
         <v>395</v>
       </c>
-      <c r="B2" s="97"/>
-      <c r="C2" s="97"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -24788,217 +25424,217 @@
       <c r="C4" s="60"/>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="93" t="s">
+      <c r="A5" s="99" t="s">
         <v>397</v>
       </c>
-      <c r="B5" s="115" t="s">
+      <c r="B5" s="119" t="s">
         <v>396</v>
       </c>
-      <c r="C5" s="93" t="s">
+      <c r="C5" s="99" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="283" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="104"/>
-      <c r="B6" s="116"/>
-      <c r="C6" s="104"/>
+      <c r="A6" s="110"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="110"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="104"/>
-      <c r="B7" s="116"/>
-      <c r="C7" s="104"/>
+      <c r="A7" s="110"/>
+      <c r="B7" s="120"/>
+      <c r="C7" s="110"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="104"/>
-      <c r="B8" s="116"/>
-      <c r="C8" s="104"/>
+      <c r="A8" s="110"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="110"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="104"/>
-      <c r="B9" s="116"/>
-      <c r="C9" s="104"/>
+      <c r="A9" s="110"/>
+      <c r="B9" s="120"/>
+      <c r="C9" s="110"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="104"/>
-      <c r="B10" s="116"/>
-      <c r="C10" s="104"/>
+      <c r="A10" s="110"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="110"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="104"/>
-      <c r="B11" s="116"/>
-      <c r="C11" s="104"/>
+      <c r="A11" s="110"/>
+      <c r="B11" s="120"/>
+      <c r="C11" s="110"/>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="94"/>
-      <c r="B12" s="117"/>
-      <c r="C12" s="94"/>
+      <c r="A12" s="100"/>
+      <c r="B12" s="121"/>
+      <c r="C12" s="100"/>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="93" t="s">
+      <c r="A13" s="99" t="s">
         <v>399</v>
       </c>
-      <c r="B13" s="98" t="s">
+      <c r="B13" s="104" t="s">
         <v>400</v>
       </c>
-      <c r="C13" s="93" t="s">
+      <c r="C13" s="99" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="104"/>
-      <c r="B14" s="99"/>
-      <c r="C14" s="104"/>
+      <c r="A14" s="110"/>
+      <c r="B14" s="105"/>
+      <c r="C14" s="110"/>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="104"/>
-      <c r="B15" s="99"/>
-      <c r="C15" s="104"/>
+      <c r="A15" s="110"/>
+      <c r="B15" s="105"/>
+      <c r="C15" s="110"/>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="104"/>
-      <c r="B16" s="98" t="s">
+      <c r="A16" s="110"/>
+      <c r="B16" s="104" t="s">
         <v>401</v>
       </c>
-      <c r="C16" s="104"/>
+      <c r="C16" s="110"/>
     </row>
     <row r="17" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="104"/>
-      <c r="B17" s="99"/>
-      <c r="C17" s="104"/>
+      <c r="A17" s="110"/>
+      <c r="B17" s="105"/>
+      <c r="C17" s="110"/>
     </row>
     <row r="18" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="104"/>
-      <c r="B18" s="99"/>
-      <c r="C18" s="104"/>
+      <c r="A18" s="110"/>
+      <c r="B18" s="105"/>
+      <c r="C18" s="110"/>
     </row>
     <row r="19" spans="1:3" s="13" customFormat="1" ht="159" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="104"/>
-      <c r="B19" s="99"/>
-      <c r="C19" s="104"/>
+      <c r="A19" s="110"/>
+      <c r="B19" s="105"/>
+      <c r="C19" s="110"/>
     </row>
     <row r="20" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="104"/>
-      <c r="B20" s="99" t="s">
+      <c r="A20" s="110"/>
+      <c r="B20" s="105" t="s">
         <v>402</v>
       </c>
-      <c r="C20" s="104"/>
+      <c r="C20" s="110"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="104"/>
-      <c r="B21" s="99"/>
-      <c r="C21" s="104"/>
+      <c r="A21" s="110"/>
+      <c r="B21" s="105"/>
+      <c r="C21" s="110"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="104"/>
-      <c r="B22" s="99"/>
-      <c r="C22" s="104"/>
+      <c r="A22" s="110"/>
+      <c r="B22" s="105"/>
+      <c r="C22" s="110"/>
     </row>
     <row r="23" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="104"/>
-      <c r="B23" s="99"/>
-      <c r="C23" s="104"/>
+      <c r="A23" s="110"/>
+      <c r="B23" s="105"/>
+      <c r="C23" s="110"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="104"/>
-      <c r="B24" s="99" t="s">
+      <c r="A24" s="110"/>
+      <c r="B24" s="105" t="s">
         <v>403</v>
       </c>
-      <c r="C24" s="104"/>
+      <c r="C24" s="110"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="104"/>
-      <c r="B25" s="99"/>
-      <c r="C25" s="104"/>
+      <c r="A25" s="110"/>
+      <c r="B25" s="105"/>
+      <c r="C25" s="110"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="104"/>
-      <c r="B26" s="99" t="s">
+      <c r="A26" s="110"/>
+      <c r="B26" s="105" t="s">
         <v>317</v>
       </c>
-      <c r="C26" s="104"/>
+      <c r="C26" s="110"/>
     </row>
     <row r="27" spans="1:3" ht="144" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="104"/>
-      <c r="B27" s="99"/>
-      <c r="C27" s="104"/>
+      <c r="A27" s="110"/>
+      <c r="B27" s="105"/>
+      <c r="C27" s="110"/>
     </row>
     <row r="28" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="104"/>
-      <c r="B28" s="99" t="s">
+      <c r="A28" s="110"/>
+      <c r="B28" s="105" t="s">
         <v>404</v>
       </c>
-      <c r="C28" s="104"/>
+      <c r="C28" s="110"/>
     </row>
     <row r="29" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="104"/>
-      <c r="B29" s="99"/>
-      <c r="C29" s="104"/>
+      <c r="A29" s="110"/>
+      <c r="B29" s="105"/>
+      <c r="C29" s="110"/>
     </row>
     <row r="30" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="104"/>
-      <c r="B30" s="99"/>
-      <c r="C30" s="104"/>
+      <c r="A30" s="110"/>
+      <c r="B30" s="105"/>
+      <c r="C30" s="110"/>
     </row>
     <row r="31" spans="1:3" ht="196" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="104"/>
-      <c r="B31" s="99"/>
-      <c r="C31" s="104"/>
+      <c r="A31" s="110"/>
+      <c r="B31" s="105"/>
+      <c r="C31" s="110"/>
     </row>
     <row r="32" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="104"/>
-      <c r="B32" s="99" t="s">
+      <c r="A32" s="110"/>
+      <c r="B32" s="105" t="s">
         <v>405</v>
       </c>
-      <c r="C32" s="104"/>
+      <c r="C32" s="110"/>
     </row>
     <row r="33" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="104"/>
-      <c r="B33" s="99"/>
-      <c r="C33" s="104"/>
+      <c r="A33" s="110"/>
+      <c r="B33" s="105"/>
+      <c r="C33" s="110"/>
     </row>
     <row r="34" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="104"/>
-      <c r="B34" s="99"/>
-      <c r="C34" s="104"/>
+      <c r="A34" s="110"/>
+      <c r="B34" s="105"/>
+      <c r="C34" s="110"/>
     </row>
     <row r="35" spans="1:3" ht="201" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="104"/>
-      <c r="B35" s="99"/>
-      <c r="C35" s="104"/>
+      <c r="A35" s="110"/>
+      <c r="B35" s="105"/>
+      <c r="C35" s="110"/>
     </row>
     <row r="36" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="104"/>
-      <c r="B36" s="99" t="s">
+      <c r="A36" s="110"/>
+      <c r="B36" s="105" t="s">
         <v>406</v>
       </c>
-      <c r="C36" s="104"/>
+      <c r="C36" s="110"/>
     </row>
     <row r="37" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="104"/>
-      <c r="B37" s="99"/>
-      <c r="C37" s="104"/>
+      <c r="A37" s="110"/>
+      <c r="B37" s="105"/>
+      <c r="C37" s="110"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="104"/>
-      <c r="B38" s="99"/>
-      <c r="C38" s="104"/>
+      <c r="A38" s="110"/>
+      <c r="B38" s="105"/>
+      <c r="C38" s="110"/>
     </row>
     <row r="39" spans="1:3" ht="239" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="104"/>
-      <c r="B39" s="99"/>
-      <c r="C39" s="104"/>
+      <c r="A39" s="110"/>
+      <c r="B39" s="105"/>
+      <c r="C39" s="110"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="104"/>
-      <c r="B40" s="99" t="s">
+      <c r="A40" s="110"/>
+      <c r="B40" s="105" t="s">
         <v>407</v>
       </c>
-      <c r="C40" s="104"/>
+      <c r="C40" s="110"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="94"/>
-      <c r="B41" s="100"/>
-      <c r="C41" s="94"/>
+      <c r="A41" s="100"/>
+      <c r="B41" s="106"/>
+      <c r="C41" s="100"/>
     </row>
     <row r="42" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A42" s="60" t="s">
@@ -25038,11 +25674,11 @@
       <c r="C46" s="60"/>
     </row>
     <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A47" s="97" t="s">
+      <c r="A47" s="103" t="s">
         <v>386</v>
       </c>
-      <c r="B47" s="97"/>
-      <c r="C47" s="97"/>
+      <c r="B47" s="103"/>
+      <c r="C47" s="103"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
@@ -25056,25 +25692,25 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="93" t="s">
+      <c r="A49" s="99" t="s">
         <v>388</v>
       </c>
-      <c r="B49" s="95" t="s">
+      <c r="B49" s="101" t="s">
         <v>413</v>
       </c>
-      <c r="C49" s="93" t="s">
+      <c r="C49" s="99" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="104"/>
-      <c r="B50" s="114"/>
-      <c r="C50" s="104"/>
+      <c r="A50" s="110"/>
+      <c r="B50" s="122"/>
+      <c r="C50" s="110"/>
     </row>
     <row r="51" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="94"/>
-      <c r="B51" s="96"/>
-      <c r="C51" s="94"/>
+      <c r="A51" s="100"/>
+      <c r="B51" s="102"/>
+      <c r="C51" s="100"/>
     </row>
     <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="54" t="s">
@@ -25088,91 +25724,91 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="93" t="s">
+      <c r="A53" s="99" t="s">
         <v>415</v>
       </c>
-      <c r="B53" s="113" t="s">
+      <c r="B53" s="123" t="s">
         <v>416</v>
       </c>
-      <c r="C53" s="93" t="s">
+      <c r="C53" s="99" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="238" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="104"/>
-      <c r="B54" s="113"/>
-      <c r="C54" s="104"/>
+      <c r="A54" s="110"/>
+      <c r="B54" s="123"/>
+      <c r="C54" s="110"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="104"/>
-      <c r="B55" s="95" t="s">
+      <c r="A55" s="110"/>
+      <c r="B55" s="101" t="s">
         <v>417</v>
       </c>
-      <c r="C55" s="104"/>
+      <c r="C55" s="110"/>
     </row>
     <row r="56" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="104"/>
-      <c r="B56" s="114"/>
-      <c r="C56" s="104"/>
+      <c r="A56" s="110"/>
+      <c r="B56" s="122"/>
+      <c r="C56" s="110"/>
     </row>
     <row r="57" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="104"/>
-      <c r="B57" s="114"/>
-      <c r="C57" s="104"/>
+      <c r="A57" s="110"/>
+      <c r="B57" s="122"/>
+      <c r="C57" s="110"/>
     </row>
     <row r="58" spans="1:3" ht="172" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="104"/>
-      <c r="B58" s="96"/>
-      <c r="C58" s="104"/>
+      <c r="A58" s="110"/>
+      <c r="B58" s="102"/>
+      <c r="C58" s="110"/>
     </row>
     <row r="59" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="104"/>
-      <c r="B59" s="95" t="s">
+      <c r="A59" s="110"/>
+      <c r="B59" s="101" t="s">
         <v>418</v>
       </c>
-      <c r="C59" s="104"/>
+      <c r="C59" s="110"/>
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="104"/>
-      <c r="B60" s="114"/>
-      <c r="C60" s="104"/>
+      <c r="A60" s="110"/>
+      <c r="B60" s="122"/>
+      <c r="C60" s="110"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="104"/>
-      <c r="B61" s="114"/>
-      <c r="C61" s="104"/>
+      <c r="A61" s="110"/>
+      <c r="B61" s="122"/>
+      <c r="C61" s="110"/>
     </row>
     <row r="62" spans="1:3" ht="125" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="104"/>
-      <c r="B62" s="96"/>
-      <c r="C62" s="104"/>
+      <c r="A62" s="110"/>
+      <c r="B62" s="102"/>
+      <c r="C62" s="110"/>
     </row>
     <row r="63" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="104"/>
-      <c r="B63" s="95" t="s">
+      <c r="A63" s="110"/>
+      <c r="B63" s="101" t="s">
         <v>419</v>
       </c>
-      <c r="C63" s="104"/>
+      <c r="C63" s="110"/>
     </row>
     <row r="64" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="104"/>
-      <c r="B64" s="114"/>
-      <c r="C64" s="104"/>
+      <c r="A64" s="110"/>
+      <c r="B64" s="122"/>
+      <c r="C64" s="110"/>
     </row>
     <row r="65" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="104"/>
-      <c r="B65" s="114"/>
-      <c r="C65" s="104"/>
+      <c r="A65" s="110"/>
+      <c r="B65" s="122"/>
+      <c r="C65" s="110"/>
     </row>
     <row r="66" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="104"/>
-      <c r="B66" s="114"/>
-      <c r="C66" s="104"/>
+      <c r="A66" s="110"/>
+      <c r="B66" s="122"/>
+      <c r="C66" s="110"/>
     </row>
     <row r="67" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="94"/>
-      <c r="B67" s="96"/>
-      <c r="C67" s="94"/>
+      <c r="A67" s="100"/>
+      <c r="B67" s="102"/>
+      <c r="C67" s="100"/>
     </row>
     <row r="68" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A68" s="60" t="s">
@@ -25210,18 +25846,11 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="25">
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B5:B12"/>
-    <mergeCell ref="A5:A12"/>
-    <mergeCell ref="C5:C12"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="C13:C41"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C53:C67"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="B63:B67"/>
     <mergeCell ref="A53:A67"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="B32:B35"/>
@@ -25230,11 +25859,18 @@
     <mergeCell ref="A13:A41"/>
     <mergeCell ref="B49:B51"/>
     <mergeCell ref="A49:A51"/>
-    <mergeCell ref="C53:C67"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="B63:B67"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="C13:C41"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B5:B12"/>
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="C5:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add the page session store data in the loadSurveyPageOnSpecificationClick() callback function .
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB5DC6A-A919-8B43-9938-440B3767FB1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D361DEFB-961C-B44F-99E9-D9906E3C62E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16160" firstSheet="8" activeTab="18" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16160" firstSheet="11" activeTab="19" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="SPEC - 1.1" sheetId="1" r:id="rId1"/>
@@ -32,9 +32,10 @@
     <sheet name="SPEC - 3.2" sheetId="21" r:id="rId17"/>
     <sheet name="SPEC - 3.3" sheetId="22" r:id="rId18"/>
     <sheet name="SPEC - 3.4" sheetId="23" r:id="rId19"/>
-    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId20"/>
-    <sheet name="PLAYGROUND" sheetId="6" r:id="rId21"/>
-    <sheet name="TEMPLATE" sheetId="8" r:id="rId22"/>
+    <sheet name="SPEC - 3.5" sheetId="24" r:id="rId20"/>
+    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId21"/>
+    <sheet name="PLAYGROUND" sheetId="6" r:id="rId22"/>
+    <sheet name="TEMPLATE" sheetId="8" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="737">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -20031,6 +20032,165 @@
         modified:   js/controller/lock-selection-survey-customer-card.js
         modified:   js/controller/lock-selection-survey-lock-card.js</t>
     </r>
+  </si>
+  <si>
+    <t>UPDATE THE door-specification-next RELATED CALLBACK FUCTNCTION loadSurveyPageOnSpecificationClick TO ADD SESSION DATA RELATED TO PAGE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">/* The callback function fired on 'click' - for door specification 
+ * next button control.
+ * @param    
+ * @return   
+ * */
+const loadSurveyPageOnSpecificationClick = () =&gt; {
+    // Ensure that no lock models are selected by default
+    lockModelSelectionGroup.options[0].selected = true
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+     // Save the page data to the session storage
+     sessionStorage.setItem('page', "1");
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">loadSurveyPageOnSpecificationClick() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">call back function in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller/index.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to add page data to the session data store</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">loadSurveyPageOnSpecificationClick() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">call back function in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller/index.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to add page data to the session data store</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>git status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - would display the following files.                                                                                                                                                                                                                                  On branch lock
+Changes not staged for commit:
+  (use "git add &lt;file&gt;..." to update what will be committed)
+  (use "git restore &lt;file&gt;..." to discard changes in working directory)
+        modified:   docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+        modified:   js/controller/index.js</t>
+    </r>
+  </si>
+  <si>
+    <t>git commit -m "Add the page session store data in the loadSurveyPageOnSpecificationClick() callback function ."</t>
   </si>
 </sst>
 </file>
@@ -20456,7 +20616,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -20708,6 +20868,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -21155,18 +21318,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -21451,18 +21614,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="108" t="s">
         <v>426</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -21476,7 +21639,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="128" t="s">
+      <c r="A4" s="129" t="s">
         <v>438</v>
       </c>
       <c r="B4" s="48" t="s">
@@ -21487,7 +21650,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="129"/>
+      <c r="A5" s="130"/>
       <c r="B5" s="48" t="s">
         <v>441</v>
       </c>
@@ -21496,51 +21659,51 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="129"/>
+      <c r="A6" s="130"/>
       <c r="B6" s="48" t="s">
         <v>434</v>
       </c>
-      <c r="C6" s="131" t="s">
+      <c r="C6" s="132" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="129"/>
+      <c r="A7" s="130"/>
       <c r="B7" s="48" t="s">
         <v>435</v>
       </c>
-      <c r="C7" s="132"/>
+      <c r="C7" s="133"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="129"/>
+      <c r="A8" s="130"/>
       <c r="B8" s="48" t="s">
         <v>427</v>
       </c>
-      <c r="C8" s="132"/>
+      <c r="C8" s="133"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="129"/>
+      <c r="A9" s="130"/>
       <c r="B9" s="48" t="s">
         <v>428</v>
       </c>
-      <c r="C9" s="132"/>
+      <c r="C9" s="133"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="129"/>
+      <c r="A10" s="130"/>
       <c r="B10" s="48" t="s">
         <v>436</v>
       </c>
-      <c r="C10" s="132"/>
+      <c r="C10" s="133"/>
     </row>
     <row r="11" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="129"/>
+      <c r="A11" s="130"/>
       <c r="B11" s="48" t="s">
         <v>443</v>
       </c>
-      <c r="C11" s="133"/>
+      <c r="C11" s="134"/>
     </row>
     <row r="12" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="130"/>
+      <c r="A12" s="131"/>
       <c r="B12" s="48" t="s">
         <v>445</v>
       </c>
@@ -21679,18 +21842,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="108" t="s">
         <v>464</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -21796,18 +21959,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="108" t="s">
         <v>478</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -21858,11 +22021,11 @@
       <c r="C8" s="54"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="107" t="s">
+      <c r="A9" s="108" t="s">
         <v>485</v>
       </c>
-      <c r="B9" s="107"/>
-      <c r="C9" s="107"/>
+      <c r="B9" s="108"/>
+      <c r="C9" s="108"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -21898,20 +22061,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="103" t="s">
+      <c r="A13" s="104" t="s">
         <v>490</v>
       </c>
-      <c r="B13" s="108" t="s">
+      <c r="B13" s="109" t="s">
         <v>489</v>
       </c>
-      <c r="C13" s="103" t="s">
+      <c r="C13" s="104" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="104"/>
-      <c r="B14" s="110"/>
-      <c r="C14" s="104"/>
+      <c r="A14" s="105"/>
+      <c r="B14" s="111"/>
+      <c r="C14" s="105"/>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="73" t="s">
@@ -21936,20 +22099,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="103" t="s">
+      <c r="A17" s="104" t="s">
         <v>499</v>
       </c>
-      <c r="B17" s="108" t="s">
+      <c r="B17" s="109" t="s">
         <v>498</v>
       </c>
-      <c r="C17" s="103" t="s">
+      <c r="C17" s="104" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="222" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="104"/>
-      <c r="B18" s="110"/>
-      <c r="C18" s="104"/>
+      <c r="A18" s="105"/>
+      <c r="B18" s="111"/>
+      <c r="C18" s="105"/>
     </row>
     <row r="19" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -22007,18 +22170,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="108" t="s">
         <v>505</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -22076,25 +22239,25 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="103" t="s">
+      <c r="A8" s="104" t="s">
         <v>517</v>
       </c>
-      <c r="B8" s="108" t="s">
+      <c r="B8" s="109" t="s">
         <v>516</v>
       </c>
-      <c r="C8" s="103" t="s">
+      <c r="C8" s="104" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="114"/>
-      <c r="B9" s="109"/>
-      <c r="C9" s="114"/>
+      <c r="A9" s="115"/>
+      <c r="B9" s="110"/>
+      <c r="C9" s="115"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="104"/>
-      <c r="B10" s="110"/>
-      <c r="C10" s="104"/>
+      <c r="A10" s="105"/>
+      <c r="B10" s="111"/>
+      <c r="C10" s="105"/>
     </row>
     <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="54" t="s">
@@ -22108,86 +22271,86 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="103" t="s">
+      <c r="A12" s="104" t="s">
         <v>526</v>
       </c>
-      <c r="B12" s="108" t="s">
+      <c r="B12" s="109" t="s">
         <v>527</v>
       </c>
-      <c r="C12" s="103" t="s">
+      <c r="C12" s="104" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="114"/>
-      <c r="B13" s="109"/>
-      <c r="C13" s="114"/>
+      <c r="A13" s="115"/>
+      <c r="B13" s="110"/>
+      <c r="C13" s="115"/>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="114"/>
-      <c r="B14" s="109"/>
-      <c r="C14" s="114"/>
+      <c r="A14" s="115"/>
+      <c r="B14" s="110"/>
+      <c r="C14" s="115"/>
     </row>
     <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="114"/>
-      <c r="B15" s="109"/>
-      <c r="C15" s="114"/>
+      <c r="A15" s="115"/>
+      <c r="B15" s="110"/>
+      <c r="C15" s="115"/>
     </row>
     <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="114"/>
-      <c r="B16" s="109"/>
-      <c r="C16" s="114"/>
+      <c r="A16" s="115"/>
+      <c r="B16" s="110"/>
+      <c r="C16" s="115"/>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="114"/>
-      <c r="B17" s="109"/>
-      <c r="C17" s="114"/>
+      <c r="A17" s="115"/>
+      <c r="B17" s="110"/>
+      <c r="C17" s="115"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="104"/>
-      <c r="B18" s="109"/>
-      <c r="C18" s="104"/>
+      <c r="A18" s="105"/>
+      <c r="B18" s="110"/>
+      <c r="C18" s="105"/>
     </row>
     <row r="19" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="103" t="s">
+      <c r="A19" s="104" t="s">
         <v>529</v>
       </c>
-      <c r="B19" s="108" t="s">
+      <c r="B19" s="109" t="s">
         <v>528</v>
       </c>
-      <c r="C19" s="103" t="s">
+      <c r="C19" s="104" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="114"/>
-      <c r="B20" s="109"/>
-      <c r="C20" s="114"/>
+      <c r="A20" s="115"/>
+      <c r="B20" s="110"/>
+      <c r="C20" s="115"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="114"/>
-      <c r="B21" s="109"/>
-      <c r="C21" s="114"/>
+      <c r="A21" s="115"/>
+      <c r="B21" s="110"/>
+      <c r="C21" s="115"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="114"/>
-      <c r="B22" s="109"/>
-      <c r="C22" s="114"/>
+      <c r="A22" s="115"/>
+      <c r="B22" s="110"/>
+      <c r="C22" s="115"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="114"/>
-      <c r="B23" s="109"/>
-      <c r="C23" s="114"/>
+      <c r="A23" s="115"/>
+      <c r="B23" s="110"/>
+      <c r="C23" s="115"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="114"/>
-      <c r="B24" s="109"/>
-      <c r="C24" s="114"/>
+      <c r="A24" s="115"/>
+      <c r="B24" s="110"/>
+      <c r="C24" s="115"/>
     </row>
     <row r="25" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="104"/>
-      <c r="B25" s="110"/>
-      <c r="C25" s="104"/>
+      <c r="A25" s="105"/>
+      <c r="B25" s="111"/>
+      <c r="C25" s="105"/>
     </row>
     <row r="26" spans="1:3" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
@@ -22201,51 +22364,51 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="103" t="s">
+      <c r="A27" s="104" t="s">
         <v>533</v>
       </c>
-      <c r="B27" s="108" t="s">
+      <c r="B27" s="109" t="s">
         <v>532</v>
       </c>
-      <c r="C27" s="103" t="s">
+      <c r="C27" s="104" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="114"/>
-      <c r="B28" s="109"/>
-      <c r="C28" s="114"/>
+      <c r="A28" s="115"/>
+      <c r="B28" s="110"/>
+      <c r="C28" s="115"/>
     </row>
     <row r="29" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="104"/>
-      <c r="B29" s="110"/>
-      <c r="C29" s="104"/>
+      <c r="A29" s="105"/>
+      <c r="B29" s="111"/>
+      <c r="C29" s="105"/>
     </row>
     <row r="30" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="103" t="s">
+      <c r="A30" s="104" t="s">
         <v>536</v>
       </c>
-      <c r="B30" s="108" t="s">
+      <c r="B30" s="109" t="s">
         <v>535</v>
       </c>
-      <c r="C30" s="103" t="s">
+      <c r="C30" s="104" t="s">
         <v>537</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="114"/>
-      <c r="B31" s="109"/>
-      <c r="C31" s="114"/>
+      <c r="A31" s="115"/>
+      <c r="B31" s="110"/>
+      <c r="C31" s="115"/>
     </row>
     <row r="32" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="114"/>
-      <c r="B32" s="109"/>
-      <c r="C32" s="114"/>
+      <c r="A32" s="115"/>
+      <c r="B32" s="110"/>
+      <c r="C32" s="115"/>
     </row>
     <row r="33" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="104"/>
-      <c r="B33" s="110"/>
-      <c r="C33" s="104"/>
+      <c r="A33" s="105"/>
+      <c r="B33" s="111"/>
+      <c r="C33" s="105"/>
     </row>
     <row r="34" spans="1:3" ht="255" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
@@ -22311,18 +22474,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="108" t="s">
         <v>549</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -22417,18 +22580,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="108" t="s">
         <v>560</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -22490,11 +22653,11 @@
       <c r="C9" s="54"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="107" t="s">
+      <c r="A10" s="108" t="s">
         <v>575</v>
       </c>
-      <c r="B10" s="107"/>
-      <c r="C10" s="107"/>
+      <c r="B10" s="108"/>
+      <c r="C10" s="108"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
@@ -22610,18 +22773,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="108" t="s">
         <v>661</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -22679,20 +22842,20 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="103" t="s">
+      <c r="A8" s="104" t="s">
         <v>587</v>
       </c>
-      <c r="B8" s="108" t="s">
+      <c r="B8" s="109" t="s">
         <v>590</v>
       </c>
-      <c r="C8" s="103" t="s">
+      <c r="C8" s="104" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="109" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="104"/>
-      <c r="B9" s="110"/>
-      <c r="C9" s="104"/>
+      <c r="A9" s="105"/>
+      <c r="B9" s="111"/>
+      <c r="C9" s="105"/>
     </row>
     <row r="10" spans="1:3" ht="109" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="82" t="s">
@@ -22728,20 +22891,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="103" t="s">
+      <c r="A13" s="104" t="s">
         <v>603</v>
       </c>
-      <c r="B13" s="108" t="s">
+      <c r="B13" s="109" t="s">
         <v>602</v>
       </c>
-      <c r="C13" s="103" t="s">
+      <c r="C13" s="104" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="104"/>
-      <c r="B14" s="110"/>
-      <c r="C14" s="104"/>
+      <c r="A14" s="105"/>
+      <c r="B14" s="111"/>
+      <c r="C14" s="105"/>
     </row>
     <row r="15" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="82" t="s">
@@ -22755,67 +22918,67 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="135" t="s">
+      <c r="A16" s="136" t="s">
         <v>609</v>
       </c>
-      <c r="B16" s="134" t="s">
+      <c r="B16" s="135" t="s">
         <v>608</v>
       </c>
-      <c r="C16" s="135" t="s">
+      <c r="C16" s="136" t="s">
         <v>610</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="135"/>
-      <c r="B17" s="134"/>
-      <c r="C17" s="135"/>
+      <c r="A17" s="136"/>
+      <c r="B17" s="135"/>
+      <c r="C17" s="136"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="135"/>
-      <c r="B18" s="134"/>
-      <c r="C18" s="135"/>
+      <c r="A18" s="136"/>
+      <c r="B18" s="135"/>
+      <c r="C18" s="136"/>
     </row>
     <row r="19" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="135"/>
-      <c r="B19" s="134"/>
-      <c r="C19" s="135"/>
+      <c r="A19" s="136"/>
+      <c r="B19" s="135"/>
+      <c r="C19" s="136"/>
     </row>
     <row r="20" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="135"/>
-      <c r="B20" s="134"/>
-      <c r="C20" s="135"/>
+      <c r="A20" s="136"/>
+      <c r="B20" s="135"/>
+      <c r="C20" s="136"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="135"/>
-      <c r="B21" s="134"/>
-      <c r="C21" s="135"/>
+      <c r="A21" s="136"/>
+      <c r="B21" s="135"/>
+      <c r="C21" s="136"/>
     </row>
     <row r="22" spans="1:3" ht="139" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="135"/>
-      <c r="B22" s="134"/>
-      <c r="C22" s="135"/>
+      <c r="A22" s="136"/>
+      <c r="B22" s="135"/>
+      <c r="C22" s="136"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="135"/>
-      <c r="B23" s="134" t="s">
+      <c r="A23" s="136"/>
+      <c r="B23" s="135" t="s">
         <v>611</v>
       </c>
-      <c r="C23" s="135"/>
+      <c r="C23" s="136"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="135"/>
-      <c r="B24" s="134"/>
-      <c r="C24" s="135"/>
+      <c r="A24" s="136"/>
+      <c r="B24" s="135"/>
+      <c r="C24" s="136"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="135"/>
-      <c r="B25" s="134"/>
-      <c r="C25" s="135"/>
+      <c r="A25" s="136"/>
+      <c r="B25" s="135"/>
+      <c r="C25" s="136"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="135"/>
-      <c r="B26" s="134"/>
-      <c r="C26" s="135"/>
+      <c r="A26" s="136"/>
+      <c r="B26" s="135"/>
+      <c r="C26" s="136"/>
     </row>
     <row r="27" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="85" t="s">
@@ -22884,185 +23047,185 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="103" t="s">
+      <c r="A33" s="104" t="s">
         <v>633</v>
       </c>
-      <c r="B33" s="105" t="s">
+      <c r="B33" s="106" t="s">
         <v>627</v>
       </c>
-      <c r="C33" s="103" t="s">
+      <c r="C33" s="104" t="s">
         <v>633</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="114"/>
-      <c r="B34" s="124"/>
-      <c r="C34" s="114"/>
+      <c r="A34" s="115"/>
+      <c r="B34" s="125"/>
+      <c r="C34" s="115"/>
     </row>
     <row r="35" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="114"/>
-      <c r="B35" s="124"/>
-      <c r="C35" s="114"/>
+      <c r="A35" s="115"/>
+      <c r="B35" s="125"/>
+      <c r="C35" s="115"/>
     </row>
     <row r="36" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="114"/>
-      <c r="B36" s="106"/>
-      <c r="C36" s="114"/>
+      <c r="A36" s="115"/>
+      <c r="B36" s="107"/>
+      <c r="C36" s="115"/>
     </row>
     <row r="37" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="114"/>
-      <c r="B37" s="105" t="s">
+      <c r="A37" s="115"/>
+      <c r="B37" s="106" t="s">
         <v>628</v>
       </c>
-      <c r="C37" s="114"/>
+      <c r="C37" s="115"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="114"/>
-      <c r="B38" s="124"/>
-      <c r="C38" s="114"/>
+      <c r="A38" s="115"/>
+      <c r="B38" s="125"/>
+      <c r="C38" s="115"/>
     </row>
     <row r="39" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="114"/>
-      <c r="B39" s="124"/>
-      <c r="C39" s="114"/>
+      <c r="A39" s="115"/>
+      <c r="B39" s="125"/>
+      <c r="C39" s="115"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="114"/>
-      <c r="B40" s="124"/>
-      <c r="C40" s="114"/>
+      <c r="A40" s="115"/>
+      <c r="B40" s="125"/>
+      <c r="C40" s="115"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="114"/>
-      <c r="B41" s="124"/>
-      <c r="C41" s="114"/>
+      <c r="A41" s="115"/>
+      <c r="B41" s="125"/>
+      <c r="C41" s="115"/>
     </row>
     <row r="42" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="114"/>
-      <c r="B42" s="124"/>
-      <c r="C42" s="114"/>
+      <c r="A42" s="115"/>
+      <c r="B42" s="125"/>
+      <c r="C42" s="115"/>
     </row>
     <row r="43" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="114"/>
-      <c r="B43" s="105" t="s">
+      <c r="A43" s="115"/>
+      <c r="B43" s="106" t="s">
         <v>629</v>
       </c>
-      <c r="C43" s="114"/>
+      <c r="C43" s="115"/>
     </row>
     <row r="44" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="114"/>
-      <c r="B44" s="124"/>
-      <c r="C44" s="114"/>
+      <c r="A44" s="115"/>
+      <c r="B44" s="125"/>
+      <c r="C44" s="115"/>
     </row>
     <row r="45" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="114"/>
-      <c r="B45" s="124"/>
-      <c r="C45" s="114"/>
+      <c r="A45" s="115"/>
+      <c r="B45" s="125"/>
+      <c r="C45" s="115"/>
     </row>
     <row r="46" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="114"/>
-      <c r="B46" s="124"/>
-      <c r="C46" s="114"/>
+      <c r="A46" s="115"/>
+      <c r="B46" s="125"/>
+      <c r="C46" s="115"/>
     </row>
     <row r="47" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="114"/>
-      <c r="B47" s="124"/>
-      <c r="C47" s="114"/>
+      <c r="A47" s="115"/>
+      <c r="B47" s="125"/>
+      <c r="C47" s="115"/>
     </row>
     <row r="48" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="114"/>
-      <c r="B48" s="124"/>
-      <c r="C48" s="114"/>
+      <c r="A48" s="115"/>
+      <c r="B48" s="125"/>
+      <c r="C48" s="115"/>
     </row>
     <row r="49" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="114"/>
-      <c r="B49" s="124"/>
-      <c r="C49" s="114"/>
+      <c r="A49" s="115"/>
+      <c r="B49" s="125"/>
+      <c r="C49" s="115"/>
     </row>
     <row r="50" spans="1:3" ht="320" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="114"/>
-      <c r="B50" s="106"/>
-      <c r="C50" s="114"/>
+      <c r="A50" s="115"/>
+      <c r="B50" s="107"/>
+      <c r="C50" s="115"/>
     </row>
     <row r="51" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="114"/>
-      <c r="B51" s="105" t="s">
+      <c r="A51" s="115"/>
+      <c r="B51" s="106" t="s">
         <v>630</v>
       </c>
-      <c r="C51" s="114"/>
+      <c r="C51" s="115"/>
     </row>
     <row r="52" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="114"/>
-      <c r="B52" s="124"/>
-      <c r="C52" s="114"/>
+      <c r="A52" s="115"/>
+      <c r="B52" s="125"/>
+      <c r="C52" s="115"/>
     </row>
     <row r="53" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="114"/>
-      <c r="B53" s="124"/>
-      <c r="C53" s="114"/>
+      <c r="A53" s="115"/>
+      <c r="B53" s="125"/>
+      <c r="C53" s="115"/>
     </row>
     <row r="54" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="114"/>
-      <c r="B54" s="124"/>
-      <c r="C54" s="114"/>
+      <c r="A54" s="115"/>
+      <c r="B54" s="125"/>
+      <c r="C54" s="115"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="114"/>
-      <c r="B55" s="124"/>
-      <c r="C55" s="114"/>
+      <c r="A55" s="115"/>
+      <c r="B55" s="125"/>
+      <c r="C55" s="115"/>
     </row>
     <row r="56" spans="1:3" ht="97" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="114"/>
-      <c r="B56" s="106"/>
-      <c r="C56" s="114"/>
+      <c r="A56" s="115"/>
+      <c r="B56" s="107"/>
+      <c r="C56" s="115"/>
     </row>
     <row r="57" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="114"/>
-      <c r="B57" s="105" t="s">
+      <c r="A57" s="115"/>
+      <c r="B57" s="106" t="s">
         <v>631</v>
       </c>
-      <c r="C57" s="114"/>
+      <c r="C57" s="115"/>
     </row>
     <row r="58" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="114"/>
-      <c r="B58" s="124"/>
-      <c r="C58" s="114"/>
+      <c r="A58" s="115"/>
+      <c r="B58" s="125"/>
+      <c r="C58" s="115"/>
     </row>
     <row r="59" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="114"/>
-      <c r="B59" s="124"/>
-      <c r="C59" s="114"/>
+      <c r="A59" s="115"/>
+      <c r="B59" s="125"/>
+      <c r="C59" s="115"/>
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="114"/>
-      <c r="B60" s="124"/>
-      <c r="C60" s="114"/>
+      <c r="A60" s="115"/>
+      <c r="B60" s="125"/>
+      <c r="C60" s="115"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="114"/>
-      <c r="B61" s="124"/>
-      <c r="C61" s="114"/>
+      <c r="A61" s="115"/>
+      <c r="B61" s="125"/>
+      <c r="C61" s="115"/>
     </row>
     <row r="62" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="114"/>
-      <c r="B62" s="124"/>
-      <c r="C62" s="114"/>
+      <c r="A62" s="115"/>
+      <c r="B62" s="125"/>
+      <c r="C62" s="115"/>
     </row>
     <row r="63" spans="1:3" ht="146" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="114"/>
-      <c r="B63" s="106"/>
-      <c r="C63" s="114"/>
+      <c r="A63" s="115"/>
+      <c r="B63" s="107"/>
+      <c r="C63" s="115"/>
     </row>
     <row r="64" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="114"/>
-      <c r="B64" s="105" t="s">
+      <c r="A64" s="115"/>
+      <c r="B64" s="106" t="s">
         <v>632</v>
       </c>
-      <c r="C64" s="114"/>
+      <c r="C64" s="115"/>
     </row>
     <row r="65" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="104"/>
-      <c r="B65" s="106"/>
-      <c r="C65" s="104"/>
+      <c r="A65" s="105"/>
+      <c r="B65" s="107"/>
+      <c r="C65" s="105"/>
     </row>
     <row r="66" spans="1:3" ht="397" x14ac:dyDescent="0.2">
       <c r="A66" s="85" t="s">
@@ -23076,93 +23239,93 @@
       </c>
     </row>
     <row r="67" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="115" t="s">
+      <c r="A67" s="116" t="s">
         <v>638</v>
       </c>
-      <c r="B67" s="123" t="s">
+      <c r="B67" s="124" t="s">
         <v>637</v>
       </c>
-      <c r="C67" s="115" t="s">
+      <c r="C67" s="116" t="s">
         <v>639</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="115"/>
-      <c r="B68" s="123"/>
-      <c r="C68" s="115"/>
+      <c r="A68" s="116"/>
+      <c r="B68" s="124"/>
+      <c r="C68" s="116"/>
     </row>
     <row r="69" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="115"/>
-      <c r="B69" s="123"/>
-      <c r="C69" s="115"/>
+      <c r="A69" s="116"/>
+      <c r="B69" s="124"/>
+      <c r="C69" s="116"/>
     </row>
     <row r="70" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="115" t="s">
+      <c r="A70" s="116" t="s">
         <v>643</v>
       </c>
-      <c r="B70" s="123" t="s">
+      <c r="B70" s="124" t="s">
         <v>640</v>
       </c>
-      <c r="C70" s="115" t="s">
+      <c r="C70" s="116" t="s">
         <v>642</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="115"/>
-      <c r="B71" s="123"/>
-      <c r="C71" s="115"/>
+      <c r="A71" s="116"/>
+      <c r="B71" s="124"/>
+      <c r="C71" s="116"/>
     </row>
     <row r="72" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="115"/>
-      <c r="B72" s="123"/>
-      <c r="C72" s="115"/>
+      <c r="A72" s="116"/>
+      <c r="B72" s="124"/>
+      <c r="C72" s="116"/>
     </row>
     <row r="73" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="115"/>
-      <c r="B73" s="123"/>
-      <c r="C73" s="115"/>
+      <c r="A73" s="116"/>
+      <c r="B73" s="124"/>
+      <c r="C73" s="116"/>
     </row>
     <row r="74" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="115"/>
-      <c r="B74" s="123"/>
-      <c r="C74" s="115"/>
+      <c r="A74" s="116"/>
+      <c r="B74" s="124"/>
+      <c r="C74" s="116"/>
     </row>
     <row r="75" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="115"/>
-      <c r="B75" s="123"/>
-      <c r="C75" s="115"/>
+      <c r="A75" s="116"/>
+      <c r="B75" s="124"/>
+      <c r="C75" s="116"/>
     </row>
     <row r="76" spans="1:3" ht="214" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="115"/>
-      <c r="B76" s="123"/>
-      <c r="C76" s="115"/>
+      <c r="A76" s="116"/>
+      <c r="B76" s="124"/>
+      <c r="C76" s="116"/>
     </row>
     <row r="77" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="115"/>
-      <c r="B77" s="123" t="s">
+      <c r="A77" s="116"/>
+      <c r="B77" s="124" t="s">
         <v>641</v>
       </c>
-      <c r="C77" s="115"/>
+      <c r="C77" s="116"/>
     </row>
     <row r="78" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="115"/>
-      <c r="B78" s="123"/>
-      <c r="C78" s="115"/>
+      <c r="A78" s="116"/>
+      <c r="B78" s="124"/>
+      <c r="C78" s="116"/>
     </row>
     <row r="79" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="115"/>
-      <c r="B79" s="123"/>
-      <c r="C79" s="115"/>
+      <c r="A79" s="116"/>
+      <c r="B79" s="124"/>
+      <c r="C79" s="116"/>
     </row>
     <row r="80" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="115"/>
-      <c r="B80" s="123"/>
-      <c r="C80" s="115"/>
+      <c r="A80" s="116"/>
+      <c r="B80" s="124"/>
+      <c r="C80" s="116"/>
     </row>
     <row r="81" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="115"/>
-      <c r="B81" s="123"/>
-      <c r="C81" s="115"/>
+      <c r="A81" s="116"/>
+      <c r="B81" s="124"/>
+      <c r="C81" s="116"/>
     </row>
     <row r="82" spans="1:3" ht="56" x14ac:dyDescent="0.2">
       <c r="A82" s="82" t="s">
@@ -23209,40 +23372,40 @@
       </c>
     </row>
     <row r="86" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="103" t="s">
+      <c r="A86" s="104" t="s">
         <v>657</v>
       </c>
-      <c r="B86" s="108" t="s">
+      <c r="B86" s="109" t="s">
         <v>656</v>
       </c>
-      <c r="C86" s="103" t="s">
+      <c r="C86" s="104" t="s">
         <v>658</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="114"/>
-      <c r="B87" s="109"/>
-      <c r="C87" s="114"/>
+      <c r="A87" s="115"/>
+      <c r="B87" s="110"/>
+      <c r="C87" s="115"/>
     </row>
     <row r="88" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="114"/>
-      <c r="B88" s="109"/>
-      <c r="C88" s="114"/>
+      <c r="A88" s="115"/>
+      <c r="B88" s="110"/>
+      <c r="C88" s="115"/>
     </row>
     <row r="89" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="114"/>
-      <c r="B89" s="109"/>
-      <c r="C89" s="114"/>
+      <c r="A89" s="115"/>
+      <c r="B89" s="110"/>
+      <c r="C89" s="115"/>
     </row>
     <row r="90" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="114"/>
-      <c r="B90" s="109"/>
-      <c r="C90" s="114"/>
+      <c r="A90" s="115"/>
+      <c r="B90" s="110"/>
+      <c r="C90" s="115"/>
     </row>
     <row r="91" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="104"/>
-      <c r="B91" s="110"/>
-      <c r="C91" s="104"/>
+      <c r="A91" s="105"/>
+      <c r="B91" s="111"/>
+      <c r="C91" s="105"/>
     </row>
     <row r="92" spans="1:3" ht="221" x14ac:dyDescent="0.2">
       <c r="A92" s="16" t="s">
@@ -23321,18 +23484,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="108" t="s">
         <v>662</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -23379,40 +23542,40 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="104" t="s">
         <v>672</v>
       </c>
-      <c r="B7" s="108" t="s">
+      <c r="B7" s="109" t="s">
         <v>671</v>
       </c>
-      <c r="C7" s="103" t="s">
+      <c r="C7" s="104" t="s">
         <v>673</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="114"/>
-      <c r="B8" s="109"/>
-      <c r="C8" s="114"/>
+      <c r="A8" s="115"/>
+      <c r="B8" s="110"/>
+      <c r="C8" s="115"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="114"/>
-      <c r="B9" s="109"/>
-      <c r="C9" s="114"/>
+      <c r="A9" s="115"/>
+      <c r="B9" s="110"/>
+      <c r="C9" s="115"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="114"/>
-      <c r="B10" s="109"/>
-      <c r="C10" s="114"/>
+      <c r="A10" s="115"/>
+      <c r="B10" s="110"/>
+      <c r="C10" s="115"/>
     </row>
     <row r="11" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="114"/>
-      <c r="B11" s="109"/>
-      <c r="C11" s="114"/>
+      <c r="A11" s="115"/>
+      <c r="B11" s="110"/>
+      <c r="C11" s="115"/>
     </row>
     <row r="12" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="104"/>
-      <c r="B12" s="110"/>
-      <c r="C12" s="104"/>
+      <c r="A12" s="105"/>
+      <c r="B12" s="111"/>
+      <c r="C12" s="105"/>
     </row>
     <row r="13" spans="1:3" ht="210" x14ac:dyDescent="0.2">
       <c r="A13" s="87" t="s">
@@ -23477,18 +23640,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="108" t="s">
         <v>693</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -23592,7 +23755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{558F99C8-B50E-634F-9AF4-D2E4F23D35ED}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -23605,18 +23768,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="108" t="s">
         <v>697</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -23630,36 +23793,36 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="104" t="s">
         <v>698</v>
       </c>
-      <c r="B4" s="105" t="s">
+      <c r="B4" s="106" t="s">
         <v>700</v>
       </c>
-      <c r="C4" s="103" t="s">
+      <c r="C4" s="104" t="s">
         <v>699</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="136" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="104"/>
-      <c r="B5" s="106"/>
-      <c r="C5" s="104"/>
+      <c r="A5" s="105"/>
+      <c r="B5" s="107"/>
+      <c r="C5" s="105"/>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="103" t="s">
+      <c r="A6" s="104" t="s">
         <v>702</v>
       </c>
-      <c r="B6" s="108" t="s">
+      <c r="B6" s="109" t="s">
         <v>701</v>
       </c>
-      <c r="C6" s="103" t="s">
+      <c r="C6" s="104" t="s">
         <v>703</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="202" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="104"/>
-      <c r="B7" s="110"/>
-      <c r="C7" s="104"/>
+      <c r="A7" s="105"/>
+      <c r="B7" s="111"/>
+      <c r="C7" s="105"/>
     </row>
     <row r="8" spans="1:3" ht="168" x14ac:dyDescent="0.2">
       <c r="A8" s="98" t="s">
@@ -23738,7 +23901,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A15" s="98" t="s">
         <v>721</v>
       </c>
@@ -23750,20 +23913,20 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="103" t="s">
+      <c r="A16" s="104" t="s">
         <v>723</v>
       </c>
-      <c r="B16" s="108" t="s">
+      <c r="B16" s="109" t="s">
         <v>725</v>
       </c>
-      <c r="C16" s="103" t="s">
+      <c r="C16" s="104" t="s">
         <v>724</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="104"/>
-      <c r="B17" s="110"/>
-      <c r="C17" s="104"/>
+      <c r="A17" s="105"/>
+      <c r="B17" s="111"/>
+      <c r="C17" s="105"/>
     </row>
     <row r="18" spans="1:3" ht="148" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="98" t="s">
@@ -23834,18 +23997,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="108" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -23896,11 +24059,11 @@
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="107" t="s">
+      <c r="A9" s="108" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="107"/>
-      <c r="C9" s="107"/>
+      <c r="B9" s="108"/>
+      <c r="C9" s="108"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -23936,20 +24099,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="103" t="s">
+      <c r="A13" s="104" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="105" t="s">
+      <c r="B13" s="106" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="103" t="s">
+      <c r="C13" s="104" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="104"/>
-      <c r="B14" s="106"/>
-      <c r="C14" s="104"/>
+      <c r="A14" s="105"/>
+      <c r="B14" s="107"/>
+      <c r="C14" s="105"/>
     </row>
     <row r="15" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
@@ -23974,20 +24137,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="103" t="s">
+      <c r="A17" s="104" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="105" t="s">
+      <c r="B17" s="106" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="103" t="s">
+      <c r="C17" s="104" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="104"/>
-      <c r="B18" s="106"/>
-      <c r="C18" s="104"/>
+      <c r="A18" s="105"/>
+      <c r="B18" s="107"/>
+      <c r="C18" s="105"/>
     </row>
     <row r="19" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -24029,6 +24192,90 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62229E0A-4D65-3E41-A010-6397153A086D}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="102" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="108" t="s">
+        <v>731</v>
+      </c>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="238" x14ac:dyDescent="0.2">
+      <c r="A4" s="101" t="s">
+        <v>733</v>
+      </c>
+      <c r="B4" s="58" t="s">
+        <v>732</v>
+      </c>
+      <c r="C4" s="101" t="s">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="95" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="53" t="s">
+        <v>736</v>
+      </c>
+      <c r="C6" s="95" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE113606-3FFA-8545-9BE3-5643B52A7CE9}">
   <dimension ref="A1:H116"/>
   <sheetViews>
@@ -24106,10 +24353,10 @@
       <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="139" t="s">
+      <c r="A6" s="140" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="139"/>
+      <c r="B6" s="140"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -25082,32 +25329,32 @@
       <c r="H73" s="23"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="136"/>
-      <c r="B74" s="140"/>
+      <c r="A74" s="137"/>
+      <c r="B74" s="141"/>
       <c r="C74" s="32" t="s">
         <v>225</v>
       </c>
       <c r="D74" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="E74" s="141"/>
-      <c r="F74" s="136"/>
-      <c r="G74" s="138"/>
-      <c r="H74" s="136"/>
+      <c r="E74" s="142"/>
+      <c r="F74" s="137"/>
+      <c r="G74" s="139"/>
+      <c r="H74" s="137"/>
     </row>
     <row r="75" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A75" s="136"/>
-      <c r="B75" s="140"/>
+      <c r="A75" s="137"/>
+      <c r="B75" s="141"/>
       <c r="C75" s="33" t="s">
         <v>226</v>
       </c>
       <c r="D75" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="E75" s="141"/>
-      <c r="F75" s="136"/>
-      <c r="G75" s="138"/>
-      <c r="H75" s="136"/>
+      <c r="E75" s="142"/>
+      <c r="F75" s="137"/>
+      <c r="G75" s="139"/>
+      <c r="H75" s="137"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="23"/>
@@ -25280,34 +25527,34 @@
       <c r="H88" s="23"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="136"/>
-      <c r="B89" s="136"/>
+      <c r="A89" s="137"/>
+      <c r="B89" s="137"/>
       <c r="C89" s="35" t="s">
         <v>225</v>
       </c>
       <c r="D89" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="E89" s="137" t="s">
+      <c r="E89" s="138" t="s">
         <v>121</v>
       </c>
-      <c r="F89" s="137"/>
-      <c r="G89" s="138"/>
-      <c r="H89" s="136"/>
+      <c r="F89" s="138"/>
+      <c r="G89" s="139"/>
+      <c r="H89" s="137"/>
     </row>
     <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A90" s="136"/>
-      <c r="B90" s="136"/>
+      <c r="A90" s="137"/>
+      <c r="B90" s="137"/>
       <c r="C90" s="35" t="s">
         <v>242</v>
       </c>
       <c r="D90" s="35" t="s">
         <v>243</v>
       </c>
-      <c r="E90" s="137"/>
-      <c r="F90" s="137"/>
-      <c r="G90" s="138"/>
-      <c r="H90" s="136"/>
+      <c r="E90" s="138"/>
+      <c r="F90" s="138"/>
+      <c r="G90" s="139"/>
+      <c r="H90" s="137"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="23"/>
@@ -25693,7 +25940,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -25791,7 +26038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0BB7-C151-C94B-945C-E2CA92034B13}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -25808,18 +26055,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="108" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -25936,18 +26183,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="108" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -25983,25 +26230,25 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="103" t="s">
+      <c r="A6" s="104" t="s">
         <v>292</v>
       </c>
-      <c r="B6" s="108" t="s">
+      <c r="B6" s="109" t="s">
         <v>291</v>
       </c>
-      <c r="C6" s="103" t="s">
+      <c r="C6" s="104" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="114"/>
-      <c r="B7" s="109"/>
-      <c r="C7" s="114"/>
+      <c r="A7" s="115"/>
+      <c r="B7" s="110"/>
+      <c r="C7" s="115"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="104"/>
-      <c r="B8" s="110"/>
-      <c r="C8" s="104"/>
+      <c r="A8" s="105"/>
+      <c r="B8" s="111"/>
+      <c r="C8" s="105"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -26026,25 +26273,25 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="111" t="s">
+      <c r="A11" s="112" t="s">
         <v>294</v>
       </c>
-      <c r="B11" s="108" t="s">
+      <c r="B11" s="109" t="s">
         <v>295</v>
       </c>
-      <c r="C11" s="111" t="s">
+      <c r="C11" s="112" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="112"/>
-      <c r="B12" s="109"/>
-      <c r="C12" s="112"/>
+      <c r="A12" s="113"/>
+      <c r="B12" s="110"/>
+      <c r="C12" s="113"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="113"/>
-      <c r="B13" s="110"/>
-      <c r="C13" s="113"/>
+      <c r="A13" s="114"/>
+      <c r="B13" s="111"/>
+      <c r="C13" s="114"/>
     </row>
     <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
@@ -26101,18 +26348,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="108" t="s">
         <v>299</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -26126,46 +26373,46 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="115" t="s">
+      <c r="A4" s="116" t="s">
         <v>300</v>
       </c>
-      <c r="B4" s="119" t="s">
+      <c r="B4" s="120" t="s">
         <v>305</v>
       </c>
-      <c r="C4" s="115" t="s">
+      <c r="C4" s="116" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="115"/>
-      <c r="B5" s="119"/>
-      <c r="C5" s="115"/>
+      <c r="A5" s="116"/>
+      <c r="B5" s="120"/>
+      <c r="C5" s="116"/>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="115"/>
-      <c r="B6" s="119"/>
-      <c r="C6" s="115"/>
+      <c r="A6" s="116"/>
+      <c r="B6" s="120"/>
+      <c r="C6" s="116"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="104" t="s">
         <v>302</v>
       </c>
-      <c r="B7" s="116" t="s">
+      <c r="B7" s="117" t="s">
         <v>303</v>
       </c>
-      <c r="C7" s="103" t="s">
+      <c r="C7" s="104" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="114"/>
-      <c r="B8" s="117"/>
-      <c r="C8" s="114"/>
+      <c r="A8" s="115"/>
+      <c r="B8" s="118"/>
+      <c r="C8" s="115"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="228" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="104"/>
-      <c r="B9" s="118"/>
-      <c r="C9" s="104"/>
+      <c r="A9" s="105"/>
+      <c r="B9" s="119"/>
+      <c r="C9" s="105"/>
     </row>
     <row r="10" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
@@ -26222,18 +26469,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="108" t="s">
         <v>331</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -26280,233 +26527,233 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="103" t="s">
+      <c r="A7" s="104" t="s">
         <v>314</v>
       </c>
-      <c r="B7" s="108" t="s">
+      <c r="B7" s="109" t="s">
         <v>322</v>
       </c>
-      <c r="C7" s="103" t="s">
+      <c r="C7" s="104" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="114"/>
-      <c r="B8" s="109"/>
-      <c r="C8" s="114"/>
+      <c r="A8" s="115"/>
+      <c r="B8" s="110"/>
+      <c r="C8" s="115"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="114"/>
-      <c r="B9" s="109"/>
-      <c r="C9" s="114"/>
+      <c r="A9" s="115"/>
+      <c r="B9" s="110"/>
+      <c r="C9" s="115"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="114"/>
-      <c r="B10" s="109"/>
-      <c r="C10" s="114"/>
+      <c r="A10" s="115"/>
+      <c r="B10" s="110"/>
+      <c r="C10" s="115"/>
     </row>
     <row r="11" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="114"/>
-      <c r="B11" s="109"/>
-      <c r="C11" s="114"/>
+      <c r="A11" s="115"/>
+      <c r="B11" s="110"/>
+      <c r="C11" s="115"/>
     </row>
     <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="114"/>
-      <c r="B12" s="109"/>
-      <c r="C12" s="114"/>
+      <c r="A12" s="115"/>
+      <c r="B12" s="110"/>
+      <c r="C12" s="115"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="104"/>
-      <c r="B13" s="110"/>
-      <c r="C13" s="104"/>
+      <c r="A13" s="105"/>
+      <c r="B13" s="111"/>
+      <c r="C13" s="105"/>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="103" t="s">
+      <c r="A14" s="104" t="s">
         <v>325</v>
       </c>
-      <c r="B14" s="108" t="s">
+      <c r="B14" s="109" t="s">
         <v>323</v>
       </c>
-      <c r="C14" s="103" t="s">
+      <c r="C14" s="104" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="114"/>
-      <c r="B15" s="109"/>
-      <c r="C15" s="114"/>
+      <c r="A15" s="115"/>
+      <c r="B15" s="110"/>
+      <c r="C15" s="115"/>
     </row>
     <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="114"/>
-      <c r="B16" s="109"/>
-      <c r="C16" s="114"/>
+      <c r="A16" s="115"/>
+      <c r="B16" s="110"/>
+      <c r="C16" s="115"/>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="114"/>
-      <c r="B17" s="109"/>
-      <c r="C17" s="114"/>
+      <c r="A17" s="115"/>
+      <c r="B17" s="110"/>
+      <c r="C17" s="115"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="114"/>
-      <c r="B18" s="109"/>
-      <c r="C18" s="114"/>
+      <c r="A18" s="115"/>
+      <c r="B18" s="110"/>
+      <c r="C18" s="115"/>
     </row>
     <row r="19" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="114"/>
-      <c r="B19" s="109"/>
-      <c r="C19" s="114"/>
+      <c r="A19" s="115"/>
+      <c r="B19" s="110"/>
+      <c r="C19" s="115"/>
     </row>
     <row r="20" spans="1:3" ht="155" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="114"/>
-      <c r="B20" s="110"/>
-      <c r="C20" s="114"/>
+      <c r="A20" s="115"/>
+      <c r="B20" s="111"/>
+      <c r="C20" s="115"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="114"/>
-      <c r="B21" s="108" t="s">
+      <c r="A21" s="115"/>
+      <c r="B21" s="109" t="s">
         <v>316</v>
       </c>
-      <c r="C21" s="114"/>
+      <c r="C21" s="115"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="114"/>
-      <c r="B22" s="109"/>
-      <c r="C22" s="114"/>
+      <c r="A22" s="115"/>
+      <c r="B22" s="110"/>
+      <c r="C22" s="115"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="114"/>
-      <c r="B23" s="109"/>
-      <c r="C23" s="114"/>
+      <c r="A23" s="115"/>
+      <c r="B23" s="110"/>
+      <c r="C23" s="115"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="114"/>
-      <c r="B24" s="109"/>
-      <c r="C24" s="114"/>
+      <c r="A24" s="115"/>
+      <c r="B24" s="110"/>
+      <c r="C24" s="115"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="114"/>
-      <c r="B25" s="109"/>
-      <c r="C25" s="114"/>
+      <c r="A25" s="115"/>
+      <c r="B25" s="110"/>
+      <c r="C25" s="115"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="114"/>
-      <c r="B26" s="109"/>
-      <c r="C26" s="114"/>
+      <c r="A26" s="115"/>
+      <c r="B26" s="110"/>
+      <c r="C26" s="115"/>
     </row>
     <row r="27" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="114"/>
-      <c r="B27" s="110"/>
-      <c r="C27" s="114"/>
+      <c r="A27" s="115"/>
+      <c r="B27" s="111"/>
+      <c r="C27" s="115"/>
     </row>
     <row r="28" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="114"/>
-      <c r="B28" s="108" t="s">
+      <c r="A28" s="115"/>
+      <c r="B28" s="109" t="s">
         <v>317</v>
       </c>
-      <c r="C28" s="114"/>
+      <c r="C28" s="115"/>
     </row>
     <row r="29" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="114"/>
-      <c r="B29" s="109"/>
-      <c r="C29" s="114"/>
+      <c r="A29" s="115"/>
+      <c r="B29" s="110"/>
+      <c r="C29" s="115"/>
     </row>
     <row r="30" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="114"/>
-      <c r="B30" s="109"/>
-      <c r="C30" s="114"/>
+      <c r="A30" s="115"/>
+      <c r="B30" s="110"/>
+      <c r="C30" s="115"/>
     </row>
     <row r="31" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="114"/>
-      <c r="B31" s="109"/>
-      <c r="C31" s="114"/>
+      <c r="A31" s="115"/>
+      <c r="B31" s="110"/>
+      <c r="C31" s="115"/>
     </row>
     <row r="32" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="114"/>
-      <c r="B32" s="109"/>
-      <c r="C32" s="114"/>
+      <c r="A32" s="115"/>
+      <c r="B32" s="110"/>
+      <c r="C32" s="115"/>
     </row>
     <row r="33" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="114"/>
-      <c r="B33" s="109"/>
-      <c r="C33" s="114"/>
+      <c r="A33" s="115"/>
+      <c r="B33" s="110"/>
+      <c r="C33" s="115"/>
     </row>
     <row r="34" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="114"/>
-      <c r="B34" s="109"/>
-      <c r="C34" s="114"/>
+      <c r="A34" s="115"/>
+      <c r="B34" s="110"/>
+      <c r="C34" s="115"/>
     </row>
     <row r="35" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="114"/>
-      <c r="B35" s="109"/>
-      <c r="C35" s="114"/>
+      <c r="A35" s="115"/>
+      <c r="B35" s="110"/>
+      <c r="C35" s="115"/>
     </row>
     <row r="36" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="114"/>
-      <c r="B36" s="109"/>
-      <c r="C36" s="114"/>
+      <c r="A36" s="115"/>
+      <c r="B36" s="110"/>
+      <c r="C36" s="115"/>
     </row>
     <row r="37" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="114"/>
-      <c r="B37" s="110"/>
-      <c r="C37" s="114"/>
+      <c r="A37" s="115"/>
+      <c r="B37" s="111"/>
+      <c r="C37" s="115"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="114"/>
-      <c r="B38" s="108" t="s">
+      <c r="A38" s="115"/>
+      <c r="B38" s="109" t="s">
         <v>318</v>
       </c>
-      <c r="C38" s="114"/>
+      <c r="C38" s="115"/>
     </row>
     <row r="39" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="114"/>
-      <c r="B39" s="109"/>
-      <c r="C39" s="114"/>
+      <c r="A39" s="115"/>
+      <c r="B39" s="110"/>
+      <c r="C39" s="115"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="114"/>
-      <c r="B40" s="109"/>
-      <c r="C40" s="114"/>
+      <c r="A40" s="115"/>
+      <c r="B40" s="110"/>
+      <c r="C40" s="115"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="114"/>
-      <c r="B41" s="109"/>
-      <c r="C41" s="114"/>
+      <c r="A41" s="115"/>
+      <c r="B41" s="110"/>
+      <c r="C41" s="115"/>
     </row>
     <row r="42" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="104"/>
-      <c r="B42" s="110"/>
-      <c r="C42" s="104"/>
+      <c r="A42" s="105"/>
+      <c r="B42" s="111"/>
+      <c r="C42" s="105"/>
     </row>
     <row r="43" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="103" t="s">
+      <c r="A43" s="104" t="s">
         <v>326</v>
       </c>
-      <c r="B43" s="108" t="s">
+      <c r="B43" s="109" t="s">
         <v>327</v>
       </c>
-      <c r="C43" s="103" t="s">
+      <c r="C43" s="104" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="114"/>
-      <c r="B44" s="109"/>
-      <c r="C44" s="114"/>
+      <c r="A44" s="115"/>
+      <c r="B44" s="110"/>
+      <c r="C44" s="115"/>
     </row>
     <row r="45" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="114"/>
-      <c r="B45" s="109"/>
-      <c r="C45" s="114"/>
+      <c r="A45" s="115"/>
+      <c r="B45" s="110"/>
+      <c r="C45" s="115"/>
     </row>
     <row r="46" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="114"/>
-      <c r="B46" s="109"/>
-      <c r="C46" s="114"/>
+      <c r="A46" s="115"/>
+      <c r="B46" s="110"/>
+      <c r="C46" s="115"/>
     </row>
     <row r="47" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="104"/>
-      <c r="B47" s="110"/>
-      <c r="C47" s="104"/>
+      <c r="A47" s="105"/>
+      <c r="B47" s="111"/>
+      <c r="C47" s="105"/>
     </row>
     <row r="48" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
@@ -26569,18 +26816,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="108" t="s">
         <v>332</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -26719,18 +26966,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="108" t="s">
         <v>356</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -26814,18 +27061,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="108" t="s">
         <v>365</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -26850,20 +27097,20 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="104" t="s">
         <v>369</v>
       </c>
-      <c r="B5" s="120" t="s">
+      <c r="B5" s="121" t="s">
         <v>372</v>
       </c>
-      <c r="C5" s="103" t="s">
+      <c r="C5" s="104" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="104"/>
-      <c r="B6" s="122"/>
-      <c r="C6" s="104"/>
+      <c r="A6" s="105"/>
+      <c r="B6" s="123"/>
+      <c r="C6" s="105"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A7" s="59" t="s">
@@ -26877,67 +27124,67 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="103" t="s">
+      <c r="A8" s="104" t="s">
         <v>376</v>
       </c>
-      <c r="B8" s="120" t="s">
+      <c r="B8" s="121" t="s">
         <v>375</v>
       </c>
-      <c r="C8" s="103" t="s">
+      <c r="C8" s="104" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="114"/>
-      <c r="B9" s="121"/>
-      <c r="C9" s="114"/>
+      <c r="A9" s="115"/>
+      <c r="B9" s="122"/>
+      <c r="C9" s="115"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="104"/>
-      <c r="B10" s="122"/>
-      <c r="C10" s="104"/>
+      <c r="A10" s="105"/>
+      <c r="B10" s="123"/>
+      <c r="C10" s="105"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="103" t="s">
+      <c r="A11" s="104" t="s">
         <v>378</v>
       </c>
-      <c r="B11" s="120" t="s">
+      <c r="B11" s="121" t="s">
         <v>384</v>
       </c>
-      <c r="C11" s="103" t="s">
+      <c r="C11" s="104" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="114"/>
-      <c r="B12" s="121"/>
-      <c r="C12" s="114"/>
+      <c r="A12" s="115"/>
+      <c r="B12" s="122"/>
+      <c r="C12" s="115"/>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="187" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="104"/>
-      <c r="B13" s="122"/>
-      <c r="C13" s="104"/>
+      <c r="A13" s="105"/>
+      <c r="B13" s="123"/>
+      <c r="C13" s="105"/>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="103" t="s">
+      <c r="A14" s="104" t="s">
         <v>380</v>
       </c>
-      <c r="B14" s="120" t="s">
+      <c r="B14" s="121" t="s">
         <v>383</v>
       </c>
-      <c r="C14" s="103" t="s">
+      <c r="C14" s="104" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="114"/>
-      <c r="B15" s="121"/>
-      <c r="C15" s="114"/>
+      <c r="A15" s="115"/>
+      <c r="B15" s="122"/>
+      <c r="C15" s="115"/>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="104"/>
-      <c r="B16" s="122"/>
-      <c r="C16" s="104"/>
+      <c r="A16" s="105"/>
+      <c r="B16" s="123"/>
+      <c r="C16" s="105"/>
     </row>
     <row r="17" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
@@ -27000,18 +27247,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="107" t="s">
+      <c r="A2" s="108" t="s">
         <v>395</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -27034,217 +27281,217 @@
       <c r="C4" s="60"/>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="103" t="s">
+      <c r="A5" s="104" t="s">
         <v>397</v>
       </c>
-      <c r="B5" s="125" t="s">
+      <c r="B5" s="126" t="s">
         <v>396</v>
       </c>
-      <c r="C5" s="103" t="s">
+      <c r="C5" s="104" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="283" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="114"/>
-      <c r="B6" s="126"/>
-      <c r="C6" s="114"/>
+      <c r="A6" s="115"/>
+      <c r="B6" s="127"/>
+      <c r="C6" s="115"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="114"/>
-      <c r="B7" s="126"/>
-      <c r="C7" s="114"/>
+      <c r="A7" s="115"/>
+      <c r="B7" s="127"/>
+      <c r="C7" s="115"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="114"/>
-      <c r="B8" s="126"/>
-      <c r="C8" s="114"/>
+      <c r="A8" s="115"/>
+      <c r="B8" s="127"/>
+      <c r="C8" s="115"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="114"/>
-      <c r="B9" s="126"/>
-      <c r="C9" s="114"/>
+      <c r="A9" s="115"/>
+      <c r="B9" s="127"/>
+      <c r="C9" s="115"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="114"/>
-      <c r="B10" s="126"/>
-      <c r="C10" s="114"/>
+      <c r="A10" s="115"/>
+      <c r="B10" s="127"/>
+      <c r="C10" s="115"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="114"/>
-      <c r="B11" s="126"/>
-      <c r="C11" s="114"/>
+      <c r="A11" s="115"/>
+      <c r="B11" s="127"/>
+      <c r="C11" s="115"/>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="104"/>
-      <c r="B12" s="127"/>
-      <c r="C12" s="104"/>
+      <c r="A12" s="105"/>
+      <c r="B12" s="128"/>
+      <c r="C12" s="105"/>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="103" t="s">
+      <c r="A13" s="104" t="s">
         <v>399</v>
       </c>
-      <c r="B13" s="108" t="s">
+      <c r="B13" s="109" t="s">
         <v>400</v>
       </c>
-      <c r="C13" s="103" t="s">
+      <c r="C13" s="104" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="114"/>
-      <c r="B14" s="109"/>
-      <c r="C14" s="114"/>
+      <c r="A14" s="115"/>
+      <c r="B14" s="110"/>
+      <c r="C14" s="115"/>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="114"/>
-      <c r="B15" s="109"/>
-      <c r="C15" s="114"/>
+      <c r="A15" s="115"/>
+      <c r="B15" s="110"/>
+      <c r="C15" s="115"/>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="114"/>
-      <c r="B16" s="108" t="s">
+      <c r="A16" s="115"/>
+      <c r="B16" s="109" t="s">
         <v>401</v>
       </c>
-      <c r="C16" s="114"/>
+      <c r="C16" s="115"/>
     </row>
     <row r="17" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="114"/>
-      <c r="B17" s="109"/>
-      <c r="C17" s="114"/>
+      <c r="A17" s="115"/>
+      <c r="B17" s="110"/>
+      <c r="C17" s="115"/>
     </row>
     <row r="18" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="114"/>
-      <c r="B18" s="109"/>
-      <c r="C18" s="114"/>
+      <c r="A18" s="115"/>
+      <c r="B18" s="110"/>
+      <c r="C18" s="115"/>
     </row>
     <row r="19" spans="1:3" s="13" customFormat="1" ht="159" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="114"/>
-      <c r="B19" s="109"/>
-      <c r="C19" s="114"/>
+      <c r="A19" s="115"/>
+      <c r="B19" s="110"/>
+      <c r="C19" s="115"/>
     </row>
     <row r="20" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="114"/>
-      <c r="B20" s="109" t="s">
+      <c r="A20" s="115"/>
+      <c r="B20" s="110" t="s">
         <v>402</v>
       </c>
-      <c r="C20" s="114"/>
+      <c r="C20" s="115"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="114"/>
-      <c r="B21" s="109"/>
-      <c r="C21" s="114"/>
+      <c r="A21" s="115"/>
+      <c r="B21" s="110"/>
+      <c r="C21" s="115"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="114"/>
-      <c r="B22" s="109"/>
-      <c r="C22" s="114"/>
+      <c r="A22" s="115"/>
+      <c r="B22" s="110"/>
+      <c r="C22" s="115"/>
     </row>
     <row r="23" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="114"/>
-      <c r="B23" s="109"/>
-      <c r="C23" s="114"/>
+      <c r="A23" s="115"/>
+      <c r="B23" s="110"/>
+      <c r="C23" s="115"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="114"/>
-      <c r="B24" s="109" t="s">
+      <c r="A24" s="115"/>
+      <c r="B24" s="110" t="s">
         <v>403</v>
       </c>
-      <c r="C24" s="114"/>
+      <c r="C24" s="115"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="114"/>
-      <c r="B25" s="109"/>
-      <c r="C25" s="114"/>
+      <c r="A25" s="115"/>
+      <c r="B25" s="110"/>
+      <c r="C25" s="115"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="114"/>
-      <c r="B26" s="109" t="s">
+      <c r="A26" s="115"/>
+      <c r="B26" s="110" t="s">
         <v>317</v>
       </c>
-      <c r="C26" s="114"/>
+      <c r="C26" s="115"/>
     </row>
     <row r="27" spans="1:3" ht="144" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="114"/>
-      <c r="B27" s="109"/>
-      <c r="C27" s="114"/>
+      <c r="A27" s="115"/>
+      <c r="B27" s="110"/>
+      <c r="C27" s="115"/>
     </row>
     <row r="28" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="114"/>
-      <c r="B28" s="109" t="s">
+      <c r="A28" s="115"/>
+      <c r="B28" s="110" t="s">
         <v>404</v>
       </c>
-      <c r="C28" s="114"/>
+      <c r="C28" s="115"/>
     </row>
     <row r="29" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="114"/>
-      <c r="B29" s="109"/>
-      <c r="C29" s="114"/>
+      <c r="A29" s="115"/>
+      <c r="B29" s="110"/>
+      <c r="C29" s="115"/>
     </row>
     <row r="30" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="114"/>
-      <c r="B30" s="109"/>
-      <c r="C30" s="114"/>
+      <c r="A30" s="115"/>
+      <c r="B30" s="110"/>
+      <c r="C30" s="115"/>
     </row>
     <row r="31" spans="1:3" ht="196" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="114"/>
-      <c r="B31" s="109"/>
-      <c r="C31" s="114"/>
+      <c r="A31" s="115"/>
+      <c r="B31" s="110"/>
+      <c r="C31" s="115"/>
     </row>
     <row r="32" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="114"/>
-      <c r="B32" s="109" t="s">
+      <c r="A32" s="115"/>
+      <c r="B32" s="110" t="s">
         <v>405</v>
       </c>
-      <c r="C32" s="114"/>
+      <c r="C32" s="115"/>
     </row>
     <row r="33" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="114"/>
-      <c r="B33" s="109"/>
-      <c r="C33" s="114"/>
+      <c r="A33" s="115"/>
+      <c r="B33" s="110"/>
+      <c r="C33" s="115"/>
     </row>
     <row r="34" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="114"/>
-      <c r="B34" s="109"/>
-      <c r="C34" s="114"/>
+      <c r="A34" s="115"/>
+      <c r="B34" s="110"/>
+      <c r="C34" s="115"/>
     </row>
     <row r="35" spans="1:3" ht="201" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="114"/>
-      <c r="B35" s="109"/>
-      <c r="C35" s="114"/>
+      <c r="A35" s="115"/>
+      <c r="B35" s="110"/>
+      <c r="C35" s="115"/>
     </row>
     <row r="36" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="114"/>
-      <c r="B36" s="109" t="s">
+      <c r="A36" s="115"/>
+      <c r="B36" s="110" t="s">
         <v>406</v>
       </c>
-      <c r="C36" s="114"/>
+      <c r="C36" s="115"/>
     </row>
     <row r="37" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="114"/>
-      <c r="B37" s="109"/>
-      <c r="C37" s="114"/>
+      <c r="A37" s="115"/>
+      <c r="B37" s="110"/>
+      <c r="C37" s="115"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="114"/>
-      <c r="B38" s="109"/>
-      <c r="C38" s="114"/>
+      <c r="A38" s="115"/>
+      <c r="B38" s="110"/>
+      <c r="C38" s="115"/>
     </row>
     <row r="39" spans="1:3" ht="239" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="114"/>
-      <c r="B39" s="109"/>
-      <c r="C39" s="114"/>
+      <c r="A39" s="115"/>
+      <c r="B39" s="110"/>
+      <c r="C39" s="115"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="114"/>
-      <c r="B40" s="109" t="s">
+      <c r="A40" s="115"/>
+      <c r="B40" s="110" t="s">
         <v>407</v>
       </c>
-      <c r="C40" s="114"/>
+      <c r="C40" s="115"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="104"/>
-      <c r="B41" s="110"/>
-      <c r="C41" s="104"/>
+      <c r="A41" s="105"/>
+      <c r="B41" s="111"/>
+      <c r="C41" s="105"/>
     </row>
     <row r="42" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A42" s="60" t="s">
@@ -27284,11 +27531,11 @@
       <c r="C46" s="60"/>
     </row>
     <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A47" s="107" t="s">
+      <c r="A47" s="108" t="s">
         <v>386</v>
       </c>
-      <c r="B47" s="107"/>
-      <c r="C47" s="107"/>
+      <c r="B47" s="108"/>
+      <c r="C47" s="108"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
@@ -27302,25 +27549,25 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="103" t="s">
+      <c r="A49" s="104" t="s">
         <v>388</v>
       </c>
-      <c r="B49" s="105" t="s">
+      <c r="B49" s="106" t="s">
         <v>413</v>
       </c>
-      <c r="C49" s="103" t="s">
+      <c r="C49" s="104" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="114"/>
-      <c r="B50" s="124"/>
-      <c r="C50" s="114"/>
+      <c r="A50" s="115"/>
+      <c r="B50" s="125"/>
+      <c r="C50" s="115"/>
     </row>
     <row r="51" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="104"/>
-      <c r="B51" s="106"/>
-      <c r="C51" s="104"/>
+      <c r="A51" s="105"/>
+      <c r="B51" s="107"/>
+      <c r="C51" s="105"/>
     </row>
     <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="54" t="s">
@@ -27334,91 +27581,91 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="103" t="s">
+      <c r="A53" s="104" t="s">
         <v>415</v>
       </c>
-      <c r="B53" s="123" t="s">
+      <c r="B53" s="124" t="s">
         <v>416</v>
       </c>
-      <c r="C53" s="103" t="s">
+      <c r="C53" s="104" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="238" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="114"/>
-      <c r="B54" s="123"/>
-      <c r="C54" s="114"/>
+      <c r="A54" s="115"/>
+      <c r="B54" s="124"/>
+      <c r="C54" s="115"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="114"/>
-      <c r="B55" s="105" t="s">
+      <c r="A55" s="115"/>
+      <c r="B55" s="106" t="s">
         <v>417</v>
       </c>
-      <c r="C55" s="114"/>
+      <c r="C55" s="115"/>
     </row>
     <row r="56" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="114"/>
-      <c r="B56" s="124"/>
-      <c r="C56" s="114"/>
+      <c r="A56" s="115"/>
+      <c r="B56" s="125"/>
+      <c r="C56" s="115"/>
     </row>
     <row r="57" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="114"/>
-      <c r="B57" s="124"/>
-      <c r="C57" s="114"/>
+      <c r="A57" s="115"/>
+      <c r="B57" s="125"/>
+      <c r="C57" s="115"/>
     </row>
     <row r="58" spans="1:3" ht="172" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="114"/>
-      <c r="B58" s="106"/>
-      <c r="C58" s="114"/>
+      <c r="A58" s="115"/>
+      <c r="B58" s="107"/>
+      <c r="C58" s="115"/>
     </row>
     <row r="59" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="114"/>
-      <c r="B59" s="105" t="s">
+      <c r="A59" s="115"/>
+      <c r="B59" s="106" t="s">
         <v>418</v>
       </c>
-      <c r="C59" s="114"/>
+      <c r="C59" s="115"/>
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="114"/>
-      <c r="B60" s="124"/>
-      <c r="C60" s="114"/>
+      <c r="A60" s="115"/>
+      <c r="B60" s="125"/>
+      <c r="C60" s="115"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="114"/>
-      <c r="B61" s="124"/>
-      <c r="C61" s="114"/>
+      <c r="A61" s="115"/>
+      <c r="B61" s="125"/>
+      <c r="C61" s="115"/>
     </row>
     <row r="62" spans="1:3" ht="125" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="114"/>
-      <c r="B62" s="106"/>
-      <c r="C62" s="114"/>
+      <c r="A62" s="115"/>
+      <c r="B62" s="107"/>
+      <c r="C62" s="115"/>
     </row>
     <row r="63" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="114"/>
-      <c r="B63" s="105" t="s">
+      <c r="A63" s="115"/>
+      <c r="B63" s="106" t="s">
         <v>419</v>
       </c>
-      <c r="C63" s="114"/>
+      <c r="C63" s="115"/>
     </row>
     <row r="64" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="114"/>
-      <c r="B64" s="124"/>
-      <c r="C64" s="114"/>
+      <c r="A64" s="115"/>
+      <c r="B64" s="125"/>
+      <c r="C64" s="115"/>
     </row>
     <row r="65" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="114"/>
-      <c r="B65" s="124"/>
-      <c r="C65" s="114"/>
+      <c r="A65" s="115"/>
+      <c r="B65" s="125"/>
+      <c r="C65" s="115"/>
     </row>
     <row r="66" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="114"/>
-      <c r="B66" s="124"/>
-      <c r="C66" s="114"/>
+      <c r="A66" s="115"/>
+      <c r="B66" s="125"/>
+      <c r="C66" s="115"/>
     </row>
     <row r="67" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="104"/>
-      <c r="B67" s="106"/>
-      <c r="C67" s="104"/>
+      <c r="A67" s="105"/>
+      <c r="B67" s="107"/>
+      <c r="C67" s="105"/>
     </row>
     <row r="68" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A68" s="60" t="s">

</xml_diff>

<commit_message>
Updated the css/global.css and the css/lock-selection-survey.css∫ file to support smaller screens and and updated flex properties.
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC94819A-25B3-4C49-A30B-FDD63F4C0A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB713D6-017C-0B44-8D6E-2A834E4E6C1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16160" firstSheet="11" activeTab="19" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16160" firstSheet="11" activeTab="20" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="SPEC - 1.1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,10 @@
     <sheet name="SPEC - 3.3" sheetId="22" r:id="rId18"/>
     <sheet name="SPEC - 3.4" sheetId="23" r:id="rId19"/>
     <sheet name="SPEC - 3.5" sheetId="24" r:id="rId20"/>
-    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId21"/>
-    <sheet name="PLAYGROUND" sheetId="6" r:id="rId22"/>
-    <sheet name="TEMPLATE" sheetId="8" r:id="rId23"/>
+    <sheet name="SPEC - 3.6" sheetId="25" r:id="rId21"/>
+    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId22"/>
+    <sheet name="PLAYGROUND" sheetId="6" r:id="rId23"/>
+    <sheet name="TEMPLATE" sheetId="8" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1018" uniqueCount="764">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -20214,6 +20215,942 @@
         <family val="1"/>
       </rPr>
       <t>nothing to commit, working tree clean</t>
+    </r>
+  </si>
+  <si>
+    <t>UPDATE THE css/global.css AND css/lock-selection-survey.css CSS FILES TO SUPPORT PROPER FLEX LAYOUT AND SUPPORT SMALL SCREEN DEVICES</t>
+  </si>
+  <si>
+    <t>.card-fade-in {
+    flex-basis: 50%;
+    opacity: 1;
+    overflow: hidden;
+    transition: flex-basis 1s, opacity 3000ms;
+}
+/* Styling the flex cards - on screen sizes 768px and less */
+@media screen and (max-width: 768px) {
+    .card-fade-in {
+        flex-basis: 100%;
+        opacity: 1;
+        overflow: hidden;
+        transition: flex-basis 1s, opacity 3000ms;
+    }
+}</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">.card-fade-out {
+    flex-basis: 0px !important;
+    opacity: 0;
+    overflow: hidden;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">    max-height: 0;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>card-fade-in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> class and also attach </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>media query</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> for screen with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>size less than 768px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/global.css</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>card-fade-in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> class and also attach </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>media query</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> for screen with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>size less than 768px</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/global.css</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">card-fade-out </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">class in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">css/global.css </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">to ensure that the hidden card (flex-basis : 0) has a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">max-height </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> also 0 to prevent it from getting elongated due to width compression</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">card-fade-out </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">class in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">css/global.css </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">to ensure that the hidden card (flex-basis : 0) has a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">max-height </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> also 0 to prevent it from getting elongated due to width compression</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">/*****************************************************************************/
+/* INPUT TAGS - &lt;input&gt;                                                      */
+/*****************************************************************************/
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">input,
+textarea,
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">label {
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>font-size: calc(10px + (14 - 10) * ((100vw - 500px) / (1200 - 300))) !important;
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Add the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> label </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">tag to the dynamic font size css in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/lock-selection-survey.css</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Added the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> label </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">tag to the dynamic font size css in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/lock-selection-survey.css</t>
+    </r>
+  </si>
+  <si>
+    <t>/*****************************************************************************/
+/* SURVEY HEADING &lt;div&gt;                                                      */
+/*****************************************************************************/
+/* survey-heading page heading &lt;div&gt; */
+#survey-heading {
+    padding: 0 ! important;
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add styling to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>survey-heading</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;div&gt; in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/lock-selection-survey.css</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to have no padding</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Added styling to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>survey-heading</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;div&gt; in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/lock-selection-survey.css</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to have no padding</t>
+    </r>
+  </si>
+  <si>
+    <t>/* survey-body page body &lt;div&gt; */
+#survey-body {
+    display: flex;
+    align-items: flex-start;
+    justify-content: center;
+    flex-grow: 1;
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>survey-body</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;div&gt; in the file  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">css/lock-selection-survey.css </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">to have the style </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>align-flex: start</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> so that different cards have different heights - and not one standard height - equal to the card of maximum height</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>survey-body</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;div&gt; in the file  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">css/lock-selection-survey.css </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">to have the style </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>align-flex: start</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> so that different cards have different heights - and not one standard height - equal to the card of maximum height</t>
+    </r>
+  </si>
+  <si>
+    <t>/* Flex component to layout the cards inside the survey-body &lt;div&gt; */
+.flex-component {
+    box-shadow: 0 .5rem 1rem rgba(0, 0, 0, .15) !important;
+    margin-top: 25px;
+    margin-bottom: 25px;
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>flex-component</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> class in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/lock-selection-survey.css</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to have the basic common styles for all cards</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>flex-component</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> class in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/lock-selection-survey.css</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to have the basic common styles for all cards</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">git commit -m "Updated the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">css/global.css </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">and the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">css/lock-selection-survey.css∫ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>file to support smaller screens and and updated flex properties."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>git status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - would display the following files.                                                                                                                                                                                                                                  On branch master
+Your branch is up to date with 'hafele/master'.
+Changes to be committed:
+  (use "git restore --staged &lt;file&gt;..." to unstage)
+        modified:   css/global.css
+        modified:   css/lock-selection-survey.css
+        modified:   docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">On branch </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">master </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>nothing to commit, working tree clean</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Merge the changes in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">lock branch </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>to the master branch</t>
+    </r>
+  </si>
+  <si>
+    <t>git  merge lock</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">git branch </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">displays that the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">master </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>branch is the current branch.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">master </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>branch is upto date.</t>
     </r>
   </si>
 </sst>
@@ -20640,7 +21577,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -20897,6 +21834,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -21012,6 +21955,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -21342,18 +22291,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="105" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
+      <c r="B2" s="105"/>
+      <c r="C2" s="105"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -21638,18 +22587,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="110" t="s">
         <v>426</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -21663,7 +22612,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="129" t="s">
+      <c r="A4" s="131" t="s">
         <v>438</v>
       </c>
       <c r="B4" s="48" t="s">
@@ -21674,7 +22623,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="130"/>
+      <c r="A5" s="132"/>
       <c r="B5" s="48" t="s">
         <v>441</v>
       </c>
@@ -21683,51 +22632,51 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="130"/>
+      <c r="A6" s="132"/>
       <c r="B6" s="48" t="s">
         <v>434</v>
       </c>
-      <c r="C6" s="132" t="s">
+      <c r="C6" s="134" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="130"/>
+      <c r="A7" s="132"/>
       <c r="B7" s="48" t="s">
         <v>435</v>
       </c>
-      <c r="C7" s="133"/>
+      <c r="C7" s="135"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="130"/>
+      <c r="A8" s="132"/>
       <c r="B8" s="48" t="s">
         <v>427</v>
       </c>
-      <c r="C8" s="133"/>
+      <c r="C8" s="135"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="130"/>
+      <c r="A9" s="132"/>
       <c r="B9" s="48" t="s">
         <v>428</v>
       </c>
-      <c r="C9" s="133"/>
+      <c r="C9" s="135"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="130"/>
+      <c r="A10" s="132"/>
       <c r="B10" s="48" t="s">
         <v>436</v>
       </c>
-      <c r="C10" s="133"/>
+      <c r="C10" s="135"/>
     </row>
     <row r="11" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="130"/>
+      <c r="A11" s="132"/>
       <c r="B11" s="48" t="s">
         <v>443</v>
       </c>
-      <c r="C11" s="134"/>
+      <c r="C11" s="136"/>
     </row>
     <row r="12" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="131"/>
+      <c r="A12" s="133"/>
       <c r="B12" s="48" t="s">
         <v>445</v>
       </c>
@@ -21866,18 +22815,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="110" t="s">
         <v>464</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -21983,18 +22932,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="110" t="s">
         <v>478</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -22045,11 +22994,11 @@
       <c r="C8" s="54"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="108" t="s">
+      <c r="A9" s="110" t="s">
         <v>485</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="108"/>
+      <c r="B9" s="110"/>
+      <c r="C9" s="110"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -22085,20 +23034,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="104" t="s">
+      <c r="A13" s="106" t="s">
         <v>490</v>
       </c>
-      <c r="B13" s="109" t="s">
+      <c r="B13" s="111" t="s">
         <v>489</v>
       </c>
-      <c r="C13" s="104" t="s">
+      <c r="C13" s="106" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="105"/>
-      <c r="B14" s="111"/>
-      <c r="C14" s="105"/>
+      <c r="A14" s="107"/>
+      <c r="B14" s="113"/>
+      <c r="C14" s="107"/>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="73" t="s">
@@ -22123,20 +23072,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="104" t="s">
+      <c r="A17" s="106" t="s">
         <v>499</v>
       </c>
-      <c r="B17" s="109" t="s">
+      <c r="B17" s="111" t="s">
         <v>498</v>
       </c>
-      <c r="C17" s="104" t="s">
+      <c r="C17" s="106" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="222" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="105"/>
-      <c r="B18" s="111"/>
-      <c r="C18" s="105"/>
+      <c r="A18" s="107"/>
+      <c r="B18" s="113"/>
+      <c r="C18" s="107"/>
     </row>
     <row r="19" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -22194,18 +23143,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="110" t="s">
         <v>505</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -22263,25 +23212,25 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="104" t="s">
+      <c r="A8" s="106" t="s">
         <v>517</v>
       </c>
-      <c r="B8" s="109" t="s">
+      <c r="B8" s="111" t="s">
         <v>516</v>
       </c>
-      <c r="C8" s="104" t="s">
+      <c r="C8" s="106" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="115"/>
-      <c r="B9" s="110"/>
-      <c r="C9" s="115"/>
+      <c r="A9" s="117"/>
+      <c r="B9" s="112"/>
+      <c r="C9" s="117"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="105"/>
-      <c r="B10" s="111"/>
-      <c r="C10" s="105"/>
+      <c r="A10" s="107"/>
+      <c r="B10" s="113"/>
+      <c r="C10" s="107"/>
     </row>
     <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="54" t="s">
@@ -22295,86 +23244,86 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="104" t="s">
+      <c r="A12" s="106" t="s">
         <v>526</v>
       </c>
-      <c r="B12" s="109" t="s">
+      <c r="B12" s="111" t="s">
         <v>527</v>
       </c>
-      <c r="C12" s="104" t="s">
+      <c r="C12" s="106" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="115"/>
-      <c r="B13" s="110"/>
-      <c r="C13" s="115"/>
+      <c r="A13" s="117"/>
+      <c r="B13" s="112"/>
+      <c r="C13" s="117"/>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="115"/>
-      <c r="B14" s="110"/>
-      <c r="C14" s="115"/>
+      <c r="A14" s="117"/>
+      <c r="B14" s="112"/>
+      <c r="C14" s="117"/>
     </row>
     <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="115"/>
-      <c r="B15" s="110"/>
-      <c r="C15" s="115"/>
+      <c r="A15" s="117"/>
+      <c r="B15" s="112"/>
+      <c r="C15" s="117"/>
     </row>
     <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="115"/>
-      <c r="B16" s="110"/>
-      <c r="C16" s="115"/>
+      <c r="A16" s="117"/>
+      <c r="B16" s="112"/>
+      <c r="C16" s="117"/>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="115"/>
-      <c r="B17" s="110"/>
-      <c r="C17" s="115"/>
+      <c r="A17" s="117"/>
+      <c r="B17" s="112"/>
+      <c r="C17" s="117"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="105"/>
-      <c r="B18" s="110"/>
-      <c r="C18" s="105"/>
+      <c r="A18" s="107"/>
+      <c r="B18" s="112"/>
+      <c r="C18" s="107"/>
     </row>
     <row r="19" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="104" t="s">
+      <c r="A19" s="106" t="s">
         <v>529</v>
       </c>
-      <c r="B19" s="109" t="s">
+      <c r="B19" s="111" t="s">
         <v>528</v>
       </c>
-      <c r="C19" s="104" t="s">
+      <c r="C19" s="106" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="115"/>
-      <c r="B20" s="110"/>
-      <c r="C20" s="115"/>
+      <c r="A20" s="117"/>
+      <c r="B20" s="112"/>
+      <c r="C20" s="117"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="115"/>
-      <c r="B21" s="110"/>
-      <c r="C21" s="115"/>
+      <c r="A21" s="117"/>
+      <c r="B21" s="112"/>
+      <c r="C21" s="117"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="115"/>
-      <c r="B22" s="110"/>
-      <c r="C22" s="115"/>
+      <c r="A22" s="117"/>
+      <c r="B22" s="112"/>
+      <c r="C22" s="117"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="115"/>
-      <c r="B23" s="110"/>
-      <c r="C23" s="115"/>
+      <c r="A23" s="117"/>
+      <c r="B23" s="112"/>
+      <c r="C23" s="117"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="115"/>
-      <c r="B24" s="110"/>
-      <c r="C24" s="115"/>
+      <c r="A24" s="117"/>
+      <c r="B24" s="112"/>
+      <c r="C24" s="117"/>
     </row>
     <row r="25" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="105"/>
-      <c r="B25" s="111"/>
-      <c r="C25" s="105"/>
+      <c r="A25" s="107"/>
+      <c r="B25" s="113"/>
+      <c r="C25" s="107"/>
     </row>
     <row r="26" spans="1:3" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
@@ -22388,51 +23337,51 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="104" t="s">
+      <c r="A27" s="106" t="s">
         <v>533</v>
       </c>
-      <c r="B27" s="109" t="s">
+      <c r="B27" s="111" t="s">
         <v>532</v>
       </c>
-      <c r="C27" s="104" t="s">
+      <c r="C27" s="106" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="115"/>
-      <c r="B28" s="110"/>
-      <c r="C28" s="115"/>
+      <c r="A28" s="117"/>
+      <c r="B28" s="112"/>
+      <c r="C28" s="117"/>
     </row>
     <row r="29" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="105"/>
-      <c r="B29" s="111"/>
-      <c r="C29" s="105"/>
+      <c r="A29" s="107"/>
+      <c r="B29" s="113"/>
+      <c r="C29" s="107"/>
     </row>
     <row r="30" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="104" t="s">
+      <c r="A30" s="106" t="s">
         <v>536</v>
       </c>
-      <c r="B30" s="109" t="s">
+      <c r="B30" s="111" t="s">
         <v>535</v>
       </c>
-      <c r="C30" s="104" t="s">
+      <c r="C30" s="106" t="s">
         <v>537</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="115"/>
-      <c r="B31" s="110"/>
-      <c r="C31" s="115"/>
+      <c r="A31" s="117"/>
+      <c r="B31" s="112"/>
+      <c r="C31" s="117"/>
     </row>
     <row r="32" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="115"/>
-      <c r="B32" s="110"/>
-      <c r="C32" s="115"/>
+      <c r="A32" s="117"/>
+      <c r="B32" s="112"/>
+      <c r="C32" s="117"/>
     </row>
     <row r="33" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="105"/>
-      <c r="B33" s="111"/>
-      <c r="C33" s="105"/>
+      <c r="A33" s="107"/>
+      <c r="B33" s="113"/>
+      <c r="C33" s="107"/>
     </row>
     <row r="34" spans="1:3" ht="255" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
@@ -22498,18 +23447,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="110" t="s">
         <v>549</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -22604,18 +23553,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="110" t="s">
         <v>560</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -22677,11 +23626,11 @@
       <c r="C9" s="54"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="108" t="s">
+      <c r="A10" s="110" t="s">
         <v>575</v>
       </c>
-      <c r="B10" s="108"/>
-      <c r="C10" s="108"/>
+      <c r="B10" s="110"/>
+      <c r="C10" s="110"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
@@ -22797,18 +23746,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="110" t="s">
         <v>661</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -22866,20 +23815,20 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="104" t="s">
+      <c r="A8" s="106" t="s">
         <v>587</v>
       </c>
-      <c r="B8" s="109" t="s">
+      <c r="B8" s="111" t="s">
         <v>590</v>
       </c>
-      <c r="C8" s="104" t="s">
+      <c r="C8" s="106" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="109" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="105"/>
-      <c r="B9" s="111"/>
-      <c r="C9" s="105"/>
+      <c r="A9" s="107"/>
+      <c r="B9" s="113"/>
+      <c r="C9" s="107"/>
     </row>
     <row r="10" spans="1:3" ht="109" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="82" t="s">
@@ -22915,20 +23864,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="104" t="s">
+      <c r="A13" s="106" t="s">
         <v>603</v>
       </c>
-      <c r="B13" s="109" t="s">
+      <c r="B13" s="111" t="s">
         <v>602</v>
       </c>
-      <c r="C13" s="104" t="s">
+      <c r="C13" s="106" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="105"/>
-      <c r="B14" s="111"/>
-      <c r="C14" s="105"/>
+      <c r="A14" s="107"/>
+      <c r="B14" s="113"/>
+      <c r="C14" s="107"/>
     </row>
     <row r="15" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="82" t="s">
@@ -22942,67 +23891,67 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="136" t="s">
+      <c r="A16" s="138" t="s">
         <v>609</v>
       </c>
-      <c r="B16" s="135" t="s">
+      <c r="B16" s="137" t="s">
         <v>608</v>
       </c>
-      <c r="C16" s="136" t="s">
+      <c r="C16" s="138" t="s">
         <v>610</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="136"/>
-      <c r="B17" s="135"/>
-      <c r="C17" s="136"/>
+      <c r="A17" s="138"/>
+      <c r="B17" s="137"/>
+      <c r="C17" s="138"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="136"/>
-      <c r="B18" s="135"/>
-      <c r="C18" s="136"/>
+      <c r="A18" s="138"/>
+      <c r="B18" s="137"/>
+      <c r="C18" s="138"/>
     </row>
     <row r="19" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="136"/>
-      <c r="B19" s="135"/>
-      <c r="C19" s="136"/>
+      <c r="A19" s="138"/>
+      <c r="B19" s="137"/>
+      <c r="C19" s="138"/>
     </row>
     <row r="20" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="136"/>
-      <c r="B20" s="135"/>
-      <c r="C20" s="136"/>
+      <c r="A20" s="138"/>
+      <c r="B20" s="137"/>
+      <c r="C20" s="138"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="136"/>
-      <c r="B21" s="135"/>
-      <c r="C21" s="136"/>
+      <c r="A21" s="138"/>
+      <c r="B21" s="137"/>
+      <c r="C21" s="138"/>
     </row>
     <row r="22" spans="1:3" ht="139" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="136"/>
-      <c r="B22" s="135"/>
-      <c r="C22" s="136"/>
+      <c r="A22" s="138"/>
+      <c r="B22" s="137"/>
+      <c r="C22" s="138"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="136"/>
-      <c r="B23" s="135" t="s">
+      <c r="A23" s="138"/>
+      <c r="B23" s="137" t="s">
         <v>611</v>
       </c>
-      <c r="C23" s="136"/>
+      <c r="C23" s="138"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="136"/>
-      <c r="B24" s="135"/>
-      <c r="C24" s="136"/>
+      <c r="A24" s="138"/>
+      <c r="B24" s="137"/>
+      <c r="C24" s="138"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="136"/>
-      <c r="B25" s="135"/>
-      <c r="C25" s="136"/>
+      <c r="A25" s="138"/>
+      <c r="B25" s="137"/>
+      <c r="C25" s="138"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="136"/>
-      <c r="B26" s="135"/>
-      <c r="C26" s="136"/>
+      <c r="A26" s="138"/>
+      <c r="B26" s="137"/>
+      <c r="C26" s="138"/>
     </row>
     <row r="27" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="85" t="s">
@@ -23071,185 +24020,185 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="104" t="s">
+      <c r="A33" s="106" t="s">
         <v>633</v>
       </c>
-      <c r="B33" s="106" t="s">
+      <c r="B33" s="108" t="s">
         <v>627</v>
       </c>
-      <c r="C33" s="104" t="s">
+      <c r="C33" s="106" t="s">
         <v>633</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="115"/>
-      <c r="B34" s="127"/>
-      <c r="C34" s="115"/>
+      <c r="A34" s="117"/>
+      <c r="B34" s="129"/>
+      <c r="C34" s="117"/>
     </row>
     <row r="35" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="115"/>
-      <c r="B35" s="127"/>
-      <c r="C35" s="115"/>
+      <c r="A35" s="117"/>
+      <c r="B35" s="129"/>
+      <c r="C35" s="117"/>
     </row>
     <row r="36" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="115"/>
-      <c r="B36" s="107"/>
-      <c r="C36" s="115"/>
+      <c r="A36" s="117"/>
+      <c r="B36" s="109"/>
+      <c r="C36" s="117"/>
     </row>
     <row r="37" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="115"/>
-      <c r="B37" s="106" t="s">
+      <c r="A37" s="117"/>
+      <c r="B37" s="108" t="s">
         <v>628</v>
       </c>
-      <c r="C37" s="115"/>
+      <c r="C37" s="117"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="115"/>
-      <c r="B38" s="127"/>
-      <c r="C38" s="115"/>
+      <c r="A38" s="117"/>
+      <c r="B38" s="129"/>
+      <c r="C38" s="117"/>
     </row>
     <row r="39" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="115"/>
-      <c r="B39" s="127"/>
-      <c r="C39" s="115"/>
+      <c r="A39" s="117"/>
+      <c r="B39" s="129"/>
+      <c r="C39" s="117"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="115"/>
-      <c r="B40" s="127"/>
-      <c r="C40" s="115"/>
+      <c r="A40" s="117"/>
+      <c r="B40" s="129"/>
+      <c r="C40" s="117"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="115"/>
-      <c r="B41" s="127"/>
-      <c r="C41" s="115"/>
+      <c r="A41" s="117"/>
+      <c r="B41" s="129"/>
+      <c r="C41" s="117"/>
     </row>
     <row r="42" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="115"/>
-      <c r="B42" s="127"/>
-      <c r="C42" s="115"/>
+      <c r="A42" s="117"/>
+      <c r="B42" s="129"/>
+      <c r="C42" s="117"/>
     </row>
     <row r="43" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="115"/>
-      <c r="B43" s="106" t="s">
+      <c r="A43" s="117"/>
+      <c r="B43" s="108" t="s">
         <v>629</v>
       </c>
-      <c r="C43" s="115"/>
+      <c r="C43" s="117"/>
     </row>
     <row r="44" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="115"/>
-      <c r="B44" s="127"/>
-      <c r="C44" s="115"/>
+      <c r="A44" s="117"/>
+      <c r="B44" s="129"/>
+      <c r="C44" s="117"/>
     </row>
     <row r="45" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="115"/>
-      <c r="B45" s="127"/>
-      <c r="C45" s="115"/>
+      <c r="A45" s="117"/>
+      <c r="B45" s="129"/>
+      <c r="C45" s="117"/>
     </row>
     <row r="46" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="115"/>
-      <c r="B46" s="127"/>
-      <c r="C46" s="115"/>
+      <c r="A46" s="117"/>
+      <c r="B46" s="129"/>
+      <c r="C46" s="117"/>
     </row>
     <row r="47" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="115"/>
-      <c r="B47" s="127"/>
-      <c r="C47" s="115"/>
+      <c r="A47" s="117"/>
+      <c r="B47" s="129"/>
+      <c r="C47" s="117"/>
     </row>
     <row r="48" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="115"/>
-      <c r="B48" s="127"/>
-      <c r="C48" s="115"/>
+      <c r="A48" s="117"/>
+      <c r="B48" s="129"/>
+      <c r="C48" s="117"/>
     </row>
     <row r="49" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="115"/>
-      <c r="B49" s="127"/>
-      <c r="C49" s="115"/>
+      <c r="A49" s="117"/>
+      <c r="B49" s="129"/>
+      <c r="C49" s="117"/>
     </row>
     <row r="50" spans="1:3" ht="320" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="115"/>
-      <c r="B50" s="107"/>
-      <c r="C50" s="115"/>
+      <c r="A50" s="117"/>
+      <c r="B50" s="109"/>
+      <c r="C50" s="117"/>
     </row>
     <row r="51" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="115"/>
-      <c r="B51" s="106" t="s">
+      <c r="A51" s="117"/>
+      <c r="B51" s="108" t="s">
         <v>630</v>
       </c>
-      <c r="C51" s="115"/>
+      <c r="C51" s="117"/>
     </row>
     <row r="52" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="115"/>
-      <c r="B52" s="127"/>
-      <c r="C52" s="115"/>
+      <c r="A52" s="117"/>
+      <c r="B52" s="129"/>
+      <c r="C52" s="117"/>
     </row>
     <row r="53" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="115"/>
-      <c r="B53" s="127"/>
-      <c r="C53" s="115"/>
+      <c r="A53" s="117"/>
+      <c r="B53" s="129"/>
+      <c r="C53" s="117"/>
     </row>
     <row r="54" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="115"/>
-      <c r="B54" s="127"/>
-      <c r="C54" s="115"/>
+      <c r="A54" s="117"/>
+      <c r="B54" s="129"/>
+      <c r="C54" s="117"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="115"/>
-      <c r="B55" s="127"/>
-      <c r="C55" s="115"/>
+      <c r="A55" s="117"/>
+      <c r="B55" s="129"/>
+      <c r="C55" s="117"/>
     </row>
     <row r="56" spans="1:3" ht="97" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="115"/>
-      <c r="B56" s="107"/>
-      <c r="C56" s="115"/>
+      <c r="A56" s="117"/>
+      <c r="B56" s="109"/>
+      <c r="C56" s="117"/>
     </row>
     <row r="57" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="115"/>
-      <c r="B57" s="106" t="s">
+      <c r="A57" s="117"/>
+      <c r="B57" s="108" t="s">
         <v>631</v>
       </c>
-      <c r="C57" s="115"/>
+      <c r="C57" s="117"/>
     </row>
     <row r="58" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="115"/>
-      <c r="B58" s="127"/>
-      <c r="C58" s="115"/>
+      <c r="A58" s="117"/>
+      <c r="B58" s="129"/>
+      <c r="C58" s="117"/>
     </row>
     <row r="59" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="115"/>
-      <c r="B59" s="127"/>
-      <c r="C59" s="115"/>
+      <c r="A59" s="117"/>
+      <c r="B59" s="129"/>
+      <c r="C59" s="117"/>
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="115"/>
-      <c r="B60" s="127"/>
-      <c r="C60" s="115"/>
+      <c r="A60" s="117"/>
+      <c r="B60" s="129"/>
+      <c r="C60" s="117"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="115"/>
-      <c r="B61" s="127"/>
-      <c r="C61" s="115"/>
+      <c r="A61" s="117"/>
+      <c r="B61" s="129"/>
+      <c r="C61" s="117"/>
     </row>
     <row r="62" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="115"/>
-      <c r="B62" s="127"/>
-      <c r="C62" s="115"/>
+      <c r="A62" s="117"/>
+      <c r="B62" s="129"/>
+      <c r="C62" s="117"/>
     </row>
     <row r="63" spans="1:3" ht="146" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="115"/>
-      <c r="B63" s="107"/>
-      <c r="C63" s="115"/>
+      <c r="A63" s="117"/>
+      <c r="B63" s="109"/>
+      <c r="C63" s="117"/>
     </row>
     <row r="64" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="115"/>
-      <c r="B64" s="106" t="s">
+      <c r="A64" s="117"/>
+      <c r="B64" s="108" t="s">
         <v>632</v>
       </c>
-      <c r="C64" s="115"/>
+      <c r="C64" s="117"/>
     </row>
     <row r="65" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="105"/>
-      <c r="B65" s="107"/>
-      <c r="C65" s="105"/>
+      <c r="A65" s="107"/>
+      <c r="B65" s="109"/>
+      <c r="C65" s="107"/>
     </row>
     <row r="66" spans="1:3" ht="397" x14ac:dyDescent="0.2">
       <c r="A66" s="85" t="s">
@@ -23263,93 +24212,93 @@
       </c>
     </row>
     <row r="67" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="116" t="s">
+      <c r="A67" s="118" t="s">
         <v>638</v>
       </c>
-      <c r="B67" s="128" t="s">
+      <c r="B67" s="130" t="s">
         <v>637</v>
       </c>
-      <c r="C67" s="116" t="s">
+      <c r="C67" s="118" t="s">
         <v>639</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="116"/>
-      <c r="B68" s="128"/>
-      <c r="C68" s="116"/>
+      <c r="A68" s="118"/>
+      <c r="B68" s="130"/>
+      <c r="C68" s="118"/>
     </row>
     <row r="69" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="116"/>
-      <c r="B69" s="128"/>
-      <c r="C69" s="116"/>
+      <c r="A69" s="118"/>
+      <c r="B69" s="130"/>
+      <c r="C69" s="118"/>
     </row>
     <row r="70" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="116" t="s">
+      <c r="A70" s="118" t="s">
         <v>643</v>
       </c>
-      <c r="B70" s="128" t="s">
+      <c r="B70" s="130" t="s">
         <v>640</v>
       </c>
-      <c r="C70" s="116" t="s">
+      <c r="C70" s="118" t="s">
         <v>642</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="116"/>
-      <c r="B71" s="128"/>
-      <c r="C71" s="116"/>
+      <c r="A71" s="118"/>
+      <c r="B71" s="130"/>
+      <c r="C71" s="118"/>
     </row>
     <row r="72" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="116"/>
-      <c r="B72" s="128"/>
-      <c r="C72" s="116"/>
+      <c r="A72" s="118"/>
+      <c r="B72" s="130"/>
+      <c r="C72" s="118"/>
     </row>
     <row r="73" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="116"/>
-      <c r="B73" s="128"/>
-      <c r="C73" s="116"/>
+      <c r="A73" s="118"/>
+      <c r="B73" s="130"/>
+      <c r="C73" s="118"/>
     </row>
     <row r="74" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="116"/>
-      <c r="B74" s="128"/>
-      <c r="C74" s="116"/>
+      <c r="A74" s="118"/>
+      <c r="B74" s="130"/>
+      <c r="C74" s="118"/>
     </row>
     <row r="75" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="116"/>
-      <c r="B75" s="128"/>
-      <c r="C75" s="116"/>
+      <c r="A75" s="118"/>
+      <c r="B75" s="130"/>
+      <c r="C75" s="118"/>
     </row>
     <row r="76" spans="1:3" ht="214" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="116"/>
-      <c r="B76" s="128"/>
-      <c r="C76" s="116"/>
+      <c r="A76" s="118"/>
+      <c r="B76" s="130"/>
+      <c r="C76" s="118"/>
     </row>
     <row r="77" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="116"/>
-      <c r="B77" s="128" t="s">
+      <c r="A77" s="118"/>
+      <c r="B77" s="130" t="s">
         <v>641</v>
       </c>
-      <c r="C77" s="116"/>
+      <c r="C77" s="118"/>
     </row>
     <row r="78" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="116"/>
-      <c r="B78" s="128"/>
-      <c r="C78" s="116"/>
+      <c r="A78" s="118"/>
+      <c r="B78" s="130"/>
+      <c r="C78" s="118"/>
     </row>
     <row r="79" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="116"/>
-      <c r="B79" s="128"/>
-      <c r="C79" s="116"/>
+      <c r="A79" s="118"/>
+      <c r="B79" s="130"/>
+      <c r="C79" s="118"/>
     </row>
     <row r="80" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="116"/>
-      <c r="B80" s="128"/>
-      <c r="C80" s="116"/>
+      <c r="A80" s="118"/>
+      <c r="B80" s="130"/>
+      <c r="C80" s="118"/>
     </row>
     <row r="81" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="116"/>
-      <c r="B81" s="128"/>
-      <c r="C81" s="116"/>
+      <c r="A81" s="118"/>
+      <c r="B81" s="130"/>
+      <c r="C81" s="118"/>
     </row>
     <row r="82" spans="1:3" ht="56" x14ac:dyDescent="0.2">
       <c r="A82" s="82" t="s">
@@ -23396,40 +24345,40 @@
       </c>
     </row>
     <row r="86" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="104" t="s">
+      <c r="A86" s="106" t="s">
         <v>657</v>
       </c>
-      <c r="B86" s="109" t="s">
+      <c r="B86" s="111" t="s">
         <v>656</v>
       </c>
-      <c r="C86" s="104" t="s">
+      <c r="C86" s="106" t="s">
         <v>658</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="115"/>
-      <c r="B87" s="110"/>
-      <c r="C87" s="115"/>
+      <c r="A87" s="117"/>
+      <c r="B87" s="112"/>
+      <c r="C87" s="117"/>
     </row>
     <row r="88" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="115"/>
-      <c r="B88" s="110"/>
-      <c r="C88" s="115"/>
+      <c r="A88" s="117"/>
+      <c r="B88" s="112"/>
+      <c r="C88" s="117"/>
     </row>
     <row r="89" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="115"/>
-      <c r="B89" s="110"/>
-      <c r="C89" s="115"/>
+      <c r="A89" s="117"/>
+      <c r="B89" s="112"/>
+      <c r="C89" s="117"/>
     </row>
     <row r="90" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="115"/>
-      <c r="B90" s="110"/>
-      <c r="C90" s="115"/>
+      <c r="A90" s="117"/>
+      <c r="B90" s="112"/>
+      <c r="C90" s="117"/>
     </row>
     <row r="91" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="105"/>
-      <c r="B91" s="111"/>
-      <c r="C91" s="105"/>
+      <c r="A91" s="107"/>
+      <c r="B91" s="113"/>
+      <c r="C91" s="107"/>
     </row>
     <row r="92" spans="1:3" ht="221" x14ac:dyDescent="0.2">
       <c r="A92" s="16" t="s">
@@ -23508,18 +24457,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="110" t="s">
         <v>662</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -23566,40 +24515,40 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="106" t="s">
         <v>672</v>
       </c>
-      <c r="B7" s="109" t="s">
+      <c r="B7" s="111" t="s">
         <v>671</v>
       </c>
-      <c r="C7" s="104" t="s">
+      <c r="C7" s="106" t="s">
         <v>673</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="115"/>
-      <c r="B8" s="110"/>
-      <c r="C8" s="115"/>
+      <c r="A8" s="117"/>
+      <c r="B8" s="112"/>
+      <c r="C8" s="117"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="115"/>
-      <c r="B9" s="110"/>
-      <c r="C9" s="115"/>
+      <c r="A9" s="117"/>
+      <c r="B9" s="112"/>
+      <c r="C9" s="117"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="115"/>
-      <c r="B10" s="110"/>
-      <c r="C10" s="115"/>
+      <c r="A10" s="117"/>
+      <c r="B10" s="112"/>
+      <c r="C10" s="117"/>
     </row>
     <row r="11" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="115"/>
-      <c r="B11" s="110"/>
-      <c r="C11" s="115"/>
+      <c r="A11" s="117"/>
+      <c r="B11" s="112"/>
+      <c r="C11" s="117"/>
     </row>
     <row r="12" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="105"/>
-      <c r="B12" s="111"/>
-      <c r="C12" s="105"/>
+      <c r="A12" s="107"/>
+      <c r="B12" s="113"/>
+      <c r="C12" s="107"/>
     </row>
     <row r="13" spans="1:3" ht="210" x14ac:dyDescent="0.2">
       <c r="A13" s="87" t="s">
@@ -23664,18 +24613,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="110" t="s">
         <v>693</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -23792,18 +24741,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="110" t="s">
         <v>697</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -23817,36 +24766,36 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="104" t="s">
+      <c r="A4" s="106" t="s">
         <v>698</v>
       </c>
-      <c r="B4" s="106" t="s">
+      <c r="B4" s="108" t="s">
         <v>700</v>
       </c>
-      <c r="C4" s="104" t="s">
+      <c r="C4" s="106" t="s">
         <v>699</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="136" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="105"/>
-      <c r="B5" s="107"/>
-      <c r="C5" s="105"/>
+      <c r="A5" s="107"/>
+      <c r="B5" s="109"/>
+      <c r="C5" s="107"/>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="106" t="s">
         <v>702</v>
       </c>
-      <c r="B6" s="109" t="s">
+      <c r="B6" s="111" t="s">
         <v>701</v>
       </c>
-      <c r="C6" s="104" t="s">
+      <c r="C6" s="106" t="s">
         <v>703</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="202" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="105"/>
-      <c r="B7" s="111"/>
-      <c r="C7" s="105"/>
+      <c r="A7" s="107"/>
+      <c r="B7" s="113"/>
+      <c r="C7" s="107"/>
     </row>
     <row r="8" spans="1:3" ht="168" x14ac:dyDescent="0.2">
       <c r="A8" s="98" t="s">
@@ -23937,20 +24886,20 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="104" t="s">
+      <c r="A16" s="106" t="s">
         <v>723</v>
       </c>
-      <c r="B16" s="109" t="s">
+      <c r="B16" s="111" t="s">
         <v>725</v>
       </c>
-      <c r="C16" s="104" t="s">
+      <c r="C16" s="106" t="s">
         <v>724</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="105"/>
-      <c r="B17" s="111"/>
-      <c r="C17" s="105"/>
+      <c r="A17" s="107"/>
+      <c r="B17" s="113"/>
+      <c r="C17" s="107"/>
     </row>
     <row r="18" spans="1:3" ht="148" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="98" t="s">
@@ -24021,18 +24970,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="110" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -24083,11 +25032,11 @@
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="108" t="s">
+      <c r="A9" s="110" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="108"/>
-      <c r="C9" s="108"/>
+      <c r="B9" s="110"/>
+      <c r="C9" s="110"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -24123,20 +25072,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="104" t="s">
+      <c r="A13" s="106" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="106" t="s">
+      <c r="B13" s="108" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="104" t="s">
+      <c r="C13" s="106" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="105"/>
-      <c r="B14" s="107"/>
-      <c r="C14" s="105"/>
+      <c r="A14" s="107"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="107"/>
     </row>
     <row r="15" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
@@ -24161,20 +25110,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="104" t="s">
+      <c r="A17" s="106" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="106" t="s">
+      <c r="B17" s="108" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="104" t="s">
+      <c r="C17" s="106" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="105"/>
-      <c r="B18" s="107"/>
-      <c r="C18" s="105"/>
+      <c r="A18" s="107"/>
+      <c r="B18" s="109"/>
+      <c r="C18" s="107"/>
     </row>
     <row r="19" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -24219,7 +25168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62229E0A-4D65-3E41-A010-6397153A086D}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -24232,18 +25181,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="110" t="s">
         <v>731</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -24300,6 +25249,209 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7464107A-26B7-9E4B-BF6A-1216AAA32472}">
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="104" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="110" t="s">
+        <v>738</v>
+      </c>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="103" t="s">
+        <v>447</v>
+      </c>
+      <c r="B4" s="58" t="s">
+        <v>448</v>
+      </c>
+      <c r="C4" s="103" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="103" t="s">
+        <v>760</v>
+      </c>
+      <c r="B5" s="58" t="s">
+        <v>761</v>
+      </c>
+      <c r="C5" s="103" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="103"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="103"/>
+    </row>
+    <row r="7" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="145"/>
+      <c r="B7" s="146"/>
+      <c r="C7" s="145"/>
+    </row>
+    <row r="8" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="103"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="103"/>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="104" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="104"/>
+      <c r="C9" s="104"/>
+    </row>
+    <row r="10" spans="1:3" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A10" s="110" t="s">
+        <v>738</v>
+      </c>
+      <c r="B10" s="110"/>
+      <c r="C10" s="110"/>
+    </row>
+    <row r="11" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="13" customFormat="1" ht="323" x14ac:dyDescent="0.2">
+      <c r="A12" s="102" t="s">
+        <v>741</v>
+      </c>
+      <c r="B12" s="58" t="s">
+        <v>739</v>
+      </c>
+      <c r="C12" s="102" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A13" s="102" t="s">
+        <v>743</v>
+      </c>
+      <c r="B13" s="58" t="s">
+        <v>740</v>
+      </c>
+      <c r="C13" s="102" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="153" x14ac:dyDescent="0.2">
+      <c r="A14" s="102" t="s">
+        <v>746</v>
+      </c>
+      <c r="B14" s="58" t="s">
+        <v>745</v>
+      </c>
+      <c r="C14" s="102" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="136" x14ac:dyDescent="0.2">
+      <c r="A15" s="102" t="s">
+        <v>749</v>
+      </c>
+      <c r="B15" s="58" t="s">
+        <v>748</v>
+      </c>
+      <c r="C15" s="102" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="119" x14ac:dyDescent="0.2">
+      <c r="A16" s="102" t="s">
+        <v>752</v>
+      </c>
+      <c r="B16" s="58" t="s">
+        <v>751</v>
+      </c>
+      <c r="C16" s="102" t="s">
+        <v>753</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A17" s="102" t="s">
+        <v>755</v>
+      </c>
+      <c r="B17" s="58" t="s">
+        <v>754</v>
+      </c>
+      <c r="C17" s="102" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="170" x14ac:dyDescent="0.2">
+      <c r="A18" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A19" s="95" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="53" t="s">
+        <v>757</v>
+      </c>
+      <c r="C19" s="95" t="s">
+        <v>759</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE113606-3FFA-8545-9BE3-5643B52A7CE9}">
   <dimension ref="A1:H116"/>
   <sheetViews>
@@ -24377,10 +25529,10 @@
       <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="137" t="s">
+      <c r="A6" s="139" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="137"/>
+      <c r="B6" s="139"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -25353,32 +26505,32 @@
       <c r="H73" s="23"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="138"/>
-      <c r="B74" s="139"/>
+      <c r="A74" s="140"/>
+      <c r="B74" s="141"/>
       <c r="C74" s="32" t="s">
         <v>225</v>
       </c>
       <c r="D74" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="E74" s="140"/>
-      <c r="F74" s="138"/>
-      <c r="G74" s="142"/>
-      <c r="H74" s="138"/>
+      <c r="E74" s="142"/>
+      <c r="F74" s="140"/>
+      <c r="G74" s="144"/>
+      <c r="H74" s="140"/>
     </row>
     <row r="75" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A75" s="138"/>
-      <c r="B75" s="139"/>
+      <c r="A75" s="140"/>
+      <c r="B75" s="141"/>
       <c r="C75" s="33" t="s">
         <v>226</v>
       </c>
       <c r="D75" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="E75" s="140"/>
-      <c r="F75" s="138"/>
-      <c r="G75" s="142"/>
-      <c r="H75" s="138"/>
+      <c r="E75" s="142"/>
+      <c r="F75" s="140"/>
+      <c r="G75" s="144"/>
+      <c r="H75" s="140"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="23"/>
@@ -25551,34 +26703,34 @@
       <c r="H88" s="23"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="138"/>
-      <c r="B89" s="138"/>
+      <c r="A89" s="140"/>
+      <c r="B89" s="140"/>
       <c r="C89" s="35" t="s">
         <v>225</v>
       </c>
       <c r="D89" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="E89" s="141" t="s">
+      <c r="E89" s="143" t="s">
         <v>121</v>
       </c>
-      <c r="F89" s="141"/>
-      <c r="G89" s="142"/>
-      <c r="H89" s="138"/>
+      <c r="F89" s="143"/>
+      <c r="G89" s="144"/>
+      <c r="H89" s="140"/>
     </row>
     <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A90" s="138"/>
-      <c r="B90" s="138"/>
+      <c r="A90" s="140"/>
+      <c r="B90" s="140"/>
       <c r="C90" s="35" t="s">
         <v>242</v>
       </c>
       <c r="D90" s="35" t="s">
         <v>243</v>
       </c>
-      <c r="E90" s="141"/>
-      <c r="F90" s="141"/>
-      <c r="G90" s="142"/>
-      <c r="H90" s="138"/>
+      <c r="E90" s="143"/>
+      <c r="F90" s="143"/>
+      <c r="G90" s="144"/>
+      <c r="H90" s="140"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="23"/>
@@ -25964,7 +27116,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -26062,7 +27214,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0BB7-C151-C94B-945C-E2CA92034B13}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -26079,18 +27231,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="110" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -26207,18 +27359,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="110" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -26254,25 +27406,25 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="106" t="s">
         <v>292</v>
       </c>
-      <c r="B6" s="109" t="s">
+      <c r="B6" s="111" t="s">
         <v>291</v>
       </c>
-      <c r="C6" s="104" t="s">
+      <c r="C6" s="106" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="115"/>
-      <c r="B7" s="110"/>
-      <c r="C7" s="115"/>
+      <c r="A7" s="117"/>
+      <c r="B7" s="112"/>
+      <c r="C7" s="117"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="105"/>
-      <c r="B8" s="111"/>
-      <c r="C8" s="105"/>
+      <c r="A8" s="107"/>
+      <c r="B8" s="113"/>
+      <c r="C8" s="107"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -26297,25 +27449,25 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="112" t="s">
+      <c r="A11" s="114" t="s">
         <v>294</v>
       </c>
-      <c r="B11" s="109" t="s">
+      <c r="B11" s="111" t="s">
         <v>295</v>
       </c>
-      <c r="C11" s="112" t="s">
+      <c r="C11" s="114" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="113"/>
-      <c r="B12" s="110"/>
-      <c r="C12" s="113"/>
+      <c r="A12" s="115"/>
+      <c r="B12" s="112"/>
+      <c r="C12" s="115"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="114"/>
-      <c r="B13" s="111"/>
-      <c r="C13" s="114"/>
+      <c r="A13" s="116"/>
+      <c r="B13" s="113"/>
+      <c r="C13" s="116"/>
     </row>
     <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
@@ -26372,18 +27524,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="110" t="s">
         <v>299</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -26397,46 +27549,46 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="116" t="s">
+      <c r="A4" s="118" t="s">
         <v>300</v>
       </c>
-      <c r="B4" s="120" t="s">
+      <c r="B4" s="122" t="s">
         <v>305</v>
       </c>
-      <c r="C4" s="116" t="s">
+      <c r="C4" s="118" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="116"/>
-      <c r="B5" s="120"/>
-      <c r="C5" s="116"/>
+      <c r="A5" s="118"/>
+      <c r="B5" s="122"/>
+      <c r="C5" s="118"/>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="116"/>
-      <c r="B6" s="120"/>
-      <c r="C6" s="116"/>
+      <c r="A6" s="118"/>
+      <c r="B6" s="122"/>
+      <c r="C6" s="118"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="106" t="s">
         <v>302</v>
       </c>
-      <c r="B7" s="117" t="s">
+      <c r="B7" s="119" t="s">
         <v>303</v>
       </c>
-      <c r="C7" s="104" t="s">
+      <c r="C7" s="106" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="115"/>
-      <c r="B8" s="118"/>
-      <c r="C8" s="115"/>
+      <c r="A8" s="117"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="117"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="228" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="105"/>
-      <c r="B9" s="119"/>
-      <c r="C9" s="105"/>
+      <c r="A9" s="107"/>
+      <c r="B9" s="121"/>
+      <c r="C9" s="107"/>
     </row>
     <row r="10" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
@@ -26493,18 +27645,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="110" t="s">
         <v>331</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -26551,233 +27703,233 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="104" t="s">
+      <c r="A7" s="106" t="s">
         <v>314</v>
       </c>
-      <c r="B7" s="109" t="s">
+      <c r="B7" s="111" t="s">
         <v>322</v>
       </c>
-      <c r="C7" s="104" t="s">
+      <c r="C7" s="106" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="115"/>
-      <c r="B8" s="110"/>
-      <c r="C8" s="115"/>
+      <c r="A8" s="117"/>
+      <c r="B8" s="112"/>
+      <c r="C8" s="117"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="115"/>
-      <c r="B9" s="110"/>
-      <c r="C9" s="115"/>
+      <c r="A9" s="117"/>
+      <c r="B9" s="112"/>
+      <c r="C9" s="117"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="115"/>
-      <c r="B10" s="110"/>
-      <c r="C10" s="115"/>
+      <c r="A10" s="117"/>
+      <c r="B10" s="112"/>
+      <c r="C10" s="117"/>
     </row>
     <row r="11" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="115"/>
-      <c r="B11" s="110"/>
-      <c r="C11" s="115"/>
+      <c r="A11" s="117"/>
+      <c r="B11" s="112"/>
+      <c r="C11" s="117"/>
     </row>
     <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="115"/>
-      <c r="B12" s="110"/>
-      <c r="C12" s="115"/>
+      <c r="A12" s="117"/>
+      <c r="B12" s="112"/>
+      <c r="C12" s="117"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="105"/>
-      <c r="B13" s="111"/>
-      <c r="C13" s="105"/>
+      <c r="A13" s="107"/>
+      <c r="B13" s="113"/>
+      <c r="C13" s="107"/>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="104" t="s">
+      <c r="A14" s="106" t="s">
         <v>325</v>
       </c>
-      <c r="B14" s="109" t="s">
+      <c r="B14" s="111" t="s">
         <v>323</v>
       </c>
-      <c r="C14" s="104" t="s">
+      <c r="C14" s="106" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="115"/>
-      <c r="B15" s="110"/>
-      <c r="C15" s="115"/>
+      <c r="A15" s="117"/>
+      <c r="B15" s="112"/>
+      <c r="C15" s="117"/>
     </row>
     <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="115"/>
-      <c r="B16" s="110"/>
-      <c r="C16" s="115"/>
+      <c r="A16" s="117"/>
+      <c r="B16" s="112"/>
+      <c r="C16" s="117"/>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="115"/>
-      <c r="B17" s="110"/>
-      <c r="C17" s="115"/>
+      <c r="A17" s="117"/>
+      <c r="B17" s="112"/>
+      <c r="C17" s="117"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="115"/>
-      <c r="B18" s="110"/>
-      <c r="C18" s="115"/>
+      <c r="A18" s="117"/>
+      <c r="B18" s="112"/>
+      <c r="C18" s="117"/>
     </row>
     <row r="19" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="115"/>
-      <c r="B19" s="110"/>
-      <c r="C19" s="115"/>
+      <c r="A19" s="117"/>
+      <c r="B19" s="112"/>
+      <c r="C19" s="117"/>
     </row>
     <row r="20" spans="1:3" ht="155" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="115"/>
-      <c r="B20" s="111"/>
-      <c r="C20" s="115"/>
+      <c r="A20" s="117"/>
+      <c r="B20" s="113"/>
+      <c r="C20" s="117"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="115"/>
-      <c r="B21" s="109" t="s">
+      <c r="A21" s="117"/>
+      <c r="B21" s="111" t="s">
         <v>316</v>
       </c>
-      <c r="C21" s="115"/>
+      <c r="C21" s="117"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="115"/>
-      <c r="B22" s="110"/>
-      <c r="C22" s="115"/>
+      <c r="A22" s="117"/>
+      <c r="B22" s="112"/>
+      <c r="C22" s="117"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="115"/>
-      <c r="B23" s="110"/>
-      <c r="C23" s="115"/>
+      <c r="A23" s="117"/>
+      <c r="B23" s="112"/>
+      <c r="C23" s="117"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="115"/>
-      <c r="B24" s="110"/>
-      <c r="C24" s="115"/>
+      <c r="A24" s="117"/>
+      <c r="B24" s="112"/>
+      <c r="C24" s="117"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="115"/>
-      <c r="B25" s="110"/>
-      <c r="C25" s="115"/>
+      <c r="A25" s="117"/>
+      <c r="B25" s="112"/>
+      <c r="C25" s="117"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="115"/>
-      <c r="B26" s="110"/>
-      <c r="C26" s="115"/>
+      <c r="A26" s="117"/>
+      <c r="B26" s="112"/>
+      <c r="C26" s="117"/>
     </row>
     <row r="27" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="115"/>
-      <c r="B27" s="111"/>
-      <c r="C27" s="115"/>
+      <c r="A27" s="117"/>
+      <c r="B27" s="113"/>
+      <c r="C27" s="117"/>
     </row>
     <row r="28" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="115"/>
-      <c r="B28" s="109" t="s">
+      <c r="A28" s="117"/>
+      <c r="B28" s="111" t="s">
         <v>317</v>
       </c>
-      <c r="C28" s="115"/>
+      <c r="C28" s="117"/>
     </row>
     <row r="29" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="115"/>
-      <c r="B29" s="110"/>
-      <c r="C29" s="115"/>
+      <c r="A29" s="117"/>
+      <c r="B29" s="112"/>
+      <c r="C29" s="117"/>
     </row>
     <row r="30" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="115"/>
-      <c r="B30" s="110"/>
-      <c r="C30" s="115"/>
+      <c r="A30" s="117"/>
+      <c r="B30" s="112"/>
+      <c r="C30" s="117"/>
     </row>
     <row r="31" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="115"/>
-      <c r="B31" s="110"/>
-      <c r="C31" s="115"/>
+      <c r="A31" s="117"/>
+      <c r="B31" s="112"/>
+      <c r="C31" s="117"/>
     </row>
     <row r="32" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="115"/>
-      <c r="B32" s="110"/>
-      <c r="C32" s="115"/>
+      <c r="A32" s="117"/>
+      <c r="B32" s="112"/>
+      <c r="C32" s="117"/>
     </row>
     <row r="33" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="115"/>
-      <c r="B33" s="110"/>
-      <c r="C33" s="115"/>
+      <c r="A33" s="117"/>
+      <c r="B33" s="112"/>
+      <c r="C33" s="117"/>
     </row>
     <row r="34" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="115"/>
-      <c r="B34" s="110"/>
-      <c r="C34" s="115"/>
+      <c r="A34" s="117"/>
+      <c r="B34" s="112"/>
+      <c r="C34" s="117"/>
     </row>
     <row r="35" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="115"/>
-      <c r="B35" s="110"/>
-      <c r="C35" s="115"/>
+      <c r="A35" s="117"/>
+      <c r="B35" s="112"/>
+      <c r="C35" s="117"/>
     </row>
     <row r="36" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="115"/>
-      <c r="B36" s="110"/>
-      <c r="C36" s="115"/>
+      <c r="A36" s="117"/>
+      <c r="B36" s="112"/>
+      <c r="C36" s="117"/>
     </row>
     <row r="37" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="115"/>
-      <c r="B37" s="111"/>
-      <c r="C37" s="115"/>
+      <c r="A37" s="117"/>
+      <c r="B37" s="113"/>
+      <c r="C37" s="117"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="115"/>
-      <c r="B38" s="109" t="s">
+      <c r="A38" s="117"/>
+      <c r="B38" s="111" t="s">
         <v>318</v>
       </c>
-      <c r="C38" s="115"/>
+      <c r="C38" s="117"/>
     </row>
     <row r="39" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="115"/>
-      <c r="B39" s="110"/>
-      <c r="C39" s="115"/>
+      <c r="A39" s="117"/>
+      <c r="B39" s="112"/>
+      <c r="C39" s="117"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="115"/>
-      <c r="B40" s="110"/>
-      <c r="C40" s="115"/>
+      <c r="A40" s="117"/>
+      <c r="B40" s="112"/>
+      <c r="C40" s="117"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="115"/>
-      <c r="B41" s="110"/>
-      <c r="C41" s="115"/>
+      <c r="A41" s="117"/>
+      <c r="B41" s="112"/>
+      <c r="C41" s="117"/>
     </row>
     <row r="42" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="105"/>
-      <c r="B42" s="111"/>
-      <c r="C42" s="105"/>
+      <c r="A42" s="107"/>
+      <c r="B42" s="113"/>
+      <c r="C42" s="107"/>
     </row>
     <row r="43" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="104" t="s">
+      <c r="A43" s="106" t="s">
         <v>326</v>
       </c>
-      <c r="B43" s="109" t="s">
+      <c r="B43" s="111" t="s">
         <v>327</v>
       </c>
-      <c r="C43" s="104" t="s">
+      <c r="C43" s="106" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="115"/>
-      <c r="B44" s="110"/>
-      <c r="C44" s="115"/>
+      <c r="A44" s="117"/>
+      <c r="B44" s="112"/>
+      <c r="C44" s="117"/>
     </row>
     <row r="45" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="115"/>
-      <c r="B45" s="110"/>
-      <c r="C45" s="115"/>
+      <c r="A45" s="117"/>
+      <c r="B45" s="112"/>
+      <c r="C45" s="117"/>
     </row>
     <row r="46" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="115"/>
-      <c r="B46" s="110"/>
-      <c r="C46" s="115"/>
+      <c r="A46" s="117"/>
+      <c r="B46" s="112"/>
+      <c r="C46" s="117"/>
     </row>
     <row r="47" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="105"/>
-      <c r="B47" s="111"/>
-      <c r="C47" s="105"/>
+      <c r="A47" s="107"/>
+      <c r="B47" s="113"/>
+      <c r="C47" s="107"/>
     </row>
     <row r="48" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
@@ -26840,18 +27992,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="110" t="s">
         <v>332</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -26990,18 +28142,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="110" t="s">
         <v>356</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -27085,18 +28237,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="110" t="s">
         <v>365</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -27121,20 +28273,20 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="104" t="s">
+      <c r="A5" s="106" t="s">
         <v>369</v>
       </c>
-      <c r="B5" s="121" t="s">
+      <c r="B5" s="123" t="s">
         <v>372</v>
       </c>
-      <c r="C5" s="104" t="s">
+      <c r="C5" s="106" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="105"/>
-      <c r="B6" s="123"/>
-      <c r="C6" s="105"/>
+      <c r="A6" s="107"/>
+      <c r="B6" s="125"/>
+      <c r="C6" s="107"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A7" s="59" t="s">
@@ -27148,67 +28300,67 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="104" t="s">
+      <c r="A8" s="106" t="s">
         <v>376</v>
       </c>
-      <c r="B8" s="121" t="s">
+      <c r="B8" s="123" t="s">
         <v>375</v>
       </c>
-      <c r="C8" s="104" t="s">
+      <c r="C8" s="106" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="115"/>
-      <c r="B9" s="122"/>
-      <c r="C9" s="115"/>
+      <c r="A9" s="117"/>
+      <c r="B9" s="124"/>
+      <c r="C9" s="117"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="105"/>
-      <c r="B10" s="123"/>
-      <c r="C10" s="105"/>
+      <c r="A10" s="107"/>
+      <c r="B10" s="125"/>
+      <c r="C10" s="107"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="104" t="s">
+      <c r="A11" s="106" t="s">
         <v>378</v>
       </c>
-      <c r="B11" s="121" t="s">
+      <c r="B11" s="123" t="s">
         <v>384</v>
       </c>
-      <c r="C11" s="104" t="s">
+      <c r="C11" s="106" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="115"/>
-      <c r="B12" s="122"/>
-      <c r="C12" s="115"/>
+      <c r="A12" s="117"/>
+      <c r="B12" s="124"/>
+      <c r="C12" s="117"/>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="187" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="105"/>
-      <c r="B13" s="123"/>
-      <c r="C13" s="105"/>
+      <c r="A13" s="107"/>
+      <c r="B13" s="125"/>
+      <c r="C13" s="107"/>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="104" t="s">
+      <c r="A14" s="106" t="s">
         <v>380</v>
       </c>
-      <c r="B14" s="121" t="s">
+      <c r="B14" s="123" t="s">
         <v>383</v>
       </c>
-      <c r="C14" s="104" t="s">
+      <c r="C14" s="106" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="115"/>
-      <c r="B15" s="122"/>
-      <c r="C15" s="115"/>
+      <c r="A15" s="117"/>
+      <c r="B15" s="124"/>
+      <c r="C15" s="117"/>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="105"/>
-      <c r="B16" s="123"/>
-      <c r="C16" s="105"/>
+      <c r="A16" s="107"/>
+      <c r="B16" s="125"/>
+      <c r="C16" s="107"/>
     </row>
     <row r="17" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
@@ -27271,18 +28423,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
+      <c r="A1" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="110" t="s">
         <v>395</v>
       </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
+      <c r="B2" s="110"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -27305,217 +28457,217 @@
       <c r="C4" s="60"/>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="104" t="s">
+      <c r="A5" s="106" t="s">
         <v>397</v>
       </c>
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="126" t="s">
         <v>396</v>
       </c>
-      <c r="C5" s="104" t="s">
+      <c r="C5" s="106" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="283" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="115"/>
-      <c r="B6" s="125"/>
-      <c r="C6" s="115"/>
+      <c r="A6" s="117"/>
+      <c r="B6" s="127"/>
+      <c r="C6" s="117"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="115"/>
-      <c r="B7" s="125"/>
-      <c r="C7" s="115"/>
+      <c r="A7" s="117"/>
+      <c r="B7" s="127"/>
+      <c r="C7" s="117"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="115"/>
-      <c r="B8" s="125"/>
-      <c r="C8" s="115"/>
+      <c r="A8" s="117"/>
+      <c r="B8" s="127"/>
+      <c r="C8" s="117"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="115"/>
-      <c r="B9" s="125"/>
-      <c r="C9" s="115"/>
+      <c r="A9" s="117"/>
+      <c r="B9" s="127"/>
+      <c r="C9" s="117"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="115"/>
-      <c r="B10" s="125"/>
-      <c r="C10" s="115"/>
+      <c r="A10" s="117"/>
+      <c r="B10" s="127"/>
+      <c r="C10" s="117"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="115"/>
-      <c r="B11" s="125"/>
-      <c r="C11" s="115"/>
+      <c r="A11" s="117"/>
+      <c r="B11" s="127"/>
+      <c r="C11" s="117"/>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="105"/>
-      <c r="B12" s="126"/>
-      <c r="C12" s="105"/>
+      <c r="A12" s="107"/>
+      <c r="B12" s="128"/>
+      <c r="C12" s="107"/>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="104" t="s">
+      <c r="A13" s="106" t="s">
         <v>399</v>
       </c>
-      <c r="B13" s="109" t="s">
+      <c r="B13" s="111" t="s">
         <v>400</v>
       </c>
-      <c r="C13" s="104" t="s">
+      <c r="C13" s="106" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="115"/>
-      <c r="B14" s="110"/>
-      <c r="C14" s="115"/>
+      <c r="A14" s="117"/>
+      <c r="B14" s="112"/>
+      <c r="C14" s="117"/>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="115"/>
-      <c r="B15" s="110"/>
-      <c r="C15" s="115"/>
+      <c r="A15" s="117"/>
+      <c r="B15" s="112"/>
+      <c r="C15" s="117"/>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="115"/>
-      <c r="B16" s="109" t="s">
+      <c r="A16" s="117"/>
+      <c r="B16" s="111" t="s">
         <v>401</v>
       </c>
-      <c r="C16" s="115"/>
+      <c r="C16" s="117"/>
     </row>
     <row r="17" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="115"/>
-      <c r="B17" s="110"/>
-      <c r="C17" s="115"/>
+      <c r="A17" s="117"/>
+      <c r="B17" s="112"/>
+      <c r="C17" s="117"/>
     </row>
     <row r="18" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="115"/>
-      <c r="B18" s="110"/>
-      <c r="C18" s="115"/>
+      <c r="A18" s="117"/>
+      <c r="B18" s="112"/>
+      <c r="C18" s="117"/>
     </row>
     <row r="19" spans="1:3" s="13" customFormat="1" ht="159" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="115"/>
-      <c r="B19" s="110"/>
-      <c r="C19" s="115"/>
+      <c r="A19" s="117"/>
+      <c r="B19" s="112"/>
+      <c r="C19" s="117"/>
     </row>
     <row r="20" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="115"/>
-      <c r="B20" s="110" t="s">
+      <c r="A20" s="117"/>
+      <c r="B20" s="112" t="s">
         <v>402</v>
       </c>
-      <c r="C20" s="115"/>
+      <c r="C20" s="117"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="115"/>
-      <c r="B21" s="110"/>
-      <c r="C21" s="115"/>
+      <c r="A21" s="117"/>
+      <c r="B21" s="112"/>
+      <c r="C21" s="117"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="115"/>
-      <c r="B22" s="110"/>
-      <c r="C22" s="115"/>
+      <c r="A22" s="117"/>
+      <c r="B22" s="112"/>
+      <c r="C22" s="117"/>
     </row>
     <row r="23" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="115"/>
-      <c r="B23" s="110"/>
-      <c r="C23" s="115"/>
+      <c r="A23" s="117"/>
+      <c r="B23" s="112"/>
+      <c r="C23" s="117"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="115"/>
-      <c r="B24" s="110" t="s">
+      <c r="A24" s="117"/>
+      <c r="B24" s="112" t="s">
         <v>403</v>
       </c>
-      <c r="C24" s="115"/>
+      <c r="C24" s="117"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="115"/>
-      <c r="B25" s="110"/>
-      <c r="C25" s="115"/>
+      <c r="A25" s="117"/>
+      <c r="B25" s="112"/>
+      <c r="C25" s="117"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="115"/>
-      <c r="B26" s="110" t="s">
+      <c r="A26" s="117"/>
+      <c r="B26" s="112" t="s">
         <v>317</v>
       </c>
-      <c r="C26" s="115"/>
+      <c r="C26" s="117"/>
     </row>
     <row r="27" spans="1:3" ht="144" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="115"/>
-      <c r="B27" s="110"/>
-      <c r="C27" s="115"/>
+      <c r="A27" s="117"/>
+      <c r="B27" s="112"/>
+      <c r="C27" s="117"/>
     </row>
     <row r="28" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="115"/>
-      <c r="B28" s="110" t="s">
+      <c r="A28" s="117"/>
+      <c r="B28" s="112" t="s">
         <v>404</v>
       </c>
-      <c r="C28" s="115"/>
+      <c r="C28" s="117"/>
     </row>
     <row r="29" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="115"/>
-      <c r="B29" s="110"/>
-      <c r="C29" s="115"/>
+      <c r="A29" s="117"/>
+      <c r="B29" s="112"/>
+      <c r="C29" s="117"/>
     </row>
     <row r="30" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="115"/>
-      <c r="B30" s="110"/>
-      <c r="C30" s="115"/>
+      <c r="A30" s="117"/>
+      <c r="B30" s="112"/>
+      <c r="C30" s="117"/>
     </row>
     <row r="31" spans="1:3" ht="196" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="115"/>
-      <c r="B31" s="110"/>
-      <c r="C31" s="115"/>
+      <c r="A31" s="117"/>
+      <c r="B31" s="112"/>
+      <c r="C31" s="117"/>
     </row>
     <row r="32" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="115"/>
-      <c r="B32" s="110" t="s">
+      <c r="A32" s="117"/>
+      <c r="B32" s="112" t="s">
         <v>405</v>
       </c>
-      <c r="C32" s="115"/>
+      <c r="C32" s="117"/>
     </row>
     <row r="33" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="115"/>
-      <c r="B33" s="110"/>
-      <c r="C33" s="115"/>
+      <c r="A33" s="117"/>
+      <c r="B33" s="112"/>
+      <c r="C33" s="117"/>
     </row>
     <row r="34" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="115"/>
-      <c r="B34" s="110"/>
-      <c r="C34" s="115"/>
+      <c r="A34" s="117"/>
+      <c r="B34" s="112"/>
+      <c r="C34" s="117"/>
     </row>
     <row r="35" spans="1:3" ht="201" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="115"/>
-      <c r="B35" s="110"/>
-      <c r="C35" s="115"/>
+      <c r="A35" s="117"/>
+      <c r="B35" s="112"/>
+      <c r="C35" s="117"/>
     </row>
     <row r="36" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="115"/>
-      <c r="B36" s="110" t="s">
+      <c r="A36" s="117"/>
+      <c r="B36" s="112" t="s">
         <v>406</v>
       </c>
-      <c r="C36" s="115"/>
+      <c r="C36" s="117"/>
     </row>
     <row r="37" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="115"/>
-      <c r="B37" s="110"/>
-      <c r="C37" s="115"/>
+      <c r="A37" s="117"/>
+      <c r="B37" s="112"/>
+      <c r="C37" s="117"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="115"/>
-      <c r="B38" s="110"/>
-      <c r="C38" s="115"/>
+      <c r="A38" s="117"/>
+      <c r="B38" s="112"/>
+      <c r="C38" s="117"/>
     </row>
     <row r="39" spans="1:3" ht="239" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="115"/>
-      <c r="B39" s="110"/>
-      <c r="C39" s="115"/>
+      <c r="A39" s="117"/>
+      <c r="B39" s="112"/>
+      <c r="C39" s="117"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="115"/>
-      <c r="B40" s="110" t="s">
+      <c r="A40" s="117"/>
+      <c r="B40" s="112" t="s">
         <v>407</v>
       </c>
-      <c r="C40" s="115"/>
+      <c r="C40" s="117"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="105"/>
-      <c r="B41" s="111"/>
-      <c r="C41" s="105"/>
+      <c r="A41" s="107"/>
+      <c r="B41" s="113"/>
+      <c r="C41" s="107"/>
     </row>
     <row r="42" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A42" s="60" t="s">
@@ -27555,11 +28707,11 @@
       <c r="C46" s="60"/>
     </row>
     <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A47" s="108" t="s">
+      <c r="A47" s="110" t="s">
         <v>386</v>
       </c>
-      <c r="B47" s="108"/>
-      <c r="C47" s="108"/>
+      <c r="B47" s="110"/>
+      <c r="C47" s="110"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
@@ -27573,25 +28725,25 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="104" t="s">
+      <c r="A49" s="106" t="s">
         <v>388</v>
       </c>
-      <c r="B49" s="106" t="s">
+      <c r="B49" s="108" t="s">
         <v>413</v>
       </c>
-      <c r="C49" s="104" t="s">
+      <c r="C49" s="106" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="115"/>
-      <c r="B50" s="127"/>
-      <c r="C50" s="115"/>
+      <c r="A50" s="117"/>
+      <c r="B50" s="129"/>
+      <c r="C50" s="117"/>
     </row>
     <row r="51" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="105"/>
-      <c r="B51" s="107"/>
-      <c r="C51" s="105"/>
+      <c r="A51" s="107"/>
+      <c r="B51" s="109"/>
+      <c r="C51" s="107"/>
     </row>
     <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="54" t="s">
@@ -27605,91 +28757,91 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="104" t="s">
+      <c r="A53" s="106" t="s">
         <v>415</v>
       </c>
-      <c r="B53" s="128" t="s">
+      <c r="B53" s="130" t="s">
         <v>416</v>
       </c>
-      <c r="C53" s="104" t="s">
+      <c r="C53" s="106" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="238" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="115"/>
-      <c r="B54" s="128"/>
-      <c r="C54" s="115"/>
+      <c r="A54" s="117"/>
+      <c r="B54" s="130"/>
+      <c r="C54" s="117"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="115"/>
-      <c r="B55" s="106" t="s">
+      <c r="A55" s="117"/>
+      <c r="B55" s="108" t="s">
         <v>417</v>
       </c>
-      <c r="C55" s="115"/>
+      <c r="C55" s="117"/>
     </row>
     <row r="56" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="115"/>
-      <c r="B56" s="127"/>
-      <c r="C56" s="115"/>
+      <c r="A56" s="117"/>
+      <c r="B56" s="129"/>
+      <c r="C56" s="117"/>
     </row>
     <row r="57" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="115"/>
-      <c r="B57" s="127"/>
-      <c r="C57" s="115"/>
+      <c r="A57" s="117"/>
+      <c r="B57" s="129"/>
+      <c r="C57" s="117"/>
     </row>
     <row r="58" spans="1:3" ht="172" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="115"/>
-      <c r="B58" s="107"/>
-      <c r="C58" s="115"/>
+      <c r="A58" s="117"/>
+      <c r="B58" s="109"/>
+      <c r="C58" s="117"/>
     </row>
     <row r="59" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="115"/>
-      <c r="B59" s="106" t="s">
+      <c r="A59" s="117"/>
+      <c r="B59" s="108" t="s">
         <v>418</v>
       </c>
-      <c r="C59" s="115"/>
+      <c r="C59" s="117"/>
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="115"/>
-      <c r="B60" s="127"/>
-      <c r="C60" s="115"/>
+      <c r="A60" s="117"/>
+      <c r="B60" s="129"/>
+      <c r="C60" s="117"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="115"/>
-      <c r="B61" s="127"/>
-      <c r="C61" s="115"/>
+      <c r="A61" s="117"/>
+      <c r="B61" s="129"/>
+      <c r="C61" s="117"/>
     </row>
     <row r="62" spans="1:3" ht="125" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="115"/>
-      <c r="B62" s="107"/>
-      <c r="C62" s="115"/>
+      <c r="A62" s="117"/>
+      <c r="B62" s="109"/>
+      <c r="C62" s="117"/>
     </row>
     <row r="63" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="115"/>
-      <c r="B63" s="106" t="s">
+      <c r="A63" s="117"/>
+      <c r="B63" s="108" t="s">
         <v>419</v>
       </c>
-      <c r="C63" s="115"/>
+      <c r="C63" s="117"/>
     </row>
     <row r="64" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="115"/>
-      <c r="B64" s="127"/>
-      <c r="C64" s="115"/>
+      <c r="A64" s="117"/>
+      <c r="B64" s="129"/>
+      <c r="C64" s="117"/>
     </row>
     <row r="65" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="115"/>
-      <c r="B65" s="127"/>
-      <c r="C65" s="115"/>
+      <c r="A65" s="117"/>
+      <c r="B65" s="129"/>
+      <c r="C65" s="117"/>
     </row>
     <row r="66" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="115"/>
-      <c r="B66" s="127"/>
-      <c r="C66" s="115"/>
+      <c r="A66" s="117"/>
+      <c r="B66" s="129"/>
+      <c r="C66" s="117"/>
     </row>
     <row r="67" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="105"/>
-      <c r="B67" s="107"/>
-      <c r="C67" s="105"/>
+      <c r="A67" s="107"/>
+      <c r="B67" s="109"/>
+      <c r="C67" s="107"/>
     </row>
     <row r="68" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A68" s="60" t="s">

</xml_diff>

<commit_message>
Implemented the print and download menu options in html/survey-report.html
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE2F7A3-7BF0-074A-90C9-98CAFED92332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EE6552-07B0-0C46-A498-018AE25826DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16160" firstSheet="14" activeTab="22" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16160" firstSheet="14" activeTab="23" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="SPEC - 1.1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,10 @@
     <sheet name="SPEC - 3.6" sheetId="25" r:id="rId21"/>
     <sheet name="SPEC - 3.7" sheetId="26" r:id="rId22"/>
     <sheet name="SPEC - 3.8" sheetId="27" r:id="rId23"/>
-    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId24"/>
-    <sheet name="PLAYGROUND" sheetId="6" r:id="rId25"/>
-    <sheet name="TEMPLATE" sheetId="8" r:id="rId26"/>
+    <sheet name="SPEC - 3.9" sheetId="28" r:id="rId24"/>
+    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId25"/>
+    <sheet name="PLAYGROUND" sheetId="6" r:id="rId26"/>
+    <sheet name="TEMPLATE" sheetId="8" r:id="rId27"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="831">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="850">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -23795,6 +23796,474 @@
   </si>
   <si>
     <t>git commit -m "Implemented html/survey-report.html and associated js and css files"</t>
+  </si>
+  <si>
+    <t>/* The function creates a pdf file for the report.
+ *  
+ * @param
+ * @return      
+ * */
+const createPDF = () =&gt; {
+    // Get the parent &lt;div&gt; element for the report
+    let element = document.getElementById('report-body');
+    // Configure the pdf
+    let option = {
+        margin: [0.50, 0.25, 0.25, 0.25],
+        filename: JSON.parse(sessionStorage.getItem("customerData"))
+            .customerMobile + '.pdf',
+        image: {
+            type: 'jpeg',
+            quality: 0.98
+        },
+        html2canvas: {
+            scale: window.devicePixelRatio
+        },
+        jsPDF: {
+            unit: 'in',
+            format: 'letter',
+            orientation: 'portrait'
+        }
+    };
+    // Create the pdf and provide an option to save it
+    html2pdf().set(option).from(element).save();
+}
+/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create a function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">createPDF() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller/survey-report.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to generate a pdf from athe report and provide an option to save it.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Created a function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">createPDF() </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller/survey-report.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to generate a pdf from athe report and provide an option to save it.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html/survey-report.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> file to provide links for printing and downloading the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>pdf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> file</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;!-- Main container --&gt;
+    &lt;div class="container"&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+      &lt;nav class="navbar navbar-expand-lg navbar-light bg-light"&gt;
+        &lt;button class="navbar-toggler" type="button" data-toggle="collapse"
+          data-target="#navBarMenu" aria-controls="navBarMenu"
+          aria-expanded="false" aria-label="Toggle navigation"&gt;
+          &lt;span class="navbar-toggler-icon"&gt;&lt;/span&gt;
+        &lt;/button&gt;
+        &lt;div class="collapse navbar-collapse" id="navBarMenu"&gt;
+          &lt;div class="navbar-nav"&gt;
+            &lt;a class="nav-item nav-link active report-link"
+              href="javascript:window.print()"&gt;Print &lt;span
+                class="sr-only"&gt;(current)&lt;/span&gt;&lt;/a&gt;
+            &lt;a class="nav-item nav-link active report-link"
+              href="javascript:createPDF()"&gt;Download&lt;/a&gt;
+          &lt;/div&gt;
+        &lt;/div&gt;
+      &lt;/nav&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">      &lt;!-- Report Body --&gt;
+      &lt;div id="report-body"&gt;
+        &lt;!-- Report Title --&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">        &lt;h2 id="report-title" class="report-title"&gt;&lt;/h2&gt;
+       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;!-- End Report Title --&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html/survey-report.html</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> file to provide links for printing and downloading the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>pdf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> file</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    &lt;!-- Information Capture Javascript --&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">    &lt;script src="https://apis.google.com/js/api.js"&gt;&lt;/script&gt;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">    &lt;script
+      src="https://cdnjs.cloudflare.com/ajax/libs/html2pdf.js/0.9.3/html2pdf.bundle.min.js"&gt;
+    &lt;/script&gt;
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> &lt;script src="./../lib/lang/en/enum/door/door-enum.js"
+      type="text/javascript"&gt;&lt;/script&gt;
+    &lt;script src="./../lib/lang/en/enum/page/survey-report-enum.js"
+      type="text/javascript"&gt;&lt;/script&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>/*****************************************************************************/
+/* MENU LINKS                                                                */
+/*****************************************************************************/
+a:hover{
+    color: rgb(24, 143, 223) !important;
+}
+.report-link{
+    font-family: 'Noto Sans JP', sans-serif !important;
+    color: rgb(136, 196, 236) !important;
+}
+/*****************************************************************************/
+/* SURVEY HEADING &lt;div&gt;                                                      */
+/*****************************************************************************/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Style the menu links in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/survey-report.css</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Styled the menu links in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/survey-report.css</t>
+    </r>
+  </si>
+  <si>
+    <t>.report-title{
+    border: 1px dotted #c0bdbd;
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Add borders for the report tile header in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/survey-report.css</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Added borders for the report tile header in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/survey-report.css</t>
+    </r>
+  </si>
+  <si>
+    <t>/* The report enclosing &lt;div&gt; */
+#report-body {
+    margin-top: 1rem;
+    margin-bottom: 2rem;
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Provide a bottom margin for the report body in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/survey-report.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Provided a bottom margin for the report body in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>css/survey-report.js</t>
+    </r>
+  </si>
+  <si>
+    <t>git commit -m "Implemented the print and download menu options in html/survey-report.html"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>git status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - would display the following files.                                                                                                                                                                                                                                  On branch master
+Your branch is ahead of 'hafele/master' by 2 commits.
+  (use "git push" to publish your local commits)
+Changes to be committed:
+  (use "git restore --staged &lt;file&gt;..." to unstage)
+        modified:   css/survey-report.css
+        modified:   docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+        modified:   html/survey-report.html
+        modified:   js/controller/survey-report.js</t>
+    </r>
+  </si>
+  <si>
+    <t>IMPLEMENT THE PRINT AND DOWNLOAD OPTIONS IN html/survey-report.html FILE</t>
   </si>
 </sst>
 </file>
@@ -24226,7 +24695,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -24518,6 +24987,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -24964,18 +25445,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="115" t="s">
+      <c r="A2" s="119" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="115"/>
-      <c r="C2" s="115"/>
+      <c r="B2" s="119"/>
+      <c r="C2" s="119"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -25260,18 +25741,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>426</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -25285,7 +25766,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="141" t="s">
+      <c r="A4" s="145" t="s">
         <v>438</v>
       </c>
       <c r="B4" s="48" t="s">
@@ -25296,7 +25777,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="142"/>
+      <c r="A5" s="146"/>
       <c r="B5" s="48" t="s">
         <v>441</v>
       </c>
@@ -25305,51 +25786,51 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="142"/>
+      <c r="A6" s="146"/>
       <c r="B6" s="48" t="s">
         <v>434</v>
       </c>
-      <c r="C6" s="144" t="s">
+      <c r="C6" s="148" t="s">
         <v>446</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="142"/>
+      <c r="A7" s="146"/>
       <c r="B7" s="48" t="s">
         <v>435</v>
       </c>
-      <c r="C7" s="145"/>
+      <c r="C7" s="149"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="142"/>
+      <c r="A8" s="146"/>
       <c r="B8" s="48" t="s">
         <v>427</v>
       </c>
-      <c r="C8" s="145"/>
+      <c r="C8" s="149"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="142"/>
+      <c r="A9" s="146"/>
       <c r="B9" s="48" t="s">
         <v>428</v>
       </c>
-      <c r="C9" s="145"/>
+      <c r="C9" s="149"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="142"/>
+      <c r="A10" s="146"/>
       <c r="B10" s="48" t="s">
         <v>436</v>
       </c>
-      <c r="C10" s="145"/>
+      <c r="C10" s="149"/>
     </row>
     <row r="11" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="142"/>
+      <c r="A11" s="146"/>
       <c r="B11" s="48" t="s">
         <v>443</v>
       </c>
-      <c r="C11" s="146"/>
+      <c r="C11" s="150"/>
     </row>
     <row r="12" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="143"/>
+      <c r="A12" s="147"/>
       <c r="B12" s="48" t="s">
         <v>445</v>
       </c>
@@ -25488,18 +25969,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>464</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -25605,18 +26086,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>478</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -25667,11 +26148,11 @@
       <c r="C8" s="54"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="120" t="s">
+      <c r="A9" s="124" t="s">
         <v>485</v>
       </c>
-      <c r="B9" s="120"/>
-      <c r="C9" s="120"/>
+      <c r="B9" s="124"/>
+      <c r="C9" s="124"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -25707,20 +26188,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="120" t="s">
         <v>490</v>
       </c>
-      <c r="B13" s="121" t="s">
+      <c r="B13" s="125" t="s">
         <v>489</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="120" t="s">
         <v>491</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="117"/>
-      <c r="B14" s="123"/>
-      <c r="C14" s="117"/>
+      <c r="A14" s="121"/>
+      <c r="B14" s="127"/>
+      <c r="C14" s="121"/>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="73" t="s">
@@ -25745,20 +26226,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="116" t="s">
+      <c r="A17" s="120" t="s">
         <v>499</v>
       </c>
-      <c r="B17" s="121" t="s">
+      <c r="B17" s="125" t="s">
         <v>498</v>
       </c>
-      <c r="C17" s="116" t="s">
+      <c r="C17" s="120" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="222" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="117"/>
-      <c r="B18" s="123"/>
-      <c r="C18" s="117"/>
+      <c r="A18" s="121"/>
+      <c r="B18" s="127"/>
+      <c r="C18" s="121"/>
     </row>
     <row r="19" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -25816,18 +26297,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>505</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -25885,25 +26366,25 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="116" t="s">
+      <c r="A8" s="120" t="s">
         <v>517</v>
       </c>
-      <c r="B8" s="121" t="s">
+      <c r="B8" s="125" t="s">
         <v>516</v>
       </c>
-      <c r="C8" s="116" t="s">
+      <c r="C8" s="120" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="127"/>
-      <c r="B9" s="122"/>
-      <c r="C9" s="127"/>
+      <c r="A9" s="131"/>
+      <c r="B9" s="126"/>
+      <c r="C9" s="131"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="117"/>
-      <c r="B10" s="123"/>
-      <c r="C10" s="117"/>
+      <c r="A10" s="121"/>
+      <c r="B10" s="127"/>
+      <c r="C10" s="121"/>
     </row>
     <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="54" t="s">
@@ -25917,86 +26398,86 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="116" t="s">
+      <c r="A12" s="120" t="s">
         <v>526</v>
       </c>
-      <c r="B12" s="121" t="s">
+      <c r="B12" s="125" t="s">
         <v>527</v>
       </c>
-      <c r="C12" s="116" t="s">
+      <c r="C12" s="120" t="s">
         <v>530</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="127"/>
-      <c r="B13" s="122"/>
-      <c r="C13" s="127"/>
+      <c r="A13" s="131"/>
+      <c r="B13" s="126"/>
+      <c r="C13" s="131"/>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="127"/>
-      <c r="B14" s="122"/>
-      <c r="C14" s="127"/>
+      <c r="A14" s="131"/>
+      <c r="B14" s="126"/>
+      <c r="C14" s="131"/>
     </row>
     <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="127"/>
-      <c r="B15" s="122"/>
-      <c r="C15" s="127"/>
+      <c r="A15" s="131"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="131"/>
     </row>
     <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="127"/>
-      <c r="B16" s="122"/>
-      <c r="C16" s="127"/>
+      <c r="A16" s="131"/>
+      <c r="B16" s="126"/>
+      <c r="C16" s="131"/>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="127"/>
-      <c r="B17" s="122"/>
-      <c r="C17" s="127"/>
+      <c r="A17" s="131"/>
+      <c r="B17" s="126"/>
+      <c r="C17" s="131"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="117"/>
-      <c r="B18" s="122"/>
-      <c r="C18" s="117"/>
+      <c r="A18" s="121"/>
+      <c r="B18" s="126"/>
+      <c r="C18" s="121"/>
     </row>
     <row r="19" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="116" t="s">
+      <c r="A19" s="120" t="s">
         <v>529</v>
       </c>
-      <c r="B19" s="121" t="s">
+      <c r="B19" s="125" t="s">
         <v>528</v>
       </c>
-      <c r="C19" s="116" t="s">
+      <c r="C19" s="120" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="127"/>
-      <c r="B20" s="122"/>
-      <c r="C20" s="127"/>
+      <c r="A20" s="131"/>
+      <c r="B20" s="126"/>
+      <c r="C20" s="131"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="127"/>
-      <c r="B21" s="122"/>
-      <c r="C21" s="127"/>
+      <c r="A21" s="131"/>
+      <c r="B21" s="126"/>
+      <c r="C21" s="131"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="127"/>
-      <c r="B22" s="122"/>
-      <c r="C22" s="127"/>
+      <c r="A22" s="131"/>
+      <c r="B22" s="126"/>
+      <c r="C22" s="131"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="127"/>
-      <c r="B23" s="122"/>
-      <c r="C23" s="127"/>
+      <c r="A23" s="131"/>
+      <c r="B23" s="126"/>
+      <c r="C23" s="131"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="127"/>
-      <c r="B24" s="122"/>
-      <c r="C24" s="127"/>
+      <c r="A24" s="131"/>
+      <c r="B24" s="126"/>
+      <c r="C24" s="131"/>
     </row>
     <row r="25" spans="1:3" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="117"/>
-      <c r="B25" s="123"/>
-      <c r="C25" s="117"/>
+      <c r="A25" s="121"/>
+      <c r="B25" s="127"/>
+      <c r="C25" s="121"/>
     </row>
     <row r="26" spans="1:3" s="13" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
@@ -26010,51 +26491,51 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="116" t="s">
+      <c r="A27" s="120" t="s">
         <v>533</v>
       </c>
-      <c r="B27" s="121" t="s">
+      <c r="B27" s="125" t="s">
         <v>532</v>
       </c>
-      <c r="C27" s="116" t="s">
+      <c r="C27" s="120" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="127"/>
-      <c r="B28" s="122"/>
-      <c r="C28" s="127"/>
+      <c r="A28" s="131"/>
+      <c r="B28" s="126"/>
+      <c r="C28" s="131"/>
     </row>
     <row r="29" spans="1:3" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="117"/>
-      <c r="B29" s="123"/>
-      <c r="C29" s="117"/>
+      <c r="A29" s="121"/>
+      <c r="B29" s="127"/>
+      <c r="C29" s="121"/>
     </row>
     <row r="30" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="116" t="s">
+      <c r="A30" s="120" t="s">
         <v>536</v>
       </c>
-      <c r="B30" s="121" t="s">
+      <c r="B30" s="125" t="s">
         <v>535</v>
       </c>
-      <c r="C30" s="116" t="s">
+      <c r="C30" s="120" t="s">
         <v>537</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="127"/>
-      <c r="B31" s="122"/>
-      <c r="C31" s="127"/>
+      <c r="A31" s="131"/>
+      <c r="B31" s="126"/>
+      <c r="C31" s="131"/>
     </row>
     <row r="32" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="127"/>
-      <c r="B32" s="122"/>
-      <c r="C32" s="127"/>
+      <c r="A32" s="131"/>
+      <c r="B32" s="126"/>
+      <c r="C32" s="131"/>
     </row>
     <row r="33" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="117"/>
-      <c r="B33" s="123"/>
-      <c r="C33" s="117"/>
+      <c r="A33" s="121"/>
+      <c r="B33" s="127"/>
+      <c r="C33" s="121"/>
     </row>
     <row r="34" spans="1:3" ht="255" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
@@ -26120,18 +26601,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>549</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -26226,18 +26707,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>560</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -26299,11 +26780,11 @@
       <c r="C9" s="54"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="120" t="s">
+      <c r="A10" s="124" t="s">
         <v>575</v>
       </c>
-      <c r="B10" s="120"/>
-      <c r="C10" s="120"/>
+      <c r="B10" s="124"/>
+      <c r="C10" s="124"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
@@ -26419,18 +26900,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>661</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -26488,20 +26969,20 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="116" t="s">
+      <c r="A8" s="120" t="s">
         <v>587</v>
       </c>
-      <c r="B8" s="121" t="s">
+      <c r="B8" s="125" t="s">
         <v>590</v>
       </c>
-      <c r="C8" s="116" t="s">
+      <c r="C8" s="120" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="109" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="117"/>
-      <c r="B9" s="123"/>
-      <c r="C9" s="117"/>
+      <c r="A9" s="121"/>
+      <c r="B9" s="127"/>
+      <c r="C9" s="121"/>
     </row>
     <row r="10" spans="1:3" ht="109" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="82" t="s">
@@ -26537,20 +27018,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="120" t="s">
         <v>603</v>
       </c>
-      <c r="B13" s="121" t="s">
+      <c r="B13" s="125" t="s">
         <v>602</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="120" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="117"/>
-      <c r="B14" s="123"/>
-      <c r="C14" s="117"/>
+      <c r="A14" s="121"/>
+      <c r="B14" s="127"/>
+      <c r="C14" s="121"/>
     </row>
     <row r="15" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="82" t="s">
@@ -26564,67 +27045,67 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="148" t="s">
+      <c r="A16" s="152" t="s">
         <v>609</v>
       </c>
-      <c r="B16" s="147" t="s">
+      <c r="B16" s="151" t="s">
         <v>608</v>
       </c>
-      <c r="C16" s="148" t="s">
+      <c r="C16" s="152" t="s">
         <v>610</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="148"/>
-      <c r="B17" s="147"/>
-      <c r="C17" s="148"/>
+      <c r="A17" s="152"/>
+      <c r="B17" s="151"/>
+      <c r="C17" s="152"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="148"/>
-      <c r="B18" s="147"/>
-      <c r="C18" s="148"/>
+      <c r="A18" s="152"/>
+      <c r="B18" s="151"/>
+      <c r="C18" s="152"/>
     </row>
     <row r="19" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="148"/>
-      <c r="B19" s="147"/>
-      <c r="C19" s="148"/>
+      <c r="A19" s="152"/>
+      <c r="B19" s="151"/>
+      <c r="C19" s="152"/>
     </row>
     <row r="20" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="148"/>
-      <c r="B20" s="147"/>
-      <c r="C20" s="148"/>
+      <c r="A20" s="152"/>
+      <c r="B20" s="151"/>
+      <c r="C20" s="152"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="148"/>
-      <c r="B21" s="147"/>
-      <c r="C21" s="148"/>
+      <c r="A21" s="152"/>
+      <c r="B21" s="151"/>
+      <c r="C21" s="152"/>
     </row>
     <row r="22" spans="1:3" ht="139" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="148"/>
-      <c r="B22" s="147"/>
-      <c r="C22" s="148"/>
+      <c r="A22" s="152"/>
+      <c r="B22" s="151"/>
+      <c r="C22" s="152"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="148"/>
-      <c r="B23" s="147" t="s">
+      <c r="A23" s="152"/>
+      <c r="B23" s="151" t="s">
         <v>611</v>
       </c>
-      <c r="C23" s="148"/>
+      <c r="C23" s="152"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="148"/>
-      <c r="B24" s="147"/>
-      <c r="C24" s="148"/>
+      <c r="A24" s="152"/>
+      <c r="B24" s="151"/>
+      <c r="C24" s="152"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="148"/>
-      <c r="B25" s="147"/>
-      <c r="C25" s="148"/>
+      <c r="A25" s="152"/>
+      <c r="B25" s="151"/>
+      <c r="C25" s="152"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="148"/>
-      <c r="B26" s="147"/>
-      <c r="C26" s="148"/>
+      <c r="A26" s="152"/>
+      <c r="B26" s="151"/>
+      <c r="C26" s="152"/>
     </row>
     <row r="27" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A27" s="85" t="s">
@@ -26693,185 +27174,185 @@
       </c>
     </row>
     <row r="33" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="116" t="s">
+      <c r="A33" s="120" t="s">
         <v>633</v>
       </c>
-      <c r="B33" s="118" t="s">
+      <c r="B33" s="122" t="s">
         <v>627</v>
       </c>
-      <c r="C33" s="116" t="s">
+      <c r="C33" s="120" t="s">
         <v>633</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="127"/>
-      <c r="B34" s="139"/>
-      <c r="C34" s="127"/>
+      <c r="A34" s="131"/>
+      <c r="B34" s="143"/>
+      <c r="C34" s="131"/>
     </row>
     <row r="35" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="127"/>
-      <c r="B35" s="139"/>
-      <c r="C35" s="127"/>
+      <c r="A35" s="131"/>
+      <c r="B35" s="143"/>
+      <c r="C35" s="131"/>
     </row>
     <row r="36" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="127"/>
-      <c r="B36" s="119"/>
-      <c r="C36" s="127"/>
+      <c r="A36" s="131"/>
+      <c r="B36" s="123"/>
+      <c r="C36" s="131"/>
     </row>
     <row r="37" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="127"/>
-      <c r="B37" s="118" t="s">
+      <c r="A37" s="131"/>
+      <c r="B37" s="122" t="s">
         <v>628</v>
       </c>
-      <c r="C37" s="127"/>
+      <c r="C37" s="131"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="127"/>
-      <c r="B38" s="139"/>
-      <c r="C38" s="127"/>
+      <c r="A38" s="131"/>
+      <c r="B38" s="143"/>
+      <c r="C38" s="131"/>
     </row>
     <row r="39" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="127"/>
-      <c r="B39" s="139"/>
-      <c r="C39" s="127"/>
+      <c r="A39" s="131"/>
+      <c r="B39" s="143"/>
+      <c r="C39" s="131"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="127"/>
-      <c r="B40" s="139"/>
-      <c r="C40" s="127"/>
+      <c r="A40" s="131"/>
+      <c r="B40" s="143"/>
+      <c r="C40" s="131"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="127"/>
-      <c r="B41" s="139"/>
-      <c r="C41" s="127"/>
+      <c r="A41" s="131"/>
+      <c r="B41" s="143"/>
+      <c r="C41" s="131"/>
     </row>
     <row r="42" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="127"/>
-      <c r="B42" s="139"/>
-      <c r="C42" s="127"/>
+      <c r="A42" s="131"/>
+      <c r="B42" s="143"/>
+      <c r="C42" s="131"/>
     </row>
     <row r="43" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="127"/>
-      <c r="B43" s="118" t="s">
+      <c r="A43" s="131"/>
+      <c r="B43" s="122" t="s">
         <v>629</v>
       </c>
-      <c r="C43" s="127"/>
+      <c r="C43" s="131"/>
     </row>
     <row r="44" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="127"/>
-      <c r="B44" s="139"/>
-      <c r="C44" s="127"/>
+      <c r="A44" s="131"/>
+      <c r="B44" s="143"/>
+      <c r="C44" s="131"/>
     </row>
     <row r="45" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="127"/>
-      <c r="B45" s="139"/>
-      <c r="C45" s="127"/>
+      <c r="A45" s="131"/>
+      <c r="B45" s="143"/>
+      <c r="C45" s="131"/>
     </row>
     <row r="46" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="127"/>
-      <c r="B46" s="139"/>
-      <c r="C46" s="127"/>
+      <c r="A46" s="131"/>
+      <c r="B46" s="143"/>
+      <c r="C46" s="131"/>
     </row>
     <row r="47" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="127"/>
-      <c r="B47" s="139"/>
-      <c r="C47" s="127"/>
+      <c r="A47" s="131"/>
+      <c r="B47" s="143"/>
+      <c r="C47" s="131"/>
     </row>
     <row r="48" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="127"/>
-      <c r="B48" s="139"/>
-      <c r="C48" s="127"/>
+      <c r="A48" s="131"/>
+      <c r="B48" s="143"/>
+      <c r="C48" s="131"/>
     </row>
     <row r="49" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="127"/>
-      <c r="B49" s="139"/>
-      <c r="C49" s="127"/>
+      <c r="A49" s="131"/>
+      <c r="B49" s="143"/>
+      <c r="C49" s="131"/>
     </row>
     <row r="50" spans="1:3" ht="320" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="127"/>
-      <c r="B50" s="119"/>
-      <c r="C50" s="127"/>
+      <c r="A50" s="131"/>
+      <c r="B50" s="123"/>
+      <c r="C50" s="131"/>
     </row>
     <row r="51" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="127"/>
-      <c r="B51" s="118" t="s">
+      <c r="A51" s="131"/>
+      <c r="B51" s="122" t="s">
         <v>630</v>
       </c>
-      <c r="C51" s="127"/>
+      <c r="C51" s="131"/>
     </row>
     <row r="52" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="127"/>
-      <c r="B52" s="139"/>
-      <c r="C52" s="127"/>
+      <c r="A52" s="131"/>
+      <c r="B52" s="143"/>
+      <c r="C52" s="131"/>
     </row>
     <row r="53" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="127"/>
-      <c r="B53" s="139"/>
-      <c r="C53" s="127"/>
+      <c r="A53" s="131"/>
+      <c r="B53" s="143"/>
+      <c r="C53" s="131"/>
     </row>
     <row r="54" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="127"/>
-      <c r="B54" s="139"/>
-      <c r="C54" s="127"/>
+      <c r="A54" s="131"/>
+      <c r="B54" s="143"/>
+      <c r="C54" s="131"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="127"/>
-      <c r="B55" s="139"/>
-      <c r="C55" s="127"/>
+      <c r="A55" s="131"/>
+      <c r="B55" s="143"/>
+      <c r="C55" s="131"/>
     </row>
     <row r="56" spans="1:3" ht="97" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="127"/>
-      <c r="B56" s="119"/>
-      <c r="C56" s="127"/>
+      <c r="A56" s="131"/>
+      <c r="B56" s="123"/>
+      <c r="C56" s="131"/>
     </row>
     <row r="57" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="127"/>
-      <c r="B57" s="118" t="s">
+      <c r="A57" s="131"/>
+      <c r="B57" s="122" t="s">
         <v>631</v>
       </c>
-      <c r="C57" s="127"/>
+      <c r="C57" s="131"/>
     </row>
     <row r="58" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="127"/>
-      <c r="B58" s="139"/>
-      <c r="C58" s="127"/>
+      <c r="A58" s="131"/>
+      <c r="B58" s="143"/>
+      <c r="C58" s="131"/>
     </row>
     <row r="59" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="127"/>
-      <c r="B59" s="139"/>
-      <c r="C59" s="127"/>
+      <c r="A59" s="131"/>
+      <c r="B59" s="143"/>
+      <c r="C59" s="131"/>
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="127"/>
-      <c r="B60" s="139"/>
-      <c r="C60" s="127"/>
+      <c r="A60" s="131"/>
+      <c r="B60" s="143"/>
+      <c r="C60" s="131"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="127"/>
-      <c r="B61" s="139"/>
-      <c r="C61" s="127"/>
+      <c r="A61" s="131"/>
+      <c r="B61" s="143"/>
+      <c r="C61" s="131"/>
     </row>
     <row r="62" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="127"/>
-      <c r="B62" s="139"/>
-      <c r="C62" s="127"/>
+      <c r="A62" s="131"/>
+      <c r="B62" s="143"/>
+      <c r="C62" s="131"/>
     </row>
     <row r="63" spans="1:3" ht="146" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="127"/>
-      <c r="B63" s="119"/>
-      <c r="C63" s="127"/>
+      <c r="A63" s="131"/>
+      <c r="B63" s="123"/>
+      <c r="C63" s="131"/>
     </row>
     <row r="64" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="127"/>
-      <c r="B64" s="118" t="s">
+      <c r="A64" s="131"/>
+      <c r="B64" s="122" t="s">
         <v>632</v>
       </c>
-      <c r="C64" s="127"/>
+      <c r="C64" s="131"/>
     </row>
     <row r="65" spans="1:3" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="117"/>
-      <c r="B65" s="119"/>
-      <c r="C65" s="117"/>
+      <c r="A65" s="121"/>
+      <c r="B65" s="123"/>
+      <c r="C65" s="121"/>
     </row>
     <row r="66" spans="1:3" ht="397" x14ac:dyDescent="0.2">
       <c r="A66" s="85" t="s">
@@ -26885,93 +27366,93 @@
       </c>
     </row>
     <row r="67" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="128" t="s">
+      <c r="A67" s="132" t="s">
         <v>638</v>
       </c>
-      <c r="B67" s="140" t="s">
+      <c r="B67" s="144" t="s">
         <v>637</v>
       </c>
-      <c r="C67" s="128" t="s">
+      <c r="C67" s="132" t="s">
         <v>639</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="128"/>
-      <c r="B68" s="140"/>
-      <c r="C68" s="128"/>
+      <c r="A68" s="132"/>
+      <c r="B68" s="144"/>
+      <c r="C68" s="132"/>
     </row>
     <row r="69" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="128"/>
-      <c r="B69" s="140"/>
-      <c r="C69" s="128"/>
+      <c r="A69" s="132"/>
+      <c r="B69" s="144"/>
+      <c r="C69" s="132"/>
     </row>
     <row r="70" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="128" t="s">
+      <c r="A70" s="132" t="s">
         <v>643</v>
       </c>
-      <c r="B70" s="140" t="s">
+      <c r="B70" s="144" t="s">
         <v>640</v>
       </c>
-      <c r="C70" s="128" t="s">
+      <c r="C70" s="132" t="s">
         <v>642</v>
       </c>
     </row>
     <row r="71" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="128"/>
-      <c r="B71" s="140"/>
-      <c r="C71" s="128"/>
+      <c r="A71" s="132"/>
+      <c r="B71" s="144"/>
+      <c r="C71" s="132"/>
     </row>
     <row r="72" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="128"/>
-      <c r="B72" s="140"/>
-      <c r="C72" s="128"/>
+      <c r="A72" s="132"/>
+      <c r="B72" s="144"/>
+      <c r="C72" s="132"/>
     </row>
     <row r="73" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="128"/>
-      <c r="B73" s="140"/>
-      <c r="C73" s="128"/>
+      <c r="A73" s="132"/>
+      <c r="B73" s="144"/>
+      <c r="C73" s="132"/>
     </row>
     <row r="74" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="128"/>
-      <c r="B74" s="140"/>
-      <c r="C74" s="128"/>
+      <c r="A74" s="132"/>
+      <c r="B74" s="144"/>
+      <c r="C74" s="132"/>
     </row>
     <row r="75" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="128"/>
-      <c r="B75" s="140"/>
-      <c r="C75" s="128"/>
+      <c r="A75" s="132"/>
+      <c r="B75" s="144"/>
+      <c r="C75" s="132"/>
     </row>
     <row r="76" spans="1:3" ht="214" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="128"/>
-      <c r="B76" s="140"/>
-      <c r="C76" s="128"/>
+      <c r="A76" s="132"/>
+      <c r="B76" s="144"/>
+      <c r="C76" s="132"/>
     </row>
     <row r="77" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="128"/>
-      <c r="B77" s="140" t="s">
+      <c r="A77" s="132"/>
+      <c r="B77" s="144" t="s">
         <v>641</v>
       </c>
-      <c r="C77" s="128"/>
+      <c r="C77" s="132"/>
     </row>
     <row r="78" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="128"/>
-      <c r="B78" s="140"/>
-      <c r="C78" s="128"/>
+      <c r="A78" s="132"/>
+      <c r="B78" s="144"/>
+      <c r="C78" s="132"/>
     </row>
     <row r="79" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="128"/>
-      <c r="B79" s="140"/>
-      <c r="C79" s="128"/>
+      <c r="A79" s="132"/>
+      <c r="B79" s="144"/>
+      <c r="C79" s="132"/>
     </row>
     <row r="80" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="128"/>
-      <c r="B80" s="140"/>
-      <c r="C80" s="128"/>
+      <c r="A80" s="132"/>
+      <c r="B80" s="144"/>
+      <c r="C80" s="132"/>
     </row>
     <row r="81" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="128"/>
-      <c r="B81" s="140"/>
-      <c r="C81" s="128"/>
+      <c r="A81" s="132"/>
+      <c r="B81" s="144"/>
+      <c r="C81" s="132"/>
     </row>
     <row r="82" spans="1:3" ht="56" x14ac:dyDescent="0.2">
       <c r="A82" s="82" t="s">
@@ -27018,40 +27499,40 @@
       </c>
     </row>
     <row r="86" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="116" t="s">
+      <c r="A86" s="120" t="s">
         <v>657</v>
       </c>
-      <c r="B86" s="121" t="s">
+      <c r="B86" s="125" t="s">
         <v>656</v>
       </c>
-      <c r="C86" s="116" t="s">
+      <c r="C86" s="120" t="s">
         <v>658</v>
       </c>
     </row>
     <row r="87" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="127"/>
-      <c r="B87" s="122"/>
-      <c r="C87" s="127"/>
+      <c r="A87" s="131"/>
+      <c r="B87" s="126"/>
+      <c r="C87" s="131"/>
     </row>
     <row r="88" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="127"/>
-      <c r="B88" s="122"/>
-      <c r="C88" s="127"/>
+      <c r="A88" s="131"/>
+      <c r="B88" s="126"/>
+      <c r="C88" s="131"/>
     </row>
     <row r="89" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="127"/>
-      <c r="B89" s="122"/>
-      <c r="C89" s="127"/>
+      <c r="A89" s="131"/>
+      <c r="B89" s="126"/>
+      <c r="C89" s="131"/>
     </row>
     <row r="90" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="127"/>
-      <c r="B90" s="122"/>
-      <c r="C90" s="127"/>
+      <c r="A90" s="131"/>
+      <c r="B90" s="126"/>
+      <c r="C90" s="131"/>
     </row>
     <row r="91" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="117"/>
-      <c r="B91" s="123"/>
-      <c r="C91" s="117"/>
+      <c r="A91" s="121"/>
+      <c r="B91" s="127"/>
+      <c r="C91" s="121"/>
     </row>
     <row r="92" spans="1:3" ht="221" x14ac:dyDescent="0.2">
       <c r="A92" s="16" t="s">
@@ -27130,18 +27611,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>662</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -27188,40 +27669,40 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="120" t="s">
         <v>672</v>
       </c>
-      <c r="B7" s="121" t="s">
+      <c r="B7" s="125" t="s">
         <v>671</v>
       </c>
-      <c r="C7" s="116" t="s">
+      <c r="C7" s="120" t="s">
         <v>673</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="127"/>
-      <c r="B8" s="122"/>
-      <c r="C8" s="127"/>
+      <c r="A8" s="131"/>
+      <c r="B8" s="126"/>
+      <c r="C8" s="131"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="127"/>
-      <c r="B9" s="122"/>
-      <c r="C9" s="127"/>
+      <c r="A9" s="131"/>
+      <c r="B9" s="126"/>
+      <c r="C9" s="131"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="127"/>
-      <c r="B10" s="122"/>
-      <c r="C10" s="127"/>
+      <c r="A10" s="131"/>
+      <c r="B10" s="126"/>
+      <c r="C10" s="131"/>
     </row>
     <row r="11" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="127"/>
-      <c r="B11" s="122"/>
-      <c r="C11" s="127"/>
+      <c r="A11" s="131"/>
+      <c r="B11" s="126"/>
+      <c r="C11" s="131"/>
     </row>
     <row r="12" spans="1:3" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="117"/>
-      <c r="B12" s="123"/>
-      <c r="C12" s="117"/>
+      <c r="A12" s="121"/>
+      <c r="B12" s="127"/>
+      <c r="C12" s="121"/>
     </row>
     <row r="13" spans="1:3" ht="210" x14ac:dyDescent="0.2">
       <c r="A13" s="87" t="s">
@@ -27286,18 +27767,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>693</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -27414,18 +27895,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>697</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -27439,36 +27920,36 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="116" t="s">
+      <c r="A4" s="120" t="s">
         <v>698</v>
       </c>
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="122" t="s">
         <v>700</v>
       </c>
-      <c r="C4" s="116" t="s">
+      <c r="C4" s="120" t="s">
         <v>699</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="136" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="117"/>
-      <c r="B5" s="119"/>
-      <c r="C5" s="117"/>
+      <c r="A5" s="121"/>
+      <c r="B5" s="123"/>
+      <c r="C5" s="121"/>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="120" t="s">
         <v>702</v>
       </c>
-      <c r="B6" s="121" t="s">
+      <c r="B6" s="125" t="s">
         <v>701</v>
       </c>
-      <c r="C6" s="116" t="s">
+      <c r="C6" s="120" t="s">
         <v>703</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="202" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="117"/>
-      <c r="B7" s="123"/>
-      <c r="C7" s="117"/>
+      <c r="A7" s="121"/>
+      <c r="B7" s="127"/>
+      <c r="C7" s="121"/>
     </row>
     <row r="8" spans="1:3" ht="168" x14ac:dyDescent="0.2">
       <c r="A8" s="98" t="s">
@@ -27559,20 +28040,20 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="116" t="s">
+      <c r="A16" s="120" t="s">
         <v>721</v>
       </c>
-      <c r="B16" s="121" t="s">
+      <c r="B16" s="125" t="s">
         <v>723</v>
       </c>
-      <c r="C16" s="116" t="s">
+      <c r="C16" s="120" t="s">
         <v>722</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="117"/>
-      <c r="B17" s="123"/>
-      <c r="C17" s="117"/>
+      <c r="A17" s="121"/>
+      <c r="B17" s="127"/>
+      <c r="C17" s="121"/>
     </row>
     <row r="18" spans="1:3" ht="148" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="98" t="s">
@@ -27643,18 +28124,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -27705,11 +28186,11 @@
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="120" t="s">
+      <c r="A9" s="124" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="120"/>
-      <c r="C9" s="120"/>
+      <c r="B9" s="124"/>
+      <c r="C9" s="124"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
@@ -27745,20 +28226,20 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="120" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="118" t="s">
+      <c r="B13" s="122" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="120" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="117"/>
-      <c r="B14" s="119"/>
-      <c r="C14" s="117"/>
+      <c r="A14" s="121"/>
+      <c r="B14" s="123"/>
+      <c r="C14" s="121"/>
     </row>
     <row r="15" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
@@ -27783,20 +28264,20 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="116" t="s">
+      <c r="A17" s="120" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="118" t="s">
+      <c r="B17" s="122" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="116" t="s">
+      <c r="C17" s="120" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="117"/>
-      <c r="B18" s="119"/>
-      <c r="C18" s="117"/>
+      <c r="A18" s="121"/>
+      <c r="B18" s="123"/>
+      <c r="C18" s="121"/>
     </row>
     <row r="19" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
@@ -27854,18 +28335,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>729</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -27938,18 +28419,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>736</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -28000,18 +28481,18 @@
       <c r="C8" s="103"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="114" t="s">
+      <c r="A9" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="114"/>
-      <c r="C9" s="114"/>
+      <c r="B9" s="118"/>
+      <c r="C9" s="118"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A10" s="120" t="s">
+      <c r="A10" s="124" t="s">
         <v>736</v>
       </c>
-      <c r="B10" s="120"/>
-      <c r="C10" s="120"/>
+      <c r="B10" s="124"/>
+      <c r="C10" s="124"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
@@ -28141,18 +28622,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>762</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -28243,36 +28724,36 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="116" t="s">
+      <c r="A11" s="120" t="s">
         <v>783</v>
       </c>
-      <c r="B11" s="118" t="s">
+      <c r="B11" s="122" t="s">
         <v>782</v>
       </c>
-      <c r="C11" s="116" t="s">
+      <c r="C11" s="120" t="s">
         <v>783</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="217" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="117"/>
-      <c r="B12" s="119"/>
-      <c r="C12" s="117"/>
+      <c r="A12" s="121"/>
+      <c r="B12" s="123"/>
+      <c r="C12" s="121"/>
     </row>
     <row r="13" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="120" t="s">
         <v>793</v>
       </c>
-      <c r="B13" s="118" t="s">
+      <c r="B13" s="122" t="s">
         <v>792</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="120" t="s">
         <v>794</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="116" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="117"/>
-      <c r="B14" s="119"/>
-      <c r="C14" s="117"/>
+      <c r="A14" s="121"/>
+      <c r="B14" s="123"/>
+      <c r="C14" s="121"/>
     </row>
     <row r="15" spans="1:3" ht="126" x14ac:dyDescent="0.2">
       <c r="A15" s="104" t="s">
@@ -28286,20 +28767,20 @@
       </c>
     </row>
     <row r="16" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="116" t="s">
+      <c r="A16" s="120" t="s">
         <v>790</v>
       </c>
-      <c r="B16" s="121" t="s">
+      <c r="B16" s="125" t="s">
         <v>789</v>
       </c>
-      <c r="C16" s="116" t="s">
+      <c r="C16" s="120" t="s">
         <v>791</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="117"/>
-      <c r="B17" s="123"/>
-      <c r="C17" s="117"/>
+      <c r="A17" s="121"/>
+      <c r="B17" s="127"/>
+      <c r="C17" s="121"/>
     </row>
     <row r="18" spans="1:3" ht="204" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
@@ -28346,7 +28827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3059EE9-6F6A-E343-B8C2-A80CDF8B82AA}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -28359,18 +28840,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>797</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -28384,45 +28865,45 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="116" t="s">
+      <c r="A4" s="120" t="s">
         <v>798</v>
       </c>
-      <c r="B4" s="118" t="s">
+      <c r="B4" s="122" t="s">
         <v>799</v>
       </c>
-      <c r="C4" s="116" t="s">
+      <c r="C4" s="120" t="s">
         <v>800</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="127"/>
-      <c r="B5" s="139"/>
-      <c r="C5" s="127"/>
+      <c r="A5" s="131"/>
+      <c r="B5" s="143"/>
+      <c r="C5" s="131"/>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="127"/>
-      <c r="B6" s="139"/>
-      <c r="C6" s="127"/>
+      <c r="A6" s="131"/>
+      <c r="B6" s="143"/>
+      <c r="C6" s="131"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="127"/>
-      <c r="B7" s="139"/>
-      <c r="C7" s="127"/>
+      <c r="A7" s="131"/>
+      <c r="B7" s="143"/>
+      <c r="C7" s="131"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="127"/>
-      <c r="B8" s="139"/>
-      <c r="C8" s="127"/>
+      <c r="A8" s="131"/>
+      <c r="B8" s="143"/>
+      <c r="C8" s="131"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="127"/>
-      <c r="B9" s="139"/>
-      <c r="C9" s="127"/>
+      <c r="A9" s="131"/>
+      <c r="B9" s="143"/>
+      <c r="C9" s="131"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="117"/>
-      <c r="B10" s="119"/>
-      <c r="C10" s="117"/>
+      <c r="A10" s="121"/>
+      <c r="B10" s="123"/>
+      <c r="C10" s="121"/>
     </row>
     <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="111" t="s">
@@ -28447,25 +28928,25 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="120" t="s">
         <v>808</v>
       </c>
-      <c r="B13" s="121" t="s">
+      <c r="B13" s="125" t="s">
         <v>804</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="120" t="s">
         <v>827</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="127"/>
-      <c r="B14" s="122"/>
-      <c r="C14" s="127"/>
+      <c r="A14" s="131"/>
+      <c r="B14" s="126"/>
+      <c r="C14" s="131"/>
     </row>
     <row r="15" spans="1:3" ht="118" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="117"/>
-      <c r="B15" s="123"/>
-      <c r="C15" s="117"/>
+      <c r="A15" s="121"/>
+      <c r="B15" s="127"/>
+      <c r="C15" s="121"/>
     </row>
     <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="109" t="s">
@@ -28479,62 +28960,62 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="116" t="s">
+      <c r="A17" s="120" t="s">
         <v>810</v>
       </c>
-      <c r="B17" s="121" t="s">
+      <c r="B17" s="125" t="s">
         <v>809</v>
       </c>
-      <c r="C17" s="116" t="s">
+      <c r="C17" s="120" t="s">
         <v>815</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="127"/>
-      <c r="B18" s="122"/>
-      <c r="C18" s="127"/>
+      <c r="A18" s="131"/>
+      <c r="B18" s="126"/>
+      <c r="C18" s="131"/>
     </row>
     <row r="19" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="127"/>
-      <c r="B19" s="122"/>
-      <c r="C19" s="127"/>
+      <c r="A19" s="131"/>
+      <c r="B19" s="126"/>
+      <c r="C19" s="131"/>
     </row>
     <row r="20" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="127"/>
-      <c r="B20" s="122"/>
-      <c r="C20" s="127"/>
+      <c r="A20" s="131"/>
+      <c r="B20" s="126"/>
+      <c r="C20" s="131"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="127"/>
-      <c r="B21" s="122"/>
-      <c r="C21" s="127"/>
+      <c r="A21" s="131"/>
+      <c r="B21" s="126"/>
+      <c r="C21" s="131"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="127"/>
-      <c r="B22" s="122"/>
-      <c r="C22" s="127"/>
+      <c r="A22" s="131"/>
+      <c r="B22" s="126"/>
+      <c r="C22" s="131"/>
     </row>
     <row r="23" spans="1:3" ht="135" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="127"/>
-      <c r="B23" s="123"/>
-      <c r="C23" s="127"/>
+      <c r="A23" s="131"/>
+      <c r="B23" s="127"/>
+      <c r="C23" s="131"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="127"/>
-      <c r="B24" s="121" t="s">
+      <c r="A24" s="131"/>
+      <c r="B24" s="125" t="s">
         <v>814</v>
       </c>
-      <c r="C24" s="127"/>
+      <c r="C24" s="131"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="127"/>
-      <c r="B25" s="122"/>
-      <c r="C25" s="127"/>
+      <c r="A25" s="131"/>
+      <c r="B25" s="126"/>
+      <c r="C25" s="131"/>
     </row>
     <row r="26" spans="1:3" ht="66" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="117"/>
-      <c r="B26" s="123"/>
-      <c r="C26" s="117"/>
+      <c r="A26" s="121"/>
+      <c r="B26" s="127"/>
+      <c r="C26" s="121"/>
     </row>
     <row r="27" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="109" t="s">
@@ -28548,77 +29029,77 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="116" t="s">
+      <c r="A28" s="120" t="s">
         <v>819</v>
       </c>
-      <c r="B28" s="121" t="s">
+      <c r="B28" s="125" t="s">
         <v>820</v>
       </c>
-      <c r="C28" s="116" t="s">
+      <c r="C28" s="120" t="s">
         <v>821</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="127"/>
-      <c r="B29" s="122"/>
-      <c r="C29" s="127"/>
+      <c r="A29" s="131"/>
+      <c r="B29" s="126"/>
+      <c r="C29" s="131"/>
     </row>
     <row r="30" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="127"/>
-      <c r="B30" s="122"/>
-      <c r="C30" s="127"/>
+      <c r="A30" s="131"/>
+      <c r="B30" s="126"/>
+      <c r="C30" s="131"/>
     </row>
     <row r="31" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="127"/>
-      <c r="B31" s="122"/>
-      <c r="C31" s="127"/>
+      <c r="A31" s="131"/>
+      <c r="B31" s="126"/>
+      <c r="C31" s="131"/>
     </row>
     <row r="32" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="127"/>
-      <c r="B32" s="122"/>
-      <c r="C32" s="127"/>
+      <c r="A32" s="131"/>
+      <c r="B32" s="126"/>
+      <c r="C32" s="131"/>
     </row>
     <row r="33" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="127"/>
-      <c r="B33" s="122"/>
-      <c r="C33" s="127"/>
+      <c r="A33" s="131"/>
+      <c r="B33" s="126"/>
+      <c r="C33" s="131"/>
     </row>
     <row r="34" spans="1:3" ht="107" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="117"/>
-      <c r="B34" s="123"/>
-      <c r="C34" s="117"/>
+      <c r="A34" s="121"/>
+      <c r="B34" s="127"/>
+      <c r="C34" s="121"/>
     </row>
     <row r="35" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="116" t="s">
+      <c r="A35" s="120" t="s">
         <v>822</v>
       </c>
-      <c r="B35" s="121" t="s">
+      <c r="B35" s="125" t="s">
         <v>824</v>
       </c>
-      <c r="C35" s="116" t="s">
+      <c r="C35" s="120" t="s">
         <v>823</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="192" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="117"/>
-      <c r="B36" s="123"/>
-      <c r="C36" s="117"/>
+      <c r="A36" s="121"/>
+      <c r="B36" s="127"/>
+      <c r="C36" s="121"/>
     </row>
     <row r="37" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="116" t="s">
+      <c r="A37" s="120" t="s">
         <v>825</v>
       </c>
-      <c r="B37" s="121" t="s">
+      <c r="B37" s="125" t="s">
         <v>828</v>
       </c>
-      <c r="C37" s="116" t="s">
+      <c r="C37" s="120" t="s">
         <v>826</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="117"/>
-      <c r="B38" s="123"/>
-      <c r="C38" s="117"/>
+      <c r="A38" s="121"/>
+      <c r="B38" s="127"/>
+      <c r="C38" s="121"/>
     </row>
     <row r="39" spans="1:3" ht="255" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="s">
@@ -28672,6 +29153,151 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B662A0C-FC58-1247-9CFE-8CF17A7630A5}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="118" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+    </row>
+    <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="124" t="s">
+        <v>849</v>
+      </c>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
+    </row>
+    <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="132" t="s">
+        <v>832</v>
+      </c>
+      <c r="B4" s="144" t="s">
+        <v>831</v>
+      </c>
+      <c r="C4" s="132" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="13" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="132"/>
+      <c r="B5" s="144"/>
+      <c r="C5" s="132"/>
+    </row>
+    <row r="6" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="132" t="s">
+        <v>834</v>
+      </c>
+      <c r="B6" s="117" t="s">
+        <v>835</v>
+      </c>
+      <c r="C6" s="132" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="13" customFormat="1" ht="174" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="132"/>
+      <c r="B7" s="117" t="s">
+        <v>837</v>
+      </c>
+      <c r="C7" s="132"/>
+    </row>
+    <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="114" t="s">
+        <v>839</v>
+      </c>
+      <c r="B8" s="117" t="s">
+        <v>838</v>
+      </c>
+      <c r="C8" s="114" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="13" customFormat="1" ht="42" x14ac:dyDescent="0.2">
+      <c r="A9" s="115" t="s">
+        <v>842</v>
+      </c>
+      <c r="B9" s="116" t="s">
+        <v>841</v>
+      </c>
+      <c r="C9" s="115" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="85" x14ac:dyDescent="0.2">
+      <c r="A10" s="114" t="s">
+        <v>845</v>
+      </c>
+      <c r="B10" s="78" t="s">
+        <v>844</v>
+      </c>
+      <c r="C10" s="114" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="204" x14ac:dyDescent="0.2">
+      <c r="A11" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="53" t="s">
+        <v>847</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>463</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="7">
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A4:A5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE113606-3FFA-8545-9BE3-5643B52A7CE9}">
   <dimension ref="A1:H116"/>
   <sheetViews>
@@ -28749,10 +29375,10 @@
       <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="149" t="s">
+      <c r="A6" s="153" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="149"/>
+      <c r="B6" s="153"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
       <c r="E6" s="23"/>
@@ -29725,32 +30351,32 @@
       <c r="H73" s="23"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="150"/>
-      <c r="B74" s="151"/>
+      <c r="A74" s="154"/>
+      <c r="B74" s="155"/>
       <c r="C74" s="32" t="s">
         <v>225</v>
       </c>
       <c r="D74" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="E74" s="152"/>
-      <c r="F74" s="150"/>
-      <c r="G74" s="154"/>
-      <c r="H74" s="150"/>
+      <c r="E74" s="156"/>
+      <c r="F74" s="154"/>
+      <c r="G74" s="158"/>
+      <c r="H74" s="154"/>
     </row>
     <row r="75" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A75" s="150"/>
-      <c r="B75" s="151"/>
+      <c r="A75" s="154"/>
+      <c r="B75" s="155"/>
       <c r="C75" s="33" t="s">
         <v>226</v>
       </c>
       <c r="D75" s="33" t="s">
         <v>228</v>
       </c>
-      <c r="E75" s="152"/>
-      <c r="F75" s="150"/>
-      <c r="G75" s="154"/>
-      <c r="H75" s="150"/>
+      <c r="E75" s="156"/>
+      <c r="F75" s="154"/>
+      <c r="G75" s="158"/>
+      <c r="H75" s="154"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="23"/>
@@ -29923,34 +30549,34 @@
       <c r="H88" s="23"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="150"/>
-      <c r="B89" s="150"/>
+      <c r="A89" s="154"/>
+      <c r="B89" s="154"/>
       <c r="C89" s="35" t="s">
         <v>225</v>
       </c>
       <c r="D89" s="35" t="s">
         <v>227</v>
       </c>
-      <c r="E89" s="153" t="s">
+      <c r="E89" s="157" t="s">
         <v>121</v>
       </c>
-      <c r="F89" s="153"/>
-      <c r="G89" s="154"/>
-      <c r="H89" s="150"/>
+      <c r="F89" s="157"/>
+      <c r="G89" s="158"/>
+      <c r="H89" s="154"/>
     </row>
     <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A90" s="150"/>
-      <c r="B90" s="150"/>
+      <c r="A90" s="154"/>
+      <c r="B90" s="154"/>
       <c r="C90" s="35" t="s">
         <v>242</v>
       </c>
       <c r="D90" s="35" t="s">
         <v>243</v>
       </c>
-      <c r="E90" s="153"/>
-      <c r="F90" s="153"/>
-      <c r="G90" s="154"/>
-      <c r="H90" s="150"/>
+      <c r="E90" s="157"/>
+      <c r="F90" s="157"/>
+      <c r="G90" s="158"/>
+      <c r="H90" s="154"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="23"/>
@@ -30336,7 +30962,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -30434,7 +31060,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0BB7-C151-C94B-945C-E2CA92034B13}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -30451,18 +31077,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -30579,18 +31205,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>290</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -30626,25 +31252,25 @@
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="120" t="s">
         <v>292</v>
       </c>
-      <c r="B6" s="121" t="s">
+      <c r="B6" s="125" t="s">
         <v>291</v>
       </c>
-      <c r="C6" s="116" t="s">
+      <c r="C6" s="120" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="127"/>
-      <c r="B7" s="122"/>
-      <c r="C7" s="127"/>
+      <c r="A7" s="131"/>
+      <c r="B7" s="126"/>
+      <c r="C7" s="131"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="59" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="117"/>
-      <c r="B8" s="123"/>
-      <c r="C8" s="117"/>
+      <c r="A8" s="121"/>
+      <c r="B8" s="127"/>
+      <c r="C8" s="121"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
@@ -30669,25 +31295,25 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="124" t="s">
+      <c r="A11" s="128" t="s">
         <v>294</v>
       </c>
-      <c r="B11" s="121" t="s">
+      <c r="B11" s="125" t="s">
         <v>295</v>
       </c>
-      <c r="C11" s="124" t="s">
+      <c r="C11" s="128" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="408" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="125"/>
-      <c r="B12" s="122"/>
-      <c r="C12" s="125"/>
+      <c r="A12" s="129"/>
+      <c r="B12" s="126"/>
+      <c r="C12" s="129"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="126"/>
-      <c r="B13" s="123"/>
-      <c r="C13" s="126"/>
+      <c r="A13" s="130"/>
+      <c r="B13" s="127"/>
+      <c r="C13" s="130"/>
     </row>
     <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
@@ -30744,18 +31370,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>299</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -30769,46 +31395,46 @@
       </c>
     </row>
     <row r="4" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="128" t="s">
+      <c r="A4" s="132" t="s">
         <v>300</v>
       </c>
-      <c r="B4" s="132" t="s">
+      <c r="B4" s="136" t="s">
         <v>305</v>
       </c>
-      <c r="C4" s="128" t="s">
+      <c r="C4" s="132" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="128"/>
-      <c r="B5" s="132"/>
-      <c r="C5" s="128"/>
+      <c r="A5" s="132"/>
+      <c r="B5" s="136"/>
+      <c r="C5" s="132"/>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="128"/>
-      <c r="B6" s="132"/>
-      <c r="C6" s="128"/>
+      <c r="A6" s="132"/>
+      <c r="B6" s="136"/>
+      <c r="C6" s="132"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="120" t="s">
         <v>302</v>
       </c>
-      <c r="B7" s="129" t="s">
+      <c r="B7" s="133" t="s">
         <v>303</v>
       </c>
-      <c r="C7" s="116" t="s">
+      <c r="C7" s="120" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="127"/>
-      <c r="B8" s="130"/>
-      <c r="C8" s="127"/>
+      <c r="A8" s="131"/>
+      <c r="B8" s="134"/>
+      <c r="C8" s="131"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="228" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="117"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="117"/>
+      <c r="A9" s="121"/>
+      <c r="B9" s="135"/>
+      <c r="C9" s="121"/>
     </row>
     <row r="10" spans="1:3" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
@@ -30865,18 +31491,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>331</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -30923,233 +31549,233 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="116" t="s">
+      <c r="A7" s="120" t="s">
         <v>314</v>
       </c>
-      <c r="B7" s="121" t="s">
+      <c r="B7" s="125" t="s">
         <v>322</v>
       </c>
-      <c r="C7" s="116" t="s">
+      <c r="C7" s="120" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="127"/>
-      <c r="B8" s="122"/>
-      <c r="C8" s="127"/>
+      <c r="A8" s="131"/>
+      <c r="B8" s="126"/>
+      <c r="C8" s="131"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="127"/>
-      <c r="B9" s="122"/>
-      <c r="C9" s="127"/>
+      <c r="A9" s="131"/>
+      <c r="B9" s="126"/>
+      <c r="C9" s="131"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="127"/>
-      <c r="B10" s="122"/>
-      <c r="C10" s="127"/>
+      <c r="A10" s="131"/>
+      <c r="B10" s="126"/>
+      <c r="C10" s="131"/>
     </row>
     <row r="11" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="127"/>
-      <c r="B11" s="122"/>
-      <c r="C11" s="127"/>
+      <c r="A11" s="131"/>
+      <c r="B11" s="126"/>
+      <c r="C11" s="131"/>
     </row>
     <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="127"/>
-      <c r="B12" s="122"/>
-      <c r="C12" s="127"/>
+      <c r="A12" s="131"/>
+      <c r="B12" s="126"/>
+      <c r="C12" s="131"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="117"/>
-      <c r="B13" s="123"/>
-      <c r="C13" s="117"/>
+      <c r="A13" s="121"/>
+      <c r="B13" s="127"/>
+      <c r="C13" s="121"/>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="116" t="s">
+      <c r="A14" s="120" t="s">
         <v>325</v>
       </c>
-      <c r="B14" s="121" t="s">
+      <c r="B14" s="125" t="s">
         <v>323</v>
       </c>
-      <c r="C14" s="116" t="s">
+      <c r="C14" s="120" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="127"/>
-      <c r="B15" s="122"/>
-      <c r="C15" s="127"/>
+      <c r="A15" s="131"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="131"/>
     </row>
     <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="127"/>
-      <c r="B16" s="122"/>
-      <c r="C16" s="127"/>
+      <c r="A16" s="131"/>
+      <c r="B16" s="126"/>
+      <c r="C16" s="131"/>
     </row>
     <row r="17" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="127"/>
-      <c r="B17" s="122"/>
-      <c r="C17" s="127"/>
+      <c r="A17" s="131"/>
+      <c r="B17" s="126"/>
+      <c r="C17" s="131"/>
     </row>
     <row r="18" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="127"/>
-      <c r="B18" s="122"/>
-      <c r="C18" s="127"/>
+      <c r="A18" s="131"/>
+      <c r="B18" s="126"/>
+      <c r="C18" s="131"/>
     </row>
     <row r="19" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="127"/>
-      <c r="B19" s="122"/>
-      <c r="C19" s="127"/>
+      <c r="A19" s="131"/>
+      <c r="B19" s="126"/>
+      <c r="C19" s="131"/>
     </row>
     <row r="20" spans="1:3" ht="155" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="127"/>
-      <c r="B20" s="123"/>
-      <c r="C20" s="127"/>
+      <c r="A20" s="131"/>
+      <c r="B20" s="127"/>
+      <c r="C20" s="131"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="127"/>
-      <c r="B21" s="121" t="s">
+      <c r="A21" s="131"/>
+      <c r="B21" s="125" t="s">
         <v>316</v>
       </c>
-      <c r="C21" s="127"/>
+      <c r="C21" s="131"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="127"/>
-      <c r="B22" s="122"/>
-      <c r="C22" s="127"/>
+      <c r="A22" s="131"/>
+      <c r="B22" s="126"/>
+      <c r="C22" s="131"/>
     </row>
     <row r="23" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="127"/>
-      <c r="B23" s="122"/>
-      <c r="C23" s="127"/>
+      <c r="A23" s="131"/>
+      <c r="B23" s="126"/>
+      <c r="C23" s="131"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="127"/>
-      <c r="B24" s="122"/>
-      <c r="C24" s="127"/>
+      <c r="A24" s="131"/>
+      <c r="B24" s="126"/>
+      <c r="C24" s="131"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="127"/>
-      <c r="B25" s="122"/>
-      <c r="C25" s="127"/>
+      <c r="A25" s="131"/>
+      <c r="B25" s="126"/>
+      <c r="C25" s="131"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="127"/>
-      <c r="B26" s="122"/>
-      <c r="C26" s="127"/>
+      <c r="A26" s="131"/>
+      <c r="B26" s="126"/>
+      <c r="C26" s="131"/>
     </row>
     <row r="27" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="127"/>
-      <c r="B27" s="123"/>
-      <c r="C27" s="127"/>
+      <c r="A27" s="131"/>
+      <c r="B27" s="127"/>
+      <c r="C27" s="131"/>
     </row>
     <row r="28" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="127"/>
-      <c r="B28" s="121" t="s">
+      <c r="A28" s="131"/>
+      <c r="B28" s="125" t="s">
         <v>317</v>
       </c>
-      <c r="C28" s="127"/>
+      <c r="C28" s="131"/>
     </row>
     <row r="29" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="127"/>
-      <c r="B29" s="122"/>
-      <c r="C29" s="127"/>
+      <c r="A29" s="131"/>
+      <c r="B29" s="126"/>
+      <c r="C29" s="131"/>
     </row>
     <row r="30" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="127"/>
-      <c r="B30" s="122"/>
-      <c r="C30" s="127"/>
+      <c r="A30" s="131"/>
+      <c r="B30" s="126"/>
+      <c r="C30" s="131"/>
     </row>
     <row r="31" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="127"/>
-      <c r="B31" s="122"/>
-      <c r="C31" s="127"/>
+      <c r="A31" s="131"/>
+      <c r="B31" s="126"/>
+      <c r="C31" s="131"/>
     </row>
     <row r="32" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="127"/>
-      <c r="B32" s="122"/>
-      <c r="C32" s="127"/>
+      <c r="A32" s="131"/>
+      <c r="B32" s="126"/>
+      <c r="C32" s="131"/>
     </row>
     <row r="33" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="127"/>
-      <c r="B33" s="122"/>
-      <c r="C33" s="127"/>
+      <c r="A33" s="131"/>
+      <c r="B33" s="126"/>
+      <c r="C33" s="131"/>
     </row>
     <row r="34" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="127"/>
-      <c r="B34" s="122"/>
-      <c r="C34" s="127"/>
+      <c r="A34" s="131"/>
+      <c r="B34" s="126"/>
+      <c r="C34" s="131"/>
     </row>
     <row r="35" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="127"/>
-      <c r="B35" s="122"/>
-      <c r="C35" s="127"/>
+      <c r="A35" s="131"/>
+      <c r="B35" s="126"/>
+      <c r="C35" s="131"/>
     </row>
     <row r="36" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="127"/>
-      <c r="B36" s="122"/>
-      <c r="C36" s="127"/>
+      <c r="A36" s="131"/>
+      <c r="B36" s="126"/>
+      <c r="C36" s="131"/>
     </row>
     <row r="37" spans="1:3" ht="289" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="127"/>
-      <c r="B37" s="123"/>
-      <c r="C37" s="127"/>
+      <c r="A37" s="131"/>
+      <c r="B37" s="127"/>
+      <c r="C37" s="131"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="127"/>
-      <c r="B38" s="121" t="s">
+      <c r="A38" s="131"/>
+      <c r="B38" s="125" t="s">
         <v>318</v>
       </c>
-      <c r="C38" s="127"/>
+      <c r="C38" s="131"/>
     </row>
     <row r="39" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="127"/>
-      <c r="B39" s="122"/>
-      <c r="C39" s="127"/>
+      <c r="A39" s="131"/>
+      <c r="B39" s="126"/>
+      <c r="C39" s="131"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="127"/>
-      <c r="B40" s="122"/>
-      <c r="C40" s="127"/>
+      <c r="A40" s="131"/>
+      <c r="B40" s="126"/>
+      <c r="C40" s="131"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="127"/>
-      <c r="B41" s="122"/>
-      <c r="C41" s="127"/>
+      <c r="A41" s="131"/>
+      <c r="B41" s="126"/>
+      <c r="C41" s="131"/>
     </row>
     <row r="42" spans="1:3" ht="165" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="117"/>
-      <c r="B42" s="123"/>
-      <c r="C42" s="117"/>
+      <c r="A42" s="121"/>
+      <c r="B42" s="127"/>
+      <c r="C42" s="121"/>
     </row>
     <row r="43" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="116" t="s">
+      <c r="A43" s="120" t="s">
         <v>326</v>
       </c>
-      <c r="B43" s="121" t="s">
+      <c r="B43" s="125" t="s">
         <v>327</v>
       </c>
-      <c r="C43" s="116" t="s">
+      <c r="C43" s="120" t="s">
         <v>328</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="127"/>
-      <c r="B44" s="122"/>
-      <c r="C44" s="127"/>
+      <c r="A44" s="131"/>
+      <c r="B44" s="126"/>
+      <c r="C44" s="131"/>
     </row>
     <row r="45" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="127"/>
-      <c r="B45" s="122"/>
-      <c r="C45" s="127"/>
+      <c r="A45" s="131"/>
+      <c r="B45" s="126"/>
+      <c r="C45" s="131"/>
     </row>
     <row r="46" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="127"/>
-      <c r="B46" s="122"/>
-      <c r="C46" s="127"/>
+      <c r="A46" s="131"/>
+      <c r="B46" s="126"/>
+      <c r="C46" s="131"/>
     </row>
     <row r="47" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="117"/>
-      <c r="B47" s="123"/>
-      <c r="C47" s="117"/>
+      <c r="A47" s="121"/>
+      <c r="B47" s="127"/>
+      <c r="C47" s="121"/>
     </row>
     <row r="48" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A48" s="16" t="s">
@@ -31212,18 +31838,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>332</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -31362,18 +31988,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>356</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -31457,18 +32083,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>365</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -31493,20 +32119,20 @@
       </c>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="120" t="s">
         <v>369</v>
       </c>
-      <c r="B5" s="133" t="s">
+      <c r="B5" s="137" t="s">
         <v>372</v>
       </c>
-      <c r="C5" s="116" t="s">
+      <c r="C5" s="120" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="117"/>
-      <c r="B6" s="135"/>
-      <c r="C6" s="117"/>
+      <c r="A6" s="121"/>
+      <c r="B6" s="139"/>
+      <c r="C6" s="121"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="153" x14ac:dyDescent="0.2">
       <c r="A7" s="59" t="s">
@@ -31520,67 +32146,67 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="116" t="s">
+      <c r="A8" s="120" t="s">
         <v>376</v>
       </c>
-      <c r="B8" s="133" t="s">
+      <c r="B8" s="137" t="s">
         <v>375</v>
       </c>
-      <c r="C8" s="116" t="s">
+      <c r="C8" s="120" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="127"/>
-      <c r="B9" s="134"/>
-      <c r="C9" s="127"/>
+      <c r="A9" s="131"/>
+      <c r="B9" s="138"/>
+      <c r="C9" s="131"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="117"/>
-      <c r="B10" s="135"/>
-      <c r="C10" s="117"/>
+      <c r="A10" s="121"/>
+      <c r="B10" s="139"/>
+      <c r="C10" s="121"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="116" t="s">
+      <c r="A11" s="120" t="s">
         <v>378</v>
       </c>
-      <c r="B11" s="133" t="s">
+      <c r="B11" s="137" t="s">
         <v>384</v>
       </c>
-      <c r="C11" s="116" t="s">
+      <c r="C11" s="120" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="127"/>
-      <c r="B12" s="134"/>
-      <c r="C12" s="127"/>
+      <c r="A12" s="131"/>
+      <c r="B12" s="138"/>
+      <c r="C12" s="131"/>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="187" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="117"/>
-      <c r="B13" s="135"/>
-      <c r="C13" s="117"/>
+      <c r="A13" s="121"/>
+      <c r="B13" s="139"/>
+      <c r="C13" s="121"/>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="116" t="s">
+      <c r="A14" s="120" t="s">
         <v>380</v>
       </c>
-      <c r="B14" s="133" t="s">
+      <c r="B14" s="137" t="s">
         <v>383</v>
       </c>
-      <c r="C14" s="116" t="s">
+      <c r="C14" s="120" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="127"/>
-      <c r="B15" s="134"/>
-      <c r="C15" s="127"/>
+      <c r="A15" s="131"/>
+      <c r="B15" s="138"/>
+      <c r="C15" s="131"/>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="117"/>
-      <c r="B16" s="135"/>
-      <c r="C16" s="117"/>
+      <c r="A16" s="121"/>
+      <c r="B16" s="139"/>
+      <c r="C16" s="121"/>
     </row>
     <row r="17" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
@@ -31643,18 +32269,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="114" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="114"/>
-      <c r="C1" s="114"/>
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
     </row>
     <row r="2" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="120" t="s">
+      <c r="A2" s="124" t="s">
         <v>395</v>
       </c>
-      <c r="B2" s="120"/>
-      <c r="C2" s="120"/>
+      <c r="B2" s="124"/>
+      <c r="C2" s="124"/>
     </row>
     <row r="3" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -31677,217 +32303,217 @@
       <c r="C4" s="60"/>
     </row>
     <row r="5" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="120" t="s">
         <v>397</v>
       </c>
-      <c r="B5" s="136" t="s">
+      <c r="B5" s="140" t="s">
         <v>396</v>
       </c>
-      <c r="C5" s="116" t="s">
+      <c r="C5" s="120" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="13" customFormat="1" ht="283" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="127"/>
-      <c r="B6" s="137"/>
-      <c r="C6" s="127"/>
+      <c r="A6" s="131"/>
+      <c r="B6" s="141"/>
+      <c r="C6" s="131"/>
     </row>
     <row r="7" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="127"/>
-      <c r="B7" s="137"/>
-      <c r="C7" s="127"/>
+      <c r="A7" s="131"/>
+      <c r="B7" s="141"/>
+      <c r="C7" s="131"/>
     </row>
     <row r="8" spans="1:3" s="13" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="127"/>
-      <c r="B8" s="137"/>
-      <c r="C8" s="127"/>
+      <c r="A8" s="131"/>
+      <c r="B8" s="141"/>
+      <c r="C8" s="131"/>
     </row>
     <row r="9" spans="1:3" s="13" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="127"/>
-      <c r="B9" s="137"/>
-      <c r="C9" s="127"/>
+      <c r="A9" s="131"/>
+      <c r="B9" s="141"/>
+      <c r="C9" s="131"/>
     </row>
     <row r="10" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="127"/>
-      <c r="B10" s="137"/>
-      <c r="C10" s="127"/>
+      <c r="A10" s="131"/>
+      <c r="B10" s="141"/>
+      <c r="C10" s="131"/>
     </row>
     <row r="11" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="127"/>
-      <c r="B11" s="137"/>
-      <c r="C11" s="127"/>
+      <c r="A11" s="131"/>
+      <c r="B11" s="141"/>
+      <c r="C11" s="131"/>
     </row>
     <row r="12" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="117"/>
-      <c r="B12" s="138"/>
-      <c r="C12" s="117"/>
+      <c r="A12" s="121"/>
+      <c r="B12" s="142"/>
+      <c r="C12" s="121"/>
     </row>
     <row r="13" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="120" t="s">
         <v>399</v>
       </c>
-      <c r="B13" s="121" t="s">
+      <c r="B13" s="125" t="s">
         <v>400</v>
       </c>
-      <c r="C13" s="116" t="s">
+      <c r="C13" s="120" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="127"/>
-      <c r="B14" s="122"/>
-      <c r="C14" s="127"/>
+      <c r="A14" s="131"/>
+      <c r="B14" s="126"/>
+      <c r="C14" s="131"/>
     </row>
     <row r="15" spans="1:3" s="13" customFormat="1" ht="247" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="127"/>
-      <c r="B15" s="122"/>
-      <c r="C15" s="127"/>
+      <c r="A15" s="131"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="131"/>
     </row>
     <row r="16" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="127"/>
-      <c r="B16" s="121" t="s">
+      <c r="A16" s="131"/>
+      <c r="B16" s="125" t="s">
         <v>401</v>
       </c>
-      <c r="C16" s="127"/>
+      <c r="C16" s="131"/>
     </row>
     <row r="17" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="127"/>
-      <c r="B17" s="122"/>
-      <c r="C17" s="127"/>
+      <c r="A17" s="131"/>
+      <c r="B17" s="126"/>
+      <c r="C17" s="131"/>
     </row>
     <row r="18" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="127"/>
-      <c r="B18" s="122"/>
-      <c r="C18" s="127"/>
+      <c r="A18" s="131"/>
+      <c r="B18" s="126"/>
+      <c r="C18" s="131"/>
     </row>
     <row r="19" spans="1:3" s="13" customFormat="1" ht="159" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="127"/>
-      <c r="B19" s="122"/>
-      <c r="C19" s="127"/>
+      <c r="A19" s="131"/>
+      <c r="B19" s="126"/>
+      <c r="C19" s="131"/>
     </row>
     <row r="20" spans="1:3" s="13" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="127"/>
-      <c r="B20" s="122" t="s">
+      <c r="A20" s="131"/>
+      <c r="B20" s="126" t="s">
         <v>402</v>
       </c>
-      <c r="C20" s="127"/>
+      <c r="C20" s="131"/>
     </row>
     <row r="21" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="127"/>
-      <c r="B21" s="122"/>
-      <c r="C21" s="127"/>
+      <c r="A21" s="131"/>
+      <c r="B21" s="126"/>
+      <c r="C21" s="131"/>
     </row>
     <row r="22" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="127"/>
-      <c r="B22" s="122"/>
-      <c r="C22" s="127"/>
+      <c r="A22" s="131"/>
+      <c r="B22" s="126"/>
+      <c r="C22" s="131"/>
     </row>
     <row r="23" spans="1:3" ht="167" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="127"/>
-      <c r="B23" s="122"/>
-      <c r="C23" s="127"/>
+      <c r="A23" s="131"/>
+      <c r="B23" s="126"/>
+      <c r="C23" s="131"/>
     </row>
     <row r="24" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="127"/>
-      <c r="B24" s="122" t="s">
+      <c r="A24" s="131"/>
+      <c r="B24" s="126" t="s">
         <v>403</v>
       </c>
-      <c r="C24" s="127"/>
+      <c r="C24" s="131"/>
     </row>
     <row r="25" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="127"/>
-      <c r="B25" s="122"/>
-      <c r="C25" s="127"/>
+      <c r="A25" s="131"/>
+      <c r="B25" s="126"/>
+      <c r="C25" s="131"/>
     </row>
     <row r="26" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="127"/>
-      <c r="B26" s="122" t="s">
+      <c r="A26" s="131"/>
+      <c r="B26" s="126" t="s">
         <v>317</v>
       </c>
-      <c r="C26" s="127"/>
+      <c r="C26" s="131"/>
     </row>
     <row r="27" spans="1:3" ht="144" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="127"/>
-      <c r="B27" s="122"/>
-      <c r="C27" s="127"/>
+      <c r="A27" s="131"/>
+      <c r="B27" s="126"/>
+      <c r="C27" s="131"/>
     </row>
     <row r="28" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="127"/>
-      <c r="B28" s="122" t="s">
+      <c r="A28" s="131"/>
+      <c r="B28" s="126" t="s">
         <v>404</v>
       </c>
-      <c r="C28" s="127"/>
+      <c r="C28" s="131"/>
     </row>
     <row r="29" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="127"/>
-      <c r="B29" s="122"/>
-      <c r="C29" s="127"/>
+      <c r="A29" s="131"/>
+      <c r="B29" s="126"/>
+      <c r="C29" s="131"/>
     </row>
     <row r="30" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="127"/>
-      <c r="B30" s="122"/>
-      <c r="C30" s="127"/>
+      <c r="A30" s="131"/>
+      <c r="B30" s="126"/>
+      <c r="C30" s="131"/>
     </row>
     <row r="31" spans="1:3" ht="196" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="127"/>
-      <c r="B31" s="122"/>
-      <c r="C31" s="127"/>
+      <c r="A31" s="131"/>
+      <c r="B31" s="126"/>
+      <c r="C31" s="131"/>
     </row>
     <row r="32" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="127"/>
-      <c r="B32" s="122" t="s">
+      <c r="A32" s="131"/>
+      <c r="B32" s="126" t="s">
         <v>405</v>
       </c>
-      <c r="C32" s="127"/>
+      <c r="C32" s="131"/>
     </row>
     <row r="33" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="127"/>
-      <c r="B33" s="122"/>
-      <c r="C33" s="127"/>
+      <c r="A33" s="131"/>
+      <c r="B33" s="126"/>
+      <c r="C33" s="131"/>
     </row>
     <row r="34" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="127"/>
-      <c r="B34" s="122"/>
-      <c r="C34" s="127"/>
+      <c r="A34" s="131"/>
+      <c r="B34" s="126"/>
+      <c r="C34" s="131"/>
     </row>
     <row r="35" spans="1:3" ht="201" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="127"/>
-      <c r="B35" s="122"/>
-      <c r="C35" s="127"/>
+      <c r="A35" s="131"/>
+      <c r="B35" s="126"/>
+      <c r="C35" s="131"/>
     </row>
     <row r="36" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="127"/>
-      <c r="B36" s="122" t="s">
+      <c r="A36" s="131"/>
+      <c r="B36" s="126" t="s">
         <v>406</v>
       </c>
-      <c r="C36" s="127"/>
+      <c r="C36" s="131"/>
     </row>
     <row r="37" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="127"/>
-      <c r="B37" s="122"/>
-      <c r="C37" s="127"/>
+      <c r="A37" s="131"/>
+      <c r="B37" s="126"/>
+      <c r="C37" s="131"/>
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="127"/>
-      <c r="B38" s="122"/>
-      <c r="C38" s="127"/>
+      <c r="A38" s="131"/>
+      <c r="B38" s="126"/>
+      <c r="C38" s="131"/>
     </row>
     <row r="39" spans="1:3" ht="239" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="127"/>
-      <c r="B39" s="122"/>
-      <c r="C39" s="127"/>
+      <c r="A39" s="131"/>
+      <c r="B39" s="126"/>
+      <c r="C39" s="131"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="127"/>
-      <c r="B40" s="122" t="s">
+      <c r="A40" s="131"/>
+      <c r="B40" s="126" t="s">
         <v>407</v>
       </c>
-      <c r="C40" s="127"/>
+      <c r="C40" s="131"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="117"/>
-      <c r="B41" s="123"/>
-      <c r="C41" s="117"/>
+      <c r="A41" s="121"/>
+      <c r="B41" s="127"/>
+      <c r="C41" s="121"/>
     </row>
     <row r="42" spans="1:3" ht="136" x14ac:dyDescent="0.2">
       <c r="A42" s="60" t="s">
@@ -31927,11 +32553,11 @@
       <c r="C46" s="60"/>
     </row>
     <row r="47" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A47" s="120" t="s">
+      <c r="A47" s="124" t="s">
         <v>386</v>
       </c>
-      <c r="B47" s="120"/>
-      <c r="C47" s="120"/>
+      <c r="B47" s="124"/>
+      <c r="C47" s="124"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="14" t="s">
@@ -31945,25 +32571,25 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="116" t="s">
+      <c r="A49" s="120" t="s">
         <v>388</v>
       </c>
-      <c r="B49" s="118" t="s">
+      <c r="B49" s="122" t="s">
         <v>413</v>
       </c>
-      <c r="C49" s="116" t="s">
+      <c r="C49" s="120" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="127"/>
-      <c r="B50" s="139"/>
-      <c r="C50" s="127"/>
+      <c r="A50" s="131"/>
+      <c r="B50" s="143"/>
+      <c r="C50" s="131"/>
     </row>
     <row r="51" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="117"/>
-      <c r="B51" s="119"/>
-      <c r="C51" s="117"/>
+      <c r="A51" s="121"/>
+      <c r="B51" s="123"/>
+      <c r="C51" s="121"/>
     </row>
     <row r="52" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="54" t="s">
@@ -31977,91 +32603,91 @@
       </c>
     </row>
     <row r="53" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="116" t="s">
+      <c r="A53" s="120" t="s">
         <v>415</v>
       </c>
-      <c r="B53" s="140" t="s">
+      <c r="B53" s="144" t="s">
         <v>416</v>
       </c>
-      <c r="C53" s="116" t="s">
+      <c r="C53" s="120" t="s">
         <v>420</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="238" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="127"/>
-      <c r="B54" s="140"/>
-      <c r="C54" s="127"/>
+      <c r="A54" s="131"/>
+      <c r="B54" s="144"/>
+      <c r="C54" s="131"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="127"/>
-      <c r="B55" s="118" t="s">
+      <c r="A55" s="131"/>
+      <c r="B55" s="122" t="s">
         <v>417</v>
       </c>
-      <c r="C55" s="127"/>
+      <c r="C55" s="131"/>
     </row>
     <row r="56" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="127"/>
-      <c r="B56" s="139"/>
-      <c r="C56" s="127"/>
+      <c r="A56" s="131"/>
+      <c r="B56" s="143"/>
+      <c r="C56" s="131"/>
     </row>
     <row r="57" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="127"/>
-      <c r="B57" s="139"/>
-      <c r="C57" s="127"/>
+      <c r="A57" s="131"/>
+      <c r="B57" s="143"/>
+      <c r="C57" s="131"/>
     </row>
     <row r="58" spans="1:3" ht="172" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="127"/>
-      <c r="B58" s="119"/>
-      <c r="C58" s="127"/>
+      <c r="A58" s="131"/>
+      <c r="B58" s="123"/>
+      <c r="C58" s="131"/>
     </row>
     <row r="59" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="127"/>
-      <c r="B59" s="118" t="s">
+      <c r="A59" s="131"/>
+      <c r="B59" s="122" t="s">
         <v>418</v>
       </c>
-      <c r="C59" s="127"/>
+      <c r="C59" s="131"/>
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="127"/>
-      <c r="B60" s="139"/>
-      <c r="C60" s="127"/>
+      <c r="A60" s="131"/>
+      <c r="B60" s="143"/>
+      <c r="C60" s="131"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="127"/>
-      <c r="B61" s="139"/>
-      <c r="C61" s="127"/>
+      <c r="A61" s="131"/>
+      <c r="B61" s="143"/>
+      <c r="C61" s="131"/>
     </row>
     <row r="62" spans="1:3" ht="125" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="127"/>
-      <c r="B62" s="119"/>
-      <c r="C62" s="127"/>
+      <c r="A62" s="131"/>
+      <c r="B62" s="123"/>
+      <c r="C62" s="131"/>
     </row>
     <row r="63" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="127"/>
-      <c r="B63" s="118" t="s">
+      <c r="A63" s="131"/>
+      <c r="B63" s="122" t="s">
         <v>419</v>
       </c>
-      <c r="C63" s="127"/>
+      <c r="C63" s="131"/>
     </row>
     <row r="64" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="127"/>
-      <c r="B64" s="139"/>
-      <c r="C64" s="127"/>
+      <c r="A64" s="131"/>
+      <c r="B64" s="143"/>
+      <c r="C64" s="131"/>
     </row>
     <row r="65" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="127"/>
-      <c r="B65" s="139"/>
-      <c r="C65" s="127"/>
+      <c r="A65" s="131"/>
+      <c r="B65" s="143"/>
+      <c r="C65" s="131"/>
     </row>
     <row r="66" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="127"/>
-      <c r="B66" s="139"/>
-      <c r="C66" s="127"/>
+      <c r="A66" s="131"/>
+      <c r="B66" s="143"/>
+      <c r="C66" s="131"/>
     </row>
     <row r="67" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="117"/>
-      <c r="B67" s="119"/>
-      <c r="C67" s="117"/>
+      <c r="A67" s="121"/>
+      <c r="B67" s="123"/>
+      <c r="C67" s="121"/>
     </row>
     <row r="68" spans="1:3" ht="105" x14ac:dyDescent="0.2">
       <c r="A68" s="60" t="s">

</xml_diff>

<commit_message>
Updated html/index.html and all associated files to remove hard coded string labels and messages
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3724C38C-00E4-0642-BB83-68D2C479E8ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91007E0E-8984-514E-8F12-6B66A0CBD483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16160" firstSheet="14" activeTab="24" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16160" firstSheet="15" activeTab="25" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="SPEC - 1.1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,10 @@
     <sheet name="SPEC - 3.8" sheetId="27" r:id="rId23"/>
     <sheet name="SPEC - 3.9" sheetId="28" r:id="rId24"/>
     <sheet name="SPEC - 4.0" sheetId="29" r:id="rId25"/>
-    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId26"/>
-    <sheet name="PLAYGROUND" sheetId="6" r:id="rId27"/>
-    <sheet name="TEMPLATE" sheetId="8" r:id="rId28"/>
+    <sheet name="SPEC - 4.1" sheetId="30" r:id="rId26"/>
+    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId27"/>
+    <sheet name="PLAYGROUND" sheetId="6" r:id="rId28"/>
+    <sheet name="TEMPLATE" sheetId="8" r:id="rId29"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="909">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1222" uniqueCount="923">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -27347,6 +27348,700 @@
         modified:   js/controller/lock-selection-survey-customer-card.js
         modified:   js/controller/lock-selection-survey-sales-person-card.js
         new file:   lib/lang/en/enum/page/lock-selection-survey-enum.js</t>
+    </r>
+  </si>
+  <si>
+    <t>UPDATE THE html/index.html FILE AND ALL ASSOCIATED FILES TO REMOVE HARD CODED STRINGS</t>
+  </si>
+  <si>
+    <r>
+      <t>Update the file</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> html/index.html </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>to remove all hard coded strings</t>
+    </r>
+  </si>
+  <si>
+    <t>&lt;!DOCTYPE html&gt;
+&lt;html lang="en"&gt;
+  &lt;head&gt;
+    &lt;!-- Required meta tags --&gt;
+    &lt;meta charset="UTF-8"&gt;
+    &lt;meta http-equiv="X-UA-Compatible" content="IE=edge"&gt;
+    &lt;meta name="viewport"
+      content="width=device-width, initial-scale=1.0, shrink-to-fit=no"&gt;
+    &lt;!-- Bootstrap v 4.6.0 Style Sheet --&gt;
+    &lt;link rel="stylesheet"
+      href="https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/css/bootstrap.min.css"
+      integrity="sha384-B0vP5xmATw1+K9KRQjQERJvTumQW0nPEzvF6L/Z6nronJ3oUOFUFpCjEUQouq2+l"
+      crossorigin="anonymous"&gt;
+    &lt;!-- Custom Styles CSS --&gt;
+    &lt;link rel="stylesheet" type="text/css" href="./../css/global.css"&gt;
+    &lt;link rel="stylesheet" type="text/css" href="./../css/index.css"&gt;
+    &lt;!-- Font Awesome Kit --&gt;
+    &lt;script src="https://kit.fontawesome.com/94f1334f9a.js"
+      crossorigin="anonymous"&gt;&lt;/script&gt;
+    &lt;!-- Google Fonts --&gt;
+    &lt;link rel="preconnect" href="https://fonts.googleapis.com"&gt;
+    &lt;link rel="preconnect" href="https://fonts.gstatic.com" crossorigin&gt;
+    &lt;link
+      href="https://fonts.googleapis.com/css2?family=Noto+Sans+JP&amp;display=swap"
+      rel="stylesheet"&gt;
+    &lt;!-- Favicon --&gt;
+    &lt;link rel="shortcut icon" type="image/ico"
+      href="./../favicon/favicon.ico" /&gt;
+    &lt;!-- Page Title --&gt;
+    &lt;title&gt;&lt;/title&gt;
+  &lt;/head&gt;
+  &lt;body class="page-fade-in"&gt;
+    &lt;!-- Page Header --&gt;
+    &lt;div id="page-header" class="container-fluid"&gt;
+    &lt;/div&gt;
+    &lt;!-- End Page Header --&gt;
+    &lt;!-- Hafele Logo --&gt;
+    &lt;div id="hafele-logo"&gt;
+      &lt;img id="hafele-logo-img" src="./../assets/images/HAFELE-LOGO.jpg"
+        alt="Hafele"&gt;
+    &lt;/div&gt;
+    &lt;!-- End Hafele Logo --&gt;
+    &lt;!-- Main container --&gt;
+    &lt;div id="page-body" class="container"&gt;
+      &lt;!-- Row 1  --&gt;
+      &lt;div class="row"&gt;
+        &lt;!-- Row 1 Column 1 --&gt;
+        &lt;div class="col-lg-6 col-md-6 col-margin"&gt;
+          &lt;!-- Lock Selection Card --&gt;
+          &lt;div class="card h-100"&gt;
+            &lt;!-- Lock Selection Card Header --&gt;
+            &lt;div class="card-header card-header-extended"&gt;
+              &lt;h5 id="lock-selection-card-header"&gt;&lt;/h5&gt;
+            &lt;/div&gt;
+            &lt;!-- End Lock Selection Card Header --&gt;
+            &lt;!-- Lock Selection Card Body --&gt;
+            &lt;div class="card-body"&gt;
+              &lt;!-- Lock Model Selection Field --&gt;
+              &lt;div id="lock-model-selection-div" class="form-group"&gt;
+                &lt;div class="input-group"&gt;
+                  &lt;div class="input-group-prepend"&gt;
+                    &lt;span class="input-group-text"&gt;&lt;i
+                        class="fa-solid fa-lock"&gt;&lt;/i&gt;&lt;/span&gt;
+                  &lt;/div&gt;
+                  &lt;select id="lock-model-group"
+                    class="custom-select custom-select-extended"&gt;
+                    &lt;optgroup&gt;
+                      &lt;option id="label-lock-model" value="" selected&gt;&lt;/option&gt;
+                    &lt;/optgroup&gt;
+                  &lt;/select&gt;
+                &lt;/div&gt;
+              &lt;/div&gt;
+              &lt;!-- End Lock Model Selection Field --&gt;
+              &lt;div id="suggestion" class="hide-suggestion"&gt;
+                &lt;p id="suitability-message"&gt;&lt;/p&gt;
+                &lt;p id="door-type"&gt;&lt;/p&gt;
+                &lt;p id="door-thickness"&gt;&lt;/p&gt;
+              &lt;/div&gt;
+            &lt;/div&gt;
+            &lt;!-- End Lock Selection Card Body --&gt;
+            &lt;!-- Lock Selection Card Footer --&gt;
+            &lt;div class="card-footer text-center card-footer-extended"&gt;
+              &lt;form action="./lock-selection-survey.html"&gt;
+                &lt;input id="lock-selection-next" class="btn btn-success"
+                  type="submit" value=""&gt;
+              &lt;/form&gt;
+            &lt;/div&gt;
+            &lt;!-- End Lock Selection Card Footer --&gt;
+          &lt;/div&gt;
+          &lt;!-- End Lock Selection Card --&gt;
+        &lt;/div&gt;
+        &lt;!-- End Row 1 Column 1 --&gt;
+        &lt;!-- Row 1 Column 2 --&gt;
+        &lt;div class="col-lg-6 col-md-6 col-margin"&gt;
+          &lt;!-- Door Specification Card --&gt;
+          &lt;div class="card h-100"&gt;
+            &lt;!-- Door Specification Card Header --&gt;
+            &lt;div class="card-header card-header-extended"&gt;
+              &lt;h5 id="door-specification-header"&gt;&lt;/h5&gt;
+            &lt;/div&gt;
+            &lt;!-- End Door Specification Card Header --&gt;
+            &lt;!-- Door Specification Card Body --&gt;
+            &lt;div class="card-body"&gt;
+              &lt;div id="message"&gt;
+                &lt;p id="proceed-message"&gt;&lt;/p&gt;
+              &lt;/div&gt;
+            &lt;/div&gt;
+            &lt;!-- End Door Specification Card Body --&gt;
+            &lt;!-- Door Specification Card Footer --&gt;
+            &lt;div class="card-footer text-center card-footer-extended"&gt;
+              &lt;form action="./lock-selection-survey.html"&gt;
+                &lt;input id="door-specification-next" class="btn btn-primary"
+                  type="submit" value=""&gt;
+              &lt;/form&gt;
+            &lt;/div&gt;
+            &lt;!-- End Door Specification Card Footer --&gt;
+          &lt;/div&gt;
+          &lt;!-- End Door Specification Card --&gt;
+        &lt;/div&gt;
+        &lt;!-- End Row 1 Column 2 --&gt;
+      &lt;/div&gt;
+      &lt;!-- End Row 1  --&gt;
+    &lt;/div&gt;
+    &lt;!-- End Main container --&gt;
+    &lt;!-- Spacer div --&gt;
+    &lt;div id="spacer"&gt;
+      &lt;!-- A &lt;div&gt; having the same heigh as the &lt;footer&gt; tag to prevent contents of &lt;body&gt;
+        from going under the absolutely positioned &lt;footer&gt; tag when screen resizes. --&gt;
+    &lt;/div&gt;
+    &lt;!-- End div --&gt;
+    &lt;!-- Page Footer --&gt;
+    &lt;footer id="page-footer" class="container-fluid" text-center&gt;
+      &lt;p class="copyright"&gt;Copyright © Hafele 2022&lt;/p&gt;
+    &lt;/footer&gt;
+    &lt;!-- End Page Footer --&gt;
+    &lt;!-- Bootstrap v 4.6.0 javascript --&gt;
+    &lt;script src="https://code.jquery.com/jquery-3.5.1.slim.min.js"
+      integrity="sha384-DfXdz2htPH0lsSSs5nCTpuj/zy4C+OGpamoFVy38MVBnE+IbbVYUew+OrCXaRkfj"
+      crossorigin="anonymous"&gt;
+    &lt;/script&gt;
+    &lt;script
+      src="https://cdn.jsdelivr.net/npm/popper.js@1.16.1/dist/umd/popper.min.js"
+      integrity="sha384-9/reFTGAW83EW2RDu2S0VKaIzap3H66lZH81PoYlFhbGU+6BZp6G7niu735Sk7lN"
+      crossorigin="anonymous"&gt;
+    &lt;/script&gt;
+    &lt;script
+      src="https://cdn.jsdelivr.net/npm/bootstrap@4.6.0/dist/js/bootstrap.min.js"
+      integrity="sha384-+YQ4JLhjyBLPDQt//I+STsc9iw4uQqACwlvpslubQzn4u2UU2UFM80nGisd026JF"
+      crossorigin="anonymous"&gt;
+    &lt;/script&gt;
+    &lt;!-- Information Capture Javascript --&gt;
+    &lt;script src="https://apis.google.com/js/api.js"&gt;&lt;/script&gt;
+    &lt;script src="./../lib/lang/en/enum/page/index-enum.js"
+      type="text/javascript"&gt;&lt;/script&gt;
+    &lt;script src="./../lib/lang/en/enum/door/door-enum.js"
+      type="text/javascript"&gt;&lt;/script&gt;
+    &lt;script src="./../lib/lang/en/enum/lock/lock-enum.js"
+      type="text/javascript"&gt;&lt;/script&gt;
+    &lt;script src="./../js/controller/lock-compatibility.js"
+      type="text/javascript"&gt;&lt;/script&gt;
+    &lt;script src="./../js/controller/index.js" type="text/javascript"&gt;&lt;/script&gt;
+  &lt;/body&gt;
+&lt;/html&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lib/lang/en/enum/page/index-enum.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Created the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lib/lang/en/enum/page/index-enum.js</t>
+    </r>
+  </si>
+  <si>
+    <t>touch lib/lang/en/enum/page/index-enum.js</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implement the constant </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>INDEX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>LOCK_SELECTION_CARD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>DOOR_SPECIFICATION_CARD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>NAVIGATION_BUTTONS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">lib/lang/en/enum/page/index-enum.js </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">to hold all string constants related to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html/index.html</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Implemented the constant </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>INDEX</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>LOCK_SELECTION_CARD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>DOOR_SPECIFICATION_CARD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>NAVIGATION_BUTTONS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">lib/lang/en/enum/page/index-enum.js </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">to hold all string constants related to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html/index.html</t>
+    </r>
+  </si>
+  <si>
+    <t>"use strict";
+/* * JavaScript for the file index.html
+ *  @author Sanket Rajgarhia
+ *  @date   22/04/2022 (dd/mm/yyyy)
+ *  @version 1.0
+ * */
+/*****************************************************************************/
+/* PAGE COMPONENT ENUMERATIONS                                               */
+/*****************************************************************************/
+// index page title (EN)
+const INDEX = {
+    TITLE: "Lock Selection Survey",
+};
+// Lock selection card
+const LOCK_SELECTION_CARD = {
+    HEADER: "Lock Model Lookup",
+    LABEL_LOCK_MODEL: "Lock Model",
+    SUITABILITY_MESSAGE: "This lock is suitable for the following door type",
+    LABEL_DOOR_TYPE: "Door Type : ",
+    LABEL_DOOR_THICKNESS: "Door Thickness Range : ",
+};
+// Door specification card
+const DOOR_SPECIFICATION_CARD = {
+    HEADER: "Door Specification",
+    PROCEED_MESSAGE: `Click on the ` +
+        `&lt;span id="label-next" class="highlight-text"&gt;&lt;/span&gt; ` +
+        `button and provide the door specification to determine the ` +
+        `suitability of a lock model.`,
+    LABEL_NEXT: "Next",
+};
+// Navigation buttons
+const NAVIGATION_BUTTONS = {
+    SELECT_BUTTON: "     Select     ",
+    NEXT_BUTTON: "      Next      "
+};
+/*****************************************************************************/
+/* FREEZE - TO EMULATE ENUMERATION                                           */
+/*****************************************************************************/
+// Prevent addition of properties to the json Object
+Object.freeze(INDEX);
+Object.freeze(LOCK_SELECTION_CARD);
+Object.freeze(DOOR_SPECIFICATION_CARD);
+Object.freeze(NAVIGATION_BUTTONS);
+/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">/* Anonymous function fired on window load. 
+ * @param    
+ * @return   
+ * */
+window.onload = function() {
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">// Setup the index page
+    let titleElement = document.getElementsByTagName("title")[0];
+    titleElement.innerHTML = INDEX.TITLE;
+    // Lock selection card setup
+    let lockSelectionCardHeader = document.getElementById("lock-selection-card-header");
+    lockSelectionCardHeader.innerHTML = LOCK_SELECTION_CARD.HEADER;
+    let labelLockModel = document.getElementById("label-lock-model");
+    labelLockModel.innerHTML = LOCK_SELECTION_CARD.LABEL_LOCK_MODEL;
+    let suitabilityMessage = document.getElementById("suitability-message");
+    suitabilityMessage.innerHTML = LOCK_SELECTION_CARD.SUITABILITY_MESSAGE;
+    let doorType = document.getElementById("door-type");
+    doorType.innerHTML = `&lt;span class="field-name"&gt;` +
+        LOCK_SELECTION_CARD.LABEL_DOOR_TYPE + `&lt;/span&gt;` +
+        `&lt;span id="type-value"&gt;&lt;/span&gt;`;
+    let doorThicknessRange = document.getElementById("door-thickness");
+    doorThicknessRange.innerHTML = `&lt;span class="field-name"&gt;` +
+        LOCK_SELECTION_CARD.LABEL_DOOR_THICKNESS + `&lt;/span&gt;` +
+        `&lt;span id="thickness-value"&gt;&lt;/span&gt;`;
+    // Select buttons of the lock selection card
+    let navLockSelectionNextButton = document.getElementById("lock-selection-next");
+    navLockSelectionNextButton.setAttribute("value", NAVIGATION_BUTTONS.SELECT_BUTTON);
+    // Door selection card setup
+    let doorSelectionCardHeader = document.getElementById("door-specification-header");
+    doorSelectionCardHeader.innerHTML = DOOR_SPECIFICATION_CARD.HEADER;
+    let proceedMessage = document.getElementById("proceed-message");
+    proceedMessage.innerHTML = DOOR_SPECIFICATION_CARD.PROCEED_MESSAGE;
+    let labelNext = document.getElementById("label-next");
+    labelNext.innerHTML = DOOR_SPECIFICATION_CARD.LABEL_NEXT;
+    // Next buttons of the door selection card
+    let navDoorSpecificationNextButton = document.getElementById("door-specification-next");
+    navDoorSpecificationNextButton.setAttribute("value", NAVIGATION_BUTTONS.NEXT_BUTTON);
+   </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> // Add all the swing door - lock model name options to the lock model
+    // group selection combo box
+    let optionGroup = document.createElement("optgroup");
+    optionGroup.setAttribute("label", DOOR_TYPE.SWING_DOOR);
+    let optionGroupAdded = false;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>window.onload</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> function in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller/index.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to accommodate page heading strings for the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html/index.html</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>window.onload</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> function in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller/index.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to accommodate page heading strings for the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>html/index.html</t>
+    </r>
+  </si>
+  <si>
+    <t>git commit -m "Updated html/index.html and all associated files to remove hard coded string labels and messages"</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>git status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - would display the following files.                                                                                                                                                                                                                                  On branch master
+On branch master
+Your branch is up to date with 'hafele/master'.
+Changes to be committed:
+  (use "git restore --staged &lt;file&gt;..." to unstage)
+        modified:   docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+        modified:   html/index.html
+        modified:   js/controller/index.js
+        new file:   lib/lang/en/enum/page/index-enum.js</t>
     </r>
   </si>
 </sst>
@@ -27791,7 +28486,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -28121,6 +28816,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -32319,7 +33017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE904D94-AEA6-6F4F-8A3D-7CB349DD1102}">
   <dimension ref="A1:C60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -32823,6 +33521,172 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6E753B-E0CC-704C-B072-EF39993671C4}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+    </row>
+    <row r="2" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="94" t="s">
+        <v>909</v>
+      </c>
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+    </row>
+    <row r="3" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="90" t="s">
+        <v>910</v>
+      </c>
+      <c r="B4" s="92" t="s">
+        <v>911</v>
+      </c>
+      <c r="C4" s="90" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="101"/>
+      <c r="B5" s="113"/>
+      <c r="C5" s="101"/>
+    </row>
+    <row r="6" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="101"/>
+      <c r="B6" s="113"/>
+      <c r="C6" s="101"/>
+    </row>
+    <row r="7" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="101"/>
+      <c r="B7" s="113"/>
+      <c r="C7" s="101"/>
+    </row>
+    <row r="8" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="101"/>
+      <c r="B8" s="113"/>
+      <c r="C8" s="101"/>
+    </row>
+    <row r="9" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="101"/>
+      <c r="B9" s="113"/>
+      <c r="C9" s="101"/>
+    </row>
+    <row r="10" spans="1:3" ht="337" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="101"/>
+      <c r="B10" s="93"/>
+      <c r="C10" s="101"/>
+    </row>
+    <row r="11" spans="1:3" s="86" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="87" t="s">
+        <v>912</v>
+      </c>
+      <c r="B11" s="61" t="s">
+        <v>914</v>
+      </c>
+      <c r="C11" s="53" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="86" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="90" t="s">
+        <v>915</v>
+      </c>
+      <c r="B12" s="92" t="s">
+        <v>917</v>
+      </c>
+      <c r="C12" s="90" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="101"/>
+      <c r="B13" s="113"/>
+      <c r="C13" s="101"/>
+    </row>
+    <row r="14" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="90" t="s">
+        <v>919</v>
+      </c>
+      <c r="B14" s="127" t="s">
+        <v>918</v>
+      </c>
+      <c r="C14" s="90" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="86" customFormat="1" ht="283" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="91"/>
+      <c r="B15" s="93"/>
+      <c r="C15" s="91"/>
+    </row>
+    <row r="16" spans="1:3" ht="204" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" s="49" t="s">
+        <v>921</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>463</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="11">
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="A4:A10"/>
+    <mergeCell ref="C4:C10"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE113606-3FFA-8545-9BE3-5643B52A7CE9}">
   <dimension ref="A1:H116"/>
   <sheetViews>
@@ -32900,10 +33764,10 @@
       <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="127" t="s">
+      <c r="A6" s="128" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="127"/>
+      <c r="B6" s="128"/>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
@@ -33876,32 +34740,32 @@
       <c r="H73" s="20"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="128"/>
-      <c r="B74" s="129"/>
+      <c r="A74" s="129"/>
+      <c r="B74" s="130"/>
       <c r="C74" s="29" t="s">
         <v>225</v>
       </c>
       <c r="D74" s="29" t="s">
         <v>227</v>
       </c>
-      <c r="E74" s="130"/>
-      <c r="F74" s="128"/>
-      <c r="G74" s="132"/>
-      <c r="H74" s="128"/>
+      <c r="E74" s="131"/>
+      <c r="F74" s="129"/>
+      <c r="G74" s="133"/>
+      <c r="H74" s="129"/>
     </row>
     <row r="75" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A75" s="128"/>
-      <c r="B75" s="129"/>
+      <c r="A75" s="129"/>
+      <c r="B75" s="130"/>
       <c r="C75" s="30" t="s">
         <v>226</v>
       </c>
       <c r="D75" s="30" t="s">
         <v>228</v>
       </c>
-      <c r="E75" s="130"/>
-      <c r="F75" s="128"/>
-      <c r="G75" s="132"/>
-      <c r="H75" s="128"/>
+      <c r="E75" s="131"/>
+      <c r="F75" s="129"/>
+      <c r="G75" s="133"/>
+      <c r="H75" s="129"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="20"/>
@@ -34074,34 +34938,34 @@
       <c r="H88" s="20"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="128"/>
-      <c r="B89" s="128"/>
+      <c r="A89" s="129"/>
+      <c r="B89" s="129"/>
       <c r="C89" s="32" t="s">
         <v>225</v>
       </c>
       <c r="D89" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="E89" s="131" t="s">
+      <c r="E89" s="132" t="s">
         <v>121</v>
       </c>
-      <c r="F89" s="131"/>
-      <c r="G89" s="132"/>
-      <c r="H89" s="128"/>
+      <c r="F89" s="132"/>
+      <c r="G89" s="133"/>
+      <c r="H89" s="129"/>
     </row>
     <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A90" s="128"/>
-      <c r="B90" s="128"/>
+      <c r="A90" s="129"/>
+      <c r="B90" s="129"/>
       <c r="C90" s="32" t="s">
         <v>242</v>
       </c>
       <c r="D90" s="32" t="s">
         <v>243</v>
       </c>
-      <c r="E90" s="131"/>
-      <c r="F90" s="131"/>
-      <c r="G90" s="132"/>
-      <c r="H90" s="128"/>
+      <c r="E90" s="132"/>
+      <c r="F90" s="132"/>
+      <c r="G90" s="133"/>
+      <c r="H90" s="129"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="20"/>
@@ -34487,7 +35351,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -34585,7 +35449,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0BB7-C151-C94B-945C-E2CA92034B13}">
   <dimension ref="A1:C15"/>
   <sheetViews>

</xml_diff>

<commit_message>
Implemented changes to the report for Customer Additional Information and Sales Location fields being empty
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8217A3A-1E54-6D43-9061-B8DF480FE091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BE7088-F391-7040-8EF6-A3D0ACFFCDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" firstSheet="23" activeTab="33" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" firstSheet="24" activeTab="34" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="SPEC - 1.1" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,10 @@
     <sheet name="SPEC - 4.7" sheetId="37" r:id="rId32"/>
     <sheet name="SPEC - 4.8" sheetId="38" r:id="rId33"/>
     <sheet name="SPEC - 4.9" sheetId="39" r:id="rId34"/>
-    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId35"/>
-    <sheet name="PLAYGROUND" sheetId="6" r:id="rId36"/>
-    <sheet name="TEMPLATE" sheetId="8" r:id="rId37"/>
+    <sheet name="SPEC - 5.0" sheetId="40" r:id="rId35"/>
+    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId36"/>
+    <sheet name="PLAYGROUND" sheetId="6" r:id="rId37"/>
+    <sheet name="TEMPLATE" sheetId="8" r:id="rId38"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -69,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1580" uniqueCount="1196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1594" uniqueCount="1202">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -40142,6 +40143,219 @@
   </si>
   <si>
     <t>git commit -m "Updated the mechanism for displaying and hiding options for door leaf field and installation location field."</t>
+  </si>
+  <si>
+    <t>UPDATE MULTILINE HANDLING OF CUSTOMER ADDITIONAL INFORMATION AND SALES PERSON LOCATION IN js/controller/survey-report.js</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">    let customerData = sessionStorage.getItem("customerData");
+        if (customerData !== null) {
+            customerData = JSON.parse(customerData);
+            formatReportFields("customerName",
+                REPORT_FIELD.CUSTOMER_NAME.toUpperCase(),
+                customerData.customerName.toUpperCase());
+            formatReportFields("customerMobile",
+                REPORT_FIELD.CUSTOMER_MOBILE.toUpperCase(),
+                customerData.customerMobile.toUpperCase());
+            formatReportFields("customerAddress",
+                REPORT_FIELD.CUSTOMER_ADDRESS.toUpperCase(),
+                customerData.customerAddress1.toUpperCase() + "\n" +
+                customerData.customerAddress2.toUpperCase() + "\n" +
+                customerData.customerAddress3.toUpperCase());
+            let customerInformation = customerData.customerInformation.toUpperCase();
+            let customerInformationLines = customerInformation.match(/(.|[\r\n]){1,50}/g);
+            customerInformation = "";
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">            if (customerInformationLines !== null) {
+                for (let line of customerInformationLines) {
+                    customerInformation += line + "\n ";
+                }
+            }
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">           formatReportFields("customerInformation",
+                REPORT_FIELD.CUSTOMER_INFORMATION.toUpperCase(), customerInformation);
+        }
+        let salesPersonData = sessionStorage.getItem("salesPersonData");
+        if (salesPersonData !== null) {
+            salesPersonData = JSON.parse(salesPersonData);
+            formatReportFields("salesPersonID",
+                REPORT_FIELD.SALES_PERSON_ID.toUpperCase(),
+                salesPersonData.salesPersonID.toUpperCase());
+            formatReportFields("salesPersonName",
+                REPORT_FIELD.SALES_PERSON_NAME.toUpperCase(),
+                salesPersonData.salesPersonName.toUpperCase());
+            let salesPersonLocation = salesPersonData.salesPersonLocation.toUpperCase();
+            let salesPersonLocationLines = salesPersonLocation.match(/(.|[\r\n]){1,50}/g);
+            salesPersonLocation = "";</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+            if (salesPersonLocationLines !== null) {
+                for (let line of salesPersonLocationLines) {
+                    salesPersonLocation += line + "\n ";
+                }
+            }
+            </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>formatReportFields("salesPersonLocation",
+                REPORT_FIELD.SALES_PERSON_LOCATION.toUpperCase(),
+                salesPersonLocation.toUpperCase());
+        }
+        let lockAndDoorData = sessionStorage.getItem("lockAndDoorData");
+        if (lockAndDoorData !== null) {</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">window.onload </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">function in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller/survey-report.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to handle for cases when Customer additional information and Sales Location does not have any value.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">window.onload </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">function in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller/survey-report.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to handle for cases when Customer additional information and Sales Location does not have any value.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>git status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - would display the following files.                                                                                                                                                                                                                                  On branch master
+Your branch is up to date with 'hafele/master'.
+Changes to be committed:
+  (use "git restore --staged &lt;file&gt;..." to unstage)
+        modified:   docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+        modified:   js/controller/survey-report.js
+</t>
+    </r>
+  </si>
+  <si>
+    <t>git commit -m "Implemented changes to the report for Customer Additional Information and Sales Location fields being empty"</t>
   </si>
 </sst>
 </file>
@@ -40952,12 +41166,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -40965,6 +41173,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -40991,16 +41205,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -41018,19 +41232,19 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -42478,14 +42692,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="17">
-    <mergeCell ref="B12:B18"/>
-    <mergeCell ref="A12:A18"/>
-    <mergeCell ref="C12:C18"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="C8:C10"/>
     <mergeCell ref="B30:B33"/>
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="C30:C33"/>
@@ -42495,6 +42701,14 @@
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="C27:C29"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="A12:A18"/>
+    <mergeCell ref="C12:C18"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -43102,12 +43316,12 @@
     </row>
     <row r="34" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="115"/>
-      <c r="B34" s="125"/>
+      <c r="B34" s="127"/>
       <c r="C34" s="115"/>
     </row>
     <row r="35" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="115"/>
-      <c r="B35" s="125"/>
+      <c r="B35" s="127"/>
       <c r="C35" s="115"/>
     </row>
     <row r="36" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
@@ -43124,27 +43338,27 @@
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="115"/>
-      <c r="B38" s="125"/>
+      <c r="B38" s="127"/>
       <c r="C38" s="115"/>
     </row>
     <row r="39" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="115"/>
-      <c r="B39" s="125"/>
+      <c r="B39" s="127"/>
       <c r="C39" s="115"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="115"/>
-      <c r="B40" s="125"/>
+      <c r="B40" s="127"/>
       <c r="C40" s="115"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="115"/>
-      <c r="B41" s="125"/>
+      <c r="B41" s="127"/>
       <c r="C41" s="115"/>
     </row>
     <row r="42" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="115"/>
-      <c r="B42" s="125"/>
+      <c r="B42" s="127"/>
       <c r="C42" s="115"/>
     </row>
     <row r="43" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -43156,32 +43370,32 @@
     </row>
     <row r="44" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="115"/>
-      <c r="B44" s="125"/>
+      <c r="B44" s="127"/>
       <c r="C44" s="115"/>
     </row>
     <row r="45" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="115"/>
-      <c r="B45" s="125"/>
+      <c r="B45" s="127"/>
       <c r="C45" s="115"/>
     </row>
     <row r="46" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="115"/>
-      <c r="B46" s="125"/>
+      <c r="B46" s="127"/>
       <c r="C46" s="115"/>
     </row>
     <row r="47" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="115"/>
-      <c r="B47" s="125"/>
+      <c r="B47" s="127"/>
       <c r="C47" s="115"/>
     </row>
     <row r="48" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="115"/>
-      <c r="B48" s="125"/>
+      <c r="B48" s="127"/>
       <c r="C48" s="115"/>
     </row>
     <row r="49" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="115"/>
-      <c r="B49" s="125"/>
+      <c r="B49" s="127"/>
       <c r="C49" s="115"/>
     </row>
     <row r="50" spans="1:3" ht="320" customHeight="1" x14ac:dyDescent="0.2">
@@ -43198,22 +43412,22 @@
     </row>
     <row r="52" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="115"/>
-      <c r="B52" s="125"/>
+      <c r="B52" s="127"/>
       <c r="C52" s="115"/>
     </row>
     <row r="53" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="115"/>
-      <c r="B53" s="125"/>
+      <c r="B53" s="127"/>
       <c r="C53" s="115"/>
     </row>
     <row r="54" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="115"/>
-      <c r="B54" s="125"/>
+      <c r="B54" s="127"/>
       <c r="C54" s="115"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="115"/>
-      <c r="B55" s="125"/>
+      <c r="B55" s="127"/>
       <c r="C55" s="115"/>
     </row>
     <row r="56" spans="1:3" ht="97" customHeight="1" x14ac:dyDescent="0.2">
@@ -43230,27 +43444,27 @@
     </row>
     <row r="58" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="115"/>
-      <c r="B58" s="125"/>
+      <c r="B58" s="127"/>
       <c r="C58" s="115"/>
     </row>
     <row r="59" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="115"/>
-      <c r="B59" s="125"/>
+      <c r="B59" s="127"/>
       <c r="C59" s="115"/>
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="115"/>
-      <c r="B60" s="125"/>
+      <c r="B60" s="127"/>
       <c r="C60" s="115"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="115"/>
-      <c r="B61" s="125"/>
+      <c r="B61" s="127"/>
       <c r="C61" s="115"/>
     </row>
     <row r="62" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="115"/>
-      <c r="B62" s="125"/>
+      <c r="B62" s="127"/>
       <c r="C62" s="115"/>
     </row>
     <row r="63" spans="1:3" ht="146" customHeight="1" x14ac:dyDescent="0.2">
@@ -43285,7 +43499,7 @@
       <c r="A67" s="116" t="s">
         <v>638</v>
       </c>
-      <c r="B67" s="124" t="s">
+      <c r="B67" s="128" t="s">
         <v>637</v>
       </c>
       <c r="C67" s="116" t="s">
@@ -43294,19 +43508,19 @@
     </row>
     <row r="68" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="116"/>
-      <c r="B68" s="124"/>
+      <c r="B68" s="128"/>
       <c r="C68" s="116"/>
     </row>
     <row r="69" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="116"/>
-      <c r="B69" s="124"/>
+      <c r="B69" s="128"/>
       <c r="C69" s="116"/>
     </row>
     <row r="70" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="116" t="s">
         <v>643</v>
       </c>
-      <c r="B70" s="124" t="s">
+      <c r="B70" s="128" t="s">
         <v>640</v>
       </c>
       <c r="C70" s="116" t="s">
@@ -43315,59 +43529,59 @@
     </row>
     <row r="71" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="116"/>
-      <c r="B71" s="124"/>
+      <c r="B71" s="128"/>
       <c r="C71" s="116"/>
     </row>
     <row r="72" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="116"/>
-      <c r="B72" s="124"/>
+      <c r="B72" s="128"/>
       <c r="C72" s="116"/>
     </row>
     <row r="73" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="116"/>
-      <c r="B73" s="124"/>
+      <c r="B73" s="128"/>
       <c r="C73" s="116"/>
     </row>
     <row r="74" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="116"/>
-      <c r="B74" s="124"/>
+      <c r="B74" s="128"/>
       <c r="C74" s="116"/>
     </row>
     <row r="75" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="116"/>
-      <c r="B75" s="124"/>
+      <c r="B75" s="128"/>
       <c r="C75" s="116"/>
     </row>
     <row r="76" spans="1:3" ht="214" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="116"/>
-      <c r="B76" s="124"/>
+      <c r="B76" s="128"/>
       <c r="C76" s="116"/>
     </row>
     <row r="77" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="116"/>
-      <c r="B77" s="124" t="s">
+      <c r="B77" s="128" t="s">
         <v>641</v>
       </c>
       <c r="C77" s="116"/>
     </row>
     <row r="78" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="116"/>
-      <c r="B78" s="124"/>
+      <c r="B78" s="128"/>
       <c r="C78" s="116"/>
     </row>
     <row r="79" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="116"/>
-      <c r="B79" s="124"/>
+      <c r="B79" s="128"/>
       <c r="C79" s="116"/>
     </row>
     <row r="80" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="116"/>
-      <c r="B80" s="124"/>
+      <c r="B80" s="128"/>
       <c r="C80" s="116"/>
     </row>
     <row r="81" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="116"/>
-      <c r="B81" s="124"/>
+      <c r="B81" s="128"/>
       <c r="C81" s="116"/>
     </row>
     <row r="82" spans="1:3" ht="56" x14ac:dyDescent="0.2">
@@ -43475,18 +43689,12 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="30">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="A16:A26"/>
-    <mergeCell ref="C16:C26"/>
+    <mergeCell ref="B77:B81"/>
+    <mergeCell ref="A70:A81"/>
+    <mergeCell ref="C70:C81"/>
+    <mergeCell ref="B86:B91"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="C86:C91"/>
     <mergeCell ref="B67:B69"/>
     <mergeCell ref="A67:A69"/>
     <mergeCell ref="C67:C69"/>
@@ -43499,12 +43707,18 @@
     <mergeCell ref="B33:B36"/>
     <mergeCell ref="B37:B42"/>
     <mergeCell ref="B43:B50"/>
-    <mergeCell ref="B77:B81"/>
-    <mergeCell ref="A70:A81"/>
-    <mergeCell ref="C70:C81"/>
-    <mergeCell ref="B86:B91"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="C86:C91"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="A16:A26"/>
+    <mergeCell ref="C16:C26"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="C8:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -44168,7 +44382,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="319" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="306" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
         <v>90</v>
       </c>
@@ -44723,17 +44937,17 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="11">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C11:C12"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="C13:C14"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="C11:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -44793,27 +45007,27 @@
     </row>
     <row r="5" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="115"/>
-      <c r="B5" s="125"/>
+      <c r="B5" s="127"/>
       <c r="C5" s="115"/>
     </row>
     <row r="6" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="115"/>
-      <c r="B6" s="125"/>
+      <c r="B6" s="127"/>
       <c r="C6" s="115"/>
     </row>
     <row r="7" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="115"/>
-      <c r="B7" s="125"/>
+      <c r="B7" s="127"/>
       <c r="C7" s="115"/>
     </row>
     <row r="8" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="115"/>
-      <c r="B8" s="125"/>
+      <c r="B8" s="127"/>
       <c r="C8" s="115"/>
     </row>
     <row r="9" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="115"/>
-      <c r="B9" s="125"/>
+      <c r="B9" s="127"/>
       <c r="C9" s="115"/>
     </row>
     <row r="10" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -45042,18 +45256,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="21">
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="A17:A26"/>
-    <mergeCell ref="C17:C26"/>
-    <mergeCell ref="B28:B34"/>
-    <mergeCell ref="A28:A34"/>
-    <mergeCell ref="C28:C34"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="C13:C15"/>
@@ -45063,6 +45265,18 @@
     <mergeCell ref="B4:B10"/>
     <mergeCell ref="A4:A10"/>
     <mergeCell ref="C4:C10"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A17:A26"/>
+    <mergeCell ref="C17:C26"/>
+    <mergeCell ref="B28:B34"/>
+    <mergeCell ref="A28:A34"/>
+    <mergeCell ref="C28:C34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="C37:C38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -45113,7 +45327,7 @@
       <c r="A4" s="116" t="s">
         <v>832</v>
       </c>
-      <c r="B4" s="124" t="s">
+      <c r="B4" s="128" t="s">
         <v>831</v>
       </c>
       <c r="C4" s="116" t="s">
@@ -45122,7 +45336,7 @@
     </row>
     <row r="5" spans="1:3" s="10" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="116"/>
-      <c r="B5" s="124"/>
+      <c r="B5" s="128"/>
       <c r="C5" s="116"/>
     </row>
     <row r="6" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -45267,27 +45481,27 @@
     </row>
     <row r="5" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="115"/>
-      <c r="B5" s="125"/>
+      <c r="B5" s="127"/>
       <c r="C5" s="115"/>
     </row>
     <row r="6" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="115"/>
-      <c r="B6" s="125"/>
+      <c r="B6" s="127"/>
       <c r="C6" s="115"/>
     </row>
     <row r="7" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="115"/>
-      <c r="B7" s="125"/>
+      <c r="B7" s="127"/>
       <c r="C7" s="115"/>
     </row>
     <row r="8" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="115"/>
-      <c r="B8" s="125"/>
+      <c r="B8" s="127"/>
       <c r="C8" s="115"/>
     </row>
     <row r="9" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="115"/>
-      <c r="B9" s="125"/>
+      <c r="B9" s="127"/>
       <c r="C9" s="115"/>
     </row>
     <row r="10" spans="1:3" ht="337" customHeight="1" x14ac:dyDescent="0.2">
@@ -45304,27 +45518,27 @@
     </row>
     <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="115"/>
-      <c r="B12" s="125"/>
+      <c r="B12" s="127"/>
       <c r="C12" s="115"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="115"/>
-      <c r="B13" s="125"/>
+      <c r="B13" s="127"/>
       <c r="C13" s="115"/>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="115"/>
-      <c r="B14" s="125"/>
+      <c r="B14" s="127"/>
       <c r="C14" s="115"/>
     </row>
     <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="115"/>
-      <c r="B15" s="125"/>
+      <c r="B15" s="127"/>
       <c r="C15" s="115"/>
     </row>
     <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="115"/>
-      <c r="B16" s="125"/>
+      <c r="B16" s="127"/>
       <c r="C16" s="115"/>
     </row>
     <row r="17" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
@@ -45341,27 +45555,27 @@
     </row>
     <row r="19" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="115"/>
-      <c r="B19" s="125"/>
+      <c r="B19" s="127"/>
       <c r="C19" s="115"/>
     </row>
     <row r="20" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="115"/>
-      <c r="B20" s="125"/>
+      <c r="B20" s="127"/>
       <c r="C20" s="115"/>
     </row>
     <row r="21" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="115"/>
-      <c r="B21" s="125"/>
+      <c r="B21" s="127"/>
       <c r="C21" s="115"/>
     </row>
     <row r="22" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="115"/>
-      <c r="B22" s="125"/>
+      <c r="B22" s="127"/>
       <c r="C22" s="115"/>
     </row>
     <row r="23" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="115"/>
-      <c r="B23" s="125"/>
+      <c r="B23" s="127"/>
       <c r="C23" s="115"/>
     </row>
     <row r="24" spans="1:3" s="86" customFormat="1" ht="121" customHeight="1" x14ac:dyDescent="0.2">
@@ -45405,7 +45619,7 @@
     </row>
     <row r="29" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="115"/>
-      <c r="B29" s="125"/>
+      <c r="B29" s="127"/>
       <c r="C29" s="115"/>
     </row>
     <row r="30" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -45433,7 +45647,7 @@
       <c r="A33" s="104" t="s">
         <v>865</v>
       </c>
-      <c r="B33" s="137" t="s">
+      <c r="B33" s="139" t="s">
         <v>864</v>
       </c>
       <c r="C33" s="104" t="s">
@@ -45449,7 +45663,7 @@
       <c r="A35" s="104" t="s">
         <v>868</v>
       </c>
-      <c r="B35" s="137" t="s">
+      <c r="B35" s="139" t="s">
         <v>867</v>
       </c>
       <c r="C35" s="104" t="s">
@@ -45458,7 +45672,7 @@
     </row>
     <row r="36" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="115"/>
-      <c r="B36" s="139"/>
+      <c r="B36" s="140"/>
       <c r="C36" s="115"/>
     </row>
     <row r="37" spans="1:3" s="86" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.2">
@@ -45470,7 +45684,7 @@
       <c r="A38" s="104" t="s">
         <v>871</v>
       </c>
-      <c r="B38" s="137" t="s">
+      <c r="B38" s="139" t="s">
         <v>870</v>
       </c>
       <c r="C38" s="104" t="s">
@@ -45497,7 +45711,7 @@
       <c r="A41" s="104" t="s">
         <v>876</v>
       </c>
-      <c r="B41" s="137" t="s">
+      <c r="B41" s="139" t="s">
         <v>877</v>
       </c>
       <c r="C41" s="104" t="s">
@@ -45513,7 +45727,7 @@
       <c r="A43" s="104" t="s">
         <v>880</v>
       </c>
-      <c r="B43" s="140" t="s">
+      <c r="B43" s="137" t="s">
         <v>879</v>
       </c>
       <c r="C43" s="104" t="s">
@@ -45529,7 +45743,7 @@
       <c r="A45" s="104" t="s">
         <v>883</v>
       </c>
-      <c r="B45" s="140" t="s">
+      <c r="B45" s="137" t="s">
         <v>882</v>
       </c>
       <c r="C45" s="104" t="s">
@@ -45545,7 +45759,7 @@
       <c r="A47" s="104" t="s">
         <v>885</v>
       </c>
-      <c r="B47" s="140" t="s">
+      <c r="B47" s="137" t="s">
         <v>887</v>
       </c>
       <c r="C47" s="104" t="s">
@@ -45561,7 +45775,7 @@
       <c r="A49" s="104" t="s">
         <v>888</v>
       </c>
-      <c r="B49" s="140" t="s">
+      <c r="B49" s="137" t="s">
         <v>890</v>
       </c>
       <c r="C49" s="104" t="s">
@@ -45577,7 +45791,7 @@
       <c r="A51" s="104" t="s">
         <v>892</v>
       </c>
-      <c r="B51" s="140" t="s">
+      <c r="B51" s="137" t="s">
         <v>891</v>
       </c>
       <c r="C51" s="104" t="s">
@@ -45593,7 +45807,7 @@
       <c r="A53" s="104" t="s">
         <v>895</v>
       </c>
-      <c r="B53" s="140" t="s">
+      <c r="B53" s="137" t="s">
         <v>894</v>
       </c>
       <c r="C53" s="104" t="s">
@@ -45609,7 +45823,7 @@
       <c r="A55" s="104" t="s">
         <v>898</v>
       </c>
-      <c r="B55" s="140" t="s">
+      <c r="B55" s="137" t="s">
         <v>897</v>
       </c>
       <c r="C55" s="104" t="s">
@@ -45668,53 +45882,53 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="47">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A4:A26"/>
+    <mergeCell ref="C4:C26"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
     <mergeCell ref="A53:A54"/>
     <mergeCell ref="B53:B54"/>
     <mergeCell ref="C53:C54"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="B55:B56"/>
     <mergeCell ref="C55:C56"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A4:A26"/>
-    <mergeCell ref="C4:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -45774,27 +45988,27 @@
     </row>
     <row r="5" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="115"/>
-      <c r="B5" s="125"/>
+      <c r="B5" s="127"/>
       <c r="C5" s="115"/>
     </row>
     <row r="6" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="115"/>
-      <c r="B6" s="125"/>
+      <c r="B6" s="127"/>
       <c r="C6" s="115"/>
     </row>
     <row r="7" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="115"/>
-      <c r="B7" s="125"/>
+      <c r="B7" s="127"/>
       <c r="C7" s="115"/>
     </row>
     <row r="8" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="115"/>
-      <c r="B8" s="125"/>
+      <c r="B8" s="127"/>
       <c r="C8" s="115"/>
     </row>
     <row r="9" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="115"/>
-      <c r="B9" s="125"/>
+      <c r="B9" s="127"/>
       <c r="C9" s="115"/>
     </row>
     <row r="10" spans="1:3" ht="337" customHeight="1" x14ac:dyDescent="0.2">
@@ -45826,7 +46040,7 @@
     </row>
     <row r="13" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="115"/>
-      <c r="B13" s="125"/>
+      <c r="B13" s="127"/>
       <c r="C13" s="115"/>
     </row>
     <row r="14" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -46037,7 +46251,7 @@
       <c r="A16" s="104" t="s">
         <v>944</v>
       </c>
-      <c r="B16" s="125" t="s">
+      <c r="B16" s="127" t="s">
         <v>943</v>
       </c>
       <c r="C16" s="104" t="s">
@@ -46046,12 +46260,12 @@
     </row>
     <row r="17" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="115"/>
-      <c r="B17" s="125"/>
+      <c r="B17" s="127"/>
       <c r="C17" s="115"/>
     </row>
     <row r="18" spans="1:3" ht="337" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="115"/>
-      <c r="B18" s="125"/>
+      <c r="B18" s="127"/>
       <c r="C18" s="115"/>
     </row>
     <row r="19" spans="1:3" ht="108" customHeight="1" x14ac:dyDescent="0.2">
@@ -46074,7 +46288,7 @@
       <c r="A21" s="116" t="s">
         <v>950</v>
       </c>
-      <c r="B21" s="124" t="s">
+      <c r="B21" s="128" t="s">
         <v>949</v>
       </c>
       <c r="C21" s="116" t="s">
@@ -46083,7 +46297,7 @@
     </row>
     <row r="22" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="116"/>
-      <c r="B22" s="124"/>
+      <c r="B22" s="128"/>
       <c r="C22" s="116"/>
     </row>
     <row r="23" spans="1:3" s="86" customFormat="1" ht="122" customHeight="1" x14ac:dyDescent="0.2">
@@ -46759,6 +46973,31 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="35">
+    <mergeCell ref="B41:B46"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="C41:C46"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="B28:B34"/>
+    <mergeCell ref="A28:A34"/>
+    <mergeCell ref="C28:C34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="C21:C22"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="B12:B13"/>
@@ -46769,31 +47008,6 @@
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B28:B34"/>
-    <mergeCell ref="A28:A34"/>
-    <mergeCell ref="C28:C34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="B41:B46"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="C41:C46"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="C39:C40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -47202,6 +47416,12 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="13">
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="B15:B21"/>
@@ -47209,12 +47429,6 @@
     <mergeCell ref="C15:C21"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -47525,7 +47739,7 @@
         <v>1116</v>
       </c>
     </row>
-    <row r="14" spans="1:3" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A14" s="83" t="s">
         <v>1118</v>
       </c>
@@ -47658,6 +47872,12 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="13">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="C20:C21"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="C23:C24"/>
@@ -47665,12 +47885,6 @@
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="C20:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -47905,6 +48119,8 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="C18:C19"/>
@@ -47917,8 +48133,6 @@
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -47927,6 +48141,198 @@
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F79AE45-5159-704E-840B-28E9AA6EEEF5}">
   <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="102" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+    </row>
+    <row r="2" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="108" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+    </row>
+    <row r="3" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="10" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="104" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B4" s="143" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C4" s="104" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="105"/>
+      <c r="B5" s="144"/>
+      <c r="C5" s="105"/>
+    </row>
+    <row r="6" spans="1:3" s="10" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="104" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B6" s="143" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C6" s="104" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="10" customFormat="1" ht="196" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="115"/>
+      <c r="B7" s="146"/>
+      <c r="C7" s="115"/>
+    </row>
+    <row r="8" spans="1:3" s="10" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="115"/>
+      <c r="B8" s="146"/>
+      <c r="C8" s="115"/>
+    </row>
+    <row r="9" spans="1:3" s="10" customFormat="1" ht="128" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="115"/>
+      <c r="B9" s="146"/>
+      <c r="C9" s="115"/>
+    </row>
+    <row r="10" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="115"/>
+      <c r="B10" s="146"/>
+      <c r="C10" s="115"/>
+    </row>
+    <row r="11" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="115"/>
+      <c r="B11" s="146"/>
+      <c r="C11" s="115"/>
+    </row>
+    <row r="12" spans="1:3" s="10" customFormat="1" ht="296" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="115"/>
+      <c r="B12" s="146"/>
+      <c r="C12" s="115"/>
+    </row>
+    <row r="13" spans="1:3" s="10" customFormat="1" ht="254" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="115"/>
+      <c r="B13" s="146"/>
+      <c r="C13" s="115"/>
+    </row>
+    <row r="14" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="115"/>
+      <c r="B14" s="146"/>
+      <c r="C14" s="115"/>
+    </row>
+    <row r="15" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="105"/>
+      <c r="B15" s="144"/>
+      <c r="C15" s="105"/>
+    </row>
+    <row r="16" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="115" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B16" s="109" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C16" s="115" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="105"/>
+      <c r="B17" s="111"/>
+      <c r="C17" s="105"/>
+    </row>
+    <row r="18" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="50" t="s">
+        <v>1099</v>
+      </c>
+      <c r="B18" s="93" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C18" s="50" t="s">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="50" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B19" s="93" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C19" s="50" t="s">
+        <v>1193</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="187" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>1194</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A21" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="77" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>463</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="11">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B6:B15"/>
+    <mergeCell ref="A6:A15"/>
+    <mergeCell ref="C6:C15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7233BF6C-AE1E-4A45-856B-624E3EF2A9FC}">
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -47949,7 +48355,7 @@
     </row>
     <row r="2" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="108" t="s">
-        <v>1181</v>
+        <v>1196</v>
       </c>
       <c r="B2" s="108"/>
       <c r="C2" s="108"/>
@@ -47965,15 +48371,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="10" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="10" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="104" t="s">
-        <v>1183</v>
+        <v>1198</v>
       </c>
       <c r="B4" s="143" t="s">
-        <v>1182</v>
+        <v>1197</v>
       </c>
       <c r="C4" s="104" t="s">
-        <v>1184</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -47981,142 +48387,42 @@
       <c r="B5" s="144"/>
       <c r="C5" s="105"/>
     </row>
-    <row r="6" spans="1:3" s="10" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="104" t="s">
-        <v>1186</v>
-      </c>
-      <c r="B6" s="143" t="s">
-        <v>1185</v>
-      </c>
-      <c r="C6" s="104" t="s">
-        <v>1187</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="10" customFormat="1" ht="196" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="115"/>
-      <c r="B7" s="152"/>
-      <c r="C7" s="115"/>
-    </row>
-    <row r="8" spans="1:3" s="10" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="115"/>
-      <c r="B8" s="152"/>
-      <c r="C8" s="115"/>
-    </row>
-    <row r="9" spans="1:3" s="10" customFormat="1" ht="128" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="115"/>
-      <c r="B9" s="152"/>
-      <c r="C9" s="115"/>
-    </row>
-    <row r="10" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="115"/>
-      <c r="B10" s="152"/>
-      <c r="C10" s="115"/>
-    </row>
-    <row r="11" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="115"/>
-      <c r="B11" s="152"/>
-      <c r="C11" s="115"/>
-    </row>
-    <row r="12" spans="1:3" s="10" customFormat="1" ht="296" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="115"/>
-      <c r="B12" s="152"/>
-      <c r="C12" s="115"/>
-    </row>
-    <row r="13" spans="1:3" s="10" customFormat="1" ht="254" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="115"/>
-      <c r="B13" s="152"/>
-      <c r="C13" s="115"/>
-    </row>
-    <row r="14" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="115"/>
-      <c r="B14" s="152"/>
-      <c r="C14" s="115"/>
-    </row>
-    <row r="15" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="105"/>
-      <c r="B15" s="144"/>
-      <c r="C15" s="105"/>
-    </row>
-    <row r="16" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="115" t="s">
-        <v>1189</v>
-      </c>
-      <c r="B16" s="109" t="s">
-        <v>1188</v>
-      </c>
-      <c r="C16" s="115" t="s">
-        <v>1190</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="105"/>
-      <c r="B17" s="111"/>
-      <c r="C17" s="105"/>
-    </row>
-    <row r="18" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="50" t="s">
-        <v>1099</v>
-      </c>
-      <c r="B18" s="93" t="s">
-        <v>1098</v>
-      </c>
-      <c r="C18" s="50" t="s">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="50" t="s">
-        <v>1191</v>
-      </c>
-      <c r="B19" s="93" t="s">
-        <v>1192</v>
-      </c>
-      <c r="C19" s="50" t="s">
-        <v>1193</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="187" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
+    <row r="6" spans="1:3" ht="170" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B6" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="14" t="s">
-        <v>1194</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
+      <c r="C6" s="14" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="B21" s="77" t="s">
-        <v>1195</v>
-      </c>
-      <c r="C21" s="13" t="s">
+      <c r="B7" s="77" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>463</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="11">
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B6:B15"/>
-    <mergeCell ref="A6:A15"/>
-    <mergeCell ref="C6:C15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
+  <mergeCells count="5">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="C4:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE113606-3FFA-8545-9BE3-5643B52A7CE9}">
   <dimension ref="A1:H116"/>
   <sheetViews>
@@ -48194,10 +48500,10 @@
       <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="149" t="s">
+      <c r="A6" s="147" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="149"/>
+      <c r="B6" s="147"/>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
@@ -49170,32 +49476,32 @@
       <c r="H73" s="20"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="146"/>
-      <c r="B74" s="150"/>
+      <c r="A74" s="148"/>
+      <c r="B74" s="149"/>
       <c r="C74" s="29" t="s">
         <v>225</v>
       </c>
       <c r="D74" s="29" t="s">
         <v>227</v>
       </c>
-      <c r="E74" s="151"/>
-      <c r="F74" s="146"/>
-      <c r="G74" s="148"/>
-      <c r="H74" s="146"/>
+      <c r="E74" s="150"/>
+      <c r="F74" s="148"/>
+      <c r="G74" s="152"/>
+      <c r="H74" s="148"/>
     </row>
     <row r="75" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A75" s="146"/>
-      <c r="B75" s="150"/>
+      <c r="A75" s="148"/>
+      <c r="B75" s="149"/>
       <c r="C75" s="30" t="s">
         <v>226</v>
       </c>
       <c r="D75" s="30" t="s">
         <v>228</v>
       </c>
-      <c r="E75" s="151"/>
-      <c r="F75" s="146"/>
-      <c r="G75" s="148"/>
-      <c r="H75" s="146"/>
+      <c r="E75" s="150"/>
+      <c r="F75" s="148"/>
+      <c r="G75" s="152"/>
+      <c r="H75" s="148"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="20"/>
@@ -49368,34 +49674,34 @@
       <c r="H88" s="20"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="146"/>
-      <c r="B89" s="146"/>
+      <c r="A89" s="148"/>
+      <c r="B89" s="148"/>
       <c r="C89" s="32" t="s">
         <v>225</v>
       </c>
       <c r="D89" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="E89" s="147" t="s">
+      <c r="E89" s="151" t="s">
         <v>121</v>
       </c>
-      <c r="F89" s="147"/>
-      <c r="G89" s="148"/>
-      <c r="H89" s="146"/>
+      <c r="F89" s="151"/>
+      <c r="G89" s="152"/>
+      <c r="H89" s="148"/>
     </row>
     <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A90" s="146"/>
-      <c r="B90" s="146"/>
+      <c r="A90" s="148"/>
+      <c r="B90" s="148"/>
       <c r="C90" s="32" t="s">
         <v>242</v>
       </c>
       <c r="D90" s="32" t="s">
         <v>243</v>
       </c>
-      <c r="E90" s="147"/>
-      <c r="F90" s="147"/>
-      <c r="G90" s="148"/>
-      <c r="H90" s="146"/>
+      <c r="E90" s="151"/>
+      <c r="F90" s="151"/>
+      <c r="G90" s="152"/>
+      <c r="H90" s="148"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="20"/>
@@ -49763,11 +50069,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F74:F75"/>
     <mergeCell ref="H74:H75"/>
     <mergeCell ref="A89:A90"/>
     <mergeCell ref="B89:B90"/>
@@ -49776,12 +50077,17 @@
     <mergeCell ref="G89:G90"/>
     <mergeCell ref="H89:H90"/>
     <mergeCell ref="G74:G75"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F74:F75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -49879,7 +50185,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0BB7-C151-C94B-945C-E2CA92034B13}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -50456,6 +50762,11 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B7:B13"/>
+    <mergeCell ref="A7:A13"/>
+    <mergeCell ref="C7:C13"/>
     <mergeCell ref="B38:B42"/>
     <mergeCell ref="A14:A42"/>
     <mergeCell ref="C14:C42"/>
@@ -50465,11 +50776,6 @@
     <mergeCell ref="B28:B37"/>
     <mergeCell ref="B14:B20"/>
     <mergeCell ref="B21:B27"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B7:B13"/>
-    <mergeCell ref="A7:A13"/>
-    <mergeCell ref="C7:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -50887,12 +51193,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="C14:C16"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="C8:C10"/>
@@ -50901,6 +51201,12 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C14:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -50960,7 +51266,7 @@
       <c r="A5" s="104" t="s">
         <v>397</v>
       </c>
-      <c r="B5" s="126" t="s">
+      <c r="B5" s="124" t="s">
         <v>396</v>
       </c>
       <c r="C5" s="104" t="s">
@@ -50969,37 +51275,37 @@
     </row>
     <row r="6" spans="1:3" s="10" customFormat="1" ht="283" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="115"/>
-      <c r="B6" s="127"/>
+      <c r="B6" s="125"/>
       <c r="C6" s="115"/>
     </row>
     <row r="7" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="115"/>
-      <c r="B7" s="127"/>
+      <c r="B7" s="125"/>
       <c r="C7" s="115"/>
     </row>
     <row r="8" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="115"/>
-      <c r="B8" s="127"/>
+      <c r="B8" s="125"/>
       <c r="C8" s="115"/>
     </row>
     <row r="9" spans="1:3" s="10" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="115"/>
-      <c r="B9" s="127"/>
+      <c r="B9" s="125"/>
       <c r="C9" s="115"/>
     </row>
     <row r="10" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="115"/>
-      <c r="B10" s="127"/>
+      <c r="B10" s="125"/>
       <c r="C10" s="115"/>
     </row>
     <row r="11" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="115"/>
-      <c r="B11" s="127"/>
+      <c r="B11" s="125"/>
       <c r="C11" s="115"/>
     </row>
     <row r="12" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="105"/>
-      <c r="B12" s="128"/>
+      <c r="B12" s="126"/>
       <c r="C12" s="105"/>
     </row>
     <row r="13" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -51237,7 +51543,7 @@
     </row>
     <row r="50" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="115"/>
-      <c r="B50" s="125"/>
+      <c r="B50" s="127"/>
       <c r="C50" s="115"/>
     </row>
     <row r="51" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -51260,7 +51566,7 @@
       <c r="A53" s="104" t="s">
         <v>415</v>
       </c>
-      <c r="B53" s="124" t="s">
+      <c r="B53" s="128" t="s">
         <v>416</v>
       </c>
       <c r="C53" s="104" t="s">
@@ -51269,7 +51575,7 @@
     </row>
     <row r="54" spans="1:3" ht="238" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="115"/>
-      <c r="B54" s="124"/>
+      <c r="B54" s="128"/>
       <c r="C54" s="115"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -51281,12 +51587,12 @@
     </row>
     <row r="56" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="115"/>
-      <c r="B56" s="125"/>
+      <c r="B56" s="127"/>
       <c r="C56" s="115"/>
     </row>
     <row r="57" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="115"/>
-      <c r="B57" s="125"/>
+      <c r="B57" s="127"/>
       <c r="C57" s="115"/>
     </row>
     <row r="58" spans="1:3" ht="172" customHeight="1" x14ac:dyDescent="0.2">
@@ -51303,12 +51609,12 @@
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="115"/>
-      <c r="B60" s="125"/>
+      <c r="B60" s="127"/>
       <c r="C60" s="115"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="115"/>
-      <c r="B61" s="125"/>
+      <c r="B61" s="127"/>
       <c r="C61" s="115"/>
     </row>
     <row r="62" spans="1:3" ht="125" customHeight="1" x14ac:dyDescent="0.2">
@@ -51325,17 +51631,17 @@
     </row>
     <row r="64" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="115"/>
-      <c r="B64" s="125"/>
+      <c r="B64" s="127"/>
       <c r="C64" s="115"/>
     </row>
     <row r="65" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="115"/>
-      <c r="B65" s="125"/>
+      <c r="B65" s="127"/>
       <c r="C65" s="115"/>
     </row>
     <row r="66" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="115"/>
-      <c r="B66" s="125"/>
+      <c r="B66" s="127"/>
       <c r="C66" s="115"/>
     </row>
     <row r="67" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -51379,18 +51685,11 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="25">
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B5:B12"/>
-    <mergeCell ref="A5:A12"/>
-    <mergeCell ref="C5:C12"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="C13:C41"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C53:C67"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="B63:B67"/>
     <mergeCell ref="A53:A67"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="B32:B35"/>
@@ -51399,11 +51698,18 @@
     <mergeCell ref="A13:A41"/>
     <mergeCell ref="B49:B51"/>
     <mergeCell ref="A49:A51"/>
-    <mergeCell ref="C53:C67"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="B63:B67"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="C13:C41"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B5:B12"/>
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="C5:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ER5200 is now in the swing door and sliding door section and also provided validation messages for locks ER5200 and DL6600 as per validation request sought.
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10418"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10502"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63BE7088-F391-7040-8EF6-A3D0ACFFCDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588D9048-2FD3-6F4B-8840-00C79F0E8920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" firstSheet="24" activeTab="34" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" firstSheet="25" activeTab="35" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="SPEC - 1.1" sheetId="1" r:id="rId1"/>
@@ -48,10 +48,14 @@
     <sheet name="SPEC - 4.8" sheetId="38" r:id="rId33"/>
     <sheet name="SPEC - 4.9" sheetId="39" r:id="rId34"/>
     <sheet name="SPEC - 5.0" sheetId="40" r:id="rId35"/>
-    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId36"/>
-    <sheet name="PLAYGROUND" sheetId="6" r:id="rId37"/>
-    <sheet name="TEMPLATE" sheetId="8" r:id="rId38"/>
+    <sheet name="SPEC - 5.1" sheetId="41" r:id="rId36"/>
+    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId37"/>
+    <sheet name="PLAYGROUND" sheetId="6" r:id="rId38"/>
+    <sheet name="TEMPLATE" sheetId="8" r:id="rId39"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="35">'SPEC - 5.1'!$A:$C</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -70,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1594" uniqueCount="1202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="1211">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -40356,6 +40360,482 @@
   </si>
   <si>
     <t>git commit -m "Implemented changes to the report for Customer Additional Information and Sales Location fields being empty"</t>
+  </si>
+  <si>
+    <t>UPDATE MESSAGES FOR LOCK ER5200 AND DL6600 AND MOVED ER5200 INTO SWING DOOR / SLIDING DOOR SECTION OF LOCK SELECTION</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">/* The function forms an object containing  the door type and door thickness 
+ * range - determined by the lock model value.
+ * name input control. 
+ * @param    {LOCK_MODEL} lockModel The model of the lock
+ * @return   {Object}   An Object containing doorType and doorThickness
+ * */
+const lockCompatibility = (lockModel) =&gt; {
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+    switch (lockModel) {
+        case LOCK_MODEL.DC1000:
+        case LOCK_MODEL.ER4900:
+        case LOCK_MODEL.ER5100:
+            return {
+                doorType: DOOR_TYPE.SWING_DOOR,
+                    doorThickness: DOOR_THICKNESS_IN_MM.MM_30_TO_50
+            };
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">        case LOCK_MODEL.ER5200:
+            return {
+                 doorType: DOOR_TYPE.SWING_DOOR + "/" + DOOR_TYPE.SLIDING_DOOR,
+                    doorThickness: DOOR_THICKNESS_IN_MM.MM_30_TO_50
+            };
+        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>case LOCK_MODEL.DH2000:
+            return {
+                doorType: DOOR_TYPE.SWING_DOOR,
+                    doorThickness: DOOR_THICKNESS_IN_MM.MM_32_TO_50
+            };
+        case LOCK_MODEL.DL6500:
+        case LOCK_MODEL.DL7000:
+        case LOCK_MODEL.DL7100:
+        case LOCK_MODEL.DL7900:
+        case LOCK_MODEL.EL6000:
+        case LOCK_MODEL.EL7200:
+        case LOCK_MODEL.EL7500:
+            return {
+                doorType: DOOR_TYPE.SWING_DOOR,
+                    doorThickness: DOOR_THICKNESS_IN_MM.MM_35_TO_50
+            };
+        case LOCK_MODEL.DL7600:
+        case LOCK_MODEL.PP8100:
+        case LOCK_MODEL.PP9000:
+            return {
+                doorType: DOOR_TYPE.SWING_DOOR,
+                    doorThickness: DOOR_THICKNESS_IN_MM.MM_35_TO_60
+            };
+        case LOCK_MODEL.DL6600:
+            return {
+                doorType: DOOR_TYPE.SWING_DOOR + "/" + DOOR_TYPE.SLIDING_DOOR,
+                    doorThickness: DOOR_THICKNESS_IN_MM.MM_35_TO_90
+            };
+        default:
+            return {
+                doorType: "",
+                    doorThickness: ""
+            }
+    }
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the lock model </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>ER5200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to be into the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>SWING DOOR / SLIDING DOOR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> category in the file  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> js/controller/lock-compatibility.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the lock model </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>ER5200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to be into the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>SWING DOOR / SLIDING DOOR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> category in the file  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> js/controller/lock-compatibility.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                   case LOCK_MODEL.ER5200:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">                        if (selectedValue ===
+                            SWING_DOOR_LEAF.DOOR_LEAF_WITH_MULLION_LESS_THAN_50_MM ||
+                            selectedValue ===
+                            SWING_DOOR_LEAF.DOOR_LEAF_WITH_FRAME_LESS_THAN_50_MM) {
+                            messageLabelShow(doorLeafMessageLabel, true,
+                                MESSAGE.MESSAGE_DOOR_LEAF_FRAME_THICKNESS_INADEQUATE);
+                        }
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">                        if (selectedValue ===
+                            SLIDING_DOOR_LEAF.WOODEN_LEAF_LESS_THAN_50_MM ||
+                            selectedValue ===
+                            SLIDING_DOOR_LEAF.ALUMINIUM_LEAF_LESS_THAN_50_MM ||
+                            selectedValue ===
+                            SLIDING_DOOR_LEAF.STEEL_LEAF_LESS_THAN_50_MM) {
+                            messageLabelShow(doorLeafMessageLabel, true,
+                                MESSAGE.MESSAGE_DOOR_LEAF_THICKNESS_INADEQUATE);
+                        }
+                        break;
+                    case LOCK_MODEL.DL6600:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">                        if (selectedValue ===
+                            SWING_DOOR_LEAF.DOOR_LEAF_WITH_MULLION_LESS_THAN_60_MM ||
+                            selectedValue ===
+                            SWING_DOOR_LEAF.DOOR_LEAF_WITH_FRAME_LESS_THAN_60_MM) {
+                            messageLabelShow(doorLeafMessageLabel, true,
+                                MESSAGE.MESSAGE_DOOR_LEAF_FRAME_THICKNESS_INADEQUATE);
+                        }
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF002060"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">                        if (selectedValue ===
+                            SLIDING_DOOR_LEAF.WOODEN_LEAF_LESS_THAN_50_MM ||
+                            selectedValue ===
+                            SLIDING_DOOR_LEAF.ALUMINIUM_LEAF_LESS_THAN_50_MM ||
+                            selectedValue ===
+                            SLIDING_DOOR_LEAF.STEEL_LEAF_LESS_THAN_50_MM) {
+                            messageLabelShow(doorLeafMessageLabel, true,
+                                MESSAGE.MESSAGE_DOOR_LEAF_THICKNESS_INADEQUATE);
+                        }
+                        break;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="2" tint="-9.9978637043366805E-2"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">                    case LOCK_MODEL.EL6000:
+                    case LOCK_MODEL.EL7200:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the validation messages for lock model </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>ER5200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>DL6600</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the callback function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>doorLeafSelectionChange</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller/lock-selection-survey-lock-card.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the validation messages for lock model </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>ER5200</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>DL6600</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the callback function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>doorLeafSelectionChange</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>js/controller/lock-selection-survey-lock-card.js</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>git status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - would display the following files.                                                                                                                                                                                                                                  On branch master
+Your branch is up to date with 'hafele/master'.
+Changes to be committed:
+  (use "git restore --staged &lt;file&gt;..." to unstage)
+        modified:   docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+        modified:   js/controller/lock-compatibility.js
+        modified:   js/controller/lock-selection-survey-lock-card.js
+</t>
+    </r>
+  </si>
+  <si>
+    <t>git commit -m "ER5200 is now in the swing door and sliding door section and also provided validation messages for locks ER5200 and DL6600 as per validation request sought. "</t>
   </si>
 </sst>
 </file>
@@ -41166,6 +41646,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -41173,12 +41659,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -41205,16 +41685,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -41235,16 +41715,16 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -41850,7 +42330,8 @@
   <hyperlinks>
     <hyperlink ref="B19" r:id="rId1" xr:uid="{82A47956-2C1F-B942-93C6-EE56AEAFA3A5}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -42079,6 +42560,7 @@
     <hyperlink ref="C12" r:id="rId1" xr:uid="{A4CA5643-C4DB-104D-8F62-BC3D176D48F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -42196,6 +42678,7 @@
     <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -42407,6 +42890,7 @@
     <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -42692,6 +43176,14 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="17">
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="A12:A18"/>
+    <mergeCell ref="C12:C18"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:C10"/>
     <mergeCell ref="B30:B33"/>
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="C30:C33"/>
@@ -42701,16 +43193,9 @@
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="C27:C29"/>
-    <mergeCell ref="B12:B18"/>
-    <mergeCell ref="A12:A18"/>
-    <mergeCell ref="C12:C18"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="C8:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -42817,6 +43302,7 @@
     <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -43010,6 +43496,7 @@
     <mergeCell ref="A10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -43316,12 +43803,12 @@
     </row>
     <row r="34" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="115"/>
-      <c r="B34" s="127"/>
+      <c r="B34" s="125"/>
       <c r="C34" s="115"/>
     </row>
     <row r="35" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="115"/>
-      <c r="B35" s="127"/>
+      <c r="B35" s="125"/>
       <c r="C35" s="115"/>
     </row>
     <row r="36" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
@@ -43338,27 +43825,27 @@
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="115"/>
-      <c r="B38" s="127"/>
+      <c r="B38" s="125"/>
       <c r="C38" s="115"/>
     </row>
     <row r="39" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="115"/>
-      <c r="B39" s="127"/>
+      <c r="B39" s="125"/>
       <c r="C39" s="115"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="115"/>
-      <c r="B40" s="127"/>
+      <c r="B40" s="125"/>
       <c r="C40" s="115"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="115"/>
-      <c r="B41" s="127"/>
+      <c r="B41" s="125"/>
       <c r="C41" s="115"/>
     </row>
     <row r="42" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="115"/>
-      <c r="B42" s="127"/>
+      <c r="B42" s="125"/>
       <c r="C42" s="115"/>
     </row>
     <row r="43" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -43370,32 +43857,32 @@
     </row>
     <row r="44" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="115"/>
-      <c r="B44" s="127"/>
+      <c r="B44" s="125"/>
       <c r="C44" s="115"/>
     </row>
     <row r="45" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="115"/>
-      <c r="B45" s="127"/>
+      <c r="B45" s="125"/>
       <c r="C45" s="115"/>
     </row>
     <row r="46" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="115"/>
-      <c r="B46" s="127"/>
+      <c r="B46" s="125"/>
       <c r="C46" s="115"/>
     </row>
     <row r="47" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="115"/>
-      <c r="B47" s="127"/>
+      <c r="B47" s="125"/>
       <c r="C47" s="115"/>
     </row>
     <row r="48" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="115"/>
-      <c r="B48" s="127"/>
+      <c r="B48" s="125"/>
       <c r="C48" s="115"/>
     </row>
     <row r="49" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="115"/>
-      <c r="B49" s="127"/>
+      <c r="B49" s="125"/>
       <c r="C49" s="115"/>
     </row>
     <row r="50" spans="1:3" ht="320" customHeight="1" x14ac:dyDescent="0.2">
@@ -43412,22 +43899,22 @@
     </row>
     <row r="52" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="115"/>
-      <c r="B52" s="127"/>
+      <c r="B52" s="125"/>
       <c r="C52" s="115"/>
     </row>
     <row r="53" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="115"/>
-      <c r="B53" s="127"/>
+      <c r="B53" s="125"/>
       <c r="C53" s="115"/>
     </row>
     <row r="54" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="115"/>
-      <c r="B54" s="127"/>
+      <c r="B54" s="125"/>
       <c r="C54" s="115"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="115"/>
-      <c r="B55" s="127"/>
+      <c r="B55" s="125"/>
       <c r="C55" s="115"/>
     </row>
     <row r="56" spans="1:3" ht="97" customHeight="1" x14ac:dyDescent="0.2">
@@ -43444,27 +43931,27 @@
     </row>
     <row r="58" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="115"/>
-      <c r="B58" s="127"/>
+      <c r="B58" s="125"/>
       <c r="C58" s="115"/>
     </row>
     <row r="59" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="115"/>
-      <c r="B59" s="127"/>
+      <c r="B59" s="125"/>
       <c r="C59" s="115"/>
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="115"/>
-      <c r="B60" s="127"/>
+      <c r="B60" s="125"/>
       <c r="C60" s="115"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="115"/>
-      <c r="B61" s="127"/>
+      <c r="B61" s="125"/>
       <c r="C61" s="115"/>
     </row>
     <row r="62" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="115"/>
-      <c r="B62" s="127"/>
+      <c r="B62" s="125"/>
       <c r="C62" s="115"/>
     </row>
     <row r="63" spans="1:3" ht="146" customHeight="1" x14ac:dyDescent="0.2">
@@ -43499,7 +43986,7 @@
       <c r="A67" s="116" t="s">
         <v>638</v>
       </c>
-      <c r="B67" s="128" t="s">
+      <c r="B67" s="124" t="s">
         <v>637</v>
       </c>
       <c r="C67" s="116" t="s">
@@ -43508,19 +43995,19 @@
     </row>
     <row r="68" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="116"/>
-      <c r="B68" s="128"/>
+      <c r="B68" s="124"/>
       <c r="C68" s="116"/>
     </row>
     <row r="69" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="116"/>
-      <c r="B69" s="128"/>
+      <c r="B69" s="124"/>
       <c r="C69" s="116"/>
     </row>
     <row r="70" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="116" t="s">
         <v>643</v>
       </c>
-      <c r="B70" s="128" t="s">
+      <c r="B70" s="124" t="s">
         <v>640</v>
       </c>
       <c r="C70" s="116" t="s">
@@ -43529,59 +44016,59 @@
     </row>
     <row r="71" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="116"/>
-      <c r="B71" s="128"/>
+      <c r="B71" s="124"/>
       <c r="C71" s="116"/>
     </row>
     <row r="72" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="116"/>
-      <c r="B72" s="128"/>
+      <c r="B72" s="124"/>
       <c r="C72" s="116"/>
     </row>
     <row r="73" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="116"/>
-      <c r="B73" s="128"/>
+      <c r="B73" s="124"/>
       <c r="C73" s="116"/>
     </row>
     <row r="74" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="116"/>
-      <c r="B74" s="128"/>
+      <c r="B74" s="124"/>
       <c r="C74" s="116"/>
     </row>
     <row r="75" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="116"/>
-      <c r="B75" s="128"/>
+      <c r="B75" s="124"/>
       <c r="C75" s="116"/>
     </row>
     <row r="76" spans="1:3" ht="214" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="116"/>
-      <c r="B76" s="128"/>
+      <c r="B76" s="124"/>
       <c r="C76" s="116"/>
     </row>
     <row r="77" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="116"/>
-      <c r="B77" s="128" t="s">
+      <c r="B77" s="124" t="s">
         <v>641</v>
       </c>
       <c r="C77" s="116"/>
     </row>
     <row r="78" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="116"/>
-      <c r="B78" s="128"/>
+      <c r="B78" s="124"/>
       <c r="C78" s="116"/>
     </row>
     <row r="79" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="116"/>
-      <c r="B79" s="128"/>
+      <c r="B79" s="124"/>
       <c r="C79" s="116"/>
     </row>
     <row r="80" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="116"/>
-      <c r="B80" s="128"/>
+      <c r="B80" s="124"/>
       <c r="C80" s="116"/>
     </row>
     <row r="81" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="116"/>
-      <c r="B81" s="128"/>
+      <c r="B81" s="124"/>
       <c r="C81" s="116"/>
     </row>
     <row r="82" spans="1:3" ht="56" x14ac:dyDescent="0.2">
@@ -43689,12 +44176,18 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="30">
-    <mergeCell ref="B77:B81"/>
-    <mergeCell ref="A70:A81"/>
-    <mergeCell ref="C70:C81"/>
-    <mergeCell ref="B86:B91"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="C86:C91"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="A16:A26"/>
+    <mergeCell ref="C16:C26"/>
     <mergeCell ref="B67:B69"/>
     <mergeCell ref="A67:A69"/>
     <mergeCell ref="C67:C69"/>
@@ -43707,20 +44200,15 @@
     <mergeCell ref="B33:B36"/>
     <mergeCell ref="B37:B42"/>
     <mergeCell ref="B43:B50"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="A16:A26"/>
-    <mergeCell ref="C16:C26"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B77:B81"/>
+    <mergeCell ref="A70:A81"/>
+    <mergeCell ref="C70:C81"/>
+    <mergeCell ref="B86:B91"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="C86:C91"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -43877,6 +44365,7 @@
     <mergeCell ref="C7:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -44005,6 +44494,7 @@
     <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -44234,6 +44724,7 @@
     <mergeCell ref="C6:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -44445,6 +44936,7 @@
     <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -44529,6 +45021,7 @@
     <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -44732,6 +45225,7 @@
     <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -44937,19 +45431,20 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="11">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="C11:C12"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="C13:C14"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C11:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -45007,27 +45502,27 @@
     </row>
     <row r="5" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="115"/>
-      <c r="B5" s="127"/>
+      <c r="B5" s="125"/>
       <c r="C5" s="115"/>
     </row>
     <row r="6" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="115"/>
-      <c r="B6" s="127"/>
+      <c r="B6" s="125"/>
       <c r="C6" s="115"/>
     </row>
     <row r="7" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="115"/>
-      <c r="B7" s="127"/>
+      <c r="B7" s="125"/>
       <c r="C7" s="115"/>
     </row>
     <row r="8" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="115"/>
-      <c r="B8" s="127"/>
+      <c r="B8" s="125"/>
       <c r="C8" s="115"/>
     </row>
     <row r="9" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="115"/>
-      <c r="B9" s="127"/>
+      <c r="B9" s="125"/>
       <c r="C9" s="115"/>
     </row>
     <row r="10" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -45256,6 +45751,18 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="21">
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A17:A26"/>
+    <mergeCell ref="C17:C26"/>
+    <mergeCell ref="B28:B34"/>
+    <mergeCell ref="A28:A34"/>
+    <mergeCell ref="C28:C34"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="C13:C15"/>
@@ -45265,20 +45772,9 @@
     <mergeCell ref="B4:B10"/>
     <mergeCell ref="A4:A10"/>
     <mergeCell ref="C4:C10"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="A17:A26"/>
-    <mergeCell ref="C17:C26"/>
-    <mergeCell ref="B28:B34"/>
-    <mergeCell ref="A28:A34"/>
-    <mergeCell ref="C28:C34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="C37:C38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -45327,7 +45823,7 @@
       <c r="A4" s="116" t="s">
         <v>832</v>
       </c>
-      <c r="B4" s="128" t="s">
+      <c r="B4" s="124" t="s">
         <v>831</v>
       </c>
       <c r="C4" s="116" t="s">
@@ -45336,7 +45832,7 @@
     </row>
     <row r="5" spans="1:3" s="10" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="116"/>
-      <c r="B5" s="128"/>
+      <c r="B5" s="124"/>
       <c r="C5" s="116"/>
     </row>
     <row r="6" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -45424,6 +45920,7 @@
     <mergeCell ref="A4:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -45481,27 +45978,27 @@
     </row>
     <row r="5" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="115"/>
-      <c r="B5" s="127"/>
+      <c r="B5" s="125"/>
       <c r="C5" s="115"/>
     </row>
     <row r="6" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="115"/>
-      <c r="B6" s="127"/>
+      <c r="B6" s="125"/>
       <c r="C6" s="115"/>
     </row>
     <row r="7" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="115"/>
-      <c r="B7" s="127"/>
+      <c r="B7" s="125"/>
       <c r="C7" s="115"/>
     </row>
     <row r="8" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="115"/>
-      <c r="B8" s="127"/>
+      <c r="B8" s="125"/>
       <c r="C8" s="115"/>
     </row>
     <row r="9" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="115"/>
-      <c r="B9" s="127"/>
+      <c r="B9" s="125"/>
       <c r="C9" s="115"/>
     </row>
     <row r="10" spans="1:3" ht="337" customHeight="1" x14ac:dyDescent="0.2">
@@ -45518,27 +46015,27 @@
     </row>
     <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="115"/>
-      <c r="B12" s="127"/>
+      <c r="B12" s="125"/>
       <c r="C12" s="115"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="115"/>
-      <c r="B13" s="127"/>
+      <c r="B13" s="125"/>
       <c r="C13" s="115"/>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="115"/>
-      <c r="B14" s="127"/>
+      <c r="B14" s="125"/>
       <c r="C14" s="115"/>
     </row>
     <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="115"/>
-      <c r="B15" s="127"/>
+      <c r="B15" s="125"/>
       <c r="C15" s="115"/>
     </row>
     <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="115"/>
-      <c r="B16" s="127"/>
+      <c r="B16" s="125"/>
       <c r="C16" s="115"/>
     </row>
     <row r="17" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
@@ -45555,27 +46052,27 @@
     </row>
     <row r="19" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="115"/>
-      <c r="B19" s="127"/>
+      <c r="B19" s="125"/>
       <c r="C19" s="115"/>
     </row>
     <row r="20" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="115"/>
-      <c r="B20" s="127"/>
+      <c r="B20" s="125"/>
       <c r="C20" s="115"/>
     </row>
     <row r="21" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="115"/>
-      <c r="B21" s="127"/>
+      <c r="B21" s="125"/>
       <c r="C21" s="115"/>
     </row>
     <row r="22" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="115"/>
-      <c r="B22" s="127"/>
+      <c r="B22" s="125"/>
       <c r="C22" s="115"/>
     </row>
     <row r="23" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="115"/>
-      <c r="B23" s="127"/>
+      <c r="B23" s="125"/>
       <c r="C23" s="115"/>
     </row>
     <row r="24" spans="1:3" s="86" customFormat="1" ht="121" customHeight="1" x14ac:dyDescent="0.2">
@@ -45619,7 +46116,7 @@
     </row>
     <row r="29" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="115"/>
-      <c r="B29" s="127"/>
+      <c r="B29" s="125"/>
       <c r="C29" s="115"/>
     </row>
     <row r="30" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -45647,7 +46144,7 @@
       <c r="A33" s="104" t="s">
         <v>865</v>
       </c>
-      <c r="B33" s="139" t="s">
+      <c r="B33" s="137" t="s">
         <v>864</v>
       </c>
       <c r="C33" s="104" t="s">
@@ -45663,7 +46160,7 @@
       <c r="A35" s="104" t="s">
         <v>868</v>
       </c>
-      <c r="B35" s="139" t="s">
+      <c r="B35" s="137" t="s">
         <v>867</v>
       </c>
       <c r="C35" s="104" t="s">
@@ -45672,7 +46169,7 @@
     </row>
     <row r="36" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="115"/>
-      <c r="B36" s="140"/>
+      <c r="B36" s="139"/>
       <c r="C36" s="115"/>
     </row>
     <row r="37" spans="1:3" s="86" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.2">
@@ -45684,7 +46181,7 @@
       <c r="A38" s="104" t="s">
         <v>871</v>
       </c>
-      <c r="B38" s="139" t="s">
+      <c r="B38" s="137" t="s">
         <v>870</v>
       </c>
       <c r="C38" s="104" t="s">
@@ -45711,7 +46208,7 @@
       <c r="A41" s="104" t="s">
         <v>876</v>
       </c>
-      <c r="B41" s="139" t="s">
+      <c r="B41" s="137" t="s">
         <v>877</v>
       </c>
       <c r="C41" s="104" t="s">
@@ -45727,7 +46224,7 @@
       <c r="A43" s="104" t="s">
         <v>880</v>
       </c>
-      <c r="B43" s="137" t="s">
+      <c r="B43" s="140" t="s">
         <v>879</v>
       </c>
       <c r="C43" s="104" t="s">
@@ -45743,7 +46240,7 @@
       <c r="A45" s="104" t="s">
         <v>883</v>
       </c>
-      <c r="B45" s="137" t="s">
+      <c r="B45" s="140" t="s">
         <v>882</v>
       </c>
       <c r="C45" s="104" t="s">
@@ -45759,7 +46256,7 @@
       <c r="A47" s="104" t="s">
         <v>885</v>
       </c>
-      <c r="B47" s="137" t="s">
+      <c r="B47" s="140" t="s">
         <v>887</v>
       </c>
       <c r="C47" s="104" t="s">
@@ -45775,7 +46272,7 @@
       <c r="A49" s="104" t="s">
         <v>888</v>
       </c>
-      <c r="B49" s="137" t="s">
+      <c r="B49" s="140" t="s">
         <v>890</v>
       </c>
       <c r="C49" s="104" t="s">
@@ -45791,7 +46288,7 @@
       <c r="A51" s="104" t="s">
         <v>892</v>
       </c>
-      <c r="B51" s="137" t="s">
+      <c r="B51" s="140" t="s">
         <v>891</v>
       </c>
       <c r="C51" s="104" t="s">
@@ -45807,7 +46304,7 @@
       <c r="A53" s="104" t="s">
         <v>895</v>
       </c>
-      <c r="B53" s="137" t="s">
+      <c r="B53" s="140" t="s">
         <v>894</v>
       </c>
       <c r="C53" s="104" t="s">
@@ -45823,7 +46320,7 @@
       <c r="A55" s="104" t="s">
         <v>898</v>
       </c>
-      <c r="B55" s="137" t="s">
+      <c r="B55" s="140" t="s">
         <v>897</v>
       </c>
       <c r="C55" s="104" t="s">
@@ -45882,55 +46379,56 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="47">
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="B18:B24"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="B4:B10"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="A4:A26"/>
     <mergeCell ref="C4:C26"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="C55:C56"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -45988,27 +46486,27 @@
     </row>
     <row r="5" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="115"/>
-      <c r="B5" s="127"/>
+      <c r="B5" s="125"/>
       <c r="C5" s="115"/>
     </row>
     <row r="6" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="115"/>
-      <c r="B6" s="127"/>
+      <c r="B6" s="125"/>
       <c r="C6" s="115"/>
     </row>
     <row r="7" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="115"/>
-      <c r="B7" s="127"/>
+      <c r="B7" s="125"/>
       <c r="C7" s="115"/>
     </row>
     <row r="8" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="115"/>
-      <c r="B8" s="127"/>
+      <c r="B8" s="125"/>
       <c r="C8" s="115"/>
     </row>
     <row r="9" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="115"/>
-      <c r="B9" s="127"/>
+      <c r="B9" s="125"/>
       <c r="C9" s="115"/>
     </row>
     <row r="10" spans="1:3" ht="337" customHeight="1" x14ac:dyDescent="0.2">
@@ -46040,7 +46538,7 @@
     </row>
     <row r="13" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="115"/>
-      <c r="B13" s="127"/>
+      <c r="B13" s="125"/>
       <c r="C13" s="115"/>
     </row>
     <row r="14" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -46097,6 +46595,7 @@
     <mergeCell ref="C12:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -46251,7 +46750,7 @@
       <c r="A16" s="104" t="s">
         <v>944</v>
       </c>
-      <c r="B16" s="127" t="s">
+      <c r="B16" s="125" t="s">
         <v>943</v>
       </c>
       <c r="C16" s="104" t="s">
@@ -46260,12 +46759,12 @@
     </row>
     <row r="17" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="115"/>
-      <c r="B17" s="127"/>
+      <c r="B17" s="125"/>
       <c r="C17" s="115"/>
     </row>
     <row r="18" spans="1:3" ht="337" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="115"/>
-      <c r="B18" s="127"/>
+      <c r="B18" s="125"/>
       <c r="C18" s="115"/>
     </row>
     <row r="19" spans="1:3" ht="108" customHeight="1" x14ac:dyDescent="0.2">
@@ -46288,7 +46787,7 @@
       <c r="A21" s="116" t="s">
         <v>950</v>
       </c>
-      <c r="B21" s="128" t="s">
+      <c r="B21" s="124" t="s">
         <v>949</v>
       </c>
       <c r="C21" s="116" t="s">
@@ -46297,7 +46796,7 @@
     </row>
     <row r="22" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="116"/>
-      <c r="B22" s="128"/>
+      <c r="B22" s="124"/>
       <c r="C22" s="116"/>
     </row>
     <row r="23" spans="1:3" s="86" customFormat="1" ht="122" customHeight="1" x14ac:dyDescent="0.2">
@@ -46381,6 +46880,7 @@
     <mergeCell ref="C16:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -46558,6 +47058,7 @@
     <mergeCell ref="C12:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -46973,21 +47474,16 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="35">
-    <mergeCell ref="B41:B46"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="C41:C46"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="B28:B34"/>
-    <mergeCell ref="A28:A34"/>
-    <mergeCell ref="C28:C34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="C10:C11"/>
     <mergeCell ref="B23:B27"/>
     <mergeCell ref="A23:A27"/>
     <mergeCell ref="C23:C27"/>
@@ -46998,18 +47494,24 @@
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="A21:A22"/>
     <mergeCell ref="C21:C22"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="B28:B34"/>
+    <mergeCell ref="A28:A34"/>
+    <mergeCell ref="C28:C34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="B41:B46"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="C41:C46"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="C39:C40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -47175,6 +47677,7 @@
     <mergeCell ref="C6:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -47416,12 +47919,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="13">
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="B15:B21"/>
@@ -47429,8 +47926,15 @@
     <mergeCell ref="C15:C21"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A10:C10"/>
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -47611,6 +48115,7 @@
     <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -47872,12 +48377,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="13">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="C20:C21"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="C23:C24"/>
@@ -47885,8 +48384,15 @@
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="B20:B21"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="C20:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -48135,6 +48641,7 @@
     <mergeCell ref="C16:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -48314,25 +48821,122 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="11">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="C4:C5"/>
     <mergeCell ref="B6:B15"/>
     <mergeCell ref="A6:A15"/>
     <mergeCell ref="C6:C15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="C4:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7233BF6C-AE1E-4A45-856B-624E3EF2A9FC}">
   <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="102" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+    </row>
+    <row r="2" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="108" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+    </row>
+    <row r="3" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="10" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="104" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B4" s="143" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C4" s="104" t="s">
+        <v>1199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="105"/>
+      <c r="B5" s="144"/>
+      <c r="C5" s="105"/>
+    </row>
+    <row r="6" spans="1:3" ht="170" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="77" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>463</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="5">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0656269A-CEF8-D441-9F32-A5C2519234DA}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection sqref="A1:C1"/>
@@ -48355,7 +48959,7 @@
     </row>
     <row r="2" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="108" t="s">
-        <v>1196</v>
+        <v>1202</v>
       </c>
       <c r="B2" s="108"/>
       <c r="C2" s="108"/>
@@ -48373,13 +48977,13 @@
     </row>
     <row r="4" spans="1:3" s="10" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="104" t="s">
-        <v>1198</v>
+        <v>1204</v>
       </c>
       <c r="B4" s="143" t="s">
-        <v>1197</v>
+        <v>1203</v>
       </c>
       <c r="C4" s="104" t="s">
-        <v>1199</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -48387,42 +48991,62 @@
       <c r="B5" s="144"/>
       <c r="C5" s="105"/>
     </row>
-    <row r="6" spans="1:3" ht="170" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="104" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B6" s="143" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C6" s="104" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="105"/>
+      <c r="B7" s="144"/>
+      <c r="C7" s="105"/>
+    </row>
+    <row r="8" spans="1:3" ht="187" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B8" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
+      <c r="C8" s="14" t="s">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A9" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="77" t="s">
-        <v>1201</v>
-      </c>
-      <c r="C7" s="13" t="s">
+      <c r="B9" s="77" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>463</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="5">
+  <mergeCells count="8">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:C7"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="40" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE113606-3FFA-8545-9BE3-5643B52A7CE9}">
   <dimension ref="A1:H116"/>
   <sheetViews>
@@ -48500,10 +49124,10 @@
       <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="147" t="s">
+      <c r="A6" s="150" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="147"/>
+      <c r="B6" s="150"/>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
@@ -49476,32 +50100,32 @@
       <c r="H73" s="20"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="148"/>
-      <c r="B74" s="149"/>
+      <c r="A74" s="147"/>
+      <c r="B74" s="151"/>
       <c r="C74" s="29" t="s">
         <v>225</v>
       </c>
       <c r="D74" s="29" t="s">
         <v>227</v>
       </c>
-      <c r="E74" s="150"/>
-      <c r="F74" s="148"/>
-      <c r="G74" s="152"/>
-      <c r="H74" s="148"/>
+      <c r="E74" s="152"/>
+      <c r="F74" s="147"/>
+      <c r="G74" s="149"/>
+      <c r="H74" s="147"/>
     </row>
     <row r="75" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A75" s="148"/>
-      <c r="B75" s="149"/>
+      <c r="A75" s="147"/>
+      <c r="B75" s="151"/>
       <c r="C75" s="30" t="s">
         <v>226</v>
       </c>
       <c r="D75" s="30" t="s">
         <v>228</v>
       </c>
-      <c r="E75" s="150"/>
-      <c r="F75" s="148"/>
-      <c r="G75" s="152"/>
-      <c r="H75" s="148"/>
+      <c r="E75" s="152"/>
+      <c r="F75" s="147"/>
+      <c r="G75" s="149"/>
+      <c r="H75" s="147"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="20"/>
@@ -49674,34 +50298,34 @@
       <c r="H88" s="20"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="148"/>
-      <c r="B89" s="148"/>
+      <c r="A89" s="147"/>
+      <c r="B89" s="147"/>
       <c r="C89" s="32" t="s">
         <v>225</v>
       </c>
       <c r="D89" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="E89" s="151" t="s">
+      <c r="E89" s="148" t="s">
         <v>121</v>
       </c>
-      <c r="F89" s="151"/>
-      <c r="G89" s="152"/>
-      <c r="H89" s="148"/>
+      <c r="F89" s="148"/>
+      <c r="G89" s="149"/>
+      <c r="H89" s="147"/>
     </row>
     <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A90" s="148"/>
-      <c r="B90" s="148"/>
+      <c r="A90" s="147"/>
+      <c r="B90" s="147"/>
       <c r="C90" s="32" t="s">
         <v>242</v>
       </c>
       <c r="D90" s="32" t="s">
         <v>243</v>
       </c>
-      <c r="E90" s="151"/>
-      <c r="F90" s="151"/>
-      <c r="G90" s="152"/>
-      <c r="H90" s="148"/>
+      <c r="E90" s="148"/>
+      <c r="F90" s="148"/>
+      <c r="G90" s="149"/>
+      <c r="H90" s="147"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="20"/>
@@ -50069,6 +50693,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F74:F75"/>
     <mergeCell ref="H74:H75"/>
     <mergeCell ref="A89:A90"/>
     <mergeCell ref="B89:B90"/>
@@ -50077,17 +50706,13 @@
     <mergeCell ref="G89:G90"/>
     <mergeCell ref="H89:H90"/>
     <mergeCell ref="G74:G75"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F74:F75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -50182,10 +50807,11 @@
     <sortCondition ref="A1:A16"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0BB7-C151-C94B-945C-E2CA92034B13}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -50310,6 +50936,7 @@
     <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -50431,6 +51058,7 @@
     <mergeCell ref="A4:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -50762,11 +51390,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B7:B13"/>
-    <mergeCell ref="A7:A13"/>
-    <mergeCell ref="C7:C13"/>
     <mergeCell ref="B38:B42"/>
     <mergeCell ref="A14:A42"/>
     <mergeCell ref="C14:C42"/>
@@ -50776,8 +51399,14 @@
     <mergeCell ref="B28:B37"/>
     <mergeCell ref="B14:B20"/>
     <mergeCell ref="B21:B27"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B7:B13"/>
+    <mergeCell ref="A7:A13"/>
+    <mergeCell ref="C7:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -50928,6 +51557,7 @@
     <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -51023,6 +51653,7 @@
     <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -51193,6 +51824,12 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C14:C16"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="C8:C10"/>
@@ -51201,14 +51838,9 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="C14:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -51266,7 +51898,7 @@
       <c r="A5" s="104" t="s">
         <v>397</v>
       </c>
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="126" t="s">
         <v>396</v>
       </c>
       <c r="C5" s="104" t="s">
@@ -51275,37 +51907,37 @@
     </row>
     <row r="6" spans="1:3" s="10" customFormat="1" ht="283" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="115"/>
-      <c r="B6" s="125"/>
+      <c r="B6" s="127"/>
       <c r="C6" s="115"/>
     </row>
     <row r="7" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="115"/>
-      <c r="B7" s="125"/>
+      <c r="B7" s="127"/>
       <c r="C7" s="115"/>
     </row>
     <row r="8" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="115"/>
-      <c r="B8" s="125"/>
+      <c r="B8" s="127"/>
       <c r="C8" s="115"/>
     </row>
     <row r="9" spans="1:3" s="10" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="115"/>
-      <c r="B9" s="125"/>
+      <c r="B9" s="127"/>
       <c r="C9" s="115"/>
     </row>
     <row r="10" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="115"/>
-      <c r="B10" s="125"/>
+      <c r="B10" s="127"/>
       <c r="C10" s="115"/>
     </row>
     <row r="11" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="115"/>
-      <c r="B11" s="125"/>
+      <c r="B11" s="127"/>
       <c r="C11" s="115"/>
     </row>
     <row r="12" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="105"/>
-      <c r="B12" s="126"/>
+      <c r="B12" s="128"/>
       <c r="C12" s="105"/>
     </row>
     <row r="13" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -51543,7 +52175,7 @@
     </row>
     <row r="50" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="115"/>
-      <c r="B50" s="127"/>
+      <c r="B50" s="125"/>
       <c r="C50" s="115"/>
     </row>
     <row r="51" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -51566,7 +52198,7 @@
       <c r="A53" s="104" t="s">
         <v>415</v>
       </c>
-      <c r="B53" s="128" t="s">
+      <c r="B53" s="124" t="s">
         <v>416</v>
       </c>
       <c r="C53" s="104" t="s">
@@ -51575,7 +52207,7 @@
     </row>
     <row r="54" spans="1:3" ht="238" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="115"/>
-      <c r="B54" s="128"/>
+      <c r="B54" s="124"/>
       <c r="C54" s="115"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -51587,12 +52219,12 @@
     </row>
     <row r="56" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="115"/>
-      <c r="B56" s="127"/>
+      <c r="B56" s="125"/>
       <c r="C56" s="115"/>
     </row>
     <row r="57" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="115"/>
-      <c r="B57" s="127"/>
+      <c r="B57" s="125"/>
       <c r="C57" s="115"/>
     </row>
     <row r="58" spans="1:3" ht="172" customHeight="1" x14ac:dyDescent="0.2">
@@ -51609,12 +52241,12 @@
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="115"/>
-      <c r="B60" s="127"/>
+      <c r="B60" s="125"/>
       <c r="C60" s="115"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="115"/>
-      <c r="B61" s="127"/>
+      <c r="B61" s="125"/>
       <c r="C61" s="115"/>
     </row>
     <row r="62" spans="1:3" ht="125" customHeight="1" x14ac:dyDescent="0.2">
@@ -51631,17 +52263,17 @@
     </row>
     <row r="64" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="115"/>
-      <c r="B64" s="127"/>
+      <c r="B64" s="125"/>
       <c r="C64" s="115"/>
     </row>
     <row r="65" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="115"/>
-      <c r="B65" s="127"/>
+      <c r="B65" s="125"/>
       <c r="C65" s="115"/>
     </row>
     <row r="66" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="115"/>
-      <c r="B66" s="127"/>
+      <c r="B66" s="125"/>
       <c r="C66" s="115"/>
     </row>
     <row r="67" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -51685,11 +52317,18 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="25">
-    <mergeCell ref="C53:C67"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="B63:B67"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B5:B12"/>
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="C5:C12"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="C13:C41"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B24:B27"/>
     <mergeCell ref="A53:A67"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="B32:B35"/>
@@ -51698,19 +52337,13 @@
     <mergeCell ref="A13:A41"/>
     <mergeCell ref="B49:B51"/>
     <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="C13:C41"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B5:B12"/>
-    <mergeCell ref="A5:A12"/>
-    <mergeCell ref="C5:C12"/>
+    <mergeCell ref="C53:C67"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="B63:B67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the files under lib/lang/th for supporting the thai language.
</commit_message>
<xml_diff>
--- a/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+++ b/docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10503"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanket/Desktop/DBOT/HAFELE/docs/specification/hafele-v1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{588D9048-2FD3-6F4B-8840-00C79F0E8920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5174E7-2105-2F4D-90CA-A34415759F99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" firstSheet="25" activeTab="35" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" firstSheet="26" activeTab="36" xr2:uid="{F796B3DD-3F44-644C-8065-1F1566EFA78E}"/>
   </bookViews>
   <sheets>
     <sheet name="SPEC - 1.1" sheetId="1" r:id="rId1"/>
@@ -49,12 +49,14 @@
     <sheet name="SPEC - 4.9" sheetId="39" r:id="rId34"/>
     <sheet name="SPEC - 5.0" sheetId="40" r:id="rId35"/>
     <sheet name="SPEC - 5.1" sheetId="41" r:id="rId36"/>
-    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId37"/>
-    <sheet name="PLAYGROUND" sheetId="6" r:id="rId38"/>
-    <sheet name="TEMPLATE" sheetId="8" r:id="rId39"/>
+    <sheet name="SPEC - 6" sheetId="42" r:id="rId37"/>
+    <sheet name="ORIGINAL SURVEY" sheetId="5" r:id="rId38"/>
+    <sheet name="PLAYGROUND" sheetId="6" r:id="rId39"/>
+    <sheet name="TEMPLATE" sheetId="8" r:id="rId40"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="35">'SPEC - 5.1'!$A:$C</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="36">'SPEC - 6'!$A:$C</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -74,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="1211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="1229">
   <si>
     <t>mkdir HAFELE</t>
   </si>
@@ -40836,6 +40838,632 @@
   </si>
   <si>
     <t>git commit -m "ER5200 is now in the swing door and sliding door section and also provided validation messages for locks ER5200 and DL6600 as per validation request sought. "</t>
+  </si>
+  <si>
+    <t>LANGUAGE TRANSLATION - AS PER FTRANSLAED FILES RECEIVED FROM HAFELE</t>
+  </si>
+  <si>
+    <t>use strict';
+/* * The Door Enumeration Values (TH).
+ *  @author   Sanket Rajgarhia
+ *  @date 31/03/2022 (dd/mm/yyyy)
+ *  @version 1.0
+ *  @language: th
+ * */
+/*****************************************************************************/
+/* DOOR ENUMERATION (TH)                                                     */
+/*****************************************************************************/
+/* Door Material specification */
+const DOOR_MATERIAL = {
+    WOOD: "ไม้",
+    GLASS: "กระจกเปลือย",
+    STEEL: "เหล็ก",
+    ALUMINIUM: "อะลูมิเนียม",
+    PVC: "พลาสติกPVC",
+    UPVC: "UPVC",
+    WPC: "WPC"
+};
+/* Door Condition Specification */
+const DOOR_CONDITION = {
+    INSTALLED: "บานประตูเดิมที่มีการติดตั้งมือจับมาแล้ว",
+    NEW: "บานประตูใหม่ ไม่เคยติดตั้งมือจับมาก่อน"
+}
+/* Door Installation Location */
+const DOOR_INSTALLATION_LOCATION = {
+    INDOOR: "ติดตั้งภายในร่ม",
+    OUTDOOR_PROTECTED: "ติดตั้งภายนอก (มีการป้องกันจากน้ำฝนและแดดจัด)",
+    OUTDOOR_EXPOSED: "ติดตั้งภายนอก (ถูกน้ำฝนและแสงแดดโดยตรง)",
+    GARAGE_DOOR_EXAMPLE: "GARAGE DOOR"
+}
+/* Thickness of the door */
+const DOOR_THICKNESS_IN_MM = {
+    MM_30_TO_50: "30-50 มม.",
+    MM_32_TO_50: "32-50 มม.",
+    MM_35_TO_50: "35-50 มม.",
+    MM_35_TO_60: "35-60 มม.",
+    MM_35_TO_90: "35-90 มม.",
+    MM_OTHER: "กรอกความหนาที่วัดได้ "
+}
+/* Door Type */
+const DOOR_TYPE = {
+    SLIDING_DOOR: "บานเลื่อน",
+    SWING_DOOR: "บานเปิดเข้า - ออก ทางเดียว"
+}
+/* Swing Door Type */
+const SWING_DOOR_TYPE = {
+    SWING_DOOR_SINGLE: "ประตูบานเดี่ยว",
+    SWING_DOOR_DOUBLE: "ประตูบานคู่"
+}
+/* Swing Door Jamb */
+const SWING_DOOR_JAMB = {
+    FLUSH_DOOR: "แบบไม่มีซับวงกบ",
+    REBATED_DOOR: "แบบมีซับวงกบ",
+    DOUBLE_LEAF_DOOR: "แบบประตูบานคู่(บานฟิกซ์)"
+}
+/* Door Retrofit */
+const DOOR_RETROFIT = {
+    LEVER_HANDLE: "ติดตั้งชุดล็อคระบบมอทิส",
+    KNOB: "ติดตั้งชุดล็อคลูกบิดหรือลูกบิดก้านโยก",
+    GRIP: "ติดตั้งชุดล็อค Grip Handle"
+}
+/* Swing Door Leaf Types */
+const SWING_DOOR_LEAF = {
+    PLAIN_LEAF: "บานประตูแบบเรียบทั้งบาน",
+    DOOR_LEAF_WITH_MULLION_LESS_THAN_50_MM: "บานประตูมีลูกฟัก กรอบบานกว้างน้อยกว่า 50 มม.",
+    DOOR_LEAF_WITH_MULLION_EQUAL_OR_MORE_THAN_50_MM: "บานประตูมีลูกฟัก กรอบบานกว้างมากกว่า 50 มม.",
+    DOOR_LEAF_WITH_MULLION_LESS_THAN_60_MM: "บานประตูมีลูกฟัก กรอบบานกว้างน้อยกว่า 60 มม.",
+    DOOR_LEAF_WITH_MULLION_EQUAL_OR_MORE_THAN_60_MM: "บานประตูมีลูกฟัก กรอบบานกว้างมากกว่า 60 มม.",
+    DOOR_LEAF_WITH_MULLION_LESS_THAN_100_MM: "บานประตูมีลูกฟัก กรอบบานกว้างน้อยกว่า 100 มม.",
+    DOOR_LEAF_WITH_MULLION_EQUAL_OR_MORE_THAN_100_MM: "บานประตูมีลูกฟัก กรอบบานกว้างมากกว่า 100 มม.",
+    DOOR_LEAF_WITH_MULLION_LESS_THAN_130_MM: "บานประตูมีลูกฟัก กรอบบานกว้างน้อยกว่า 130 มม.",
+    DOOR_LEAF_WITH_MULLION_EQUAL_OR_MORE_THAN_130_MM: "บานประตูมีลูกฟัก กรอบบานกว้างมากกว่า 130 มม.",
+    DOOR_LEAF_WITH_FRAME_LESS_THAN_50_MM: "ประตูกระจกมีกรอบบาน กรอบบานกว้างน้อยกว่า 50 มม.",
+    DOOR_LEAF_WITH_FRAME_EQUAL_OR_MORE_THAN_50_MM: "ประตูกระจกมีกรอบบาน กรอบบานกว้างมากกว่า 50 มม.",
+    DOOR_LEAF_WITH_FRAME_LESS_THAN_60_MM: "ประตูกระจกมีกรอบบาน กรอบบานกว้างน้อยกว่า 60 มม.",
+    DOOR_LEAF_WITH_FRAME_EQUAL_OR_MORE_THAN_60_MM: "ประตูกระจกมีกรอบบาน กรอบบานกว้างมากกว่า 60 มม.",
+    DOOR_LEAF_WITH_FRAME_LESS_THAN_100_MM: "ประตูกระจกมีกรอบบาน กรอบบานกว้างน้อยกว่า 100 มม.",
+    DOOR_LEAF_WITH_FRAME_EQUAL_OR_MORE_THAN_100_MM: "ประตูกระจกมีกรอบบาน กรอบบานกว้างมากกว่า 100 มม.",
+    DOOR_LEAF_WITH_FRAME_LESS_THAN_130_MM: "ประตูกระจกมีกรอบบาน กรอบบานกว้างน้อยกว่า 130 มม.",
+    DOOR_LEAF_WITH_FRAME_EQUAL_OR_MORE_THAN_130_MM: "ประตูกระจกมีกรอบบาน กรอบบานกว้างมากกว่า 130 มม."
+}
+/* Sliding Door Leaf Types */
+const SLIDING_DOOR_LEAF = {
+    PLAIN_LEAF: "บานประตูแบบเรียบทั้งบาน",
+    WOODEN_LEAF_LESS_THAN_50_MM: "ประตูกระจกกรอบบานไม้ กรอบบานกว้างน้อยกว่า 50 มม.",
+    WOODEN_LEAF_EQUAL_OR_MORE_THAN_50_MM: "ประตูกระจกกรอบบานไม้ กรอบบานกว้างมากกว่า 50 มม.",
+    ALUMINIUM_LEAF_LESS_THAN_50_MM: "ประตูกระจกกรอบบานอะลูมิเนียม กรอบบานกว้างน้อยกว่า 50 มม.",
+    ALUMINIUM_LEAF_EQUAL_OR_MORE_THAN_50_MM: "ประตูกระจกกรอบบานอะลูมิเนียม กรอบบานกว้างมากกว่า 50 มม.",
+    STEEL_LEAF_LESS_THAN_50_MM: "ประตูกระจกกรอบบานเหล็ก กรอบบานกว้างน้อยกว่า 50 มม.",
+    STEEL_LEAF_EQUAL_OR_MORE_THAN_50_MM: "ประตูกระจกกรอบบานเหล็ก กรอบบานกว้างมากกว่า 50 มม."
+}
+/*****************************************************************************/
+/* FREEZE - TO EMULATE ENUMERATION                                           */
+/*****************************************************************************/
+// Prevent addition of properties to the json Object
+Object.freeze(DOOR_MATERIAL);
+Object.freeze(DOOR_CONDITION);
+Object.freeze(DOOR_INSTALLATION_LOCATION);
+Object.freeze(DOOR_THICKNESS_IN_MM);
+Object.freeze(DOOR_TYPE);
+Object.freeze(SWING_DOOR_TYPE);
+Object.freeze(SWING_DOOR_JAMB);
+Object.freeze(DOOR_RETROFIT);
+Object.freeze(SWING_DOOR_LEAF);
+Object.freeze(SLIDING_DOOR_LEAF);
+/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lib/lang/th/enum/door/door-enum.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> for language translation to thai.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lib/lang/th/enum/door/door-enum.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> for language translation to thai.</t>
+    </r>
+  </si>
+  <si>
+    <t>use strict';
+/* * The Message Enumeration Values (TH).
+ *  @author   Sanket Rajgarhia
+ *  @date 05/04/2022 (dd/mm/yyyy)
+ *  @version 1.0
+ *  @language: th
+ * */
+/*****************************************************************************/
+/* MESSAGE ENUMERATION (TH)                                                  */
+/*****************************************************************************/
+// Messages
+const MESSAGE = {
+    MESSAGE_FAILURE: "ขออภัย ไม่สามารถติดตั้งล็อคที่เลือกได้",
+    MESSAGE_DOOR_TYPE_AND_LOCK_MISMATCH: "ประเภทของประตู ไม่เหมาะกับล็อครุ่นนี้ กรุณาเลือกล็อครุ่นอื่นแทน",
+    MESSAGE_JAMB_AND_LOCK_TYPE_MISMATCH: "ไม่แนะนำให้ใช้ล็อครุ่นนี้กับประตูบานคู่",
+    MESSAGE_DOOR_THICKNESS_AND_LOCK_MISMATCH: "ไม่สามารถติดตั้งล็อคกับความหนาประตูนี้ได้",
+    MESSAGE_MATERIAL_FAILURE: "วัสดุของประตูไม่สามารถติดตั้งล็อครุ่นนี้ได้",
+    MESSAGE_DOOR_LEAF_AND_DOOR_TYPE_MISMATCH: "ไม่สามารถติดตั้งล็อคกับกรอบบานนี้ได้",
+    MESSAGE_DOOR_LEAF_FRAME_THICKNESS_INADEQUATE: "ไม่สามารถติดตั้งล็อคกับกรอบบานเปิดนี้ได้",
+    MESSAGE_DOOR_LEAF_THICKNESS_INADEQUATE: "ไม่สามารถติดตั้งล็อคกับกรอบบานเลื่อนนี้ได้",
+    MESSAGE_MISSING_INPUT: "กรุณากรอกข้อมูลในช่องแดงให้ครบถ้วน"
+}
+// Caution messages
+const CAUTION = {
+    EXISTING_DOOR_RETROFIT_CAUTION: "หมายเหตุ :\n" +
+        "ล็อคอาจะปิดรูเจาะเดิมไม่หมด ช่างติดตั้งจะทำการอุดรูเจาะเดิมที่บานประตู ด้วย ซิลิโคน หรือวัสดุอื่นๆ",
+    EXISTING_DOOR_RETROFIT_RIM_LOCK_CAUTION: "หมายเหตุ: \n" +
+        "ล็อครุ่นนี้จะติดเสริมมือจับประตูเดิมที่ด้านบน",
+    SWING_DOOR_JAMB_CAUTION: "หมายเหตุ: \n" +
+        "ช่างติดตั้งอาจจะต้องทำการตัด เซาะ จุดที่จะต้องติดตั้งอุปกรณ์เพื่อให้ล็อคทำงานได้ดีที่สุด"
+}
+/*****************************************************************************/
+/* FREEZE - TO EMULATE ENUMERATION                                           */
+/*****************************************************************************/
+// Prevent addition of properties to the json Object
+Object.freeze(MESSAGE);
+Object.freeze(CAUTION);
+/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lib/lang/th/enum/message/message-enum.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> for language translation to thai.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lib/lang/th/enum/message/message-enum.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> for language translation to thai.</t>
+    </r>
+  </si>
+  <si>
+    <t>"use strict";
+/* * JavaScript for the file index.html
+ *  @author Sanket Rajgarhia
+ *  @date   22/04/2022 (dd/mm/yyyy)
+ *  @version 1.0
+ *  @language: th
+ * */
+/*****************************************************************************/
+/* PAGE COMPONENT ENUMERATIONS (TH)                                          */
+/*****************************************************************************/
+// index page title (TH)
+const INDEX = {
+    TITLE: "แบบสำรวจการเลือกรุ่นล็อคและสเปคประตูของลูกค้า",
+};
+// Lock selection card
+const LOCK_SELECTION_CARD = {
+    HEADER: "กรุณเลือกล็อคที่ท่านต้องการ",
+    LABEL_LOCK_MODEL: "ค้นหาล็อคที่ต้องการจากแถบเมนูนี้",
+    SUITABILITY_MESSAGE: "ล็อคนี้เหมาะสำหรับประเภทประตูต่อไปนี้",
+    LABEL_DOOR_TYPE: "ประเภทประตู : ",
+    LABEL_DOOR_THICKNESS: "ช่วงความหนาของประตู : ",
+};
+// Door specification card
+const DOOR_SPECIFICATION_CARD = {
+    HEADER: "เลือกขนาดประตู และรุ่นล็อคด้วยตนเอง",
+    PROCEED_MESSAGE: `คลิกที่ปุ่ม ` +
+        `&lt;span id="label-next" class="highlight-text"&gt;&lt;/span&gt; ` +
+        `และระบุข้อกำหนดของประตูเพื่อตรวจสอบความเหมาะสมของรุ่นล็อคกับประตูของท่าน`,
+    LABEL_NEXT: "ถัดไป",
+};
+// Navigation buttons
+const NAVIGATION_BUTTONS = {
+    SELECT_BUTTON: "     เลือก     ",
+    NEXT_BUTTON: "      ถัดไป      "
+};
+/*****************************************************************************/
+/* FREEZE - TO EMULATE ENUMERATION                                           */
+/*****************************************************************************/
+// Prevent addition of properties to the json Object
+Object.freeze(INDEX);
+Object.freeze(LOCK_SELECTION_CARD);
+Object.freeze(DOOR_SPECIFICATION_CARD);
+Object.freeze(NAVIGATION_BUTTONS);
+/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">lib/lang/th/enum/page/index-enum.js </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>to thai</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">lib/lang/th/enum/page/index-enum.js </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>to thai</t>
+    </r>
+  </si>
+  <si>
+    <t>"use strict";
+/* * JavaScript for the file survey-report.html
+ *  @author Sanket Rajgarhia
+ *  @date   17/04/2022 (dd/mm/yyyy)
+ *  @version 1.0
+ *  @language: th
+ * */
+/*****************************************************************************/
+/* PAGE COMPONENT ENUMERATIONS (TH)                                          */
+/*****************************************************************************/
+// Lock selection survey (TH)
+const LOCK_SELECTION_SURVEY = {
+    TITLE: "Lock Selection Survey",
+    PAGE_HEADING: "แบบสำรวจการเลือกรุ่นล็อคและสเปคประตูของลูกค้า",
+    LOCK_CARD_HEADING: "ข้อมูลประตูและล็อค",
+    LOCK_MODEL: "กรุณาเลือกรุ่นล็อค",
+    LOCK_INSTALLATION_LOCATION: "สภาพแวดล้อมที่จะติดตั้ง",
+    LOCK_DOOR_CONDITION: "ประตูที่จะติดตั้ง",
+    LOCK_DOOR_RETROFIT: "ประเภทของล็อคที่มีการติดตั้งไว้แล้ว",
+    LOCK_DOOR_TYPE: "ประเภทประตูตามวิธีการเปิด",
+    LOCK_SWING_DOOR_TYPE: "บานเปิดเข้า/ออก ทางเดียว",
+    LOCK_SWING_DOOR_JAMB: "ชนิดของวงกบ",
+    LOCK_DOOR_THICKNESS: "ช่วงความหนาบานประตู",
+    LOCK_DOOR_THICKNESS_INPUT: "กรุณากรอกความหนาในหน่วยมิลลิเมตร (มม.)",
+    LOCK_DOOR_MATERIAL: "วัสดุของประตู",
+    LOCK_DOOR_LEAF: "ชนิดบานประตูและความกว้างกรอบบาน",
+    LOCK_DOOR_LEAF_GROUP_LABEL_START: "",
+    LOCK_DOOR_LEAF_GROUP_LABEL_SWING_DOOR: "บานเปิดเข้า/ออก ทางเดียว",
+    LOCK_DOOR_LEAF_GROUP_LABEL_SLIDING_DOOR: "บานเลื่อน",
+    CUSTOMER_CARD_HEADING: "ข้อมูลของลูกค้า",
+    CUSTOMER_NAME_PLACEHOLDER: "ชื่อ-นามสกุล ลูกค้า",
+    CUSTOMER_NAME_INVALID_MESSAGE_FEEDBACK: "กรุณาใส่ชื่อและนามสกุล",
+    CUSTOMER_NAME_LENGTH_INVALID_MESSAGE_FEEDBACK: "ไม่สามารถใส่ชื่อและนามสกุล " +
+        "ได้เกิน 50 ตัวอักษร",
+    CUSTOMER_MOBILE_PLACEHOLDER: "เบอร์มือถือลูกค้า",
+    CUSTOMER_MOBILE_INVALID_MESSAGE_FEEDBACK: "กรุณาใส่เบอร์มือถือลูกค้าที่ติดต่อได้",
+    CUSTOMER_MOBILE_DIGITS_INVALID_MESSAGE_FEEDBACK: "เบอร์มือถือจะต้องประกอบด้วย " +
+        "ตัวเลข 10 หลัก และขึ้นต้นด้วย 0",
+    CUSTOMER_ADDRESS1_PLACEHOLDER: "กรุณใส่ที่อยู่ที่ต้องการติดตั้งล็อค - แถวที่ 1",
+    CUSTOMER_ADDRESS1_INVALID_MESSAGE_FEEDBACK: "กรุณใส่ที่อยู่ที่ต้องการติดตั้งล็อค",
+    CUSTOMER_ADDRESS1_LENGTH_INVALID_MESSAGE_FEEDBACK: "ไม่สามารถใส่ตัวอักษรได้เกิน 50 ตัว " +
+        "กรุณาใส่ต่อในแถวถัดไป",
+    CUSTOMER_ADDRESS2_PLACEHOLDER: "กรุณใส่ที่อยู่ที่ต้องการติดตั้งล็อค - แถวที่ 2",
+    CUSTOMER_ADDRESS2_INVALID_MESSAGE_FEEDBACK: "ไม่สามารถใส่ตัวอักษรได้เกิน 50 ตัว " +
+        "กรุณาใส่ต่อในแถวถัดไป",
+    CUSTOMER_ADDRESS3_PLACEHOLDER: "กรุณใส่ที่อยู่ที่ต้องการติดตั้งล็อค - แถวที่ 3",
+    CUSTOMER_ADDRESS3_INVALID_MESSAGE_FEEDBACK: "ไม่สามารถใส่ตัวอักษรได้เกิน 50 ตัว " +
+        "กรุณาใส่ต่อในแถวถัดไป",
+    CUSTOMER_ADDITIONAL_INFORMATION_PLACEHOLDER: "ข้อมูลเพิ่มเติม เช่น จุดสังเกตุของบ้าน ฯลฯ ",
+    CUSTOMER_ADDITIONAL_INFORMATION_INVALID_MESSAGE_FEEDBACK: "ข้อมูลเพิ่มเติมนี้ " +
+        "ไม่สามารถใส่ตัวอักษรได้เกิน 250 ตัว.",
+    SALES_PERSON_CARD_HEADING: "ข้อมูลพนักงานตัวแทนขาย",
+    SALES_PERSON_ID_PLACEHOLDER: "รหัสพนักงานขาย	",
+    SALES_PERSON_ID_INVALID_MESSAGE_FEEDBACK: "กรุณาใส่รหัสพนักงานขาย",
+    SALES_PERSON_ID_LENGTH_INVALID_MESSAGE_FEEDBACK: "รหัสพนักงานขาย " +
+        " ไม่สามารถใส่ได้เกิน 50 ตัวอักษร",
+    SALES_PERSON_NAME_PLACEHOLDER: "ชื่อ-สกุล พนักงานขาย",
+    SALES_PERSON_NAME_INVALID_MESSAGE_FEEDBACK: "กรุณาใส่ ชื่อ-สกุล พนักงานขาย",
+    SALES_PERSON_NAME_LENGTH_INVALID_MESSAGE_FEEDBACK: "ชื่อ-สกุล พนักงานขาย " +
+        "ไม่สามารถใส่ได้เกิน 50 ตัวอักษร",
+    SALES_PERSON_LOCATION_PLACEHOLDER: "สถานที่,ห้างร้าน - สาขาที่ขายล็อค",
+    SALES_PERSON_LOCATION_INVALID_MESSAGE_FEEDBACK: "ไม่สามารถ " +
+        "ใส่ข้อมูลได้เกิน 150 ตัวอักษร"
+};
+// Navigation buttons
+const NAVIGATION_BUTTONS = {
+    LOCK_PREVIOUS_BUTTON: "    กลับไป    ",
+    LOCK_NEXT_BUTTON: "      ต่อไป      "
+}
+/*****************************************************************************/
+/* FREEZE - TO EMULATE ENUMERATION                                           */
+/*****************************************************************************/
+// Prevent addition of properties to the json Object
+Object.freeze(LOCK_SELECTION_SURVEY);
+Object.freeze(NAVIGATION_BUTTONS);
+/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lib/lang/th/enum/page/lock-selection-survey-enum.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to thai</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lib/lang/th/enum/page/lock-selection-survey-enum.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to thai</t>
+    </r>
+  </si>
+  <si>
+    <t>"use strict";
+/* * JavaScript for the file survey-report.html
+ *  @author Sanket Rajgarhia
+ *  @date   09/04/2022 (dd/mm/yyyy)
+ *  @version 1.0
+ *  @language th
+ * */
+/*****************************************************************************/
+/* PAGE COMPONENT ENUMERATIONS (TH)                                          */
+/*****************************************************************************/
+// Report title (TH)
+const SURVEY_REPORT = {
+    TITLE: "Lock Selection Survey Report",
+    PAGE_HEADING: "แบบสำรวจการเลือกรุ่นล็อคและสเปคประตูของลูกค้า",
+    REPORT_TITLE: "ข้อมูลลูกค้าและข้อมูลพนักงานขาย",
+    PRINT_BUTTON: "  พิมพ์  &lt;span class=\"sr-only\"&gt;(current)&lt;/span&gt;",
+    DOWNLOAD_BUTTON: "ดาวน์โหลด "
+};
+/*****************************************************************************/
+/* REPORT_FIELDS ENUMERATIONS                                               */
+/*****************************************************************************/
+// Report Field labels (EN)
+const REPORT_FIELD = {
+    CUSTOMER_NAME: "ชื่อลูกค้า",
+    CUSTOMER_MOBILE: "เบอร์มือถือลูกค้า",
+    CUSTOMER_ADDRESS: "ที่อยู่ลูกค้า",
+    CUSTOMER_INFORMATION: "รายละเอียดเพิ่มเติม",
+    SALES_PERSON_ID: "รหัสพนักงานขาย",
+    SALES_PERSON_NAME: "ชื่อพนักงานขาย",
+    SALES_PERSON_LOCATION: "สถานที่,ห้างร้าน - สาขาที่ขายล็อค",
+    SURVEY_DETAILS: "ข้อมูลประตูและล็อคที่จะติดตั้ง",
+    LOCK_MODEL: "รุ่นโมเดลล็อค",
+    LOCK_INSTALLATION_LOCATION: "สภาพแวดล้อมที่จะติดตั้ง",
+    LOCK_INSTALLATION_LOCATION_MESSAGE: "",
+    LOCK_DOOR_CONDITION: "ประตูที่จะติดตั้ง",
+    LOCK_DOOR_CONDITION_MESSAGE: "",
+    LOCK_DOOR_RETROFIT: "บานประตูเดิมที่มีการติดตั้งมือจับมาแล้ว",
+    LOCK_DOOR_RETROFIT_MESSAGE: "",
+    LOCK_DOOR_RETROFIT_CAUTION: "",
+    LOCK_DOOR_TYPE: "ประเภทประตูตามวิธีการเปิด",
+    LOCK_DOOR_TYPE_MESSAGE: "",
+    LOCK_SWING_DOOR_TYPE: "บานเปิดเข้า - ออก ทางเดียว",
+    LOCK_SWING_DOOR_TYPE_MESSAGE: "",
+    LOCK_SWING_DOOR_JAMB: "ชนิดของวงกบ",
+    LOCK_SWING_DOOR_JAMB_MESSAGE: "",
+    LOCK_SWING_DOOR_JAMB_CAUTION: "",
+    LOCK_DOOR_THICKNESS: "ความหนาบานประตู",
+    LOCK_DOOR_THICKNESS_MESSAGE: "",
+    LOCK_DOOR_THICKNESS_INPUT: "ความหนาบานประตู",
+    LOCK_DOOR_THICKNESS_INPUT_MESSAGE: "",
+    LOCK_THICKNESS_MM: "มม.",
+    LOCK_DOOR_MATERIAL: "วัสดุของประตู",
+    LOCK_DOOR_MATERIAL_MESSAGE: "",
+    LOCK_DOOR_LEAF: "ชนิดบานประตูและความกว้างกรอบบาน",
+    LOCK_DOOR_LEAF_MESSAGE: ""
+};
+/*****************************************************************************/
+/* FREEZE - TO EMULATE ENUMERATION                                           */
+/*****************************************************************************/
+// Prevent addition of properties to the json Object
+Object.freeze(SURVEY_REPORT);
+Object.freeze(REPORT_FIELD);
+/*****************************************************************************/
+/* END OF FILE                                                               */
+/*****************************************************************************/</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Update the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lib/lang/th/enum/page/survey-report-enum.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to thai</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updated the file </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>lib/lang/th/enum/page/survey-report-enum.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to thai</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t>git status</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> - would display the following files.                                                                                                                                                                                                                                  On branch master
+Your branch is up to date with 'hafele/master'.
+Changes to be committed:
+  (use "git restore --staged &lt;file&gt;..." to unstage)
+        modified:   docs/specification/hafele-v1/HAFELE-SPEC-V-01.xlsx
+        modified:   lib/lang/th/enum/door/door-enum.js
+        modified:   lib/lang/th/enum/message/message-enum.js
+        modified:   lib/lang/th/enum/page/index-enum.js
+        modified:   lib/lang/th/enum/page/lock-selection-survey-enum.js
+        modified:   lib/lang/th/enum/page/survey-report-enum.js
+</t>
+    </r>
+  </si>
+  <si>
+    <t>git commit -m "Updated the files under lib/lang/th for supporting the thai language."</t>
   </si>
 </sst>
 </file>
@@ -41323,7 +41951,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -41646,12 +42274,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -41659,6 +42281,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -41685,16 +42313,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -41715,16 +42343,34 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -43176,14 +43822,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="17">
-    <mergeCell ref="B12:B18"/>
-    <mergeCell ref="A12:A18"/>
-    <mergeCell ref="C12:C18"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="C8:C10"/>
     <mergeCell ref="B30:B33"/>
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="C30:C33"/>
@@ -43193,6 +43831,14 @@
     <mergeCell ref="B27:B29"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="C27:C29"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="A12:A18"/>
+    <mergeCell ref="C12:C18"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="C8:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -43803,12 +44449,12 @@
     </row>
     <row r="34" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="115"/>
-      <c r="B34" s="125"/>
+      <c r="B34" s="127"/>
       <c r="C34" s="115"/>
     </row>
     <row r="35" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="115"/>
-      <c r="B35" s="125"/>
+      <c r="B35" s="127"/>
       <c r="C35" s="115"/>
     </row>
     <row r="36" spans="1:3" ht="126" customHeight="1" x14ac:dyDescent="0.2">
@@ -43825,27 +44471,27 @@
     </row>
     <row r="38" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="115"/>
-      <c r="B38" s="125"/>
+      <c r="B38" s="127"/>
       <c r="C38" s="115"/>
     </row>
     <row r="39" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="115"/>
-      <c r="B39" s="125"/>
+      <c r="B39" s="127"/>
       <c r="C39" s="115"/>
     </row>
     <row r="40" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="115"/>
-      <c r="B40" s="125"/>
+      <c r="B40" s="127"/>
       <c r="C40" s="115"/>
     </row>
     <row r="41" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="115"/>
-      <c r="B41" s="125"/>
+      <c r="B41" s="127"/>
       <c r="C41" s="115"/>
     </row>
     <row r="42" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="115"/>
-      <c r="B42" s="125"/>
+      <c r="B42" s="127"/>
       <c r="C42" s="115"/>
     </row>
     <row r="43" spans="1:3" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -43857,32 +44503,32 @@
     </row>
     <row r="44" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="115"/>
-      <c r="B44" s="125"/>
+      <c r="B44" s="127"/>
       <c r="C44" s="115"/>
     </row>
     <row r="45" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="115"/>
-      <c r="B45" s="125"/>
+      <c r="B45" s="127"/>
       <c r="C45" s="115"/>
     </row>
     <row r="46" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="115"/>
-      <c r="B46" s="125"/>
+      <c r="B46" s="127"/>
       <c r="C46" s="115"/>
     </row>
     <row r="47" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="115"/>
-      <c r="B47" s="125"/>
+      <c r="B47" s="127"/>
       <c r="C47" s="115"/>
     </row>
     <row r="48" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="115"/>
-      <c r="B48" s="125"/>
+      <c r="B48" s="127"/>
       <c r="C48" s="115"/>
     </row>
     <row r="49" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="115"/>
-      <c r="B49" s="125"/>
+      <c r="B49" s="127"/>
       <c r="C49" s="115"/>
     </row>
     <row r="50" spans="1:3" ht="320" customHeight="1" x14ac:dyDescent="0.2">
@@ -43899,22 +44545,22 @@
     </row>
     <row r="52" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="115"/>
-      <c r="B52" s="125"/>
+      <c r="B52" s="127"/>
       <c r="C52" s="115"/>
     </row>
     <row r="53" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="115"/>
-      <c r="B53" s="125"/>
+      <c r="B53" s="127"/>
       <c r="C53" s="115"/>
     </row>
     <row r="54" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="115"/>
-      <c r="B54" s="125"/>
+      <c r="B54" s="127"/>
       <c r="C54" s="115"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="115"/>
-      <c r="B55" s="125"/>
+      <c r="B55" s="127"/>
       <c r="C55" s="115"/>
     </row>
     <row r="56" spans="1:3" ht="97" customHeight="1" x14ac:dyDescent="0.2">
@@ -43931,27 +44577,27 @@
     </row>
     <row r="58" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="115"/>
-      <c r="B58" s="125"/>
+      <c r="B58" s="127"/>
       <c r="C58" s="115"/>
     </row>
     <row r="59" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="115"/>
-      <c r="B59" s="125"/>
+      <c r="B59" s="127"/>
       <c r="C59" s="115"/>
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="115"/>
-      <c r="B60" s="125"/>
+      <c r="B60" s="127"/>
       <c r="C60" s="115"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="115"/>
-      <c r="B61" s="125"/>
+      <c r="B61" s="127"/>
       <c r="C61" s="115"/>
     </row>
     <row r="62" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="115"/>
-      <c r="B62" s="125"/>
+      <c r="B62" s="127"/>
       <c r="C62" s="115"/>
     </row>
     <row r="63" spans="1:3" ht="146" customHeight="1" x14ac:dyDescent="0.2">
@@ -43986,7 +44632,7 @@
       <c r="A67" s="116" t="s">
         <v>638</v>
       </c>
-      <c r="B67" s="124" t="s">
+      <c r="B67" s="128" t="s">
         <v>637</v>
       </c>
       <c r="C67" s="116" t="s">
@@ -43995,19 +44641,19 @@
     </row>
     <row r="68" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="116"/>
-      <c r="B68" s="124"/>
+      <c r="B68" s="128"/>
       <c r="C68" s="116"/>
     </row>
     <row r="69" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="116"/>
-      <c r="B69" s="124"/>
+      <c r="B69" s="128"/>
       <c r="C69" s="116"/>
     </row>
     <row r="70" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="116" t="s">
         <v>643</v>
       </c>
-      <c r="B70" s="124" t="s">
+      <c r="B70" s="128" t="s">
         <v>640</v>
       </c>
       <c r="C70" s="116" t="s">
@@ -44016,59 +44662,59 @@
     </row>
     <row r="71" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="116"/>
-      <c r="B71" s="124"/>
+      <c r="B71" s="128"/>
       <c r="C71" s="116"/>
     </row>
     <row r="72" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="116"/>
-      <c r="B72" s="124"/>
+      <c r="B72" s="128"/>
       <c r="C72" s="116"/>
     </row>
     <row r="73" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="116"/>
-      <c r="B73" s="124"/>
+      <c r="B73" s="128"/>
       <c r="C73" s="116"/>
     </row>
     <row r="74" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="116"/>
-      <c r="B74" s="124"/>
+      <c r="B74" s="128"/>
       <c r="C74" s="116"/>
     </row>
     <row r="75" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="116"/>
-      <c r="B75" s="124"/>
+      <c r="B75" s="128"/>
       <c r="C75" s="116"/>
     </row>
     <row r="76" spans="1:3" ht="214" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="116"/>
-      <c r="B76" s="124"/>
+      <c r="B76" s="128"/>
       <c r="C76" s="116"/>
     </row>
     <row r="77" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="116"/>
-      <c r="B77" s="124" t="s">
+      <c r="B77" s="128" t="s">
         <v>641</v>
       </c>
       <c r="C77" s="116"/>
     </row>
     <row r="78" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="116"/>
-      <c r="B78" s="124"/>
+      <c r="B78" s="128"/>
       <c r="C78" s="116"/>
     </row>
     <row r="79" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="116"/>
-      <c r="B79" s="124"/>
+      <c r="B79" s="128"/>
       <c r="C79" s="116"/>
     </row>
     <row r="80" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="116"/>
-      <c r="B80" s="124"/>
+      <c r="B80" s="128"/>
       <c r="C80" s="116"/>
     </row>
     <row r="81" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="116"/>
-      <c r="B81" s="124"/>
+      <c r="B81" s="128"/>
       <c r="C81" s="116"/>
     </row>
     <row r="82" spans="1:3" ht="56" x14ac:dyDescent="0.2">
@@ -44176,18 +44822,12 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="30">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="A16:A26"/>
-    <mergeCell ref="C16:C26"/>
+    <mergeCell ref="B77:B81"/>
+    <mergeCell ref="A70:A81"/>
+    <mergeCell ref="C70:C81"/>
+    <mergeCell ref="B86:B91"/>
+    <mergeCell ref="A86:A91"/>
+    <mergeCell ref="C86:C91"/>
     <mergeCell ref="B67:B69"/>
     <mergeCell ref="A67:A69"/>
     <mergeCell ref="C67:C69"/>
@@ -44200,12 +44840,18 @@
     <mergeCell ref="B33:B36"/>
     <mergeCell ref="B37:B42"/>
     <mergeCell ref="B43:B50"/>
-    <mergeCell ref="B77:B81"/>
-    <mergeCell ref="A70:A81"/>
-    <mergeCell ref="C70:C81"/>
-    <mergeCell ref="B86:B91"/>
-    <mergeCell ref="A86:A91"/>
-    <mergeCell ref="C86:C91"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="B16:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="A16:A26"/>
+    <mergeCell ref="C16:C26"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="C8:C9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -45431,17 +46077,17 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="11">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="C11:C12"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="C13:C14"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="C11:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -45502,27 +46148,27 @@
     </row>
     <row r="5" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="115"/>
-      <c r="B5" s="125"/>
+      <c r="B5" s="127"/>
       <c r="C5" s="115"/>
     </row>
     <row r="6" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="115"/>
-      <c r="B6" s="125"/>
+      <c r="B6" s="127"/>
       <c r="C6" s="115"/>
     </row>
     <row r="7" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="115"/>
-      <c r="B7" s="125"/>
+      <c r="B7" s="127"/>
       <c r="C7" s="115"/>
     </row>
     <row r="8" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="115"/>
-      <c r="B8" s="125"/>
+      <c r="B8" s="127"/>
       <c r="C8" s="115"/>
     </row>
     <row r="9" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="115"/>
-      <c r="B9" s="125"/>
+      <c r="B9" s="127"/>
       <c r="C9" s="115"/>
     </row>
     <row r="10" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -45751,18 +46397,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="21">
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="A17:A26"/>
-    <mergeCell ref="C17:C26"/>
-    <mergeCell ref="B28:B34"/>
-    <mergeCell ref="A28:A34"/>
-    <mergeCell ref="C28:C34"/>
     <mergeCell ref="B13:B15"/>
     <mergeCell ref="A13:A15"/>
     <mergeCell ref="C13:C15"/>
@@ -45772,6 +46406,18 @@
     <mergeCell ref="B4:B10"/>
     <mergeCell ref="A4:A10"/>
     <mergeCell ref="C4:C10"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="A17:A26"/>
+    <mergeCell ref="C17:C26"/>
+    <mergeCell ref="B28:B34"/>
+    <mergeCell ref="A28:A34"/>
+    <mergeCell ref="C28:C34"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="C37:C38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -45823,7 +46469,7 @@
       <c r="A4" s="116" t="s">
         <v>832</v>
       </c>
-      <c r="B4" s="124" t="s">
+      <c r="B4" s="128" t="s">
         <v>831</v>
       </c>
       <c r="C4" s="116" t="s">
@@ -45832,7 +46478,7 @@
     </row>
     <row r="5" spans="1:3" s="10" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="116"/>
-      <c r="B5" s="124"/>
+      <c r="B5" s="128"/>
       <c r="C5" s="116"/>
     </row>
     <row r="6" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -45978,27 +46624,27 @@
     </row>
     <row r="5" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="115"/>
-      <c r="B5" s="125"/>
+      <c r="B5" s="127"/>
       <c r="C5" s="115"/>
     </row>
     <row r="6" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="115"/>
-      <c r="B6" s="125"/>
+      <c r="B6" s="127"/>
       <c r="C6" s="115"/>
     </row>
     <row r="7" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="115"/>
-      <c r="B7" s="125"/>
+      <c r="B7" s="127"/>
       <c r="C7" s="115"/>
     </row>
     <row r="8" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="115"/>
-      <c r="B8" s="125"/>
+      <c r="B8" s="127"/>
       <c r="C8" s="115"/>
     </row>
     <row r="9" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="115"/>
-      <c r="B9" s="125"/>
+      <c r="B9" s="127"/>
       <c r="C9" s="115"/>
     </row>
     <row r="10" spans="1:3" ht="337" customHeight="1" x14ac:dyDescent="0.2">
@@ -46015,27 +46661,27 @@
     </row>
     <row r="12" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="115"/>
-      <c r="B12" s="125"/>
+      <c r="B12" s="127"/>
       <c r="C12" s="115"/>
     </row>
     <row r="13" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="115"/>
-      <c r="B13" s="125"/>
+      <c r="B13" s="127"/>
       <c r="C13" s="115"/>
     </row>
     <row r="14" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="115"/>
-      <c r="B14" s="125"/>
+      <c r="B14" s="127"/>
       <c r="C14" s="115"/>
     </row>
     <row r="15" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="115"/>
-      <c r="B15" s="125"/>
+      <c r="B15" s="127"/>
       <c r="C15" s="115"/>
     </row>
     <row r="16" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="115"/>
-      <c r="B16" s="125"/>
+      <c r="B16" s="127"/>
       <c r="C16" s="115"/>
     </row>
     <row r="17" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
@@ -46052,27 +46698,27 @@
     </row>
     <row r="19" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="115"/>
-      <c r="B19" s="125"/>
+      <c r="B19" s="127"/>
       <c r="C19" s="115"/>
     </row>
     <row r="20" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="115"/>
-      <c r="B20" s="125"/>
+      <c r="B20" s="127"/>
       <c r="C20" s="115"/>
     </row>
     <row r="21" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="115"/>
-      <c r="B21" s="125"/>
+      <c r="B21" s="127"/>
       <c r="C21" s="115"/>
     </row>
     <row r="22" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="115"/>
-      <c r="B22" s="125"/>
+      <c r="B22" s="127"/>
       <c r="C22" s="115"/>
     </row>
     <row r="23" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="115"/>
-      <c r="B23" s="125"/>
+      <c r="B23" s="127"/>
       <c r="C23" s="115"/>
     </row>
     <row r="24" spans="1:3" s="86" customFormat="1" ht="121" customHeight="1" x14ac:dyDescent="0.2">
@@ -46116,7 +46762,7 @@
     </row>
     <row r="29" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="115"/>
-      <c r="B29" s="125"/>
+      <c r="B29" s="127"/>
       <c r="C29" s="115"/>
     </row>
     <row r="30" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -46144,7 +46790,7 @@
       <c r="A33" s="104" t="s">
         <v>865</v>
       </c>
-      <c r="B33" s="137" t="s">
+      <c r="B33" s="139" t="s">
         <v>864</v>
       </c>
       <c r="C33" s="104" t="s">
@@ -46160,7 +46806,7 @@
       <c r="A35" s="104" t="s">
         <v>868</v>
       </c>
-      <c r="B35" s="137" t="s">
+      <c r="B35" s="139" t="s">
         <v>867</v>
       </c>
       <c r="C35" s="104" t="s">
@@ -46169,7 +46815,7 @@
     </row>
     <row r="36" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="115"/>
-      <c r="B36" s="139"/>
+      <c r="B36" s="140"/>
       <c r="C36" s="115"/>
     </row>
     <row r="37" spans="1:3" s="86" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.2">
@@ -46181,7 +46827,7 @@
       <c r="A38" s="104" t="s">
         <v>871</v>
       </c>
-      <c r="B38" s="137" t="s">
+      <c r="B38" s="139" t="s">
         <v>870</v>
       </c>
       <c r="C38" s="104" t="s">
@@ -46208,7 +46854,7 @@
       <c r="A41" s="104" t="s">
         <v>876</v>
       </c>
-      <c r="B41" s="137" t="s">
+      <c r="B41" s="139" t="s">
         <v>877</v>
       </c>
       <c r="C41" s="104" t="s">
@@ -46224,7 +46870,7 @@
       <c r="A43" s="104" t="s">
         <v>880</v>
       </c>
-      <c r="B43" s="140" t="s">
+      <c r="B43" s="137" t="s">
         <v>879</v>
       </c>
       <c r="C43" s="104" t="s">
@@ -46240,7 +46886,7 @@
       <c r="A45" s="104" t="s">
         <v>883</v>
       </c>
-      <c r="B45" s="140" t="s">
+      <c r="B45" s="137" t="s">
         <v>882</v>
       </c>
       <c r="C45" s="104" t="s">
@@ -46256,7 +46902,7 @@
       <c r="A47" s="104" t="s">
         <v>885</v>
       </c>
-      <c r="B47" s="140" t="s">
+      <c r="B47" s="137" t="s">
         <v>887</v>
       </c>
       <c r="C47" s="104" t="s">
@@ -46272,7 +46918,7 @@
       <c r="A49" s="104" t="s">
         <v>888</v>
       </c>
-      <c r="B49" s="140" t="s">
+      <c r="B49" s="137" t="s">
         <v>890</v>
       </c>
       <c r="C49" s="104" t="s">
@@ -46288,7 +46934,7 @@
       <c r="A51" s="104" t="s">
         <v>892</v>
       </c>
-      <c r="B51" s="140" t="s">
+      <c r="B51" s="137" t="s">
         <v>891</v>
       </c>
       <c r="C51" s="104" t="s">
@@ -46304,7 +46950,7 @@
       <c r="A53" s="104" t="s">
         <v>895</v>
       </c>
-      <c r="B53" s="140" t="s">
+      <c r="B53" s="137" t="s">
         <v>894</v>
       </c>
       <c r="C53" s="104" t="s">
@@ -46320,7 +46966,7 @@
       <c r="A55" s="104" t="s">
         <v>898</v>
       </c>
-      <c r="B55" s="140" t="s">
+      <c r="B55" s="137" t="s">
         <v>897</v>
       </c>
       <c r="C55" s="104" t="s">
@@ -46379,53 +47025,53 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="47">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B4:B10"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A4:A26"/>
+    <mergeCell ref="C4:C26"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="C28:C30"/>
+    <mergeCell ref="B11:B17"/>
+    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="B31:B32"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
     <mergeCell ref="A53:A54"/>
     <mergeCell ref="B53:B54"/>
     <mergeCell ref="C53:C54"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="B55:B56"/>
     <mergeCell ref="C55:C56"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="C28:C30"/>
-    <mergeCell ref="B11:B17"/>
-    <mergeCell ref="B18:B24"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B4:B10"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A4:A26"/>
-    <mergeCell ref="C4:C26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -46486,27 +47132,27 @@
     </row>
     <row r="5" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="115"/>
-      <c r="B5" s="125"/>
+      <c r="B5" s="127"/>
       <c r="C5" s="115"/>
     </row>
     <row r="6" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="115"/>
-      <c r="B6" s="125"/>
+      <c r="B6" s="127"/>
       <c r="C6" s="115"/>
     </row>
     <row r="7" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="115"/>
-      <c r="B7" s="125"/>
+      <c r="B7" s="127"/>
       <c r="C7" s="115"/>
     </row>
     <row r="8" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="115"/>
-      <c r="B8" s="125"/>
+      <c r="B8" s="127"/>
       <c r="C8" s="115"/>
     </row>
     <row r="9" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="115"/>
-      <c r="B9" s="125"/>
+      <c r="B9" s="127"/>
       <c r="C9" s="115"/>
     </row>
     <row r="10" spans="1:3" ht="337" customHeight="1" x14ac:dyDescent="0.2">
@@ -46538,7 +47184,7 @@
     </row>
     <row r="13" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="115"/>
-      <c r="B13" s="125"/>
+      <c r="B13" s="127"/>
       <c r="C13" s="115"/>
     </row>
     <row r="14" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -46750,7 +47396,7 @@
       <c r="A16" s="104" t="s">
         <v>944</v>
       </c>
-      <c r="B16" s="125" t="s">
+      <c r="B16" s="127" t="s">
         <v>943</v>
       </c>
       <c r="C16" s="104" t="s">
@@ -46759,12 +47405,12 @@
     </row>
     <row r="17" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="115"/>
-      <c r="B17" s="125"/>
+      <c r="B17" s="127"/>
       <c r="C17" s="115"/>
     </row>
     <row r="18" spans="1:3" ht="337" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="115"/>
-      <c r="B18" s="125"/>
+      <c r="B18" s="127"/>
       <c r="C18" s="115"/>
     </row>
     <row r="19" spans="1:3" ht="108" customHeight="1" x14ac:dyDescent="0.2">
@@ -46787,7 +47433,7 @@
       <c r="A21" s="116" t="s">
         <v>950</v>
       </c>
-      <c r="B21" s="124" t="s">
+      <c r="B21" s="128" t="s">
         <v>949</v>
       </c>
       <c r="C21" s="116" t="s">
@@ -46796,7 +47442,7 @@
     </row>
     <row r="22" spans="1:3" s="86" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="116"/>
-      <c r="B22" s="124"/>
+      <c r="B22" s="128"/>
       <c r="C22" s="116"/>
     </row>
     <row r="23" spans="1:3" s="86" customFormat="1" ht="122" customHeight="1" x14ac:dyDescent="0.2">
@@ -47474,6 +48120,31 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="35">
+    <mergeCell ref="B41:B46"/>
+    <mergeCell ref="A41:A46"/>
+    <mergeCell ref="C41:C46"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="B28:B34"/>
+    <mergeCell ref="A28:A34"/>
+    <mergeCell ref="C28:C34"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="C21:C22"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="B12:B13"/>
@@ -47484,31 +48155,6 @@
     <mergeCell ref="B10:B11"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="C10:C11"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="B28:B34"/>
-    <mergeCell ref="A28:A34"/>
-    <mergeCell ref="C28:C34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="B41:B46"/>
-    <mergeCell ref="A41:A46"/>
-    <mergeCell ref="C41:C46"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="C39:C40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -47919,6 +48565,12 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="13">
+    <mergeCell ref="B22:B26"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="B15:B21"/>
@@ -47926,12 +48578,6 @@
     <mergeCell ref="C15:C21"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="B22:B26"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="C22:C26"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -48377,6 +49023,12 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="13">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="C20:C21"/>
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="C23:C24"/>
@@ -48384,12 +49036,6 @@
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="B20:B21"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="C20:C21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -48821,17 +49467,17 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="11">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="C4:C5"/>
     <mergeCell ref="B6:B15"/>
     <mergeCell ref="A6:A15"/>
     <mergeCell ref="C6:C15"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="C4:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -48938,7 +49584,7 @@
   </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -49032,14 +49678,14 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="8">
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:C7"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C6:C7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="40" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -49047,6 +49693,198 @@
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E82AD59D-FFDA-9448-BCC8-2130B8CA82A4}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="102" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+    </row>
+    <row r="2" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="108" t="s">
+        <v>1211</v>
+      </c>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+    </row>
+    <row r="3" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="10" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="116" t="s">
+        <v>1213</v>
+      </c>
+      <c r="B4" s="150" t="s">
+        <v>1212</v>
+      </c>
+      <c r="C4" s="116" t="s">
+        <v>1214</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="116"/>
+      <c r="B5" s="150"/>
+      <c r="C5" s="116"/>
+    </row>
+    <row r="6" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="116"/>
+      <c r="B6" s="150"/>
+      <c r="C6" s="116"/>
+    </row>
+    <row r="7" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="116"/>
+      <c r="B7" s="150"/>
+      <c r="C7" s="116"/>
+    </row>
+    <row r="8" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="104" t="s">
+        <v>1216</v>
+      </c>
+      <c r="B8" s="151" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C8" s="104" t="s">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" s="10" customFormat="1" ht="145" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="105"/>
+      <c r="B9" s="152"/>
+      <c r="C9" s="105"/>
+    </row>
+    <row r="10" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="136" t="s">
+        <v>1220</v>
+      </c>
+      <c r="B10" s="145" t="s">
+        <v>1218</v>
+      </c>
+      <c r="C10" s="136" t="s">
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="136"/>
+      <c r="B11" s="145"/>
+      <c r="C11" s="136"/>
+    </row>
+    <row r="12" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="116" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B12" s="145" t="s">
+        <v>1221</v>
+      </c>
+      <c r="C12" s="116" t="s">
+        <v>1223</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="116"/>
+      <c r="B13" s="145"/>
+      <c r="C13" s="116"/>
+    </row>
+    <row r="14" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="116"/>
+      <c r="B14" s="145"/>
+      <c r="C14" s="116"/>
+    </row>
+    <row r="15" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="104" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B15" s="147" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C15" s="104" t="s">
+        <v>1226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="115"/>
+      <c r="B16" s="148"/>
+      <c r="C16" s="115"/>
+    </row>
+    <row r="17" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="105"/>
+      <c r="B17" s="149"/>
+      <c r="C17" s="105"/>
+    </row>
+    <row r="18" spans="1:3" ht="238" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="77" t="s">
+        <v>1228</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>463</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
+  <mergeCells count="17">
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="C15:C17"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="40" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE113606-3FFA-8545-9BE3-5643B52A7CE9}">
   <dimension ref="A1:H116"/>
   <sheetViews>
@@ -49124,10 +49962,10 @@
       <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="150" t="s">
+      <c r="A6" s="153" t="s">
         <v>110</v>
       </c>
-      <c r="B6" s="150"/>
+      <c r="B6" s="153"/>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
@@ -50100,32 +50938,32 @@
       <c r="H73" s="20"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" s="147"/>
-      <c r="B74" s="151"/>
+      <c r="A74" s="154"/>
+      <c r="B74" s="155"/>
       <c r="C74" s="29" t="s">
         <v>225</v>
       </c>
       <c r="D74" s="29" t="s">
         <v>227</v>
       </c>
-      <c r="E74" s="152"/>
-      <c r="F74" s="147"/>
-      <c r="G74" s="149"/>
-      <c r="H74" s="147"/>
+      <c r="E74" s="156"/>
+      <c r="F74" s="154"/>
+      <c r="G74" s="158"/>
+      <c r="H74" s="154"/>
     </row>
     <row r="75" spans="1:8" ht="64" x14ac:dyDescent="0.2">
-      <c r="A75" s="147"/>
-      <c r="B75" s="151"/>
+      <c r="A75" s="154"/>
+      <c r="B75" s="155"/>
       <c r="C75" s="30" t="s">
         <v>226</v>
       </c>
       <c r="D75" s="30" t="s">
         <v>228</v>
       </c>
-      <c r="E75" s="152"/>
-      <c r="F75" s="147"/>
-      <c r="G75" s="149"/>
-      <c r="H75" s="147"/>
+      <c r="E75" s="156"/>
+      <c r="F75" s="154"/>
+      <c r="G75" s="158"/>
+      <c r="H75" s="154"/>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="20"/>
@@ -50298,34 +51136,34 @@
       <c r="H88" s="20"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" s="147"/>
-      <c r="B89" s="147"/>
+      <c r="A89" s="154"/>
+      <c r="B89" s="154"/>
       <c r="C89" s="32" t="s">
         <v>225</v>
       </c>
       <c r="D89" s="32" t="s">
         <v>227</v>
       </c>
-      <c r="E89" s="148" t="s">
+      <c r="E89" s="157" t="s">
         <v>121</v>
       </c>
-      <c r="F89" s="148"/>
-      <c r="G89" s="149"/>
-      <c r="H89" s="147"/>
+      <c r="F89" s="157"/>
+      <c r="G89" s="158"/>
+      <c r="H89" s="154"/>
     </row>
     <row r="90" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A90" s="147"/>
-      <c r="B90" s="147"/>
+      <c r="A90" s="154"/>
+      <c r="B90" s="154"/>
       <c r="C90" s="32" t="s">
         <v>242</v>
       </c>
       <c r="D90" s="32" t="s">
         <v>243</v>
       </c>
-      <c r="E90" s="148"/>
-      <c r="F90" s="148"/>
-      <c r="G90" s="149"/>
-      <c r="H90" s="147"/>
+      <c r="E90" s="157"/>
+      <c r="F90" s="157"/>
+      <c r="G90" s="158"/>
+      <c r="H90" s="154"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" s="20"/>
@@ -50693,11 +51531,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="F74:F75"/>
     <mergeCell ref="H74:H75"/>
     <mergeCell ref="A89:A90"/>
     <mergeCell ref="B89:B90"/>
@@ -50706,13 +51539,18 @@
     <mergeCell ref="G89:G90"/>
     <mergeCell ref="H89:H90"/>
     <mergeCell ref="G74:G75"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A74:A75"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="F74:F75"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF614A6-3B18-F548-8BDD-6DF53FE907E8}">
   <dimension ref="A1:A16"/>
   <sheetViews>
@@ -50806,135 +51644,6 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A16">
     <sortCondition ref="A1:A16"/>
   </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0BB7-C151-C94B-945C-E2CA92034B13}">
-  <dimension ref="A1:C15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="7"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="102" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-    </row>
-    <row r="2" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="108" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2" s="108"/>
-      <c r="C2" s="108"/>
-    </row>
-    <row r="3" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="B4" s="45" t="s">
-        <v>279</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="6"/>
-    </row>
-    <row r="6" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="50"/>
-      <c r="B6" s="51"/>
-      <c r="C6" s="50"/>
-    </row>
-    <row r="7" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="50"/>
-      <c r="B7" s="51"/>
-      <c r="C7" s="50"/>
-    </row>
-    <row r="8" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="50"/>
-      <c r="B8" s="51"/>
-      <c r="C8" s="50"/>
-    </row>
-    <row r="9" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-      <c r="B9" s="45"/>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3"/>
-      <c r="B10" s="45"/>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="52"/>
-      <c r="B11" s="51"/>
-      <c r="C11" s="52"/>
-    </row>
-    <row r="12" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="52"/>
-      <c r="B12" s="51"/>
-      <c r="C12" s="52"/>
-    </row>
-    <row r="13" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="52"/>
-      <c r="B13" s="51"/>
-      <c r="C13" s="52"/>
-    </row>
-    <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>298</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -51056,6 +51765,135 @@
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="B4:B6"/>
     <mergeCell ref="A4:A6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A08F0BB7-C151-C94B-945C-E2CA92034B13}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="48.6640625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="82.83203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="76.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="102" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+    </row>
+    <row r="2" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="108" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+    </row>
+    <row r="3" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>279</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="50"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="50"/>
+    </row>
+    <row r="7" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="50"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="50"/>
+    </row>
+    <row r="8" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="50"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="50"/>
+    </row>
+    <row r="9" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="52"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="52"/>
+    </row>
+    <row r="12" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="52"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="52"/>
+    </row>
+    <row r="13" spans="1:3" ht="23" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="52"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="52"/>
+    </row>
+    <row r="14" spans="1:3" ht="102" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>298</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -51390,6 +52228,11 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B7:B13"/>
+    <mergeCell ref="A7:A13"/>
+    <mergeCell ref="C7:C13"/>
     <mergeCell ref="B38:B42"/>
     <mergeCell ref="A14:A42"/>
     <mergeCell ref="C14:C42"/>
@@ -51399,11 +52242,6 @@
     <mergeCell ref="B28:B37"/>
     <mergeCell ref="B14:B20"/>
     <mergeCell ref="B21:B27"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B7:B13"/>
-    <mergeCell ref="A7:A13"/>
-    <mergeCell ref="C7:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -51824,12 +52662,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="14">
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="C14:C16"/>
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="C8:C10"/>
@@ -51838,6 +52670,12 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="C14:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -51898,7 +52736,7 @@
       <c r="A5" s="104" t="s">
         <v>397</v>
       </c>
-      <c r="B5" s="126" t="s">
+      <c r="B5" s="124" t="s">
         <v>396</v>
       </c>
       <c r="C5" s="104" t="s">
@@ -51907,37 +52745,37 @@
     </row>
     <row r="6" spans="1:3" s="10" customFormat="1" ht="283" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="115"/>
-      <c r="B6" s="127"/>
+      <c r="B6" s="125"/>
       <c r="C6" s="115"/>
     </row>
     <row r="7" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="115"/>
-      <c r="B7" s="127"/>
+      <c r="B7" s="125"/>
       <c r="C7" s="115"/>
     </row>
     <row r="8" spans="1:3" s="10" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="115"/>
-      <c r="B8" s="127"/>
+      <c r="B8" s="125"/>
       <c r="C8" s="115"/>
     </row>
     <row r="9" spans="1:3" s="10" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="115"/>
-      <c r="B9" s="127"/>
+      <c r="B9" s="125"/>
       <c r="C9" s="115"/>
     </row>
     <row r="10" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="115"/>
-      <c r="B10" s="127"/>
+      <c r="B10" s="125"/>
       <c r="C10" s="115"/>
     </row>
     <row r="11" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="115"/>
-      <c r="B11" s="127"/>
+      <c r="B11" s="125"/>
       <c r="C11" s="115"/>
     </row>
     <row r="12" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="105"/>
-      <c r="B12" s="128"/>
+      <c r="B12" s="126"/>
       <c r="C12" s="105"/>
     </row>
     <row r="13" spans="1:3" s="10" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -52175,7 +53013,7 @@
     </row>
     <row r="50" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="115"/>
-      <c r="B50" s="125"/>
+      <c r="B50" s="127"/>
       <c r="C50" s="115"/>
     </row>
     <row r="51" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -52198,7 +53036,7 @@
       <c r="A53" s="104" t="s">
         <v>415</v>
       </c>
-      <c r="B53" s="124" t="s">
+      <c r="B53" s="128" t="s">
         <v>416</v>
       </c>
       <c r="C53" s="104" t="s">
@@ -52207,7 +53045,7 @@
     </row>
     <row r="54" spans="1:3" ht="238" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="115"/>
-      <c r="B54" s="124"/>
+      <c r="B54" s="128"/>
       <c r="C54" s="115"/>
     </row>
     <row r="55" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -52219,12 +53057,12 @@
     </row>
     <row r="56" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="115"/>
-      <c r="B56" s="125"/>
+      <c r="B56" s="127"/>
       <c r="C56" s="115"/>
     </row>
     <row r="57" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="115"/>
-      <c r="B57" s="125"/>
+      <c r="B57" s="127"/>
       <c r="C57" s="115"/>
     </row>
     <row r="58" spans="1:3" ht="172" customHeight="1" x14ac:dyDescent="0.2">
@@ -52241,12 +53079,12 @@
     </row>
     <row r="60" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="115"/>
-      <c r="B60" s="125"/>
+      <c r="B60" s="127"/>
       <c r="C60" s="115"/>
     </row>
     <row r="61" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="115"/>
-      <c r="B61" s="125"/>
+      <c r="B61" s="127"/>
       <c r="C61" s="115"/>
     </row>
     <row r="62" spans="1:3" ht="125" customHeight="1" x14ac:dyDescent="0.2">
@@ -52263,17 +53101,17 @@
     </row>
     <row r="64" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="115"/>
-      <c r="B64" s="125"/>
+      <c r="B64" s="127"/>
       <c r="C64" s="115"/>
     </row>
     <row r="65" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="115"/>
-      <c r="B65" s="125"/>
+      <c r="B65" s="127"/>
       <c r="C65" s="115"/>
     </row>
     <row r="66" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="115"/>
-      <c r="B66" s="125"/>
+      <c r="B66" s="127"/>
       <c r="C66" s="115"/>
     </row>
     <row r="67" spans="1:3" ht="409" customHeight="1" x14ac:dyDescent="0.2">
@@ -52317,18 +53155,11 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="25">
-    <mergeCell ref="C49:C51"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="B5:B12"/>
-    <mergeCell ref="A5:A12"/>
-    <mergeCell ref="C5:C12"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A47:C47"/>
-    <mergeCell ref="C13:C41"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B16:B19"/>
-    <mergeCell ref="B20:B23"/>
-    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C53:C67"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="B59:B62"/>
+    <mergeCell ref="B63:B67"/>
     <mergeCell ref="A53:A67"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="B32:B35"/>
@@ -52337,11 +53168,18 @@
     <mergeCell ref="A13:A41"/>
     <mergeCell ref="B49:B51"/>
     <mergeCell ref="A49:A51"/>
-    <mergeCell ref="C53:C67"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B58"/>
-    <mergeCell ref="B59:B62"/>
-    <mergeCell ref="B63:B67"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="C13:C41"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="C49:C51"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B5:B12"/>
+    <mergeCell ref="A5:A12"/>
+    <mergeCell ref="C5:C12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>